<commit_message>
Excel format Adding some 'food'
Former-commit-id: ed57717198f08d9a33488c8ec3a602074d0adec9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3827,8 +3827,8 @@
   </sheetPr>
   <dimension ref="B1:BI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP13" workbookViewId="0">
-      <selection activeCell="BE18" sqref="BE18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16:V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3837,7 +3837,7 @@
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Dragon fat: +drifting, +speed
Former-commit-id: df49b04c0d737bf93fe91f8f420bc815627961fb
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3827,8 +3827,8 @@
   </sheetPr>
   <dimension ref="B1:BI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16:V27"/>
+    <sheetView tabSelected="1" topLeftCell="AP7" workbookViewId="0">
+      <selection activeCell="BC31" sqref="BC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4942,7 +4942,7 @@
         <v>4.5</v>
       </c>
       <c r="BC19" s="59">
-        <v>6.3</v>
+        <v>5</v>
       </c>
       <c r="BD19" s="59">
         <v>0.5</v>

</xml_diff>

<commit_message>
Dragon Fat mass increased
Former-commit-id: 2b2eca29df7aef3b21bb2db6337775bdb1bf90e3
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3828,7 +3828,7 @@
   <dimension ref="B1:BI55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AP7" workbookViewId="0">
-      <selection activeCell="BC31" sqref="BC31"/>
+      <selection activeCell="BB20" sqref="BB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4939,7 +4939,7 @@
         <v>360</v>
       </c>
       <c r="BB19" s="59">
-        <v>4.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="BC19" s="59">
         <v>5</v>

</xml_diff>

<commit_message>
Changed interpolation to calculate FrameWidth: lineal to cubic Setting some dragons FrameWidth modifiers
Former-commit-id: 1487807568cb2ad62892cc8b13910e58ab0d22ad
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3827,8 +3827,8 @@
   </sheetPr>
   <dimension ref="B1:BI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP7" workbookViewId="0">
-      <selection activeCell="BB20" sqref="BB20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4283,7 +4283,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="66">
-        <v>-5</v>
+        <v>-2.5</v>
       </c>
       <c r="M16" s="65">
         <v>75</v>
@@ -4461,7 +4461,7 @@
         <v>3</v>
       </c>
       <c r="L17" s="66">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="M17" s="65">
         <v>95</v>
@@ -4639,7 +4639,7 @@
         <v>5</v>
       </c>
       <c r="L18" s="66">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="M18" s="65">
         <v>140</v>
@@ -4817,7 +4817,7 @@
         <v>6</v>
       </c>
       <c r="L19" s="66">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="M19" s="65">
         <v>190</v>

</xml_diff>

<commit_message>
Super size mode duration increased
Former-commit-id: e91f61ec64242ab51a0ab5aaad0374f7796155ee
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3827,8 +3827,8 @@
   </sheetPr>
   <dimension ref="B1:BI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="AJ10" workbookViewId="0">
+      <selection activeCell="AU29" sqref="AU29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4384,7 +4384,7 @@
         <v>1</v>
       </c>
       <c r="AU16" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV16" s="24">
         <v>0.55999999999999994</v>
@@ -4562,7 +4562,7 @@
         <v>1</v>
       </c>
       <c r="AU17" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV17" s="24">
         <v>0.7</v>
@@ -4740,7 +4740,7 @@
         <v>1</v>
       </c>
       <c r="AU18" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV18" s="24">
         <v>0.7</v>
@@ -4918,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="AU19" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV19" s="24">
         <v>0.7</v>
@@ -5096,7 +5096,7 @@
         <v>1</v>
       </c>
       <c r="AU20" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV20" s="24">
         <v>0.7</v>
@@ -5274,7 +5274,7 @@
         <v>1</v>
       </c>
       <c r="AU21" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV21" s="24">
         <v>0.7</v>
@@ -5452,7 +5452,7 @@
         <v>1</v>
       </c>
       <c r="AU22" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV22" s="24">
         <v>0.7</v>
@@ -5634,7 +5634,7 @@
         <v>1</v>
       </c>
       <c r="AU23" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV23" s="24">
         <v>0.7</v>
@@ -5816,7 +5816,7 @@
         <v>1</v>
       </c>
       <c r="AU24" s="99">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV24" s="99">
         <v>0.7</v>
@@ -5998,7 +5998,7 @@
         <v>1</v>
       </c>
       <c r="AU25" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV25" s="24">
         <v>0.7</v>
@@ -6180,7 +6180,7 @@
         <v>1</v>
       </c>
       <c r="AU26" s="24">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AV26" s="24">
         <v>0.75</v>

</xml_diff>

<commit_message>
Modified maxScale for most of the dragons. Try to make notice player dragons scale when level up
Former-commit-id: 5c47d2e7417547115dadba0660952c67e08f2d0e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3827,8 +3827,8 @@
   </sheetPr>
   <dimension ref="B1:BI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ10" workbookViewId="0">
-      <selection activeCell="AU29" sqref="AU29"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4310,7 +4310,7 @@
         <v>0.46</v>
       </c>
       <c r="U16" s="29">
-        <v>0.56000000000000005</v>
+        <v>0.76</v>
       </c>
       <c r="V16" s="69">
         <v>14</v>
@@ -4488,7 +4488,7 @@
         <v>0.8</v>
       </c>
       <c r="U17" s="26">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V17" s="69">
         <v>16</v>
@@ -4666,7 +4666,7 @@
         <v>0.85</v>
       </c>
       <c r="U18" s="29">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="V18" s="50">
         <v>23.5</v>
@@ -4844,7 +4844,7 @@
         <v>0.9</v>
       </c>
       <c r="U19" s="26">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="V19" s="69">
         <v>19</v>
@@ -5022,7 +5022,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="29">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="V20" s="69">
         <v>20</v>
@@ -5200,7 +5200,7 @@
         <v>1.05</v>
       </c>
       <c r="U21" s="29">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="V21" s="69">
         <v>21</v>
@@ -5378,7 +5378,7 @@
         <v>1.35</v>
       </c>
       <c r="U22" s="29">
-        <v>1.45</v>
+        <v>1.55</v>
       </c>
       <c r="V22" s="69">
         <v>23.5</v>
@@ -5556,7 +5556,7 @@
         <v>1.54</v>
       </c>
       <c r="U23" s="29">
-        <v>1.7</v>
+        <v>1.74</v>
       </c>
       <c r="V23" s="50">
         <v>25</v>
@@ -5920,7 +5920,7 @@
         <v>1.37</v>
       </c>
       <c r="U25" s="26">
-        <v>1.47</v>
+        <v>1.57</v>
       </c>
       <c r="V25" s="50">
         <v>28</v>

</xml_diff>

<commit_message>
Dragons' force increased by leveling up
Former-commit-id: 8a2057f38f9b06b93730f8a843fc163612817469
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="193">
   <si>
     <t>[sku]</t>
   </si>
@@ -413,9 +413,6 @@
     <t>[mass]</t>
   </si>
   <si>
-    <t>[force]</t>
-  </si>
-  <si>
     <t>[furyBarRatio]</t>
   </si>
   <si>
@@ -600,6 +597,12 @@
   </si>
   <si>
     <t>TID_DRAGON_JAWFREY_DESC</t>
+  </si>
+  <si>
+    <t>[forceMin]</t>
+  </si>
+  <si>
+    <t>[forceMax]</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1484,11 +1487,94 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="97">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3344,56 +3430,6 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3408,88 +3444,91 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BI26" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87" totalsRowBorderDxfId="86">
-  <autoFilter ref="B15:BI26"/>
-  <tableColumns count="60">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="85"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="84"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="83"/>
-    <tableColumn id="3" name="[order]" dataDxfId="82"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="81"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="80"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="79"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="78"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="77"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="76"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="75"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="74"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="73"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="72"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="71"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="70"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="69"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="68"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="67"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="66"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="65"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="64"/>
-    <tableColumn id="41" name="[energyBase]" dataDxfId="63"/>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="62"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="61"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="60"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="59"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="58"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="57"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="56"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="55"/>
-    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="54"/>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="53"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="52"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="51"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="50"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="49"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="48"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="47"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="46"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="45"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="44"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="43"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="42"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="41"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="40"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="39"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BJ26" totalsRowShown="0" headerRowDxfId="96" dataDxfId="94" headerRowBorderDxfId="95" tableBorderDxfId="93" totalsRowBorderDxfId="92">
+  <autoFilter ref="B15:BJ26"/>
+  <tableColumns count="61">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="91"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="90"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="89"/>
+    <tableColumn id="3" name="[order]" dataDxfId="88"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="87"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="86"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="85"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="84"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="83"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="82"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="81"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="80"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="79"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="78"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="77"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="76"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="75"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="74"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="73"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="72"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="71"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="70"/>
+    <tableColumn id="41" name="[energyBase]" dataDxfId="69"/>
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="68"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="67"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="66"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="65"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="64"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="63"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="62"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="61"/>
+    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="60"/>
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="59"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="58"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="57"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="56"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="55"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="54"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="53"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="52"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="51"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="50"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="49"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="48"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="47"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="46"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="45"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="44">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="37">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="43">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="36"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="35"/>
-    <tableColumn id="34" name="[force]" dataDxfId="34"/>
-    <tableColumn id="35" name="[mass]" dataDxfId="33"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="32"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="31"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="30"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="29"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="28"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="27"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="42"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="41"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="40"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="0">
+      <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="35" name="[mass]" dataDxfId="39"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="38"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="37"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="36"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="35"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="34"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="33"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="18">
+    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3498,11 +3537,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B32:I33"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3515,7 +3554,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B44:W55"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3546,14 +3585,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B37:F40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="9"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="7"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3825,10 +3864,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BI55"/>
+  <dimension ref="B1:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="AP10" workbookViewId="0">
+      <selection activeCell="BB17" sqref="BB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3856,10 +3895,10 @@
     <col min="61" max="61" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:61" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:61" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3886,7 +3925,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3894,9 +3933,9 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:61" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:62" ht="117" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -3908,13 +3947,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -3925,7 +3964,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F5" s="13">
         <v>1</v>
@@ -3935,7 +3974,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -3946,7 +3985,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F6" s="13">
         <v>2</v>
@@ -3956,7 +3995,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -3967,7 +4006,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F7" s="16">
         <v>3</v>
@@ -3977,7 +4016,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -3988,7 +4027,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F8" s="13">
         <v>4</v>
@@ -3998,7 +4037,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4009,7 +4048,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F9" s="13">
         <v>4</v>
@@ -4019,10 +4058,10 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:61" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:61" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -4049,31 +4088,31 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:61" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:62" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W14"/>
       <c r="AA14" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AO14" s="115"/>
       <c r="AP14" s="115"/>
       <c r="AQ14" s="115"/>
       <c r="AR14" s="115"/>
     </row>
-    <row r="15" spans="2:61" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:62" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="76" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" s="79" t="s">
         <v>0</v>
@@ -4085,94 +4124,94 @@
         <v>15</v>
       </c>
       <c r="F15" s="77" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G15" s="94" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H15" s="93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I15" s="92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J15" s="91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K15" s="90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L15" s="88" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M15" s="86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N15" s="90" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O15" s="88" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P15" s="88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q15" s="87" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R15" s="87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S15" s="87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="T15" s="86" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U15" s="88" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V15" s="89" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="W15" s="86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X15" s="90" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y15" s="90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z15" s="88" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AA15" s="89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB15" s="88" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AC15" s="88" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AD15" s="88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AE15" s="88" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AF15" s="87" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AG15" s="86" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AH15" s="86" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AI15" s="86" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AJ15" s="85" t="s">
         <v>17</v>
@@ -4181,37 +4220,37 @@
         <v>18</v>
       </c>
       <c r="AL15" s="83" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AM15" s="83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AN15" s="83" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AO15" s="83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AP15" s="84" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AQ15" s="83" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AR15" s="83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AS15" s="83" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AT15" s="83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AU15" s="83" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AV15" s="83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AW15" s="3" t="s">
         <v>4</v>
@@ -4220,40 +4259,43 @@
         <v>16</v>
       </c>
       <c r="AY15" s="81" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AZ15" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="BA15" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="BB15" s="79" t="s">
+        <v>191</v>
+      </c>
+      <c r="BB15" s="76" t="s">
+        <v>192</v>
+      </c>
+      <c r="BC15" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="BC15" s="79" t="s">
+      <c r="BD15" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="BD15" s="79" t="s">
+      <c r="BE15" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="BE15" s="76" t="s">
+      <c r="BF15" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="BF15" s="76" t="s">
+      <c r="BG15" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="BG15" s="78" t="s">
+      <c r="BH15" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="BH15" s="77" t="s">
+      <c r="BI15" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="BI15" s="76" t="s">
+      <c r="BJ15" s="76" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4404,32 +4446,36 @@
       <c r="BA16" s="40">
         <v>175</v>
       </c>
-      <c r="BB16" s="59">
+      <c r="BB16" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>225</v>
+      </c>
+      <c r="BC16" s="59">
         <v>2</v>
       </c>
-      <c r="BC16" s="59">
+      <c r="BD16" s="59">
         <v>9.5</v>
       </c>
-      <c r="BD16" s="59">
+      <c r="BE16" s="59">
         <v>1</v>
       </c>
-      <c r="BE16" s="74">
+      <c r="BF16" s="74">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BF16" s="74">
+      <c r="BG16" s="74">
         <v>1.75</v>
       </c>
-      <c r="BG16" s="74">
+      <c r="BH16" s="74">
         <v>0</v>
       </c>
-      <c r="BH16" s="74">
+      <c r="BI16" s="74">
         <v>6</v>
       </c>
-      <c r="BI16" s="59" t="s">
+      <c r="BJ16" s="59" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -4582,32 +4628,36 @@
       <c r="BA17" s="40">
         <v>210</v>
       </c>
-      <c r="BB17" s="59">
+      <c r="BB17" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>260</v>
+      </c>
+      <c r="BC17" s="59">
         <v>2.1</v>
       </c>
-      <c r="BC17" s="59">
+      <c r="BD17" s="59">
         <v>9.5</v>
       </c>
-      <c r="BD17" s="59">
+      <c r="BE17" s="59">
         <v>1.7</v>
       </c>
-      <c r="BE17" s="59">
+      <c r="BF17" s="59">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BF17" s="59">
+      <c r="BG17" s="59">
         <v>2.1</v>
       </c>
-      <c r="BG17" s="59">
+      <c r="BH17" s="59">
         <v>0</v>
       </c>
-      <c r="BH17" s="59">
+      <c r="BI17" s="59">
         <v>6</v>
       </c>
-      <c r="BI17" s="59" t="s">
+      <c r="BJ17" s="59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -4760,32 +4810,36 @@
       <c r="BA18" s="40">
         <v>240</v>
       </c>
-      <c r="BB18" s="59">
+      <c r="BB18" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>290</v>
+      </c>
+      <c r="BC18" s="59">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BC18" s="59">
+      <c r="BD18" s="59">
         <v>9.5</v>
       </c>
-      <c r="BD18" s="59">
+      <c r="BE18" s="59">
         <v>1.7</v>
       </c>
-      <c r="BE18" s="59">
+      <c r="BF18" s="59">
         <v>0.9</v>
       </c>
-      <c r="BF18" s="59">
+      <c r="BG18" s="59">
         <v>2.25</v>
       </c>
-      <c r="BG18" s="59">
+      <c r="BH18" s="59">
         <v>0</v>
       </c>
-      <c r="BH18" s="59">
+      <c r="BI18" s="59">
         <v>6</v>
       </c>
-      <c r="BI18" s="38" t="s">
+      <c r="BJ18" s="38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -4938,32 +4992,36 @@
       <c r="BA19" s="40">
         <v>360</v>
       </c>
-      <c r="BB19" s="59">
+      <c r="BB19" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>410</v>
+      </c>
+      <c r="BC19" s="59">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BC19" s="59">
+      <c r="BD19" s="59">
         <v>5</v>
       </c>
-      <c r="BD19" s="59">
+      <c r="BE19" s="59">
         <v>0.5</v>
       </c>
-      <c r="BE19" s="59">
+      <c r="BF19" s="59">
         <v>1</v>
       </c>
-      <c r="BF19" s="59">
+      <c r="BG19" s="59">
         <v>1.3</v>
       </c>
-      <c r="BG19" s="59">
+      <c r="BH19" s="59">
         <v>0</v>
       </c>
-      <c r="BH19" s="59">
+      <c r="BI19" s="59">
         <v>6</v>
       </c>
-      <c r="BI19" s="38" t="s">
+      <c r="BJ19" s="38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5116,32 +5174,36 @@
       <c r="BA20" s="40">
         <v>300</v>
       </c>
-      <c r="BB20" s="59">
+      <c r="BB20" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>350</v>
+      </c>
+      <c r="BC20" s="59">
         <v>2.4</v>
       </c>
-      <c r="BC20" s="59">
+      <c r="BD20" s="59">
         <v>9.5</v>
       </c>
-      <c r="BD20" s="59">
+      <c r="BE20" s="59">
         <v>1.7</v>
       </c>
-      <c r="BE20" s="59">
+      <c r="BF20" s="59">
         <v>1</v>
       </c>
-      <c r="BF20" s="59">
+      <c r="BG20" s="59">
         <v>1.6</v>
       </c>
-      <c r="BG20" s="59">
+      <c r="BH20" s="59">
         <v>9</v>
       </c>
-      <c r="BH20" s="59">
+      <c r="BI20" s="59">
         <v>6</v>
       </c>
-      <c r="BI20" s="38" t="s">
+      <c r="BJ20" s="38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5294,32 +5356,36 @@
       <c r="BA21" s="40">
         <v>322</v>
       </c>
-      <c r="BB21" s="59">
+      <c r="BB21" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>372</v>
+      </c>
+      <c r="BC21" s="59">
         <v>2.5</v>
       </c>
-      <c r="BC21" s="59">
+      <c r="BD21" s="59">
         <v>9.5</v>
       </c>
-      <c r="BD21" s="59">
+      <c r="BE21" s="59">
         <v>1.7</v>
       </c>
-      <c r="BE21" s="59">
+      <c r="BF21" s="59">
         <v>0.5</v>
       </c>
-      <c r="BF21" s="59">
+      <c r="BG21" s="59">
         <v>1.9</v>
       </c>
-      <c r="BG21" s="59">
+      <c r="BH21" s="59">
         <v>9</v>
       </c>
-      <c r="BH21" s="59">
+      <c r="BI21" s="59">
         <v>6</v>
       </c>
-      <c r="BI21" s="38" t="s">
+      <c r="BJ21" s="38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -5472,32 +5538,36 @@
       <c r="BA22" s="40">
         <v>343</v>
       </c>
-      <c r="BB22" s="59">
+      <c r="BB22" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>393</v>
+      </c>
+      <c r="BC22" s="59">
         <v>2.6</v>
       </c>
-      <c r="BC22" s="59">
+      <c r="BD22" s="59">
         <v>9.5</v>
       </c>
-      <c r="BD22" s="59">
+      <c r="BE22" s="59">
         <v>1.7</v>
       </c>
-      <c r="BE22" s="59">
+      <c r="BF22" s="59">
         <v>0.5</v>
       </c>
-      <c r="BF22" s="59">
+      <c r="BG22" s="59">
         <v>2</v>
       </c>
-      <c r="BG22" s="59">
+      <c r="BH22" s="59">
         <v>9</v>
       </c>
-      <c r="BH22" s="59">
+      <c r="BI22" s="59">
         <v>6</v>
       </c>
-      <c r="BI22" s="38" t="s">
+      <c r="BJ22" s="38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -5654,37 +5724,41 @@
       <c r="BA23" s="40">
         <v>425</v>
       </c>
-      <c r="BB23" s="59">
+      <c r="BB23" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>475</v>
+      </c>
+      <c r="BC23" s="59">
         <v>3.2</v>
       </c>
-      <c r="BC23" s="59">
+      <c r="BD23" s="59">
         <v>9.5</v>
       </c>
-      <c r="BD23" s="59">
+      <c r="BE23" s="59">
         <v>1.7</v>
       </c>
-      <c r="BE23" s="59">
+      <c r="BF23" s="59">
         <v>0.5</v>
       </c>
-      <c r="BF23" s="59">
+      <c r="BG23" s="59">
         <v>1.2</v>
       </c>
-      <c r="BG23" s="59">
+      <c r="BH23" s="59">
         <v>45</v>
       </c>
-      <c r="BH23" s="59">
+      <c r="BI23" s="59">
         <v>15</v>
       </c>
-      <c r="BI23" s="38" t="s">
+      <c r="BJ23" s="38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="101" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D24" s="101" t="s">
         <v>84</v>
@@ -5783,13 +5857,13 @@
         <v>12</v>
       </c>
       <c r="AJ24" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK24" s="99" t="s">
         <v>188</v>
       </c>
-      <c r="AK24" s="99" t="s">
-        <v>189</v>
-      </c>
       <c r="AL24" s="99" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AM24" s="99" t="s">
         <v>5</v>
@@ -5822,10 +5896,10 @@
         <v>0.7</v>
       </c>
       <c r="AW24" s="103" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX24" s="21" t="s">
         <v>190</v>
-      </c>
-      <c r="AX24" s="21" t="s">
-        <v>191</v>
       </c>
       <c r="AY24" s="107">
         <v>1.6000000000000001E-3</v>
@@ -5836,32 +5910,36 @@
       <c r="BA24" s="109">
         <v>440</v>
       </c>
-      <c r="BB24" s="104">
+      <c r="BB24" s="128">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>490</v>
+      </c>
+      <c r="BC24" s="104">
         <v>3.4</v>
       </c>
-      <c r="BC24" s="104">
+      <c r="BD24" s="104">
         <v>9.5</v>
       </c>
-      <c r="BD24" s="104">
+      <c r="BE24" s="104">
         <v>1.7</v>
       </c>
-      <c r="BE24" s="104">
+      <c r="BF24" s="104">
         <v>0.6</v>
       </c>
-      <c r="BF24" s="104">
+      <c r="BG24" s="104">
         <v>1.2</v>
       </c>
-      <c r="BG24" s="104">
+      <c r="BH24" s="104">
         <v>45</v>
       </c>
-      <c r="BH24" s="104">
+      <c r="BI24" s="104">
         <v>15</v>
       </c>
-      <c r="BI24" s="101" t="s">
-        <v>187</v>
+      <c r="BJ24" s="101" t="s">
+        <v>186</v>
       </c>
     </row>
-    <row r="25" spans="2:61" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -5875,7 +5953,7 @@
         <v>9</v>
       </c>
       <c r="F25" s="57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G25" s="30">
         <v>2900000</v>
@@ -5977,7 +6055,7 @@
         <v>5</v>
       </c>
       <c r="AN25" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AO25" s="24">
         <v>1.2</v>
@@ -6018,32 +6096,36 @@
       <c r="BA25" s="40">
         <v>540</v>
       </c>
-      <c r="BB25" s="59">
+      <c r="BB25" s="127">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>590</v>
+      </c>
+      <c r="BC25" s="59">
         <v>3.9</v>
       </c>
-      <c r="BC25" s="59">
+      <c r="BD25" s="59">
         <v>9.5</v>
       </c>
-      <c r="BD25" s="59">
+      <c r="BE25" s="59">
         <v>1.7</v>
       </c>
-      <c r="BE25" s="59">
+      <c r="BF25" s="59">
         <v>0.3</v>
       </c>
-      <c r="BF25" s="59">
+      <c r="BG25" s="59">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BG25" s="59">
+      <c r="BH25" s="59">
         <v>45</v>
       </c>
-      <c r="BH25" s="59">
+      <c r="BI25" s="59">
         <v>15</v>
       </c>
-      <c r="BI25" s="38" t="s">
+      <c r="BJ25" s="38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:61" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6200,32 +6282,36 @@
       <c r="BA26" s="40">
         <v>680</v>
       </c>
-      <c r="BB26" s="39">
+      <c r="BB26" s="129">
+        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>730</v>
+      </c>
+      <c r="BC26" s="39">
         <v>4.7</v>
       </c>
-      <c r="BC26" s="39">
+      <c r="BD26" s="39">
         <v>9.5</v>
       </c>
-      <c r="BD26" s="39">
+      <c r="BE26" s="39">
         <v>1.7</v>
       </c>
-      <c r="BE26" s="39">
+      <c r="BF26" s="39">
         <v>0.2</v>
       </c>
-      <c r="BF26" s="39">
+      <c r="BG26" s="39">
         <v>0.15</v>
       </c>
-      <c r="BG26" s="39">
+      <c r="BH26" s="39">
         <v>59</v>
       </c>
-      <c r="BH26" s="39">
+      <c r="BI26" s="39">
         <v>15</v>
       </c>
-      <c r="BI26" s="38" t="s">
+      <c r="BJ26" s="38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:61" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:62" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
@@ -6284,8 +6370,8 @@
       <c r="BF27" s="114"/>
       <c r="BH27"/>
     </row>
-    <row r="29" spans="2:61" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:61" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -6299,7 +6385,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:61" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:62" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
@@ -6308,7 +6394,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:61" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:62" ht="140.25" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>64</v>
       </c>
@@ -7092,7 +7178,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D53">
         <v>20</v>
@@ -7302,19 +7388,19 @@
     <mergeCell ref="AA27:AF27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="95" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="94" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BI16:BI23 BI25:BI26">
-    <cfRule type="duplicateValues" dxfId="93" priority="3"/>
+  <conditionalFormatting sqref="BJ16:BJ23 BJ25:BJ26">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="92" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BI24">
-    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
+  <conditionalFormatting sqref="BJ24">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">

</xml_diff>

<commit_message>
energyBase increased by leveling up
Former-commit-id: b428aa7d7cbb327a7df67f6bdf08e83d87cd2296
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="194">
   <si>
     <t>[sku]</t>
   </si>
@@ -485,9 +485,6 @@
     <t>[energyDrain]</t>
   </si>
   <si>
-    <t>[energyBase]</t>
-  </si>
-  <si>
     <t>[boostMultiplier]</t>
   </si>
   <si>
@@ -603,6 +600,12 @@
   </si>
   <si>
     <t>[forceMax]</t>
+  </si>
+  <si>
+    <t>[energyBaseMin]</t>
+  </si>
+  <si>
+    <t>[energyBaseMax]</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1448,6 +1451,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1466,9 +1478,6 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1478,53 +1487,20 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="97">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="98">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1574,6 +1550,30 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2255,6 +2255,30 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3444,66 +3468,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BJ26" totalsRowShown="0" headerRowDxfId="96" dataDxfId="94" headerRowBorderDxfId="95" tableBorderDxfId="93" totalsRowBorderDxfId="92">
-  <autoFilter ref="B15:BJ26"/>
-  <tableColumns count="61">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="91"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="90"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="89"/>
-    <tableColumn id="3" name="[order]" dataDxfId="88"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="87"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="86"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="85"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="84"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="83"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="82"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="81"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="80"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="79"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="78"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="77"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="76"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="75"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="74"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="73"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="72"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="71"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="70"/>
-    <tableColumn id="41" name="[energyBase]" dataDxfId="69"/>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="68"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="67"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="66"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="65"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="64"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="63"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="62"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="61"/>
-    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="60"/>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="59"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="58"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="57"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="56"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="55"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="54"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="53"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="52"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="51"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="50"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="49"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="48"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="47"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="46"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="45"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BK26" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+  <autoFilter ref="B15:BK26"/>
+  <tableColumns count="62">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="92"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="91"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="90"/>
+    <tableColumn id="3" name="[order]" dataDxfId="89"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="88"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="87"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="86"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="85"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="84"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="83"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="82"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="81"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="80"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="79"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="78"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="77"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="76"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="75"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="74"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="73"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="72"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="71"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="70"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="5">
+      <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="69"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="68"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="67"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="66"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="65"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="64"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="63"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="62"/>
+    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="61"/>
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="60"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="59"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="58"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="57"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="56"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="55"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="54"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="53"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="52"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="51"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="50"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="49"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="48"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="47"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="46"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="45">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="43">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="44">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="42"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="41"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="40"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="0">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="43"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="42"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="41"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="40">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" name="[mass]" dataDxfId="39"/>
@@ -3864,10 +3891,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BJ55"/>
+  <dimension ref="B1:BK55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP10" workbookViewId="0">
-      <selection activeCell="BB17" sqref="BB17"/>
+    <sheetView tabSelected="1" topLeftCell="R10" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27:AA27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3895,10 +3922,10 @@
     <col min="61" max="61" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:63" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3925,7 +3952,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3933,9 +3960,9 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:62" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:63" ht="117" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -3947,13 +3974,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -3964,7 +3991,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F5" s="13">
         <v>1</v>
@@ -3974,7 +4001,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -3985,7 +4012,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F6" s="13">
         <v>2</v>
@@ -3995,7 +4022,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4006,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F7" s="16">
         <v>3</v>
@@ -4016,7 +4043,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4027,7 +4054,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F8" s="13">
         <v>4</v>
@@ -4037,7 +4064,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4048,7 +4075,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="13">
         <v>4</v>
@@ -4058,10 +4085,10 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:63" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -4088,31 +4115,31 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:62" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:63" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="W14"/>
       <c r="AA14" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="AO14" s="115"/>
-      <c r="AP14" s="115"/>
-      <c r="AQ14" s="115"/>
-      <c r="AR14" s="115"/>
+        <v>172</v>
+      </c>
+      <c r="AO14" s="118"/>
+      <c r="AP14" s="118"/>
+      <c r="AQ14" s="118"/>
+      <c r="AR14" s="118"/>
     </row>
-    <row r="15" spans="2:62" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:63" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="76" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C15" s="79" t="s">
         <v>0</v>
@@ -4124,178 +4151,181 @@
         <v>15</v>
       </c>
       <c r="F15" s="77" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G15" s="94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H15" s="93" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I15" s="92" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J15" s="91" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K15" s="90" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L15" s="88" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M15" s="86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N15" s="90" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O15" s="88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P15" s="88" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q15" s="87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R15" s="87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S15" s="87" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="T15" s="86" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U15" s="88" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="V15" s="89" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="W15" s="86" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X15" s="90" t="s">
-        <v>153</v>
+        <v>192</v>
       </c>
       <c r="Y15" s="90" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z15" s="90" t="s">
         <v>152</v>
       </c>
-      <c r="Z15" s="88" t="s">
+      <c r="AA15" s="88" t="s">
         <v>151</v>
       </c>
-      <c r="AA15" s="89" t="s">
+      <c r="AB15" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="AB15" s="88" t="s">
+      <c r="AC15" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="AC15" s="88" t="s">
+      <c r="AD15" s="88" t="s">
         <v>148</v>
       </c>
-      <c r="AD15" s="88" t="s">
+      <c r="AE15" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="AE15" s="88" t="s">
+      <c r="AF15" s="128" t="s">
         <v>146</v>
       </c>
-      <c r="AF15" s="87" t="s">
+      <c r="AG15" s="87" t="s">
         <v>145</v>
       </c>
-      <c r="AG15" s="86" t="s">
+      <c r="AH15" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="AH15" s="86" t="s">
+      <c r="AI15" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="AI15" s="86" t="s">
+      <c r="AJ15" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="AJ15" s="85" t="s">
+      <c r="AK15" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="AK15" s="83" t="s">
+      <c r="AL15" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="AL15" s="83" t="s">
+      <c r="AM15" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="AM15" s="83" t="s">
+      <c r="AN15" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="AN15" s="83" t="s">
+      <c r="AO15" s="83" t="s">
         <v>139</v>
       </c>
-      <c r="AO15" s="83" t="s">
+      <c r="AP15" s="83" t="s">
         <v>138</v>
       </c>
-      <c r="AP15" s="84" t="s">
+      <c r="AQ15" s="84" t="s">
         <v>137</v>
       </c>
-      <c r="AQ15" s="83" t="s">
+      <c r="AR15" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="AR15" s="83" t="s">
+      <c r="AS15" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="AS15" s="83" t="s">
+      <c r="AT15" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="AT15" s="83" t="s">
+      <c r="AU15" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="AU15" s="83" t="s">
+      <c r="AV15" s="83" t="s">
         <v>132</v>
       </c>
-      <c r="AV15" s="83" t="s">
+      <c r="AW15" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="AW15" s="3" t="s">
+      <c r="AX15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AX15" s="82" t="s">
+      <c r="AY15" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="AY15" s="81" t="s">
+      <c r="AZ15" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="AZ15" s="77" t="s">
+      <c r="BA15" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="BA15" s="80" t="s">
+      <c r="BB15" s="80" t="s">
+        <v>190</v>
+      </c>
+      <c r="BC15" s="76" t="s">
         <v>191</v>
       </c>
-      <c r="BB15" s="76" t="s">
-        <v>192</v>
-      </c>
-      <c r="BC15" s="79" t="s">
+      <c r="BD15" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="BD15" s="79" t="s">
+      <c r="BE15" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="BE15" s="79" t="s">
+      <c r="BF15" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="BF15" s="76" t="s">
+      <c r="BG15" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="BG15" s="76" t="s">
+      <c r="BH15" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="BH15" s="78" t="s">
+      <c r="BI15" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="BI15" s="77" t="s">
+      <c r="BJ15" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="BJ15" s="76" t="s">
+      <c r="BK15" s="76" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4364,60 +4394,61 @@
         <v>100</v>
       </c>
       <c r="Y16" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z16" s="29">
         <v>40</v>
       </c>
-      <c r="Z16" s="29">
+      <c r="AA16" s="29">
         <v>28</v>
       </c>
-      <c r="AA16" s="69">
+      <c r="AB16" s="69">
         <v>250</v>
       </c>
-      <c r="AB16" s="51">
+      <c r="AC16" s="51">
         <v>7.5</v>
       </c>
-      <c r="AC16" s="29">
+      <c r="AD16" s="29">
         <v>2</v>
       </c>
-      <c r="AD16" s="51">
+      <c r="AE16" s="51">
         <v>8</v>
       </c>
-      <c r="AE16" s="29">
+      <c r="AF16" s="29">
         <v>3000</v>
       </c>
-      <c r="AF16" s="68">
+      <c r="AG16" s="68">
         <v>1</v>
       </c>
-      <c r="AG16" s="65">
+      <c r="AH16" s="65">
         <v>0.23</v>
       </c>
-      <c r="AH16" s="75">
+      <c r="AI16" s="75">
         <v>0</v>
       </c>
-      <c r="AI16" s="75">
+      <c r="AJ16" s="75">
         <v>6</v>
       </c>
-      <c r="AJ16" s="24" t="s">
+      <c r="AK16" s="24" t="s">
         <v>120</v>
-      </c>
-      <c r="AK16" s="24" t="s">
-        <v>119</v>
       </c>
       <c r="AL16" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="AM16" s="24"/>
+      <c r="AM16" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="AN16" s="24"/>
-      <c r="AO16" s="24">
+      <c r="AO16" s="24"/>
+      <c r="AP16" s="24">
         <v>4.0999999999999996</v>
-      </c>
-      <c r="AP16" s="24">
-        <v>2</v>
       </c>
       <c r="AQ16" s="24">
         <v>2</v>
       </c>
-      <c r="AR16" s="24" t="b">
-        <v>1</v>
+      <c r="AR16" s="24">
+        <v>2</v>
       </c>
       <c r="AS16" s="24" t="b">
         <v>1</v>
@@ -4425,57 +4456,60 @@
       <c r="AT16" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU16" s="24">
+      <c r="AU16" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV16" s="24">
         <v>23</v>
       </c>
-      <c r="AV16" s="24">
+      <c r="AW16" s="24">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AW16" s="73" t="s">
+      <c r="AX16" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="AX16" s="72" t="s">
+      <c r="AY16" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="AY16" s="42">
+      <c r="AZ16" s="42">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AZ16" s="41">
+      <c r="BA16" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA16" s="40">
+      <c r="BB16" s="40">
         <v>175</v>
       </c>
-      <c r="BB16" s="127">
+      <c r="BC16" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>225</v>
       </c>
-      <c r="BC16" s="59">
+      <c r="BD16" s="59">
         <v>2</v>
       </c>
-      <c r="BD16" s="59">
+      <c r="BE16" s="59">
         <v>9.5</v>
       </c>
-      <c r="BE16" s="59">
+      <c r="BF16" s="59">
         <v>1</v>
       </c>
-      <c r="BF16" s="74">
+      <c r="BG16" s="74">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BG16" s="74">
+      <c r="BH16" s="74">
         <v>1.75</v>
       </c>
-      <c r="BH16" s="74">
+      <c r="BI16" s="74">
         <v>0</v>
       </c>
-      <c r="BI16" s="74">
+      <c r="BJ16" s="74">
         <v>6</v>
       </c>
-      <c r="BJ16" s="59" t="s">
+      <c r="BK16" s="59" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -4546,60 +4580,61 @@
         <v>100</v>
       </c>
       <c r="Y17" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z17" s="29">
         <v>20</v>
       </c>
-      <c r="Z17" s="29">
+      <c r="AA17" s="29">
         <v>10</v>
       </c>
-      <c r="AA17" s="69">
+      <c r="AB17" s="69">
         <v>275</v>
       </c>
-      <c r="AB17" s="51">
+      <c r="AC17" s="51">
         <v>8</v>
       </c>
-      <c r="AC17" s="29">
+      <c r="AD17" s="29">
         <v>3</v>
       </c>
-      <c r="AD17" s="51">
+      <c r="AE17" s="51">
         <v>9</v>
       </c>
-      <c r="AE17" s="29">
+      <c r="AF17" s="29">
         <v>7000</v>
       </c>
-      <c r="AF17" s="68">
+      <c r="AG17" s="68">
         <v>2</v>
       </c>
-      <c r="AG17" s="65">
+      <c r="AH17" s="65">
         <v>0.19</v>
       </c>
-      <c r="AH17" s="46">
+      <c r="AI17" s="46">
         <v>0</v>
       </c>
-      <c r="AI17" s="46">
+      <c r="AJ17" s="46">
         <v>6</v>
       </c>
-      <c r="AJ17" s="45" t="s">
+      <c r="AK17" s="45" t="s">
         <v>116</v>
-      </c>
-      <c r="AK17" s="24" t="s">
-        <v>115</v>
       </c>
       <c r="AL17" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="AM17" s="24"/>
+      <c r="AM17" s="24" t="s">
+        <v>115</v>
+      </c>
       <c r="AN17" s="24"/>
-      <c r="AO17" s="24">
+      <c r="AO17" s="24"/>
+      <c r="AP17" s="24">
         <v>2.2999999999999998</v>
-      </c>
-      <c r="AP17" s="24">
-        <v>2</v>
       </c>
       <c r="AQ17" s="24">
         <v>2</v>
       </c>
-      <c r="AR17" s="24" t="b">
-        <v>1</v>
+      <c r="AR17" s="24">
+        <v>2</v>
       </c>
       <c r="AS17" s="24" t="b">
         <v>1</v>
@@ -4607,57 +4642,60 @@
       <c r="AT17" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU17" s="24">
+      <c r="AU17" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV17" s="24">
         <v>23</v>
       </c>
-      <c r="AV17" s="24">
+      <c r="AW17" s="24">
         <v>0.7</v>
       </c>
-      <c r="AW17" s="73" t="s">
+      <c r="AX17" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="AX17" s="72" t="s">
+      <c r="AY17" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="AY17" s="42">
+      <c r="AZ17" s="42">
         <v>2.3E-3</v>
       </c>
-      <c r="AZ17" s="41">
+      <c r="BA17" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA17" s="40">
+      <c r="BB17" s="40">
         <v>210</v>
       </c>
-      <c r="BB17" s="127">
+      <c r="BC17" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>260</v>
       </c>
-      <c r="BC17" s="59">
+      <c r="BD17" s="59">
         <v>2.1</v>
       </c>
-      <c r="BD17" s="59">
+      <c r="BE17" s="59">
         <v>9.5</v>
       </c>
-      <c r="BE17" s="59">
+      <c r="BF17" s="59">
         <v>1.7</v>
       </c>
-      <c r="BF17" s="59">
+      <c r="BG17" s="59">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BG17" s="59">
+      <c r="BH17" s="59">
         <v>2.1</v>
       </c>
-      <c r="BH17" s="59">
+      <c r="BI17" s="59">
         <v>0</v>
       </c>
-      <c r="BI17" s="59">
+      <c r="BJ17" s="59">
         <v>6</v>
       </c>
-      <c r="BJ17" s="59" t="s">
+      <c r="BK17" s="59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -4728,60 +4766,61 @@
         <v>100</v>
       </c>
       <c r="Y18" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z18" s="29">
         <v>40</v>
       </c>
-      <c r="Z18" s="29">
+      <c r="AA18" s="29">
         <v>14</v>
       </c>
-      <c r="AA18" s="50">
+      <c r="AB18" s="50">
         <v>300</v>
       </c>
-      <c r="AB18" s="51">
+      <c r="AC18" s="51">
         <v>9</v>
       </c>
-      <c r="AC18" s="26">
+      <c r="AD18" s="26">
         <v>3</v>
       </c>
-      <c r="AD18" s="64">
+      <c r="AE18" s="64">
         <v>9</v>
       </c>
-      <c r="AE18" s="29">
+      <c r="AF18" s="29">
         <v>8000</v>
       </c>
-      <c r="AF18" s="63">
+      <c r="AG18" s="63">
         <v>2</v>
       </c>
-      <c r="AG18" s="47">
+      <c r="AH18" s="47">
         <v>0.15</v>
       </c>
-      <c r="AH18" s="62">
+      <c r="AI18" s="62">
         <v>0</v>
       </c>
-      <c r="AI18" s="62">
+      <c r="AJ18" s="62">
         <v>6</v>
       </c>
-      <c r="AJ18" s="45" t="s">
+      <c r="AK18" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="AK18" s="24" t="s">
+      <c r="AL18" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="AL18" s="24" t="s">
+      <c r="AM18" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AM18" s="24"/>
       <c r="AN18" s="24"/>
-      <c r="AO18" s="24">
+      <c r="AO18" s="24"/>
+      <c r="AP18" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AP18" s="24">
-        <v>2</v>
       </c>
       <c r="AQ18" s="24">
         <v>2</v>
       </c>
-      <c r="AR18" s="24" t="b">
-        <v>1</v>
+      <c r="AR18" s="24">
+        <v>2</v>
       </c>
       <c r="AS18" s="24" t="b">
         <v>1</v>
@@ -4789,57 +4828,60 @@
       <c r="AT18" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU18" s="24">
+      <c r="AU18" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV18" s="24">
         <v>23</v>
       </c>
-      <c r="AV18" s="24">
+      <c r="AW18" s="24">
         <v>0.7</v>
       </c>
-      <c r="AW18" s="61" t="s">
+      <c r="AX18" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="AX18" s="60" t="s">
+      <c r="AY18" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="AY18" s="42">
+      <c r="AZ18" s="42">
         <v>2E-3</v>
       </c>
-      <c r="AZ18" s="41">
+      <c r="BA18" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA18" s="40">
+      <c r="BB18" s="40">
         <v>240</v>
       </c>
-      <c r="BB18" s="127">
+      <c r="BC18" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>290</v>
       </c>
-      <c r="BC18" s="59">
+      <c r="BD18" s="59">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BD18" s="59">
+      <c r="BE18" s="59">
         <v>9.5</v>
       </c>
-      <c r="BE18" s="59">
+      <c r="BF18" s="59">
         <v>1.7</v>
       </c>
-      <c r="BF18" s="59">
+      <c r="BG18" s="59">
         <v>0.9</v>
       </c>
-      <c r="BG18" s="59">
+      <c r="BH18" s="59">
         <v>2.25</v>
       </c>
-      <c r="BH18" s="59">
+      <c r="BI18" s="59">
         <v>0</v>
       </c>
-      <c r="BI18" s="59">
+      <c r="BJ18" s="59">
         <v>6</v>
       </c>
-      <c r="BJ18" s="38" t="s">
+      <c r="BK18" s="38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -4910,60 +4952,61 @@
         <v>100</v>
       </c>
       <c r="Y19" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z19" s="29">
         <v>18</v>
       </c>
-      <c r="Z19" s="26">
+      <c r="AA19" s="26">
         <v>22</v>
       </c>
-      <c r="AA19" s="69">
+      <c r="AB19" s="69">
         <v>325</v>
       </c>
-      <c r="AB19" s="51">
+      <c r="AC19" s="51">
         <v>10</v>
       </c>
-      <c r="AC19" s="29">
+      <c r="AD19" s="29">
         <v>3</v>
       </c>
-      <c r="AD19" s="51">
+      <c r="AE19" s="51">
         <v>9</v>
       </c>
-      <c r="AE19" s="29">
+      <c r="AF19" s="29">
         <v>9000</v>
       </c>
-      <c r="AF19" s="68">
+      <c r="AG19" s="68">
         <v>2</v>
       </c>
-      <c r="AG19" s="65">
+      <c r="AH19" s="65">
         <v>0.13</v>
       </c>
-      <c r="AH19" s="46">
+      <c r="AI19" s="46">
         <v>0</v>
       </c>
-      <c r="AI19" s="46">
+      <c r="AJ19" s="46">
         <v>6</v>
       </c>
-      <c r="AJ19" s="45" t="s">
+      <c r="AK19" s="45" t="s">
         <v>106</v>
-      </c>
-      <c r="AK19" s="24" t="s">
-        <v>105</v>
       </c>
       <c r="AL19" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="AM19" s="24"/>
+      <c r="AM19" s="24" t="s">
+        <v>105</v>
+      </c>
       <c r="AN19" s="24"/>
-      <c r="AO19" s="24">
+      <c r="AO19" s="24"/>
+      <c r="AP19" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AP19" s="24">
-        <v>2</v>
       </c>
       <c r="AQ19" s="24">
         <v>2</v>
       </c>
-      <c r="AR19" s="24" t="b">
-        <v>1</v>
+      <c r="AR19" s="24">
+        <v>2</v>
       </c>
       <c r="AS19" s="24" t="b">
         <v>1</v>
@@ -4971,57 +5014,60 @@
       <c r="AT19" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU19" s="24">
+      <c r="AU19" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV19" s="24">
         <v>23</v>
       </c>
-      <c r="AV19" s="24">
+      <c r="AW19" s="24">
         <v>0.7</v>
       </c>
-      <c r="AW19" s="61" t="s">
+      <c r="AX19" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="AX19" s="60" t="s">
+      <c r="AY19" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="AY19" s="42">
+      <c r="AZ19" s="42">
         <v>2E-3</v>
       </c>
-      <c r="AZ19" s="41">
+      <c r="BA19" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA19" s="40">
+      <c r="BB19" s="40">
         <v>360</v>
       </c>
-      <c r="BB19" s="127">
+      <c r="BC19" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>410</v>
       </c>
-      <c r="BC19" s="59">
+      <c r="BD19" s="59">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BD19" s="59">
+      <c r="BE19" s="59">
         <v>5</v>
       </c>
-      <c r="BE19" s="59">
+      <c r="BF19" s="59">
         <v>0.5</v>
       </c>
-      <c r="BF19" s="59">
+      <c r="BG19" s="59">
         <v>1</v>
       </c>
-      <c r="BG19" s="59">
+      <c r="BH19" s="59">
         <v>1.3</v>
       </c>
-      <c r="BH19" s="59">
+      <c r="BI19" s="59">
         <v>0</v>
       </c>
-      <c r="BI19" s="59">
+      <c r="BJ19" s="59">
         <v>6</v>
       </c>
-      <c r="BJ19" s="38" t="s">
+      <c r="BK19" s="38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5092,60 +5138,61 @@
         <v>100</v>
       </c>
       <c r="Y20" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z20" s="29">
         <v>31</v>
       </c>
-      <c r="Z20" s="29">
+      <c r="AA20" s="29">
         <v>34</v>
       </c>
-      <c r="AA20" s="69">
+      <c r="AB20" s="69">
         <v>350</v>
       </c>
-      <c r="AB20" s="51">
+      <c r="AC20" s="51">
         <v>11</v>
       </c>
-      <c r="AC20" s="29">
+      <c r="AD20" s="29">
         <v>4</v>
       </c>
-      <c r="AD20" s="51">
+      <c r="AE20" s="51">
         <v>10</v>
       </c>
-      <c r="AE20" s="29">
+      <c r="AF20" s="29">
         <v>10000</v>
       </c>
-      <c r="AF20" s="68">
+      <c r="AG20" s="68">
         <v>3</v>
       </c>
-      <c r="AG20" s="65">
+      <c r="AH20" s="65">
         <v>0.11</v>
       </c>
-      <c r="AH20" s="46">
+      <c r="AI20" s="46">
         <v>0</v>
       </c>
-      <c r="AI20" s="46">
+      <c r="AJ20" s="46">
         <v>12</v>
       </c>
-      <c r="AJ20" s="45" t="s">
+      <c r="AK20" s="45" t="s">
         <v>102</v>
-      </c>
-      <c r="AK20" s="24" t="s">
-        <v>101</v>
       </c>
       <c r="AL20" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="AM20" s="24"/>
+      <c r="AM20" s="24" t="s">
+        <v>101</v>
+      </c>
       <c r="AN20" s="24"/>
-      <c r="AO20" s="24">
+      <c r="AO20" s="24"/>
+      <c r="AP20" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AP20" s="24">
-        <v>2</v>
       </c>
       <c r="AQ20" s="24">
         <v>2</v>
       </c>
-      <c r="AR20" s="24" t="b">
-        <v>1</v>
+      <c r="AR20" s="24">
+        <v>2</v>
       </c>
       <c r="AS20" s="24" t="b">
         <v>1</v>
@@ -5153,57 +5200,60 @@
       <c r="AT20" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU20" s="24">
+      <c r="AU20" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV20" s="24">
         <v>23</v>
       </c>
-      <c r="AV20" s="24">
+      <c r="AW20" s="24">
         <v>0.7</v>
       </c>
-      <c r="AW20" s="61" t="s">
+      <c r="AX20" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="AX20" s="60" t="s">
+      <c r="AY20" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="AY20" s="42">
+      <c r="AZ20" s="42">
         <v>1.9E-3</v>
       </c>
-      <c r="AZ20" s="41">
+      <c r="BA20" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA20" s="40">
+      <c r="BB20" s="40">
         <v>300</v>
       </c>
-      <c r="BB20" s="127">
+      <c r="BC20" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>350</v>
       </c>
-      <c r="BC20" s="59">
+      <c r="BD20" s="59">
         <v>2.4</v>
       </c>
-      <c r="BD20" s="59">
+      <c r="BE20" s="59">
         <v>9.5</v>
       </c>
-      <c r="BE20" s="59">
+      <c r="BF20" s="59">
         <v>1.7</v>
       </c>
-      <c r="BF20" s="59">
+      <c r="BG20" s="59">
         <v>1</v>
       </c>
-      <c r="BG20" s="59">
+      <c r="BH20" s="59">
         <v>1.6</v>
       </c>
-      <c r="BH20" s="59">
+      <c r="BI20" s="59">
         <v>9</v>
       </c>
-      <c r="BI20" s="59">
+      <c r="BJ20" s="59">
         <v>6</v>
       </c>
-      <c r="BJ20" s="38" t="s">
+      <c r="BK20" s="38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5274,60 +5324,61 @@
         <v>100</v>
       </c>
       <c r="Y21" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z21" s="29">
         <v>50</v>
       </c>
-      <c r="Z21" s="29">
+      <c r="AA21" s="29">
         <v>14</v>
       </c>
-      <c r="AA21" s="69">
+      <c r="AB21" s="69">
         <v>375</v>
       </c>
-      <c r="AB21" s="51">
+      <c r="AC21" s="51">
         <v>11</v>
       </c>
-      <c r="AC21" s="29">
+      <c r="AD21" s="29">
         <v>4</v>
       </c>
-      <c r="AD21" s="51">
+      <c r="AE21" s="51">
         <v>10</v>
       </c>
-      <c r="AE21" s="29">
+      <c r="AF21" s="29">
         <v>10000</v>
       </c>
-      <c r="AF21" s="68">
+      <c r="AG21" s="68">
         <v>3</v>
       </c>
-      <c r="AG21" s="65">
+      <c r="AH21" s="65">
         <v>0.09</v>
       </c>
-      <c r="AH21" s="46">
+      <c r="AI21" s="46">
         <v>0</v>
       </c>
-      <c r="AI21" s="46">
+      <c r="AJ21" s="46">
         <v>12</v>
       </c>
-      <c r="AJ21" s="45" t="s">
+      <c r="AK21" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="AK21" s="24" t="s">
+      <c r="AL21" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AL21" s="24" t="s">
+      <c r="AM21" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AM21" s="24"/>
       <c r="AN21" s="24"/>
-      <c r="AO21" s="24">
-        <v>2</v>
-      </c>
+      <c r="AO21" s="24"/>
       <c r="AP21" s="24">
         <v>2</v>
       </c>
       <c r="AQ21" s="24">
         <v>2</v>
       </c>
-      <c r="AR21" s="24" t="b">
-        <v>1</v>
+      <c r="AR21" s="24">
+        <v>2</v>
       </c>
       <c r="AS21" s="24" t="b">
         <v>1</v>
@@ -5335,57 +5386,60 @@
       <c r="AT21" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU21" s="24">
+      <c r="AU21" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV21" s="24">
         <v>23</v>
       </c>
-      <c r="AV21" s="24">
+      <c r="AW21" s="24">
         <v>0.7</v>
       </c>
-      <c r="AW21" s="61" t="s">
+      <c r="AX21" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="AX21" s="60" t="s">
+      <c r="AY21" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="AY21" s="42">
+      <c r="AZ21" s="42">
         <v>1.8E-3</v>
       </c>
-      <c r="AZ21" s="41">
+      <c r="BA21" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA21" s="40">
+      <c r="BB21" s="40">
         <v>322</v>
       </c>
-      <c r="BB21" s="127">
+      <c r="BC21" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>372</v>
       </c>
-      <c r="BC21" s="59">
+      <c r="BD21" s="59">
         <v>2.5</v>
       </c>
-      <c r="BD21" s="59">
+      <c r="BE21" s="59">
         <v>9.5</v>
       </c>
-      <c r="BE21" s="59">
+      <c r="BF21" s="59">
         <v>1.7</v>
       </c>
-      <c r="BF21" s="59">
+      <c r="BG21" s="59">
         <v>0.5</v>
       </c>
-      <c r="BG21" s="59">
+      <c r="BH21" s="59">
         <v>1.9</v>
       </c>
-      <c r="BH21" s="59">
+      <c r="BI21" s="59">
         <v>9</v>
       </c>
-      <c r="BI21" s="59">
+      <c r="BJ21" s="59">
         <v>6</v>
       </c>
-      <c r="BJ21" s="38" t="s">
+      <c r="BK21" s="38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -5456,60 +5510,61 @@
         <v>100</v>
       </c>
       <c r="Y22" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z22" s="29">
         <v>29</v>
       </c>
-      <c r="Z22" s="29">
+      <c r="AA22" s="29">
         <v>17</v>
       </c>
-      <c r="AA22" s="69">
+      <c r="AB22" s="69">
         <v>400</v>
       </c>
-      <c r="AB22" s="51">
+      <c r="AC22" s="51">
         <v>11</v>
       </c>
-      <c r="AC22" s="29">
+      <c r="AD22" s="29">
         <v>4</v>
       </c>
-      <c r="AD22" s="51">
+      <c r="AE22" s="51">
         <v>10</v>
       </c>
-      <c r="AE22" s="29">
+      <c r="AF22" s="29">
         <v>10000</v>
       </c>
-      <c r="AF22" s="68">
+      <c r="AG22" s="68">
         <v>3</v>
       </c>
-      <c r="AG22" s="65">
+      <c r="AH22" s="65">
         <v>0.08</v>
       </c>
-      <c r="AH22" s="46">
+      <c r="AI22" s="46">
         <v>0</v>
       </c>
-      <c r="AI22" s="46">
+      <c r="AJ22" s="46">
         <v>12</v>
       </c>
-      <c r="AJ22" s="45" t="s">
+      <c r="AK22" s="45" t="s">
         <v>92</v>
-      </c>
-      <c r="AK22" s="24" t="s">
-        <v>91</v>
       </c>
       <c r="AL22" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="AM22" s="24"/>
+      <c r="AM22" s="24" t="s">
+        <v>91</v>
+      </c>
       <c r="AN22" s="24"/>
-      <c r="AO22" s="24">
+      <c r="AO22" s="24"/>
+      <c r="AP22" s="24">
         <v>1.6</v>
-      </c>
-      <c r="AP22" s="24">
-        <v>2</v>
       </c>
       <c r="AQ22" s="24">
         <v>2</v>
       </c>
-      <c r="AR22" s="24" t="b">
-        <v>1</v>
+      <c r="AR22" s="24">
+        <v>2</v>
       </c>
       <c r="AS22" s="24" t="b">
         <v>1</v>
@@ -5517,57 +5572,60 @@
       <c r="AT22" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU22" s="24">
+      <c r="AU22" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV22" s="24">
         <v>23</v>
       </c>
-      <c r="AV22" s="24">
+      <c r="AW22" s="24">
         <v>0.7</v>
       </c>
-      <c r="AW22" s="61" t="s">
+      <c r="AX22" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="AX22" s="60" t="s">
+      <c r="AY22" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="AY22" s="42">
+      <c r="AZ22" s="42">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="AZ22" s="41">
+      <c r="BA22" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA22" s="40">
+      <c r="BB22" s="40">
         <v>343</v>
       </c>
-      <c r="BB22" s="127">
+      <c r="BC22" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>393</v>
       </c>
-      <c r="BC22" s="59">
+      <c r="BD22" s="59">
         <v>2.6</v>
       </c>
-      <c r="BD22" s="59">
+      <c r="BE22" s="59">
         <v>9.5</v>
       </c>
-      <c r="BE22" s="59">
+      <c r="BF22" s="59">
         <v>1.7</v>
       </c>
-      <c r="BF22" s="59">
+      <c r="BG22" s="59">
         <v>0.5</v>
       </c>
-      <c r="BG22" s="59">
+      <c r="BH22" s="59">
         <v>2</v>
       </c>
-      <c r="BH22" s="59">
+      <c r="BI22" s="59">
         <v>9</v>
       </c>
-      <c r="BI22" s="59">
+      <c r="BJ22" s="59">
         <v>6</v>
       </c>
-      <c r="BJ22" s="38" t="s">
+      <c r="BK22" s="38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -5638,64 +5696,65 @@
         <v>100</v>
       </c>
       <c r="Y23" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z23" s="29">
         <v>20</v>
       </c>
-      <c r="Z23" s="29">
+      <c r="AA23" s="29">
         <v>18</v>
       </c>
-      <c r="AA23" s="50">
+      <c r="AB23" s="50">
         <v>425</v>
       </c>
-      <c r="AB23" s="51">
+      <c r="AC23" s="51">
         <v>11.5</v>
       </c>
-      <c r="AC23" s="26">
+      <c r="AD23" s="26">
         <v>5</v>
       </c>
-      <c r="AD23" s="64">
+      <c r="AE23" s="64">
         <v>10</v>
       </c>
-      <c r="AE23" s="29">
+      <c r="AF23" s="29">
         <v>20000</v>
       </c>
-      <c r="AF23" s="63">
+      <c r="AG23" s="63">
         <v>4</v>
       </c>
-      <c r="AG23" s="47">
+      <c r="AH23" s="47">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AH23" s="62">
+      <c r="AI23" s="62">
         <v>0</v>
       </c>
-      <c r="AI23" s="62">
+      <c r="AJ23" s="62">
         <v>12</v>
       </c>
-      <c r="AJ23" s="45" t="s">
+      <c r="AK23" s="45" t="s">
         <v>88</v>
-      </c>
-      <c r="AK23" s="24" t="s">
-        <v>87</v>
       </c>
       <c r="AL23" s="24" t="s">
         <v>87</v>
       </c>
       <c r="AM23" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN23" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AN23" s="24" t="s">
+      <c r="AO23" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AO23" s="24">
+      <c r="AP23" s="24">
         <v>1.4</v>
-      </c>
-      <c r="AP23" s="24">
-        <v>2</v>
       </c>
       <c r="AQ23" s="24">
         <v>2</v>
       </c>
-      <c r="AR23" s="24" t="b">
-        <v>1</v>
+      <c r="AR23" s="24">
+        <v>2</v>
       </c>
       <c r="AS23" s="24" t="b">
         <v>1</v>
@@ -5703,62 +5762,65 @@
       <c r="AT23" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU23" s="24">
+      <c r="AU23" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV23" s="24">
         <v>23</v>
       </c>
-      <c r="AV23" s="24">
+      <c r="AW23" s="24">
         <v>0.7</v>
       </c>
-      <c r="AW23" s="61" t="s">
+      <c r="AX23" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="AX23" s="60" t="s">
+      <c r="AY23" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="AY23" s="42">
+      <c r="AZ23" s="42">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AZ23" s="41">
+      <c r="BA23" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA23" s="40">
+      <c r="BB23" s="40">
         <v>425</v>
       </c>
-      <c r="BB23" s="127">
+      <c r="BC23" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>475</v>
       </c>
-      <c r="BC23" s="59">
+      <c r="BD23" s="59">
         <v>3.2</v>
       </c>
-      <c r="BD23" s="59">
+      <c r="BE23" s="59">
         <v>9.5</v>
       </c>
-      <c r="BE23" s="59">
+      <c r="BF23" s="59">
         <v>1.7</v>
       </c>
-      <c r="BF23" s="59">
+      <c r="BG23" s="59">
         <v>0.5</v>
       </c>
-      <c r="BG23" s="59">
+      <c r="BH23" s="59">
         <v>1.2</v>
       </c>
-      <c r="BH23" s="59">
+      <c r="BI23" s="59">
         <v>45</v>
       </c>
-      <c r="BI23" s="59">
+      <c r="BJ23" s="59">
         <v>15</v>
       </c>
-      <c r="BJ23" s="38" t="s">
+      <c r="BK23" s="38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="101" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D24" s="101" t="s">
         <v>84</v>
@@ -5824,64 +5886,65 @@
         <v>100</v>
       </c>
       <c r="Y24" s="51">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z24" s="51">
         <v>40</v>
       </c>
-      <c r="Z24" s="51">
+      <c r="AA24" s="51">
         <v>14</v>
       </c>
-      <c r="AA24" s="50">
+      <c r="AB24" s="50">
         <v>425</v>
       </c>
-      <c r="AB24" s="51">
+      <c r="AC24" s="51">
         <v>11.5</v>
       </c>
-      <c r="AC24" s="49">
+      <c r="AD24" s="49">
         <v>5</v>
       </c>
-      <c r="AD24" s="64">
+      <c r="AE24" s="64">
         <v>10</v>
       </c>
-      <c r="AE24" s="51">
+      <c r="AF24" s="51">
         <v>20000</v>
       </c>
-      <c r="AF24" s="110">
+      <c r="AG24" s="110">
         <v>4</v>
       </c>
-      <c r="AG24" s="111">
+      <c r="AH24" s="111">
         <v>0.06</v>
       </c>
-      <c r="AH24" s="62">
+      <c r="AI24" s="62">
         <v>0</v>
       </c>
-      <c r="AI24" s="62">
+      <c r="AJ24" s="62">
         <v>12</v>
       </c>
-      <c r="AJ24" s="100" t="s">
+      <c r="AK24" s="100" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL24" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="AK24" s="99" t="s">
-        <v>188</v>
-      </c>
-      <c r="AL24" s="99" t="s">
-        <v>188</v>
-      </c>
       <c r="AM24" s="99" t="s">
+        <v>187</v>
+      </c>
+      <c r="AN24" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="AN24" s="99" t="s">
+      <c r="AO24" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="AO24" s="99">
+      <c r="AP24" s="99">
         <v>1.3</v>
-      </c>
-      <c r="AP24" s="99">
-        <v>2</v>
       </c>
       <c r="AQ24" s="99">
         <v>2</v>
       </c>
-      <c r="AR24" s="99" t="b">
-        <v>1</v>
+      <c r="AR24" s="99">
+        <v>2</v>
       </c>
       <c r="AS24" s="99" t="b">
         <v>1</v>
@@ -5889,57 +5952,60 @@
       <c r="AT24" s="99" t="b">
         <v>1</v>
       </c>
-      <c r="AU24" s="99">
+      <c r="AU24" s="99" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV24" s="99">
         <v>23</v>
       </c>
-      <c r="AV24" s="99">
+      <c r="AW24" s="99">
         <v>0.7</v>
       </c>
-      <c r="AW24" s="103" t="s">
+      <c r="AX24" s="103" t="s">
+        <v>188</v>
+      </c>
+      <c r="AY24" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="AX24" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="AY24" s="107">
+      <c r="AZ24" s="107">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AZ24" s="108">
+      <c r="BA24" s="108">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA24" s="109">
+      <c r="BB24" s="109">
         <v>440</v>
       </c>
-      <c r="BB24" s="128">
+      <c r="BC24" s="115">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>490</v>
       </c>
-      <c r="BC24" s="104">
+      <c r="BD24" s="104">
         <v>3.4</v>
       </c>
-      <c r="BD24" s="104">
+      <c r="BE24" s="104">
         <v>9.5</v>
       </c>
-      <c r="BE24" s="104">
+      <c r="BF24" s="104">
         <v>1.7</v>
       </c>
-      <c r="BF24" s="104">
+      <c r="BG24" s="104">
         <v>0.6</v>
       </c>
-      <c r="BG24" s="104">
+      <c r="BH24" s="104">
         <v>1.2</v>
       </c>
-      <c r="BH24" s="104">
+      <c r="BI24" s="104">
         <v>45</v>
       </c>
-      <c r="BI24" s="104">
+      <c r="BJ24" s="104">
         <v>15</v>
       </c>
-      <c r="BJ24" s="101" t="s">
-        <v>186</v>
+      <c r="BK24" s="101" t="s">
+        <v>185</v>
       </c>
     </row>
-    <row r="25" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -5953,7 +6019,7 @@
         <v>9</v>
       </c>
       <c r="F25" s="57" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G25" s="30">
         <v>2900000</v>
@@ -6010,64 +6076,65 @@
         <v>100</v>
       </c>
       <c r="Y25" s="29">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z25" s="29">
         <v>50</v>
       </c>
-      <c r="Z25" s="26">
+      <c r="AA25" s="26">
         <v>34</v>
       </c>
-      <c r="AA25" s="50">
+      <c r="AB25" s="50">
         <v>450</v>
       </c>
-      <c r="AB25" s="51">
+      <c r="AC25" s="51">
         <v>11.5</v>
       </c>
-      <c r="AC25" s="26">
+      <c r="AD25" s="26">
         <v>5</v>
       </c>
-      <c r="AD25" s="64">
+      <c r="AE25" s="64">
         <v>10</v>
       </c>
-      <c r="AE25" s="29">
+      <c r="AF25" s="29">
         <v>20000</v>
       </c>
-      <c r="AF25" s="63">
+      <c r="AG25" s="63">
         <v>4</v>
       </c>
-      <c r="AG25" s="47">
+      <c r="AH25" s="47">
         <v>0.06</v>
       </c>
-      <c r="AH25" s="62">
+      <c r="AI25" s="62">
         <v>0</v>
       </c>
-      <c r="AI25" s="62">
+      <c r="AJ25" s="62">
         <v>12</v>
       </c>
-      <c r="AJ25" s="45" t="s">
+      <c r="AK25" s="45" t="s">
         <v>83</v>
-      </c>
-      <c r="AK25" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="AL25" s="24" t="s">
         <v>82</v>
       </c>
       <c r="AM25" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN25" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AN25" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO25" s="24">
+      <c r="AO25" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="AP25" s="24">
         <v>1.2</v>
-      </c>
-      <c r="AP25" s="24">
-        <v>2</v>
       </c>
       <c r="AQ25" s="24">
         <v>2</v>
       </c>
-      <c r="AR25" s="24" t="b">
-        <v>1</v>
+      <c r="AR25" s="24">
+        <v>2</v>
       </c>
       <c r="AS25" s="24" t="b">
         <v>1</v>
@@ -6075,57 +6142,60 @@
       <c r="AT25" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU25" s="24">
+      <c r="AU25" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV25" s="24">
         <v>23</v>
       </c>
-      <c r="AV25" s="24">
+      <c r="AW25" s="24">
         <v>0.7</v>
       </c>
-      <c r="AW25" s="61" t="s">
+      <c r="AX25" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="AX25" s="60" t="s">
+      <c r="AY25" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="AY25" s="42">
+      <c r="AZ25" s="42">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AZ25" s="41">
+      <c r="BA25" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA25" s="40">
+      <c r="BB25" s="40">
         <v>540</v>
       </c>
-      <c r="BB25" s="127">
+      <c r="BC25" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>590</v>
       </c>
-      <c r="BC25" s="59">
+      <c r="BD25" s="59">
         <v>3.9</v>
       </c>
-      <c r="BD25" s="59">
+      <c r="BE25" s="59">
         <v>9.5</v>
       </c>
-      <c r="BE25" s="59">
+      <c r="BF25" s="59">
         <v>1.7</v>
       </c>
-      <c r="BF25" s="59">
+      <c r="BG25" s="59">
         <v>0.3</v>
       </c>
-      <c r="BG25" s="59">
+      <c r="BH25" s="59">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BH25" s="59">
+      <c r="BI25" s="59">
         <v>45</v>
       </c>
-      <c r="BI25" s="59">
+      <c r="BJ25" s="59">
         <v>15</v>
       </c>
-      <c r="BJ25" s="38" t="s">
+      <c r="BK25" s="38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6196,64 +6266,65 @@
         <v>100</v>
       </c>
       <c r="Y26" s="26">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z26" s="26">
         <v>33</v>
       </c>
-      <c r="Z26" s="26">
+      <c r="AA26" s="26">
         <v>34</v>
       </c>
-      <c r="AA26" s="50">
+      <c r="AB26" s="50">
         <v>475</v>
       </c>
-      <c r="AB26" s="49">
+      <c r="AC26" s="49">
         <v>12</v>
       </c>
-      <c r="AC26" s="26">
+      <c r="AD26" s="26">
         <v>6</v>
       </c>
-      <c r="AD26" s="49">
+      <c r="AE26" s="49">
         <v>10</v>
       </c>
-      <c r="AE26" s="26">
+      <c r="AF26" s="26">
         <v>30000</v>
       </c>
-      <c r="AF26" s="48">
+      <c r="AG26" s="48">
         <v>5</v>
       </c>
-      <c r="AG26" s="47">
+      <c r="AH26" s="47">
         <v>0.05</v>
       </c>
-      <c r="AH26" s="46">
+      <c r="AI26" s="46">
         <v>0</v>
       </c>
-      <c r="AI26" s="46">
+      <c r="AJ26" s="46">
         <v>12</v>
       </c>
-      <c r="AJ26" s="45" t="s">
+      <c r="AK26" s="45" t="s">
         <v>78</v>
-      </c>
-      <c r="AK26" s="24" t="s">
-        <v>77</v>
       </c>
       <c r="AL26" s="24" t="s">
         <v>77</v>
       </c>
       <c r="AM26" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN26" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AN26" s="24" t="s">
+      <c r="AO26" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AO26" s="24">
+      <c r="AP26" s="24">
         <v>1.1000000000000001</v>
-      </c>
-      <c r="AP26" s="24">
-        <v>2</v>
       </c>
       <c r="AQ26" s="24">
         <v>2</v>
       </c>
-      <c r="AR26" s="24" t="b">
-        <v>1</v>
+      <c r="AR26" s="24">
+        <v>2</v>
       </c>
       <c r="AS26" s="24" t="b">
         <v>1</v>
@@ -6261,57 +6332,60 @@
       <c r="AT26" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AU26" s="24">
+      <c r="AU26" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV26" s="24">
         <v>23</v>
       </c>
-      <c r="AV26" s="24">
+      <c r="AW26" s="24">
         <v>0.75</v>
       </c>
-      <c r="AW26" s="44" t="s">
+      <c r="AX26" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="AX26" s="43" t="s">
+      <c r="AY26" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="AY26" s="42">
+      <c r="AZ26" s="42">
         <v>1.5E-3</v>
       </c>
-      <c r="AZ26" s="41">
+      <c r="BA26" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA26" s="40">
+      <c r="BB26" s="40">
         <v>680</v>
       </c>
-      <c r="BB26" s="129">
+      <c r="BC26" s="116">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>730</v>
       </c>
-      <c r="BC26" s="39">
+      <c r="BD26" s="39">
         <v>4.7</v>
       </c>
-      <c r="BD26" s="39">
+      <c r="BE26" s="39">
         <v>9.5</v>
       </c>
-      <c r="BE26" s="39">
+      <c r="BF26" s="39">
         <v>1.7</v>
       </c>
-      <c r="BF26" s="39">
+      <c r="BG26" s="39">
         <v>0.2</v>
       </c>
-      <c r="BG26" s="39">
+      <c r="BH26" s="39">
         <v>0.15</v>
       </c>
-      <c r="BH26" s="39">
+      <c r="BI26" s="39">
         <v>59</v>
       </c>
-      <c r="BI26" s="39">
+      <c r="BJ26" s="39">
         <v>15</v>
       </c>
-      <c r="BJ26" s="38" t="s">
+      <c r="BK26" s="38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:62" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:63" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
@@ -6319,59 +6393,58 @@
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="116" t="s">
+      <c r="I27" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="117"/>
-      <c r="K27" s="117"/>
-      <c r="L27" s="118"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="121"/>
       <c r="M27" s="37"/>
-      <c r="N27" s="122" t="s">
+      <c r="N27" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="O27" s="122"/>
-      <c r="P27" s="122"/>
-      <c r="Q27" s="122"/>
-      <c r="R27" s="122"/>
-      <c r="S27" s="123"/>
-      <c r="T27" s="121" t="s">
+      <c r="O27" s="124"/>
+      <c r="P27" s="124"/>
+      <c r="Q27" s="124"/>
+      <c r="R27" s="124"/>
+      <c r="S27" s="125"/>
+      <c r="T27" s="123" t="s">
         <v>72</v>
       </c>
-      <c r="U27" s="121"/>
+      <c r="U27" s="123"/>
       <c r="V27" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="W27" s="119" t="s">
+      <c r="W27" s="122" t="s">
         <v>70</v>
       </c>
-      <c r="X27" s="119"/>
-      <c r="Y27" s="119"/>
-      <c r="Z27" s="120"/>
-      <c r="AA27" s="124" t="s">
+      <c r="X27" s="122"/>
+      <c r="Y27" s="122"/>
+      <c r="Z27" s="122"/>
+      <c r="AA27" s="122"/>
+      <c r="AB27" s="126" t="s">
         <v>69</v>
       </c>
-      <c r="AB27" s="125"/>
-      <c r="AC27" s="125"/>
-      <c r="AD27" s="125"/>
-      <c r="AE27" s="125"/>
-      <c r="AF27" s="126"/>
-      <c r="AG27" s="35" t="s">
+      <c r="AC27" s="126"/>
+      <c r="AD27" s="126"/>
+      <c r="AE27" s="126"/>
+      <c r="AF27" s="127"/>
+      <c r="AH27" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="AH27" s="34"/>
       <c r="AI27" s="34"/>
-      <c r="BA27" s="114" t="s">
+      <c r="BA27" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="BB27" s="114"/>
-      <c r="BC27" s="114"/>
-      <c r="BD27" s="114"/>
-      <c r="BE27" s="114"/>
-      <c r="BF27" s="114"/>
+      <c r="BB27" s="117"/>
+      <c r="BC27" s="117"/>
+      <c r="BD27" s="117"/>
+      <c r="BE27" s="117"/>
+      <c r="BF27" s="117"/>
       <c r="BH27"/>
     </row>
-    <row r="29" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:63" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -6385,7 +6458,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:62" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:63" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
@@ -6394,7 +6467,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:62" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:63" ht="140.25" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>64</v>
       </c>
@@ -7178,7 +7251,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D53">
         <v>20</v>
@@ -7382,25 +7455,25 @@
     <mergeCell ref="BA27:BF27"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="I27:L27"/>
-    <mergeCell ref="W27:Z27"/>
     <mergeCell ref="T27:U27"/>
     <mergeCell ref="N27:S27"/>
-    <mergeCell ref="AA27:AF27"/>
+    <mergeCell ref="W27:AA27"/>
+    <mergeCell ref="AB27:AF27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BJ16:BJ23 BJ25:BJ26">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  <conditionalFormatting sqref="BK16:BK23 BK25:BK26">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BJ24">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="BK24">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">

</xml_diff>

<commit_message>
Setting min/max values for airGravitymodifier, Size, baseEnergy and Force
Former-commit-id: cb6f041dbb55c6f30ac0c4670c0048aeb0226bad
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="195">
   <si>
     <t>[sku]</t>
   </si>
@@ -401,9 +401,6 @@
     <t>[waterGravityModifier]</t>
   </si>
   <si>
-    <t>[airGravityModifier]</t>
-  </si>
-  <si>
     <t>[gravityModifier]</t>
   </si>
   <si>
@@ -606,6 +603,12 @@
   </si>
   <si>
     <t>[energyBaseMax]</t>
+  </si>
+  <si>
+    <t>[airGravityModifierMin]</t>
+  </si>
+  <si>
+    <t>[airGravityModifierMax]</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1503,33 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="99">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3468,94 +3497,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BK26" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
-  <autoFilter ref="B15:BK26"/>
-  <tableColumns count="62">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="92"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="91"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="90"/>
-    <tableColumn id="3" name="[order]" dataDxfId="89"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="88"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="87"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="86"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="85"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="84"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="83"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="82"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="81"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="80"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="79"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="78"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="77"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="76"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="75"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="74"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="73"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="72"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="71"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="70"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BL26" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+  <autoFilter ref="B15:BL26"/>
+  <tableColumns count="63">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="93"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="92"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="91"/>
+    <tableColumn id="3" name="[order]" dataDxfId="90"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="89"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="88"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="87"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="86"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="85"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="84"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="83"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="82"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="81"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="80"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="79"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="78"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="77"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="76"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="75"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="74"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="73"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="72"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="71"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="6">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="69"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="68"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="67"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="66"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="65"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="64"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="63"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="62"/>
-    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="61"/>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="60"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="59"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="58"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="57"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="56"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="55"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="54"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="53"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="52"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="51"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="50"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="49"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="48"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="47"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="46"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="45">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="70"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="69"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="68"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="67"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="66"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="65"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="64"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="63"/>
+    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="62"/>
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="61"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="60"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="59"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="58"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="57"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="56"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="55"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="54"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="53"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="52"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="51"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="50"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="49"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="48"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="47"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="46">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="44">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="45">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="43"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="42"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="41"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="40">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="44"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="43"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="42"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="41">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="39"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="38"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="37"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="36"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="35"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="34"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="33"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="40"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="39"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="38"/>
+    <tableColumn id="43" name="[airGravityModifierMin]" dataDxfId="37"/>
+    <tableColumn id="63" name="[airGravityModifierMax]" dataDxfId="0">
+      <calculatedColumnFormula>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="36"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="35"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="34"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="28"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="24">
+    <tableColumn id="10" name="[icon]" dataDxfId="27"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="26"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="25">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3564,11 +3596,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="B32:I33"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="20"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="19"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3581,7 +3613,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B44:W55"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3612,14 +3644,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="B37:F40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="9"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="10"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="9"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="7"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="6"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="8"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3891,10 +3923,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BK55"/>
+  <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R10" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27:AA27"/>
+    <sheetView tabSelected="1" topLeftCell="AM10" workbookViewId="0">
+      <selection activeCell="BC25" sqref="BC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,10 +3954,10 @@
     <col min="61" max="61" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:63" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3952,7 +3984,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3960,9 +3992,9 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:63" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:64" ht="117" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -3974,13 +4006,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -3991,7 +4023,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F5" s="13">
         <v>1</v>
@@ -4001,7 +4033,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -4012,7 +4044,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F6" s="13">
         <v>2</v>
@@ -4022,7 +4054,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4033,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F7" s="16">
         <v>3</v>
@@ -4043,7 +4075,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4054,7 +4086,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F8" s="13">
         <v>4</v>
@@ -4064,7 +4096,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4075,7 +4107,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F9" s="13">
         <v>4</v>
@@ -4085,10 +4117,10 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:63" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -4115,31 +4147,31 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:63" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:64" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W14"/>
       <c r="AA14" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AO14" s="118"/>
       <c r="AP14" s="118"/>
       <c r="AQ14" s="118"/>
       <c r="AR14" s="118"/>
     </row>
-    <row r="15" spans="2:63" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:64" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="79" t="s">
         <v>0</v>
@@ -4151,97 +4183,97 @@
         <v>15</v>
       </c>
       <c r="F15" s="77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G15" s="94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H15" s="93" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I15" s="92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J15" s="91" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K15" s="90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L15" s="88" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M15" s="86" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N15" s="90" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O15" s="88" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P15" s="88" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q15" s="87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R15" s="87" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S15" s="87" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T15" s="86" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U15" s="88" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V15" s="89" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W15" s="86" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X15" s="90" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y15" s="90" t="s">
         <v>192</v>
       </c>
-      <c r="Y15" s="90" t="s">
-        <v>193</v>
-      </c>
       <c r="Z15" s="90" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AA15" s="88" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB15" s="89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AC15" s="88" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AD15" s="88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AE15" s="88" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AF15" s="128" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AG15" s="87" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AH15" s="86" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AI15" s="86" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AJ15" s="86" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AK15" s="85" t="s">
         <v>17</v>
@@ -4250,37 +4282,37 @@
         <v>18</v>
       </c>
       <c r="AM15" s="83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AN15" s="83" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AO15" s="83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AP15" s="83" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AQ15" s="84" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AR15" s="83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AS15" s="83" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AT15" s="83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AU15" s="83" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AV15" s="83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AW15" s="83" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AX15" s="3" t="s">
         <v>4</v>
@@ -4289,43 +4321,46 @@
         <v>16</v>
       </c>
       <c r="AZ15" s="81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="BA15" s="77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="BB15" s="80" t="s">
+        <v>189</v>
+      </c>
+      <c r="BC15" s="76" t="s">
         <v>190</v>
       </c>
-      <c r="BC15" s="76" t="s">
-        <v>191</v>
-      </c>
       <c r="BD15" s="79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="BE15" s="79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BF15" s="79" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG15" s="76" t="s">
-        <v>125</v>
+        <v>193</v>
       </c>
       <c r="BH15" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="BI15" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="BI15" s="78" t="s">
+      <c r="BJ15" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="BJ15" s="77" t="s">
+      <c r="BK15" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="BK15" s="76" t="s">
+      <c r="BL15" s="76" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4481,8 +4516,7 @@
         <v>175</v>
       </c>
       <c r="BC16" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="BD16" s="59">
         <v>2</v>
@@ -4497,19 +4531,23 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="BH16" s="74">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="BI16" s="74">
         <v>1.75</v>
       </c>
-      <c r="BI16" s="74">
+      <c r="BJ16" s="74">
         <v>0</v>
       </c>
-      <c r="BJ16" s="74">
+      <c r="BK16" s="74">
         <v>6</v>
       </c>
-      <c r="BK16" s="59" t="s">
+      <c r="BL16" s="59" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -4667,8 +4705,7 @@
         <v>210</v>
       </c>
       <c r="BC17" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="BD17" s="59">
         <v>2.1</v>
@@ -4683,19 +4720,23 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="BH17" s="59">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="BI17" s="59">
         <v>2.1</v>
       </c>
-      <c r="BI17" s="59">
+      <c r="BJ17" s="59">
         <v>0</v>
       </c>
-      <c r="BJ17" s="59">
+      <c r="BK17" s="59">
         <v>6</v>
       </c>
-      <c r="BK17" s="59" t="s">
+      <c r="BL17" s="59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -4853,8 +4894,7 @@
         <v>240</v>
       </c>
       <c r="BC18" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="BD18" s="59">
         <v>2.2000000000000002</v>
@@ -4869,19 +4909,23 @@
         <v>0.9</v>
       </c>
       <c r="BH18" s="59">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.75</v>
+      </c>
+      <c r="BI18" s="59">
         <v>2.25</v>
       </c>
-      <c r="BI18" s="59">
+      <c r="BJ18" s="59">
         <v>0</v>
       </c>
-      <c r="BJ18" s="59">
+      <c r="BK18" s="59">
         <v>6</v>
       </c>
-      <c r="BK18" s="38" t="s">
+      <c r="BL18" s="38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -5039,8 +5083,7 @@
         <v>360</v>
       </c>
       <c r="BC19" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>410</v>
+        <v>380</v>
       </c>
       <c r="BD19" s="59">
         <v>5.0999999999999996</v>
@@ -5055,19 +5098,23 @@
         <v>1</v>
       </c>
       <c r="BH19" s="59">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.85</v>
+      </c>
+      <c r="BI19" s="59">
         <v>1.3</v>
       </c>
-      <c r="BI19" s="59">
+      <c r="BJ19" s="59">
         <v>0</v>
       </c>
-      <c r="BJ19" s="59">
+      <c r="BK19" s="59">
         <v>6</v>
       </c>
-      <c r="BK19" s="38" t="s">
+      <c r="BL19" s="38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5225,8 +5272,7 @@
         <v>300</v>
       </c>
       <c r="BC20" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="BD20" s="59">
         <v>2.4</v>
@@ -5241,19 +5287,23 @@
         <v>1</v>
       </c>
       <c r="BH20" s="59">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.85</v>
+      </c>
+      <c r="BI20" s="59">
         <v>1.6</v>
       </c>
-      <c r="BI20" s="59">
+      <c r="BJ20" s="59">
         <v>9</v>
       </c>
-      <c r="BJ20" s="59">
+      <c r="BK20" s="59">
         <v>6</v>
       </c>
-      <c r="BK20" s="38" t="s">
+      <c r="BL20" s="38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5411,8 +5461,7 @@
         <v>322</v>
       </c>
       <c r="BC21" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>372</v>
+        <v>347</v>
       </c>
       <c r="BD21" s="59">
         <v>2.5</v>
@@ -5427,19 +5476,23 @@
         <v>0.5</v>
       </c>
       <c r="BH21" s="59">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.35</v>
+      </c>
+      <c r="BI21" s="59">
         <v>1.9</v>
       </c>
-      <c r="BI21" s="59">
+      <c r="BJ21" s="59">
         <v>9</v>
       </c>
-      <c r="BJ21" s="59">
+      <c r="BK21" s="59">
         <v>6</v>
       </c>
-      <c r="BK21" s="38" t="s">
+      <c r="BL21" s="38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -5597,8 +5650,7 @@
         <v>343</v>
       </c>
       <c r="BC22" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="BD22" s="59">
         <v>2.6</v>
@@ -5613,19 +5665,23 @@
         <v>0.5</v>
       </c>
       <c r="BH22" s="59">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.35</v>
+      </c>
+      <c r="BI22" s="59">
         <v>2</v>
       </c>
-      <c r="BI22" s="59">
+      <c r="BJ22" s="59">
         <v>9</v>
       </c>
-      <c r="BJ22" s="59">
+      <c r="BK22" s="59">
         <v>6</v>
       </c>
-      <c r="BK22" s="38" t="s">
+      <c r="BL22" s="38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -5787,8 +5843,7 @@
         <v>425</v>
       </c>
       <c r="BC23" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>475</v>
+        <v>455</v>
       </c>
       <c r="BD23" s="59">
         <v>3.2</v>
@@ -5803,24 +5858,28 @@
         <v>0.5</v>
       </c>
       <c r="BH23" s="59">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.35</v>
+      </c>
+      <c r="BI23" s="59">
         <v>1.2</v>
       </c>
-      <c r="BI23" s="59">
+      <c r="BJ23" s="59">
         <v>45</v>
       </c>
-      <c r="BJ23" s="59">
+      <c r="BK23" s="59">
         <v>15</v>
       </c>
-      <c r="BK23" s="38" t="s">
+      <c r="BL23" s="38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="101" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D24" s="101" t="s">
         <v>84</v>
@@ -5923,13 +5982,13 @@
         <v>12</v>
       </c>
       <c r="AK24" s="100" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL24" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="AL24" s="99" t="s">
-        <v>187</v>
-      </c>
       <c r="AM24" s="99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AN24" s="99" t="s">
         <v>5</v>
@@ -5962,10 +6021,10 @@
         <v>0.7</v>
       </c>
       <c r="AX24" s="103" t="s">
+        <v>187</v>
+      </c>
+      <c r="AY24" s="21" t="s">
         <v>188</v>
-      </c>
-      <c r="AY24" s="21" t="s">
-        <v>189</v>
       </c>
       <c r="AZ24" s="107">
         <v>1.6000000000000001E-3</v>
@@ -5977,8 +6036,7 @@
         <v>440</v>
       </c>
       <c r="BC24" s="115">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="BD24" s="104">
         <v>3.4</v>
@@ -5993,19 +6051,23 @@
         <v>0.6</v>
       </c>
       <c r="BH24" s="104">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="BI24" s="104">
         <v>1.2</v>
       </c>
-      <c r="BI24" s="104">
+      <c r="BJ24" s="104">
         <v>45</v>
       </c>
-      <c r="BJ24" s="104">
+      <c r="BK24" s="104">
         <v>15</v>
       </c>
-      <c r="BK24" s="101" t="s">
-        <v>185</v>
+      <c r="BL24" s="101" t="s">
+        <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:63" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -6019,7 +6081,7 @@
         <v>9</v>
       </c>
       <c r="F25" s="57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G25" s="30">
         <v>2900000</v>
@@ -6125,7 +6187,7 @@
         <v>5</v>
       </c>
       <c r="AO25" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AP25" s="24">
         <v>1.2</v>
@@ -6183,19 +6245,23 @@
         <v>0.3</v>
       </c>
       <c r="BH25" s="59">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>0.15</v>
+      </c>
+      <c r="BI25" s="59">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BI25" s="59">
+      <c r="BJ25" s="59">
         <v>45</v>
       </c>
-      <c r="BJ25" s="59">
+      <c r="BK25" s="59">
         <v>15</v>
       </c>
-      <c r="BK25" s="38" t="s">
+      <c r="BL25" s="38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6373,19 +6439,23 @@
         <v>0.2</v>
       </c>
       <c r="BH26" s="39">
+        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
+        <v>5.0000000000000017E-2</v>
+      </c>
+      <c r="BI26" s="39">
         <v>0.15</v>
       </c>
-      <c r="BI26" s="39">
+      <c r="BJ26" s="39">
         <v>59</v>
       </c>
-      <c r="BJ26" s="39">
+      <c r="BK26" s="39">
         <v>15</v>
       </c>
-      <c r="BK26" s="38" t="s">
+      <c r="BL26" s="38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:63" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:64" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
@@ -6443,8 +6513,8 @@
       <c r="BF27" s="117"/>
       <c r="BH27"/>
     </row>
-    <row r="29" spans="2:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:63" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -6458,7 +6528,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:63" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:64" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
@@ -6467,7 +6537,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:63" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:64" ht="140.25" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>64</v>
       </c>
@@ -7251,7 +7321,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D53">
         <v>20</v>
@@ -7461,19 +7531,19 @@
     <mergeCell ref="AB27:AF27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BK16:BK23 BK25:BK26">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="BL16:BL23 BL25:BL26">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BK24">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="BL24">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">

</xml_diff>

<commit_message>
Dragons stats that improve when leveling up: boost, speed, eat, hp and size
Former-commit-id: 4c5241d29916b94c816979852cb23ac2d43fe58d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -401,6 +401,9 @@
     <t>[waterGravityModifier]</t>
   </si>
   <si>
+    <t>[airGravityModifier]</t>
+  </si>
+  <si>
     <t>[gravityModifier]</t>
   </si>
   <si>
@@ -455,9 +458,6 @@
     <t>[maxAlcohol]</t>
   </si>
   <si>
-    <t>[eatSpeedFactor]</t>
-  </si>
-  <si>
     <t>[scoreTextThresholdMultiplier]</t>
   </si>
   <si>
@@ -605,10 +605,10 @@
     <t>[energyBaseMax]</t>
   </si>
   <si>
-    <t>[airGravityModifierMin]</t>
-  </si>
-  <si>
-    <t>[airGravityModifierMax]</t>
+    <t>[eatSpeedFactorMin]</t>
+  </si>
+  <si>
+    <t>[eatSpeedFactorMax]</t>
   </si>
 </sst>
 </file>
@@ -761,7 +761,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1145,11 +1145,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1229,9 +1242,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1447,9 +1457,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1496,8 +1503,26 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1505,11 +1530,61 @@
   </cellStyles>
   <dxfs count="99">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1517,7 +1592,7 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
+        <right style="medium">
           <color auto="1"/>
         </right>
         <top style="thin">
@@ -1527,58 +1602,10 @@
           <color auto="1"/>
         </bottom>
         <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3534,7 +3561,10 @@
     <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="65"/>
     <tableColumn id="25" name="[furyMax]" dataDxfId="64"/>
     <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="63"/>
-    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="62"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="62"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="5">
+      <calculatedColumnFormula>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="15" name="[maxAlcohol]" dataDxfId="61"/>
     <tableColumn id="13" name="[alcoholDrain]" dataDxfId="60"/>
     <tableColumn id="6" name="[gamePrefab]" dataDxfId="59"/>
@@ -3565,10 +3595,7 @@
     <tableColumn id="35" name="[mass]" dataDxfId="40"/>
     <tableColumn id="36" name="[friction]" dataDxfId="39"/>
     <tableColumn id="37" name="[gravityModifier]" dataDxfId="38"/>
-    <tableColumn id="43" name="[airGravityModifierMin]" dataDxfId="37"/>
-    <tableColumn id="63" name="[airGravityModifierMax]" dataDxfId="0">
-      <calculatedColumnFormula>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="37"/>
     <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="36"/>
     <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="35"/>
     <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="34"/>
@@ -3925,8 +3952,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM10" workbookViewId="0">
-      <selection activeCell="BC25" sqref="BC25"/>
+    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
+      <selection activeCell="BB29" sqref="BB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,7 +4085,7 @@
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="95" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="9">
@@ -4070,7 +4097,7 @@
       <c r="F7" s="16">
         <v>3</v>
       </c>
-      <c r="G7" s="97" t="str">
+      <c r="G7" s="96" t="str">
         <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
@@ -4079,7 +4106,7 @@
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="96" t="s">
+      <c r="C8" s="95" t="s">
         <v>84</v>
       </c>
       <c r="D8" s="9">
@@ -4091,7 +4118,7 @@
       <c r="F8" s="13">
         <v>4</v>
       </c>
-      <c r="G8" s="95" t="str">
+      <c r="G8" s="94" t="str">
         <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
@@ -4100,7 +4127,7 @@
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="C9" s="95" t="s">
         <v>79</v>
       </c>
       <c r="D9" s="9">
@@ -4112,7 +4139,7 @@
       <c r="F9" s="13">
         <v>4</v>
       </c>
-      <c r="G9" s="95" t="str">
+      <c r="G9" s="94" t="str">
         <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
@@ -4164,199 +4191,199 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="118"/>
-      <c r="AP14" s="118"/>
-      <c r="AQ14" s="118"/>
-      <c r="AR14" s="118"/>
+      <c r="AO14" s="116"/>
+      <c r="AP14" s="116"/>
+      <c r="AQ14" s="116"/>
+      <c r="AR14" s="116"/>
     </row>
     <row r="15" spans="2:64" ht="163.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="C15" s="79" t="s">
+      <c r="C15" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="79" t="s">
+      <c r="D15" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="77" t="s">
+      <c r="F15" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="94" t="s">
+      <c r="G15" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="H15" s="93" t="s">
+      <c r="H15" s="92" t="s">
         <v>167</v>
       </c>
-      <c r="I15" s="92" t="s">
+      <c r="I15" s="91" t="s">
         <v>166</v>
       </c>
-      <c r="J15" s="91" t="s">
+      <c r="J15" s="90" t="s">
         <v>165</v>
       </c>
-      <c r="K15" s="90" t="s">
+      <c r="K15" s="89" t="s">
         <v>164</v>
       </c>
-      <c r="L15" s="88" t="s">
+      <c r="L15" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="M15" s="86" t="s">
+      <c r="M15" s="85" t="s">
         <v>162</v>
       </c>
-      <c r="N15" s="90" t="s">
+      <c r="N15" s="89" t="s">
         <v>161</v>
       </c>
-      <c r="O15" s="88" t="s">
+      <c r="O15" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="P15" s="88" t="s">
+      <c r="P15" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="Q15" s="87" t="s">
+      <c r="Q15" s="86" t="s">
         <v>158</v>
       </c>
-      <c r="R15" s="87" t="s">
+      <c r="R15" s="86" t="s">
         <v>157</v>
       </c>
-      <c r="S15" s="87" t="s">
+      <c r="S15" s="86" t="s">
         <v>156</v>
       </c>
-      <c r="T15" s="86" t="s">
+      <c r="T15" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="U15" s="88" t="s">
+      <c r="U15" s="87" t="s">
         <v>154</v>
       </c>
-      <c r="V15" s="89" t="s">
+      <c r="V15" s="88" t="s">
         <v>153</v>
       </c>
-      <c r="W15" s="86" t="s">
+      <c r="W15" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="X15" s="90" t="s">
+      <c r="X15" s="89" t="s">
         <v>191</v>
       </c>
-      <c r="Y15" s="90" t="s">
+      <c r="Y15" s="89" t="s">
         <v>192</v>
       </c>
-      <c r="Z15" s="90" t="s">
+      <c r="Z15" s="89" t="s">
         <v>151</v>
       </c>
-      <c r="AA15" s="88" t="s">
+      <c r="AA15" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="AB15" s="89" t="s">
+      <c r="AB15" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="AC15" s="88" t="s">
+      <c r="AC15" s="87" t="s">
         <v>148</v>
       </c>
-      <c r="AD15" s="88" t="s">
+      <c r="AD15" s="87" t="s">
         <v>147</v>
       </c>
-      <c r="AE15" s="88" t="s">
+      <c r="AE15" s="87" t="s">
         <v>146</v>
       </c>
-      <c r="AF15" s="128" t="s">
+      <c r="AF15" s="127" t="s">
         <v>145</v>
       </c>
-      <c r="AG15" s="87" t="s">
+      <c r="AG15" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="AH15" s="86" t="s">
+      <c r="AH15" s="85" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI15" s="85" t="s">
+        <v>194</v>
+      </c>
+      <c r="AJ15" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="AI15" s="86" t="s">
+      <c r="AK15" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="AJ15" s="86" t="s">
+      <c r="AL15" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM15" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN15" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="AK15" s="85" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL15" s="83" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM15" s="83" t="s">
+      <c r="AO15" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="AN15" s="83" t="s">
+      <c r="AP15" s="82" t="s">
         <v>139</v>
       </c>
-      <c r="AO15" s="83" t="s">
+      <c r="AQ15" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="AP15" s="83" t="s">
+      <c r="AR15" s="83" t="s">
         <v>137</v>
       </c>
-      <c r="AQ15" s="84" t="s">
+      <c r="AS15" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="AR15" s="83" t="s">
+      <c r="AT15" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="AS15" s="83" t="s">
+      <c r="AU15" s="82" t="s">
         <v>134</v>
       </c>
-      <c r="AT15" s="83" t="s">
+      <c r="AV15" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="AU15" s="83" t="s">
+      <c r="AW15" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="AV15" s="83" t="s">
+      <c r="AX15" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="AW15" s="83" t="s">
+      <c r="AY15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ15" s="81" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA15" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="AX15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AY15" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="AZ15" s="81" t="s">
+      <c r="BB15" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="BA15" s="77" t="s">
+      <c r="BC15" s="79" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD15" s="75" t="s">
+        <v>190</v>
+      </c>
+      <c r="BE15" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="BB15" s="80" t="s">
-        <v>189</v>
-      </c>
-      <c r="BC15" s="76" t="s">
-        <v>190</v>
-      </c>
-      <c r="BD15" s="79" t="s">
+      <c r="BF15" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="BE15" s="79" t="s">
+      <c r="BG15" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="BF15" s="79" t="s">
+      <c r="BH15" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="BG15" s="76" t="s">
-        <v>193</v>
-      </c>
-      <c r="BH15" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="BI15" s="76" t="s">
+      <c r="BI15" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="BJ15" s="78" t="s">
+      <c r="BJ15" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="BK15" s="77" t="s">
+      <c r="BK15" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="BL15" s="76" t="s">
+      <c r="BL15" s="75" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4364,35 +4391,35 @@
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="57">
         <v>0</v>
       </c>
-      <c r="F16" s="58"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="28">
         <v>0</v>
       </c>
       <c r="H16" s="27">
         <v>0</v>
       </c>
-      <c r="I16" s="71">
+      <c r="I16" s="70">
         <v>35</v>
       </c>
-      <c r="J16" s="70">
+      <c r="J16" s="69">
         <v>45</v>
       </c>
       <c r="K16" s="25">
         <v>1</v>
       </c>
-      <c r="L16" s="66">
+      <c r="L16" s="65">
         <v>-2.5</v>
       </c>
-      <c r="M16" s="65">
+      <c r="M16" s="64">
         <v>75</v>
       </c>
       <c r="N16" s="29">
@@ -4407,19 +4434,19 @@
       <c r="Q16" s="29">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="R16" s="51">
+      <c r="R16" s="50">
         <v>30</v>
       </c>
-      <c r="S16" s="51">
+      <c r="S16" s="50">
         <v>0.5</v>
       </c>
-      <c r="T16" s="65">
+      <c r="T16" s="64">
         <v>0.46</v>
       </c>
       <c r="U16" s="29">
         <v>0.76</v>
       </c>
-      <c r="V16" s="69">
+      <c r="V16" s="68">
         <v>14</v>
       </c>
       <c r="W16" s="29">
@@ -4438,55 +4465,56 @@
       <c r="AA16" s="29">
         <v>28</v>
       </c>
-      <c r="AB16" s="69">
+      <c r="AB16" s="68">
         <v>250</v>
       </c>
-      <c r="AC16" s="51">
+      <c r="AC16" s="50">
         <v>7.5</v>
       </c>
       <c r="AD16" s="29">
         <v>2</v>
       </c>
-      <c r="AE16" s="51">
+      <c r="AE16" s="50">
         <v>8</v>
       </c>
       <c r="AF16" s="29">
         <v>3000</v>
       </c>
-      <c r="AG16" s="68">
+      <c r="AG16" s="67">
         <v>1</v>
       </c>
-      <c r="AH16" s="65">
+      <c r="AH16" s="129">
         <v>0.23</v>
       </c>
-      <c r="AI16" s="75">
+      <c r="AI16" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>0.20500000000000002</v>
+      </c>
+      <c r="AJ16" s="74">
         <v>0</v>
       </c>
-      <c r="AJ16" s="75">
+      <c r="AK16" s="74">
         <v>6</v>
       </c>
-      <c r="AK16" s="24" t="s">
+      <c r="AL16" s="24" t="s">
         <v>120</v>
-      </c>
-      <c r="AL16" s="24" t="s">
-        <v>119</v>
       </c>
       <c r="AM16" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="AN16" s="24"/>
+      <c r="AN16" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="AO16" s="24"/>
-      <c r="AP16" s="24">
+      <c r="AP16" s="24"/>
+      <c r="AQ16" s="24">
         <v>4.0999999999999996</v>
-      </c>
-      <c r="AQ16" s="24">
-        <v>2</v>
       </c>
       <c r="AR16" s="24">
         <v>2</v>
       </c>
-      <c r="AS16" s="24" t="b">
-        <v>1</v>
+      <c r="AS16" s="24">
+        <v>2</v>
       </c>
       <c r="AT16" s="24" t="b">
         <v>1</v>
@@ -4494,56 +4522,55 @@
       <c r="AU16" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV16" s="24">
+      <c r="AV16" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW16" s="24">
         <v>23</v>
       </c>
-      <c r="AW16" s="24">
+      <c r="AX16" s="24">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AX16" s="73" t="s">
+      <c r="AY16" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="AY16" s="72" t="s">
+      <c r="AZ16" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="AZ16" s="42">
+      <c r="BA16" s="41">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="BA16" s="41">
+      <c r="BB16" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB16" s="40">
+      <c r="BC16" s="39">
         <v>175</v>
       </c>
-      <c r="BC16" s="114">
+      <c r="BD16" s="112">
         <v>200</v>
       </c>
-      <c r="BD16" s="59">
+      <c r="BE16" s="58">
         <v>2</v>
       </c>
-      <c r="BE16" s="59">
+      <c r="BF16" s="58">
         <v>9.5</v>
       </c>
-      <c r="BF16" s="59">
+      <c r="BG16" s="58">
         <v>1</v>
       </c>
-      <c r="BG16" s="74">
+      <c r="BH16" s="73">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BH16" s="74">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="BI16" s="74">
+      <c r="BI16" s="73">
         <v>1.75</v>
       </c>
-      <c r="BJ16" s="74">
+      <c r="BJ16" s="73">
         <v>0</v>
       </c>
-      <c r="BK16" s="74">
+      <c r="BK16" s="73">
         <v>6</v>
       </c>
-      <c r="BL16" s="59" t="s">
+      <c r="BL16" s="58" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4551,16 +4578,16 @@
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="58">
+      <c r="E17" s="57">
         <v>1</v>
       </c>
-      <c r="F17" s="57" t="s">
+      <c r="F17" s="56" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="28">
@@ -4569,19 +4596,19 @@
       <c r="H17" s="27">
         <v>60</v>
       </c>
-      <c r="I17" s="71">
+      <c r="I17" s="70">
         <v>35</v>
       </c>
-      <c r="J17" s="70">
+      <c r="J17" s="69">
         <v>45</v>
       </c>
       <c r="K17" s="25">
         <v>3</v>
       </c>
-      <c r="L17" s="66">
+      <c r="L17" s="65">
         <v>-2.5</v>
       </c>
-      <c r="M17" s="65">
+      <c r="M17" s="64">
         <v>95</v>
       </c>
       <c r="N17" s="29">
@@ -4596,19 +4623,19 @@
       <c r="Q17" s="29">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="R17" s="51">
+      <c r="R17" s="50">
         <v>30</v>
       </c>
-      <c r="S17" s="51">
+      <c r="S17" s="50">
         <v>0.5</v>
       </c>
-      <c r="T17" s="47">
+      <c r="T17" s="46">
         <v>0.8</v>
       </c>
       <c r="U17" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V17" s="69">
+      <c r="V17" s="68">
         <v>16</v>
       </c>
       <c r="W17" s="29">
@@ -4627,55 +4654,56 @@
       <c r="AA17" s="29">
         <v>10</v>
       </c>
-      <c r="AB17" s="69">
+      <c r="AB17" s="68">
         <v>275</v>
       </c>
-      <c r="AC17" s="51">
+      <c r="AC17" s="50">
         <v>8</v>
       </c>
       <c r="AD17" s="29">
         <v>3</v>
       </c>
-      <c r="AE17" s="51">
+      <c r="AE17" s="50">
         <v>9</v>
       </c>
       <c r="AF17" s="29">
         <v>7000</v>
       </c>
-      <c r="AG17" s="68">
+      <c r="AG17" s="67">
         <v>2</v>
       </c>
-      <c r="AH17" s="65">
+      <c r="AH17" s="129">
         <v>0.19</v>
       </c>
-      <c r="AI17" s="46">
+      <c r="AI17" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="AJ17" s="74">
         <v>0</v>
       </c>
-      <c r="AJ17" s="46">
+      <c r="AK17" s="45">
         <v>6</v>
       </c>
-      <c r="AK17" s="45" t="s">
+      <c r="AL17" s="44" t="s">
         <v>116</v>
-      </c>
-      <c r="AL17" s="24" t="s">
-        <v>115</v>
       </c>
       <c r="AM17" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="AN17" s="24"/>
+      <c r="AN17" s="24" t="s">
+        <v>115</v>
+      </c>
       <c r="AO17" s="24"/>
-      <c r="AP17" s="24">
+      <c r="AP17" s="24"/>
+      <c r="AQ17" s="24">
         <v>2.2999999999999998</v>
-      </c>
-      <c r="AQ17" s="24">
-        <v>2</v>
       </c>
       <c r="AR17" s="24">
         <v>2</v>
       </c>
-      <c r="AS17" s="24" t="b">
-        <v>1</v>
+      <c r="AS17" s="24">
+        <v>2</v>
       </c>
       <c r="AT17" s="24" t="b">
         <v>1</v>
@@ -4683,56 +4711,55 @@
       <c r="AU17" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV17" s="24">
+      <c r="AV17" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW17" s="24">
         <v>23</v>
       </c>
-      <c r="AW17" s="24">
+      <c r="AX17" s="24">
         <v>0.7</v>
       </c>
-      <c r="AX17" s="73" t="s">
+      <c r="AY17" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="AY17" s="72" t="s">
+      <c r="AZ17" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="AZ17" s="42">
+      <c r="BA17" s="41">
         <v>2.3E-3</v>
       </c>
-      <c r="BA17" s="41">
+      <c r="BB17" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB17" s="40">
+      <c r="BC17" s="39">
         <v>210</v>
       </c>
-      <c r="BC17" s="114">
+      <c r="BD17" s="112">
         <v>235</v>
       </c>
-      <c r="BD17" s="59">
+      <c r="BE17" s="58">
         <v>2.1</v>
       </c>
-      <c r="BE17" s="59">
+      <c r="BF17" s="58">
         <v>9.5</v>
       </c>
-      <c r="BF17" s="59">
+      <c r="BG17" s="58">
         <v>1.7</v>
       </c>
-      <c r="BG17" s="59">
+      <c r="BH17" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BH17" s="59">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="BI17" s="59">
+      <c r="BI17" s="58">
         <v>2.1</v>
       </c>
-      <c r="BJ17" s="59">
+      <c r="BJ17" s="58">
         <v>0</v>
       </c>
-      <c r="BK17" s="59">
+      <c r="BK17" s="58">
         <v>6</v>
       </c>
-      <c r="BL17" s="59" t="s">
+      <c r="BL17" s="58" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4740,37 +4767,37 @@
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="58">
+      <c r="E18" s="57">
         <v>2</v>
       </c>
-      <c r="F18" s="58" t="s">
+      <c r="F18" s="57" t="s">
         <v>6</v>
       </c>
       <c r="G18" s="30">
         <v>11000</v>
       </c>
-      <c r="H18" s="56">
+      <c r="H18" s="55">
         <v>100</v>
       </c>
-      <c r="I18" s="55">
+      <c r="I18" s="54">
         <v>35</v>
       </c>
-      <c r="J18" s="67">
+      <c r="J18" s="66">
         <v>45</v>
       </c>
       <c r="K18" s="25">
         <v>5</v>
       </c>
-      <c r="L18" s="66">
+      <c r="L18" s="65">
         <v>-2.5</v>
       </c>
-      <c r="M18" s="65">
+      <c r="M18" s="64">
         <v>140</v>
       </c>
       <c r="N18" s="26">
@@ -4785,19 +4812,19 @@
       <c r="Q18" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="R18" s="51">
+      <c r="R18" s="50">
         <v>30</v>
       </c>
-      <c r="S18" s="51">
+      <c r="S18" s="50">
         <v>0.5</v>
       </c>
-      <c r="T18" s="65">
+      <c r="T18" s="64">
         <v>0.85</v>
       </c>
       <c r="U18" s="29">
         <v>1.1499999999999999</v>
       </c>
-      <c r="V18" s="50">
+      <c r="V18" s="49">
         <v>23.5</v>
       </c>
       <c r="W18" s="29">
@@ -4816,55 +4843,56 @@
       <c r="AA18" s="29">
         <v>14</v>
       </c>
-      <c r="AB18" s="50">
+      <c r="AB18" s="49">
         <v>300</v>
       </c>
-      <c r="AC18" s="51">
+      <c r="AC18" s="50">
         <v>9</v>
       </c>
       <c r="AD18" s="26">
         <v>3</v>
       </c>
-      <c r="AE18" s="64">
+      <c r="AE18" s="63">
         <v>9</v>
       </c>
       <c r="AF18" s="29">
         <v>8000</v>
       </c>
-      <c r="AG18" s="63">
+      <c r="AG18" s="62">
         <v>2</v>
       </c>
-      <c r="AH18" s="47">
+      <c r="AH18" s="130">
         <v>0.15</v>
       </c>
-      <c r="AI18" s="62">
+      <c r="AI18" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>0.125</v>
+      </c>
+      <c r="AJ18" s="132">
         <v>0</v>
       </c>
-      <c r="AJ18" s="62">
+      <c r="AK18" s="61">
         <v>6</v>
       </c>
-      <c r="AK18" s="45" t="s">
+      <c r="AL18" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="AL18" s="24" t="s">
+      <c r="AM18" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="AM18" s="24" t="s">
+      <c r="AN18" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AN18" s="24"/>
       <c r="AO18" s="24"/>
-      <c r="AP18" s="24">
+      <c r="AP18" s="24"/>
+      <c r="AQ18" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AQ18" s="24">
-        <v>2</v>
       </c>
       <c r="AR18" s="24">
         <v>2</v>
       </c>
-      <c r="AS18" s="24" t="b">
-        <v>1</v>
+      <c r="AS18" s="24">
+        <v>2</v>
       </c>
       <c r="AT18" s="24" t="b">
         <v>1</v>
@@ -4872,56 +4900,55 @@
       <c r="AU18" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV18" s="24">
+      <c r="AV18" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW18" s="24">
         <v>23</v>
       </c>
-      <c r="AW18" s="24">
+      <c r="AX18" s="24">
         <v>0.7</v>
       </c>
-      <c r="AX18" s="61" t="s">
+      <c r="AY18" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="AY18" s="60" t="s">
+      <c r="AZ18" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="AZ18" s="42">
+      <c r="BA18" s="41">
         <v>2E-3</v>
       </c>
-      <c r="BA18" s="41">
+      <c r="BB18" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB18" s="40">
+      <c r="BC18" s="39">
         <v>240</v>
       </c>
-      <c r="BC18" s="114">
+      <c r="BD18" s="112">
         <v>280</v>
       </c>
-      <c r="BD18" s="59">
+      <c r="BE18" s="58">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BE18" s="59">
+      <c r="BF18" s="58">
         <v>9.5</v>
       </c>
-      <c r="BF18" s="59">
+      <c r="BG18" s="58">
         <v>1.7</v>
       </c>
-      <c r="BG18" s="59">
+      <c r="BH18" s="58">
         <v>0.9</v>
       </c>
-      <c r="BH18" s="59">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.75</v>
-      </c>
-      <c r="BI18" s="59">
+      <c r="BI18" s="58">
         <v>2.25</v>
       </c>
-      <c r="BJ18" s="59">
+      <c r="BJ18" s="58">
         <v>0</v>
       </c>
-      <c r="BK18" s="59">
+      <c r="BK18" s="58">
         <v>6</v>
       </c>
-      <c r="BL18" s="38" t="s">
+      <c r="BL18" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4929,16 +4956,16 @@
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="59" t="s">
+      <c r="D19" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="58">
+      <c r="E19" s="57">
         <v>3</v>
       </c>
-      <c r="F19" s="58" t="s">
+      <c r="F19" s="57" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="28">
@@ -4947,19 +4974,19 @@
       <c r="H19" s="27">
         <v>150</v>
       </c>
-      <c r="I19" s="71">
+      <c r="I19" s="70">
         <v>35</v>
       </c>
-      <c r="J19" s="70">
+      <c r="J19" s="69">
         <v>45</v>
       </c>
       <c r="K19" s="25">
         <v>6</v>
       </c>
-      <c r="L19" s="66">
+      <c r="L19" s="65">
         <v>-2.5</v>
       </c>
-      <c r="M19" s="65">
+      <c r="M19" s="64">
         <v>190</v>
       </c>
       <c r="N19" s="29">
@@ -4974,19 +5001,19 @@
       <c r="Q19" s="29">
         <v>0.01</v>
       </c>
-      <c r="R19" s="51">
+      <c r="R19" s="50">
         <v>30</v>
       </c>
-      <c r="S19" s="51">
+      <c r="S19" s="50">
         <v>0.6</v>
       </c>
-      <c r="T19" s="47">
+      <c r="T19" s="46">
         <v>0.9</v>
       </c>
       <c r="U19" s="26">
         <v>1.1499999999999999</v>
       </c>
-      <c r="V19" s="69">
+      <c r="V19" s="68">
         <v>19</v>
       </c>
       <c r="W19" s="29">
@@ -5005,55 +5032,56 @@
       <c r="AA19" s="26">
         <v>22</v>
       </c>
-      <c r="AB19" s="69">
+      <c r="AB19" s="68">
         <v>325</v>
       </c>
-      <c r="AC19" s="51">
+      <c r="AC19" s="50">
         <v>10</v>
       </c>
       <c r="AD19" s="29">
         <v>3</v>
       </c>
-      <c r="AE19" s="51">
+      <c r="AE19" s="50">
         <v>9</v>
       </c>
       <c r="AF19" s="29">
         <v>9000</v>
       </c>
-      <c r="AG19" s="68">
+      <c r="AG19" s="67">
         <v>2</v>
       </c>
-      <c r="AH19" s="65">
+      <c r="AH19" s="129">
         <v>0.13</v>
       </c>
-      <c r="AI19" s="46">
+      <c r="AI19" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>0.10500000000000001</v>
+      </c>
+      <c r="AJ19" s="74">
         <v>0</v>
       </c>
-      <c r="AJ19" s="46">
+      <c r="AK19" s="45">
         <v>6</v>
       </c>
-      <c r="AK19" s="45" t="s">
+      <c r="AL19" s="44" t="s">
         <v>106</v>
-      </c>
-      <c r="AL19" s="24" t="s">
-        <v>105</v>
       </c>
       <c r="AM19" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="AN19" s="24"/>
+      <c r="AN19" s="24" t="s">
+        <v>105</v>
+      </c>
       <c r="AO19" s="24"/>
-      <c r="AP19" s="24">
+      <c r="AP19" s="24"/>
+      <c r="AQ19" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AQ19" s="24">
-        <v>2</v>
       </c>
       <c r="AR19" s="24">
         <v>2</v>
       </c>
-      <c r="AS19" s="24" t="b">
-        <v>1</v>
+      <c r="AS19" s="24">
+        <v>2</v>
       </c>
       <c r="AT19" s="24" t="b">
         <v>1</v>
@@ -5061,56 +5089,55 @@
       <c r="AU19" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV19" s="24">
+      <c r="AV19" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW19" s="24">
         <v>23</v>
       </c>
-      <c r="AW19" s="24">
+      <c r="AX19" s="24">
         <v>0.7</v>
       </c>
-      <c r="AX19" s="61" t="s">
+      <c r="AY19" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="AY19" s="60" t="s">
+      <c r="AZ19" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="AZ19" s="42">
+      <c r="BA19" s="41">
         <v>2E-3</v>
       </c>
-      <c r="BA19" s="41">
+      <c r="BB19" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB19" s="40">
+      <c r="BC19" s="39">
         <v>360</v>
       </c>
-      <c r="BC19" s="114">
+      <c r="BD19" s="112">
         <v>380</v>
       </c>
-      <c r="BD19" s="59">
+      <c r="BE19" s="58">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BE19" s="59">
+      <c r="BF19" s="58">
         <v>5</v>
       </c>
-      <c r="BF19" s="59">
+      <c r="BG19" s="58">
         <v>0.5</v>
       </c>
-      <c r="BG19" s="59">
+      <c r="BH19" s="58">
         <v>1</v>
       </c>
-      <c r="BH19" s="59">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.85</v>
-      </c>
-      <c r="BI19" s="59">
+      <c r="BI19" s="58">
         <v>1.3</v>
       </c>
-      <c r="BJ19" s="59">
+      <c r="BJ19" s="58">
         <v>0</v>
       </c>
-      <c r="BK19" s="59">
+      <c r="BK19" s="58">
         <v>6</v>
       </c>
-      <c r="BL19" s="38" t="s">
+      <c r="BL19" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5118,16 +5145,16 @@
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="58">
+      <c r="E20" s="57">
         <v>4</v>
       </c>
-      <c r="F20" s="58" t="s">
+      <c r="F20" s="57" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="28">
@@ -5136,19 +5163,19 @@
       <c r="H20" s="27">
         <v>200</v>
       </c>
-      <c r="I20" s="71">
+      <c r="I20" s="70">
         <v>35</v>
       </c>
-      <c r="J20" s="70">
+      <c r="J20" s="69">
         <v>45</v>
       </c>
       <c r="K20" s="25">
         <v>8</v>
       </c>
-      <c r="L20" s="66">
+      <c r="L20" s="65">
         <v>0</v>
       </c>
-      <c r="M20" s="65">
+      <c r="M20" s="64">
         <v>210</v>
       </c>
       <c r="N20" s="29">
@@ -5163,19 +5190,19 @@
       <c r="Q20" s="29">
         <v>1.2E-2</v>
       </c>
-      <c r="R20" s="51">
+      <c r="R20" s="50">
         <v>30</v>
       </c>
-      <c r="S20" s="51">
+      <c r="S20" s="50">
         <v>0.6</v>
       </c>
-      <c r="T20" s="65">
+      <c r="T20" s="64">
         <v>1</v>
       </c>
       <c r="U20" s="29">
         <v>1.25</v>
       </c>
-      <c r="V20" s="69">
+      <c r="V20" s="68">
         <v>20</v>
       </c>
       <c r="W20" s="29">
@@ -5194,55 +5221,56 @@
       <c r="AA20" s="29">
         <v>34</v>
       </c>
-      <c r="AB20" s="69">
+      <c r="AB20" s="68">
         <v>350</v>
       </c>
-      <c r="AC20" s="51">
+      <c r="AC20" s="50">
         <v>11</v>
       </c>
       <c r="AD20" s="29">
         <v>4</v>
       </c>
-      <c r="AE20" s="51">
+      <c r="AE20" s="50">
         <v>10</v>
       </c>
       <c r="AF20" s="29">
         <v>10000</v>
       </c>
-      <c r="AG20" s="68">
+      <c r="AG20" s="67">
         <v>3</v>
       </c>
-      <c r="AH20" s="65">
+      <c r="AH20" s="129">
         <v>0.11</v>
       </c>
-      <c r="AI20" s="46">
+      <c r="AI20" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>8.4999999999999992E-2</v>
+      </c>
+      <c r="AJ20" s="74">
         <v>0</v>
       </c>
-      <c r="AJ20" s="46">
+      <c r="AK20" s="45">
         <v>12</v>
       </c>
-      <c r="AK20" s="45" t="s">
+      <c r="AL20" s="44" t="s">
         <v>102</v>
-      </c>
-      <c r="AL20" s="24" t="s">
-        <v>101</v>
       </c>
       <c r="AM20" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="AN20" s="24"/>
+      <c r="AN20" s="24" t="s">
+        <v>101</v>
+      </c>
       <c r="AO20" s="24"/>
-      <c r="AP20" s="24">
+      <c r="AP20" s="24"/>
+      <c r="AQ20" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AQ20" s="24">
-        <v>2</v>
       </c>
       <c r="AR20" s="24">
         <v>2</v>
       </c>
-      <c r="AS20" s="24" t="b">
-        <v>1</v>
+      <c r="AS20" s="24">
+        <v>2</v>
       </c>
       <c r="AT20" s="24" t="b">
         <v>1</v>
@@ -5250,56 +5278,55 @@
       <c r="AU20" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV20" s="24">
+      <c r="AV20" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW20" s="24">
         <v>23</v>
       </c>
-      <c r="AW20" s="24">
+      <c r="AX20" s="24">
         <v>0.7</v>
       </c>
-      <c r="AX20" s="61" t="s">
+      <c r="AY20" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="AY20" s="60" t="s">
+      <c r="AZ20" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="AZ20" s="42">
+      <c r="BA20" s="41">
         <v>1.9E-3</v>
       </c>
-      <c r="BA20" s="41">
+      <c r="BB20" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB20" s="40">
+      <c r="BC20" s="39">
         <v>300</v>
       </c>
-      <c r="BC20" s="114">
+      <c r="BD20" s="112">
         <v>325</v>
       </c>
-      <c r="BD20" s="59">
+      <c r="BE20" s="58">
         <v>2.4</v>
       </c>
-      <c r="BE20" s="59">
+      <c r="BF20" s="58">
         <v>9.5</v>
       </c>
-      <c r="BF20" s="59">
+      <c r="BG20" s="58">
         <v>1.7</v>
       </c>
-      <c r="BG20" s="59">
+      <c r="BH20" s="58">
         <v>1</v>
       </c>
-      <c r="BH20" s="59">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.85</v>
-      </c>
-      <c r="BI20" s="59">
+      <c r="BI20" s="58">
         <v>1.6</v>
       </c>
-      <c r="BJ20" s="59">
+      <c r="BJ20" s="58">
         <v>9</v>
       </c>
-      <c r="BK20" s="59">
+      <c r="BK20" s="58">
         <v>6</v>
       </c>
-      <c r="BL20" s="38" t="s">
+      <c r="BL20" s="37" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5307,16 +5334,16 @@
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="59" t="s">
+      <c r="D21" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="58">
+      <c r="E21" s="57">
         <v>5</v>
       </c>
-      <c r="F21" s="58" t="s">
+      <c r="F21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="28">
@@ -5325,19 +5352,19 @@
       <c r="H21" s="27">
         <v>400</v>
       </c>
-      <c r="I21" s="71">
+      <c r="I21" s="70">
         <v>35</v>
       </c>
-      <c r="J21" s="70">
+      <c r="J21" s="69">
         <v>45</v>
       </c>
       <c r="K21" s="25">
         <v>10</v>
       </c>
-      <c r="L21" s="66">
+      <c r="L21" s="65">
         <v>0</v>
       </c>
-      <c r="M21" s="65">
+      <c r="M21" s="64">
         <v>250</v>
       </c>
       <c r="N21" s="26">
@@ -5352,19 +5379,19 @@
       <c r="Q21" s="29">
         <v>1.2E-2</v>
       </c>
-      <c r="R21" s="51">
+      <c r="R21" s="50">
         <v>30</v>
       </c>
-      <c r="S21" s="51">
+      <c r="S21" s="50">
         <v>0.6</v>
       </c>
-      <c r="T21" s="65">
+      <c r="T21" s="64">
         <v>1.05</v>
       </c>
       <c r="U21" s="29">
         <v>1.3</v>
       </c>
-      <c r="V21" s="69">
+      <c r="V21" s="68">
         <v>21</v>
       </c>
       <c r="W21" s="29">
@@ -5383,55 +5410,56 @@
       <c r="AA21" s="29">
         <v>14</v>
       </c>
-      <c r="AB21" s="69">
+      <c r="AB21" s="68">
         <v>375</v>
       </c>
-      <c r="AC21" s="51">
+      <c r="AC21" s="50">
         <v>11</v>
       </c>
       <c r="AD21" s="29">
         <v>4</v>
       </c>
-      <c r="AE21" s="51">
+      <c r="AE21" s="50">
         <v>10</v>
       </c>
       <c r="AF21" s="29">
         <v>10000</v>
       </c>
-      <c r="AG21" s="68">
+      <c r="AG21" s="67">
         <v>3</v>
       </c>
-      <c r="AH21" s="65">
+      <c r="AH21" s="129">
         <v>0.09</v>
       </c>
-      <c r="AI21" s="46">
+      <c r="AI21" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AJ21" s="74">
         <v>0</v>
       </c>
-      <c r="AJ21" s="46">
+      <c r="AK21" s="45">
         <v>12</v>
       </c>
-      <c r="AK21" s="45" t="s">
+      <c r="AL21" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="AL21" s="24" t="s">
+      <c r="AM21" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AM21" s="24" t="s">
+      <c r="AN21" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AN21" s="24"/>
       <c r="AO21" s="24"/>
-      <c r="AP21" s="24">
-        <v>2</v>
-      </c>
+      <c r="AP21" s="24"/>
       <c r="AQ21" s="24">
         <v>2</v>
       </c>
       <c r="AR21" s="24">
         <v>2</v>
       </c>
-      <c r="AS21" s="24" t="b">
-        <v>1</v>
+      <c r="AS21" s="24">
+        <v>2</v>
       </c>
       <c r="AT21" s="24" t="b">
         <v>1</v>
@@ -5439,56 +5467,55 @@
       <c r="AU21" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV21" s="24">
+      <c r="AV21" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW21" s="24">
         <v>23</v>
       </c>
-      <c r="AW21" s="24">
+      <c r="AX21" s="24">
         <v>0.7</v>
       </c>
-      <c r="AX21" s="61" t="s">
+      <c r="AY21" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="AY21" s="60" t="s">
+      <c r="AZ21" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="AZ21" s="42">
+      <c r="BA21" s="41">
         <v>1.8E-3</v>
       </c>
-      <c r="BA21" s="41">
+      <c r="BB21" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB21" s="40">
+      <c r="BC21" s="39">
         <v>322</v>
       </c>
-      <c r="BC21" s="114">
+      <c r="BD21" s="112">
         <v>347</v>
       </c>
-      <c r="BD21" s="59">
+      <c r="BE21" s="58">
         <v>2.5</v>
       </c>
-      <c r="BE21" s="59">
+      <c r="BF21" s="58">
         <v>9.5</v>
       </c>
-      <c r="BF21" s="59">
+      <c r="BG21" s="58">
         <v>1.7</v>
       </c>
-      <c r="BG21" s="59">
+      <c r="BH21" s="58">
         <v>0.5</v>
       </c>
-      <c r="BH21" s="59">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.35</v>
-      </c>
-      <c r="BI21" s="59">
+      <c r="BI21" s="58">
         <v>1.9</v>
       </c>
-      <c r="BJ21" s="59">
+      <c r="BJ21" s="58">
         <v>9</v>
       </c>
-      <c r="BK21" s="59">
+      <c r="BK21" s="58">
         <v>6</v>
       </c>
-      <c r="BL21" s="38" t="s">
+      <c r="BL21" s="37" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5496,16 +5523,16 @@
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="58">
+      <c r="E22" s="57">
         <v>6</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F22" s="56" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="28">
@@ -5514,19 +5541,19 @@
       <c r="H22" s="27">
         <v>550</v>
       </c>
-      <c r="I22" s="71">
+      <c r="I22" s="70">
         <v>35</v>
       </c>
-      <c r="J22" s="70">
+      <c r="J22" s="69">
         <v>45</v>
       </c>
       <c r="K22" s="25">
         <v>12.5</v>
       </c>
-      <c r="L22" s="66">
+      <c r="L22" s="65">
         <v>0</v>
       </c>
-      <c r="M22" s="65">
+      <c r="M22" s="64">
         <v>290</v>
       </c>
       <c r="N22" s="29">
@@ -5541,19 +5568,19 @@
       <c r="Q22" s="29">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="R22" s="51">
+      <c r="R22" s="50">
         <v>25</v>
       </c>
-      <c r="S22" s="51">
+      <c r="S22" s="50">
         <v>0.6</v>
       </c>
-      <c r="T22" s="65">
+      <c r="T22" s="64">
         <v>1.35</v>
       </c>
       <c r="U22" s="29">
         <v>1.55</v>
       </c>
-      <c r="V22" s="69">
+      <c r="V22" s="68">
         <v>23.5</v>
       </c>
       <c r="W22" s="29">
@@ -5572,55 +5599,56 @@
       <c r="AA22" s="29">
         <v>17</v>
       </c>
-      <c r="AB22" s="69">
+      <c r="AB22" s="68">
         <v>400</v>
       </c>
-      <c r="AC22" s="51">
+      <c r="AC22" s="50">
         <v>11</v>
       </c>
       <c r="AD22" s="29">
         <v>4</v>
       </c>
-      <c r="AE22" s="51">
+      <c r="AE22" s="50">
         <v>10</v>
       </c>
       <c r="AF22" s="29">
         <v>10000</v>
       </c>
-      <c r="AG22" s="68">
+      <c r="AG22" s="67">
         <v>3</v>
       </c>
-      <c r="AH22" s="65">
+      <c r="AH22" s="129">
         <v>0.08</v>
       </c>
-      <c r="AI22" s="46">
+      <c r="AI22" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="AJ22" s="74">
         <v>0</v>
       </c>
-      <c r="AJ22" s="46">
+      <c r="AK22" s="45">
         <v>12</v>
       </c>
-      <c r="AK22" s="45" t="s">
+      <c r="AL22" s="44" t="s">
         <v>92</v>
-      </c>
-      <c r="AL22" s="24" t="s">
-        <v>91</v>
       </c>
       <c r="AM22" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="AN22" s="24"/>
+      <c r="AN22" s="24" t="s">
+        <v>91</v>
+      </c>
       <c r="AO22" s="24"/>
-      <c r="AP22" s="24">
+      <c r="AP22" s="24"/>
+      <c r="AQ22" s="24">
         <v>1.6</v>
-      </c>
-      <c r="AQ22" s="24">
-        <v>2</v>
       </c>
       <c r="AR22" s="24">
         <v>2</v>
       </c>
-      <c r="AS22" s="24" t="b">
-        <v>1</v>
+      <c r="AS22" s="24">
+        <v>2</v>
       </c>
       <c r="AT22" s="24" t="b">
         <v>1</v>
@@ -5628,56 +5656,55 @@
       <c r="AU22" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV22" s="24">
+      <c r="AV22" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW22" s="24">
         <v>23</v>
       </c>
-      <c r="AW22" s="24">
+      <c r="AX22" s="24">
         <v>0.7</v>
       </c>
-      <c r="AX22" s="61" t="s">
+      <c r="AY22" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="AY22" s="60" t="s">
+      <c r="AZ22" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="AZ22" s="42">
+      <c r="BA22" s="41">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="BA22" s="41">
+      <c r="BB22" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB22" s="40">
+      <c r="BC22" s="39">
         <v>343</v>
       </c>
-      <c r="BC22" s="114">
+      <c r="BD22" s="112">
         <v>372</v>
       </c>
-      <c r="BD22" s="59">
+      <c r="BE22" s="58">
         <v>2.6</v>
       </c>
-      <c r="BE22" s="59">
+      <c r="BF22" s="58">
         <v>9.5</v>
       </c>
-      <c r="BF22" s="59">
+      <c r="BG22" s="58">
         <v>1.7</v>
       </c>
-      <c r="BG22" s="59">
+      <c r="BH22" s="58">
         <v>0.5</v>
       </c>
-      <c r="BH22" s="59">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.35</v>
-      </c>
-      <c r="BI22" s="59">
+      <c r="BI22" s="58">
         <v>2</v>
       </c>
-      <c r="BJ22" s="59">
+      <c r="BJ22" s="58">
         <v>9</v>
       </c>
-      <c r="BK22" s="59">
+      <c r="BK22" s="58">
         <v>6</v>
       </c>
-      <c r="BL22" s="38" t="s">
+      <c r="BL22" s="37" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5685,37 +5712,37 @@
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="58">
+      <c r="E23" s="57">
         <v>7</v>
       </c>
-      <c r="F23" s="57" t="s">
+      <c r="F23" s="56" t="s">
         <v>11</v>
       </c>
       <c r="G23" s="30">
         <v>1100000</v>
       </c>
-      <c r="H23" s="56">
+      <c r="H23" s="55">
         <v>800</v>
       </c>
-      <c r="I23" s="55">
+      <c r="I23" s="54">
         <v>35</v>
       </c>
-      <c r="J23" s="67">
+      <c r="J23" s="66">
         <v>45</v>
       </c>
       <c r="K23" s="25">
         <v>17</v>
       </c>
-      <c r="L23" s="66">
+      <c r="L23" s="65">
         <v>0</v>
       </c>
-      <c r="M23" s="65">
+      <c r="M23" s="64">
         <v>330</v>
       </c>
       <c r="N23" s="29">
@@ -5730,19 +5757,19 @@
       <c r="Q23" s="29">
         <v>1.4E-2</v>
       </c>
-      <c r="R23" s="51">
+      <c r="R23" s="50">
         <v>25</v>
       </c>
-      <c r="S23" s="51">
+      <c r="S23" s="50">
         <v>0.7</v>
       </c>
-      <c r="T23" s="65">
+      <c r="T23" s="64">
         <v>1.54</v>
       </c>
       <c r="U23" s="29">
         <v>1.74</v>
       </c>
-      <c r="V23" s="50">
+      <c r="V23" s="49">
         <v>25</v>
       </c>
       <c r="W23" s="29">
@@ -5761,59 +5788,60 @@
       <c r="AA23" s="29">
         <v>18</v>
       </c>
-      <c r="AB23" s="50">
+      <c r="AB23" s="49">
         <v>425</v>
       </c>
-      <c r="AC23" s="51">
+      <c r="AC23" s="50">
         <v>11.5</v>
       </c>
       <c r="AD23" s="26">
         <v>5</v>
       </c>
-      <c r="AE23" s="64">
+      <c r="AE23" s="63">
         <v>10</v>
       </c>
       <c r="AF23" s="29">
         <v>20000</v>
       </c>
-      <c r="AG23" s="63">
+      <c r="AG23" s="62">
         <v>4</v>
       </c>
-      <c r="AH23" s="47">
+      <c r="AH23" s="130">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI23" s="62">
+      <c r="AI23" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="AJ23" s="132">
         <v>0</v>
       </c>
-      <c r="AJ23" s="62">
+      <c r="AK23" s="61">
         <v>12</v>
       </c>
-      <c r="AK23" s="45" t="s">
+      <c r="AL23" s="44" t="s">
         <v>88</v>
-      </c>
-      <c r="AL23" s="24" t="s">
-        <v>87</v>
       </c>
       <c r="AM23" s="24" t="s">
         <v>87</v>
       </c>
       <c r="AN23" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO23" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AO23" s="24" t="s">
+      <c r="AP23" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AP23" s="24">
+      <c r="AQ23" s="24">
         <v>1.4</v>
-      </c>
-      <c r="AQ23" s="24">
-        <v>2</v>
       </c>
       <c r="AR23" s="24">
         <v>2</v>
       </c>
-      <c r="AS23" s="24" t="b">
-        <v>1</v>
+      <c r="AS23" s="24">
+        <v>2</v>
       </c>
       <c r="AT23" s="24" t="b">
         <v>1</v>
@@ -5821,56 +5849,55 @@
       <c r="AU23" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV23" s="24">
+      <c r="AV23" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW23" s="24">
         <v>23</v>
       </c>
-      <c r="AW23" s="24">
+      <c r="AX23" s="24">
         <v>0.7</v>
       </c>
-      <c r="AX23" s="61" t="s">
+      <c r="AY23" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="AY23" s="60" t="s">
+      <c r="AZ23" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="AZ23" s="42">
+      <c r="BA23" s="41">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BA23" s="41">
+      <c r="BB23" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB23" s="40">
+      <c r="BC23" s="39">
         <v>425</v>
       </c>
-      <c r="BC23" s="114">
+      <c r="BD23" s="112">
         <v>455</v>
       </c>
-      <c r="BD23" s="59">
+      <c r="BE23" s="58">
         <v>3.2</v>
       </c>
-      <c r="BE23" s="59">
+      <c r="BF23" s="58">
         <v>9.5</v>
       </c>
-      <c r="BF23" s="59">
+      <c r="BG23" s="58">
         <v>1.7</v>
       </c>
-      <c r="BG23" s="59">
+      <c r="BH23" s="58">
         <v>0.5</v>
       </c>
-      <c r="BH23" s="59">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.35</v>
-      </c>
-      <c r="BI23" s="59">
+      <c r="BI23" s="58">
         <v>1.2</v>
       </c>
-      <c r="BJ23" s="59">
+      <c r="BJ23" s="58">
         <v>45</v>
       </c>
-      <c r="BK23" s="59">
+      <c r="BK23" s="58">
         <v>15</v>
       </c>
-      <c r="BL23" s="38" t="s">
+      <c r="BL23" s="37" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5878,192 +5905,192 @@
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="D24" s="101" t="s">
+      <c r="D24" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="98">
+      <c r="E24" s="97">
         <v>8</v>
       </c>
-      <c r="F24" s="102" t="s">
+      <c r="F24" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="112">
+      <c r="G24" s="110">
         <v>1800000</v>
       </c>
       <c r="H24" s="22">
         <v>800</v>
       </c>
-      <c r="I24" s="55">
+      <c r="I24" s="54">
         <v>35</v>
       </c>
-      <c r="J24" s="67">
+      <c r="J24" s="66">
         <v>45</v>
       </c>
-      <c r="K24" s="105">
+      <c r="K24" s="104">
         <v>17</v>
       </c>
-      <c r="L24" s="106">
+      <c r="L24" s="105">
         <v>0</v>
       </c>
-      <c r="M24" s="46">
+      <c r="M24" s="45">
         <v>360</v>
       </c>
-      <c r="N24" s="51">
+      <c r="N24" s="50">
         <v>430</v>
       </c>
-      <c r="O24" s="51">
+      <c r="O24" s="50">
         <v>2.2999999999999998</v>
       </c>
-      <c r="P24" s="51">
+      <c r="P24" s="50">
         <v>1</v>
       </c>
-      <c r="Q24" s="51">
+      <c r="Q24" s="50">
         <v>1.4E-2</v>
       </c>
-      <c r="R24" s="51">
+      <c r="R24" s="50">
         <v>25</v>
       </c>
-      <c r="S24" s="51">
+      <c r="S24" s="50">
         <v>0.7</v>
       </c>
-      <c r="T24" s="46">
+      <c r="T24" s="45">
         <v>1.7</v>
       </c>
-      <c r="U24" s="51">
+      <c r="U24" s="50">
         <v>2</v>
       </c>
-      <c r="V24" s="50">
+      <c r="V24" s="49">
         <v>25</v>
       </c>
-      <c r="W24" s="51">
+      <c r="W24" s="50">
         <v>1.8</v>
       </c>
-      <c r="X24" s="51">
+      <c r="X24" s="50">
         <v>100</v>
       </c>
-      <c r="Y24" s="51">
+      <c r="Y24" s="50">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z24" s="51">
+      <c r="Z24" s="50">
         <v>40</v>
       </c>
-      <c r="AA24" s="51">
+      <c r="AA24" s="50">
         <v>14</v>
       </c>
-      <c r="AB24" s="50">
+      <c r="AB24" s="49">
         <v>425</v>
       </c>
-      <c r="AC24" s="51">
+      <c r="AC24" s="50">
         <v>11.5</v>
       </c>
-      <c r="AD24" s="49">
+      <c r="AD24" s="48">
         <v>5</v>
       </c>
-      <c r="AE24" s="64">
+      <c r="AE24" s="63">
         <v>10</v>
       </c>
-      <c r="AF24" s="51">
+      <c r="AF24" s="50">
         <v>20000</v>
       </c>
-      <c r="AG24" s="110">
+      <c r="AG24" s="109">
         <v>4</v>
       </c>
-      <c r="AH24" s="111">
+      <c r="AH24" s="131">
         <v>0.06</v>
       </c>
-      <c r="AI24" s="62">
+      <c r="AI24" s="126">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>3.4999999999999996E-2</v>
+      </c>
+      <c r="AJ24" s="132">
         <v>0</v>
       </c>
-      <c r="AJ24" s="62">
+      <c r="AK24" s="61">
         <v>12</v>
       </c>
-      <c r="AK24" s="100" t="s">
+      <c r="AL24" s="99" t="s">
         <v>185</v>
       </c>
-      <c r="AL24" s="99" t="s">
+      <c r="AM24" s="98" t="s">
         <v>186</v>
       </c>
-      <c r="AM24" s="99" t="s">
+      <c r="AN24" s="98" t="s">
         <v>186</v>
       </c>
-      <c r="AN24" s="99" t="s">
+      <c r="AO24" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="AO24" s="99" t="s">
+      <c r="AP24" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="AP24" s="99">
+      <c r="AQ24" s="98">
         <v>1.3</v>
       </c>
-      <c r="AQ24" s="99">
+      <c r="AR24" s="98">
         <v>2</v>
       </c>
-      <c r="AR24" s="99">
+      <c r="AS24" s="98">
         <v>2</v>
       </c>
-      <c r="AS24" s="99" t="b">
+      <c r="AT24" s="98" t="b">
         <v>1</v>
       </c>
-      <c r="AT24" s="99" t="b">
+      <c r="AU24" s="98" t="b">
         <v>1</v>
       </c>
-      <c r="AU24" s="99" t="b">
+      <c r="AV24" s="98" t="b">
         <v>1</v>
       </c>
-      <c r="AV24" s="99">
+      <c r="AW24" s="98">
         <v>23</v>
       </c>
-      <c r="AW24" s="99">
+      <c r="AX24" s="98">
         <v>0.7</v>
       </c>
-      <c r="AX24" s="103" t="s">
+      <c r="AY24" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="AY24" s="21" t="s">
+      <c r="AZ24" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="AZ24" s="107">
+      <c r="BA24" s="106">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BA24" s="108">
+      <c r="BB24" s="107">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB24" s="109">
+      <c r="BC24" s="108">
         <v>440</v>
       </c>
-      <c r="BC24" s="115">
+      <c r="BD24" s="113">
         <v>495</v>
       </c>
-      <c r="BD24" s="104">
+      <c r="BE24" s="103">
         <v>3.4</v>
       </c>
-      <c r="BE24" s="104">
+      <c r="BF24" s="103">
         <v>9.5</v>
       </c>
-      <c r="BF24" s="104">
+      <c r="BG24" s="103">
         <v>1.7</v>
       </c>
-      <c r="BG24" s="104">
+      <c r="BH24" s="103">
         <v>0.6</v>
       </c>
-      <c r="BH24" s="104">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="BI24" s="104">
+      <c r="BI24" s="103">
         <v>1.2</v>
       </c>
-      <c r="BJ24" s="104">
+      <c r="BJ24" s="103">
         <v>45</v>
       </c>
-      <c r="BK24" s="104">
+      <c r="BK24" s="103">
         <v>15</v>
       </c>
-      <c r="BL24" s="101" t="s">
+      <c r="BL24" s="100" t="s">
         <v>184</v>
       </c>
     </row>
@@ -6071,37 +6098,37 @@
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="58">
+      <c r="E25" s="57">
         <v>9</v>
       </c>
-      <c r="F25" s="57" t="s">
+      <c r="F25" s="56" t="s">
         <v>184</v>
       </c>
       <c r="G25" s="30">
         <v>2900000</v>
       </c>
-      <c r="H25" s="56">
+      <c r="H25" s="55">
         <v>800</v>
       </c>
-      <c r="I25" s="55">
+      <c r="I25" s="54">
         <v>35</v>
       </c>
-      <c r="J25" s="67">
+      <c r="J25" s="66">
         <v>45</v>
       </c>
       <c r="K25" s="25">
         <v>10</v>
       </c>
-      <c r="L25" s="66">
+      <c r="L25" s="65">
         <v>0</v>
       </c>
-      <c r="M25" s="65">
+      <c r="M25" s="64">
         <v>375</v>
       </c>
       <c r="N25" s="26">
@@ -6116,19 +6143,19 @@
       <c r="Q25" s="29">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="R25" s="51">
+      <c r="R25" s="50">
         <v>25</v>
       </c>
-      <c r="S25" s="51">
+      <c r="S25" s="50">
         <v>0.7</v>
       </c>
-      <c r="T25" s="47">
+      <c r="T25" s="46">
         <v>1.37</v>
       </c>
       <c r="U25" s="26">
         <v>1.57</v>
       </c>
-      <c r="V25" s="50">
+      <c r="V25" s="49">
         <v>28</v>
       </c>
       <c r="W25" s="29">
@@ -6147,59 +6174,60 @@
       <c r="AA25" s="26">
         <v>34</v>
       </c>
-      <c r="AB25" s="50">
+      <c r="AB25" s="49">
         <v>450</v>
       </c>
-      <c r="AC25" s="51">
+      <c r="AC25" s="50">
         <v>11.5</v>
       </c>
       <c r="AD25" s="26">
         <v>5</v>
       </c>
-      <c r="AE25" s="64">
+      <c r="AE25" s="63">
         <v>10</v>
       </c>
       <c r="AF25" s="29">
         <v>20000</v>
       </c>
-      <c r="AG25" s="63">
+      <c r="AG25" s="62">
         <v>4</v>
       </c>
-      <c r="AH25" s="47">
+      <c r="AH25" s="130">
         <v>0.06</v>
       </c>
-      <c r="AI25" s="62">
+      <c r="AI25" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>3.4999999999999996E-2</v>
+      </c>
+      <c r="AJ25" s="132">
         <v>0</v>
       </c>
-      <c r="AJ25" s="62">
+      <c r="AK25" s="61">
         <v>12</v>
       </c>
-      <c r="AK25" s="45" t="s">
+      <c r="AL25" s="44" t="s">
         <v>83</v>
-      </c>
-      <c r="AL25" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="AM25" s="24" t="s">
         <v>82</v>
       </c>
       <c r="AN25" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO25" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AO25" s="24" t="s">
+      <c r="AP25" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="AP25" s="24">
+      <c r="AQ25" s="24">
         <v>1.2</v>
-      </c>
-      <c r="AQ25" s="24">
-        <v>2</v>
       </c>
       <c r="AR25" s="24">
         <v>2</v>
       </c>
-      <c r="AS25" s="24" t="b">
-        <v>1</v>
+      <c r="AS25" s="24">
+        <v>2</v>
       </c>
       <c r="AT25" s="24" t="b">
         <v>1</v>
@@ -6207,57 +6235,56 @@
       <c r="AU25" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV25" s="24">
+      <c r="AV25" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW25" s="24">
         <v>23</v>
       </c>
-      <c r="AW25" s="24">
+      <c r="AX25" s="24">
         <v>0.7</v>
       </c>
-      <c r="AX25" s="61" t="s">
+      <c r="AY25" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="AY25" s="60" t="s">
+      <c r="AZ25" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="AZ25" s="42">
+      <c r="BA25" s="41">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BA25" s="41">
+      <c r="BB25" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB25" s="40">
+      <c r="BC25" s="39">
         <v>540</v>
       </c>
-      <c r="BC25" s="114">
+      <c r="BD25" s="112">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>590</v>
       </c>
-      <c r="BD25" s="59">
+      <c r="BE25" s="58">
         <v>3.9</v>
       </c>
-      <c r="BE25" s="59">
+      <c r="BF25" s="58">
         <v>9.5</v>
       </c>
-      <c r="BF25" s="59">
+      <c r="BG25" s="58">
         <v>1.7</v>
       </c>
-      <c r="BG25" s="59">
+      <c r="BH25" s="58">
         <v>0.3</v>
       </c>
-      <c r="BH25" s="59">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>0.15</v>
-      </c>
-      <c r="BI25" s="59">
+      <c r="BI25" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BJ25" s="59">
+      <c r="BJ25" s="58">
         <v>45</v>
       </c>
-      <c r="BK25" s="59">
+      <c r="BK25" s="58">
         <v>15</v>
       </c>
-      <c r="BL25" s="38" t="s">
+      <c r="BL25" s="37" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6265,37 +6292,37 @@
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="58">
+      <c r="E26" s="57">
         <v>10</v>
       </c>
-      <c r="F26" s="57" t="s">
+      <c r="F26" s="56" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="30">
         <v>4300000</v>
       </c>
-      <c r="H26" s="56">
+      <c r="H26" s="55">
         <v>1100</v>
       </c>
-      <c r="I26" s="55">
+      <c r="I26" s="54">
         <v>35</v>
       </c>
-      <c r="J26" s="54">
+      <c r="J26" s="53">
         <v>45</v>
       </c>
       <c r="K26" s="25">
         <v>25</v>
       </c>
-      <c r="L26" s="53">
+      <c r="L26" s="52">
         <v>0</v>
       </c>
-      <c r="M26" s="52">
+      <c r="M26" s="51">
         <v>425</v>
       </c>
       <c r="N26" s="26">
@@ -6310,19 +6337,19 @@
       <c r="Q26" s="29">
         <v>1.6E-2</v>
       </c>
-      <c r="R26" s="51">
+      <c r="R26" s="50">
         <v>20</v>
       </c>
-      <c r="S26" s="51">
+      <c r="S26" s="50">
         <v>0.8</v>
       </c>
-      <c r="T26" s="47">
+      <c r="T26" s="46">
         <v>2</v>
       </c>
       <c r="U26" s="26">
         <v>2.1</v>
       </c>
-      <c r="V26" s="50">
+      <c r="V26" s="49">
         <v>31</v>
       </c>
       <c r="W26" s="26">
@@ -6341,59 +6368,60 @@
       <c r="AA26" s="26">
         <v>34</v>
       </c>
-      <c r="AB26" s="50">
+      <c r="AB26" s="49">
         <v>475</v>
       </c>
-      <c r="AC26" s="49">
+      <c r="AC26" s="48">
         <v>12</v>
       </c>
       <c r="AD26" s="26">
         <v>6</v>
       </c>
-      <c r="AE26" s="49">
+      <c r="AE26" s="48">
         <v>10</v>
       </c>
       <c r="AF26" s="26">
         <v>30000</v>
       </c>
-      <c r="AG26" s="48">
+      <c r="AG26" s="47">
         <v>5</v>
       </c>
-      <c r="AH26" s="47">
+      <c r="AH26" s="130">
         <v>0.05</v>
       </c>
-      <c r="AI26" s="46">
+      <c r="AI26" s="67">
+        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AJ26" s="74">
         <v>0</v>
       </c>
-      <c r="AJ26" s="46">
+      <c r="AK26" s="45">
         <v>12</v>
       </c>
-      <c r="AK26" s="45" t="s">
+      <c r="AL26" s="44" t="s">
         <v>78</v>
-      </c>
-      <c r="AL26" s="24" t="s">
-        <v>77</v>
       </c>
       <c r="AM26" s="24" t="s">
         <v>77</v>
       </c>
       <c r="AN26" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO26" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AO26" s="24" t="s">
+      <c r="AP26" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AP26" s="24">
+      <c r="AQ26" s="24">
         <v>1.1000000000000001</v>
-      </c>
-      <c r="AQ26" s="24">
-        <v>2</v>
       </c>
       <c r="AR26" s="24">
         <v>2</v>
       </c>
-      <c r="AS26" s="24" t="b">
-        <v>1</v>
+      <c r="AS26" s="24">
+        <v>2</v>
       </c>
       <c r="AT26" s="24" t="b">
         <v>1</v>
@@ -6401,57 +6429,56 @@
       <c r="AU26" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AV26" s="24">
+      <c r="AV26" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW26" s="24">
         <v>23</v>
       </c>
-      <c r="AW26" s="24">
+      <c r="AX26" s="24">
         <v>0.75</v>
       </c>
-      <c r="AX26" s="44" t="s">
+      <c r="AY26" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="AY26" s="43" t="s">
+      <c r="AZ26" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="AZ26" s="42">
+      <c r="BA26" s="41">
         <v>1.5E-3</v>
       </c>
-      <c r="BA26" s="41">
+      <c r="BB26" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BB26" s="40">
+      <c r="BC26" s="39">
         <v>680</v>
       </c>
-      <c r="BC26" s="116">
+      <c r="BD26" s="114">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>730</v>
       </c>
-      <c r="BD26" s="39">
+      <c r="BE26" s="38">
         <v>4.7</v>
       </c>
-      <c r="BE26" s="39">
+      <c r="BF26" s="38">
         <v>9.5</v>
       </c>
-      <c r="BF26" s="39">
+      <c r="BG26" s="38">
         <v>1.7</v>
       </c>
-      <c r="BG26" s="39">
+      <c r="BH26" s="38">
         <v>0.2</v>
       </c>
-      <c r="BH26" s="39">
-        <f>dragonDefinitions[[#This Row],['[airGravityModifierMin']]]-0.15</f>
-        <v>5.0000000000000017E-2</v>
-      </c>
-      <c r="BI26" s="39">
+      <c r="BI26" s="38">
         <v>0.15</v>
       </c>
-      <c r="BJ26" s="39">
+      <c r="BJ26" s="38">
         <v>59</v>
       </c>
-      <c r="BK26" s="39">
+      <c r="BK26" s="38">
         <v>15</v>
       </c>
-      <c r="BL26" s="38" t="s">
+      <c r="BL26" s="37" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6463,55 +6490,55 @@
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="119" t="s">
+      <c r="I27" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="120"/>
-      <c r="K27" s="120"/>
-      <c r="L27" s="121"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="124" t="s">
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="119"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="O27" s="124"/>
-      <c r="P27" s="124"/>
-      <c r="Q27" s="124"/>
-      <c r="R27" s="124"/>
-      <c r="S27" s="125"/>
-      <c r="T27" s="123" t="s">
+      <c r="O27" s="122"/>
+      <c r="P27" s="122"/>
+      <c r="Q27" s="122"/>
+      <c r="R27" s="122"/>
+      <c r="S27" s="123"/>
+      <c r="T27" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="U27" s="123"/>
-      <c r="V27" s="36" t="s">
+      <c r="U27" s="121"/>
+      <c r="V27" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W27" s="122" t="s">
+      <c r="W27" s="120" t="s">
         <v>70</v>
       </c>
-      <c r="X27" s="122"/>
-      <c r="Y27" s="122"/>
-      <c r="Z27" s="122"/>
-      <c r="AA27" s="122"/>
-      <c r="AB27" s="126" t="s">
+      <c r="X27" s="120"/>
+      <c r="Y27" s="120"/>
+      <c r="Z27" s="120"/>
+      <c r="AA27" s="120"/>
+      <c r="AB27" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="AC27" s="126"/>
-      <c r="AD27" s="126"/>
-      <c r="AE27" s="126"/>
-      <c r="AF27" s="127"/>
-      <c r="AH27" s="35" t="s">
+      <c r="AC27" s="124"/>
+      <c r="AD27" s="124"/>
+      <c r="AE27" s="124"/>
+      <c r="AF27" s="125"/>
+      <c r="AH27" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="AI27" s="34"/>
-      <c r="BA27" s="117" t="s">
+      <c r="AI27" s="128"/>
+      <c r="BC27" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="BB27" s="117"/>
-      <c r="BC27" s="117"/>
-      <c r="BD27" s="117"/>
-      <c r="BE27" s="117"/>
-      <c r="BF27" s="117"/>
-      <c r="BH27"/>
+      <c r="BD27" s="115"/>
+      <c r="BE27" s="115"/>
+      <c r="BF27" s="115"/>
+      <c r="BG27" s="115"/>
+      <c r="BH27" s="115"/>
+      <c r="BI27" s="115"/>
     </row>
     <row r="29" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">
@@ -7326,61 +7353,61 @@
       <c r="D53">
         <v>20</v>
       </c>
-      <c r="E53" s="113">
+      <c r="E53" s="111">
         <v>2940</v>
       </c>
-      <c r="F53" s="113">
+      <c r="F53" s="111">
         <v>8821</v>
       </c>
-      <c r="G53" s="113">
+      <c r="G53" s="111">
         <v>17642</v>
       </c>
-      <c r="H53" s="113">
+      <c r="H53" s="111">
         <v>29403</v>
       </c>
-      <c r="I53" s="113">
+      <c r="I53" s="111">
         <v>44105</v>
       </c>
-      <c r="J53" s="113">
+      <c r="J53" s="111">
         <v>61747</v>
       </c>
-      <c r="K53" s="113">
+      <c r="K53" s="111">
         <v>82329</v>
       </c>
-      <c r="L53" s="113">
+      <c r="L53" s="111">
         <v>105851</v>
       </c>
-      <c r="M53" s="113">
+      <c r="M53" s="111">
         <v>132314</v>
       </c>
-      <c r="N53" s="113">
+      <c r="N53" s="111">
         <v>161717</v>
       </c>
-      <c r="O53" s="113">
+      <c r="O53" s="111">
         <v>194061</v>
       </c>
-      <c r="P53" s="113">
+      <c r="P53" s="111">
         <v>229345</v>
       </c>
-      <c r="Q53" s="113">
+      <c r="Q53" s="111">
         <v>267569</v>
       </c>
-      <c r="R53" s="113">
+      <c r="R53" s="111">
         <v>308733</v>
       </c>
-      <c r="S53" s="113">
+      <c r="S53" s="111">
         <v>352838</v>
       </c>
-      <c r="T53" s="113">
+      <c r="T53" s="111">
         <v>399883</v>
       </c>
-      <c r="U53" s="113">
+      <c r="U53" s="111">
         <v>449868</v>
       </c>
-      <c r="V53" s="113">
+      <c r="V53" s="111">
         <v>502794</v>
       </c>
-      <c r="W53" s="113">
+      <c r="W53" s="111">
         <v>558660</v>
       </c>
     </row>
@@ -7521,29 +7548,30 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="BA27:BF27"/>
+  <mergeCells count="8">
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="I27:L27"/>
     <mergeCell ref="T27:U27"/>
     <mergeCell ref="N27:S27"/>
     <mergeCell ref="W27:AA27"/>
     <mergeCell ref="AB27:AF27"/>
+    <mergeCell ref="AH27:AI27"/>
+    <mergeCell ref="BC27:BI27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL16:BL23 BL25:BL26">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL24">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">

</xml_diff>

<commit_message>
Setting values for eatSpeedFactor
Former-commit-id: 931848d087a2d6a8ad4c963a27c6ca6fe5c576d0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1470,167 +1470,65 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="99">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2787,6 +2685,34 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2974,6 +2900,30 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3510,6 +3460,56 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3524,97 +3524,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BL26" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BL26" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90" totalsRowBorderDxfId="89">
   <autoFilter ref="B15:BL26"/>
   <tableColumns count="63">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="93"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="92"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="91"/>
-    <tableColumn id="3" name="[order]" dataDxfId="90"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="89"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="88"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="87"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="86"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="85"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="84"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="83"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="82"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="81"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="80"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="79"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="78"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="77"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="76"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="75"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="74"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="73"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="72"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="71"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="6">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="88"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="86"/>
+    <tableColumn id="3" name="[order]" dataDxfId="85"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="84"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="83"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="82"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="81"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="80"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="79"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="78"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="77"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="76"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="75"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="74"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="73"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="72"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="71"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="70"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="69"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="68"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="67"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="66"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="65">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="70"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="69"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="68"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="67"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="66"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="65"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="64"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="63"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="62"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="5">
-      <calculatedColumnFormula>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</calculatedColumnFormula>
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="64"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="63"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="62"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="61"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="60"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="59"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="58"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="57"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="56"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="55">
+      <calculatedColumnFormula>AH17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="61"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="60"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="59"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="58"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="57"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="56"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="55"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="54"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="53"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="52"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="51"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="50"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="49"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="48"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="47"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="46">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="54"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="53"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="52"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="51"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="50"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="49"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="48"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="47"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="46"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="45"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="44"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="43"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="42"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="41"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="40"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="39">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="45">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="38">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="44"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="43"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="42"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="41">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="37"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="36"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="35"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="34">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="40"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="39"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="38"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="37"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="36"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="35"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="34"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="33"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="33"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="32"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="31"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="30"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="29"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="28"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="27"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="28"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="27"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="26"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="25">
+    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="18">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3623,11 +3623,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B32:I33"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="20"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="19"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3640,7 +3640,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B44:W55"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3671,14 +3671,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B37:F40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="10"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="9"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="8"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="7"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3952,8 +3952,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
-      <selection activeCell="BB29" sqref="BB29"/>
+    <sheetView tabSelected="1" topLeftCell="W10" workbookViewId="0">
+      <selection activeCell="AJ28" sqref="AJ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4191,10 +4191,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="116"/>
-      <c r="AP14" s="116"/>
-      <c r="AQ14" s="116"/>
-      <c r="AR14" s="116"/>
+      <c r="AO14" s="121"/>
+      <c r="AP14" s="121"/>
+      <c r="AQ14" s="121"/>
+      <c r="AR14" s="121"/>
     </row>
     <row r="15" spans="2:64" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="75" t="s">
@@ -4287,7 +4287,7 @@
       <c r="AE15" s="87" t="s">
         <v>146</v>
       </c>
-      <c r="AF15" s="127" t="s">
+      <c r="AF15" s="116" t="s">
         <v>145</v>
       </c>
       <c r="AG15" s="86" t="s">
@@ -4483,12 +4483,12 @@
       <c r="AG16" s="67">
         <v>1</v>
       </c>
-      <c r="AH16" s="129">
+      <c r="AH16" s="117">
         <v>0.23</v>
       </c>
       <c r="AI16" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>0.20500000000000002</v>
+        <f t="shared" ref="AI16:AI25" si="0">AH17</f>
+        <v>0.19</v>
       </c>
       <c r="AJ16" s="74">
         <v>0</v>
@@ -4672,12 +4672,12 @@
       <c r="AG17" s="67">
         <v>2</v>
       </c>
-      <c r="AH17" s="129">
+      <c r="AH17" s="117">
         <v>0.19</v>
       </c>
       <c r="AI17" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>0.16500000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.15</v>
       </c>
       <c r="AJ17" s="74">
         <v>0</v>
@@ -4861,14 +4861,14 @@
       <c r="AG18" s="62">
         <v>2</v>
       </c>
-      <c r="AH18" s="130">
+      <c r="AH18" s="118">
         <v>0.15</v>
       </c>
       <c r="AI18" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>0.125</v>
-      </c>
-      <c r="AJ18" s="132">
+        <f t="shared" si="0"/>
+        <v>0.13</v>
+      </c>
+      <c r="AJ18" s="120">
         <v>0</v>
       </c>
       <c r="AK18" s="61">
@@ -5050,12 +5050,12 @@
       <c r="AG19" s="67">
         <v>2</v>
       </c>
-      <c r="AH19" s="129">
+      <c r="AH19" s="117">
         <v>0.13</v>
       </c>
       <c r="AI19" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>0.10500000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.11</v>
       </c>
       <c r="AJ19" s="74">
         <v>0</v>
@@ -5239,12 +5239,12 @@
       <c r="AG20" s="67">
         <v>3</v>
       </c>
-      <c r="AH20" s="129">
+      <c r="AH20" s="117">
         <v>0.11</v>
       </c>
       <c r="AI20" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>8.4999999999999992E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.09</v>
       </c>
       <c r="AJ20" s="74">
         <v>0</v>
@@ -5428,12 +5428,12 @@
       <c r="AG21" s="67">
         <v>3</v>
       </c>
-      <c r="AH21" s="129">
+      <c r="AH21" s="117">
         <v>0.09</v>
       </c>
       <c r="AI21" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.08</v>
       </c>
       <c r="AJ21" s="74">
         <v>0</v>
@@ -5617,12 +5617,12 @@
       <c r="AG22" s="67">
         <v>3</v>
       </c>
-      <c r="AH22" s="129">
+      <c r="AH22" s="117">
         <v>0.08</v>
       </c>
       <c r="AI22" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>5.5E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ22" s="74">
         <v>0</v>
@@ -5806,14 +5806,14 @@
       <c r="AG23" s="62">
         <v>4</v>
       </c>
-      <c r="AH23" s="130">
+      <c r="AH23" s="118">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI23" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>4.5000000000000005E-2</v>
-      </c>
-      <c r="AJ23" s="132">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="AJ23" s="120">
         <v>0</v>
       </c>
       <c r="AK23" s="61">
@@ -5999,14 +5999,13 @@
       <c r="AG24" s="109">
         <v>4</v>
       </c>
-      <c r="AH24" s="131">
+      <c r="AH24" s="119">
         <v>0.06</v>
       </c>
-      <c r="AI24" s="126">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>3.4999999999999996E-2</v>
-      </c>
-      <c r="AJ24" s="132">
+      <c r="AI24" s="115">
+        <v>0.05</v>
+      </c>
+      <c r="AJ24" s="120">
         <v>0</v>
       </c>
       <c r="AK24" s="61">
@@ -6192,14 +6191,14 @@
       <c r="AG25" s="62">
         <v>4</v>
       </c>
-      <c r="AH25" s="130">
+      <c r="AH25" s="118">
         <v>0.06</v>
       </c>
       <c r="AI25" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>3.4999999999999996E-2</v>
-      </c>
-      <c r="AJ25" s="132">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="AJ25" s="120">
         <v>0</v>
       </c>
       <c r="AK25" s="61">
@@ -6386,12 +6385,11 @@
       <c r="AG26" s="47">
         <v>5</v>
       </c>
-      <c r="AH26" s="130">
+      <c r="AH26" s="118">
         <v>0.05</v>
       </c>
       <c r="AI26" s="67">
-        <f>dragonDefinitions[[#This Row],['[eatSpeedFactorMin']]]-0.025</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="AJ26" s="74">
         <v>0</v>
@@ -6490,55 +6488,55 @@
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="117" t="s">
+      <c r="I27" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="119"/>
+      <c r="J27" s="123"/>
+      <c r="K27" s="123"/>
+      <c r="L27" s="124"/>
       <c r="M27" s="36"/>
-      <c r="N27" s="122" t="s">
+      <c r="N27" s="126" t="s">
         <v>73</v>
       </c>
-      <c r="O27" s="122"/>
-      <c r="P27" s="122"/>
-      <c r="Q27" s="122"/>
-      <c r="R27" s="122"/>
-      <c r="S27" s="123"/>
-      <c r="T27" s="121" t="s">
+      <c r="O27" s="126"/>
+      <c r="P27" s="126"/>
+      <c r="Q27" s="126"/>
+      <c r="R27" s="126"/>
+      <c r="S27" s="127"/>
+      <c r="T27" s="125" t="s">
         <v>72</v>
       </c>
-      <c r="U27" s="121"/>
+      <c r="U27" s="125"/>
       <c r="V27" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W27" s="120" t="s">
+      <c r="W27" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="X27" s="120"/>
-      <c r="Y27" s="120"/>
-      <c r="Z27" s="120"/>
-      <c r="AA27" s="120"/>
-      <c r="AB27" s="124" t="s">
+      <c r="X27" s="128"/>
+      <c r="Y27" s="128"/>
+      <c r="Z27" s="128"/>
+      <c r="AA27" s="128"/>
+      <c r="AB27" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="AC27" s="124"/>
-      <c r="AD27" s="124"/>
-      <c r="AE27" s="124"/>
-      <c r="AF27" s="125"/>
-      <c r="AH27" s="128" t="s">
+      <c r="AC27" s="129"/>
+      <c r="AD27" s="129"/>
+      <c r="AE27" s="129"/>
+      <c r="AF27" s="130"/>
+      <c r="AH27" s="131" t="s">
         <v>68</v>
       </c>
-      <c r="AI27" s="128"/>
-      <c r="BC27" s="115" t="s">
+      <c r="AI27" s="131"/>
+      <c r="BC27" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="BD27" s="115"/>
-      <c r="BE27" s="115"/>
-      <c r="BF27" s="115"/>
-      <c r="BG27" s="115"/>
-      <c r="BH27" s="115"/>
-      <c r="BI27" s="115"/>
+      <c r="BD27" s="132"/>
+      <c r="BE27" s="132"/>
+      <c r="BF27" s="132"/>
+      <c r="BG27" s="132"/>
+      <c r="BH27" s="132"/>
+      <c r="BI27" s="132"/>
     </row>
     <row r="29" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">
@@ -7549,6 +7547,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="BC27:BI27"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="I27:L27"/>
     <mergeCell ref="T27:U27"/>
@@ -7556,22 +7555,21 @@
     <mergeCell ref="W27:AA27"/>
     <mergeCell ref="AB27:AF27"/>
     <mergeCell ref="AH27:AI27"/>
-    <mergeCell ref="BC27:BI27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL16:BL23 BL25:BL26">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL24">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">

</xml_diff>

<commit_message>
Setting scale max values
Former-commit-id: d665a4ebea0709bf648786e96a1b5cef0bc953bf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1488,6 +1488,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1519,9 +1522,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3952,8 +3952,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W10" workbookViewId="0">
-      <selection activeCell="AJ28" sqref="AJ28"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4191,10 +4191,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="121"/>
-      <c r="AP14" s="121"/>
-      <c r="AQ14" s="121"/>
-      <c r="AR14" s="121"/>
+      <c r="AO14" s="122"/>
+      <c r="AP14" s="122"/>
+      <c r="AQ14" s="122"/>
+      <c r="AR14" s="122"/>
     </row>
     <row r="15" spans="2:64" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="75" t="s">
@@ -4444,7 +4444,7 @@
         <v>0.46</v>
       </c>
       <c r="U16" s="29">
-        <v>0.76</v>
+        <v>0.66</v>
       </c>
       <c r="V16" s="68">
         <v>14</v>
@@ -4633,7 +4633,7 @@
         <v>0.8</v>
       </c>
       <c r="U17" s="26">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="V17" s="68">
         <v>16</v>
@@ -4822,7 +4822,7 @@
         <v>0.85</v>
       </c>
       <c r="U18" s="29">
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V18" s="49">
         <v>23.5</v>
@@ -5011,7 +5011,7 @@
         <v>0.9</v>
       </c>
       <c r="U19" s="26">
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V19" s="68">
         <v>19</v>
@@ -5200,7 +5200,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="29">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="V20" s="68">
         <v>20</v>
@@ -6488,55 +6488,55 @@
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="122" t="s">
+      <c r="I27" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="123"/>
-      <c r="K27" s="123"/>
-      <c r="L27" s="124"/>
+      <c r="J27" s="124"/>
+      <c r="K27" s="124"/>
+      <c r="L27" s="125"/>
       <c r="M27" s="36"/>
-      <c r="N27" s="126" t="s">
+      <c r="N27" s="127" t="s">
         <v>73</v>
       </c>
-      <c r="O27" s="126"/>
-      <c r="P27" s="126"/>
-      <c r="Q27" s="126"/>
-      <c r="R27" s="126"/>
-      <c r="S27" s="127"/>
-      <c r="T27" s="125" t="s">
+      <c r="O27" s="127"/>
+      <c r="P27" s="127"/>
+      <c r="Q27" s="127"/>
+      <c r="R27" s="127"/>
+      <c r="S27" s="128"/>
+      <c r="T27" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="U27" s="125"/>
+      <c r="U27" s="126"/>
       <c r="V27" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W27" s="128" t="s">
+      <c r="W27" s="129" t="s">
         <v>70</v>
       </c>
-      <c r="X27" s="128"/>
-      <c r="Y27" s="128"/>
-      <c r="Z27" s="128"/>
-      <c r="AA27" s="128"/>
-      <c r="AB27" s="129" t="s">
+      <c r="X27" s="129"/>
+      <c r="Y27" s="129"/>
+      <c r="Z27" s="129"/>
+      <c r="AA27" s="129"/>
+      <c r="AB27" s="130" t="s">
         <v>69</v>
       </c>
-      <c r="AC27" s="129"/>
-      <c r="AD27" s="129"/>
-      <c r="AE27" s="129"/>
-      <c r="AF27" s="130"/>
-      <c r="AH27" s="131" t="s">
+      <c r="AC27" s="130"/>
+      <c r="AD27" s="130"/>
+      <c r="AE27" s="130"/>
+      <c r="AF27" s="131"/>
+      <c r="AH27" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="AI27" s="131"/>
-      <c r="BC27" s="132" t="s">
+      <c r="AI27" s="132"/>
+      <c r="BC27" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="BD27" s="132"/>
-      <c r="BE27" s="132"/>
-      <c r="BF27" s="132"/>
-      <c r="BG27" s="132"/>
-      <c r="BH27" s="132"/>
-      <c r="BI27" s="132"/>
+      <c r="BD27" s="121"/>
+      <c r="BE27" s="121"/>
+      <c r="BF27" s="121"/>
+      <c r="BG27" s="121"/>
+      <c r="BH27" s="121"/>
+      <c r="BI27" s="121"/>
     </row>
     <row r="29" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
dot threshold increased from 6 to 8 for some dragons
Former-commit-id: 0fa8aa628b794e981e3952fb3b7d256a8b2ed05f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3952,8 +3952,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
+      <selection activeCell="BK29" sqref="BK29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4568,7 +4568,7 @@
         <v>0</v>
       </c>
       <c r="BK16" s="73">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BL16" s="58" t="s">
         <v>5</v>
@@ -4757,7 +4757,7 @@
         <v>0</v>
       </c>
       <c r="BK17" s="58">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BL17" s="58" t="s">
         <v>6</v>
@@ -4946,7 +4946,7 @@
         <v>0</v>
       </c>
       <c r="BK18" s="58">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BL18" s="37" t="s">
         <v>7</v>
@@ -5135,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="BK19" s="58">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BL19" s="37" t="s">
         <v>8</v>
@@ -5324,7 +5324,7 @@
         <v>9</v>
       </c>
       <c r="BK20" s="58">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BL20" s="37" t="s">
         <v>9</v>
@@ -5513,7 +5513,7 @@
         <v>9</v>
       </c>
       <c r="BK21" s="58">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BL21" s="37" t="s">
         <v>10</v>
@@ -5702,7 +5702,7 @@
         <v>9</v>
       </c>
       <c r="BK22" s="58">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BL22" s="37" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Dragon Titan: fix water and air gravity. They were too low, making dragon almost not affected by gravity. To fix this, also some 'boost' parameters have been modified
Former-commit-id: f803fcbf315049ab70d8d53a1a0684054fbfec37
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3952,8 +3952,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO10" workbookViewId="0">
-      <selection activeCell="BA30" sqref="BA30"/>
+    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
+      <selection activeCell="BC27" sqref="BC27:BI27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6352,7 +6352,7 @@
         <v>31</v>
       </c>
       <c r="W26" s="26">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="X26" s="26">
         <v>100</v>
@@ -6362,10 +6362,10 @@
         <v>125</v>
       </c>
       <c r="Z26" s="26">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="AA26" s="26">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="AB26" s="49">
         <v>475</v>
@@ -6465,10 +6465,10 @@
         <v>1.7</v>
       </c>
       <c r="BH26" s="38">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="BI26" s="38">
-        <v>0.15</v>
+        <v>1.03</v>
       </c>
       <c r="BJ26" s="38">
         <v>59</v>

</xml_diff>

<commit_message>
I forgot to update [energyRefillRate]
Former-commit-id: 761993bfa9da5c50bb8f833e2add34137c872472
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3952,8 +3952,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
-      <selection activeCell="BC27" sqref="BC27:BI27"/>
+    <sheetView tabSelected="1" topLeftCell="O10" workbookViewId="0">
+      <selection activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6365,7 +6365,7 @@
         <v>19</v>
       </c>
       <c r="AA26" s="26">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AB26" s="49">
         <v>475</v>

</xml_diff>

<commit_message>
- TIDs added for level area - Dragons spin in space when falling and reach max speed - Dragon Fat space stats modified
Former-commit-id: a59f2e6ba315ef12b08ec9d01ada0f59b5f6905e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3952,8 +3952,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O10" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26"/>
+    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
+      <selection activeCell="BH19" sqref="BH19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5126,7 +5126,7 @@
         <v>0.5</v>
       </c>
       <c r="BH19" s="58">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="BI19" s="58">
         <v>1.3</v>

</xml_diff>

<commit_message>
Multiple stats upgrades available
Former-commit-id: e6443e717b42b99052edd3f55398df47d5a1653a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="221">
   <si>
     <t>[sku]</t>
   </si>
@@ -633,9 +633,6 @@
     <t>[percentage]</t>
   </si>
   <si>
-    <t>health</t>
-  </si>
-  <si>
     <t>mass</t>
   </si>
   <si>
@@ -685,6 +682,12 @@
   </si>
   <si>
     <t>En las escenas, poder añadir (y quitar?) spawners para los dragones especiales</t>
+  </si>
+  <si>
+    <t>health;mass;force;healthDrain</t>
+  </si>
+  <si>
+    <t>2;3;1;6</t>
   </si>
 </sst>
 </file>
@@ -1833,6 +1836,67 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1887,612 +1951,11 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="183">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
+  <dxfs count="182">
     <dxf>
       <font>
         <b val="0"/>
@@ -3012,23 +2475,543 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4385,6 +4368,16 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -6303,88 +6296,88 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BI26" totalsRowShown="0" headerRowDxfId="177" dataDxfId="175" headerRowBorderDxfId="176" tableBorderDxfId="174" totalsRowBorderDxfId="173">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BI26" totalsRowShown="0" headerRowDxfId="176" dataDxfId="174" headerRowBorderDxfId="175" tableBorderDxfId="173" totalsRowBorderDxfId="172">
   <autoFilter ref="B15:BI26"/>
   <tableColumns count="60">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="172"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="171"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="170"/>
-    <tableColumn id="3" name="[order]" dataDxfId="169"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="168"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="167"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="166"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="165"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="164"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="163"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="162"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="161"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="160"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="159"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="158"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="157"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="156"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="155"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="154"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="153"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="152"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="151"/>
-    <tableColumn id="41" name="[energyBase]" dataDxfId="150"/>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="149"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="148"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="147"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="146"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="145"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="144"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="143"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="142"/>
-    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="141"/>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="140"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="139"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="138"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="137"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="136"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="135"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="134"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="133"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="132"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="131"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="130"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="129"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="128"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="127"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="126"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="125">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="171"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="170"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="169"/>
+    <tableColumn id="3" name="[order]" dataDxfId="168"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="167"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="166"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="165"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="164"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="163"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="162"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="161"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="160"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="159"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="158"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="157"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="156"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="155"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="154"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="153"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="152"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="151"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="150"/>
+    <tableColumn id="41" name="[energyBase]" dataDxfId="149"/>
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="148"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="147"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="146"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="145"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="144"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="143"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="142"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="141"/>
+    <tableColumn id="14" name="[eatSpeedFactor]" dataDxfId="140"/>
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="139"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="138"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="137"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="136"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="135"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="134"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="133"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="132"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="131"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="130"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="129"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="128"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="127"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="126"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="125"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="124">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="124">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="123">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="123"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="122"/>
-    <tableColumn id="34" name="[force]" dataDxfId="121"/>
-    <tableColumn id="35" name="[mass]" dataDxfId="120"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="119"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="118"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="117"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="116"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="115"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="114"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="113"/>
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="122"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="121"/>
+    <tableColumn id="34" name="[force]" dataDxfId="120"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="119"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="118"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="117"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="116"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="115"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="114"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="113"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="112" headerRowBorderDxfId="111" tableBorderDxfId="110" totalsRowBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="111" headerRowBorderDxfId="110" tableBorderDxfId="109" totalsRowBorderDxfId="108">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="108"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="107"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="107"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="106"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="105">
+    <tableColumn id="10" name="[icon]" dataDxfId="106"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="105"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="104">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6393,11 +6386,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="104" headerRowBorderDxfId="103" tableBorderDxfId="102" totalsRowBorderDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="103" headerRowBorderDxfId="102" tableBorderDxfId="101" totalsRowBorderDxfId="100">
   <autoFilter ref="B32:I33"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="100"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="99"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="99"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="98"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -6410,7 +6403,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="98" headerRowBorderDxfId="97" tableBorderDxfId="96" totalsRowBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="97" headerRowBorderDxfId="96" tableBorderDxfId="95" totalsRowBorderDxfId="94">
   <autoFilter ref="B44:W55"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -6441,106 +6434,106 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93" tableBorderDxfId="92" totalsRowBorderDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
   <autoFilter ref="B37:F40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="90"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="89"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="89"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="88"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="87"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="87"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table6" displayName="Table6" ref="B19:G25" totalsRowShown="0" headerRowBorderDxfId="74" tableBorderDxfId="73" totalsRowBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table6" displayName="Table6" ref="B19:G25" totalsRowShown="0" headerRowBorderDxfId="72" tableBorderDxfId="71" totalsRowBorderDxfId="70">
   <autoFilter ref="B19:G25"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{specialDragonStatsUpgradeDefinitions}" dataDxfId="71"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="70"/>
-    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="69"/>
-    <tableColumn id="3" name="[unlockPricePC]" dataDxfId="68"/>
-    <tableColumn id="4" name="[stat]" dataDxfId="67"/>
-    <tableColumn id="5" name="[percentage]" dataDxfId="66"/>
+    <tableColumn id="1" name="{specialDragonStatsUpgradeDefinitions}" dataDxfId="69"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="68"/>
+    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="67"/>
+    <tableColumn id="3" name="[unlockPricePC]" dataDxfId="66"/>
+    <tableColumn id="4" name="[stat]" dataDxfId="65"/>
+    <tableColumn id="5" name="[percentage]" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table63" displayName="Table63" ref="B36:F42" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64" totalsRowBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table63" displayName="Table63" ref="B36:F42" totalsRowShown="0" headerRowBorderDxfId="63" tableBorderDxfId="62" totalsRowBorderDxfId="61">
   <autoFilter ref="B36:F42"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPetsUpgradeDefinitions}" dataDxfId="62"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="61"/>
-    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="60"/>
-    <tableColumn id="3" name="[unlockPricePC]" dataDxfId="59"/>
-    <tableColumn id="4" name="[maxPets]" dataDxfId="58"/>
+    <tableColumn id="1" name="{specialDragonPetsUpgradeDefinitions}" dataDxfId="60"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="59"/>
+    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="58"/>
+    <tableColumn id="3" name="[unlockPricePC]" dataDxfId="57"/>
+    <tableColumn id="4" name="[maxPets]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B6:BC12" totalsRowShown="0" headerRowBorderDxfId="57" totalsRowBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B6:BC12" totalsRowShown="0" headerRowBorderDxfId="55" totalsRowBorderDxfId="54">
   <autoFilter ref="B6:BC12"/>
   <tableColumns count="54">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="55"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="54"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="53"/>
-    <tableColumn id="4" name="[order]" dataDxfId="52"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="51"/>
-    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="50"/>
-    <tableColumn id="7" name="[unlockPricePC]" dataDxfId="49"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="48"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="47"/>
-    <tableColumn id="10" name="[health]" dataDxfId="46"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="45"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="44"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="43"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="42"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="41"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="40"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="39"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="38"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="37"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="36"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="35"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="34"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="33"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="32"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="31"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="30"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="29"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="0"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="13"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="12"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="11"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="10"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="9"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="8"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="7"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="6"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="5"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="4"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="3"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="2"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="1"/>
-    <tableColumn id="42" name="[tidName]" dataDxfId="26"/>
-    <tableColumn id="43" name="[tidDesc]" dataDxfId="25"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="24"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="23"/>
-    <tableColumn id="46" name="[force]" dataDxfId="22"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="21"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="20"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="19"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="18"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="17"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="16"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="15"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="14"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="53"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="51"/>
+    <tableColumn id="4" name="[order]" dataDxfId="50"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="49"/>
+    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="48"/>
+    <tableColumn id="7" name="[unlockPricePC]" dataDxfId="47"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="46"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="45"/>
+    <tableColumn id="10" name="[health]" dataDxfId="44"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="43"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="42"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="41"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="40"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="39"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="38"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="37"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="36"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="35"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="34"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="33"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="32"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="31"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="30"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="29"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="28"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="27"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="26"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="25"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="24"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="23"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="22"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="21"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="20"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="19"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="18"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="17"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="16"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="15"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="14"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="13"/>
+    <tableColumn id="42" name="[tidName]" dataDxfId="12"/>
+    <tableColumn id="43" name="[tidDesc]" dataDxfId="11"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="10"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="9"/>
+    <tableColumn id="46" name="[force]" dataDxfId="8"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="7"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="6"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="5"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="4"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="3"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="2"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="1"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7053,10 +7046,10 @@
       <c r="AG14" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="AO14" s="154"/>
-      <c r="AP14" s="154"/>
-      <c r="AQ14" s="154"/>
-      <c r="AR14" s="154"/>
+      <c r="AO14" s="175"/>
+      <c r="AP14" s="175"/>
+      <c r="AQ14" s="175"/>
+      <c r="AR14" s="175"/>
     </row>
     <row r="15" spans="2:61" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="76" t="s">
@@ -9220,55 +9213,55 @@
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="155" t="s">
+      <c r="I27" s="176" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="156"/>
-      <c r="K27" s="156"/>
-      <c r="L27" s="157"/>
+      <c r="J27" s="177"/>
+      <c r="K27" s="177"/>
+      <c r="L27" s="178"/>
       <c r="M27" s="37"/>
-      <c r="N27" s="161" t="s">
+      <c r="N27" s="182" t="s">
         <v>73</v>
       </c>
-      <c r="O27" s="161"/>
-      <c r="P27" s="161"/>
-      <c r="Q27" s="161"/>
-      <c r="R27" s="161"/>
-      <c r="S27" s="162"/>
-      <c r="T27" s="160" t="s">
+      <c r="O27" s="182"/>
+      <c r="P27" s="182"/>
+      <c r="Q27" s="182"/>
+      <c r="R27" s="182"/>
+      <c r="S27" s="183"/>
+      <c r="T27" s="181" t="s">
         <v>72</v>
       </c>
-      <c r="U27" s="160"/>
+      <c r="U27" s="181"/>
       <c r="V27" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="W27" s="158" t="s">
+      <c r="W27" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="X27" s="158"/>
-      <c r="Y27" s="158"/>
-      <c r="Z27" s="159"/>
-      <c r="AA27" s="163" t="s">
+      <c r="X27" s="179"/>
+      <c r="Y27" s="179"/>
+      <c r="Z27" s="180"/>
+      <c r="AA27" s="184" t="s">
         <v>69</v>
       </c>
-      <c r="AB27" s="164"/>
-      <c r="AC27" s="164"/>
-      <c r="AD27" s="164"/>
-      <c r="AE27" s="164"/>
-      <c r="AF27" s="165"/>
+      <c r="AB27" s="185"/>
+      <c r="AC27" s="185"/>
+      <c r="AD27" s="185"/>
+      <c r="AE27" s="185"/>
+      <c r="AF27" s="186"/>
       <c r="AG27" s="35" t="s">
         <v>68</v>
       </c>
       <c r="AH27" s="34"/>
       <c r="AI27" s="34"/>
-      <c r="BA27" s="153" t="s">
+      <c r="BA27" s="174" t="s">
         <v>67</v>
       </c>
-      <c r="BB27" s="153"/>
-      <c r="BC27" s="153"/>
-      <c r="BD27" s="153"/>
-      <c r="BE27" s="153"/>
-      <c r="BF27" s="153"/>
+      <c r="BB27" s="174"/>
+      <c r="BC27" s="174"/>
+      <c r="BD27" s="174"/>
+      <c r="BE27" s="174"/>
+      <c r="BF27" s="174"/>
       <c r="BH27"/>
     </row>
     <row r="29" spans="2:61" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -10289,19 +10282,19 @@
     <mergeCell ref="AA27:AF27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="182" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="181" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="181" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="180" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI16:BI23 BI25:BI26">
-    <cfRule type="duplicateValues" dxfId="180" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="179" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI24">
-    <cfRule type="duplicateValues" dxfId="178" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">
@@ -10332,8 +10325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BC42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6:R12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10372,14 +10365,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="F2" s="191" t="s">
-        <v>219</v>
+      <c r="F2" s="173" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:55" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -10518,76 +10511,76 @@
       <c r="AB6" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="AC6" s="186" t="s">
+      <c r="AC6" s="168" t="s">
         <v>143</v>
       </c>
-      <c r="AD6" s="178" t="s">
+      <c r="AD6" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="AE6" s="177" t="s">
+      <c r="AE6" s="159" t="s">
         <v>18</v>
       </c>
-      <c r="AF6" s="177" t="s">
+      <c r="AF6" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="AG6" s="177" t="s">
+      <c r="AG6" s="159" t="s">
         <v>141</v>
       </c>
-      <c r="AH6" s="177" t="s">
+      <c r="AH6" s="159" t="s">
         <v>140</v>
       </c>
-      <c r="AI6" s="177" t="s">
+      <c r="AI6" s="159" t="s">
         <v>139</v>
       </c>
-      <c r="AJ6" s="177" t="s">
+      <c r="AJ6" s="159" t="s">
         <v>138</v>
       </c>
-      <c r="AK6" s="177" t="s">
+      <c r="AK6" s="159" t="s">
         <v>137</v>
       </c>
-      <c r="AL6" s="177" t="s">
+      <c r="AL6" s="159" t="s">
         <v>136</v>
       </c>
-      <c r="AM6" s="177" t="s">
+      <c r="AM6" s="159" t="s">
         <v>135</v>
       </c>
-      <c r="AN6" s="177" t="s">
+      <c r="AN6" s="159" t="s">
         <v>134</v>
       </c>
-      <c r="AO6" s="177" t="s">
+      <c r="AO6" s="159" t="s">
         <v>133</v>
       </c>
-      <c r="AP6" s="183" t="s">
+      <c r="AP6" s="165" t="s">
         <v>132</v>
       </c>
-      <c r="AQ6" s="187" t="s">
+      <c r="AQ6" s="169" t="s">
         <v>4</v>
       </c>
-      <c r="AR6" s="189" t="s">
+      <c r="AR6" s="171" t="s">
         <v>16</v>
       </c>
-      <c r="AS6" s="188" t="s">
+      <c r="AS6" s="170" t="s">
         <v>131</v>
       </c>
-      <c r="AT6" s="190" t="s">
+      <c r="AT6" s="172" t="s">
         <v>130</v>
       </c>
-      <c r="AU6" s="180" t="s">
+      <c r="AU6" s="162" t="s">
         <v>129</v>
       </c>
-      <c r="AV6" s="179" t="s">
+      <c r="AV6" s="161" t="s">
         <v>128</v>
       </c>
-      <c r="AW6" s="179" t="s">
+      <c r="AW6" s="161" t="s">
         <v>127</v>
       </c>
-      <c r="AX6" s="179" t="s">
+      <c r="AX6" s="161" t="s">
         <v>126</v>
       </c>
-      <c r="AY6" s="179" t="s">
+      <c r="AY6" s="161" t="s">
         <v>125</v>
       </c>
-      <c r="AZ6" s="179" t="s">
+      <c r="AZ6" s="161" t="s">
         <v>124</v>
       </c>
       <c r="BA6" s="147" t="s">
@@ -10596,7 +10589,7 @@
       <c r="BB6" s="147" t="s">
         <v>122</v>
       </c>
-      <c r="BC6" s="179" t="s">
+      <c r="BC6" s="161" t="s">
         <v>2</v>
       </c>
     </row>
@@ -10605,7 +10598,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D7" s="59" t="s">
         <v>107</v>
@@ -10682,10 +10675,10 @@
       <c r="AB7" s="132">
         <v>0</v>
       </c>
-      <c r="AC7" s="171">
+      <c r="AC7" s="153">
         <v>6</v>
       </c>
-      <c r="AD7" s="185" t="s">
+      <c r="AD7" s="167" t="s">
         <v>120</v>
       </c>
       <c r="AE7" s="99" t="s">
@@ -10717,13 +10710,13 @@
       <c r="AO7" s="99">
         <v>10</v>
       </c>
-      <c r="AP7" s="184">
+      <c r="AP7" s="166">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AQ7" s="181" t="s">
+      <c r="AQ7" s="163" t="s">
         <v>118</v>
       </c>
-      <c r="AR7" s="173" t="s">
+      <c r="AR7" s="155" t="s">
         <v>117</v>
       </c>
       <c r="AS7" s="107">
@@ -10744,16 +10737,16 @@
       <c r="AX7" s="104">
         <v>1</v>
       </c>
-      <c r="AY7" s="174">
+      <c r="AY7" s="156">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AZ7" s="174">
+      <c r="AZ7" s="156">
         <v>1.75</v>
       </c>
-      <c r="BA7" s="174">
+      <c r="BA7" s="156">
         <v>0</v>
       </c>
-      <c r="BB7" s="174">
+      <c r="BB7" s="156">
         <v>6</v>
       </c>
       <c r="BC7" s="104" t="s">
@@ -10765,7 +10758,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="124" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D8" s="59" t="s">
         <v>93</v>
@@ -10845,7 +10838,7 @@
       <c r="AC8" s="132">
         <v>6</v>
       </c>
-      <c r="AD8" s="185" t="s">
+      <c r="AD8" s="167" t="s">
         <v>116</v>
       </c>
       <c r="AE8" s="99" t="s">
@@ -10877,13 +10870,13 @@
       <c r="AO8" s="99">
         <v>10</v>
       </c>
-      <c r="AP8" s="184">
+      <c r="AP8" s="166">
         <v>0.7</v>
       </c>
-      <c r="AQ8" s="181" t="s">
+      <c r="AQ8" s="163" t="s">
         <v>114</v>
       </c>
-      <c r="AR8" s="173" t="s">
+      <c r="AR8" s="155" t="s">
         <v>113</v>
       </c>
       <c r="AS8" s="107">
@@ -10925,7 +10918,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="124" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D9" s="59" t="s">
         <v>84</v>
@@ -11002,10 +10995,10 @@
       <c r="AB9" s="132">
         <v>0</v>
       </c>
-      <c r="AC9" s="172">
+      <c r="AC9" s="154">
         <v>6</v>
       </c>
-      <c r="AD9" s="185" t="s">
+      <c r="AD9" s="167" t="s">
         <v>112</v>
       </c>
       <c r="AE9" s="99" t="s">
@@ -11037,13 +11030,13 @@
       <c r="AO9" s="99">
         <v>10</v>
       </c>
-      <c r="AP9" s="184">
+      <c r="AP9" s="166">
         <v>0.7</v>
       </c>
-      <c r="AQ9" s="182" t="s">
+      <c r="AQ9" s="164" t="s">
         <v>109</v>
       </c>
-      <c r="AR9" s="175" t="s">
+      <c r="AR9" s="157" t="s">
         <v>108</v>
       </c>
       <c r="AS9" s="107">
@@ -11076,7 +11069,7 @@
       <c r="BB9" s="104">
         <v>6</v>
       </c>
-      <c r="BC9" s="176" t="s">
+      <c r="BC9" s="158" t="s">
         <v>7</v>
       </c>
     </row>
@@ -11086,7 +11079,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="124" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" s="59" t="s">
         <v>79</v>
@@ -11166,7 +11159,7 @@
       <c r="AC10" s="132">
         <v>6</v>
       </c>
-      <c r="AD10" s="185" t="s">
+      <c r="AD10" s="167" t="s">
         <v>106</v>
       </c>
       <c r="AE10" s="99" t="s">
@@ -11198,13 +11191,13 @@
       <c r="AO10" s="99">
         <v>10</v>
       </c>
-      <c r="AP10" s="184">
+      <c r="AP10" s="166">
         <v>0.7</v>
       </c>
-      <c r="AQ10" s="182" t="s">
+      <c r="AQ10" s="164" t="s">
         <v>104</v>
       </c>
-      <c r="AR10" s="175" t="s">
+      <c r="AR10" s="157" t="s">
         <v>103</v>
       </c>
       <c r="AS10" s="107">
@@ -11237,7 +11230,7 @@
       <c r="BB10" s="104">
         <v>6</v>
       </c>
-      <c r="BC10" s="176" t="s">
+      <c r="BC10" s="158" t="s">
         <v>8</v>
       </c>
     </row>
@@ -11326,7 +11319,7 @@
       <c r="AC11" s="132">
         <v>12</v>
       </c>
-      <c r="AD11" s="185" t="s">
+      <c r="AD11" s="167" t="s">
         <v>102</v>
       </c>
       <c r="AE11" s="99" t="s">
@@ -11358,13 +11351,13 @@
       <c r="AO11" s="99">
         <v>10</v>
       </c>
-      <c r="AP11" s="184">
+      <c r="AP11" s="166">
         <v>0.7</v>
       </c>
-      <c r="AQ11" s="182" t="s">
+      <c r="AQ11" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="AR11" s="175" t="s">
+      <c r="AR11" s="157" t="s">
         <v>99</v>
       </c>
       <c r="AS11" s="107">
@@ -11397,7 +11390,7 @@
       <c r="BB11" s="104">
         <v>6</v>
       </c>
-      <c r="BC11" s="176" t="s">
+      <c r="BC11" s="158" t="s">
         <v>9</v>
       </c>
     </row>
@@ -11486,7 +11479,7 @@
       <c r="AC12" s="132">
         <v>12</v>
       </c>
-      <c r="AD12" s="185" t="s">
+      <c r="AD12" s="167" t="s">
         <v>98</v>
       </c>
       <c r="AE12" s="99" t="s">
@@ -11518,13 +11511,13 @@
       <c r="AO12" s="99">
         <v>10</v>
       </c>
-      <c r="AP12" s="184">
+      <c r="AP12" s="166">
         <v>0.7</v>
       </c>
-      <c r="AQ12" s="182" t="s">
+      <c r="AQ12" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="AR12" s="175" t="s">
+      <c r="AR12" s="157" t="s">
         <v>94</v>
       </c>
       <c r="AS12" s="107">
@@ -11557,7 +11550,7 @@
       <c r="BB12" s="104">
         <v>6</v>
       </c>
-      <c r="BC12" s="176" t="s">
+      <c r="BC12" s="158" t="s">
         <v>10</v>
       </c>
     </row>
@@ -11569,33 +11562,33 @@
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
-      <c r="I13" s="155" t="s">
+      <c r="I13" s="176" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="157"/>
-      <c r="K13" s="166" t="s">
+      <c r="J13" s="178"/>
+      <c r="K13" s="187" t="s">
         <v>73</v>
       </c>
-      <c r="L13" s="161"/>
-      <c r="M13" s="161"/>
-      <c r="N13" s="161"/>
-      <c r="O13" s="161"/>
-      <c r="P13" s="167"/>
+      <c r="L13" s="182"/>
+      <c r="M13" s="182"/>
+      <c r="N13" s="182"/>
+      <c r="O13" s="182"/>
+      <c r="P13" s="188"/>
       <c r="Q13" s="144" t="s">
         <v>72</v>
       </c>
-      <c r="R13" s="168" t="s">
+      <c r="R13" s="189" t="s">
         <v>70</v>
       </c>
-      <c r="S13" s="169"/>
-      <c r="T13" s="169"/>
-      <c r="U13" s="170"/>
-      <c r="V13" s="163" t="s">
+      <c r="S13" s="190"/>
+      <c r="T13" s="190"/>
+      <c r="U13" s="191"/>
+      <c r="V13" s="184" t="s">
         <v>69</v>
       </c>
-      <c r="W13" s="164"/>
-      <c r="X13" s="164"/>
-      <c r="Y13" s="165"/>
+      <c r="W13" s="185"/>
+      <c r="X13" s="185"/>
+      <c r="Y13" s="186"/>
       <c r="Z13" s="145"/>
       <c r="AA13" s="145"/>
       <c r="AB13" s="145"/>
@@ -11606,7 +11599,7 @@
     <row r="16" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -11641,7 +11634,7 @@
     </row>
     <row r="19" spans="2:27" ht="187.5" x14ac:dyDescent="0.25">
       <c r="B19" s="114" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C19" s="146" t="s">
         <v>0</v>
@@ -11673,10 +11666,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="98" t="s">
-        <v>202</v>
-      </c>
-      <c r="G20" s="149">
-        <v>2</v>
+        <v>219</v>
+      </c>
+      <c r="G20" s="149" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
@@ -11693,7 +11686,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="98" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G21" s="150">
         <v>1</v>
@@ -11713,7 +11706,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="98" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G22" s="150">
         <v>2</v>
@@ -11733,7 +11726,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G23" s="150">
         <v>3</v>
@@ -11753,7 +11746,7 @@
         <v>60</v>
       </c>
       <c r="F24" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G24" s="150">
         <v>1</v>
@@ -11773,7 +11766,7 @@
         <v>100</v>
       </c>
       <c r="F25" s="98" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G25" s="152">
         <v>1</v>
@@ -11782,7 +11775,7 @@
     <row r="26" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -11813,7 +11806,7 @@
     <row r="33" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -11843,7 +11836,7 @@
     </row>
     <row r="36" spans="2:27" ht="184.5" x14ac:dyDescent="0.25">
       <c r="B36" s="114" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C36" s="146" t="s">
         <v>0</v>
@@ -11855,7 +11848,7 @@
         <v>170</v>
       </c>
       <c r="F36" s="147" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.25">
@@ -11968,43 +11961,43 @@
     <mergeCell ref="V13:Y13"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C12 C7">
-    <cfRule type="duplicateValues" dxfId="86" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="duplicateValues" dxfId="85" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="duplicateValues" dxfId="84" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="83" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C25 C20">
-    <cfRule type="duplicateValues" dxfId="82" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="duplicateValues" dxfId="81" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="duplicateValues" dxfId="80" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="duplicateValues" dxfId="79" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C42 C37">
-    <cfRule type="duplicateValues" dxfId="78" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="duplicateValues" dxfId="77" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="duplicateValues" dxfId="76" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="duplicateValues" dxfId="75" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC7:BC12">
-    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D7:D12">

</xml_diff>

<commit_message>
Dragons HP drain in space WAS +1, now is +0
Former-commit-id: 767219c6ffec367e55913125275b51eb666575c8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="196">
   <si>
     <t>[sku]</t>
   </si>
@@ -609,6 +609,9 @@
   </si>
   <si>
     <t>[eatSpeedFactorMax]</t>
+  </si>
+  <si>
+    <t>damage added to the dragon in space</t>
   </si>
 </sst>
 </file>
@@ -3952,8 +3955,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
-      <selection activeCell="BH19" sqref="BH19"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4174,9 +4177,12 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:64" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:64" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
         <v>174</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>173</v>
@@ -4429,7 +4435,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P16" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="29">
         <v>8.0000000000000002E-3</v>
@@ -4618,7 +4624,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="P17" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="29">
         <v>8.5000000000000006E-3</v>
@@ -4807,7 +4813,7 @@
         <v>1.5</v>
       </c>
       <c r="P18" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="29">
         <v>8.9999999999999993E-3</v>
@@ -4996,7 +5002,7 @@
         <v>1.44</v>
       </c>
       <c r="P19" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="29">
         <v>0.01</v>
@@ -5185,7 +5191,7 @@
         <v>1.7</v>
       </c>
       <c r="P20" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="29">
         <v>1.2E-2</v>
@@ -5374,7 +5380,7 @@
         <v>1.9</v>
       </c>
       <c r="P21" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="29">
         <v>1.2E-2</v>
@@ -5563,7 +5569,7 @@
         <v>2.1</v>
       </c>
       <c r="P22" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="29">
         <v>1.2999999999999999E-2</v>
@@ -5752,7 +5758,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="P23" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="29">
         <v>1.4E-2</v>
@@ -5945,7 +5951,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="P24" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="50">
         <v>1.4E-2</v>
@@ -6137,7 +6143,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="P25" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="29">
         <v>1.4999999999999999E-2</v>
@@ -6331,7 +6337,7 @@
         <v>2.4</v>
       </c>
       <c r="P26" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="29">
         <v>1.6E-2</v>

</xml_diff>

<commit_message>
Just checking some values
Former-commit-id: 26a4a864a6cb19e7007994ff3dd12312c73a0888
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3955,8 +3955,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
+      <selection activeCell="BD26" sqref="BD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6265,7 +6265,6 @@
         <v>540</v>
       </c>
       <c r="BD25" s="112">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>590</v>
       </c>
       <c r="BE25" s="58">
@@ -6458,7 +6457,6 @@
         <v>680</v>
       </c>
       <c r="BD26" s="114">
-        <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>730</v>
       </c>
       <c r="BE26" s="38">

</xml_diff>

<commit_message>
Content - Change tier of some dragons
Former-commit-id: 0d0f05e34307f956e1582787de5bb675b1bf8d3a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3955,8 +3955,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4966,7 +4966,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E19" s="57">
         <v>3</v>
@@ -5532,8 +5532,8 @@
       <c r="C22" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="58" t="s">
-        <v>93</v>
+      <c r="D22" s="37" t="s">
+        <v>84</v>
       </c>
       <c r="E22" s="57">
         <v>6</v>
@@ -6107,7 +6107,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E25" s="57">
         <v>9</v>

</xml_diff>

<commit_message>
Update dragon content to dragon Fat moved to tier M
Former-commit-id: 8b641d7d57bc559b1f9ccde8c5f2e04c383d95dc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3955,8 +3955,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS10" workbookViewId="0">
-      <selection activeCell="BD26" sqref="BD26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4966,7 +4966,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E19" s="57">
         <v>3</v>
@@ -5533,7 +5533,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E22" s="57">
         <v>6</v>
@@ -6107,7 +6107,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E25" s="57">
         <v>9</v>

</xml_diff>

<commit_message>
Dragons get drunk again: - Eat the drunken monk rewards with a lot of HP and Energy - Drunk duration last 10 seconds - "Dizzy" texts last 10 seconds and text is modified to explain (more or less) what is happening
Former-commit-id: 6febe88c9ec38e6ab821b3393e33c806bbba4954
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3955,8 +3955,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="X13" workbookViewId="0">
+      <selection activeCell="AK20" sqref="AK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4500,7 +4500,7 @@
         <v>0</v>
       </c>
       <c r="AK16" s="74">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AL16" s="24" t="s">
         <v>120</v>
@@ -4689,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="AK17" s="45">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AL17" s="44" t="s">
         <v>116</v>
@@ -4878,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="AK18" s="61">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AL18" s="44" t="s">
         <v>112</v>
@@ -5067,7 +5067,7 @@
         <v>0</v>
       </c>
       <c r="AK19" s="45">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AL19" s="44" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Water mod for some dragons
Former-commit-id: bda4d33ff97d8036990664272304a067513bc460
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3955,8 +3955,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X13" workbookViewId="0">
-      <selection activeCell="AK20" sqref="AK20"/>
+    <sheetView tabSelected="1" topLeftCell="AS13" workbookViewId="0">
+      <selection activeCell="BI25" sqref="BI25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5135,7 +5135,7 @@
         <v>1.2</v>
       </c>
       <c r="BI19" s="58">
-        <v>1.3</v>
+        <v>0.74</v>
       </c>
       <c r="BJ19" s="58">
         <v>0</v>
@@ -5702,7 +5702,7 @@
         <v>0.5</v>
       </c>
       <c r="BI22" s="58">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="BJ22" s="58">
         <v>9</v>
@@ -6280,7 +6280,7 @@
         <v>0.3</v>
       </c>
       <c r="BI25" s="58">
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="BJ25" s="58">
         <v>45</v>

</xml_diff>

<commit_message>
Review water gravity mod.
Former-commit-id: 2909c944029d26f270c2e76f00589a910ced599a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3956,7 +3956,7 @@
   <dimension ref="B1:BL55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AS13" workbookViewId="0">
-      <selection activeCell="BI25" sqref="BI25"/>
+      <selection activeCell="BJ29" sqref="BJ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5135,7 +5135,7 @@
         <v>1.2</v>
       </c>
       <c r="BI19" s="58">
-        <v>0.74</v>
+        <v>0.77</v>
       </c>
       <c r="BJ19" s="58">
         <v>0</v>
@@ -5513,7 +5513,7 @@
         <v>0.5</v>
       </c>
       <c r="BI21" s="58">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="BJ21" s="58">
         <v>9</v>
@@ -6087,7 +6087,7 @@
         <v>0.6</v>
       </c>
       <c r="BI24" s="103">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="BJ24" s="103">
         <v>45</v>
@@ -6280,7 +6280,7 @@
         <v>0.3</v>
       </c>
       <c r="BI25" s="58">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="BJ25" s="58">
         <v>45</v>

</xml_diff>

<commit_message>
fix furyDragonMult. to new dragon's tiers
Former-commit-id: 75776bd68e3b6faab813101e61f97d4810893fe1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3956,7 +3956,7 @@
   <dimension ref="B1:BL55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AS13" workbookViewId="0">
-      <selection activeCell="BJ29" sqref="BJ29"/>
+      <selection activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5045,7 +5045,7 @@
         <v>10</v>
       </c>
       <c r="AD19" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE19" s="50">
         <v>9</v>
@@ -5612,7 +5612,7 @@
         <v>11</v>
       </c>
       <c r="AD22" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE22" s="50">
         <v>10</v>
@@ -6186,7 +6186,7 @@
         <v>11.5</v>
       </c>
       <c r="AD25" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AE25" s="63">
         <v>10</v>

</xml_diff>

<commit_message>
Jawfrey's camera is now same as Draconi's one
Former-commit-id: 64dbf7af6337308ed8d9580d1fb8bbfcab71b416
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3955,8 +3955,8 @@
   </sheetPr>
   <dimension ref="B1:BL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS13" workbookViewId="0">
-      <selection activeCell="AF20" sqref="AF20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5936,7 +5936,7 @@
         <v>45</v>
       </c>
       <c r="K24" s="104">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L24" s="105">
         <v>0</v>

</xml_diff>

<commit_message>
Added new column [PetScaleMenu]
Former-commit-id: 21859b73719db6cf205664392553ce37b5f15e29
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="197">
   <si>
     <t>[sku]</t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>damage added to the dragon in space</t>
+  </si>
+  <si>
+    <t>[petScaleMenu]</t>
   </si>
 </sst>
 </file>
@@ -1531,7 +1534,82 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="100">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3463,56 +3541,6 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3527,97 +3555,98 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BL26" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90" totalsRowBorderDxfId="89">
-  <autoFilter ref="B15:BL26"/>
-  <tableColumns count="63">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="88"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="86"/>
-    <tableColumn id="3" name="[order]" dataDxfId="85"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="84"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="83"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="82"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="81"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="80"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="79"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="78"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="77"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="76"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="75"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="74"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="73"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="72"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="71"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="70"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="69"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="68"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="67"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="66"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM26" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
+  <autoFilter ref="B15:BM26"/>
+  <tableColumns count="64">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="94"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="93"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="92"/>
+    <tableColumn id="3" name="[order]" dataDxfId="91"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="90"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="89"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="88"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="87"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="86"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="85"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="84"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="83"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="82"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="81"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="80"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="79"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="78"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="77"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="76"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="75"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="74"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="73"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="72"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="71">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="64"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="63"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="62"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="61"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="60"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="59"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="58"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="57"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="56"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="55">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="70"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="69"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="68"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="67"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="66"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="65"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="64"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="63"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="62"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="61">
       <calculatedColumnFormula>AH17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="54"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="53"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="52"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="51"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="50"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="49"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="48"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="47"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="46"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="45"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="44"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="43"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="42"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="41"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="40"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="39">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="60"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="59"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="58"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="57"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="56"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="55"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="54"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="53"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="52"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="51"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="50"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="49"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="48"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="47"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="46"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="0"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="45">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="38">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="44">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="37"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="36"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="35"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="34">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="43"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="42"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="41"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="40">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="33"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="32"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="31"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="30"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="29"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="28"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="27"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="39"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="38"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="37"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="36"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="35"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="34"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="33"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="18">
+    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3626,11 +3655,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B32:I33"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3643,7 +3672,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B44:W55"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3674,14 +3703,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B37:F40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="9"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="7"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3953,10 +3982,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BL55"/>
+  <dimension ref="B1:BM55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="AP13" workbookViewId="0">
+      <selection activeCell="AX28" sqref="AX28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3981,11 +4010,11 @@
     <col min="41" max="44" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="16.5703125" customWidth="1"/>
+    <col min="62" max="62" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>183</v>
       </c>
@@ -4014,7 +4043,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4022,7 +4051,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:64" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:65" ht="117" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>182</v>
       </c>
@@ -4042,7 +4071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -4063,7 +4092,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -4084,7 +4113,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4105,7 +4134,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4126,7 +4155,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4147,8 +4176,8 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4177,7 +4206,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:64" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:65" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
         <v>174</v>
       </c>
@@ -4202,7 +4231,7 @@
       <c r="AQ14" s="122"/>
       <c r="AR14" s="122"/>
     </row>
-    <row r="15" spans="2:64" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:65" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="75" t="s">
         <v>170</v>
       </c>
@@ -4350,50 +4379,53 @@
       <c r="AX15" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="AY15" s="3" t="s">
+      <c r="AY15" s="82" t="s">
+        <v>196</v>
+      </c>
+      <c r="AZ15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AZ15" s="81" t="s">
+      <c r="BA15" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="BA15" s="80" t="s">
+      <c r="BB15" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="BB15" s="76" t="s">
+      <c r="BC15" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="BC15" s="79" t="s">
+      <c r="BD15" s="79" t="s">
         <v>189</v>
       </c>
-      <c r="BD15" s="75" t="s">
+      <c r="BE15" s="75" t="s">
         <v>190</v>
       </c>
-      <c r="BE15" s="78" t="s">
+      <c r="BF15" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="BF15" s="78" t="s">
+      <c r="BG15" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="BG15" s="78" t="s">
+      <c r="BH15" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="BH15" s="75" t="s">
+      <c r="BI15" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="BI15" s="75" t="s">
+      <c r="BJ15" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="BJ15" s="77" t="s">
+      <c r="BK15" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="BK15" s="76" t="s">
+      <c r="BL15" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="BL15" s="75" t="s">
+      <c r="BM15" s="75" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4537,50 +4569,53 @@
       <c r="AX16" s="24">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AY16" s="72" t="s">
+      <c r="AY16" s="24">
+        <v>0.55999999999999994</v>
+      </c>
+      <c r="AZ16" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="AZ16" s="71" t="s">
+      <c r="BA16" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="BA16" s="41">
+      <c r="BB16" s="41">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="BB16" s="40">
+      <c r="BC16" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC16" s="39">
+      <c r="BD16" s="39">
         <v>175</v>
       </c>
-      <c r="BD16" s="112">
+      <c r="BE16" s="112">
         <v>200</v>
       </c>
-      <c r="BE16" s="58">
+      <c r="BF16" s="58">
         <v>2</v>
       </c>
-      <c r="BF16" s="58">
+      <c r="BG16" s="58">
         <v>9.5</v>
       </c>
-      <c r="BG16" s="58">
+      <c r="BH16" s="58">
         <v>1</v>
       </c>
-      <c r="BH16" s="73">
+      <c r="BI16" s="73">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BI16" s="73">
+      <c r="BJ16" s="73">
         <v>1.75</v>
       </c>
-      <c r="BJ16" s="73">
+      <c r="BK16" s="73">
         <v>0</v>
       </c>
-      <c r="BK16" s="73">
+      <c r="BL16" s="73">
         <v>8</v>
       </c>
-      <c r="BL16" s="58" t="s">
+      <c r="BM16" s="58" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -4726,50 +4761,53 @@
       <c r="AX17" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY17" s="72" t="s">
+      <c r="AY17" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ17" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="AZ17" s="71" t="s">
+      <c r="BA17" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="BA17" s="41">
+      <c r="BB17" s="41">
         <v>2.3E-3</v>
       </c>
-      <c r="BB17" s="40">
+      <c r="BC17" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC17" s="39">
+      <c r="BD17" s="39">
         <v>210</v>
       </c>
-      <c r="BD17" s="112">
+      <c r="BE17" s="112">
         <v>235</v>
       </c>
-      <c r="BE17" s="58">
+      <c r="BF17" s="58">
         <v>2.1</v>
       </c>
-      <c r="BF17" s="58">
+      <c r="BG17" s="58">
         <v>9.5</v>
       </c>
-      <c r="BG17" s="58">
+      <c r="BH17" s="58">
         <v>1.7</v>
       </c>
-      <c r="BH17" s="58">
+      <c r="BI17" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BI17" s="58">
+      <c r="BJ17" s="58">
         <v>2.1</v>
       </c>
-      <c r="BJ17" s="58">
+      <c r="BK17" s="58">
         <v>0</v>
       </c>
-      <c r="BK17" s="58">
+      <c r="BL17" s="58">
         <v>8</v>
       </c>
-      <c r="BL17" s="58" t="s">
+      <c r="BM17" s="58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -4915,50 +4953,53 @@
       <c r="AX18" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY18" s="60" t="s">
+      <c r="AY18" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ18" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="AZ18" s="59" t="s">
+      <c r="BA18" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="BA18" s="41">
+      <c r="BB18" s="41">
         <v>2E-3</v>
       </c>
-      <c r="BB18" s="40">
+      <c r="BC18" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC18" s="39">
+      <c r="BD18" s="39">
         <v>240</v>
       </c>
-      <c r="BD18" s="112">
+      <c r="BE18" s="112">
         <v>280</v>
       </c>
-      <c r="BE18" s="58">
+      <c r="BF18" s="58">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BF18" s="58">
+      <c r="BG18" s="58">
         <v>9.5</v>
       </c>
-      <c r="BG18" s="58">
+      <c r="BH18" s="58">
         <v>1.7</v>
       </c>
-      <c r="BH18" s="58">
+      <c r="BI18" s="58">
         <v>0.9</v>
       </c>
-      <c r="BI18" s="58">
+      <c r="BJ18" s="58">
         <v>2.25</v>
       </c>
-      <c r="BJ18" s="58">
+      <c r="BK18" s="58">
         <v>0</v>
       </c>
-      <c r="BK18" s="58">
+      <c r="BL18" s="58">
         <v>8</v>
       </c>
-      <c r="BL18" s="37" t="s">
+      <c r="BM18" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -5104,50 +5145,53 @@
       <c r="AX19" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY19" s="60" t="s">
+      <c r="AY19" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ19" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="AZ19" s="59" t="s">
+      <c r="BA19" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="BA19" s="41">
+      <c r="BB19" s="41">
         <v>2E-3</v>
       </c>
-      <c r="BB19" s="40">
+      <c r="BC19" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC19" s="39">
+      <c r="BD19" s="39">
         <v>345</v>
       </c>
-      <c r="BD19" s="112">
+      <c r="BE19" s="112">
         <v>365</v>
       </c>
-      <c r="BE19" s="58">
+      <c r="BF19" s="58">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BF19" s="58">
+      <c r="BG19" s="58">
         <v>5</v>
       </c>
-      <c r="BG19" s="58">
+      <c r="BH19" s="58">
         <v>0.5</v>
       </c>
-      <c r="BH19" s="58">
+      <c r="BI19" s="58">
         <v>1.2</v>
       </c>
-      <c r="BI19" s="58">
+      <c r="BJ19" s="58">
         <v>0.77</v>
       </c>
-      <c r="BJ19" s="58">
+      <c r="BK19" s="58">
         <v>0</v>
       </c>
-      <c r="BK19" s="58">
+      <c r="BL19" s="58">
         <v>8</v>
       </c>
-      <c r="BL19" s="37" t="s">
+      <c r="BM19" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5293,50 +5337,53 @@
       <c r="AX20" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY20" s="60" t="s">
+      <c r="AY20" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ20" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="AZ20" s="59" t="s">
+      <c r="BA20" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="BA20" s="41">
+      <c r="BB20" s="41">
         <v>1.9E-3</v>
       </c>
-      <c r="BB20" s="40">
+      <c r="BC20" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC20" s="39">
+      <c r="BD20" s="39">
         <v>310</v>
       </c>
-      <c r="BD20" s="112">
+      <c r="BE20" s="112">
         <v>335</v>
       </c>
-      <c r="BE20" s="58">
+      <c r="BF20" s="58">
         <v>2.4</v>
       </c>
-      <c r="BF20" s="58">
+      <c r="BG20" s="58">
         <v>9.5</v>
       </c>
-      <c r="BG20" s="58">
+      <c r="BH20" s="58">
         <v>1.7</v>
       </c>
-      <c r="BH20" s="58">
+      <c r="BI20" s="58">
         <v>1</v>
       </c>
-      <c r="BI20" s="58">
+      <c r="BJ20" s="58">
         <v>1.6</v>
       </c>
-      <c r="BJ20" s="58">
+      <c r="BK20" s="58">
         <v>9</v>
       </c>
-      <c r="BK20" s="58">
+      <c r="BL20" s="58">
         <v>8</v>
       </c>
-      <c r="BL20" s="37" t="s">
+      <c r="BM20" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5482,50 +5529,53 @@
       <c r="AX21" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY21" s="60" t="s">
+      <c r="AY21" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ21" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="AZ21" s="59" t="s">
+      <c r="BA21" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="BA21" s="41">
+      <c r="BB21" s="41">
         <v>1.8E-3</v>
       </c>
-      <c r="BB21" s="40">
+      <c r="BC21" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC21" s="39">
+      <c r="BD21" s="39">
         <v>322</v>
       </c>
-      <c r="BD21" s="112">
+      <c r="BE21" s="112">
         <v>347</v>
       </c>
-      <c r="BE21" s="58">
+      <c r="BF21" s="58">
         <v>2.5</v>
       </c>
-      <c r="BF21" s="58">
+      <c r="BG21" s="58">
         <v>9.5</v>
       </c>
-      <c r="BG21" s="58">
+      <c r="BH21" s="58">
         <v>1.7</v>
       </c>
-      <c r="BH21" s="58">
+      <c r="BI21" s="58">
         <v>0.5</v>
       </c>
-      <c r="BI21" s="58">
+      <c r="BJ21" s="58">
         <v>1.7</v>
       </c>
-      <c r="BJ21" s="58">
+      <c r="BK21" s="58">
         <v>9</v>
       </c>
-      <c r="BK21" s="58">
+      <c r="BL21" s="58">
         <v>8</v>
       </c>
-      <c r="BL21" s="37" t="s">
+      <c r="BM21" s="37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -5671,50 +5721,53 @@
       <c r="AX22" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY22" s="60" t="s">
+      <c r="AY22" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ22" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="AZ22" s="59" t="s">
+      <c r="BA22" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="BA22" s="41">
+      <c r="BB22" s="41">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="BB22" s="40">
+      <c r="BC22" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC22" s="39">
+      <c r="BD22" s="39">
         <v>343</v>
       </c>
-      <c r="BD22" s="112">
+      <c r="BE22" s="112">
         <v>372</v>
       </c>
-      <c r="BE22" s="58">
+      <c r="BF22" s="58">
         <v>2.6</v>
       </c>
-      <c r="BF22" s="58">
+      <c r="BG22" s="58">
         <v>9.5</v>
       </c>
-      <c r="BG22" s="58">
+      <c r="BH22" s="58">
         <v>1.7</v>
       </c>
-      <c r="BH22" s="58">
+      <c r="BI22" s="58">
         <v>0.5</v>
       </c>
-      <c r="BI22" s="58">
+      <c r="BJ22" s="58">
         <v>0.9</v>
       </c>
-      <c r="BJ22" s="58">
+      <c r="BK22" s="58">
         <v>9</v>
       </c>
-      <c r="BK22" s="58">
+      <c r="BL22" s="58">
         <v>8</v>
       </c>
-      <c r="BL22" s="37" t="s">
+      <c r="BM22" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -5864,50 +5917,53 @@
       <c r="AX23" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY23" s="60" t="s">
+      <c r="AY23" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ23" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="AZ23" s="59" t="s">
+      <c r="BA23" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="BA23" s="41">
+      <c r="BB23" s="41">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BB23" s="40">
+      <c r="BC23" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC23" s="39">
+      <c r="BD23" s="39">
         <v>435</v>
       </c>
-      <c r="BD23" s="112">
+      <c r="BE23" s="112">
         <v>465</v>
       </c>
-      <c r="BE23" s="58">
+      <c r="BF23" s="58">
         <v>3.2</v>
       </c>
-      <c r="BF23" s="58">
+      <c r="BG23" s="58">
         <v>9.5</v>
       </c>
-      <c r="BG23" s="58">
+      <c r="BH23" s="58">
         <v>1.7</v>
       </c>
-      <c r="BH23" s="58">
+      <c r="BI23" s="58">
         <v>0.5</v>
       </c>
-      <c r="BI23" s="58">
+      <c r="BJ23" s="58">
         <v>1.2</v>
       </c>
-      <c r="BJ23" s="58">
+      <c r="BK23" s="58">
         <v>45</v>
       </c>
-      <c r="BK23" s="58">
+      <c r="BL23" s="58">
         <v>15</v>
       </c>
-      <c r="BL23" s="37" t="s">
+      <c r="BM23" s="37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
@@ -6056,50 +6112,53 @@
       <c r="AX24" s="98">
         <v>0.7</v>
       </c>
-      <c r="AY24" s="102" t="s">
+      <c r="AY24" s="98">
+        <v>0.7</v>
+      </c>
+      <c r="AZ24" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="AZ24" s="21" t="s">
+      <c r="BA24" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BA24" s="106">
+      <c r="BB24" s="106">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BB24" s="107">
+      <c r="BC24" s="107">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC24" s="108">
+      <c r="BD24" s="108">
         <v>450</v>
       </c>
-      <c r="BD24" s="113">
+      <c r="BE24" s="113">
         <v>505</v>
       </c>
-      <c r="BE24" s="103">
+      <c r="BF24" s="103">
         <v>3.4</v>
       </c>
-      <c r="BF24" s="103">
+      <c r="BG24" s="103">
         <v>9.5</v>
       </c>
-      <c r="BG24" s="103">
+      <c r="BH24" s="103">
         <v>1.7</v>
       </c>
-      <c r="BH24" s="103">
+      <c r="BI24" s="103">
         <v>0.6</v>
       </c>
-      <c r="BI24" s="103">
+      <c r="BJ24" s="103">
         <v>1</v>
       </c>
-      <c r="BJ24" s="103">
+      <c r="BK24" s="103">
         <v>45</v>
       </c>
-      <c r="BK24" s="103">
+      <c r="BL24" s="103">
         <v>15</v>
       </c>
-      <c r="BL24" s="100" t="s">
+      <c r="BM24" s="100" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -6249,50 +6308,53 @@
       <c r="AX25" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY25" s="60" t="s">
+      <c r="AY25" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ25" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="AZ25" s="59" t="s">
+      <c r="BA25" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="BA25" s="41">
+      <c r="BB25" s="41">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BB25" s="40">
+      <c r="BC25" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC25" s="39">
+      <c r="BD25" s="39">
         <v>540</v>
       </c>
-      <c r="BD25" s="112">
+      <c r="BE25" s="112">
         <v>590</v>
       </c>
-      <c r="BE25" s="58">
+      <c r="BF25" s="58">
         <v>3.9</v>
       </c>
-      <c r="BF25" s="58">
+      <c r="BG25" s="58">
         <v>9.5</v>
       </c>
-      <c r="BG25" s="58">
+      <c r="BH25" s="58">
         <v>1.7</v>
       </c>
-      <c r="BH25" s="58">
+      <c r="BI25" s="58">
         <v>0.3</v>
       </c>
-      <c r="BI25" s="58">
+      <c r="BJ25" s="58">
         <v>0.4</v>
       </c>
-      <c r="BJ25" s="58">
+      <c r="BK25" s="58">
         <v>45</v>
       </c>
-      <c r="BK25" s="58">
+      <c r="BL25" s="58">
         <v>15</v>
       </c>
-      <c r="BL25" s="37" t="s">
+      <c r="BM25" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6441,50 +6503,53 @@
       <c r="AX26" s="24">
         <v>0.75</v>
       </c>
-      <c r="AY26" s="43" t="s">
+      <c r="AY26" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="AZ26" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="AZ26" s="42" t="s">
+      <c r="BA26" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="BA26" s="41">
+      <c r="BB26" s="41">
         <v>1.5E-3</v>
       </c>
-      <c r="BB26" s="40">
+      <c r="BC26" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BC26" s="39">
+      <c r="BD26" s="39">
         <v>680</v>
       </c>
-      <c r="BD26" s="114">
+      <c r="BE26" s="114">
         <v>730</v>
       </c>
-      <c r="BE26" s="38">
+      <c r="BF26" s="38">
         <v>4.7</v>
       </c>
-      <c r="BF26" s="38">
+      <c r="BG26" s="38">
         <v>9.5</v>
       </c>
-      <c r="BG26" s="38">
+      <c r="BH26" s="38">
         <v>1.7</v>
       </c>
-      <c r="BH26" s="38">
+      <c r="BI26" s="38">
         <v>0.7</v>
       </c>
-      <c r="BI26" s="38">
+      <c r="BJ26" s="38">
         <v>1.03</v>
       </c>
-      <c r="BJ26" s="38">
+      <c r="BK26" s="38">
         <v>59</v>
       </c>
-      <c r="BK26" s="38">
+      <c r="BL26" s="38">
         <v>15</v>
       </c>
-      <c r="BL26" s="37" t="s">
+      <c r="BM26" s="37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:64" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:65" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
@@ -6532,18 +6597,18 @@
         <v>68</v>
       </c>
       <c r="AI27" s="132"/>
-      <c r="BC27" s="121" t="s">
+      <c r="BD27" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="BD27" s="121"/>
       <c r="BE27" s="121"/>
       <c r="BF27" s="121"/>
       <c r="BG27" s="121"/>
       <c r="BH27" s="121"/>
       <c r="BI27" s="121"/>
+      <c r="BJ27" s="121"/>
     </row>
-    <row r="29" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:64" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -6557,7 +6622,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:64" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:65" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
@@ -6566,7 +6631,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:64" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:65" ht="140.25" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>64</v>
       </c>
@@ -7551,7 +7616,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="BC27:BI27"/>
+    <mergeCell ref="BD27:BJ27"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="I27:L27"/>
     <mergeCell ref="T27:U27"/>
@@ -7561,19 +7626,19 @@
     <mergeCell ref="AH27:AI27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="98" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="97" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL16:BL23 BL25:BL26">
-    <cfRule type="duplicateValues" dxfId="96" priority="3"/>
+  <conditionalFormatting sqref="BM16:BM23 BM25:BM26">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="95" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL24">
-    <cfRule type="duplicateValues" dxfId="94" priority="1"/>
+  <conditionalFormatting sqref="BM24">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">

</xml_diff>

<commit_message>
Added pet scale menu
Former-commit-id: 890bd7a44a957f0390757bff1c3e62eb35487544
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1536,81 +1536,6 @@
   </cellStyles>
   <dxfs count="100">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -2435,6 +2360,31 @@
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -3541,6 +3491,56 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3555,98 +3555,98 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM26" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM26" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
   <autoFilter ref="B15:BM26"/>
   <tableColumns count="64">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="94"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="93"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="92"/>
-    <tableColumn id="3" name="[order]" dataDxfId="91"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="90"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="89"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="88"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="87"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="86"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="85"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="84"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="83"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="82"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="81"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="80"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="79"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="78"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="77"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="76"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="75"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="74"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="73"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="72"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="71">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="89"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="87"/>
+    <tableColumn id="3" name="[order]" dataDxfId="86"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="85"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="84"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="83"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="82"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="81"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="80"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="79"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="78"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="77"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="76"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="75"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="74"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="73"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="72"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="71"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="70"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="69"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="68"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="67"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="66">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="70"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="69"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="68"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="67"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="66"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="65"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="64"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="63"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="62"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="61">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="65"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="64"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="63"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="62"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="61"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="60"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="59"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="58"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="57"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="56">
       <calculatedColumnFormula>AH17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="60"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="59"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="58"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="57"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="56"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="55"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="54"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="53"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="52"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="51"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="50"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="49"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="48"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="47"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="46"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="0"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="45">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="55"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="54"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="53"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="52"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="51"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="50"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="49"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="48"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="47"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="46"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="45"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="44"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="43"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="42"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="41"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="40"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="39">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="44">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="38">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="43"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="42"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="41"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="40">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="37"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="36"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="35"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="34">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="39"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="38"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="37"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="36"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="35"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="34"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="33"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="33"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="32"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="31"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="30"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="29"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="28"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="27"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="24">
+    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="18">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3655,11 +3655,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B32:I33"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3672,7 +3672,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B44:W55"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3703,14 +3703,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B37:F40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="9"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="7"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="6"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3985,7 +3985,7 @@
   <dimension ref="B1:BM55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AP13" workbookViewId="0">
-      <selection activeCell="AX28" sqref="AX28"/>
+      <selection activeCell="AY27" sqref="AY27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4570,7 +4570,7 @@
         <v>0.55999999999999994</v>
       </c>
       <c r="AY16" s="24">
-        <v>0.55999999999999994</v>
+        <v>0.6</v>
       </c>
       <c r="AZ16" s="72" t="s">
         <v>118</v>
@@ -4762,7 +4762,7 @@
         <v>0.7</v>
       </c>
       <c r="AY17" s="24">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="AZ17" s="72" t="s">
         <v>114</v>
@@ -5338,7 +5338,7 @@
         <v>0.7</v>
       </c>
       <c r="AY20" s="24">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AZ20" s="60" t="s">
         <v>100</v>
@@ -5530,7 +5530,7 @@
         <v>0.7</v>
       </c>
       <c r="AY21" s="24">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AZ21" s="60" t="s">
         <v>95</v>
@@ -5722,7 +5722,7 @@
         <v>0.7</v>
       </c>
       <c r="AY22" s="24">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AZ22" s="60" t="s">
         <v>90</v>
@@ -5918,7 +5918,7 @@
         <v>0.7</v>
       </c>
       <c r="AY23" s="24">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AZ23" s="60" t="s">
         <v>86</v>
@@ -6113,7 +6113,7 @@
         <v>0.7</v>
       </c>
       <c r="AY24" s="98">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AZ24" s="102" t="s">
         <v>187</v>
@@ -6309,7 +6309,7 @@
         <v>0.7</v>
       </c>
       <c r="AY25" s="24">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AZ25" s="60" t="s">
         <v>81</v>
@@ -6504,7 +6504,7 @@
         <v>0.75</v>
       </c>
       <c r="AY26" s="24">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="AZ26" s="43" t="s">
         <v>76</v>
@@ -7626,19 +7626,19 @@
     <mergeCell ref="AH27:AI27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM16:BM23 BM25:BM26">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM24">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">

</xml_diff>

<commit_message>
Content - Add dragon 12 def :)
Former-commit-id: e7eedcf7d367009c49e53d4443efa94a66622820
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="202">
   <si>
     <t>[sku]</t>
   </si>
@@ -615,6 +615,21 @@
   </si>
   <si>
     <t>[petScaleMenu]</t>
+  </si>
+  <si>
+    <t>dragon_goldheist</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_GOLDHEIST_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_GOLDHEIST_DESC</t>
+  </si>
+  <si>
+    <t>PF_DragonGoldheist</t>
+  </si>
+  <si>
+    <t>PF_DragonGoldheistMenu</t>
   </si>
 </sst>
 </file>
@@ -3555,8 +3570,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM26" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
-  <autoFilter ref="B15:BM26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM27" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+  <autoFilter ref="B15:BM27"/>
   <tableColumns count="64">
     <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="89"/>
     <tableColumn id="2" name="[sku]" dataDxfId="88"/>
@@ -3655,8 +3670,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B32:I33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B33:I34"/>
   <tableColumns count="8">
     <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
     <tableColumn id="2" name="[sku]" dataDxfId="12"/>
@@ -3672,8 +3687,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B44:W55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="B45:W57"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
     <tableColumn id="2" name="[sku]"/>
@@ -3703,8 +3718,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B37:F40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B38:F41"/>
   <tableColumns count="5">
     <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
     <tableColumn id="2" name="[sku]" dataDxfId="2"/>
@@ -3982,10 +3997,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BM55"/>
+  <dimension ref="B1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP13" workbookViewId="0">
-      <selection activeCell="AY27" sqref="AY27"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4011,6 +4026,7 @@
     <col min="47" max="47" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="16.5703125" customWidth="1"/>
+    <col min="65" max="65" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4088,7 +4104,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="14" t="str">
-        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
@@ -4109,7 +4125,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="14" t="str">
-        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
@@ -4130,7 +4146,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="96" t="str">
-        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
@@ -4151,7 +4167,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="94" t="str">
-        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
@@ -4172,7 +4188,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="94" t="str">
-        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
@@ -4494,7 +4510,7 @@
         <v>100</v>
       </c>
       <c r="Y16" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z16" s="29">
@@ -4525,7 +4541,7 @@
         <v>0.23</v>
       </c>
       <c r="AI16" s="67">
-        <f t="shared" ref="AI16:AI25" si="0">AH17</f>
+        <f t="shared" ref="AI16:AI23" ca="1" si="0">AH17</f>
         <v>0.19</v>
       </c>
       <c r="AJ16" s="74">
@@ -4686,7 +4702,7 @@
         <v>100</v>
       </c>
       <c r="Y17" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z17" s="29">
@@ -4717,7 +4733,7 @@
         <v>0.19</v>
       </c>
       <c r="AI17" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.15</v>
       </c>
       <c r="AJ17" s="74">
@@ -4878,7 +4894,7 @@
         <v>100</v>
       </c>
       <c r="Y18" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z18" s="29">
@@ -4909,7 +4925,7 @@
         <v>0.15</v>
       </c>
       <c r="AI18" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.13</v>
       </c>
       <c r="AJ18" s="120">
@@ -5070,7 +5086,7 @@
         <v>100</v>
       </c>
       <c r="Y19" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z19" s="29">
@@ -5101,7 +5117,7 @@
         <v>0.13</v>
       </c>
       <c r="AI19" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.11</v>
       </c>
       <c r="AJ19" s="74">
@@ -5262,7 +5278,7 @@
         <v>100</v>
       </c>
       <c r="Y20" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z20" s="29">
@@ -5293,7 +5309,7 @@
         <v>0.11</v>
       </c>
       <c r="AI20" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.09</v>
       </c>
       <c r="AJ20" s="74">
@@ -5454,7 +5470,7 @@
         <v>100</v>
       </c>
       <c r="Y21" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z21" s="29">
@@ -5485,7 +5501,7 @@
         <v>0.09</v>
       </c>
       <c r="AI21" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.08</v>
       </c>
       <c r="AJ21" s="74">
@@ -5646,7 +5662,7 @@
         <v>100</v>
       </c>
       <c r="Y22" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z22" s="29">
@@ -5677,7 +5693,7 @@
         <v>0.08</v>
       </c>
       <c r="AI22" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ22" s="74">
@@ -5838,7 +5854,7 @@
         <v>100</v>
       </c>
       <c r="Y23" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z23" s="29">
@@ -5869,7 +5885,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI23" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.06</v>
       </c>
       <c r="AJ23" s="120">
@@ -6034,7 +6050,7 @@
         <v>100</v>
       </c>
       <c r="Y24" s="50">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z24" s="50">
@@ -6229,7 +6245,7 @@
         <v>100</v>
       </c>
       <c r="Y25" s="29">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z25" s="29">
@@ -6260,7 +6276,7 @@
         <v>0.06</v>
       </c>
       <c r="AI25" s="67">
-        <f t="shared" si="0"/>
+        <f ca="1">AH26</f>
         <v>0.05</v>
       </c>
       <c r="AJ25" s="120">
@@ -6425,7 +6441,7 @@
         <v>100</v>
       </c>
       <c r="Y26" s="26">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z26" s="26">
@@ -6549,199 +6565,377 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:65" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="123" t="s">
+    <row r="27" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="57">
+        <v>10</v>
+      </c>
+      <c r="F27" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="30">
+        <v>4300000</v>
+      </c>
+      <c r="H27" s="55">
+        <v>1100</v>
+      </c>
+      <c r="I27" s="54">
+        <v>35</v>
+      </c>
+      <c r="J27" s="53">
+        <v>45</v>
+      </c>
+      <c r="K27" s="25">
+        <v>25</v>
+      </c>
+      <c r="L27" s="52">
+        <v>0</v>
+      </c>
+      <c r="M27" s="51">
+        <v>425</v>
+      </c>
+      <c r="N27" s="26">
+        <v>500</v>
+      </c>
+      <c r="O27" s="26">
+        <v>2.4</v>
+      </c>
+      <c r="P27" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="29">
+        <v>1.6E-2</v>
+      </c>
+      <c r="R27" s="50">
+        <v>20</v>
+      </c>
+      <c r="S27" s="50">
+        <v>0.8</v>
+      </c>
+      <c r="T27" s="46">
+        <v>2</v>
+      </c>
+      <c r="U27" s="26">
+        <v>2.1</v>
+      </c>
+      <c r="V27" s="49">
+        <v>31</v>
+      </c>
+      <c r="W27" s="26">
+        <v>1.9</v>
+      </c>
+      <c r="X27" s="26">
+        <v>100</v>
+      </c>
+      <c r="Y27" s="26">
+        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="Z27" s="26">
+        <v>19</v>
+      </c>
+      <c r="AA27" s="26">
+        <v>12</v>
+      </c>
+      <c r="AB27" s="49">
+        <v>475</v>
+      </c>
+      <c r="AC27" s="48">
+        <v>12</v>
+      </c>
+      <c r="AD27" s="26">
+        <v>6</v>
+      </c>
+      <c r="AE27" s="48">
+        <v>10</v>
+      </c>
+      <c r="AF27" s="26">
+        <v>30000</v>
+      </c>
+      <c r="AG27" s="47">
+        <v>5</v>
+      </c>
+      <c r="AH27" s="118">
+        <v>0.05</v>
+      </c>
+      <c r="AI27" s="67">
+        <v>0.04</v>
+      </c>
+      <c r="AJ27" s="74">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="45">
+        <v>12</v>
+      </c>
+      <c r="AL27" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM27" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN27" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO27" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP27" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ27" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AR27" s="24">
+        <v>2</v>
+      </c>
+      <c r="AS27" s="24">
+        <v>2</v>
+      </c>
+      <c r="AT27" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU27" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV27" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW27" s="24">
+        <v>23</v>
+      </c>
+      <c r="AX27" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="AY27" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="AZ27" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="BA27" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="BB27" s="41">
+        <v>1.5E-3</v>
+      </c>
+      <c r="BC27" s="40">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="BD27" s="39">
+        <v>680</v>
+      </c>
+      <c r="BE27" s="114">
+        <v>730</v>
+      </c>
+      <c r="BF27" s="38">
+        <v>4.7</v>
+      </c>
+      <c r="BG27" s="38">
+        <v>9.5</v>
+      </c>
+      <c r="BH27" s="38">
+        <v>1.7</v>
+      </c>
+      <c r="BI27" s="38">
+        <v>0.7</v>
+      </c>
+      <c r="BJ27" s="38">
+        <v>1.03</v>
+      </c>
+      <c r="BK27" s="38">
+        <v>59</v>
+      </c>
+      <c r="BL27" s="38">
+        <v>15</v>
+      </c>
+      <c r="BM27" s="37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="2:65" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="124"/>
-      <c r="K27" s="124"/>
-      <c r="L27" s="125"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="127" t="s">
+      <c r="J28" s="124"/>
+      <c r="K28" s="124"/>
+      <c r="L28" s="125"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="127" t="s">
         <v>73</v>
       </c>
-      <c r="O27" s="127"/>
-      <c r="P27" s="127"/>
-      <c r="Q27" s="127"/>
-      <c r="R27" s="127"/>
-      <c r="S27" s="128"/>
-      <c r="T27" s="126" t="s">
+      <c r="O28" s="127"/>
+      <c r="P28" s="127"/>
+      <c r="Q28" s="127"/>
+      <c r="R28" s="127"/>
+      <c r="S28" s="128"/>
+      <c r="T28" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="U27" s="126"/>
-      <c r="V27" s="35" t="s">
+      <c r="U28" s="126"/>
+      <c r="V28" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W27" s="129" t="s">
+      <c r="W28" s="129" t="s">
         <v>70</v>
       </c>
-      <c r="X27" s="129"/>
-      <c r="Y27" s="129"/>
-      <c r="Z27" s="129"/>
-      <c r="AA27" s="129"/>
-      <c r="AB27" s="130" t="s">
+      <c r="X28" s="129"/>
+      <c r="Y28" s="129"/>
+      <c r="Z28" s="129"/>
+      <c r="AA28" s="129"/>
+      <c r="AB28" s="130" t="s">
         <v>69</v>
       </c>
-      <c r="AC27" s="130"/>
-      <c r="AD27" s="130"/>
-      <c r="AE27" s="130"/>
-      <c r="AF27" s="131"/>
-      <c r="AH27" s="132" t="s">
+      <c r="AC28" s="130"/>
+      <c r="AD28" s="130"/>
+      <c r="AE28" s="130"/>
+      <c r="AF28" s="131"/>
+      <c r="AH28" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="AI27" s="132"/>
-      <c r="BD27" s="121" t="s">
+      <c r="AI28" s="132"/>
+      <c r="BD28" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="BE27" s="121"/>
-      <c r="BF27" s="121"/>
-      <c r="BG27" s="121"/>
-      <c r="BH27" s="121"/>
-      <c r="BI27" s="121"/>
-      <c r="BJ27" s="121"/>
+      <c r="BE28" s="121"/>
+      <c r="BF28" s="121"/>
+      <c r="BG28" s="121"/>
+      <c r="BH28" s="121"/>
+      <c r="BI28" s="121"/>
+      <c r="BJ28" s="121"/>
     </row>
-    <row r="29" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B30" s="1" t="s">
+    <row r="30" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
     </row>
-    <row r="31" spans="2:65" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
+    <row r="32" spans="2:65" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B32" s="19"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
     </row>
-    <row r="32" spans="2:65" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
+    <row r="33" spans="2:23" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D33" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B33" s="8" t="s">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C34" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D34" s="32">
         <v>0.2</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>8</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>1.5</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <v>1.2</v>
       </c>
-      <c r="H33">
+      <c r="H34">
         <v>1.2</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B35" s="1" t="s">
+    <row r="35" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
     </row>
-    <row r="36" spans="2:23" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
+    <row r="37" spans="2:23" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" s="19"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
-    <row r="37" spans="2:23" ht="169.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="10" t="s">
+    <row r="38" spans="2:23" ht="169.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D38" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E38" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="32">
-        <v>0.25</v>
-      </c>
-      <c r="E38" s="32">
-        <v>1</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
@@ -6749,16 +6943,16 @@
         <v>3</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D39" s="32">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="E39" s="32">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
@@ -6766,172 +6960,121 @@
         <v>3</v>
       </c>
       <c r="C40" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E40" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="32">
+      <c r="D41" s="32">
         <v>0.05</v>
       </c>
-      <c r="E40" s="32">
+      <c r="E41" s="32">
         <v>0.4</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F41" s="14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B42" s="1" t="s">
+    <row r="42" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E43" t="s">
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:23" ht="150" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
+    <row r="45" spans="2:23" ht="150" x14ac:dyDescent="0.25">
+      <c r="B45" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F45" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="G45" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H45" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I45" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J45" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K44" s="5" t="s">
+      <c r="K45" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L44" s="5" t="s">
+      <c r="L45" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="M45" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N44" s="5" t="s">
+      <c r="N45" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O44" s="5" t="s">
+      <c r="O45" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P44" s="5" t="s">
+      <c r="P45" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Q44" s="5" t="s">
+      <c r="Q45" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R44" s="5" t="s">
+      <c r="R45" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S44" s="5" t="s">
+      <c r="S45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="T44" s="5" t="s">
+      <c r="T45" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="U44" s="5" t="s">
+      <c r="U45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="V44" s="5" t="s">
+      <c r="V45" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W44" s="5" t="s">
+      <c r="W45" s="5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45">
-        <v>8</v>
-      </c>
-      <c r="E45">
-        <v>571</v>
-      </c>
-      <c r="F45">
-        <v>1714</v>
-      </c>
-      <c r="G45">
-        <v>3429</v>
-      </c>
-      <c r="H45">
-        <v>5714</v>
-      </c>
-      <c r="I45">
-        <v>8571</v>
-      </c>
-      <c r="J45">
-        <v>12000</v>
-      </c>
-      <c r="K45">
-        <v>16000</v>
-      </c>
-      <c r="L45" t="s">
-        <v>20</v>
-      </c>
-      <c r="M45" t="s">
-        <v>20</v>
-      </c>
-      <c r="N45" t="s">
-        <v>20</v>
-      </c>
-      <c r="O45" t="s">
-        <v>20</v>
-      </c>
-      <c r="P45" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>20</v>
-      </c>
-      <c r="R45" t="s">
-        <v>20</v>
-      </c>
-      <c r="S45" t="s">
-        <v>20</v>
-      </c>
-      <c r="T45" t="s">
-        <v>20</v>
-      </c>
-      <c r="U45" t="s">
-        <v>20</v>
-      </c>
-      <c r="V45" t="s">
-        <v>20</v>
-      </c>
-      <c r="W45" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
@@ -6939,37 +7082,37 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E46">
-        <v>1021</v>
+        <v>571</v>
       </c>
       <c r="F46">
-        <v>3063</v>
+        <v>1714</v>
       </c>
       <c r="G46">
-        <v>6127</v>
+        <v>3429</v>
       </c>
       <c r="H46">
-        <v>10211</v>
+        <v>5714</v>
       </c>
       <c r="I46">
-        <v>15317</v>
+        <v>8571</v>
       </c>
       <c r="J46">
-        <v>21443</v>
+        <v>12000</v>
       </c>
       <c r="K46">
-        <v>28591</v>
-      </c>
-      <c r="L46">
-        <v>36760</v>
-      </c>
-      <c r="M46">
-        <v>45950</v>
+        <v>16000</v>
+      </c>
+      <c r="L46" t="s">
+        <v>20</v>
+      </c>
+      <c r="M46" t="s">
+        <v>20</v>
       </c>
       <c r="N46" t="s">
         <v>20</v>
@@ -7007,37 +7150,37 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47">
         <v>10</v>
       </c>
       <c r="E47">
-        <v>1661</v>
+        <v>1021</v>
       </c>
       <c r="F47">
-        <v>4983</v>
+        <v>3063</v>
       </c>
       <c r="G47">
-        <v>9966</v>
+        <v>6127</v>
       </c>
       <c r="H47">
-        <v>16610</v>
+        <v>10211</v>
       </c>
       <c r="I47">
-        <v>24915</v>
+        <v>15317</v>
       </c>
       <c r="J47">
-        <v>34881</v>
+        <v>21443</v>
       </c>
       <c r="K47">
-        <v>46508</v>
+        <v>28591</v>
       </c>
       <c r="L47">
-        <v>59796</v>
+        <v>36760</v>
       </c>
       <c r="M47">
-        <v>74745</v>
+        <v>45950</v>
       </c>
       <c r="N47" t="s">
         <v>20</v>
@@ -7075,37 +7218,37 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D48">
         <v>10</v>
       </c>
       <c r="E48">
-        <v>2346</v>
+        <v>1661</v>
       </c>
       <c r="F48">
-        <v>7037</v>
+        <v>4983</v>
       </c>
       <c r="G48">
-        <v>14075</v>
+        <v>9966</v>
       </c>
       <c r="H48">
-        <v>23458</v>
+        <v>16610</v>
       </c>
       <c r="I48">
-        <v>35187</v>
+        <v>24915</v>
       </c>
       <c r="J48">
-        <v>49261</v>
+        <v>34881</v>
       </c>
       <c r="K48">
-        <v>65682</v>
+        <v>46508</v>
       </c>
       <c r="L48">
-        <v>84448</v>
+        <v>59796</v>
       </c>
       <c r="M48">
-        <v>105560</v>
+        <v>74745</v>
       </c>
       <c r="N48" t="s">
         <v>20</v>
@@ -7143,52 +7286,52 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D49">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E49">
-        <v>1971</v>
+        <v>2346</v>
       </c>
       <c r="F49">
-        <v>5913</v>
+        <v>7037</v>
       </c>
       <c r="G49">
-        <v>11826</v>
+        <v>14075</v>
       </c>
       <c r="H49">
-        <v>19711</v>
+        <v>23458</v>
       </c>
       <c r="I49">
-        <v>29566</v>
+        <v>35187</v>
       </c>
       <c r="J49">
-        <v>41393</v>
+        <v>49261</v>
       </c>
       <c r="K49">
-        <v>55190</v>
+        <v>65682</v>
       </c>
       <c r="L49">
-        <v>70959</v>
+        <v>84448</v>
       </c>
       <c r="M49">
-        <v>88698</v>
-      </c>
-      <c r="N49">
-        <v>108409</v>
-      </c>
-      <c r="O49">
-        <v>130091</v>
-      </c>
-      <c r="P49">
-        <v>153744</v>
-      </c>
-      <c r="Q49">
-        <v>179368</v>
-      </c>
-      <c r="R49">
-        <v>206963</v>
+        <v>105560</v>
+      </c>
+      <c r="N49" t="s">
+        <v>20</v>
+      </c>
+      <c r="O49" t="s">
+        <v>20</v>
+      </c>
+      <c r="P49" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>20</v>
+      </c>
+      <c r="R49" t="s">
+        <v>20</v>
       </c>
       <c r="S49" t="s">
         <v>20</v>
@@ -7211,52 +7354,52 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D50">
         <v>15</v>
       </c>
       <c r="E50">
-        <v>2453</v>
+        <v>1971</v>
       </c>
       <c r="F50">
-        <v>7359</v>
+        <v>5913</v>
       </c>
       <c r="G50">
-        <v>14718</v>
+        <v>11826</v>
       </c>
       <c r="H50">
-        <v>24531</v>
+        <v>19711</v>
       </c>
       <c r="I50">
-        <v>36796</v>
+        <v>29566</v>
       </c>
       <c r="J50">
-        <v>51515</v>
+        <v>41393</v>
       </c>
       <c r="K50">
-        <v>68686</v>
+        <v>55190</v>
       </c>
       <c r="L50">
-        <v>88311</v>
+        <v>70959</v>
       </c>
       <c r="M50">
-        <v>110388</v>
+        <v>88698</v>
       </c>
       <c r="N50">
-        <v>134919</v>
+        <v>108409</v>
       </c>
       <c r="O50">
-        <v>161903</v>
+        <v>130091</v>
       </c>
       <c r="P50">
-        <v>191340</v>
+        <v>153744</v>
       </c>
       <c r="Q50">
-        <v>223230</v>
+        <v>179368</v>
       </c>
       <c r="R50">
-        <v>257573</v>
+        <v>206963</v>
       </c>
       <c r="S50" t="s">
         <v>20</v>
@@ -7279,52 +7422,52 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D51">
         <v>15</v>
       </c>
       <c r="E51">
-        <v>2952</v>
+        <v>2453</v>
       </c>
       <c r="F51">
-        <v>8855</v>
+        <v>7359</v>
       </c>
       <c r="G51">
-        <v>17709</v>
+        <v>14718</v>
       </c>
       <c r="H51">
-        <v>29516</v>
+        <v>24531</v>
       </c>
       <c r="I51">
-        <v>44274</v>
+        <v>36796</v>
       </c>
       <c r="J51">
-        <v>61983</v>
+        <v>51515</v>
       </c>
       <c r="K51">
-        <v>82644</v>
+        <v>68686</v>
       </c>
       <c r="L51">
-        <v>106257</v>
+        <v>88311</v>
       </c>
       <c r="M51">
-        <v>132821</v>
+        <v>110388</v>
       </c>
       <c r="N51">
-        <v>162336</v>
+        <v>134919</v>
       </c>
       <c r="O51">
-        <v>194804</v>
+        <v>161903</v>
       </c>
       <c r="P51">
-        <v>230223</v>
+        <v>191340</v>
       </c>
       <c r="Q51">
-        <v>268593</v>
+        <v>223230</v>
       </c>
       <c r="R51">
-        <v>309915</v>
+        <v>257573</v>
       </c>
       <c r="S51" t="s">
         <v>20</v>
@@ -7347,67 +7490,67 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D52">
+        <v>15</v>
+      </c>
+      <c r="E52">
+        <v>2952</v>
+      </c>
+      <c r="F52">
+        <v>8855</v>
+      </c>
+      <c r="G52">
+        <v>17709</v>
+      </c>
+      <c r="H52">
+        <v>29516</v>
+      </c>
+      <c r="I52">
+        <v>44274</v>
+      </c>
+      <c r="J52">
+        <v>61983</v>
+      </c>
+      <c r="K52">
+        <v>82644</v>
+      </c>
+      <c r="L52">
+        <v>106257</v>
+      </c>
+      <c r="M52">
+        <v>132821</v>
+      </c>
+      <c r="N52">
+        <v>162336</v>
+      </c>
+      <c r="O52">
+        <v>194804</v>
+      </c>
+      <c r="P52">
+        <v>230223</v>
+      </c>
+      <c r="Q52">
+        <v>268593</v>
+      </c>
+      <c r="R52">
+        <v>309915</v>
+      </c>
+      <c r="S52" t="s">
         <v>20</v>
       </c>
-      <c r="E52">
-        <v>2553</v>
-      </c>
-      <c r="F52">
-        <v>7658</v>
-      </c>
-      <c r="G52">
-        <v>15317</v>
-      </c>
-      <c r="H52">
-        <v>25528</v>
-      </c>
-      <c r="I52">
-        <v>38292</v>
-      </c>
-      <c r="J52">
-        <v>53609</v>
-      </c>
-      <c r="K52">
-        <v>71478</v>
-      </c>
-      <c r="L52">
-        <v>91900</v>
-      </c>
-      <c r="M52">
-        <v>114876</v>
-      </c>
-      <c r="N52">
-        <v>140403</v>
-      </c>
-      <c r="O52">
-        <v>168484</v>
-      </c>
-      <c r="P52">
-        <v>199118</v>
-      </c>
-      <c r="Q52">
-        <v>232304</v>
-      </c>
-      <c r="R52">
-        <v>268043</v>
-      </c>
-      <c r="S52">
-        <v>306335</v>
-      </c>
-      <c r="T52">
-        <v>347179</v>
-      </c>
-      <c r="U52">
-        <v>390577</v>
-      </c>
-      <c r="V52">
-        <v>436527</v>
-      </c>
-      <c r="W52">
-        <v>485030</v>
+      <c r="T52" t="s">
+        <v>20</v>
+      </c>
+      <c r="U52" t="s">
+        <v>20</v>
+      </c>
+      <c r="V52" t="s">
+        <v>20</v>
+      </c>
+      <c r="W52" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
@@ -7415,67 +7558,67 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="D53">
         <v>20</v>
       </c>
-      <c r="E53" s="111">
-        <v>2940</v>
-      </c>
-      <c r="F53" s="111">
-        <v>8821</v>
-      </c>
-      <c r="G53" s="111">
-        <v>17642</v>
-      </c>
-      <c r="H53" s="111">
-        <v>29403</v>
-      </c>
-      <c r="I53" s="111">
-        <v>44105</v>
-      </c>
-      <c r="J53" s="111">
-        <v>61747</v>
-      </c>
-      <c r="K53" s="111">
-        <v>82329</v>
-      </c>
-      <c r="L53" s="111">
-        <v>105851</v>
-      </c>
-      <c r="M53" s="111">
-        <v>132314</v>
-      </c>
-      <c r="N53" s="111">
-        <v>161717</v>
-      </c>
-      <c r="O53" s="111">
-        <v>194061</v>
-      </c>
-      <c r="P53" s="111">
-        <v>229345</v>
-      </c>
-      <c r="Q53" s="111">
-        <v>267569</v>
-      </c>
-      <c r="R53" s="111">
-        <v>308733</v>
-      </c>
-      <c r="S53" s="111">
-        <v>352838</v>
-      </c>
-      <c r="T53" s="111">
-        <v>399883</v>
-      </c>
-      <c r="U53" s="111">
-        <v>449868</v>
-      </c>
-      <c r="V53" s="111">
-        <v>502794</v>
-      </c>
-      <c r="W53" s="111">
-        <v>558660</v>
+      <c r="E53">
+        <v>2553</v>
+      </c>
+      <c r="F53">
+        <v>7658</v>
+      </c>
+      <c r="G53">
+        <v>15317</v>
+      </c>
+      <c r="H53">
+        <v>25528</v>
+      </c>
+      <c r="I53">
+        <v>38292</v>
+      </c>
+      <c r="J53">
+        <v>53609</v>
+      </c>
+      <c r="K53">
+        <v>71478</v>
+      </c>
+      <c r="L53">
+        <v>91900</v>
+      </c>
+      <c r="M53">
+        <v>114876</v>
+      </c>
+      <c r="N53">
+        <v>140403</v>
+      </c>
+      <c r="O53">
+        <v>168484</v>
+      </c>
+      <c r="P53">
+        <v>199118</v>
+      </c>
+      <c r="Q53">
+        <v>232304</v>
+      </c>
+      <c r="R53">
+        <v>268043</v>
+      </c>
+      <c r="S53">
+        <v>306335</v>
+      </c>
+      <c r="T53">
+        <v>347179</v>
+      </c>
+      <c r="U53">
+        <v>390577</v>
+      </c>
+      <c r="V53">
+        <v>436527</v>
+      </c>
+      <c r="W53">
+        <v>485030</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
@@ -7483,67 +7626,67 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D54">
         <v>20</v>
       </c>
-      <c r="E54">
-        <v>3337</v>
-      </c>
-      <c r="F54">
-        <v>10010</v>
-      </c>
-      <c r="G54">
-        <v>20020</v>
-      </c>
-      <c r="H54">
-        <v>33366</v>
-      </c>
-      <c r="I54">
-        <v>50049</v>
-      </c>
-      <c r="J54">
-        <v>70069</v>
-      </c>
-      <c r="K54">
-        <v>93426</v>
-      </c>
-      <c r="L54">
-        <v>120119</v>
-      </c>
-      <c r="M54">
-        <v>150148</v>
-      </c>
-      <c r="N54">
-        <v>183515</v>
-      </c>
-      <c r="O54">
-        <v>220218</v>
-      </c>
-      <c r="P54">
-        <v>260257</v>
-      </c>
-      <c r="Q54">
-        <v>303633</v>
-      </c>
-      <c r="R54">
-        <v>350346</v>
-      </c>
-      <c r="S54">
-        <v>400396</v>
-      </c>
-      <c r="T54">
-        <v>453782</v>
-      </c>
-      <c r="U54">
-        <v>510505</v>
-      </c>
-      <c r="V54">
-        <v>570564</v>
-      </c>
-      <c r="W54">
-        <v>633960</v>
+      <c r="E54" s="111">
+        <v>2940</v>
+      </c>
+      <c r="F54" s="111">
+        <v>8821</v>
+      </c>
+      <c r="G54" s="111">
+        <v>17642</v>
+      </c>
+      <c r="H54" s="111">
+        <v>29403</v>
+      </c>
+      <c r="I54" s="111">
+        <v>44105</v>
+      </c>
+      <c r="J54" s="111">
+        <v>61747</v>
+      </c>
+      <c r="K54" s="111">
+        <v>82329</v>
+      </c>
+      <c r="L54" s="111">
+        <v>105851</v>
+      </c>
+      <c r="M54" s="111">
+        <v>132314</v>
+      </c>
+      <c r="N54" s="111">
+        <v>161717</v>
+      </c>
+      <c r="O54" s="111">
+        <v>194061</v>
+      </c>
+      <c r="P54" s="111">
+        <v>229345</v>
+      </c>
+      <c r="Q54" s="111">
+        <v>267569</v>
+      </c>
+      <c r="R54" s="111">
+        <v>308733</v>
+      </c>
+      <c r="S54" s="111">
+        <v>352838</v>
+      </c>
+      <c r="T54" s="111">
+        <v>399883</v>
+      </c>
+      <c r="U54" s="111">
+        <v>449868</v>
+      </c>
+      <c r="V54" s="111">
+        <v>502794</v>
+      </c>
+      <c r="W54" s="111">
+        <v>558660</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
@@ -7551,87 +7694,223 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D55">
         <v>20</v>
       </c>
       <c r="E55">
+        <v>3337</v>
+      </c>
+      <c r="F55">
+        <v>10010</v>
+      </c>
+      <c r="G55">
+        <v>20020</v>
+      </c>
+      <c r="H55">
+        <v>33366</v>
+      </c>
+      <c r="I55">
+        <v>50049</v>
+      </c>
+      <c r="J55">
+        <v>70069</v>
+      </c>
+      <c r="K55">
+        <v>93426</v>
+      </c>
+      <c r="L55">
+        <v>120119</v>
+      </c>
+      <c r="M55">
+        <v>150148</v>
+      </c>
+      <c r="N55">
+        <v>183515</v>
+      </c>
+      <c r="O55">
+        <v>220218</v>
+      </c>
+      <c r="P55">
+        <v>260257</v>
+      </c>
+      <c r="Q55">
+        <v>303633</v>
+      </c>
+      <c r="R55">
+        <v>350346</v>
+      </c>
+      <c r="S55">
+        <v>400396</v>
+      </c>
+      <c r="T55">
+        <v>453782</v>
+      </c>
+      <c r="U55">
+        <v>510505</v>
+      </c>
+      <c r="V55">
+        <v>570564</v>
+      </c>
+      <c r="W55">
+        <v>633960</v>
+      </c>
+    </row>
+    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56">
+        <v>20</v>
+      </c>
+      <c r="E56">
         <v>3741</v>
       </c>
-      <c r="F55">
+      <c r="F56">
         <v>11223</v>
       </c>
-      <c r="G55">
+      <c r="G56">
         <v>22445</v>
       </c>
-      <c r="H55">
+      <c r="H56">
         <v>37409</v>
       </c>
-      <c r="I55">
+      <c r="I56">
         <v>56113</v>
       </c>
-      <c r="J55">
+      <c r="J56">
         <v>78559</v>
       </c>
-      <c r="K55">
+      <c r="K56">
         <v>104745</v>
       </c>
-      <c r="L55">
+      <c r="L56">
         <v>134672</v>
       </c>
-      <c r="M55">
+      <c r="M56">
         <v>168340</v>
       </c>
-      <c r="N55">
+      <c r="N56">
         <v>205749</v>
       </c>
-      <c r="O55">
+      <c r="O56">
         <v>246899</v>
       </c>
-      <c r="P55">
+      <c r="P56">
         <v>291790</v>
       </c>
-      <c r="Q55">
+      <c r="Q56">
         <v>340421</v>
       </c>
-      <c r="R55">
+      <c r="R56">
         <v>392794</v>
       </c>
-      <c r="S55">
+      <c r="S56">
         <v>448907</v>
       </c>
-      <c r="T55">
+      <c r="T56">
         <v>508762</v>
       </c>
-      <c r="U55">
+      <c r="U56">
         <v>572357</v>
       </c>
-      <c r="V55">
+      <c r="V56">
         <v>639693</v>
       </c>
-      <c r="W55">
+      <c r="W56">
+        <v>710770</v>
+      </c>
+    </row>
+    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57">
+        <v>20</v>
+      </c>
+      <c r="E57">
+        <v>3741</v>
+      </c>
+      <c r="F57">
+        <v>11223</v>
+      </c>
+      <c r="G57">
+        <v>22445</v>
+      </c>
+      <c r="H57">
+        <v>37409</v>
+      </c>
+      <c r="I57">
+        <v>56113</v>
+      </c>
+      <c r="J57">
+        <v>78559</v>
+      </c>
+      <c r="K57">
+        <v>104745</v>
+      </c>
+      <c r="L57">
+        <v>134672</v>
+      </c>
+      <c r="M57">
+        <v>168340</v>
+      </c>
+      <c r="N57">
+        <v>205749</v>
+      </c>
+      <c r="O57">
+        <v>246899</v>
+      </c>
+      <c r="P57">
+        <v>291790</v>
+      </c>
+      <c r="Q57">
+        <v>340421</v>
+      </c>
+      <c r="R57">
+        <v>392794</v>
+      </c>
+      <c r="S57">
+        <v>448907</v>
+      </c>
+      <c r="T57">
+        <v>508762</v>
+      </c>
+      <c r="U57">
+        <v>572357</v>
+      </c>
+      <c r="V57">
+        <v>639693</v>
+      </c>
+      <c r="W57">
         <v>710770</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="BD27:BJ27"/>
+    <mergeCell ref="BD28:BJ28"/>
     <mergeCell ref="AO14:AR14"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="W27:AA27"/>
-    <mergeCell ref="AB27:AF27"/>
-    <mergeCell ref="AH27:AI27"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="W28:AA28"/>
+    <mergeCell ref="AB28:AF28"/>
+    <mergeCell ref="AH28:AI28"/>
   </mergeCells>
-  <conditionalFormatting sqref="C16:C23 C25:C26">
+  <conditionalFormatting sqref="C16:C23 C25:C27">
     <cfRule type="duplicateValues" dxfId="99" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
     <cfRule type="duplicateValues" dxfId="98" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM16:BM23 BM25:BM26">
+  <conditionalFormatting sqref="BM16:BM23 BM25:BM27">
     <cfRule type="duplicateValues" dxfId="97" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
@@ -7641,11 +7920,11 @@
     <cfRule type="duplicateValues" dxfId="95" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">
       <formula1>INDIRECT("dragonTierDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D45:D55 F45:W55 E46:E55"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D33:D34 D38:D40">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D46:D57 F46:W57 E47:E57"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D34:D35 D39:D41">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Content - Add order to dragon 12
Former-commit-id: 81a4e9bbbc1edcbf371028460f1ac05781961427
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -3999,8 +3999,8 @@
   </sheetPr>
   <dimension ref="B1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6576,7 +6576,7 @@
         <v>79</v>
       </c>
       <c r="E27" s="57">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F27" s="56" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Content - Add result PF for Dragon 12
Former-commit-id: ec6335fa22fb6c55e3f92855a785bb67c9eaa1d1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="203">
   <si>
     <t>[sku]</t>
   </si>
@@ -630,6 +630,9 @@
   </si>
   <si>
     <t>PF_DragonGoldheistMenu</t>
+  </si>
+  <si>
+    <t>PF_DragonGoldheistResults</t>
   </si>
 </sst>
 </file>
@@ -3999,8 +4002,8 @@
   </sheetPr>
   <dimension ref="B1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="Y13" workbookViewId="0">
+      <selection activeCell="AN27" sqref="AN27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6682,7 +6685,7 @@
         <v>201</v>
       </c>
       <c r="AN27" s="24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AO27" s="24" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Content - XP and prices for Dragon 12 + Global prices rebalancing in SC
Former-commit-id: 802ebcf38b0e8aef31d5cd91f15ef0b319f8fd72
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4002,8 +4002,8 @@
   </sheetPr>
   <dimension ref="B1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y13" workbookViewId="0">
-      <selection activeCell="AN27" sqref="AN27"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4107,7 +4107,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="14" t="str">
-        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
@@ -4128,7 +4128,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="14" t="str">
-        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
@@ -4149,7 +4149,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="96" t="str">
-        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
@@ -4170,7 +4170,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="94" t="str">
-        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="94" t="str">
-        <f ca="1">CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
+        <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
@@ -4513,7 +4513,7 @@
         <v>100</v>
       </c>
       <c r="Y16" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z16" s="29">
@@ -4544,7 +4544,7 @@
         <v>0.23</v>
       </c>
       <c r="AI16" s="67">
-        <f t="shared" ref="AI16:AI23" ca="1" si="0">AH17</f>
+        <f t="shared" ref="AI16:AI23" si="0">AH17</f>
         <v>0.19</v>
       </c>
       <c r="AJ16" s="74">
@@ -4705,7 +4705,7 @@
         <v>100</v>
       </c>
       <c r="Y17" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z17" s="29">
@@ -4736,7 +4736,7 @@
         <v>0.19</v>
       </c>
       <c r="AI17" s="67">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
       <c r="AJ17" s="74">
@@ -4897,7 +4897,7 @@
         <v>100</v>
       </c>
       <c r="Y18" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z18" s="29">
@@ -4928,7 +4928,7 @@
         <v>0.15</v>
       </c>
       <c r="AI18" s="67">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
       <c r="AJ18" s="120">
@@ -5035,7 +5035,7 @@
         <v>7</v>
       </c>
       <c r="G19" s="28">
-        <v>47000</v>
+        <v>35000</v>
       </c>
       <c r="H19" s="27">
         <v>150</v>
@@ -5089,7 +5089,7 @@
         <v>100</v>
       </c>
       <c r="Y19" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z19" s="29">
@@ -5120,7 +5120,7 @@
         <v>0.13</v>
       </c>
       <c r="AI19" s="67">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
       <c r="AJ19" s="74">
@@ -5227,7 +5227,7 @@
         <v>8</v>
       </c>
       <c r="G20" s="28">
-        <v>120000</v>
+        <v>88000</v>
       </c>
       <c r="H20" s="27">
         <v>200</v>
@@ -5281,7 +5281,7 @@
         <v>100</v>
       </c>
       <c r="Y20" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z20" s="29">
@@ -5312,7 +5312,7 @@
         <v>0.11</v>
       </c>
       <c r="AI20" s="67">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
       <c r="AJ20" s="74">
@@ -5473,7 +5473,7 @@
         <v>100</v>
       </c>
       <c r="Y21" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z21" s="29">
@@ -5504,7 +5504,7 @@
         <v>0.09</v>
       </c>
       <c r="AI21" s="67">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
       <c r="AJ21" s="74">
@@ -5665,7 +5665,7 @@
         <v>100</v>
       </c>
       <c r="Y22" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z22" s="29">
@@ -5696,7 +5696,7 @@
         <v>0.08</v>
       </c>
       <c r="AI22" s="67">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ22" s="74">
@@ -5803,7 +5803,7 @@
         <v>11</v>
       </c>
       <c r="G23" s="30">
-        <v>1100000</v>
+        <v>870000</v>
       </c>
       <c r="H23" s="55">
         <v>800</v>
@@ -5857,7 +5857,7 @@
         <v>100</v>
       </c>
       <c r="Y23" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z23" s="29">
@@ -5888,7 +5888,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI23" s="67">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
       <c r="AJ23" s="120">
@@ -5999,7 +5999,7 @@
         <v>12</v>
       </c>
       <c r="G24" s="110">
-        <v>1800000</v>
+        <v>1400000</v>
       </c>
       <c r="H24" s="22">
         <v>800</v>
@@ -6053,7 +6053,7 @@
         <v>100</v>
       </c>
       <c r="Y24" s="50">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z24" s="50">
@@ -6194,7 +6194,7 @@
         <v>184</v>
       </c>
       <c r="G25" s="30">
-        <v>2900000</v>
+        <v>2200000</v>
       </c>
       <c r="H25" s="55">
         <v>800</v>
@@ -6248,7 +6248,7 @@
         <v>100</v>
       </c>
       <c r="Y25" s="29">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z25" s="29">
@@ -6279,7 +6279,7 @@
         <v>0.06</v>
       </c>
       <c r="AI25" s="67">
-        <f ca="1">AH26</f>
+        <f>AH26</f>
         <v>0.05</v>
       </c>
       <c r="AJ25" s="120">
@@ -6390,7 +6390,7 @@
         <v>13</v>
       </c>
       <c r="G26" s="30">
-        <v>4300000</v>
+        <v>3300000</v>
       </c>
       <c r="H26" s="55">
         <v>1100</v>
@@ -6444,7 +6444,7 @@
         <v>100</v>
       </c>
       <c r="Y26" s="26">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z26" s="26">
@@ -6585,7 +6585,7 @@
         <v>14</v>
       </c>
       <c r="G27" s="30">
-        <v>4300000</v>
+        <v>4800000</v>
       </c>
       <c r="H27" s="55">
         <v>1100</v>
@@ -6639,7 +6639,7 @@
         <v>100</v>
       </c>
       <c r="Y27" s="26">
-        <f ca="1">dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="Z27" s="26">
@@ -7839,61 +7839,61 @@
         <v>20</v>
       </c>
       <c r="E57">
-        <v>3741</v>
+        <v>4153</v>
       </c>
       <c r="F57">
-        <v>11223</v>
+        <v>12458</v>
       </c>
       <c r="G57">
-        <v>22445</v>
+        <v>24916</v>
       </c>
       <c r="H57">
-        <v>37409</v>
+        <v>41526</v>
       </c>
       <c r="I57">
-        <v>56113</v>
+        <v>62289</v>
       </c>
       <c r="J57">
-        <v>78559</v>
+        <v>87205</v>
       </c>
       <c r="K57">
-        <v>104745</v>
+        <v>116274</v>
       </c>
       <c r="L57">
-        <v>134672</v>
+        <v>149495</v>
       </c>
       <c r="M57">
-        <v>168340</v>
+        <v>186868</v>
       </c>
       <c r="N57">
-        <v>205749</v>
+        <v>228395</v>
       </c>
       <c r="O57">
-        <v>246899</v>
+        <v>274074</v>
       </c>
       <c r="P57">
-        <v>291790</v>
+        <v>323905</v>
       </c>
       <c r="Q57">
-        <v>340421</v>
+        <v>377889</v>
       </c>
       <c r="R57">
-        <v>392794</v>
+        <v>436026</v>
       </c>
       <c r="S57">
-        <v>448907</v>
+        <v>498316</v>
       </c>
       <c r="T57">
-        <v>508762</v>
+        <v>564758</v>
       </c>
       <c r="U57">
-        <v>572357</v>
+        <v>635353</v>
       </c>
       <c r="V57">
-        <v>639693</v>
+        <v>710100</v>
       </c>
       <c r="W57">
-        <v>710770</v>
+        <v>789000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Content - Skins + Missions modifiers for D12
Former-commit-id: 57ba7ea2e47a0064916ec66e3bcaeab004680668
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -4002,8 +4002,8 @@
   </sheetPr>
   <dimension ref="B1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Dragon Data: Development - Split DragonData class into an abstract shared base and different implementations for CLASSIC and SPECIAL dragons. Dragons: Content - Added "type" column to dragonDefinitions and specialDragonDefinitions tables.
Former-commit-id: 937cbdd097b4172b85c5627b301148f4b8c78c65
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DA5035-0AA0-0648-839A-6DB281F6C8A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="199">
   <si>
     <t>[sku]</t>
   </si>
@@ -615,12 +616,18 @@
   </si>
   <si>
     <t>[petScaleMenu]</t>
+  </si>
+  <si>
+    <t>[type]</t>
+  </si>
+  <si>
+    <t>classic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1534,7 +1541,81 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="100">
+  <dxfs count="101">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3491,56 +3572,6 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3555,98 +3586,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM26" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
-  <autoFilter ref="B15:BM26"/>
-  <tableColumns count="64">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="89"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="87"/>
-    <tableColumn id="3" name="[order]" dataDxfId="86"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="85"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="84"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="83"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="82"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="81"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="80"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="79"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="78"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="77"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="76"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="75"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="74"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="73"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="72"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="71"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="70"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="69"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="68"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="67"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BN26" totalsRowShown="0" headerRowDxfId="100" dataDxfId="98" headerRowBorderDxfId="99" tableBorderDxfId="97" totalsRowBorderDxfId="96">
+  <autoFilter ref="B15:BN26" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
+  <tableColumns count="65">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{dragonDefinitions}" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="94"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[tier]" dataDxfId="93"/>
+    <tableColumn id="65" xr3:uid="{FC0CBF2D-8363-8A46-A4C5-787BE12BCEBD}" name="[type]" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[order]" dataDxfId="92"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[previousDragonSku]" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[unlockPriceCoins]" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[unlockPricePC]" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[cameraDefaultZoom]" dataDxfId="88"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[cameraFarZoom]" dataDxfId="87"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[defaultSize]" dataDxfId="86"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[cameraFrameWidthModifier]" dataDxfId="85"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[healthMin]" dataDxfId="84"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[healthMax]" dataDxfId="83"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[healthDrain]" dataDxfId="82"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="[healthDrainSpacePlus]" dataDxfId="81"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[healthDrainAmpPerSecond]" dataDxfId="80"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[sessionStartHealthDrainTime]" dataDxfId="79"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[sessionStartHealthDrainModifier]" dataDxfId="78"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[scaleMin]" dataDxfId="77"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[scaleMax]" dataDxfId="76"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[speedBase]" dataDxfId="75"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[boostMultiplier]" dataDxfId="74"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[energyBaseMin]" dataDxfId="73"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="[energyBaseMax]" dataDxfId="72">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="65"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="64"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="63"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="62"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="61"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="60"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="59"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="58"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="57"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="56">
-      <calculatedColumnFormula>AH17</calculatedColumnFormula>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[energyDrain]" dataDxfId="71"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[energyRefillRate]" dataDxfId="70"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[furyBaseDamage]" dataDxfId="69"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[furyBaseLength]" dataDxfId="68"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[furyScoreMultiplier]" dataDxfId="67"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[furyBaseDuration]" dataDxfId="66"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[furyMax]" dataDxfId="65"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="[scoreTextThresholdMultiplier]" dataDxfId="64"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[eatSpeedFactorMin]" dataDxfId="63"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="[eatSpeedFactorMax]" dataDxfId="62">
+      <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="55"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="54"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="53"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="52"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="51"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="50"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="49"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="48"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="47"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="46"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="45"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="44"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="43"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="42"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="41"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="40"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="39">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAlcohol]" dataDxfId="61"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[alcoholDrain]" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[gamePrefab]" dataDxfId="59"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[menuPrefab]" dataDxfId="58"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="[resultsPrefab]" dataDxfId="57"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="[shadowFromDragon]" dataDxfId="56"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="[revealFromDragon]" dataDxfId="55"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="[sizeUpMultiplier]" dataDxfId="54"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="[speedUpMultiplier]" dataDxfId="53"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="[biteUpMultiplier]" dataDxfId="52"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="[invincible]" dataDxfId="51"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="[infiniteBoost]" dataDxfId="50"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[eatEverything]" dataDxfId="49"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[modeDuration]" dataDxfId="48"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="[petScale]" dataDxfId="47"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="[petScaleMenu]" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="45">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="38">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[tidDesc]" dataDxfId="44">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="37"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="36"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="35"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="34">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[statsBarRatio]" dataDxfId="43"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[furyBarRatio]" dataDxfId="42"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[forceMin]" dataDxfId="41"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="[forceMax]" dataDxfId="40">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="33"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="32"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="31"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="30"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="29"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="28"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="27"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[mass]" dataDxfId="39"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[friction]" dataDxfId="38"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[gravityModifier]" dataDxfId="37"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[airGravityModifier]" dataDxfId="36"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[waterGravityModifier]" dataDxfId="35"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="[damageAnimationThreshold]" dataDxfId="34"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="[dotAnimationThreshold]" dataDxfId="33"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="[trackingSku]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
-  <autoFilter ref="B4:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="B4:G9" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
-    <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{dragonTierDefinitions}" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="[order]"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[icon]" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[maxPetEquipped]" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3655,62 +3687,62 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B32:I33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="dragonSettings" displayName="dragonSettings" ref="B32:I33" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="B32:I33" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{dragonSettings}" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="[energyRequiredToBoost]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="[superfuryMax]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="[superFuryLengthModifier]"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="[superFuryCoinsMultiplier]"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="[superFuryDurationModifier]"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="[superFuryDamageModifier]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B44:W55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="dragonSettings22" displayName="dragonSettings22" ref="B44:W55" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B44:W55" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <tableColumns count="22">
-    <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
-    <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[maxLevel]"/>
-    <tableColumn id="4" name="[xpLevel1]"/>
-    <tableColumn id="5" name="[xpLevel2]"/>
-    <tableColumn id="6" name="[xpLevel3]"/>
-    <tableColumn id="7" name="[xpLevel4]"/>
-    <tableColumn id="8" name="[xpLevel5]"/>
-    <tableColumn id="9" name="[xpLevel6]"/>
-    <tableColumn id="10" name="[xpLevel7]"/>
-    <tableColumn id="11" name="[xpLevel8]"/>
-    <tableColumn id="12" name="[xpLevel9]"/>
-    <tableColumn id="13" name="[xpLevel10]"/>
-    <tableColumn id="14" name="[xpLevel11]"/>
-    <tableColumn id="15" name="[xpLevel12]"/>
-    <tableColumn id="16" name="[xpLevel13]"/>
-    <tableColumn id="17" name="[xpLevel14]"/>
-    <tableColumn id="18" name="[xpLevel15]"/>
-    <tableColumn id="19" name="[xpLevel16]"/>
-    <tableColumn id="20" name="[xpLevel17]"/>
-    <tableColumn id="21" name="[xpLevel18]"/>
-    <tableColumn id="22" name="[xpLevel19]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{dragonProgressionDefinitions}"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[sku]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[maxLevel]"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[xpLevel1]"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[xpLevel2]"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[xpLevel3]"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="[xpLevel4]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="[xpLevel5]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="[xpLevel6]"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="[xpLevel7]"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="[xpLevel8]"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="[xpLevel9]"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="[xpLevel10]"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="[xpLevel11]"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="[xpLevel12]"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="[xpLevel13]"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="[xpLevel14]"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="[xpLevel15]"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="[xpLevel16]"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0300-000014000000}" name="[xpLevel17]"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0300-000015000000}" name="[xpLevel18]"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0300-000016000000}" name="[xpLevel19]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B37:F40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B37:F40" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="B37:F40" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{dragonHealthModifiersDefinitions}" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="[threshold]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[modifier]" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="[tid]" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3978,43 +4010,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BM55"/>
+  <dimension ref="B1:BN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP13" workbookViewId="0">
-      <selection activeCell="AY27" sqref="AY27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.42578125" customWidth="1"/>
-    <col min="39" max="39" width="18.85546875" customWidth="1"/>
-    <col min="40" max="40" width="23.7109375" customWidth="1"/>
-    <col min="41" max="44" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="32" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.5" customWidth="1"/>
+    <col min="39" max="39" width="18.83203125" customWidth="1"/>
+    <col min="40" max="40" width="23.6640625" customWidth="1"/>
+    <col min="41" max="44" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:66" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:66" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>183</v>
       </c>
@@ -4043,7 +4075,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4051,7 +4083,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:65" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:66" ht="115" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>182</v>
       </c>
@@ -4071,7 +4103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -4092,7 +4124,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -4113,7 +4145,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4134,7 +4166,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4155,7 +4187,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4176,8 +4208,8 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:66" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:66" ht="24" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4206,7 +4238,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:65" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:66" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="J14" s="2" t="s">
         <v>174</v>
       </c>
@@ -4231,7 +4263,7 @@
       <c r="AQ14" s="122"/>
       <c r="AR14" s="122"/>
     </row>
-    <row r="15" spans="2:65" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:66" ht="161" x14ac:dyDescent="0.2">
       <c r="B15" s="75" t="s">
         <v>170</v>
       </c>
@@ -4241,191 +4273,194 @@
       <c r="D15" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="76" t="s">
+      <c r="E15" s="78" t="s">
+        <v>197</v>
+      </c>
+      <c r="F15" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="G15" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="93" t="s">
+      <c r="H15" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="H15" s="92" t="s">
+      <c r="I15" s="92" t="s">
         <v>167</v>
       </c>
-      <c r="I15" s="91" t="s">
+      <c r="J15" s="91" t="s">
         <v>166</v>
       </c>
-      <c r="J15" s="90" t="s">
+      <c r="K15" s="90" t="s">
         <v>165</v>
       </c>
-      <c r="K15" s="89" t="s">
+      <c r="L15" s="89" t="s">
         <v>164</v>
       </c>
-      <c r="L15" s="87" t="s">
+      <c r="M15" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="M15" s="85" t="s">
+      <c r="N15" s="85" t="s">
         <v>162</v>
       </c>
-      <c r="N15" s="89" t="s">
+      <c r="O15" s="89" t="s">
         <v>161</v>
       </c>
-      <c r="O15" s="87" t="s">
+      <c r="P15" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="P15" s="87" t="s">
+      <c r="Q15" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="Q15" s="86" t="s">
+      <c r="R15" s="86" t="s">
         <v>158</v>
       </c>
-      <c r="R15" s="86" t="s">
+      <c r="S15" s="86" t="s">
         <v>157</v>
       </c>
-      <c r="S15" s="86" t="s">
+      <c r="T15" s="86" t="s">
         <v>156</v>
       </c>
-      <c r="T15" s="85" t="s">
+      <c r="U15" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="U15" s="87" t="s">
+      <c r="V15" s="87" t="s">
         <v>154</v>
       </c>
-      <c r="V15" s="88" t="s">
+      <c r="W15" s="88" t="s">
         <v>153</v>
       </c>
-      <c r="W15" s="85" t="s">
+      <c r="X15" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="X15" s="89" t="s">
+      <c r="Y15" s="89" t="s">
         <v>191</v>
       </c>
-      <c r="Y15" s="89" t="s">
+      <c r="Z15" s="89" t="s">
         <v>192</v>
       </c>
-      <c r="Z15" s="89" t="s">
+      <c r="AA15" s="89" t="s">
         <v>151</v>
       </c>
-      <c r="AA15" s="87" t="s">
+      <c r="AB15" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="AB15" s="88" t="s">
+      <c r="AC15" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="AC15" s="87" t="s">
+      <c r="AD15" s="87" t="s">
         <v>148</v>
       </c>
-      <c r="AD15" s="87" t="s">
+      <c r="AE15" s="87" t="s">
         <v>147</v>
       </c>
-      <c r="AE15" s="87" t="s">
+      <c r="AF15" s="87" t="s">
         <v>146</v>
       </c>
-      <c r="AF15" s="116" t="s">
+      <c r="AG15" s="116" t="s">
         <v>145</v>
       </c>
-      <c r="AG15" s="86" t="s">
+      <c r="AH15" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="AH15" s="85" t="s">
+      <c r="AI15" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="AI15" s="85" t="s">
+      <c r="AJ15" s="85" t="s">
         <v>194</v>
       </c>
-      <c r="AJ15" s="85" t="s">
+      <c r="AK15" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="AK15" s="85" t="s">
+      <c r="AL15" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="AL15" s="84" t="s">
+      <c r="AM15" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="AM15" s="82" t="s">
+      <c r="AN15" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="AN15" s="82" t="s">
+      <c r="AO15" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="AO15" s="82" t="s">
+      <c r="AP15" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="AP15" s="82" t="s">
+      <c r="AQ15" s="82" t="s">
         <v>139</v>
       </c>
-      <c r="AQ15" s="82" t="s">
+      <c r="AR15" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="AR15" s="83" t="s">
+      <c r="AS15" s="83" t="s">
         <v>137</v>
       </c>
-      <c r="AS15" s="82" t="s">
+      <c r="AT15" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="AT15" s="82" t="s">
+      <c r="AU15" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="AU15" s="82" t="s">
+      <c r="AV15" s="82" t="s">
         <v>134</v>
       </c>
-      <c r="AV15" s="82" t="s">
+      <c r="AW15" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="AW15" s="82" t="s">
+      <c r="AX15" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="AX15" s="82" t="s">
+      <c r="AY15" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="AY15" s="82" t="s">
+      <c r="AZ15" s="82" t="s">
         <v>196</v>
       </c>
-      <c r="AZ15" s="3" t="s">
+      <c r="BA15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BA15" s="81" t="s">
+      <c r="BB15" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="BB15" s="80" t="s">
+      <c r="BC15" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="BC15" s="76" t="s">
+      <c r="BD15" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="BD15" s="79" t="s">
+      <c r="BE15" s="79" t="s">
         <v>189</v>
       </c>
-      <c r="BE15" s="75" t="s">
+      <c r="BF15" s="75" t="s">
         <v>190</v>
       </c>
-      <c r="BF15" s="78" t="s">
+      <c r="BG15" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="BG15" s="78" t="s">
+      <c r="BH15" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="BH15" s="78" t="s">
+      <c r="BI15" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="BI15" s="75" t="s">
+      <c r="BJ15" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="BJ15" s="75" t="s">
+      <c r="BK15" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="BK15" s="77" t="s">
+      <c r="BL15" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="BL15" s="76" t="s">
+      <c r="BM15" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="BM15" s="75" t="s">
+      <c r="BN15" s="75" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4435,127 +4470,127 @@
       <c r="D16" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="57">
+      <c r="E16" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="57">
         <v>0</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="28">
+      <c r="G16" s="57"/>
+      <c r="H16" s="28">
         <v>0</v>
       </c>
-      <c r="H16" s="27">
+      <c r="I16" s="27">
         <v>0</v>
       </c>
-      <c r="I16" s="70">
+      <c r="J16" s="70">
         <v>35</v>
       </c>
-      <c r="J16" s="69">
+      <c r="K16" s="69">
         <v>45</v>
       </c>
-      <c r="K16" s="25">
+      <c r="L16" s="25">
         <v>1</v>
       </c>
-      <c r="L16" s="65">
+      <c r="M16" s="65">
         <v>-2</v>
       </c>
-      <c r="M16" s="64">
+      <c r="N16" s="64">
         <v>75</v>
       </c>
-      <c r="N16" s="29">
+      <c r="O16" s="29">
         <v>105</v>
       </c>
-      <c r="O16" s="29">
+      <c r="P16" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P16" s="29">
+      <c r="Q16" s="29">
         <v>0</v>
       </c>
-      <c r="Q16" s="29">
+      <c r="R16" s="29">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="R16" s="50">
+      <c r="S16" s="50">
         <v>30</v>
       </c>
-      <c r="S16" s="50">
+      <c r="T16" s="50">
         <v>0.5</v>
       </c>
-      <c r="T16" s="64">
+      <c r="U16" s="64">
         <v>0.46</v>
       </c>
-      <c r="U16" s="29">
+      <c r="V16" s="29">
         <v>0.71</v>
       </c>
-      <c r="V16" s="68">
+      <c r="W16" s="68">
         <v>14</v>
       </c>
-      <c r="W16" s="29">
+      <c r="X16" s="29">
         <v>1.95</v>
       </c>
-      <c r="X16" s="29">
+      <c r="Y16" s="29">
         <v>100</v>
       </c>
-      <c r="Y16" s="29">
+      <c r="Z16" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z16" s="29">
+      <c r="AA16" s="29">
         <v>40</v>
       </c>
-      <c r="AA16" s="29">
+      <c r="AB16" s="29">
         <v>28</v>
       </c>
-      <c r="AB16" s="68">
+      <c r="AC16" s="68">
         <v>250</v>
       </c>
-      <c r="AC16" s="50">
+      <c r="AD16" s="50">
         <v>7.5</v>
       </c>
-      <c r="AD16" s="29">
+      <c r="AE16" s="29">
         <v>2</v>
       </c>
-      <c r="AE16" s="50">
+      <c r="AF16" s="50">
         <v>8</v>
       </c>
-      <c r="AF16" s="29">
+      <c r="AG16" s="29">
         <v>3000</v>
       </c>
-      <c r="AG16" s="67">
+      <c r="AH16" s="67">
         <v>1</v>
       </c>
-      <c r="AH16" s="117">
+      <c r="AI16" s="117">
         <v>0.23</v>
       </c>
-      <c r="AI16" s="67">
-        <f t="shared" ref="AI16:AI25" si="0">AH17</f>
+      <c r="AJ16" s="67">
+        <f t="shared" ref="AJ16:AJ25" si="0">AI17</f>
         <v>0.19</v>
       </c>
-      <c r="AJ16" s="74">
+      <c r="AK16" s="74">
         <v>0</v>
       </c>
-      <c r="AK16" s="74">
+      <c r="AL16" s="74">
         <v>12</v>
       </c>
-      <c r="AL16" s="24" t="s">
+      <c r="AM16" s="24" t="s">
         <v>120</v>
-      </c>
-      <c r="AM16" s="24" t="s">
-        <v>119</v>
       </c>
       <c r="AN16" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="AO16" s="24"/>
+      <c r="AO16" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="AP16" s="24"/>
-      <c r="AQ16" s="24">
+      <c r="AQ16" s="24"/>
+      <c r="AR16" s="24">
         <v>4.0999999999999996</v>
-      </c>
-      <c r="AR16" s="24">
-        <v>2</v>
       </c>
       <c r="AS16" s="24">
         <v>2</v>
       </c>
-      <c r="AT16" s="24" t="b">
-        <v>1</v>
+      <c r="AT16" s="24">
+        <v>2</v>
       </c>
       <c r="AU16" s="24" t="b">
         <v>1</v>
@@ -4563,59 +4598,62 @@
       <c r="AV16" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW16" s="24">
+      <c r="AW16" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX16" s="24">
         <v>23</v>
       </c>
-      <c r="AX16" s="24">
+      <c r="AY16" s="24">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AY16" s="24">
+      <c r="AZ16" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ16" s="72" t="s">
+      <c r="BA16" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="BA16" s="71" t="s">
+      <c r="BB16" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="BB16" s="41">
+      <c r="BC16" s="41">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="BC16" s="40">
+      <c r="BD16" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD16" s="39">
+      <c r="BE16" s="39">
         <v>175</v>
       </c>
-      <c r="BE16" s="112">
+      <c r="BF16" s="112">
         <v>200</v>
       </c>
-      <c r="BF16" s="58">
+      <c r="BG16" s="58">
         <v>2</v>
       </c>
-      <c r="BG16" s="58">
+      <c r="BH16" s="58">
         <v>9.5</v>
       </c>
-      <c r="BH16" s="58">
+      <c r="BI16" s="58">
         <v>1</v>
       </c>
-      <c r="BI16" s="73">
+      <c r="BJ16" s="73">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BJ16" s="73">
+      <c r="BK16" s="73">
         <v>1.75</v>
       </c>
-      <c r="BK16" s="73">
+      <c r="BL16" s="73">
         <v>0</v>
       </c>
-      <c r="BL16" s="73">
+      <c r="BM16" s="73">
         <v>8</v>
       </c>
-      <c r="BM16" s="58" t="s">
+      <c r="BN16" s="58" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -4625,129 +4663,129 @@
       <c r="D17" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="57">
+      <c r="E17" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17" s="57">
         <v>1</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="G17" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="28">
+      <c r="H17" s="28">
         <v>2000</v>
       </c>
-      <c r="H17" s="27">
+      <c r="I17" s="27">
         <v>60</v>
       </c>
-      <c r="I17" s="70">
+      <c r="J17" s="70">
         <v>35</v>
       </c>
-      <c r="J17" s="69">
+      <c r="K17" s="69">
         <v>45</v>
       </c>
-      <c r="K17" s="25">
+      <c r="L17" s="25">
         <v>3</v>
       </c>
-      <c r="L17" s="65">
+      <c r="M17" s="65">
         <v>-2</v>
       </c>
-      <c r="M17" s="64">
+      <c r="N17" s="64">
         <v>95</v>
       </c>
-      <c r="N17" s="29">
+      <c r="O17" s="29">
         <v>145</v>
       </c>
-      <c r="O17" s="29">
+      <c r="P17" s="29">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P17" s="29">
+      <c r="Q17" s="29">
         <v>0</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="R17" s="29">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="R17" s="50">
+      <c r="S17" s="50">
         <v>30</v>
       </c>
-      <c r="S17" s="50">
+      <c r="T17" s="50">
         <v>0.5</v>
       </c>
-      <c r="T17" s="46">
+      <c r="U17" s="46">
         <v>0.8</v>
       </c>
-      <c r="U17" s="26">
+      <c r="V17" s="26">
         <v>0.95</v>
       </c>
-      <c r="V17" s="68">
+      <c r="W17" s="68">
         <v>16</v>
       </c>
-      <c r="W17" s="29">
+      <c r="X17" s="29">
         <v>1.75</v>
       </c>
-      <c r="X17" s="29">
+      <c r="Y17" s="29">
         <v>100</v>
       </c>
-      <c r="Y17" s="29">
+      <c r="Z17" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z17" s="29">
+      <c r="AA17" s="29">
         <v>20</v>
       </c>
-      <c r="AA17" s="29">
+      <c r="AB17" s="29">
         <v>10</v>
       </c>
-      <c r="AB17" s="68">
+      <c r="AC17" s="68">
         <v>275</v>
       </c>
-      <c r="AC17" s="50">
+      <c r="AD17" s="50">
         <v>8</v>
       </c>
-      <c r="AD17" s="29">
+      <c r="AE17" s="29">
         <v>3</v>
       </c>
-      <c r="AE17" s="50">
+      <c r="AF17" s="50">
         <v>9</v>
       </c>
-      <c r="AF17" s="29">
+      <c r="AG17" s="29">
         <v>7000</v>
       </c>
-      <c r="AG17" s="67">
+      <c r="AH17" s="67">
         <v>2</v>
       </c>
-      <c r="AH17" s="117">
+      <c r="AI17" s="117">
         <v>0.19</v>
       </c>
-      <c r="AI17" s="67">
+      <c r="AJ17" s="67">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="AJ17" s="74">
+      <c r="AK17" s="74">
         <v>0</v>
       </c>
-      <c r="AK17" s="45">
+      <c r="AL17" s="45">
         <v>12</v>
       </c>
-      <c r="AL17" s="44" t="s">
+      <c r="AM17" s="44" t="s">
         <v>116</v>
-      </c>
-      <c r="AM17" s="24" t="s">
-        <v>115</v>
       </c>
       <c r="AN17" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="AO17" s="24"/>
+      <c r="AO17" s="24" t="s">
+        <v>115</v>
+      </c>
       <c r="AP17" s="24"/>
-      <c r="AQ17" s="24">
+      <c r="AQ17" s="24"/>
+      <c r="AR17" s="24">
         <v>2.2999999999999998</v>
-      </c>
-      <c r="AR17" s="24">
-        <v>2</v>
       </c>
       <c r="AS17" s="24">
         <v>2</v>
       </c>
-      <c r="AT17" s="24" t="b">
-        <v>1</v>
+      <c r="AT17" s="24">
+        <v>2</v>
       </c>
       <c r="AU17" s="24" t="b">
         <v>1</v>
@@ -4755,59 +4793,62 @@
       <c r="AV17" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW17" s="24">
+      <c r="AW17" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX17" s="24">
         <v>23</v>
       </c>
-      <c r="AX17" s="24">
+      <c r="AY17" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY17" s="24">
+      <c r="AZ17" s="24">
         <v>0.8</v>
       </c>
-      <c r="AZ17" s="72" t="s">
+      <c r="BA17" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="BA17" s="71" t="s">
+      <c r="BB17" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="BB17" s="41">
+      <c r="BC17" s="41">
         <v>2.3E-3</v>
       </c>
-      <c r="BC17" s="40">
+      <c r="BD17" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD17" s="39">
+      <c r="BE17" s="39">
         <v>210</v>
       </c>
-      <c r="BE17" s="112">
+      <c r="BF17" s="112">
         <v>235</v>
       </c>
-      <c r="BF17" s="58">
+      <c r="BG17" s="58">
         <v>2.1</v>
       </c>
-      <c r="BG17" s="58">
+      <c r="BH17" s="58">
         <v>9.5</v>
       </c>
-      <c r="BH17" s="58">
+      <c r="BI17" s="58">
         <v>1.7</v>
       </c>
-      <c r="BI17" s="58">
+      <c r="BJ17" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BJ17" s="58">
+      <c r="BK17" s="58">
         <v>2.1</v>
       </c>
-      <c r="BK17" s="58">
+      <c r="BL17" s="58">
         <v>0</v>
       </c>
-      <c r="BL17" s="58">
+      <c r="BM17" s="58">
         <v>8</v>
       </c>
-      <c r="BM17" s="58" t="s">
+      <c r="BN17" s="58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -4817,129 +4858,129 @@
       <c r="D18" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="57">
+      <c r="E18" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18" s="57">
         <v>2</v>
       </c>
-      <c r="F18" s="57" t="s">
+      <c r="G18" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="30">
+      <c r="H18" s="30">
         <v>11000</v>
       </c>
-      <c r="H18" s="55">
+      <c r="I18" s="55">
         <v>100</v>
       </c>
-      <c r="I18" s="54">
+      <c r="J18" s="54">
         <v>35</v>
       </c>
-      <c r="J18" s="66">
+      <c r="K18" s="66">
         <v>45</v>
       </c>
-      <c r="K18" s="25">
+      <c r="L18" s="25">
         <v>5</v>
       </c>
-      <c r="L18" s="65">
+      <c r="M18" s="65">
         <v>-2</v>
       </c>
-      <c r="M18" s="64">
+      <c r="N18" s="64">
         <v>140</v>
       </c>
-      <c r="N18" s="26">
+      <c r="O18" s="26">
         <v>200</v>
       </c>
-      <c r="O18" s="26">
+      <c r="P18" s="26">
         <v>1.5</v>
       </c>
-      <c r="P18" s="26">
+      <c r="Q18" s="26">
         <v>0</v>
       </c>
-      <c r="Q18" s="29">
+      <c r="R18" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="R18" s="50">
+      <c r="S18" s="50">
         <v>30</v>
       </c>
-      <c r="S18" s="50">
+      <c r="T18" s="50">
         <v>0.5</v>
       </c>
-      <c r="T18" s="64">
+      <c r="U18" s="64">
         <v>0.85</v>
       </c>
-      <c r="U18" s="29">
+      <c r="V18" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V18" s="49">
+      <c r="W18" s="49">
         <v>23.5</v>
       </c>
-      <c r="W18" s="29">
+      <c r="X18" s="29">
         <v>2.0099999999999998</v>
       </c>
-      <c r="X18" s="29">
+      <c r="Y18" s="29">
         <v>100</v>
       </c>
-      <c r="Y18" s="29">
+      <c r="Z18" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z18" s="29">
+      <c r="AA18" s="29">
         <v>40</v>
       </c>
-      <c r="AA18" s="29">
+      <c r="AB18" s="29">
         <v>14</v>
       </c>
-      <c r="AB18" s="49">
+      <c r="AC18" s="49">
         <v>300</v>
       </c>
-      <c r="AC18" s="50">
+      <c r="AD18" s="50">
         <v>9</v>
       </c>
-      <c r="AD18" s="26">
+      <c r="AE18" s="26">
         <v>3</v>
       </c>
-      <c r="AE18" s="63">
+      <c r="AF18" s="63">
         <v>9</v>
       </c>
-      <c r="AF18" s="29">
+      <c r="AG18" s="29">
         <v>8000</v>
       </c>
-      <c r="AG18" s="62">
+      <c r="AH18" s="62">
         <v>2</v>
       </c>
-      <c r="AH18" s="118">
+      <c r="AI18" s="118">
         <v>0.15</v>
       </c>
-      <c r="AI18" s="67">
+      <c r="AJ18" s="67">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="AJ18" s="120">
+      <c r="AK18" s="120">
         <v>0</v>
       </c>
-      <c r="AK18" s="61">
+      <c r="AL18" s="61">
         <v>12</v>
       </c>
-      <c r="AL18" s="44" t="s">
+      <c r="AM18" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="AM18" s="24" t="s">
+      <c r="AN18" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="AN18" s="24" t="s">
+      <c r="AO18" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AO18" s="24"/>
       <c r="AP18" s="24"/>
-      <c r="AQ18" s="24">
+      <c r="AQ18" s="24"/>
+      <c r="AR18" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AR18" s="24">
-        <v>2</v>
       </c>
       <c r="AS18" s="24">
         <v>2</v>
       </c>
-      <c r="AT18" s="24" t="b">
-        <v>1</v>
+      <c r="AT18" s="24">
+        <v>2</v>
       </c>
       <c r="AU18" s="24" t="b">
         <v>1</v>
@@ -4947,59 +4988,62 @@
       <c r="AV18" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW18" s="24">
+      <c r="AW18" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX18" s="24">
         <v>23</v>
-      </c>
-      <c r="AX18" s="24">
-        <v>0.7</v>
       </c>
       <c r="AY18" s="24">
         <v>0.7</v>
       </c>
-      <c r="AZ18" s="60" t="s">
+      <c r="AZ18" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="BA18" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="BA18" s="59" t="s">
+      <c r="BB18" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="BB18" s="41">
+      <c r="BC18" s="41">
         <v>2E-3</v>
       </c>
-      <c r="BC18" s="40">
+      <c r="BD18" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD18" s="39">
+      <c r="BE18" s="39">
         <v>240</v>
       </c>
-      <c r="BE18" s="112">
+      <c r="BF18" s="112">
         <v>280</v>
       </c>
-      <c r="BF18" s="58">
+      <c r="BG18" s="58">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BG18" s="58">
+      <c r="BH18" s="58">
         <v>9.5</v>
       </c>
-      <c r="BH18" s="58">
+      <c r="BI18" s="58">
         <v>1.7</v>
       </c>
-      <c r="BI18" s="58">
+      <c r="BJ18" s="58">
         <v>0.9</v>
       </c>
-      <c r="BJ18" s="58">
+      <c r="BK18" s="58">
         <v>2.25</v>
       </c>
-      <c r="BK18" s="58">
+      <c r="BL18" s="58">
         <v>0</v>
       </c>
-      <c r="BL18" s="58">
+      <c r="BM18" s="58">
         <v>8</v>
       </c>
-      <c r="BM18" s="37" t="s">
+      <c r="BN18" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -5009,129 +5053,129 @@
       <c r="D19" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="57">
+      <c r="E19" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F19" s="57">
         <v>3</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="G19" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="28">
+      <c r="H19" s="28">
         <v>47000</v>
       </c>
-      <c r="H19" s="27">
+      <c r="I19" s="27">
         <v>150</v>
       </c>
-      <c r="I19" s="70">
+      <c r="J19" s="70">
         <v>35</v>
       </c>
-      <c r="J19" s="69">
+      <c r="K19" s="69">
         <v>45</v>
       </c>
-      <c r="K19" s="25">
+      <c r="L19" s="25">
         <v>6</v>
       </c>
-      <c r="L19" s="65">
+      <c r="M19" s="65">
         <v>-2</v>
       </c>
-      <c r="M19" s="64">
+      <c r="N19" s="64">
         <v>190</v>
       </c>
-      <c r="N19" s="29">
+      <c r="O19" s="29">
         <v>240</v>
       </c>
-      <c r="O19" s="29">
+      <c r="P19" s="29">
         <v>1.44</v>
       </c>
-      <c r="P19" s="29">
+      <c r="Q19" s="29">
         <v>0</v>
       </c>
-      <c r="Q19" s="29">
+      <c r="R19" s="29">
         <v>0.01</v>
       </c>
-      <c r="R19" s="50">
+      <c r="S19" s="50">
         <v>30</v>
       </c>
-      <c r="S19" s="50">
+      <c r="T19" s="50">
         <v>0.6</v>
       </c>
-      <c r="T19" s="46">
+      <c r="U19" s="46">
         <v>0.9</v>
       </c>
-      <c r="U19" s="26">
+      <c r="V19" s="26">
         <v>1.1499999999999999</v>
       </c>
-      <c r="V19" s="68">
+      <c r="W19" s="68">
         <v>19</v>
       </c>
-      <c r="W19" s="29">
+      <c r="X19" s="29">
         <v>1.3</v>
       </c>
-      <c r="X19" s="29">
+      <c r="Y19" s="29">
         <v>100</v>
       </c>
-      <c r="Y19" s="29">
+      <c r="Z19" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z19" s="29">
+      <c r="AA19" s="29">
         <v>18</v>
       </c>
-      <c r="AA19" s="26">
+      <c r="AB19" s="26">
         <v>22</v>
       </c>
-      <c r="AB19" s="68">
+      <c r="AC19" s="68">
         <v>325</v>
       </c>
-      <c r="AC19" s="50">
+      <c r="AD19" s="50">
         <v>10</v>
       </c>
-      <c r="AD19" s="29">
+      <c r="AE19" s="29">
         <v>4</v>
       </c>
-      <c r="AE19" s="50">
+      <c r="AF19" s="50">
         <v>9</v>
       </c>
-      <c r="AF19" s="29">
+      <c r="AG19" s="29">
         <v>9000</v>
       </c>
-      <c r="AG19" s="67">
+      <c r="AH19" s="67">
         <v>2</v>
       </c>
-      <c r="AH19" s="117">
+      <c r="AI19" s="117">
         <v>0.13</v>
       </c>
-      <c r="AI19" s="67">
+      <c r="AJ19" s="67">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="AJ19" s="74">
+      <c r="AK19" s="74">
         <v>0</v>
       </c>
-      <c r="AK19" s="45">
+      <c r="AL19" s="45">
         <v>12</v>
       </c>
-      <c r="AL19" s="44" t="s">
+      <c r="AM19" s="44" t="s">
         <v>106</v>
-      </c>
-      <c r="AM19" s="24" t="s">
-        <v>105</v>
       </c>
       <c r="AN19" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="AO19" s="24"/>
+      <c r="AO19" s="24" t="s">
+        <v>105</v>
+      </c>
       <c r="AP19" s="24"/>
-      <c r="AQ19" s="24">
+      <c r="AQ19" s="24"/>
+      <c r="AR19" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AR19" s="24">
-        <v>2</v>
       </c>
       <c r="AS19" s="24">
         <v>2</v>
       </c>
-      <c r="AT19" s="24" t="b">
-        <v>1</v>
+      <c r="AT19" s="24">
+        <v>2</v>
       </c>
       <c r="AU19" s="24" t="b">
         <v>1</v>
@@ -5139,59 +5183,62 @@
       <c r="AV19" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW19" s="24">
+      <c r="AW19" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX19" s="24">
         <v>23</v>
-      </c>
-      <c r="AX19" s="24">
-        <v>0.7</v>
       </c>
       <c r="AY19" s="24">
         <v>0.7</v>
       </c>
-      <c r="AZ19" s="60" t="s">
+      <c r="AZ19" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="BA19" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="BA19" s="59" t="s">
+      <c r="BB19" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="BB19" s="41">
+      <c r="BC19" s="41">
         <v>2E-3</v>
       </c>
-      <c r="BC19" s="40">
+      <c r="BD19" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD19" s="39">
+      <c r="BE19" s="39">
         <v>345</v>
       </c>
-      <c r="BE19" s="112">
+      <c r="BF19" s="112">
         <v>365</v>
       </c>
-      <c r="BF19" s="58">
+      <c r="BG19" s="58">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BG19" s="58">
+      <c r="BH19" s="58">
         <v>5</v>
       </c>
-      <c r="BH19" s="58">
+      <c r="BI19" s="58">
         <v>0.5</v>
       </c>
-      <c r="BI19" s="58">
+      <c r="BJ19" s="58">
         <v>1.2</v>
       </c>
-      <c r="BJ19" s="58">
+      <c r="BK19" s="58">
         <v>0.77</v>
       </c>
-      <c r="BK19" s="58">
+      <c r="BL19" s="58">
         <v>0</v>
       </c>
-      <c r="BL19" s="58">
+      <c r="BM19" s="58">
         <v>8</v>
       </c>
-      <c r="BM19" s="37" t="s">
+      <c r="BN19" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5201,129 +5248,129 @@
       <c r="D20" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="57">
+      <c r="E20" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20" s="57">
         <v>4</v>
       </c>
-      <c r="F20" s="57" t="s">
+      <c r="G20" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="28">
+      <c r="H20" s="28">
         <v>120000</v>
       </c>
-      <c r="H20" s="27">
+      <c r="I20" s="27">
         <v>200</v>
       </c>
-      <c r="I20" s="70">
+      <c r="J20" s="70">
         <v>35</v>
       </c>
-      <c r="J20" s="69">
+      <c r="K20" s="69">
         <v>45</v>
       </c>
-      <c r="K20" s="25">
+      <c r="L20" s="25">
         <v>8</v>
       </c>
-      <c r="L20" s="65">
+      <c r="M20" s="65">
         <v>0</v>
       </c>
-      <c r="M20" s="64">
+      <c r="N20" s="64">
         <v>210</v>
       </c>
-      <c r="N20" s="29">
+      <c r="O20" s="29">
         <v>270</v>
       </c>
-      <c r="O20" s="29">
+      <c r="P20" s="29">
         <v>1.7</v>
       </c>
-      <c r="P20" s="29">
+      <c r="Q20" s="29">
         <v>0</v>
       </c>
-      <c r="Q20" s="29">
+      <c r="R20" s="29">
         <v>1.2E-2</v>
       </c>
-      <c r="R20" s="50">
+      <c r="S20" s="50">
         <v>30</v>
       </c>
-      <c r="S20" s="50">
+      <c r="T20" s="50">
         <v>0.6</v>
       </c>
-      <c r="T20" s="64">
+      <c r="U20" s="64">
         <v>1</v>
       </c>
-      <c r="U20" s="29">
+      <c r="V20" s="29">
         <v>1.25</v>
       </c>
-      <c r="V20" s="68">
+      <c r="W20" s="68">
         <v>20</v>
       </c>
-      <c r="W20" s="29">
+      <c r="X20" s="29">
         <v>1.4</v>
       </c>
-      <c r="X20" s="29">
+      <c r="Y20" s="29">
         <v>100</v>
       </c>
-      <c r="Y20" s="29">
+      <c r="Z20" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z20" s="29">
+      <c r="AA20" s="29">
         <v>31</v>
       </c>
-      <c r="AA20" s="29">
+      <c r="AB20" s="29">
         <v>34</v>
       </c>
-      <c r="AB20" s="68">
+      <c r="AC20" s="68">
         <v>350</v>
       </c>
-      <c r="AC20" s="50">
+      <c r="AD20" s="50">
         <v>11</v>
       </c>
-      <c r="AD20" s="29">
+      <c r="AE20" s="29">
         <v>4</v>
       </c>
-      <c r="AE20" s="50">
+      <c r="AF20" s="50">
         <v>10</v>
       </c>
-      <c r="AF20" s="29">
+      <c r="AG20" s="29">
         <v>10000</v>
       </c>
-      <c r="AG20" s="67">
+      <c r="AH20" s="67">
         <v>3</v>
       </c>
-      <c r="AH20" s="117">
+      <c r="AI20" s="117">
         <v>0.11</v>
       </c>
-      <c r="AI20" s="67">
+      <c r="AJ20" s="67">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="AJ20" s="74">
+      <c r="AK20" s="74">
         <v>0</v>
       </c>
-      <c r="AK20" s="45">
+      <c r="AL20" s="45">
         <v>12</v>
       </c>
-      <c r="AL20" s="44" t="s">
+      <c r="AM20" s="44" t="s">
         <v>102</v>
-      </c>
-      <c r="AM20" s="24" t="s">
-        <v>101</v>
       </c>
       <c r="AN20" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="AO20" s="24"/>
+      <c r="AO20" s="24" t="s">
+        <v>101</v>
+      </c>
       <c r="AP20" s="24"/>
-      <c r="AQ20" s="24">
+      <c r="AQ20" s="24"/>
+      <c r="AR20" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AR20" s="24">
-        <v>2</v>
       </c>
       <c r="AS20" s="24">
         <v>2</v>
       </c>
-      <c r="AT20" s="24" t="b">
-        <v>1</v>
+      <c r="AT20" s="24">
+        <v>2</v>
       </c>
       <c r="AU20" s="24" t="b">
         <v>1</v>
@@ -5331,59 +5378,62 @@
       <c r="AV20" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW20" s="24">
+      <c r="AW20" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX20" s="24">
         <v>23</v>
       </c>
-      <c r="AX20" s="24">
+      <c r="AY20" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY20" s="24">
+      <c r="AZ20" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ20" s="60" t="s">
+      <c r="BA20" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="BA20" s="59" t="s">
+      <c r="BB20" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="BB20" s="41">
+      <c r="BC20" s="41">
         <v>1.9E-3</v>
       </c>
-      <c r="BC20" s="40">
+      <c r="BD20" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD20" s="39">
+      <c r="BE20" s="39">
         <v>310</v>
       </c>
-      <c r="BE20" s="112">
+      <c r="BF20" s="112">
         <v>335</v>
       </c>
-      <c r="BF20" s="58">
+      <c r="BG20" s="58">
         <v>2.4</v>
       </c>
-      <c r="BG20" s="58">
+      <c r="BH20" s="58">
         <v>9.5</v>
       </c>
-      <c r="BH20" s="58">
+      <c r="BI20" s="58">
         <v>1.7</v>
       </c>
-      <c r="BI20" s="58">
+      <c r="BJ20" s="58">
         <v>1</v>
       </c>
-      <c r="BJ20" s="58">
+      <c r="BK20" s="58">
         <v>1.6</v>
       </c>
-      <c r="BK20" s="58">
+      <c r="BL20" s="58">
         <v>9</v>
       </c>
-      <c r="BL20" s="58">
+      <c r="BM20" s="58">
         <v>8</v>
       </c>
-      <c r="BM20" s="37" t="s">
+      <c r="BN20" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5393,129 +5443,129 @@
       <c r="D21" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="57">
+      <c r="E21" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" s="57">
         <v>5</v>
       </c>
-      <c r="F21" s="57" t="s">
+      <c r="G21" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="28">
+      <c r="H21" s="28">
         <v>260000</v>
       </c>
-      <c r="H21" s="27">
+      <c r="I21" s="27">
         <v>400</v>
       </c>
-      <c r="I21" s="70">
+      <c r="J21" s="70">
         <v>35</v>
       </c>
-      <c r="J21" s="69">
+      <c r="K21" s="69">
         <v>45</v>
       </c>
-      <c r="K21" s="25">
+      <c r="L21" s="25">
         <v>10</v>
       </c>
-      <c r="L21" s="65">
+      <c r="M21" s="65">
         <v>0</v>
       </c>
-      <c r="M21" s="64">
+      <c r="N21" s="64">
         <v>250</v>
       </c>
-      <c r="N21" s="26">
+      <c r="O21" s="26">
         <v>310</v>
       </c>
-      <c r="O21" s="26">
+      <c r="P21" s="26">
         <v>1.9</v>
       </c>
-      <c r="P21" s="26">
+      <c r="Q21" s="26">
         <v>0</v>
       </c>
-      <c r="Q21" s="29">
+      <c r="R21" s="29">
         <v>1.2E-2</v>
       </c>
-      <c r="R21" s="50">
+      <c r="S21" s="50">
         <v>30</v>
       </c>
-      <c r="S21" s="50">
+      <c r="T21" s="50">
         <v>0.6</v>
       </c>
-      <c r="T21" s="64">
+      <c r="U21" s="64">
         <v>1.05</v>
       </c>
-      <c r="U21" s="29">
+      <c r="V21" s="29">
         <v>1.3</v>
       </c>
-      <c r="V21" s="68">
+      <c r="W21" s="68">
         <v>21</v>
       </c>
-      <c r="W21" s="29">
+      <c r="X21" s="29">
         <v>2.0099999999999998</v>
       </c>
-      <c r="X21" s="29">
+      <c r="Y21" s="29">
         <v>100</v>
       </c>
-      <c r="Y21" s="29">
+      <c r="Z21" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z21" s="29">
+      <c r="AA21" s="29">
         <v>50</v>
       </c>
-      <c r="AA21" s="29">
+      <c r="AB21" s="29">
         <v>14</v>
       </c>
-      <c r="AB21" s="68">
+      <c r="AC21" s="68">
         <v>375</v>
       </c>
-      <c r="AC21" s="50">
+      <c r="AD21" s="50">
         <v>11</v>
       </c>
-      <c r="AD21" s="29">
+      <c r="AE21" s="29">
         <v>4</v>
       </c>
-      <c r="AE21" s="50">
+      <c r="AF21" s="50">
         <v>10</v>
       </c>
-      <c r="AF21" s="29">
+      <c r="AG21" s="29">
         <v>10000</v>
       </c>
-      <c r="AG21" s="67">
+      <c r="AH21" s="67">
         <v>3</v>
       </c>
-      <c r="AH21" s="117">
+      <c r="AI21" s="117">
         <v>0.09</v>
       </c>
-      <c r="AI21" s="67">
+      <c r="AJ21" s="67">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="AJ21" s="74">
+      <c r="AK21" s="74">
         <v>0</v>
       </c>
-      <c r="AK21" s="45">
+      <c r="AL21" s="45">
         <v>12</v>
       </c>
-      <c r="AL21" s="44" t="s">
+      <c r="AM21" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="AM21" s="24" t="s">
+      <c r="AN21" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AN21" s="24" t="s">
+      <c r="AO21" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AO21" s="24"/>
       <c r="AP21" s="24"/>
-      <c r="AQ21" s="24">
-        <v>2</v>
-      </c>
+      <c r="AQ21" s="24"/>
       <c r="AR21" s="24">
         <v>2</v>
       </c>
       <c r="AS21" s="24">
         <v>2</v>
       </c>
-      <c r="AT21" s="24" t="b">
-        <v>1</v>
+      <c r="AT21" s="24">
+        <v>2</v>
       </c>
       <c r="AU21" s="24" t="b">
         <v>1</v>
@@ -5523,59 +5573,62 @@
       <c r="AV21" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW21" s="24">
+      <c r="AW21" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX21" s="24">
         <v>23</v>
       </c>
-      <c r="AX21" s="24">
+      <c r="AY21" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY21" s="24">
+      <c r="AZ21" s="24">
         <v>0.5</v>
       </c>
-      <c r="AZ21" s="60" t="s">
+      <c r="BA21" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="BA21" s="59" t="s">
+      <c r="BB21" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="BB21" s="41">
+      <c r="BC21" s="41">
         <v>1.8E-3</v>
       </c>
-      <c r="BC21" s="40">
+      <c r="BD21" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD21" s="39">
+      <c r="BE21" s="39">
         <v>322</v>
       </c>
-      <c r="BE21" s="112">
+      <c r="BF21" s="112">
         <v>347</v>
       </c>
-      <c r="BF21" s="58">
+      <c r="BG21" s="58">
         <v>2.5</v>
       </c>
-      <c r="BG21" s="58">
+      <c r="BH21" s="58">
         <v>9.5</v>
       </c>
-      <c r="BH21" s="58">
+      <c r="BI21" s="58">
         <v>1.7</v>
       </c>
-      <c r="BI21" s="58">
+      <c r="BJ21" s="58">
         <v>0.5</v>
       </c>
-      <c r="BJ21" s="58">
+      <c r="BK21" s="58">
         <v>1.7</v>
       </c>
-      <c r="BK21" s="58">
+      <c r="BL21" s="58">
         <v>9</v>
       </c>
-      <c r="BL21" s="58">
+      <c r="BM21" s="58">
         <v>8</v>
       </c>
-      <c r="BM21" s="37" t="s">
+      <c r="BN21" s="37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -5585,129 +5638,129 @@
       <c r="D22" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="57">
+      <c r="E22" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22" s="57">
         <v>6</v>
       </c>
-      <c r="F22" s="56" t="s">
+      <c r="G22" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="28">
+      <c r="H22" s="28">
         <v>500000</v>
       </c>
-      <c r="H22" s="27">
+      <c r="I22" s="27">
         <v>550</v>
       </c>
-      <c r="I22" s="70">
+      <c r="J22" s="70">
         <v>35</v>
       </c>
-      <c r="J22" s="69">
+      <c r="K22" s="69">
         <v>45</v>
       </c>
-      <c r="K22" s="25">
+      <c r="L22" s="25">
         <v>12.5</v>
       </c>
-      <c r="L22" s="65">
+      <c r="M22" s="65">
         <v>0</v>
       </c>
-      <c r="M22" s="64">
+      <c r="N22" s="64">
         <v>290</v>
       </c>
-      <c r="N22" s="29">
+      <c r="O22" s="29">
         <v>350</v>
       </c>
-      <c r="O22" s="29">
+      <c r="P22" s="29">
         <v>2.1</v>
       </c>
-      <c r="P22" s="29">
+      <c r="Q22" s="29">
         <v>0</v>
       </c>
-      <c r="Q22" s="29">
+      <c r="R22" s="29">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="R22" s="50">
+      <c r="S22" s="50">
         <v>25</v>
       </c>
-      <c r="S22" s="50">
+      <c r="T22" s="50">
         <v>0.6</v>
       </c>
-      <c r="T22" s="64">
+      <c r="U22" s="64">
         <v>1.35</v>
       </c>
-      <c r="U22" s="29">
+      <c r="V22" s="29">
         <v>1.55</v>
       </c>
-      <c r="V22" s="68">
+      <c r="W22" s="68">
         <v>23.5</v>
       </c>
-      <c r="W22" s="29">
+      <c r="X22" s="29">
         <v>1.5</v>
       </c>
-      <c r="X22" s="29">
+      <c r="Y22" s="29">
         <v>100</v>
       </c>
-      <c r="Y22" s="29">
+      <c r="Z22" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z22" s="29">
+      <c r="AA22" s="29">
         <v>29</v>
       </c>
-      <c r="AA22" s="29">
+      <c r="AB22" s="29">
         <v>17</v>
       </c>
-      <c r="AB22" s="68">
+      <c r="AC22" s="68">
         <v>400</v>
       </c>
-      <c r="AC22" s="50">
+      <c r="AD22" s="50">
         <v>11</v>
       </c>
-      <c r="AD22" s="29">
+      <c r="AE22" s="29">
         <v>5</v>
       </c>
-      <c r="AE22" s="50">
+      <c r="AF22" s="50">
         <v>10</v>
       </c>
-      <c r="AF22" s="29">
+      <c r="AG22" s="29">
         <v>10000</v>
       </c>
-      <c r="AG22" s="67">
+      <c r="AH22" s="67">
         <v>3</v>
       </c>
-      <c r="AH22" s="117">
+      <c r="AI22" s="117">
         <v>0.08</v>
       </c>
-      <c r="AI22" s="67">
+      <c r="AJ22" s="67">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ22" s="74">
+      <c r="AK22" s="74">
         <v>0</v>
       </c>
-      <c r="AK22" s="45">
+      <c r="AL22" s="45">
         <v>12</v>
       </c>
-      <c r="AL22" s="44" t="s">
+      <c r="AM22" s="44" t="s">
         <v>92</v>
-      </c>
-      <c r="AM22" s="24" t="s">
-        <v>91</v>
       </c>
       <c r="AN22" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="AO22" s="24"/>
+      <c r="AO22" s="24" t="s">
+        <v>91</v>
+      </c>
       <c r="AP22" s="24"/>
-      <c r="AQ22" s="24">
+      <c r="AQ22" s="24"/>
+      <c r="AR22" s="24">
         <v>1.6</v>
-      </c>
-      <c r="AR22" s="24">
-        <v>2</v>
       </c>
       <c r="AS22" s="24">
         <v>2</v>
       </c>
-      <c r="AT22" s="24" t="b">
-        <v>1</v>
+      <c r="AT22" s="24">
+        <v>2</v>
       </c>
       <c r="AU22" s="24" t="b">
         <v>1</v>
@@ -5715,59 +5768,62 @@
       <c r="AV22" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW22" s="24">
+      <c r="AW22" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX22" s="24">
         <v>23</v>
       </c>
-      <c r="AX22" s="24">
+      <c r="AY22" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY22" s="24">
+      <c r="AZ22" s="24">
         <v>0.5</v>
       </c>
-      <c r="AZ22" s="60" t="s">
+      <c r="BA22" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="BA22" s="59" t="s">
+      <c r="BB22" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="BB22" s="41">
+      <c r="BC22" s="41">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="BC22" s="40">
+      <c r="BD22" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD22" s="39">
+      <c r="BE22" s="39">
         <v>343</v>
       </c>
-      <c r="BE22" s="112">
+      <c r="BF22" s="112">
         <v>372</v>
       </c>
-      <c r="BF22" s="58">
+      <c r="BG22" s="58">
         <v>2.6</v>
       </c>
-      <c r="BG22" s="58">
+      <c r="BH22" s="58">
         <v>9.5</v>
       </c>
-      <c r="BH22" s="58">
+      <c r="BI22" s="58">
         <v>1.7</v>
       </c>
-      <c r="BI22" s="58">
+      <c r="BJ22" s="58">
         <v>0.5</v>
       </c>
-      <c r="BJ22" s="58">
+      <c r="BK22" s="58">
         <v>0.9</v>
       </c>
-      <c r="BK22" s="58">
+      <c r="BL22" s="58">
         <v>9</v>
       </c>
-      <c r="BL22" s="58">
+      <c r="BM22" s="58">
         <v>8</v>
       </c>
-      <c r="BM22" s="37" t="s">
+      <c r="BN22" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -5777,133 +5833,133 @@
       <c r="D23" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="57">
+      <c r="E23" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23" s="57">
         <v>7</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="G23" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="30">
+      <c r="H23" s="30">
         <v>1100000</v>
       </c>
-      <c r="H23" s="55">
+      <c r="I23" s="55">
         <v>800</v>
       </c>
-      <c r="I23" s="54">
+      <c r="J23" s="54">
         <v>35</v>
       </c>
-      <c r="J23" s="66">
+      <c r="K23" s="66">
         <v>45</v>
       </c>
-      <c r="K23" s="25">
+      <c r="L23" s="25">
         <v>17</v>
       </c>
-      <c r="L23" s="65">
+      <c r="M23" s="65">
         <v>0</v>
       </c>
-      <c r="M23" s="64">
+      <c r="N23" s="64">
         <v>330</v>
       </c>
-      <c r="N23" s="29">
+      <c r="O23" s="29">
         <v>400</v>
       </c>
-      <c r="O23" s="29">
+      <c r="P23" s="29">
         <v>2.2999999999999998</v>
       </c>
-      <c r="P23" s="29">
+      <c r="Q23" s="29">
         <v>0</v>
       </c>
-      <c r="Q23" s="29">
+      <c r="R23" s="29">
         <v>1.4E-2</v>
       </c>
-      <c r="R23" s="50">
+      <c r="S23" s="50">
         <v>25</v>
       </c>
-      <c r="S23" s="50">
+      <c r="T23" s="50">
         <v>0.7</v>
       </c>
-      <c r="T23" s="64">
+      <c r="U23" s="64">
         <v>1.54</v>
       </c>
-      <c r="U23" s="29">
+      <c r="V23" s="29">
         <v>1.74</v>
       </c>
-      <c r="V23" s="49">
+      <c r="W23" s="49">
         <v>25</v>
       </c>
-      <c r="W23" s="29">
+      <c r="X23" s="29">
         <v>1.4</v>
       </c>
-      <c r="X23" s="29">
+      <c r="Y23" s="29">
         <v>100</v>
       </c>
-      <c r="Y23" s="29">
+      <c r="Z23" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z23" s="29">
+      <c r="AA23" s="29">
         <v>20</v>
       </c>
-      <c r="AA23" s="29">
+      <c r="AB23" s="29">
         <v>18</v>
       </c>
-      <c r="AB23" s="49">
+      <c r="AC23" s="49">
         <v>425</v>
       </c>
-      <c r="AC23" s="50">
+      <c r="AD23" s="50">
         <v>11.5</v>
       </c>
-      <c r="AD23" s="26">
+      <c r="AE23" s="26">
         <v>5</v>
       </c>
-      <c r="AE23" s="63">
+      <c r="AF23" s="63">
         <v>10</v>
       </c>
-      <c r="AF23" s="29">
+      <c r="AG23" s="29">
         <v>20000</v>
       </c>
-      <c r="AG23" s="62">
+      <c r="AH23" s="62">
         <v>4</v>
       </c>
-      <c r="AH23" s="118">
+      <c r="AI23" s="118">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI23" s="67">
+      <c r="AJ23" s="67">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="AJ23" s="120">
+      <c r="AK23" s="120">
         <v>0</v>
       </c>
-      <c r="AK23" s="61">
+      <c r="AL23" s="61">
         <v>12</v>
       </c>
-      <c r="AL23" s="44" t="s">
+      <c r="AM23" s="44" t="s">
         <v>88</v>
-      </c>
-      <c r="AM23" s="24" t="s">
-        <v>87</v>
       </c>
       <c r="AN23" s="24" t="s">
         <v>87</v>
       </c>
       <c r="AO23" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP23" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AP23" s="24" t="s">
+      <c r="AQ23" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AQ23" s="24">
+      <c r="AR23" s="24">
         <v>1.4</v>
-      </c>
-      <c r="AR23" s="24">
-        <v>2</v>
       </c>
       <c r="AS23" s="24">
         <v>2</v>
       </c>
-      <c r="AT23" s="24" t="b">
-        <v>1</v>
+      <c r="AT23" s="24">
+        <v>2</v>
       </c>
       <c r="AU23" s="24" t="b">
         <v>1</v>
@@ -5911,59 +5967,62 @@
       <c r="AV23" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW23" s="24">
+      <c r="AW23" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX23" s="24">
         <v>23</v>
       </c>
-      <c r="AX23" s="24">
+      <c r="AY23" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY23" s="24">
+      <c r="AZ23" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ23" s="60" t="s">
+      <c r="BA23" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="BA23" s="59" t="s">
+      <c r="BB23" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="BB23" s="41">
+      <c r="BC23" s="41">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BC23" s="40">
+      <c r="BD23" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD23" s="39">
+      <c r="BE23" s="39">
         <v>435</v>
       </c>
-      <c r="BE23" s="112">
+      <c r="BF23" s="112">
         <v>465</v>
       </c>
-      <c r="BF23" s="58">
+      <c r="BG23" s="58">
         <v>3.2</v>
       </c>
-      <c r="BG23" s="58">
+      <c r="BH23" s="58">
         <v>9.5</v>
       </c>
-      <c r="BH23" s="58">
+      <c r="BI23" s="58">
         <v>1.7</v>
       </c>
-      <c r="BI23" s="58">
+      <c r="BJ23" s="58">
         <v>0.5</v>
       </c>
-      <c r="BJ23" s="58">
+      <c r="BK23" s="58">
         <v>1.2</v>
       </c>
-      <c r="BK23" s="58">
+      <c r="BL23" s="58">
         <v>45</v>
       </c>
-      <c r="BL23" s="58">
+      <c r="BM23" s="58">
         <v>15</v>
       </c>
-      <c r="BM23" s="37" t="s">
+      <c r="BN23" s="37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
@@ -5973,132 +6032,132 @@
       <c r="D24" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="97">
+      <c r="E24" s="100" t="s">
+        <v>198</v>
+      </c>
+      <c r="F24" s="97">
         <v>8</v>
       </c>
-      <c r="F24" s="101" t="s">
+      <c r="G24" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="110">
+      <c r="H24" s="110">
         <v>1800000</v>
       </c>
-      <c r="H24" s="22">
+      <c r="I24" s="22">
         <v>800</v>
       </c>
-      <c r="I24" s="54">
+      <c r="J24" s="54">
         <v>35</v>
       </c>
-      <c r="J24" s="66">
+      <c r="K24" s="66">
         <v>45</v>
       </c>
-      <c r="K24" s="104">
+      <c r="L24" s="104">
         <v>25</v>
       </c>
-      <c r="L24" s="105">
+      <c r="M24" s="105">
         <v>0</v>
       </c>
-      <c r="M24" s="45">
+      <c r="N24" s="45">
         <v>360</v>
       </c>
-      <c r="N24" s="50">
+      <c r="O24" s="50">
         <v>430</v>
       </c>
-      <c r="O24" s="50">
+      <c r="P24" s="50">
         <v>2.2999999999999998</v>
       </c>
-      <c r="P24" s="50">
+      <c r="Q24" s="50">
         <v>0</v>
       </c>
-      <c r="Q24" s="50">
+      <c r="R24" s="50">
         <v>1.4E-2</v>
       </c>
-      <c r="R24" s="50">
+      <c r="S24" s="50">
         <v>25</v>
       </c>
-      <c r="S24" s="50">
+      <c r="T24" s="50">
         <v>0.7</v>
       </c>
-      <c r="T24" s="45">
+      <c r="U24" s="45">
         <v>1.7</v>
       </c>
-      <c r="U24" s="50">
+      <c r="V24" s="50">
         <v>1.95</v>
       </c>
-      <c r="V24" s="49">
+      <c r="W24" s="49">
         <v>25</v>
       </c>
-      <c r="W24" s="50">
+      <c r="X24" s="50">
         <v>1.8</v>
       </c>
-      <c r="X24" s="50">
+      <c r="Y24" s="50">
         <v>100</v>
       </c>
-      <c r="Y24" s="50">
+      <c r="Z24" s="50">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z24" s="50">
+      <c r="AA24" s="50">
         <v>40</v>
       </c>
-      <c r="AA24" s="50">
+      <c r="AB24" s="50">
         <v>14</v>
       </c>
-      <c r="AB24" s="49">
+      <c r="AC24" s="49">
         <v>425</v>
       </c>
-      <c r="AC24" s="50">
+      <c r="AD24" s="50">
         <v>11.5</v>
       </c>
-      <c r="AD24" s="48">
+      <c r="AE24" s="48">
         <v>5</v>
       </c>
-      <c r="AE24" s="63">
+      <c r="AF24" s="63">
         <v>10</v>
       </c>
-      <c r="AF24" s="50">
+      <c r="AG24" s="50">
         <v>20000</v>
       </c>
-      <c r="AG24" s="109">
+      <c r="AH24" s="109">
         <v>4</v>
       </c>
-      <c r="AH24" s="119">
+      <c r="AI24" s="119">
         <v>0.06</v>
       </c>
-      <c r="AI24" s="115">
+      <c r="AJ24" s="115">
         <v>0.05</v>
       </c>
-      <c r="AJ24" s="120">
+      <c r="AK24" s="120">
         <v>0</v>
       </c>
-      <c r="AK24" s="61">
+      <c r="AL24" s="61">
         <v>12</v>
       </c>
-      <c r="AL24" s="99" t="s">
+      <c r="AM24" s="99" t="s">
         <v>185</v>
-      </c>
-      <c r="AM24" s="98" t="s">
-        <v>186</v>
       </c>
       <c r="AN24" s="98" t="s">
         <v>186</v>
       </c>
       <c r="AO24" s="98" t="s">
+        <v>186</v>
+      </c>
+      <c r="AP24" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="AP24" s="98" t="s">
+      <c r="AQ24" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="AQ24" s="98">
+      <c r="AR24" s="98">
         <v>1.3</v>
-      </c>
-      <c r="AR24" s="98">
-        <v>2</v>
       </c>
       <c r="AS24" s="98">
         <v>2</v>
       </c>
-      <c r="AT24" s="98" t="b">
-        <v>1</v>
+      <c r="AT24" s="98">
+        <v>2</v>
       </c>
       <c r="AU24" s="98" t="b">
         <v>1</v>
@@ -6106,59 +6165,62 @@
       <c r="AV24" s="98" t="b">
         <v>1</v>
       </c>
-      <c r="AW24" s="98">
+      <c r="AW24" s="98" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX24" s="98">
         <v>23</v>
       </c>
-      <c r="AX24" s="98">
+      <c r="AY24" s="98">
         <v>0.7</v>
       </c>
-      <c r="AY24" s="98">
+      <c r="AZ24" s="98">
         <v>0.6</v>
       </c>
-      <c r="AZ24" s="102" t="s">
+      <c r="BA24" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="BA24" s="21" t="s">
+      <c r="BB24" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BB24" s="106">
+      <c r="BC24" s="106">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BC24" s="107">
+      <c r="BD24" s="107">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD24" s="108">
+      <c r="BE24" s="108">
         <v>450</v>
       </c>
-      <c r="BE24" s="113">
+      <c r="BF24" s="113">
         <v>505</v>
       </c>
-      <c r="BF24" s="103">
+      <c r="BG24" s="103">
         <v>3.4</v>
       </c>
-      <c r="BG24" s="103">
+      <c r="BH24" s="103">
         <v>9.5</v>
       </c>
-      <c r="BH24" s="103">
+      <c r="BI24" s="103">
         <v>1.7</v>
       </c>
-      <c r="BI24" s="103">
+      <c r="BJ24" s="103">
         <v>0.6</v>
       </c>
-      <c r="BJ24" s="103">
+      <c r="BK24" s="103">
         <v>1</v>
       </c>
-      <c r="BK24" s="103">
+      <c r="BL24" s="103">
         <v>45</v>
       </c>
-      <c r="BL24" s="103">
+      <c r="BM24" s="103">
         <v>15</v>
       </c>
-      <c r="BM24" s="100" t="s">
+      <c r="BN24" s="100" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -6168,133 +6230,133 @@
       <c r="D25" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="57">
+      <c r="E25" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F25" s="57">
         <v>9</v>
       </c>
-      <c r="F25" s="56" t="s">
+      <c r="G25" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="G25" s="30">
+      <c r="H25" s="30">
         <v>2900000</v>
       </c>
-      <c r="H25" s="55">
+      <c r="I25" s="55">
         <v>800</v>
       </c>
-      <c r="I25" s="54">
+      <c r="J25" s="54">
         <v>35</v>
       </c>
-      <c r="J25" s="66">
+      <c r="K25" s="66">
         <v>45</v>
       </c>
-      <c r="K25" s="25">
+      <c r="L25" s="25">
         <v>10</v>
       </c>
-      <c r="L25" s="65">
+      <c r="M25" s="65">
         <v>0</v>
       </c>
-      <c r="M25" s="64">
+      <c r="N25" s="64">
         <v>375</v>
       </c>
-      <c r="N25" s="26">
+      <c r="O25" s="26">
         <v>445</v>
       </c>
-      <c r="O25" s="26">
+      <c r="P25" s="26">
         <v>2.2999999999999998</v>
       </c>
-      <c r="P25" s="26">
+      <c r="Q25" s="26">
         <v>0</v>
       </c>
-      <c r="Q25" s="29">
+      <c r="R25" s="29">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="R25" s="50">
+      <c r="S25" s="50">
         <v>25</v>
       </c>
-      <c r="S25" s="50">
+      <c r="T25" s="50">
         <v>0.7</v>
       </c>
-      <c r="T25" s="46">
+      <c r="U25" s="46">
         <v>1.37</v>
       </c>
-      <c r="U25" s="26">
+      <c r="V25" s="26">
         <v>1.57</v>
       </c>
-      <c r="V25" s="49">
+      <c r="W25" s="49">
         <v>28</v>
       </c>
-      <c r="W25" s="29">
+      <c r="X25" s="29">
         <v>1.6</v>
       </c>
-      <c r="X25" s="29">
+      <c r="Y25" s="29">
         <v>100</v>
       </c>
-      <c r="Y25" s="29">
+      <c r="Z25" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z25" s="29">
+      <c r="AA25" s="29">
         <v>50</v>
       </c>
-      <c r="AA25" s="26">
+      <c r="AB25" s="26">
         <v>34</v>
       </c>
-      <c r="AB25" s="49">
+      <c r="AC25" s="49">
         <v>450</v>
       </c>
-      <c r="AC25" s="50">
+      <c r="AD25" s="50">
         <v>11.5</v>
       </c>
-      <c r="AD25" s="26">
+      <c r="AE25" s="26">
         <v>6</v>
       </c>
-      <c r="AE25" s="63">
+      <c r="AF25" s="63">
         <v>10</v>
       </c>
-      <c r="AF25" s="29">
+      <c r="AG25" s="29">
         <v>20000</v>
       </c>
-      <c r="AG25" s="62">
+      <c r="AH25" s="62">
         <v>4</v>
       </c>
-      <c r="AH25" s="118">
+      <c r="AI25" s="118">
         <v>0.06</v>
       </c>
-      <c r="AI25" s="67">
+      <c r="AJ25" s="67">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="AJ25" s="120">
+      <c r="AK25" s="120">
         <v>0</v>
       </c>
-      <c r="AK25" s="61">
+      <c r="AL25" s="61">
         <v>12</v>
       </c>
-      <c r="AL25" s="44" t="s">
+      <c r="AM25" s="44" t="s">
         <v>83</v>
-      </c>
-      <c r="AM25" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="AN25" s="24" t="s">
         <v>82</v>
       </c>
       <c r="AO25" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP25" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AP25" s="24" t="s">
+      <c r="AQ25" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="AQ25" s="24">
+      <c r="AR25" s="24">
         <v>1.2</v>
-      </c>
-      <c r="AR25" s="24">
-        <v>2</v>
       </c>
       <c r="AS25" s="24">
         <v>2</v>
       </c>
-      <c r="AT25" s="24" t="b">
-        <v>1</v>
+      <c r="AT25" s="24">
+        <v>2</v>
       </c>
       <c r="AU25" s="24" t="b">
         <v>1</v>
@@ -6302,59 +6364,62 @@
       <c r="AV25" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW25" s="24">
+      <c r="AW25" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX25" s="24">
         <v>23</v>
       </c>
-      <c r="AX25" s="24">
+      <c r="AY25" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY25" s="24">
+      <c r="AZ25" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ25" s="60" t="s">
+      <c r="BA25" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="BA25" s="59" t="s">
+      <c r="BB25" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="BB25" s="41">
+      <c r="BC25" s="41">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BC25" s="40">
+      <c r="BD25" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD25" s="39">
+      <c r="BE25" s="39">
         <v>540</v>
       </c>
-      <c r="BE25" s="112">
+      <c r="BF25" s="112">
         <v>590</v>
       </c>
-      <c r="BF25" s="58">
+      <c r="BG25" s="58">
         <v>3.9</v>
       </c>
-      <c r="BG25" s="58">
+      <c r="BH25" s="58">
         <v>9.5</v>
       </c>
-      <c r="BH25" s="58">
+      <c r="BI25" s="58">
         <v>1.7</v>
       </c>
-      <c r="BI25" s="58">
+      <c r="BJ25" s="58">
         <v>0.3</v>
       </c>
-      <c r="BJ25" s="58">
+      <c r="BK25" s="58">
         <v>0.4</v>
       </c>
-      <c r="BK25" s="58">
+      <c r="BL25" s="58">
         <v>45</v>
       </c>
-      <c r="BL25" s="58">
+      <c r="BM25" s="58">
         <v>15</v>
       </c>
-      <c r="BM25" s="37" t="s">
+      <c r="BN25" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:66" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6364,132 +6429,132 @@
       <c r="D26" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="57">
+      <c r="E26" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F26" s="57">
         <v>10</v>
       </c>
-      <c r="F26" s="56" t="s">
+      <c r="G26" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="30">
+      <c r="H26" s="30">
         <v>4300000</v>
       </c>
-      <c r="H26" s="55">
+      <c r="I26" s="55">
         <v>1100</v>
       </c>
-      <c r="I26" s="54">
+      <c r="J26" s="54">
         <v>35</v>
       </c>
-      <c r="J26" s="53">
+      <c r="K26" s="53">
         <v>45</v>
       </c>
-      <c r="K26" s="25">
+      <c r="L26" s="25">
         <v>25</v>
       </c>
-      <c r="L26" s="52">
+      <c r="M26" s="52">
         <v>0</v>
       </c>
-      <c r="M26" s="51">
+      <c r="N26" s="51">
         <v>425</v>
       </c>
-      <c r="N26" s="26">
+      <c r="O26" s="26">
         <v>500</v>
       </c>
-      <c r="O26" s="26">
+      <c r="P26" s="26">
         <v>2.4</v>
       </c>
-      <c r="P26" s="26">
+      <c r="Q26" s="26">
         <v>0</v>
       </c>
-      <c r="Q26" s="29">
+      <c r="R26" s="29">
         <v>1.6E-2</v>
       </c>
-      <c r="R26" s="50">
+      <c r="S26" s="50">
         <v>20</v>
       </c>
-      <c r="S26" s="50">
+      <c r="T26" s="50">
         <v>0.8</v>
       </c>
-      <c r="T26" s="46">
+      <c r="U26" s="46">
         <v>2</v>
       </c>
-      <c r="U26" s="26">
+      <c r="V26" s="26">
         <v>2.1</v>
       </c>
-      <c r="V26" s="49">
+      <c r="W26" s="49">
         <v>31</v>
       </c>
-      <c r="W26" s="26">
+      <c r="X26" s="26">
         <v>1.9</v>
       </c>
-      <c r="X26" s="26">
+      <c r="Y26" s="26">
         <v>100</v>
       </c>
-      <c r="Y26" s="26">
+      <c r="Z26" s="26">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z26" s="26">
+      <c r="AA26" s="26">
         <v>19</v>
       </c>
-      <c r="AA26" s="26">
+      <c r="AB26" s="26">
         <v>12</v>
       </c>
-      <c r="AB26" s="49">
+      <c r="AC26" s="49">
         <v>475</v>
       </c>
-      <c r="AC26" s="48">
+      <c r="AD26" s="48">
         <v>12</v>
       </c>
-      <c r="AD26" s="26">
+      <c r="AE26" s="26">
         <v>6</v>
       </c>
-      <c r="AE26" s="48">
+      <c r="AF26" s="48">
         <v>10</v>
       </c>
-      <c r="AF26" s="26">
+      <c r="AG26" s="26">
         <v>30000</v>
       </c>
-      <c r="AG26" s="47">
+      <c r="AH26" s="47">
         <v>5</v>
       </c>
-      <c r="AH26" s="118">
+      <c r="AI26" s="118">
         <v>0.05</v>
       </c>
-      <c r="AI26" s="67">
+      <c r="AJ26" s="67">
         <v>0.04</v>
       </c>
-      <c r="AJ26" s="74">
+      <c r="AK26" s="74">
         <v>0</v>
       </c>
-      <c r="AK26" s="45">
+      <c r="AL26" s="45">
         <v>12</v>
       </c>
-      <c r="AL26" s="44" t="s">
+      <c r="AM26" s="44" t="s">
         <v>78</v>
-      </c>
-      <c r="AM26" s="24" t="s">
-        <v>77</v>
       </c>
       <c r="AN26" s="24" t="s">
         <v>77</v>
       </c>
       <c r="AO26" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP26" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AP26" s="24" t="s">
+      <c r="AQ26" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AQ26" s="24">
+      <c r="AR26" s="24">
         <v>1.1000000000000001</v>
-      </c>
-      <c r="AR26" s="24">
-        <v>2</v>
       </c>
       <c r="AS26" s="24">
         <v>2</v>
       </c>
-      <c r="AT26" s="24" t="b">
-        <v>1</v>
+      <c r="AT26" s="24">
+        <v>2</v>
       </c>
       <c r="AU26" s="24" t="b">
         <v>1</v>
@@ -6497,59 +6562,62 @@
       <c r="AV26" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW26" s="24">
+      <c r="AW26" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX26" s="24">
         <v>23</v>
       </c>
-      <c r="AX26" s="24">
+      <c r="AY26" s="24">
         <v>0.75</v>
       </c>
-      <c r="AY26" s="24">
+      <c r="AZ26" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ26" s="43" t="s">
+      <c r="BA26" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="BA26" s="42" t="s">
+      <c r="BB26" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="BB26" s="41">
+      <c r="BC26" s="41">
         <v>1.5E-3</v>
       </c>
-      <c r="BC26" s="40">
+      <c r="BD26" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD26" s="39">
+      <c r="BE26" s="39">
         <v>680</v>
       </c>
-      <c r="BE26" s="114">
+      <c r="BF26" s="114">
         <v>730</v>
       </c>
-      <c r="BF26" s="38">
+      <c r="BG26" s="38">
         <v>4.7</v>
       </c>
-      <c r="BG26" s="38">
+      <c r="BH26" s="38">
         <v>9.5</v>
       </c>
-      <c r="BH26" s="38">
+      <c r="BI26" s="38">
         <v>1.7</v>
       </c>
-      <c r="BI26" s="38">
+      <c r="BJ26" s="38">
         <v>0.7</v>
       </c>
-      <c r="BJ26" s="38">
+      <c r="BK26" s="38">
         <v>1.03</v>
       </c>
-      <c r="BK26" s="38">
+      <c r="BL26" s="38">
         <v>59</v>
       </c>
-      <c r="BL26" s="38">
+      <c r="BM26" s="38">
         <v>15</v>
       </c>
-      <c r="BM26" s="37" t="s">
+      <c r="BN26" s="37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:65" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:66" s="33" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
@@ -6607,8 +6675,8 @@
       <c r="BI27" s="121"/>
       <c r="BJ27" s="121"/>
     </row>
-    <row r="29" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:66" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:66" ht="24" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -6622,7 +6690,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:65" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:66" s="20" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="B31" s="19"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
@@ -6631,7 +6699,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:65" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:66" ht="139" x14ac:dyDescent="0.2">
       <c r="B32" s="10" t="s">
         <v>64</v>
       </c>
@@ -6657,7 +6725,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B33" s="8" t="s">
         <v>3</v>
       </c>
@@ -6683,8 +6751,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:23" ht="24" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
@@ -6698,7 +6766,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="2:23" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:23" s="20" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="B36" s="19"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
@@ -6710,7 +6778,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="2:23" ht="169.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:23" ht="166" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
         <v>53</v>
       </c>
@@ -6727,7 +6795,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38" s="8" t="s">
         <v>3</v>
       </c>
@@ -6744,7 +6812,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B39" s="8" t="s">
         <v>3</v>
       </c>
@@ -6761,7 +6829,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B40" s="8" t="s">
         <v>3</v>
       </c>
@@ -6778,8 +6846,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:23" ht="24" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
@@ -6793,12 +6861,12 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
       <c r="E43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:23" ht="150" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:23" ht="149" x14ac:dyDescent="0.2">
       <c r="B44" s="10" t="s">
         <v>41</v>
       </c>
@@ -6866,7 +6934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>3</v>
       </c>
@@ -6934,7 +7002,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>3</v>
       </c>
@@ -7002,7 +7070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>3</v>
       </c>
@@ -7070,7 +7138,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>3</v>
       </c>
@@ -7138,7 +7206,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>3</v>
       </c>
@@ -7206,7 +7274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>3</v>
       </c>
@@ -7274,7 +7342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -7342,7 +7410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -7410,7 +7478,7 @@
         <v>485030</v>
       </c>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -7478,7 +7546,7 @@
         <v>558660</v>
       </c>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -7546,7 +7614,7 @@
         <v>633960</v>
       </c>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>3</v>
       </c>
@@ -7626,28 +7694,31 @@
     <mergeCell ref="AH27:AI27"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="99" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="98" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM16:BM23 BM25:BM26">
-    <cfRule type="duplicateValues" dxfId="97" priority="3"/>
+  <conditionalFormatting sqref="BN16:BN23 BN25:BN26">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM24">
-    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
+  <conditionalFormatting sqref="BN24">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26">
+  <dataValidations count="4">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D26" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT("dragonTierDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D45:D55 F45:W55 E46:E55"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D33:D34 D38:D40">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D45:D55 F45:W55 E46:E55" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D33:D34 D38:D40" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E16:E26" xr:uid="{339AE3F0-A4FE-8C4C-801E-BA3C16FB83C5}">
+      <formula1>"classic,special"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dragon 12 final stats
Former-commit-id: b9dda54074fe867358ed35adc44379db5e911e2f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -923,21 +923,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1025,36 +1010,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -1179,6 +1134,45 @@
       </top>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1267,20 +1261,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1289,85 +1283,76 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1394,10 +1379,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1409,10 +1394,10 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1421,7 +1406,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1430,7 +1415,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1448,7 +1433,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1466,19 +1451,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1494,22 +1479,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1518,41 +1503,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="100">
+  <dxfs count="102">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3573,98 +3587,98 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM27" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM27" totalsRowShown="0" headerRowDxfId="96" dataDxfId="94" headerRowBorderDxfId="95" tableBorderDxfId="93" totalsRowBorderDxfId="92">
   <autoFilter ref="B15:BM27"/>
   <tableColumns count="64">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="89"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="87"/>
-    <tableColumn id="3" name="[order]" dataDxfId="86"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="85"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="84"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="83"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="82"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="81"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="80"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="79"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="78"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="77"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="76"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="75"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="74"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="73"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="72"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="71"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="70"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="69"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="68"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="67"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="66">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="91"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="90"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="89"/>
+    <tableColumn id="3" name="[order]" dataDxfId="88"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="87"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="86"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="85"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="84"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="83"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="82"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="81"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="80"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="79"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="78"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="77"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="76"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="75"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="74"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="73"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="72"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="71"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="70"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="69"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="68">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="65"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="64"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="63"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="62"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="61"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="60"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="59"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="58"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="57"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="56">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="67"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="66"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="65"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="64"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="63"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="62"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="61"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="60"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="59"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="58">
       <calculatedColumnFormula>AH17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="55"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="54"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="53"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="52"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="51"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="50"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="49"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="48"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="47"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="46"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="45"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="44"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="43"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="42"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="41"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="40"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="39">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="57"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="56"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="55"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="54"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="53"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="52"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="51"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="50"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="49"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="48"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="47"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="46"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="45"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="44"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="43"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="42"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="41">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="38">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="40">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="37"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="36"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="35"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="34">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="39"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="38"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="37"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="36">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="33"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="32"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="31"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="30"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="29"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="28"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="27"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="35"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="34"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="33"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="32"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="31"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="30"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="29"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="23"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="18">
+    <tableColumn id="10" name="[icon]" dataDxfId="22"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="21"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="20">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3673,11 +3687,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B33:I34"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3690,7 +3704,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B45:W57"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3721,14 +3735,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B38:F41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="5"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="3"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4002,8 +4016,8 @@
   </sheetPr>
   <dimension ref="B1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="AR13" workbookViewId="0">
+      <selection activeCell="BB29" sqref="BB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4136,7 +4150,7 @@
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="92" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="9">
@@ -4148,7 +4162,7 @@
       <c r="F7" s="16">
         <v>3</v>
       </c>
-      <c r="G7" s="96" t="str">
+      <c r="G7" s="93" t="str">
         <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
@@ -4157,7 +4171,7 @@
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="92" t="s">
         <v>84</v>
       </c>
       <c r="D8" s="9">
@@ -4169,7 +4183,7 @@
       <c r="F8" s="13">
         <v>4</v>
       </c>
-      <c r="G8" s="94" t="str">
+      <c r="G8" s="91" t="str">
         <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
@@ -4178,7 +4192,7 @@
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="92" t="s">
         <v>79</v>
       </c>
       <c r="D9" s="9">
@@ -4190,7 +4204,7 @@
       <c r="F9" s="13">
         <v>4</v>
       </c>
-      <c r="G9" s="94" t="str">
+      <c r="G9" s="91" t="str">
         <f>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</f>
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
@@ -4245,202 +4259,202 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="122"/>
-      <c r="AP14" s="122"/>
-      <c r="AQ14" s="122"/>
-      <c r="AR14" s="122"/>
+      <c r="AO14" s="119"/>
+      <c r="AP14" s="119"/>
+      <c r="AQ14" s="119"/>
+      <c r="AR14" s="119"/>
     </row>
     <row r="15" spans="2:65" ht="163.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="72" t="s">
         <v>170</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="78" t="s">
+      <c r="D15" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="76" t="s">
+      <c r="E15" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="93" t="s">
+      <c r="G15" s="90" t="s">
         <v>168</v>
       </c>
-      <c r="H15" s="92" t="s">
+      <c r="H15" s="89" t="s">
         <v>167</v>
       </c>
-      <c r="I15" s="91" t="s">
+      <c r="I15" s="88" t="s">
         <v>166</v>
       </c>
-      <c r="J15" s="90" t="s">
+      <c r="J15" s="87" t="s">
         <v>165</v>
       </c>
-      <c r="K15" s="89" t="s">
+      <c r="K15" s="86" t="s">
         <v>164</v>
       </c>
-      <c r="L15" s="87" t="s">
+      <c r="L15" s="84" t="s">
         <v>163</v>
       </c>
-      <c r="M15" s="85" t="s">
+      <c r="M15" s="82" t="s">
         <v>162</v>
       </c>
-      <c r="N15" s="89" t="s">
+      <c r="N15" s="86" t="s">
         <v>161</v>
       </c>
-      <c r="O15" s="87" t="s">
+      <c r="O15" s="84" t="s">
         <v>160</v>
       </c>
-      <c r="P15" s="87" t="s">
+      <c r="P15" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="Q15" s="86" t="s">
+      <c r="Q15" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="R15" s="86" t="s">
+      <c r="R15" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="S15" s="86" t="s">
+      <c r="S15" s="83" t="s">
         <v>156</v>
       </c>
-      <c r="T15" s="85" t="s">
+      <c r="T15" s="82" t="s">
         <v>155</v>
       </c>
-      <c r="U15" s="87" t="s">
+      <c r="U15" s="84" t="s">
         <v>154</v>
       </c>
-      <c r="V15" s="88" t="s">
+      <c r="V15" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="W15" s="85" t="s">
+      <c r="W15" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="X15" s="89" t="s">
+      <c r="X15" s="86" t="s">
         <v>191</v>
       </c>
-      <c r="Y15" s="89" t="s">
+      <c r="Y15" s="86" t="s">
         <v>192</v>
       </c>
-      <c r="Z15" s="89" t="s">
+      <c r="Z15" s="86" t="s">
         <v>151</v>
       </c>
-      <c r="AA15" s="87" t="s">
+      <c r="AA15" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="AB15" s="88" t="s">
+      <c r="AB15" s="85" t="s">
         <v>149</v>
       </c>
-      <c r="AC15" s="87" t="s">
+      <c r="AC15" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="AD15" s="87" t="s">
+      <c r="AD15" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="AE15" s="87" t="s">
+      <c r="AE15" s="84" t="s">
         <v>146</v>
       </c>
-      <c r="AF15" s="116" t="s">
+      <c r="AF15" s="113" t="s">
         <v>145</v>
       </c>
-      <c r="AG15" s="86" t="s">
+      <c r="AG15" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="AH15" s="85" t="s">
+      <c r="AH15" s="82" t="s">
         <v>193</v>
       </c>
-      <c r="AI15" s="85" t="s">
+      <c r="AI15" s="82" t="s">
         <v>194</v>
       </c>
-      <c r="AJ15" s="85" t="s">
+      <c r="AJ15" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="AK15" s="85" t="s">
+      <c r="AK15" s="82" t="s">
         <v>142</v>
       </c>
-      <c r="AL15" s="84" t="s">
+      <c r="AL15" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="AM15" s="82" t="s">
+      <c r="AM15" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="AN15" s="82" t="s">
+      <c r="AN15" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="AO15" s="82" t="s">
+      <c r="AO15" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="AP15" s="82" t="s">
+      <c r="AP15" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="AQ15" s="82" t="s">
+      <c r="AQ15" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="AR15" s="83" t="s">
+      <c r="AR15" s="80" t="s">
         <v>137</v>
       </c>
-      <c r="AS15" s="82" t="s">
+      <c r="AS15" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="AT15" s="82" t="s">
+      <c r="AT15" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="AU15" s="82" t="s">
+      <c r="AU15" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="AV15" s="82" t="s">
+      <c r="AV15" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="AW15" s="82" t="s">
+      <c r="AW15" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="AX15" s="82" t="s">
+      <c r="AX15" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="AY15" s="82" t="s">
+      <c r="AY15" s="79" t="s">
         <v>196</v>
       </c>
       <c r="AZ15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BA15" s="81" t="s">
+      <c r="BA15" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="BB15" s="80" t="s">
+      <c r="BB15" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="BC15" s="76" t="s">
+      <c r="BC15" s="73" t="s">
         <v>129</v>
       </c>
-      <c r="BD15" s="79" t="s">
+      <c r="BD15" s="76" t="s">
         <v>189</v>
       </c>
-      <c r="BE15" s="75" t="s">
+      <c r="BE15" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="BF15" s="78" t="s">
+      <c r="BF15" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="BG15" s="78" t="s">
+      <c r="BG15" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="BH15" s="78" t="s">
+      <c r="BH15" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="BI15" s="75" t="s">
+      <c r="BI15" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="BJ15" s="75" t="s">
+      <c r="BJ15" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="BK15" s="77" t="s">
+      <c r="BK15" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="BL15" s="76" t="s">
+      <c r="BL15" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="BM15" s="75" t="s">
+      <c r="BM15" s="72" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4448,35 +4462,35 @@
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="57">
+      <c r="E16" s="54">
         <v>0</v>
       </c>
-      <c r="F16" s="57"/>
+      <c r="F16" s="54"/>
       <c r="G16" s="28">
         <v>0</v>
       </c>
       <c r="H16" s="27">
         <v>0</v>
       </c>
-      <c r="I16" s="70">
+      <c r="I16" s="67">
         <v>35</v>
       </c>
-      <c r="J16" s="69">
+      <c r="J16" s="66">
         <v>45</v>
       </c>
       <c r="K16" s="25">
         <v>1</v>
       </c>
-      <c r="L16" s="65">
+      <c r="L16" s="62">
         <v>-2</v>
       </c>
-      <c r="M16" s="64">
+      <c r="M16" s="61">
         <v>75</v>
       </c>
       <c r="N16" s="29">
@@ -4491,19 +4505,19 @@
       <c r="Q16" s="29">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="R16" s="50">
+      <c r="R16" s="49">
         <v>30</v>
       </c>
-      <c r="S16" s="50">
+      <c r="S16" s="49">
         <v>0.5</v>
       </c>
-      <c r="T16" s="64">
+      <c r="T16" s="61">
         <v>0.46</v>
       </c>
       <c r="U16" s="29">
         <v>0.71</v>
       </c>
-      <c r="V16" s="68">
+      <c r="V16" s="65">
         <v>14</v>
       </c>
       <c r="W16" s="29">
@@ -4522,35 +4536,35 @@
       <c r="AA16" s="29">
         <v>28</v>
       </c>
-      <c r="AB16" s="68">
+      <c r="AB16" s="65">
         <v>250</v>
       </c>
-      <c r="AC16" s="50">
+      <c r="AC16" s="49">
         <v>7.5</v>
       </c>
       <c r="AD16" s="29">
         <v>2</v>
       </c>
-      <c r="AE16" s="50">
+      <c r="AE16" s="49">
         <v>8</v>
       </c>
       <c r="AF16" s="29">
         <v>3000</v>
       </c>
-      <c r="AG16" s="67">
+      <c r="AG16" s="64">
         <v>1</v>
       </c>
-      <c r="AH16" s="117">
+      <c r="AH16" s="114">
         <v>0.23</v>
       </c>
-      <c r="AI16" s="67">
+      <c r="AI16" s="64">
         <f t="shared" ref="AI16:AI23" si="0">AH17</f>
         <v>0.19</v>
       </c>
-      <c r="AJ16" s="74">
+      <c r="AJ16" s="71">
         <v>0</v>
       </c>
-      <c r="AK16" s="74">
+      <c r="AK16" s="71">
         <v>12</v>
       </c>
       <c r="AL16" s="24" t="s">
@@ -4591,10 +4605,10 @@
       <c r="AY16" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ16" s="72" t="s">
+      <c r="AZ16" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="BA16" s="71" t="s">
+      <c r="BA16" s="68" t="s">
         <v>117</v>
       </c>
       <c r="BB16" s="41">
@@ -4606,31 +4620,31 @@
       <c r="BD16" s="39">
         <v>175</v>
       </c>
-      <c r="BE16" s="112">
+      <c r="BE16" s="109">
         <v>200</v>
       </c>
-      <c r="BF16" s="58">
+      <c r="BF16" s="55">
         <v>2</v>
       </c>
-      <c r="BG16" s="58">
+      <c r="BG16" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH16" s="58">
+      <c r="BH16" s="55">
         <v>1</v>
       </c>
-      <c r="BI16" s="73">
+      <c r="BI16" s="70">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BJ16" s="73">
+      <c r="BJ16" s="70">
         <v>1.75</v>
       </c>
-      <c r="BK16" s="73">
+      <c r="BK16" s="70">
         <v>0</v>
       </c>
-      <c r="BL16" s="73">
+      <c r="BL16" s="70">
         <v>8</v>
       </c>
-      <c r="BM16" s="58" t="s">
+      <c r="BM16" s="55" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4638,16 +4652,16 @@
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="57">
+      <c r="E17" s="54">
         <v>1</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="53" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="28">
@@ -4656,19 +4670,19 @@
       <c r="H17" s="27">
         <v>60</v>
       </c>
-      <c r="I17" s="70">
+      <c r="I17" s="67">
         <v>35</v>
       </c>
-      <c r="J17" s="69">
+      <c r="J17" s="66">
         <v>45</v>
       </c>
       <c r="K17" s="25">
         <v>3</v>
       </c>
-      <c r="L17" s="65">
+      <c r="L17" s="62">
         <v>-2</v>
       </c>
-      <c r="M17" s="64">
+      <c r="M17" s="61">
         <v>95</v>
       </c>
       <c r="N17" s="29">
@@ -4683,10 +4697,10 @@
       <c r="Q17" s="29">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="R17" s="50">
+      <c r="R17" s="49">
         <v>30</v>
       </c>
-      <c r="S17" s="50">
+      <c r="S17" s="49">
         <v>0.5</v>
       </c>
       <c r="T17" s="46">
@@ -4695,7 +4709,7 @@
       <c r="U17" s="26">
         <v>0.95</v>
       </c>
-      <c r="V17" s="68">
+      <c r="V17" s="65">
         <v>16</v>
       </c>
       <c r="W17" s="29">
@@ -4714,32 +4728,32 @@
       <c r="AA17" s="29">
         <v>10</v>
       </c>
-      <c r="AB17" s="68">
+      <c r="AB17" s="65">
         <v>275</v>
       </c>
-      <c r="AC17" s="50">
+      <c r="AC17" s="49">
         <v>8</v>
       </c>
       <c r="AD17" s="29">
         <v>3</v>
       </c>
-      <c r="AE17" s="50">
+      <c r="AE17" s="49">
         <v>9</v>
       </c>
       <c r="AF17" s="29">
         <v>7000</v>
       </c>
-      <c r="AG17" s="67">
+      <c r="AG17" s="64">
         <v>2</v>
       </c>
-      <c r="AH17" s="117">
+      <c r="AH17" s="114">
         <v>0.19</v>
       </c>
-      <c r="AI17" s="67">
+      <c r="AI17" s="64">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="AJ17" s="74">
+      <c r="AJ17" s="71">
         <v>0</v>
       </c>
       <c r="AK17" s="45">
@@ -4783,10 +4797,10 @@
       <c r="AY17" s="24">
         <v>0.8</v>
       </c>
-      <c r="AZ17" s="72" t="s">
+      <c r="AZ17" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="BA17" s="71" t="s">
+      <c r="BA17" s="68" t="s">
         <v>113</v>
       </c>
       <c r="BB17" s="41">
@@ -4798,31 +4812,31 @@
       <c r="BD17" s="39">
         <v>210</v>
       </c>
-      <c r="BE17" s="112">
+      <c r="BE17" s="109">
         <v>235</v>
       </c>
-      <c r="BF17" s="58">
+      <c r="BF17" s="55">
         <v>2.1</v>
       </c>
-      <c r="BG17" s="58">
+      <c r="BG17" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH17" s="58">
+      <c r="BH17" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI17" s="58">
+      <c r="BI17" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BJ17" s="58">
+      <c r="BJ17" s="55">
         <v>2.1</v>
       </c>
-      <c r="BK17" s="58">
+      <c r="BK17" s="55">
         <v>0</v>
       </c>
-      <c r="BL17" s="58">
+      <c r="BL17" s="55">
         <v>8</v>
       </c>
-      <c r="BM17" s="58" t="s">
+      <c r="BM17" s="55" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4836,31 +4850,31 @@
       <c r="D18" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="57">
+      <c r="E18" s="54">
         <v>2</v>
       </c>
-      <c r="F18" s="57" t="s">
+      <c r="F18" s="54" t="s">
         <v>6</v>
       </c>
       <c r="G18" s="30">
         <v>11000</v>
       </c>
-      <c r="H18" s="55">
+      <c r="H18" s="52">
         <v>100</v>
       </c>
-      <c r="I18" s="54">
+      <c r="I18" s="51">
         <v>35</v>
       </c>
-      <c r="J18" s="66">
+      <c r="J18" s="63">
         <v>45</v>
       </c>
       <c r="K18" s="25">
         <v>5</v>
       </c>
-      <c r="L18" s="65">
+      <c r="L18" s="62">
         <v>-2</v>
       </c>
-      <c r="M18" s="64">
+      <c r="M18" s="61">
         <v>140</v>
       </c>
       <c r="N18" s="26">
@@ -4875,19 +4889,19 @@
       <c r="Q18" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="R18" s="50">
+      <c r="R18" s="49">
         <v>30</v>
       </c>
-      <c r="S18" s="50">
+      <c r="S18" s="49">
         <v>0.5</v>
       </c>
-      <c r="T18" s="64">
+      <c r="T18" s="61">
         <v>0.85</v>
       </c>
       <c r="U18" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V18" s="49">
+      <c r="V18" s="48">
         <v>23.5</v>
       </c>
       <c r="W18" s="29">
@@ -4906,35 +4920,35 @@
       <c r="AA18" s="29">
         <v>14</v>
       </c>
-      <c r="AB18" s="49">
+      <c r="AB18" s="48">
         <v>300</v>
       </c>
-      <c r="AC18" s="50">
+      <c r="AC18" s="49">
         <v>9</v>
       </c>
       <c r="AD18" s="26">
         <v>3</v>
       </c>
-      <c r="AE18" s="63">
+      <c r="AE18" s="60">
         <v>9</v>
       </c>
       <c r="AF18" s="29">
         <v>8000</v>
       </c>
-      <c r="AG18" s="62">
+      <c r="AG18" s="59">
         <v>2</v>
       </c>
-      <c r="AH18" s="118">
+      <c r="AH18" s="115">
         <v>0.15</v>
       </c>
-      <c r="AI18" s="67">
+      <c r="AI18" s="64">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="AJ18" s="120">
+      <c r="AJ18" s="117">
         <v>0</v>
       </c>
-      <c r="AK18" s="61">
+      <c r="AK18" s="58">
         <v>12</v>
       </c>
       <c r="AL18" s="44" t="s">
@@ -4975,10 +4989,10 @@
       <c r="AY18" s="24">
         <v>0.7</v>
       </c>
-      <c r="AZ18" s="60" t="s">
+      <c r="AZ18" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="BA18" s="59" t="s">
+      <c r="BA18" s="56" t="s">
         <v>108</v>
       </c>
       <c r="BB18" s="41">
@@ -4990,28 +5004,28 @@
       <c r="BD18" s="39">
         <v>240</v>
       </c>
-      <c r="BE18" s="112">
+      <c r="BE18" s="109">
         <v>280</v>
       </c>
-      <c r="BF18" s="58">
+      <c r="BF18" s="55">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BG18" s="58">
+      <c r="BG18" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH18" s="58">
+      <c r="BH18" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI18" s="58">
+      <c r="BI18" s="55">
         <v>0.9</v>
       </c>
-      <c r="BJ18" s="58">
+      <c r="BJ18" s="55">
         <v>2.25</v>
       </c>
-      <c r="BK18" s="58">
+      <c r="BK18" s="55">
         <v>0</v>
       </c>
-      <c r="BL18" s="58">
+      <c r="BL18" s="55">
         <v>8</v>
       </c>
       <c r="BM18" s="37" t="s">
@@ -5025,13 +5039,13 @@
       <c r="C19" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="57">
+      <c r="E19" s="54">
         <v>3</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="54" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="28">
@@ -5040,19 +5054,19 @@
       <c r="H19" s="27">
         <v>150</v>
       </c>
-      <c r="I19" s="70">
+      <c r="I19" s="67">
         <v>35</v>
       </c>
-      <c r="J19" s="69">
+      <c r="J19" s="66">
         <v>45</v>
       </c>
       <c r="K19" s="25">
         <v>6</v>
       </c>
-      <c r="L19" s="65">
+      <c r="L19" s="62">
         <v>-2</v>
       </c>
-      <c r="M19" s="64">
+      <c r="M19" s="61">
         <v>190</v>
       </c>
       <c r="N19" s="29">
@@ -5067,10 +5081,10 @@
       <c r="Q19" s="29">
         <v>0.01</v>
       </c>
-      <c r="R19" s="50">
+      <c r="R19" s="49">
         <v>30</v>
       </c>
-      <c r="S19" s="50">
+      <c r="S19" s="49">
         <v>0.6</v>
       </c>
       <c r="T19" s="46">
@@ -5079,7 +5093,7 @@
       <c r="U19" s="26">
         <v>1.1499999999999999</v>
       </c>
-      <c r="V19" s="68">
+      <c r="V19" s="65">
         <v>19</v>
       </c>
       <c r="W19" s="29">
@@ -5098,32 +5112,32 @@
       <c r="AA19" s="26">
         <v>22</v>
       </c>
-      <c r="AB19" s="68">
+      <c r="AB19" s="65">
         <v>325</v>
       </c>
-      <c r="AC19" s="50">
+      <c r="AC19" s="49">
         <v>10</v>
       </c>
       <c r="AD19" s="29">
         <v>4</v>
       </c>
-      <c r="AE19" s="50">
+      <c r="AE19" s="49">
         <v>9</v>
       </c>
       <c r="AF19" s="29">
         <v>9000</v>
       </c>
-      <c r="AG19" s="67">
+      <c r="AG19" s="64">
         <v>2</v>
       </c>
-      <c r="AH19" s="117">
+      <c r="AH19" s="114">
         <v>0.13</v>
       </c>
-      <c r="AI19" s="67">
+      <c r="AI19" s="64">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="AJ19" s="74">
+      <c r="AJ19" s="71">
         <v>0</v>
       </c>
       <c r="AK19" s="45">
@@ -5167,10 +5181,10 @@
       <c r="AY19" s="24">
         <v>0.7</v>
       </c>
-      <c r="AZ19" s="60" t="s">
+      <c r="AZ19" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="BA19" s="59" t="s">
+      <c r="BA19" s="56" t="s">
         <v>103</v>
       </c>
       <c r="BB19" s="41">
@@ -5182,28 +5196,28 @@
       <c r="BD19" s="39">
         <v>345</v>
       </c>
-      <c r="BE19" s="112">
+      <c r="BE19" s="109">
         <v>365</v>
       </c>
-      <c r="BF19" s="58">
+      <c r="BF19" s="55">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BG19" s="58">
+      <c r="BG19" s="55">
         <v>5</v>
       </c>
-      <c r="BH19" s="58">
+      <c r="BH19" s="55">
         <v>0.5</v>
       </c>
-      <c r="BI19" s="58">
+      <c r="BI19" s="55">
         <v>1.2</v>
       </c>
-      <c r="BJ19" s="58">
+      <c r="BJ19" s="55">
         <v>0.77</v>
       </c>
-      <c r="BK19" s="58">
+      <c r="BK19" s="55">
         <v>0</v>
       </c>
-      <c r="BL19" s="58">
+      <c r="BL19" s="55">
         <v>8</v>
       </c>
       <c r="BM19" s="37" t="s">
@@ -5217,13 +5231,13 @@
       <c r="C20" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="57">
+      <c r="E20" s="54">
         <v>4</v>
       </c>
-      <c r="F20" s="57" t="s">
+      <c r="F20" s="54" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="28">
@@ -5232,19 +5246,19 @@
       <c r="H20" s="27">
         <v>200</v>
       </c>
-      <c r="I20" s="70">
+      <c r="I20" s="67">
         <v>35</v>
       </c>
-      <c r="J20" s="69">
+      <c r="J20" s="66">
         <v>45</v>
       </c>
       <c r="K20" s="25">
         <v>8</v>
       </c>
-      <c r="L20" s="65">
+      <c r="L20" s="62">
         <v>0</v>
       </c>
-      <c r="M20" s="64">
+      <c r="M20" s="61">
         <v>210</v>
       </c>
       <c r="N20" s="29">
@@ -5259,19 +5273,19 @@
       <c r="Q20" s="29">
         <v>1.2E-2</v>
       </c>
-      <c r="R20" s="50">
+      <c r="R20" s="49">
         <v>30</v>
       </c>
-      <c r="S20" s="50">
+      <c r="S20" s="49">
         <v>0.6</v>
       </c>
-      <c r="T20" s="64">
+      <c r="T20" s="61">
         <v>1</v>
       </c>
       <c r="U20" s="29">
         <v>1.25</v>
       </c>
-      <c r="V20" s="68">
+      <c r="V20" s="65">
         <v>20</v>
       </c>
       <c r="W20" s="29">
@@ -5290,32 +5304,32 @@
       <c r="AA20" s="29">
         <v>34</v>
       </c>
-      <c r="AB20" s="68">
+      <c r="AB20" s="65">
         <v>350</v>
       </c>
-      <c r="AC20" s="50">
+      <c r="AC20" s="49">
         <v>11</v>
       </c>
       <c r="AD20" s="29">
         <v>4</v>
       </c>
-      <c r="AE20" s="50">
+      <c r="AE20" s="49">
         <v>10</v>
       </c>
       <c r="AF20" s="29">
         <v>10000</v>
       </c>
-      <c r="AG20" s="67">
+      <c r="AG20" s="64">
         <v>3</v>
       </c>
-      <c r="AH20" s="117">
+      <c r="AH20" s="114">
         <v>0.11</v>
       </c>
-      <c r="AI20" s="67">
+      <c r="AI20" s="64">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="AJ20" s="74">
+      <c r="AJ20" s="71">
         <v>0</v>
       </c>
       <c r="AK20" s="45">
@@ -5359,10 +5373,10 @@
       <c r="AY20" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ20" s="60" t="s">
+      <c r="AZ20" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="BA20" s="59" t="s">
+      <c r="BA20" s="56" t="s">
         <v>99</v>
       </c>
       <c r="BB20" s="41">
@@ -5374,28 +5388,28 @@
       <c r="BD20" s="39">
         <v>310</v>
       </c>
-      <c r="BE20" s="112">
+      <c r="BE20" s="109">
         <v>335</v>
       </c>
-      <c r="BF20" s="58">
+      <c r="BF20" s="55">
         <v>2.4</v>
       </c>
-      <c r="BG20" s="58">
+      <c r="BG20" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH20" s="58">
+      <c r="BH20" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI20" s="58">
+      <c r="BI20" s="55">
         <v>1</v>
       </c>
-      <c r="BJ20" s="58">
+      <c r="BJ20" s="55">
         <v>1.6</v>
       </c>
-      <c r="BK20" s="58">
+      <c r="BK20" s="55">
         <v>9</v>
       </c>
-      <c r="BL20" s="58">
+      <c r="BL20" s="55">
         <v>8</v>
       </c>
       <c r="BM20" s="37" t="s">
@@ -5409,13 +5423,13 @@
       <c r="C21" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="57">
+      <c r="E21" s="54">
         <v>5</v>
       </c>
-      <c r="F21" s="57" t="s">
+      <c r="F21" s="54" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="28">
@@ -5424,19 +5438,19 @@
       <c r="H21" s="27">
         <v>400</v>
       </c>
-      <c r="I21" s="70">
+      <c r="I21" s="67">
         <v>35</v>
       </c>
-      <c r="J21" s="69">
+      <c r="J21" s="66">
         <v>45</v>
       </c>
       <c r="K21" s="25">
         <v>10</v>
       </c>
-      <c r="L21" s="65">
+      <c r="L21" s="62">
         <v>0</v>
       </c>
-      <c r="M21" s="64">
+      <c r="M21" s="61">
         <v>250</v>
       </c>
       <c r="N21" s="26">
@@ -5451,19 +5465,19 @@
       <c r="Q21" s="29">
         <v>1.2E-2</v>
       </c>
-      <c r="R21" s="50">
+      <c r="R21" s="49">
         <v>30</v>
       </c>
-      <c r="S21" s="50">
+      <c r="S21" s="49">
         <v>0.6</v>
       </c>
-      <c r="T21" s="64">
+      <c r="T21" s="61">
         <v>1.05</v>
       </c>
       <c r="U21" s="29">
         <v>1.3</v>
       </c>
-      <c r="V21" s="68">
+      <c r="V21" s="65">
         <v>21</v>
       </c>
       <c r="W21" s="29">
@@ -5482,32 +5496,32 @@
       <c r="AA21" s="29">
         <v>14</v>
       </c>
-      <c r="AB21" s="68">
+      <c r="AB21" s="65">
         <v>375</v>
       </c>
-      <c r="AC21" s="50">
+      <c r="AC21" s="49">
         <v>11</v>
       </c>
       <c r="AD21" s="29">
         <v>4</v>
       </c>
-      <c r="AE21" s="50">
+      <c r="AE21" s="49">
         <v>10</v>
       </c>
       <c r="AF21" s="29">
         <v>10000</v>
       </c>
-      <c r="AG21" s="67">
+      <c r="AG21" s="64">
         <v>3</v>
       </c>
-      <c r="AH21" s="117">
+      <c r="AH21" s="114">
         <v>0.09</v>
       </c>
-      <c r="AI21" s="67">
+      <c r="AI21" s="64">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="AJ21" s="74">
+      <c r="AJ21" s="71">
         <v>0</v>
       </c>
       <c r="AK21" s="45">
@@ -5551,10 +5565,10 @@
       <c r="AY21" s="24">
         <v>0.5</v>
       </c>
-      <c r="AZ21" s="60" t="s">
+      <c r="AZ21" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="BA21" s="59" t="s">
+      <c r="BA21" s="56" t="s">
         <v>94</v>
       </c>
       <c r="BB21" s="41">
@@ -5566,28 +5580,28 @@
       <c r="BD21" s="39">
         <v>322</v>
       </c>
-      <c r="BE21" s="112">
+      <c r="BE21" s="109">
         <v>347</v>
       </c>
-      <c r="BF21" s="58">
+      <c r="BF21" s="55">
         <v>2.5</v>
       </c>
-      <c r="BG21" s="58">
+      <c r="BG21" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH21" s="58">
+      <c r="BH21" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI21" s="58">
+      <c r="BI21" s="55">
         <v>0.5</v>
       </c>
-      <c r="BJ21" s="58">
+      <c r="BJ21" s="55">
         <v>1.7</v>
       </c>
-      <c r="BK21" s="58">
+      <c r="BK21" s="55">
         <v>9</v>
       </c>
-      <c r="BL21" s="58">
+      <c r="BL21" s="55">
         <v>8</v>
       </c>
       <c r="BM21" s="37" t="s">
@@ -5601,13 +5615,13 @@
       <c r="C22" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="57">
+      <c r="E22" s="54">
         <v>6</v>
       </c>
-      <c r="F22" s="56" t="s">
+      <c r="F22" s="53" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="28">
@@ -5616,19 +5630,19 @@
       <c r="H22" s="27">
         <v>550</v>
       </c>
-      <c r="I22" s="70">
+      <c r="I22" s="67">
         <v>35</v>
       </c>
-      <c r="J22" s="69">
+      <c r="J22" s="66">
         <v>45</v>
       </c>
       <c r="K22" s="25">
         <v>12.5</v>
       </c>
-      <c r="L22" s="65">
+      <c r="L22" s="62">
         <v>0</v>
       </c>
-      <c r="M22" s="64">
+      <c r="M22" s="61">
         <v>290</v>
       </c>
       <c r="N22" s="29">
@@ -5643,19 +5657,19 @@
       <c r="Q22" s="29">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="R22" s="50">
+      <c r="R22" s="49">
         <v>25</v>
       </c>
-      <c r="S22" s="50">
+      <c r="S22" s="49">
         <v>0.6</v>
       </c>
-      <c r="T22" s="64">
+      <c r="T22" s="61">
         <v>1.35</v>
       </c>
       <c r="U22" s="29">
         <v>1.55</v>
       </c>
-      <c r="V22" s="68">
+      <c r="V22" s="65">
         <v>23.5</v>
       </c>
       <c r="W22" s="29">
@@ -5674,32 +5688,32 @@
       <c r="AA22" s="29">
         <v>17</v>
       </c>
-      <c r="AB22" s="68">
+      <c r="AB22" s="65">
         <v>400</v>
       </c>
-      <c r="AC22" s="50">
+      <c r="AC22" s="49">
         <v>11</v>
       </c>
       <c r="AD22" s="29">
         <v>5</v>
       </c>
-      <c r="AE22" s="50">
+      <c r="AE22" s="49">
         <v>10</v>
       </c>
       <c r="AF22" s="29">
         <v>10000</v>
       </c>
-      <c r="AG22" s="67">
+      <c r="AG22" s="64">
         <v>3</v>
       </c>
-      <c r="AH22" s="117">
+      <c r="AH22" s="114">
         <v>0.08</v>
       </c>
-      <c r="AI22" s="67">
+      <c r="AI22" s="64">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ22" s="74">
+      <c r="AJ22" s="71">
         <v>0</v>
       </c>
       <c r="AK22" s="45">
@@ -5743,10 +5757,10 @@
       <c r="AY22" s="24">
         <v>0.5</v>
       </c>
-      <c r="AZ22" s="60" t="s">
+      <c r="AZ22" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="BA22" s="59" t="s">
+      <c r="BA22" s="56" t="s">
         <v>89</v>
       </c>
       <c r="BB22" s="41">
@@ -5758,28 +5772,28 @@
       <c r="BD22" s="39">
         <v>343</v>
       </c>
-      <c r="BE22" s="112">
+      <c r="BE22" s="109">
         <v>372</v>
       </c>
-      <c r="BF22" s="58">
+      <c r="BF22" s="55">
         <v>2.6</v>
       </c>
-      <c r="BG22" s="58">
+      <c r="BG22" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH22" s="58">
+      <c r="BH22" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI22" s="58">
+      <c r="BI22" s="55">
         <v>0.5</v>
       </c>
-      <c r="BJ22" s="58">
+      <c r="BJ22" s="55">
         <v>0.9</v>
       </c>
-      <c r="BK22" s="58">
+      <c r="BK22" s="55">
         <v>9</v>
       </c>
-      <c r="BL22" s="58">
+      <c r="BL22" s="55">
         <v>8</v>
       </c>
       <c r="BM22" s="37" t="s">
@@ -5796,31 +5810,31 @@
       <c r="D23" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="57">
+      <c r="E23" s="54">
         <v>7</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="53" t="s">
         <v>11</v>
       </c>
       <c r="G23" s="30">
         <v>870000</v>
       </c>
-      <c r="H23" s="55">
+      <c r="H23" s="52">
         <v>800</v>
       </c>
-      <c r="I23" s="54">
+      <c r="I23" s="51">
         <v>35</v>
       </c>
-      <c r="J23" s="66">
+      <c r="J23" s="63">
         <v>45</v>
       </c>
       <c r="K23" s="25">
         <v>17</v>
       </c>
-      <c r="L23" s="65">
+      <c r="L23" s="62">
         <v>0</v>
       </c>
-      <c r="M23" s="64">
+      <c r="M23" s="61">
         <v>330</v>
       </c>
       <c r="N23" s="29">
@@ -5835,19 +5849,19 @@
       <c r="Q23" s="29">
         <v>1.4E-2</v>
       </c>
-      <c r="R23" s="50">
+      <c r="R23" s="49">
         <v>25</v>
       </c>
-      <c r="S23" s="50">
+      <c r="S23" s="49">
         <v>0.7</v>
       </c>
-      <c r="T23" s="64">
+      <c r="T23" s="61">
         <v>1.54</v>
       </c>
       <c r="U23" s="29">
         <v>1.74</v>
       </c>
-      <c r="V23" s="49">
+      <c r="V23" s="48">
         <v>25</v>
       </c>
       <c r="W23" s="29">
@@ -5866,35 +5880,35 @@
       <c r="AA23" s="29">
         <v>18</v>
       </c>
-      <c r="AB23" s="49">
+      <c r="AB23" s="48">
         <v>425</v>
       </c>
-      <c r="AC23" s="50">
+      <c r="AC23" s="49">
         <v>11.5</v>
       </c>
       <c r="AD23" s="26">
         <v>5</v>
       </c>
-      <c r="AE23" s="63">
+      <c r="AE23" s="60">
         <v>10</v>
       </c>
       <c r="AF23" s="29">
         <v>20000</v>
       </c>
-      <c r="AG23" s="62">
+      <c r="AG23" s="59">
         <v>4</v>
       </c>
-      <c r="AH23" s="118">
+      <c r="AH23" s="115">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI23" s="67">
+      <c r="AI23" s="64">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="AJ23" s="120">
+      <c r="AJ23" s="117">
         <v>0</v>
       </c>
-      <c r="AK23" s="61">
+      <c r="AK23" s="58">
         <v>12</v>
       </c>
       <c r="AL23" s="44" t="s">
@@ -5939,10 +5953,10 @@
       <c r="AY23" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ23" s="60" t="s">
+      <c r="AZ23" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="BA23" s="59" t="s">
+      <c r="BA23" s="56" t="s">
         <v>85</v>
       </c>
       <c r="BB23" s="41">
@@ -5954,28 +5968,28 @@
       <c r="BD23" s="39">
         <v>435</v>
       </c>
-      <c r="BE23" s="112">
+      <c r="BE23" s="109">
         <v>465</v>
       </c>
-      <c r="BF23" s="58">
+      <c r="BF23" s="55">
         <v>3.2</v>
       </c>
-      <c r="BG23" s="58">
+      <c r="BG23" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH23" s="58">
+      <c r="BH23" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI23" s="58">
+      <c r="BI23" s="55">
         <v>0.5</v>
       </c>
-      <c r="BJ23" s="58">
+      <c r="BJ23" s="55">
         <v>1.2</v>
       </c>
-      <c r="BK23" s="58">
+      <c r="BK23" s="55">
         <v>45</v>
       </c>
-      <c r="BL23" s="58">
+      <c r="BL23" s="55">
         <v>15</v>
       </c>
       <c r="BM23" s="37" t="s">
@@ -5986,194 +6000,194 @@
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="97" t="s">
         <v>184</v>
       </c>
-      <c r="D24" s="100" t="s">
+      <c r="D24" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="97">
+      <c r="E24" s="94">
         <v>8</v>
       </c>
-      <c r="F24" s="101" t="s">
+      <c r="F24" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="110">
+      <c r="G24" s="107">
         <v>1400000</v>
       </c>
       <c r="H24" s="22">
         <v>800</v>
       </c>
-      <c r="I24" s="54">
+      <c r="I24" s="51">
         <v>35</v>
       </c>
-      <c r="J24" s="66">
+      <c r="J24" s="63">
         <v>45</v>
       </c>
-      <c r="K24" s="104">
+      <c r="K24" s="101">
         <v>25</v>
       </c>
-      <c r="L24" s="105">
+      <c r="L24" s="102">
         <v>0</v>
       </c>
       <c r="M24" s="45">
         <v>360</v>
       </c>
-      <c r="N24" s="50">
+      <c r="N24" s="49">
         <v>430</v>
       </c>
-      <c r="O24" s="50">
+      <c r="O24" s="49">
         <v>2.2999999999999998</v>
       </c>
-      <c r="P24" s="50">
+      <c r="P24" s="49">
         <v>0</v>
       </c>
-      <c r="Q24" s="50">
+      <c r="Q24" s="49">
         <v>1.4E-2</v>
       </c>
-      <c r="R24" s="50">
+      <c r="R24" s="49">
         <v>25</v>
       </c>
-      <c r="S24" s="50">
+      <c r="S24" s="49">
         <v>0.7</v>
       </c>
       <c r="T24" s="45">
         <v>1.7</v>
       </c>
-      <c r="U24" s="50">
+      <c r="U24" s="49">
         <v>1.95</v>
       </c>
-      <c r="V24" s="49">
+      <c r="V24" s="48">
         <v>25</v>
       </c>
-      <c r="W24" s="50">
+      <c r="W24" s="49">
         <v>1.8</v>
       </c>
-      <c r="X24" s="50">
+      <c r="X24" s="49">
         <v>100</v>
       </c>
-      <c r="Y24" s="50">
+      <c r="Y24" s="49">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z24" s="50">
+      <c r="Z24" s="49">
         <v>40</v>
       </c>
-      <c r="AA24" s="50">
+      <c r="AA24" s="49">
         <v>14</v>
       </c>
-      <c r="AB24" s="49">
+      <c r="AB24" s="48">
         <v>425</v>
       </c>
-      <c r="AC24" s="50">
+      <c r="AC24" s="49">
         <v>11.5</v>
       </c>
-      <c r="AD24" s="48">
+      <c r="AD24" s="47">
         <v>5</v>
       </c>
-      <c r="AE24" s="63">
+      <c r="AE24" s="60">
         <v>10</v>
       </c>
-      <c r="AF24" s="50">
+      <c r="AF24" s="49">
         <v>20000</v>
       </c>
-      <c r="AG24" s="109">
+      <c r="AG24" s="106">
         <v>4</v>
       </c>
-      <c r="AH24" s="119">
+      <c r="AH24" s="116">
         <v>0.06</v>
       </c>
-      <c r="AI24" s="115">
+      <c r="AI24" s="112">
         <v>0.05</v>
       </c>
-      <c r="AJ24" s="120">
+      <c r="AJ24" s="117">
         <v>0</v>
       </c>
-      <c r="AK24" s="61">
+      <c r="AK24" s="58">
         <v>12</v>
       </c>
-      <c r="AL24" s="99" t="s">
+      <c r="AL24" s="96" t="s">
         <v>185</v>
       </c>
-      <c r="AM24" s="98" t="s">
+      <c r="AM24" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="AN24" s="98" t="s">
+      <c r="AN24" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="AO24" s="98" t="s">
+      <c r="AO24" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="AP24" s="98" t="s">
+      <c r="AP24" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="AQ24" s="98">
+      <c r="AQ24" s="95">
         <v>1.3</v>
       </c>
-      <c r="AR24" s="98">
+      <c r="AR24" s="95">
         <v>2</v>
       </c>
-      <c r="AS24" s="98">
+      <c r="AS24" s="95">
         <v>2</v>
       </c>
-      <c r="AT24" s="98" t="b">
+      <c r="AT24" s="95" t="b">
         <v>1</v>
       </c>
-      <c r="AU24" s="98" t="b">
+      <c r="AU24" s="95" t="b">
         <v>1</v>
       </c>
-      <c r="AV24" s="98" t="b">
+      <c r="AV24" s="95" t="b">
         <v>1</v>
       </c>
-      <c r="AW24" s="98">
+      <c r="AW24" s="95">
         <v>23</v>
       </c>
-      <c r="AX24" s="98">
+      <c r="AX24" s="95">
         <v>0.7</v>
       </c>
-      <c r="AY24" s="98">
+      <c r="AY24" s="95">
         <v>0.6</v>
       </c>
-      <c r="AZ24" s="102" t="s">
+      <c r="AZ24" s="99" t="s">
         <v>187</v>
       </c>
       <c r="BA24" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BB24" s="106">
+      <c r="BB24" s="103">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BC24" s="107">
+      <c r="BC24" s="104">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD24" s="108">
+      <c r="BD24" s="105">
         <v>450</v>
       </c>
-      <c r="BE24" s="113">
+      <c r="BE24" s="110">
         <v>505</v>
       </c>
-      <c r="BF24" s="103">
+      <c r="BF24" s="100">
         <v>3.4</v>
       </c>
-      <c r="BG24" s="103">
+      <c r="BG24" s="100">
         <v>9.5</v>
       </c>
-      <c r="BH24" s="103">
+      <c r="BH24" s="100">
         <v>1.7</v>
       </c>
-      <c r="BI24" s="103">
+      <c r="BI24" s="100">
         <v>0.6</v>
       </c>
-      <c r="BJ24" s="103">
+      <c r="BJ24" s="100">
         <v>1</v>
       </c>
-      <c r="BK24" s="103">
+      <c r="BK24" s="100">
         <v>45</v>
       </c>
-      <c r="BL24" s="103">
+      <c r="BL24" s="100">
         <v>15</v>
       </c>
-      <c r="BM24" s="100" t="s">
+      <c r="BM24" s="97" t="s">
         <v>184</v>
       </c>
     </row>
@@ -6187,31 +6201,31 @@
       <c r="D25" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="57">
+      <c r="E25" s="54">
         <v>9</v>
       </c>
-      <c r="F25" s="56" t="s">
+      <c r="F25" s="53" t="s">
         <v>184</v>
       </c>
       <c r="G25" s="30">
         <v>2200000</v>
       </c>
-      <c r="H25" s="55">
+      <c r="H25" s="52">
         <v>800</v>
       </c>
-      <c r="I25" s="54">
+      <c r="I25" s="51">
         <v>35</v>
       </c>
-      <c r="J25" s="66">
+      <c r="J25" s="63">
         <v>45</v>
       </c>
       <c r="K25" s="25">
         <v>10</v>
       </c>
-      <c r="L25" s="65">
+      <c r="L25" s="62">
         <v>0</v>
       </c>
-      <c r="M25" s="64">
+      <c r="M25" s="61">
         <v>375</v>
       </c>
       <c r="N25" s="26">
@@ -6226,10 +6240,10 @@
       <c r="Q25" s="29">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="R25" s="50">
+      <c r="R25" s="49">
         <v>25</v>
       </c>
-      <c r="S25" s="50">
+      <c r="S25" s="49">
         <v>0.7</v>
       </c>
       <c r="T25" s="46">
@@ -6238,7 +6252,7 @@
       <c r="U25" s="26">
         <v>1.57</v>
       </c>
-      <c r="V25" s="49">
+      <c r="V25" s="48">
         <v>28</v>
       </c>
       <c r="W25" s="29">
@@ -6257,35 +6271,35 @@
       <c r="AA25" s="26">
         <v>34</v>
       </c>
-      <c r="AB25" s="49">
+      <c r="AB25" s="48">
         <v>450</v>
       </c>
-      <c r="AC25" s="50">
+      <c r="AC25" s="49">
         <v>11.5</v>
       </c>
       <c r="AD25" s="26">
         <v>6</v>
       </c>
-      <c r="AE25" s="63">
+      <c r="AE25" s="60">
         <v>10</v>
       </c>
       <c r="AF25" s="29">
         <v>20000</v>
       </c>
-      <c r="AG25" s="62">
+      <c r="AG25" s="59">
         <v>4</v>
       </c>
-      <c r="AH25" s="118">
+      <c r="AH25" s="115">
         <v>0.06</v>
       </c>
-      <c r="AI25" s="67">
+      <c r="AI25" s="64">
         <f>AH26</f>
         <v>0.05</v>
       </c>
-      <c r="AJ25" s="120">
+      <c r="AJ25" s="117">
         <v>0</v>
       </c>
-      <c r="AK25" s="61">
+      <c r="AK25" s="58">
         <v>12</v>
       </c>
       <c r="AL25" s="44" t="s">
@@ -6330,10 +6344,10 @@
       <c r="AY25" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ25" s="60" t="s">
+      <c r="AZ25" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="BA25" s="59" t="s">
+      <c r="BA25" s="56" t="s">
         <v>80</v>
       </c>
       <c r="BB25" s="41">
@@ -6345,35 +6359,35 @@
       <c r="BD25" s="39">
         <v>540</v>
       </c>
-      <c r="BE25" s="112">
+      <c r="BE25" s="109">
         <v>590</v>
       </c>
-      <c r="BF25" s="58">
+      <c r="BF25" s="55">
         <v>3.9</v>
       </c>
-      <c r="BG25" s="58">
+      <c r="BG25" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH25" s="58">
+      <c r="BH25" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI25" s="58">
+      <c r="BI25" s="55">
         <v>0.3</v>
       </c>
-      <c r="BJ25" s="58">
+      <c r="BJ25" s="55">
         <v>0.4</v>
       </c>
-      <c r="BK25" s="58">
+      <c r="BK25" s="55">
         <v>45</v>
       </c>
-      <c r="BL25" s="58">
+      <c r="BL25" s="55">
         <v>15</v>
       </c>
       <c r="BM25" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6383,31 +6397,31 @@
       <c r="D26" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="57">
+      <c r="E26" s="54">
         <v>10</v>
       </c>
-      <c r="F26" s="56" t="s">
+      <c r="F26" s="53" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="30">
         <v>3300000</v>
       </c>
-      <c r="H26" s="55">
+      <c r="H26" s="52">
         <v>1100</v>
       </c>
-      <c r="I26" s="54">
+      <c r="I26" s="51">
         <v>35</v>
       </c>
-      <c r="J26" s="53">
+      <c r="J26" s="66">
         <v>45</v>
       </c>
       <c r="K26" s="25">
         <v>25</v>
       </c>
-      <c r="L26" s="52">
+      <c r="L26" s="50">
         <v>0</v>
       </c>
-      <c r="M26" s="51">
+      <c r="M26" s="25">
         <v>425</v>
       </c>
       <c r="N26" s="26">
@@ -6422,10 +6436,10 @@
       <c r="Q26" s="29">
         <v>1.6E-2</v>
       </c>
-      <c r="R26" s="50">
+      <c r="R26" s="49">
         <v>20</v>
       </c>
-      <c r="S26" s="50">
+      <c r="S26" s="49">
         <v>0.8</v>
       </c>
       <c r="T26" s="46">
@@ -6434,7 +6448,7 @@
       <c r="U26" s="26">
         <v>2.1</v>
       </c>
-      <c r="V26" s="49">
+      <c r="V26" s="48">
         <v>31</v>
       </c>
       <c r="W26" s="26">
@@ -6453,31 +6467,31 @@
       <c r="AA26" s="26">
         <v>12</v>
       </c>
-      <c r="AB26" s="49">
+      <c r="AB26" s="48">
         <v>475</v>
       </c>
-      <c r="AC26" s="48">
+      <c r="AC26" s="47">
         <v>12</v>
       </c>
       <c r="AD26" s="26">
         <v>6</v>
       </c>
-      <c r="AE26" s="48">
+      <c r="AE26" s="47">
         <v>10</v>
       </c>
       <c r="AF26" s="26">
         <v>30000</v>
       </c>
-      <c r="AG26" s="47">
+      <c r="AG26" s="25">
         <v>5</v>
       </c>
-      <c r="AH26" s="118">
+      <c r="AH26" s="50">
         <v>0.05</v>
       </c>
-      <c r="AI26" s="67">
+      <c r="AI26" s="64">
         <v>0.04</v>
       </c>
-      <c r="AJ26" s="74">
+      <c r="AJ26" s="71">
         <v>0</v>
       </c>
       <c r="AK26" s="45">
@@ -6540,7 +6554,7 @@
       <c r="BD26" s="39">
         <v>680</v>
       </c>
-      <c r="BE26" s="114">
+      <c r="BE26" s="111">
         <v>730</v>
       </c>
       <c r="BF26" s="38">
@@ -6578,49 +6592,49 @@
       <c r="D27" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="57">
+      <c r="E27" s="54">
         <v>11</v>
       </c>
-      <c r="F27" s="56" t="s">
+      <c r="F27" s="53" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="30">
         <v>4800000</v>
       </c>
-      <c r="H27" s="55">
+      <c r="H27" s="52">
         <v>1100</v>
       </c>
-      <c r="I27" s="54">
+      <c r="I27" s="51">
         <v>35</v>
       </c>
-      <c r="J27" s="53">
+      <c r="J27" s="130">
         <v>45</v>
       </c>
       <c r="K27" s="25">
         <v>25</v>
       </c>
-      <c r="L27" s="52">
+      <c r="L27" s="50">
         <v>0</v>
       </c>
-      <c r="M27" s="51">
-        <v>425</v>
+      <c r="M27" s="131">
+        <v>1000</v>
       </c>
       <c r="N27" s="26">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="O27" s="26">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="P27" s="26">
         <v>0</v>
       </c>
       <c r="Q27" s="29">
-        <v>1.6E-2</v>
-      </c>
-      <c r="R27" s="50">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="R27" s="49">
         <v>20</v>
       </c>
-      <c r="S27" s="50">
+      <c r="S27" s="49">
         <v>0.8</v>
       </c>
       <c r="T27" s="46">
@@ -6629,7 +6643,7 @@
       <c r="U27" s="26">
         <v>2.1</v>
       </c>
-      <c r="V27" s="49">
+      <c r="V27" s="48">
         <v>31</v>
       </c>
       <c r="W27" s="26">
@@ -6646,33 +6660,33 @@
         <v>19</v>
       </c>
       <c r="AA27" s="26">
-        <v>12</v>
-      </c>
-      <c r="AB27" s="49">
+        <v>19</v>
+      </c>
+      <c r="AB27" s="48">
         <v>475</v>
       </c>
-      <c r="AC27" s="48">
+      <c r="AC27" s="47">
         <v>12</v>
       </c>
       <c r="AD27" s="26">
         <v>6</v>
       </c>
-      <c r="AE27" s="48">
+      <c r="AE27" s="47">
         <v>10</v>
       </c>
       <c r="AF27" s="26">
-        <v>30000</v>
-      </c>
-      <c r="AG27" s="47">
+        <v>20000</v>
+      </c>
+      <c r="AG27" s="132">
         <v>5</v>
       </c>
-      <c r="AH27" s="118">
+      <c r="AH27" s="115">
         <v>0.05</v>
       </c>
-      <c r="AI27" s="67">
+      <c r="AI27" s="64">
         <v>0.04</v>
       </c>
-      <c r="AJ27" s="74">
+      <c r="AJ27" s="71">
         <v>0</v>
       </c>
       <c r="AK27" s="45">
@@ -6727,7 +6741,7 @@
         <v>199</v>
       </c>
       <c r="BB27" s="41">
-        <v>1.5E-3</v>
+        <v>8.7000000000000001E-4</v>
       </c>
       <c r="BC27" s="40">
         <v>5.0000000000000001E-3</v>
@@ -6735,7 +6749,7 @@
       <c r="BD27" s="39">
         <v>680</v>
       </c>
-      <c r="BE27" s="114">
+      <c r="BE27" s="111">
         <v>730</v>
       </c>
       <c r="BF27" s="38">
@@ -6771,55 +6785,55 @@
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
-      <c r="I28" s="123" t="s">
+      <c r="I28" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="124"/>
-      <c r="K28" s="124"/>
-      <c r="L28" s="125"/>
+      <c r="J28" s="121"/>
+      <c r="K28" s="121"/>
+      <c r="L28" s="122"/>
       <c r="M28" s="36"/>
-      <c r="N28" s="127" t="s">
+      <c r="N28" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="127"/>
-      <c r="P28" s="127"/>
-      <c r="Q28" s="127"/>
-      <c r="R28" s="127"/>
-      <c r="S28" s="128"/>
-      <c r="T28" s="126" t="s">
+      <c r="O28" s="124"/>
+      <c r="P28" s="124"/>
+      <c r="Q28" s="124"/>
+      <c r="R28" s="124"/>
+      <c r="S28" s="125"/>
+      <c r="T28" s="123" t="s">
         <v>72</v>
       </c>
-      <c r="U28" s="126"/>
+      <c r="U28" s="123"/>
       <c r="V28" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W28" s="129" t="s">
+      <c r="W28" s="126" t="s">
         <v>70</v>
       </c>
-      <c r="X28" s="129"/>
-      <c r="Y28" s="129"/>
-      <c r="Z28" s="129"/>
-      <c r="AA28" s="129"/>
-      <c r="AB28" s="130" t="s">
+      <c r="X28" s="126"/>
+      <c r="Y28" s="126"/>
+      <c r="Z28" s="126"/>
+      <c r="AA28" s="126"/>
+      <c r="AB28" s="127" t="s">
         <v>69</v>
       </c>
-      <c r="AC28" s="130"/>
-      <c r="AD28" s="130"/>
-      <c r="AE28" s="130"/>
-      <c r="AF28" s="131"/>
-      <c r="AH28" s="132" t="s">
+      <c r="AC28" s="127"/>
+      <c r="AD28" s="127"/>
+      <c r="AE28" s="127"/>
+      <c r="AF28" s="128"/>
+      <c r="AH28" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="AI28" s="132"/>
-      <c r="BD28" s="121" t="s">
+      <c r="AI28" s="129"/>
+      <c r="BD28" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="BE28" s="121"/>
-      <c r="BF28" s="121"/>
-      <c r="BG28" s="121"/>
-      <c r="BH28" s="121"/>
-      <c r="BI28" s="121"/>
-      <c r="BJ28" s="121"/>
+      <c r="BE28" s="118"/>
+      <c r="BF28" s="118"/>
+      <c r="BG28" s="118"/>
+      <c r="BH28" s="118"/>
+      <c r="BI28" s="118"/>
+      <c r="BJ28" s="118"/>
     </row>
     <row r="30" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
@@ -7634,61 +7648,61 @@
       <c r="D54">
         <v>20</v>
       </c>
-      <c r="E54" s="111">
+      <c r="E54" s="108">
         <v>2940</v>
       </c>
-      <c r="F54" s="111">
+      <c r="F54" s="108">
         <v>8821</v>
       </c>
-      <c r="G54" s="111">
+      <c r="G54" s="108">
         <v>17642</v>
       </c>
-      <c r="H54" s="111">
+      <c r="H54" s="108">
         <v>29403</v>
       </c>
-      <c r="I54" s="111">
+      <c r="I54" s="108">
         <v>44105</v>
       </c>
-      <c r="J54" s="111">
+      <c r="J54" s="108">
         <v>61747</v>
       </c>
-      <c r="K54" s="111">
+      <c r="K54" s="108">
         <v>82329</v>
       </c>
-      <c r="L54" s="111">
+      <c r="L54" s="108">
         <v>105851</v>
       </c>
-      <c r="M54" s="111">
+      <c r="M54" s="108">
         <v>132314</v>
       </c>
-      <c r="N54" s="111">
+      <c r="N54" s="108">
         <v>161717</v>
       </c>
-      <c r="O54" s="111">
+      <c r="O54" s="108">
         <v>194061</v>
       </c>
-      <c r="P54" s="111">
+      <c r="P54" s="108">
         <v>229345</v>
       </c>
-      <c r="Q54" s="111">
+      <c r="Q54" s="108">
         <v>267569</v>
       </c>
-      <c r="R54" s="111">
+      <c r="R54" s="108">
         <v>308733</v>
       </c>
-      <c r="S54" s="111">
+      <c r="S54" s="108">
         <v>352838</v>
       </c>
-      <c r="T54" s="111">
+      <c r="T54" s="108">
         <v>399883</v>
       </c>
-      <c r="U54" s="111">
+      <c r="U54" s="108">
         <v>449868</v>
       </c>
-      <c r="V54" s="111">
+      <c r="V54" s="108">
         <v>502794</v>
       </c>
-      <c r="W54" s="111">
+      <c r="W54" s="108">
         <v>558660</v>
       </c>
     </row>
@@ -7907,20 +7921,26 @@
     <mergeCell ref="AB28:AF28"/>
     <mergeCell ref="AH28:AI28"/>
   </mergeCells>
-  <conditionalFormatting sqref="C16:C23 C25:C27">
-    <cfRule type="duplicateValues" dxfId="99" priority="4"/>
+  <conditionalFormatting sqref="C16:C23 C25:C26">
+    <cfRule type="duplicateValues" dxfId="101" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="98" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM16:BM23 BM25:BM27">
+  <conditionalFormatting sqref="BM16:BM23 BM25:BM26">
+    <cfRule type="duplicateValues" dxfId="99" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="duplicateValues" dxfId="98" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM24">
     <cfRule type="duplicateValues" dxfId="97" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM24">
-    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
+  <conditionalFormatting sqref="BM27">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">

</xml_diff>

<commit_message>
Content - Add dragon type in dragonDef
Former-commit-id: 76104dcfc3177b4b986e3d8dc82883a8ebfebf3e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="205">
   <si>
     <t>[sku]</t>
   </si>
@@ -633,6 +633,12 @@
   </si>
   <si>
     <t>PF_DragonGoldheistResults</t>
+  </si>
+  <si>
+    <t>[type]</t>
+  </si>
+  <si>
+    <t>normal</t>
   </si>
 </sst>
 </file>
@@ -1497,6 +1503,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1532,21 +1547,86 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="103">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3523,56 +3603,6 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3587,98 +3617,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BM27" totalsRowShown="0" headerRowDxfId="96" dataDxfId="94" headerRowBorderDxfId="95" tableBorderDxfId="93" totalsRowBorderDxfId="92">
-  <autoFilter ref="B15:BM27"/>
-  <tableColumns count="64">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="91"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="90"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="89"/>
-    <tableColumn id="3" name="[order]" dataDxfId="88"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="87"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="86"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="85"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="84"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="83"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="82"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="81"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="80"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="79"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="78"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="77"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="76"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="75"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="74"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="73"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="72"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="71"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="70"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="69"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BN27" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101" tableBorderDxfId="99" totalsRowBorderDxfId="98">
+  <autoFilter ref="B15:BN27"/>
+  <tableColumns count="65">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="97"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="96"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="95"/>
+    <tableColumn id="65" name="[type]" dataDxfId="0"/>
+    <tableColumn id="3" name="[order]" dataDxfId="94"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="93"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="92"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="91"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="90"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="89"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="88"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="87"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="86"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="85"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="84"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="83"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="82"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="81"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="80"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="79"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="78"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="77"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="76"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="75"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="74">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="67"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="66"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="65"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="64"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="63"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="62"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="61"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="60"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="59"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="58">
-      <calculatedColumnFormula>AH17</calculatedColumnFormula>
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="73"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="72"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="71"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="70"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="69"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="68"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="67"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="66"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="65"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="64">
+      <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="57"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="56"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="55"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="54"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="53"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="52"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="51"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="50"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="49"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="48"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="47"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="46"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="45"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="44"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="43"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="42"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="41">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="63"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="62"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="61"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="60"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="59"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="58"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="57"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="56"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="55"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="54"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="53"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="52"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="51"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="50"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="49"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="48"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="47">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="40">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="46">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="39"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="38"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="37"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="36">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="45"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="44"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="43"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="42">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="35"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="34"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="33"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="32"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="31"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="30"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="29"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="28"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="41"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="40"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="39"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="38"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="37"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="36"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="35"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="23"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="29"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="22"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="21"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="20">
+    <tableColumn id="10" name="[icon]" dataDxfId="28"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="27"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="26">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3687,11 +3718,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B33:I34"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="21"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="20"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3704,7 +3735,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B45:W57"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3735,14 +3766,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="B38:F41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="5"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="11"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="3"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="2"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="9"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4014,10 +4045,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BM57"/>
+  <dimension ref="B1:BN57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR13" workbookViewId="0">
-      <selection activeCell="BB29" sqref="BB29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4046,8 +4077,8 @@
     <col min="65" max="65" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:66" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>183</v>
       </c>
@@ -4076,7 +4107,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4084,7 +4115,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:65" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:66" ht="117" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>182</v>
       </c>
@@ -4104,7 +4135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -4125,7 +4156,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -4146,7 +4177,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4167,7 +4198,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4188,7 +4219,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4209,8 +4240,8 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:66" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4239,7 +4270,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:65" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:66" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
         <v>174</v>
       </c>
@@ -4259,12 +4290,12 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="119"/>
-      <c r="AP14" s="119"/>
-      <c r="AQ14" s="119"/>
-      <c r="AR14" s="119"/>
+      <c r="AO14" s="122"/>
+      <c r="AP14" s="122"/>
+      <c r="AQ14" s="122"/>
+      <c r="AR14" s="122"/>
     </row>
-    <row r="15" spans="2:65" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:66" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
         <v>170</v>
       </c>
@@ -4274,191 +4305,194 @@
       <c r="D15" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="G15" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="90" t="s">
+      <c r="H15" s="90" t="s">
         <v>168</v>
       </c>
-      <c r="H15" s="89" t="s">
+      <c r="I15" s="89" t="s">
         <v>167</v>
       </c>
-      <c r="I15" s="88" t="s">
+      <c r="J15" s="88" t="s">
         <v>166</v>
       </c>
-      <c r="J15" s="87" t="s">
+      <c r="K15" s="87" t="s">
         <v>165</v>
       </c>
-      <c r="K15" s="86" t="s">
+      <c r="L15" s="86" t="s">
         <v>164</v>
       </c>
-      <c r="L15" s="84" t="s">
+      <c r="M15" s="84" t="s">
         <v>163</v>
       </c>
-      <c r="M15" s="82" t="s">
+      <c r="N15" s="82" t="s">
         <v>162</v>
       </c>
-      <c r="N15" s="86" t="s">
+      <c r="O15" s="86" t="s">
         <v>161</v>
       </c>
-      <c r="O15" s="84" t="s">
+      <c r="P15" s="84" t="s">
         <v>160</v>
       </c>
-      <c r="P15" s="84" t="s">
+      <c r="Q15" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="Q15" s="83" t="s">
+      <c r="R15" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="R15" s="83" t="s">
+      <c r="S15" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="S15" s="83" t="s">
+      <c r="T15" s="83" t="s">
         <v>156</v>
       </c>
-      <c r="T15" s="82" t="s">
+      <c r="U15" s="82" t="s">
         <v>155</v>
       </c>
-      <c r="U15" s="84" t="s">
+      <c r="V15" s="84" t="s">
         <v>154</v>
       </c>
-      <c r="V15" s="85" t="s">
+      <c r="W15" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="W15" s="82" t="s">
+      <c r="X15" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="X15" s="86" t="s">
+      <c r="Y15" s="86" t="s">
         <v>191</v>
       </c>
-      <c r="Y15" s="86" t="s">
+      <c r="Z15" s="86" t="s">
         <v>192</v>
       </c>
-      <c r="Z15" s="86" t="s">
+      <c r="AA15" s="86" t="s">
         <v>151</v>
       </c>
-      <c r="AA15" s="84" t="s">
+      <c r="AB15" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="AB15" s="85" t="s">
+      <c r="AC15" s="85" t="s">
         <v>149</v>
       </c>
-      <c r="AC15" s="84" t="s">
+      <c r="AD15" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="AD15" s="84" t="s">
+      <c r="AE15" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="AE15" s="84" t="s">
+      <c r="AF15" s="84" t="s">
         <v>146</v>
       </c>
-      <c r="AF15" s="113" t="s">
+      <c r="AG15" s="113" t="s">
         <v>145</v>
       </c>
-      <c r="AG15" s="83" t="s">
+      <c r="AH15" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="AH15" s="82" t="s">
+      <c r="AI15" s="82" t="s">
         <v>193</v>
       </c>
-      <c r="AI15" s="82" t="s">
+      <c r="AJ15" s="82" t="s">
         <v>194</v>
       </c>
-      <c r="AJ15" s="82" t="s">
+      <c r="AK15" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="AK15" s="82" t="s">
+      <c r="AL15" s="82" t="s">
         <v>142</v>
       </c>
-      <c r="AL15" s="81" t="s">
+      <c r="AM15" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="AM15" s="79" t="s">
+      <c r="AN15" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="AN15" s="79" t="s">
+      <c r="AO15" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="AO15" s="79" t="s">
+      <c r="AP15" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="AP15" s="79" t="s">
+      <c r="AQ15" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="AQ15" s="79" t="s">
+      <c r="AR15" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="AR15" s="80" t="s">
+      <c r="AS15" s="80" t="s">
         <v>137</v>
       </c>
-      <c r="AS15" s="79" t="s">
+      <c r="AT15" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="AT15" s="79" t="s">
+      <c r="AU15" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="AU15" s="79" t="s">
+      <c r="AV15" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="AV15" s="79" t="s">
+      <c r="AW15" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="AW15" s="79" t="s">
+      <c r="AX15" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="AX15" s="79" t="s">
+      <c r="AY15" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="AY15" s="79" t="s">
+      <c r="AZ15" s="79" t="s">
         <v>196</v>
       </c>
-      <c r="AZ15" s="3" t="s">
+      <c r="BA15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BA15" s="78" t="s">
+      <c r="BB15" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="BB15" s="77" t="s">
+      <c r="BC15" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="BC15" s="73" t="s">
+      <c r="BD15" s="73" t="s">
         <v>129</v>
       </c>
-      <c r="BD15" s="76" t="s">
+      <c r="BE15" s="76" t="s">
         <v>189</v>
       </c>
-      <c r="BE15" s="72" t="s">
+      <c r="BF15" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="BF15" s="75" t="s">
+      <c r="BG15" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="BG15" s="75" t="s">
+      <c r="BH15" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="BH15" s="75" t="s">
+      <c r="BI15" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="BI15" s="72" t="s">
+      <c r="BJ15" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="BJ15" s="72" t="s">
+      <c r="BK15" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="BK15" s="74" t="s">
+      <c r="BL15" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="BL15" s="73" t="s">
+      <c r="BM15" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="BM15" s="72" t="s">
+      <c r="BN15" s="72" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4468,127 +4502,127 @@
       <c r="D16" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" s="54">
         <v>0</v>
       </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="28">
+      <c r="G16" s="54"/>
+      <c r="H16" s="28">
         <v>0</v>
       </c>
-      <c r="H16" s="27">
+      <c r="I16" s="27">
         <v>0</v>
       </c>
-      <c r="I16" s="67">
+      <c r="J16" s="67">
         <v>35</v>
       </c>
-      <c r="J16" s="66">
+      <c r="K16" s="66">
         <v>45</v>
       </c>
-      <c r="K16" s="25">
+      <c r="L16" s="25">
         <v>1</v>
       </c>
-      <c r="L16" s="62">
+      <c r="M16" s="62">
         <v>-2</v>
       </c>
-      <c r="M16" s="61">
+      <c r="N16" s="61">
         <v>75</v>
       </c>
-      <c r="N16" s="29">
+      <c r="O16" s="29">
         <v>105</v>
       </c>
-      <c r="O16" s="29">
+      <c r="P16" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P16" s="29">
+      <c r="Q16" s="29">
         <v>0</v>
       </c>
-      <c r="Q16" s="29">
+      <c r="R16" s="29">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="R16" s="49">
+      <c r="S16" s="49">
         <v>30</v>
       </c>
-      <c r="S16" s="49">
+      <c r="T16" s="49">
         <v>0.5</v>
       </c>
-      <c r="T16" s="61">
+      <c r="U16" s="61">
         <v>0.46</v>
       </c>
-      <c r="U16" s="29">
+      <c r="V16" s="29">
         <v>0.71</v>
       </c>
-      <c r="V16" s="65">
+      <c r="W16" s="65">
         <v>14</v>
       </c>
-      <c r="W16" s="29">
+      <c r="X16" s="29">
         <v>1.95</v>
       </c>
-      <c r="X16" s="29">
+      <c r="Y16" s="29">
         <v>100</v>
       </c>
-      <c r="Y16" s="29">
+      <c r="Z16" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z16" s="29">
+      <c r="AA16" s="29">
         <v>40</v>
       </c>
-      <c r="AA16" s="29">
+      <c r="AB16" s="29">
         <v>28</v>
       </c>
-      <c r="AB16" s="65">
+      <c r="AC16" s="65">
         <v>250</v>
       </c>
-      <c r="AC16" s="49">
+      <c r="AD16" s="49">
         <v>7.5</v>
       </c>
-      <c r="AD16" s="29">
+      <c r="AE16" s="29">
         <v>2</v>
       </c>
-      <c r="AE16" s="49">
+      <c r="AF16" s="49">
         <v>8</v>
       </c>
-      <c r="AF16" s="29">
+      <c r="AG16" s="29">
         <v>3000</v>
       </c>
-      <c r="AG16" s="64">
+      <c r="AH16" s="64">
         <v>1</v>
       </c>
-      <c r="AH16" s="114">
+      <c r="AI16" s="114">
         <v>0.23</v>
       </c>
-      <c r="AI16" s="64">
-        <f t="shared" ref="AI16:AI23" si="0">AH17</f>
+      <c r="AJ16" s="64">
+        <f t="shared" ref="AJ16:AJ23" si="0">AI17</f>
         <v>0.19</v>
       </c>
-      <c r="AJ16" s="71">
+      <c r="AK16" s="71">
         <v>0</v>
       </c>
-      <c r="AK16" s="71">
+      <c r="AL16" s="71">
         <v>12</v>
       </c>
-      <c r="AL16" s="24" t="s">
+      <c r="AM16" s="24" t="s">
         <v>120</v>
-      </c>
-      <c r="AM16" s="24" t="s">
-        <v>119</v>
       </c>
       <c r="AN16" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="AO16" s="24"/>
+      <c r="AO16" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="AP16" s="24"/>
-      <c r="AQ16" s="24">
+      <c r="AQ16" s="24"/>
+      <c r="AR16" s="24">
         <v>4.0999999999999996</v>
-      </c>
-      <c r="AR16" s="24">
-        <v>2</v>
       </c>
       <c r="AS16" s="24">
         <v>2</v>
       </c>
-      <c r="AT16" s="24" t="b">
-        <v>1</v>
+      <c r="AT16" s="24">
+        <v>2</v>
       </c>
       <c r="AU16" s="24" t="b">
         <v>1</v>
@@ -4596,59 +4630,62 @@
       <c r="AV16" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW16" s="24">
+      <c r="AW16" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX16" s="24">
         <v>23</v>
       </c>
-      <c r="AX16" s="24">
+      <c r="AY16" s="24">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AY16" s="24">
+      <c r="AZ16" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ16" s="69" t="s">
+      <c r="BA16" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="BA16" s="68" t="s">
+      <c r="BB16" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="BB16" s="41">
+      <c r="BC16" s="41">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="BC16" s="40">
+      <c r="BD16" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD16" s="39">
+      <c r="BE16" s="39">
         <v>175</v>
       </c>
-      <c r="BE16" s="109">
+      <c r="BF16" s="109">
         <v>200</v>
       </c>
-      <c r="BF16" s="55">
+      <c r="BG16" s="55">
         <v>2</v>
       </c>
-      <c r="BG16" s="55">
+      <c r="BH16" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH16" s="55">
+      <c r="BI16" s="55">
         <v>1</v>
       </c>
-      <c r="BI16" s="70">
+      <c r="BJ16" s="70">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BJ16" s="70">
+      <c r="BK16" s="70">
         <v>1.75</v>
       </c>
-      <c r="BK16" s="70">
+      <c r="BL16" s="70">
         <v>0</v>
       </c>
-      <c r="BL16" s="70">
+      <c r="BM16" s="70">
         <v>8</v>
       </c>
-      <c r="BM16" s="55" t="s">
+      <c r="BN16" s="55" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -4658,129 +4695,129 @@
       <c r="D17" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F17" s="54">
         <v>1</v>
       </c>
-      <c r="F17" s="53" t="s">
+      <c r="G17" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="28">
+      <c r="H17" s="28">
         <v>2000</v>
       </c>
-      <c r="H17" s="27">
+      <c r="I17" s="27">
         <v>60</v>
       </c>
-      <c r="I17" s="67">
+      <c r="J17" s="67">
         <v>35</v>
       </c>
-      <c r="J17" s="66">
+      <c r="K17" s="66">
         <v>45</v>
       </c>
-      <c r="K17" s="25">
+      <c r="L17" s="25">
         <v>3</v>
       </c>
-      <c r="L17" s="62">
+      <c r="M17" s="62">
         <v>-2</v>
       </c>
-      <c r="M17" s="61">
+      <c r="N17" s="61">
         <v>95</v>
       </c>
-      <c r="N17" s="29">
+      <c r="O17" s="29">
         <v>145</v>
       </c>
-      <c r="O17" s="29">
+      <c r="P17" s="29">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P17" s="29">
+      <c r="Q17" s="29">
         <v>0</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="R17" s="29">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="R17" s="49">
+      <c r="S17" s="49">
         <v>30</v>
       </c>
-      <c r="S17" s="49">
+      <c r="T17" s="49">
         <v>0.5</v>
       </c>
-      <c r="T17" s="46">
+      <c r="U17" s="46">
         <v>0.8</v>
       </c>
-      <c r="U17" s="26">
+      <c r="V17" s="26">
         <v>0.95</v>
       </c>
-      <c r="V17" s="65">
+      <c r="W17" s="65">
         <v>16</v>
       </c>
-      <c r="W17" s="29">
+      <c r="X17" s="29">
         <v>1.75</v>
       </c>
-      <c r="X17" s="29">
+      <c r="Y17" s="29">
         <v>100</v>
       </c>
-      <c r="Y17" s="29">
+      <c r="Z17" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z17" s="29">
+      <c r="AA17" s="29">
         <v>20</v>
       </c>
-      <c r="AA17" s="29">
+      <c r="AB17" s="29">
         <v>10</v>
       </c>
-      <c r="AB17" s="65">
+      <c r="AC17" s="65">
         <v>275</v>
       </c>
-      <c r="AC17" s="49">
+      <c r="AD17" s="49">
         <v>8</v>
       </c>
-      <c r="AD17" s="29">
+      <c r="AE17" s="29">
         <v>3</v>
       </c>
-      <c r="AE17" s="49">
+      <c r="AF17" s="49">
         <v>9</v>
       </c>
-      <c r="AF17" s="29">
+      <c r="AG17" s="29">
         <v>7000</v>
       </c>
-      <c r="AG17" s="64">
+      <c r="AH17" s="64">
         <v>2</v>
       </c>
-      <c r="AH17" s="114">
+      <c r="AI17" s="114">
         <v>0.19</v>
       </c>
-      <c r="AI17" s="64">
+      <c r="AJ17" s="64">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="AJ17" s="71">
+      <c r="AK17" s="71">
         <v>0</v>
       </c>
-      <c r="AK17" s="45">
+      <c r="AL17" s="45">
         <v>12</v>
       </c>
-      <c r="AL17" s="44" t="s">
+      <c r="AM17" s="44" t="s">
         <v>116</v>
-      </c>
-      <c r="AM17" s="24" t="s">
-        <v>115</v>
       </c>
       <c r="AN17" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="AO17" s="24"/>
+      <c r="AO17" s="24" t="s">
+        <v>115</v>
+      </c>
       <c r="AP17" s="24"/>
-      <c r="AQ17" s="24">
+      <c r="AQ17" s="24"/>
+      <c r="AR17" s="24">
         <v>2.2999999999999998</v>
-      </c>
-      <c r="AR17" s="24">
-        <v>2</v>
       </c>
       <c r="AS17" s="24">
         <v>2</v>
       </c>
-      <c r="AT17" s="24" t="b">
-        <v>1</v>
+      <c r="AT17" s="24">
+        <v>2</v>
       </c>
       <c r="AU17" s="24" t="b">
         <v>1</v>
@@ -4788,59 +4825,62 @@
       <c r="AV17" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW17" s="24">
+      <c r="AW17" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX17" s="24">
         <v>23</v>
       </c>
-      <c r="AX17" s="24">
+      <c r="AY17" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY17" s="24">
+      <c r="AZ17" s="24">
         <v>0.8</v>
       </c>
-      <c r="AZ17" s="69" t="s">
+      <c r="BA17" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="BA17" s="68" t="s">
+      <c r="BB17" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="BB17" s="41">
+      <c r="BC17" s="41">
         <v>2.3E-3</v>
       </c>
-      <c r="BC17" s="40">
+      <c r="BD17" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD17" s="39">
+      <c r="BE17" s="39">
         <v>210</v>
       </c>
-      <c r="BE17" s="109">
+      <c r="BF17" s="109">
         <v>235</v>
       </c>
-      <c r="BF17" s="55">
+      <c r="BG17" s="55">
         <v>2.1</v>
       </c>
-      <c r="BG17" s="55">
+      <c r="BH17" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH17" s="55">
+      <c r="BI17" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI17" s="55">
+      <c r="BJ17" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BJ17" s="55">
+      <c r="BK17" s="55">
         <v>2.1</v>
       </c>
-      <c r="BK17" s="55">
+      <c r="BL17" s="55">
         <v>0</v>
       </c>
-      <c r="BL17" s="55">
+      <c r="BM17" s="55">
         <v>8</v>
       </c>
-      <c r="BM17" s="55" t="s">
+      <c r="BN17" s="55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -4850,129 +4890,129 @@
       <c r="D18" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F18" s="54">
         <v>2</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="G18" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="30">
+      <c r="H18" s="30">
         <v>11000</v>
       </c>
-      <c r="H18" s="52">
+      <c r="I18" s="52">
         <v>100</v>
       </c>
-      <c r="I18" s="51">
+      <c r="J18" s="51">
         <v>35</v>
       </c>
-      <c r="J18" s="63">
+      <c r="K18" s="63">
         <v>45</v>
       </c>
-      <c r="K18" s="25">
+      <c r="L18" s="25">
         <v>5</v>
       </c>
-      <c r="L18" s="62">
+      <c r="M18" s="62">
         <v>-2</v>
       </c>
-      <c r="M18" s="61">
+      <c r="N18" s="61">
         <v>140</v>
       </c>
-      <c r="N18" s="26">
+      <c r="O18" s="26">
         <v>200</v>
       </c>
-      <c r="O18" s="26">
+      <c r="P18" s="26">
         <v>1.5</v>
       </c>
-      <c r="P18" s="26">
+      <c r="Q18" s="26">
         <v>0</v>
       </c>
-      <c r="Q18" s="29">
+      <c r="R18" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="R18" s="49">
+      <c r="S18" s="49">
         <v>30</v>
       </c>
-      <c r="S18" s="49">
+      <c r="T18" s="49">
         <v>0.5</v>
       </c>
-      <c r="T18" s="61">
+      <c r="U18" s="61">
         <v>0.85</v>
       </c>
-      <c r="U18" s="29">
+      <c r="V18" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V18" s="48">
+      <c r="W18" s="48">
         <v>23.5</v>
       </c>
-      <c r="W18" s="29">
+      <c r="X18" s="29">
         <v>2.0099999999999998</v>
       </c>
-      <c r="X18" s="29">
+      <c r="Y18" s="29">
         <v>100</v>
       </c>
-      <c r="Y18" s="29">
+      <c r="Z18" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z18" s="29">
+      <c r="AA18" s="29">
         <v>40</v>
       </c>
-      <c r="AA18" s="29">
+      <c r="AB18" s="29">
         <v>14</v>
       </c>
-      <c r="AB18" s="48">
+      <c r="AC18" s="48">
         <v>300</v>
       </c>
-      <c r="AC18" s="49">
+      <c r="AD18" s="49">
         <v>9</v>
       </c>
-      <c r="AD18" s="26">
+      <c r="AE18" s="26">
         <v>3</v>
       </c>
-      <c r="AE18" s="60">
+      <c r="AF18" s="60">
         <v>9</v>
       </c>
-      <c r="AF18" s="29">
+      <c r="AG18" s="29">
         <v>8000</v>
       </c>
-      <c r="AG18" s="59">
+      <c r="AH18" s="59">
         <v>2</v>
       </c>
-      <c r="AH18" s="115">
+      <c r="AI18" s="115">
         <v>0.15</v>
       </c>
-      <c r="AI18" s="64">
+      <c r="AJ18" s="64">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="AJ18" s="117">
+      <c r="AK18" s="117">
         <v>0</v>
       </c>
-      <c r="AK18" s="58">
+      <c r="AL18" s="58">
         <v>12</v>
       </c>
-      <c r="AL18" s="44" t="s">
+      <c r="AM18" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="AM18" s="24" t="s">
+      <c r="AN18" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="AN18" s="24" t="s">
+      <c r="AO18" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AO18" s="24"/>
       <c r="AP18" s="24"/>
-      <c r="AQ18" s="24">
+      <c r="AQ18" s="24"/>
+      <c r="AR18" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AR18" s="24">
-        <v>2</v>
       </c>
       <c r="AS18" s="24">
         <v>2</v>
       </c>
-      <c r="AT18" s="24" t="b">
-        <v>1</v>
+      <c r="AT18" s="24">
+        <v>2</v>
       </c>
       <c r="AU18" s="24" t="b">
         <v>1</v>
@@ -4980,59 +5020,62 @@
       <c r="AV18" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW18" s="24">
+      <c r="AW18" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX18" s="24">
         <v>23</v>
-      </c>
-      <c r="AX18" s="24">
-        <v>0.7</v>
       </c>
       <c r="AY18" s="24">
         <v>0.7</v>
       </c>
-      <c r="AZ18" s="57" t="s">
+      <c r="AZ18" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="BA18" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="BA18" s="56" t="s">
+      <c r="BB18" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="BB18" s="41">
+      <c r="BC18" s="41">
         <v>2E-3</v>
       </c>
-      <c r="BC18" s="40">
+      <c r="BD18" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD18" s="39">
+      <c r="BE18" s="39">
         <v>240</v>
       </c>
-      <c r="BE18" s="109">
+      <c r="BF18" s="109">
         <v>280</v>
       </c>
-      <c r="BF18" s="55">
+      <c r="BG18" s="55">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BG18" s="55">
+      <c r="BH18" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH18" s="55">
+      <c r="BI18" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI18" s="55">
+      <c r="BJ18" s="55">
         <v>0.9</v>
       </c>
-      <c r="BJ18" s="55">
+      <c r="BK18" s="55">
         <v>2.25</v>
       </c>
-      <c r="BK18" s="55">
+      <c r="BL18" s="55">
         <v>0</v>
       </c>
-      <c r="BL18" s="55">
+      <c r="BM18" s="55">
         <v>8</v>
       </c>
-      <c r="BM18" s="37" t="s">
+      <c r="BN18" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -5042,129 +5085,129 @@
       <c r="D19" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F19" s="54">
         <v>3</v>
       </c>
-      <c r="F19" s="54" t="s">
+      <c r="G19" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="28">
+      <c r="H19" s="28">
         <v>35000</v>
       </c>
-      <c r="H19" s="27">
+      <c r="I19" s="27">
         <v>150</v>
       </c>
-      <c r="I19" s="67">
+      <c r="J19" s="67">
         <v>35</v>
       </c>
-      <c r="J19" s="66">
+      <c r="K19" s="66">
         <v>45</v>
       </c>
-      <c r="K19" s="25">
+      <c r="L19" s="25">
         <v>6</v>
       </c>
-      <c r="L19" s="62">
+      <c r="M19" s="62">
         <v>-2</v>
       </c>
-      <c r="M19" s="61">
+      <c r="N19" s="61">
         <v>190</v>
       </c>
-      <c r="N19" s="29">
+      <c r="O19" s="29">
         <v>240</v>
       </c>
-      <c r="O19" s="29">
+      <c r="P19" s="29">
         <v>1.44</v>
       </c>
-      <c r="P19" s="29">
+      <c r="Q19" s="29">
         <v>0</v>
       </c>
-      <c r="Q19" s="29">
+      <c r="R19" s="29">
         <v>0.01</v>
       </c>
-      <c r="R19" s="49">
+      <c r="S19" s="49">
         <v>30</v>
       </c>
-      <c r="S19" s="49">
+      <c r="T19" s="49">
         <v>0.6</v>
       </c>
-      <c r="T19" s="46">
+      <c r="U19" s="46">
         <v>0.9</v>
       </c>
-      <c r="U19" s="26">
+      <c r="V19" s="26">
         <v>1.1499999999999999</v>
       </c>
-      <c r="V19" s="65">
+      <c r="W19" s="65">
         <v>19</v>
       </c>
-      <c r="W19" s="29">
+      <c r="X19" s="29">
         <v>1.3</v>
       </c>
-      <c r="X19" s="29">
+      <c r="Y19" s="29">
         <v>100</v>
       </c>
-      <c r="Y19" s="29">
+      <c r="Z19" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z19" s="29">
+      <c r="AA19" s="29">
         <v>18</v>
       </c>
-      <c r="AA19" s="26">
+      <c r="AB19" s="26">
         <v>22</v>
       </c>
-      <c r="AB19" s="65">
+      <c r="AC19" s="65">
         <v>325</v>
       </c>
-      <c r="AC19" s="49">
+      <c r="AD19" s="49">
         <v>10</v>
       </c>
-      <c r="AD19" s="29">
+      <c r="AE19" s="29">
         <v>4</v>
       </c>
-      <c r="AE19" s="49">
+      <c r="AF19" s="49">
         <v>9</v>
       </c>
-      <c r="AF19" s="29">
+      <c r="AG19" s="29">
         <v>9000</v>
       </c>
-      <c r="AG19" s="64">
+      <c r="AH19" s="64">
         <v>2</v>
       </c>
-      <c r="AH19" s="114">
+      <c r="AI19" s="114">
         <v>0.13</v>
       </c>
-      <c r="AI19" s="64">
+      <c r="AJ19" s="64">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="AJ19" s="71">
+      <c r="AK19" s="71">
         <v>0</v>
       </c>
-      <c r="AK19" s="45">
+      <c r="AL19" s="45">
         <v>12</v>
       </c>
-      <c r="AL19" s="44" t="s">
+      <c r="AM19" s="44" t="s">
         <v>106</v>
-      </c>
-      <c r="AM19" s="24" t="s">
-        <v>105</v>
       </c>
       <c r="AN19" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="AO19" s="24"/>
+      <c r="AO19" s="24" t="s">
+        <v>105</v>
+      </c>
       <c r="AP19" s="24"/>
-      <c r="AQ19" s="24">
+      <c r="AQ19" s="24"/>
+      <c r="AR19" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AR19" s="24">
-        <v>2</v>
       </c>
       <c r="AS19" s="24">
         <v>2</v>
       </c>
-      <c r="AT19" s="24" t="b">
-        <v>1</v>
+      <c r="AT19" s="24">
+        <v>2</v>
       </c>
       <c r="AU19" s="24" t="b">
         <v>1</v>
@@ -5172,59 +5215,62 @@
       <c r="AV19" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW19" s="24">
+      <c r="AW19" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX19" s="24">
         <v>23</v>
-      </c>
-      <c r="AX19" s="24">
-        <v>0.7</v>
       </c>
       <c r="AY19" s="24">
         <v>0.7</v>
       </c>
-      <c r="AZ19" s="57" t="s">
+      <c r="AZ19" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="BA19" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="BA19" s="56" t="s">
+      <c r="BB19" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="BB19" s="41">
+      <c r="BC19" s="41">
         <v>2E-3</v>
       </c>
-      <c r="BC19" s="40">
+      <c r="BD19" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD19" s="39">
+      <c r="BE19" s="39">
         <v>345</v>
       </c>
-      <c r="BE19" s="109">
+      <c r="BF19" s="109">
         <v>365</v>
       </c>
-      <c r="BF19" s="55">
+      <c r="BG19" s="55">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BG19" s="55">
+      <c r="BH19" s="55">
         <v>5</v>
       </c>
-      <c r="BH19" s="55">
+      <c r="BI19" s="55">
         <v>0.5</v>
       </c>
-      <c r="BI19" s="55">
+      <c r="BJ19" s="55">
         <v>1.2</v>
       </c>
-      <c r="BJ19" s="55">
+      <c r="BK19" s="55">
         <v>0.77</v>
       </c>
-      <c r="BK19" s="55">
+      <c r="BL19" s="55">
         <v>0</v>
       </c>
-      <c r="BL19" s="55">
+      <c r="BM19" s="55">
         <v>8</v>
       </c>
-      <c r="BM19" s="37" t="s">
+      <c r="BN19" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5234,129 +5280,129 @@
       <c r="D20" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F20" s="54">
         <v>4</v>
       </c>
-      <c r="F20" s="54" t="s">
+      <c r="G20" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="28">
+      <c r="H20" s="28">
         <v>88000</v>
       </c>
-      <c r="H20" s="27">
+      <c r="I20" s="27">
         <v>200</v>
       </c>
-      <c r="I20" s="67">
+      <c r="J20" s="67">
         <v>35</v>
       </c>
-      <c r="J20" s="66">
+      <c r="K20" s="66">
         <v>45</v>
       </c>
-      <c r="K20" s="25">
+      <c r="L20" s="25">
         <v>8</v>
       </c>
-      <c r="L20" s="62">
+      <c r="M20" s="62">
         <v>0</v>
       </c>
-      <c r="M20" s="61">
+      <c r="N20" s="61">
         <v>210</v>
       </c>
-      <c r="N20" s="29">
+      <c r="O20" s="29">
         <v>270</v>
       </c>
-      <c r="O20" s="29">
+      <c r="P20" s="29">
         <v>1.7</v>
       </c>
-      <c r="P20" s="29">
+      <c r="Q20" s="29">
         <v>0</v>
       </c>
-      <c r="Q20" s="29">
+      <c r="R20" s="29">
         <v>1.2E-2</v>
       </c>
-      <c r="R20" s="49">
+      <c r="S20" s="49">
         <v>30</v>
       </c>
-      <c r="S20" s="49">
+      <c r="T20" s="49">
         <v>0.6</v>
       </c>
-      <c r="T20" s="61">
+      <c r="U20" s="61">
         <v>1</v>
       </c>
-      <c r="U20" s="29">
+      <c r="V20" s="29">
         <v>1.25</v>
       </c>
-      <c r="V20" s="65">
+      <c r="W20" s="65">
         <v>20</v>
       </c>
-      <c r="W20" s="29">
+      <c r="X20" s="29">
         <v>1.4</v>
       </c>
-      <c r="X20" s="29">
+      <c r="Y20" s="29">
         <v>100</v>
       </c>
-      <c r="Y20" s="29">
+      <c r="Z20" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z20" s="29">
+      <c r="AA20" s="29">
         <v>31</v>
       </c>
-      <c r="AA20" s="29">
+      <c r="AB20" s="29">
         <v>34</v>
       </c>
-      <c r="AB20" s="65">
+      <c r="AC20" s="65">
         <v>350</v>
       </c>
-      <c r="AC20" s="49">
+      <c r="AD20" s="49">
         <v>11</v>
       </c>
-      <c r="AD20" s="29">
+      <c r="AE20" s="29">
         <v>4</v>
       </c>
-      <c r="AE20" s="49">
+      <c r="AF20" s="49">
         <v>10</v>
       </c>
-      <c r="AF20" s="29">
+      <c r="AG20" s="29">
         <v>10000</v>
       </c>
-      <c r="AG20" s="64">
+      <c r="AH20" s="64">
         <v>3</v>
       </c>
-      <c r="AH20" s="114">
+      <c r="AI20" s="114">
         <v>0.11</v>
       </c>
-      <c r="AI20" s="64">
+      <c r="AJ20" s="64">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="AJ20" s="71">
+      <c r="AK20" s="71">
         <v>0</v>
       </c>
-      <c r="AK20" s="45">
+      <c r="AL20" s="45">
         <v>12</v>
       </c>
-      <c r="AL20" s="44" t="s">
+      <c r="AM20" s="44" t="s">
         <v>102</v>
-      </c>
-      <c r="AM20" s="24" t="s">
-        <v>101</v>
       </c>
       <c r="AN20" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="AO20" s="24"/>
+      <c r="AO20" s="24" t="s">
+        <v>101</v>
+      </c>
       <c r="AP20" s="24"/>
-      <c r="AQ20" s="24">
+      <c r="AQ20" s="24"/>
+      <c r="AR20" s="24">
         <v>2.1</v>
-      </c>
-      <c r="AR20" s="24">
-        <v>2</v>
       </c>
       <c r="AS20" s="24">
         <v>2</v>
       </c>
-      <c r="AT20" s="24" t="b">
-        <v>1</v>
+      <c r="AT20" s="24">
+        <v>2</v>
       </c>
       <c r="AU20" s="24" t="b">
         <v>1</v>
@@ -5364,59 +5410,62 @@
       <c r="AV20" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW20" s="24">
+      <c r="AW20" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX20" s="24">
         <v>23</v>
       </c>
-      <c r="AX20" s="24">
+      <c r="AY20" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY20" s="24">
+      <c r="AZ20" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ20" s="57" t="s">
+      <c r="BA20" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="BA20" s="56" t="s">
+      <c r="BB20" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="BB20" s="41">
+      <c r="BC20" s="41">
         <v>1.9E-3</v>
       </c>
-      <c r="BC20" s="40">
+      <c r="BD20" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD20" s="39">
+      <c r="BE20" s="39">
         <v>310</v>
       </c>
-      <c r="BE20" s="109">
+      <c r="BF20" s="109">
         <v>335</v>
       </c>
-      <c r="BF20" s="55">
+      <c r="BG20" s="55">
         <v>2.4</v>
       </c>
-      <c r="BG20" s="55">
+      <c r="BH20" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH20" s="55">
+      <c r="BI20" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI20" s="55">
+      <c r="BJ20" s="55">
         <v>1</v>
       </c>
-      <c r="BJ20" s="55">
+      <c r="BK20" s="55">
         <v>1.6</v>
       </c>
-      <c r="BK20" s="55">
+      <c r="BL20" s="55">
         <v>9</v>
       </c>
-      <c r="BL20" s="55">
+      <c r="BM20" s="55">
         <v>8</v>
       </c>
-      <c r="BM20" s="37" t="s">
+      <c r="BN20" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5426,129 +5475,129 @@
       <c r="D21" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F21" s="54">
         <v>5</v>
       </c>
-      <c r="F21" s="54" t="s">
+      <c r="G21" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="28">
+      <c r="H21" s="28">
         <v>260000</v>
       </c>
-      <c r="H21" s="27">
+      <c r="I21" s="27">
         <v>400</v>
       </c>
-      <c r="I21" s="67">
+      <c r="J21" s="67">
         <v>35</v>
       </c>
-      <c r="J21" s="66">
+      <c r="K21" s="66">
         <v>45</v>
       </c>
-      <c r="K21" s="25">
+      <c r="L21" s="25">
         <v>10</v>
       </c>
-      <c r="L21" s="62">
+      <c r="M21" s="62">
         <v>0</v>
       </c>
-      <c r="M21" s="61">
+      <c r="N21" s="61">
         <v>250</v>
       </c>
-      <c r="N21" s="26">
+      <c r="O21" s="26">
         <v>310</v>
       </c>
-      <c r="O21" s="26">
+      <c r="P21" s="26">
         <v>1.9</v>
       </c>
-      <c r="P21" s="26">
+      <c r="Q21" s="26">
         <v>0</v>
       </c>
-      <c r="Q21" s="29">
+      <c r="R21" s="29">
         <v>1.2E-2</v>
       </c>
-      <c r="R21" s="49">
+      <c r="S21" s="49">
         <v>30</v>
       </c>
-      <c r="S21" s="49">
+      <c r="T21" s="49">
         <v>0.6</v>
       </c>
-      <c r="T21" s="61">
+      <c r="U21" s="61">
         <v>1.05</v>
       </c>
-      <c r="U21" s="29">
+      <c r="V21" s="29">
         <v>1.3</v>
       </c>
-      <c r="V21" s="65">
+      <c r="W21" s="65">
         <v>21</v>
       </c>
-      <c r="W21" s="29">
+      <c r="X21" s="29">
         <v>2.0099999999999998</v>
       </c>
-      <c r="X21" s="29">
+      <c r="Y21" s="29">
         <v>100</v>
       </c>
-      <c r="Y21" s="29">
+      <c r="Z21" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z21" s="29">
+      <c r="AA21" s="29">
         <v>50</v>
       </c>
-      <c r="AA21" s="29">
+      <c r="AB21" s="29">
         <v>14</v>
       </c>
-      <c r="AB21" s="65">
+      <c r="AC21" s="65">
         <v>375</v>
       </c>
-      <c r="AC21" s="49">
+      <c r="AD21" s="49">
         <v>11</v>
       </c>
-      <c r="AD21" s="29">
+      <c r="AE21" s="29">
         <v>4</v>
       </c>
-      <c r="AE21" s="49">
+      <c r="AF21" s="49">
         <v>10</v>
       </c>
-      <c r="AF21" s="29">
+      <c r="AG21" s="29">
         <v>10000</v>
       </c>
-      <c r="AG21" s="64">
+      <c r="AH21" s="64">
         <v>3</v>
       </c>
-      <c r="AH21" s="114">
+      <c r="AI21" s="114">
         <v>0.09</v>
       </c>
-      <c r="AI21" s="64">
+      <c r="AJ21" s="64">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="AJ21" s="71">
+      <c r="AK21" s="71">
         <v>0</v>
       </c>
-      <c r="AK21" s="45">
+      <c r="AL21" s="45">
         <v>12</v>
       </c>
-      <c r="AL21" s="44" t="s">
+      <c r="AM21" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="AM21" s="24" t="s">
+      <c r="AN21" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AN21" s="24" t="s">
+      <c r="AO21" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AO21" s="24"/>
       <c r="AP21" s="24"/>
-      <c r="AQ21" s="24">
-        <v>2</v>
-      </c>
+      <c r="AQ21" s="24"/>
       <c r="AR21" s="24">
         <v>2</v>
       </c>
       <c r="AS21" s="24">
         <v>2</v>
       </c>
-      <c r="AT21" s="24" t="b">
-        <v>1</v>
+      <c r="AT21" s="24">
+        <v>2</v>
       </c>
       <c r="AU21" s="24" t="b">
         <v>1</v>
@@ -5556,59 +5605,62 @@
       <c r="AV21" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW21" s="24">
+      <c r="AW21" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX21" s="24">
         <v>23</v>
       </c>
-      <c r="AX21" s="24">
+      <c r="AY21" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY21" s="24">
+      <c r="AZ21" s="24">
         <v>0.5</v>
       </c>
-      <c r="AZ21" s="57" t="s">
+      <c r="BA21" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="BA21" s="56" t="s">
+      <c r="BB21" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="BB21" s="41">
+      <c r="BC21" s="41">
         <v>1.8E-3</v>
       </c>
-      <c r="BC21" s="40">
+      <c r="BD21" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD21" s="39">
+      <c r="BE21" s="39">
         <v>322</v>
       </c>
-      <c r="BE21" s="109">
+      <c r="BF21" s="109">
         <v>347</v>
       </c>
-      <c r="BF21" s="55">
+      <c r="BG21" s="55">
         <v>2.5</v>
       </c>
-      <c r="BG21" s="55">
+      <c r="BH21" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH21" s="55">
+      <c r="BI21" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI21" s="55">
+      <c r="BJ21" s="55">
         <v>0.5</v>
       </c>
-      <c r="BJ21" s="55">
+      <c r="BK21" s="55">
         <v>1.7</v>
       </c>
-      <c r="BK21" s="55">
+      <c r="BL21" s="55">
         <v>9</v>
       </c>
-      <c r="BL21" s="55">
+      <c r="BM21" s="55">
         <v>8</v>
       </c>
-      <c r="BM21" s="37" t="s">
+      <c r="BN21" s="37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -5618,129 +5670,129 @@
       <c r="D22" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F22" s="54">
         <v>6</v>
       </c>
-      <c r="F22" s="53" t="s">
+      <c r="G22" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="28">
+      <c r="H22" s="28">
         <v>500000</v>
       </c>
-      <c r="H22" s="27">
+      <c r="I22" s="27">
         <v>550</v>
       </c>
-      <c r="I22" s="67">
+      <c r="J22" s="67">
         <v>35</v>
       </c>
-      <c r="J22" s="66">
+      <c r="K22" s="66">
         <v>45</v>
       </c>
-      <c r="K22" s="25">
+      <c r="L22" s="25">
         <v>12.5</v>
       </c>
-      <c r="L22" s="62">
+      <c r="M22" s="62">
         <v>0</v>
       </c>
-      <c r="M22" s="61">
+      <c r="N22" s="61">
         <v>290</v>
       </c>
-      <c r="N22" s="29">
+      <c r="O22" s="29">
         <v>350</v>
       </c>
-      <c r="O22" s="29">
+      <c r="P22" s="29">
         <v>2.1</v>
       </c>
-      <c r="P22" s="29">
+      <c r="Q22" s="29">
         <v>0</v>
       </c>
-      <c r="Q22" s="29">
+      <c r="R22" s="29">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="R22" s="49">
+      <c r="S22" s="49">
         <v>25</v>
       </c>
-      <c r="S22" s="49">
+      <c r="T22" s="49">
         <v>0.6</v>
       </c>
-      <c r="T22" s="61">
+      <c r="U22" s="61">
         <v>1.35</v>
       </c>
-      <c r="U22" s="29">
+      <c r="V22" s="29">
         <v>1.55</v>
       </c>
-      <c r="V22" s="65">
+      <c r="W22" s="65">
         <v>23.5</v>
       </c>
-      <c r="W22" s="29">
+      <c r="X22" s="29">
         <v>1.5</v>
       </c>
-      <c r="X22" s="29">
+      <c r="Y22" s="29">
         <v>100</v>
       </c>
-      <c r="Y22" s="29">
+      <c r="Z22" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z22" s="29">
+      <c r="AA22" s="29">
         <v>29</v>
       </c>
-      <c r="AA22" s="29">
+      <c r="AB22" s="29">
         <v>17</v>
       </c>
-      <c r="AB22" s="65">
+      <c r="AC22" s="65">
         <v>400</v>
       </c>
-      <c r="AC22" s="49">
+      <c r="AD22" s="49">
         <v>11</v>
       </c>
-      <c r="AD22" s="29">
+      <c r="AE22" s="29">
         <v>5</v>
       </c>
-      <c r="AE22" s="49">
+      <c r="AF22" s="49">
         <v>10</v>
       </c>
-      <c r="AF22" s="29">
+      <c r="AG22" s="29">
         <v>10000</v>
       </c>
-      <c r="AG22" s="64">
+      <c r="AH22" s="64">
         <v>3</v>
       </c>
-      <c r="AH22" s="114">
+      <c r="AI22" s="114">
         <v>0.08</v>
       </c>
-      <c r="AI22" s="64">
+      <c r="AJ22" s="64">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ22" s="71">
+      <c r="AK22" s="71">
         <v>0</v>
       </c>
-      <c r="AK22" s="45">
+      <c r="AL22" s="45">
         <v>12</v>
       </c>
-      <c r="AL22" s="44" t="s">
+      <c r="AM22" s="44" t="s">
         <v>92</v>
-      </c>
-      <c r="AM22" s="24" t="s">
-        <v>91</v>
       </c>
       <c r="AN22" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="AO22" s="24"/>
+      <c r="AO22" s="24" t="s">
+        <v>91</v>
+      </c>
       <c r="AP22" s="24"/>
-      <c r="AQ22" s="24">
+      <c r="AQ22" s="24"/>
+      <c r="AR22" s="24">
         <v>1.6</v>
-      </c>
-      <c r="AR22" s="24">
-        <v>2</v>
       </c>
       <c r="AS22" s="24">
         <v>2</v>
       </c>
-      <c r="AT22" s="24" t="b">
-        <v>1</v>
+      <c r="AT22" s="24">
+        <v>2</v>
       </c>
       <c r="AU22" s="24" t="b">
         <v>1</v>
@@ -5748,59 +5800,62 @@
       <c r="AV22" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW22" s="24">
+      <c r="AW22" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX22" s="24">
         <v>23</v>
       </c>
-      <c r="AX22" s="24">
+      <c r="AY22" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY22" s="24">
+      <c r="AZ22" s="24">
         <v>0.5</v>
       </c>
-      <c r="AZ22" s="57" t="s">
+      <c r="BA22" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="BA22" s="56" t="s">
+      <c r="BB22" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="BB22" s="41">
+      <c r="BC22" s="41">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="BC22" s="40">
+      <c r="BD22" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD22" s="39">
+      <c r="BE22" s="39">
         <v>343</v>
       </c>
-      <c r="BE22" s="109">
+      <c r="BF22" s="109">
         <v>372</v>
       </c>
-      <c r="BF22" s="55">
+      <c r="BG22" s="55">
         <v>2.6</v>
       </c>
-      <c r="BG22" s="55">
+      <c r="BH22" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH22" s="55">
+      <c r="BI22" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI22" s="55">
+      <c r="BJ22" s="55">
         <v>0.5</v>
       </c>
-      <c r="BJ22" s="55">
+      <c r="BK22" s="55">
         <v>0.9</v>
       </c>
-      <c r="BK22" s="55">
+      <c r="BL22" s="55">
         <v>9</v>
       </c>
-      <c r="BL22" s="55">
+      <c r="BM22" s="55">
         <v>8</v>
       </c>
-      <c r="BM22" s="37" t="s">
+      <c r="BN22" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -5810,133 +5865,133 @@
       <c r="D23" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="54">
+      <c r="E23" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="54">
         <v>7</v>
       </c>
-      <c r="F23" s="53" t="s">
+      <c r="G23" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="30">
+      <c r="H23" s="30">
         <v>870000</v>
       </c>
-      <c r="H23" s="52">
+      <c r="I23" s="52">
         <v>800</v>
       </c>
-      <c r="I23" s="51">
+      <c r="J23" s="51">
         <v>35</v>
       </c>
-      <c r="J23" s="63">
+      <c r="K23" s="63">
         <v>45</v>
       </c>
-      <c r="K23" s="25">
+      <c r="L23" s="25">
         <v>17</v>
       </c>
-      <c r="L23" s="62">
+      <c r="M23" s="62">
         <v>0</v>
       </c>
-      <c r="M23" s="61">
+      <c r="N23" s="61">
         <v>330</v>
       </c>
-      <c r="N23" s="29">
+      <c r="O23" s="29">
         <v>400</v>
       </c>
-      <c r="O23" s="29">
+      <c r="P23" s="29">
         <v>2.2999999999999998</v>
       </c>
-      <c r="P23" s="29">
+      <c r="Q23" s="29">
         <v>0</v>
       </c>
-      <c r="Q23" s="29">
+      <c r="R23" s="29">
         <v>1.4E-2</v>
       </c>
-      <c r="R23" s="49">
+      <c r="S23" s="49">
         <v>25</v>
       </c>
-      <c r="S23" s="49">
+      <c r="T23" s="49">
         <v>0.7</v>
       </c>
-      <c r="T23" s="61">
+      <c r="U23" s="61">
         <v>1.54</v>
       </c>
-      <c r="U23" s="29">
+      <c r="V23" s="29">
         <v>1.74</v>
       </c>
-      <c r="V23" s="48">
+      <c r="W23" s="48">
         <v>25</v>
       </c>
-      <c r="W23" s="29">
+      <c r="X23" s="29">
         <v>1.4</v>
       </c>
-      <c r="X23" s="29">
+      <c r="Y23" s="29">
         <v>100</v>
       </c>
-      <c r="Y23" s="29">
+      <c r="Z23" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z23" s="29">
+      <c r="AA23" s="29">
         <v>20</v>
       </c>
-      <c r="AA23" s="29">
+      <c r="AB23" s="29">
         <v>18</v>
       </c>
-      <c r="AB23" s="48">
+      <c r="AC23" s="48">
         <v>425</v>
       </c>
-      <c r="AC23" s="49">
+      <c r="AD23" s="49">
         <v>11.5</v>
       </c>
-      <c r="AD23" s="26">
+      <c r="AE23" s="26">
         <v>5</v>
       </c>
-      <c r="AE23" s="60">
+      <c r="AF23" s="60">
         <v>10</v>
       </c>
-      <c r="AF23" s="29">
+      <c r="AG23" s="29">
         <v>20000</v>
       </c>
-      <c r="AG23" s="59">
+      <c r="AH23" s="59">
         <v>4</v>
       </c>
-      <c r="AH23" s="115">
+      <c r="AI23" s="115">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI23" s="64">
+      <c r="AJ23" s="64">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="AJ23" s="117">
+      <c r="AK23" s="117">
         <v>0</v>
       </c>
-      <c r="AK23" s="58">
+      <c r="AL23" s="58">
         <v>12</v>
       </c>
-      <c r="AL23" s="44" t="s">
+      <c r="AM23" s="44" t="s">
         <v>88</v>
-      </c>
-      <c r="AM23" s="24" t="s">
-        <v>87</v>
       </c>
       <c r="AN23" s="24" t="s">
         <v>87</v>
       </c>
       <c r="AO23" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP23" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AP23" s="24" t="s">
+      <c r="AQ23" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AQ23" s="24">
+      <c r="AR23" s="24">
         <v>1.4</v>
-      </c>
-      <c r="AR23" s="24">
-        <v>2</v>
       </c>
       <c r="AS23" s="24">
         <v>2</v>
       </c>
-      <c r="AT23" s="24" t="b">
-        <v>1</v>
+      <c r="AT23" s="24">
+        <v>2</v>
       </c>
       <c r="AU23" s="24" t="b">
         <v>1</v>
@@ -5944,59 +5999,62 @@
       <c r="AV23" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW23" s="24">
+      <c r="AW23" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX23" s="24">
         <v>23</v>
       </c>
-      <c r="AX23" s="24">
+      <c r="AY23" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY23" s="24">
+      <c r="AZ23" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ23" s="57" t="s">
+      <c r="BA23" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="BA23" s="56" t="s">
+      <c r="BB23" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="BB23" s="41">
+      <c r="BC23" s="41">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BC23" s="40">
+      <c r="BD23" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD23" s="39">
+      <c r="BE23" s="39">
         <v>435</v>
       </c>
-      <c r="BE23" s="109">
+      <c r="BF23" s="109">
         <v>465</v>
       </c>
-      <c r="BF23" s="55">
+      <c r="BG23" s="55">
         <v>3.2</v>
       </c>
-      <c r="BG23" s="55">
+      <c r="BH23" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH23" s="55">
+      <c r="BI23" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI23" s="55">
+      <c r="BJ23" s="55">
         <v>0.5</v>
       </c>
-      <c r="BJ23" s="55">
+      <c r="BK23" s="55">
         <v>1.2</v>
       </c>
-      <c r="BK23" s="55">
+      <c r="BL23" s="55">
         <v>45</v>
       </c>
-      <c r="BL23" s="55">
+      <c r="BM23" s="55">
         <v>15</v>
       </c>
-      <c r="BM23" s="37" t="s">
+      <c r="BN23" s="37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
@@ -6006,132 +6064,132 @@
       <c r="D24" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="94">
+      <c r="E24" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="94">
         <v>8</v>
       </c>
-      <c r="F24" s="98" t="s">
+      <c r="G24" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="107">
+      <c r="H24" s="107">
         <v>1400000</v>
       </c>
-      <c r="H24" s="22">
+      <c r="I24" s="22">
         <v>800</v>
       </c>
-      <c r="I24" s="51">
+      <c r="J24" s="51">
         <v>35</v>
       </c>
-      <c r="J24" s="63">
+      <c r="K24" s="63">
         <v>45</v>
       </c>
-      <c r="K24" s="101">
+      <c r="L24" s="101">
         <v>25</v>
       </c>
-      <c r="L24" s="102">
+      <c r="M24" s="102">
         <v>0</v>
       </c>
-      <c r="M24" s="45">
+      <c r="N24" s="45">
         <v>360</v>
       </c>
-      <c r="N24" s="49">
+      <c r="O24" s="49">
         <v>430</v>
       </c>
-      <c r="O24" s="49">
+      <c r="P24" s="49">
         <v>2.2999999999999998</v>
       </c>
-      <c r="P24" s="49">
+      <c r="Q24" s="49">
         <v>0</v>
       </c>
-      <c r="Q24" s="49">
+      <c r="R24" s="49">
         <v>1.4E-2</v>
       </c>
-      <c r="R24" s="49">
+      <c r="S24" s="49">
         <v>25</v>
       </c>
-      <c r="S24" s="49">
+      <c r="T24" s="49">
         <v>0.7</v>
       </c>
-      <c r="T24" s="45">
+      <c r="U24" s="45">
         <v>1.7</v>
       </c>
-      <c r="U24" s="49">
+      <c r="V24" s="49">
         <v>1.95</v>
       </c>
-      <c r="V24" s="48">
+      <c r="W24" s="48">
         <v>25</v>
       </c>
-      <c r="W24" s="49">
+      <c r="X24" s="49">
         <v>1.8</v>
       </c>
-      <c r="X24" s="49">
+      <c r="Y24" s="49">
         <v>100</v>
       </c>
-      <c r="Y24" s="49">
+      <c r="Z24" s="49">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z24" s="49">
+      <c r="AA24" s="49">
         <v>40</v>
       </c>
-      <c r="AA24" s="49">
+      <c r="AB24" s="49">
         <v>14</v>
       </c>
-      <c r="AB24" s="48">
+      <c r="AC24" s="48">
         <v>425</v>
       </c>
-      <c r="AC24" s="49">
+      <c r="AD24" s="49">
         <v>11.5</v>
       </c>
-      <c r="AD24" s="47">
+      <c r="AE24" s="47">
         <v>5</v>
       </c>
-      <c r="AE24" s="60">
+      <c r="AF24" s="60">
         <v>10</v>
       </c>
-      <c r="AF24" s="49">
+      <c r="AG24" s="49">
         <v>20000</v>
       </c>
-      <c r="AG24" s="106">
+      <c r="AH24" s="106">
         <v>4</v>
       </c>
-      <c r="AH24" s="116">
+      <c r="AI24" s="116">
         <v>0.06</v>
       </c>
-      <c r="AI24" s="112">
+      <c r="AJ24" s="112">
         <v>0.05</v>
       </c>
-      <c r="AJ24" s="117">
+      <c r="AK24" s="117">
         <v>0</v>
       </c>
-      <c r="AK24" s="58">
+      <c r="AL24" s="58">
         <v>12</v>
       </c>
-      <c r="AL24" s="96" t="s">
+      <c r="AM24" s="96" t="s">
         <v>185</v>
-      </c>
-      <c r="AM24" s="95" t="s">
-        <v>186</v>
       </c>
       <c r="AN24" s="95" t="s">
         <v>186</v>
       </c>
       <c r="AO24" s="95" t="s">
+        <v>186</v>
+      </c>
+      <c r="AP24" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="AP24" s="95" t="s">
+      <c r="AQ24" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="AQ24" s="95">
+      <c r="AR24" s="95">
         <v>1.3</v>
-      </c>
-      <c r="AR24" s="95">
-        <v>2</v>
       </c>
       <c r="AS24" s="95">
         <v>2</v>
       </c>
-      <c r="AT24" s="95" t="b">
-        <v>1</v>
+      <c r="AT24" s="95">
+        <v>2</v>
       </c>
       <c r="AU24" s="95" t="b">
         <v>1</v>
@@ -6139,59 +6197,62 @@
       <c r="AV24" s="95" t="b">
         <v>1</v>
       </c>
-      <c r="AW24" s="95">
+      <c r="AW24" s="95" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX24" s="95">
         <v>23</v>
       </c>
-      <c r="AX24" s="95">
+      <c r="AY24" s="95">
         <v>0.7</v>
       </c>
-      <c r="AY24" s="95">
+      <c r="AZ24" s="95">
         <v>0.6</v>
       </c>
-      <c r="AZ24" s="99" t="s">
+      <c r="BA24" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="BA24" s="21" t="s">
+      <c r="BB24" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BB24" s="103">
+      <c r="BC24" s="103">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BC24" s="104">
+      <c r="BD24" s="104">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD24" s="105">
+      <c r="BE24" s="105">
         <v>450</v>
       </c>
-      <c r="BE24" s="110">
+      <c r="BF24" s="110">
         <v>505</v>
       </c>
-      <c r="BF24" s="100">
+      <c r="BG24" s="100">
         <v>3.4</v>
       </c>
-      <c r="BG24" s="100">
+      <c r="BH24" s="100">
         <v>9.5</v>
       </c>
-      <c r="BH24" s="100">
+      <c r="BI24" s="100">
         <v>1.7</v>
       </c>
-      <c r="BI24" s="100">
+      <c r="BJ24" s="100">
         <v>0.6</v>
       </c>
-      <c r="BJ24" s="100">
+      <c r="BK24" s="100">
         <v>1</v>
       </c>
-      <c r="BK24" s="100">
+      <c r="BL24" s="100">
         <v>45</v>
       </c>
-      <c r="BL24" s="100">
+      <c r="BM24" s="100">
         <v>15</v>
       </c>
-      <c r="BM24" s="97" t="s">
+      <c r="BN24" s="97" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -6201,133 +6262,133 @@
       <c r="D25" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F25" s="54">
         <v>9</v>
       </c>
-      <c r="F25" s="53" t="s">
+      <c r="G25" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="G25" s="30">
+      <c r="H25" s="30">
         <v>2200000</v>
       </c>
-      <c r="H25" s="52">
+      <c r="I25" s="52">
         <v>800</v>
       </c>
-      <c r="I25" s="51">
+      <c r="J25" s="51">
         <v>35</v>
       </c>
-      <c r="J25" s="63">
+      <c r="K25" s="63">
         <v>45</v>
       </c>
-      <c r="K25" s="25">
+      <c r="L25" s="25">
         <v>10</v>
       </c>
-      <c r="L25" s="62">
+      <c r="M25" s="62">
         <v>0</v>
       </c>
-      <c r="M25" s="61">
+      <c r="N25" s="61">
         <v>375</v>
       </c>
-      <c r="N25" s="26">
+      <c r="O25" s="26">
         <v>445</v>
       </c>
-      <c r="O25" s="26">
+      <c r="P25" s="26">
         <v>2.2999999999999998</v>
       </c>
-      <c r="P25" s="26">
+      <c r="Q25" s="26">
         <v>0</v>
       </c>
-      <c r="Q25" s="29">
+      <c r="R25" s="29">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="R25" s="49">
+      <c r="S25" s="49">
         <v>25</v>
       </c>
-      <c r="S25" s="49">
+      <c r="T25" s="49">
         <v>0.7</v>
       </c>
-      <c r="T25" s="46">
+      <c r="U25" s="46">
         <v>1.37</v>
       </c>
-      <c r="U25" s="26">
+      <c r="V25" s="26">
         <v>1.57</v>
       </c>
-      <c r="V25" s="48">
+      <c r="W25" s="48">
         <v>28</v>
       </c>
-      <c r="W25" s="29">
+      <c r="X25" s="29">
         <v>1.6</v>
       </c>
-      <c r="X25" s="29">
+      <c r="Y25" s="29">
         <v>100</v>
       </c>
-      <c r="Y25" s="29">
+      <c r="Z25" s="29">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z25" s="29">
+      <c r="AA25" s="29">
         <v>50</v>
       </c>
-      <c r="AA25" s="26">
+      <c r="AB25" s="26">
         <v>34</v>
       </c>
-      <c r="AB25" s="48">
+      <c r="AC25" s="48">
         <v>450</v>
       </c>
-      <c r="AC25" s="49">
+      <c r="AD25" s="49">
         <v>11.5</v>
       </c>
-      <c r="AD25" s="26">
+      <c r="AE25" s="26">
         <v>6</v>
       </c>
-      <c r="AE25" s="60">
+      <c r="AF25" s="60">
         <v>10</v>
       </c>
-      <c r="AF25" s="29">
+      <c r="AG25" s="29">
         <v>20000</v>
       </c>
-      <c r="AG25" s="59">
+      <c r="AH25" s="59">
         <v>4</v>
       </c>
-      <c r="AH25" s="115">
+      <c r="AI25" s="115">
         <v>0.06</v>
       </c>
-      <c r="AI25" s="64">
-        <f>AH26</f>
+      <c r="AJ25" s="64">
+        <f>AI26</f>
         <v>0.05</v>
       </c>
-      <c r="AJ25" s="117">
+      <c r="AK25" s="117">
         <v>0</v>
       </c>
-      <c r="AK25" s="58">
+      <c r="AL25" s="58">
         <v>12</v>
       </c>
-      <c r="AL25" s="44" t="s">
+      <c r="AM25" s="44" t="s">
         <v>83</v>
-      </c>
-      <c r="AM25" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="AN25" s="24" t="s">
         <v>82</v>
       </c>
       <c r="AO25" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP25" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AP25" s="24" t="s">
+      <c r="AQ25" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="AQ25" s="24">
+      <c r="AR25" s="24">
         <v>1.2</v>
-      </c>
-      <c r="AR25" s="24">
-        <v>2</v>
       </c>
       <c r="AS25" s="24">
         <v>2</v>
       </c>
-      <c r="AT25" s="24" t="b">
-        <v>1</v>
+      <c r="AT25" s="24">
+        <v>2</v>
       </c>
       <c r="AU25" s="24" t="b">
         <v>1</v>
@@ -6335,59 +6396,62 @@
       <c r="AV25" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW25" s="24">
+      <c r="AW25" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX25" s="24">
         <v>23</v>
       </c>
-      <c r="AX25" s="24">
+      <c r="AY25" s="24">
         <v>0.7</v>
       </c>
-      <c r="AY25" s="24">
+      <c r="AZ25" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ25" s="57" t="s">
+      <c r="BA25" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="BA25" s="56" t="s">
+      <c r="BB25" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="BB25" s="41">
+      <c r="BC25" s="41">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BC25" s="40">
+      <c r="BD25" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD25" s="39">
+      <c r="BE25" s="39">
         <v>540</v>
       </c>
-      <c r="BE25" s="109">
+      <c r="BF25" s="109">
         <v>590</v>
       </c>
-      <c r="BF25" s="55">
+      <c r="BG25" s="55">
         <v>3.9</v>
       </c>
-      <c r="BG25" s="55">
+      <c r="BH25" s="55">
         <v>9.5</v>
       </c>
-      <c r="BH25" s="55">
+      <c r="BI25" s="55">
         <v>1.7</v>
       </c>
-      <c r="BI25" s="55">
+      <c r="BJ25" s="55">
         <v>0.3</v>
       </c>
-      <c r="BJ25" s="55">
+      <c r="BK25" s="55">
         <v>0.4</v>
       </c>
-      <c r="BK25" s="55">
+      <c r="BL25" s="55">
         <v>45</v>
       </c>
-      <c r="BL25" s="55">
+      <c r="BM25" s="55">
         <v>15</v>
       </c>
-      <c r="BM25" s="37" t="s">
+      <c r="BN25" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:65" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6397,132 +6461,132 @@
       <c r="D26" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="54">
+      <c r="E26" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F26" s="54">
         <v>10</v>
       </c>
-      <c r="F26" s="53" t="s">
+      <c r="G26" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="30">
+      <c r="H26" s="30">
         <v>3300000</v>
       </c>
-      <c r="H26" s="52">
+      <c r="I26" s="52">
         <v>1100</v>
       </c>
-      <c r="I26" s="51">
+      <c r="J26" s="51">
         <v>35</v>
       </c>
-      <c r="J26" s="66">
+      <c r="K26" s="66">
         <v>45</v>
       </c>
-      <c r="K26" s="25">
+      <c r="L26" s="25">
         <v>25</v>
       </c>
-      <c r="L26" s="50">
+      <c r="M26" s="50">
         <v>0</v>
       </c>
-      <c r="M26" s="25">
+      <c r="N26" s="25">
         <v>425</v>
       </c>
-      <c r="N26" s="26">
+      <c r="O26" s="26">
         <v>500</v>
       </c>
-      <c r="O26" s="26">
+      <c r="P26" s="26">
         <v>2.4</v>
       </c>
-      <c r="P26" s="26">
+      <c r="Q26" s="26">
         <v>0</v>
       </c>
-      <c r="Q26" s="29">
+      <c r="R26" s="29">
         <v>1.6E-2</v>
       </c>
-      <c r="R26" s="49">
+      <c r="S26" s="49">
         <v>20</v>
       </c>
-      <c r="S26" s="49">
+      <c r="T26" s="49">
         <v>0.8</v>
       </c>
-      <c r="T26" s="46">
+      <c r="U26" s="46">
         <v>2</v>
       </c>
-      <c r="U26" s="26">
+      <c r="V26" s="26">
         <v>2.1</v>
       </c>
-      <c r="V26" s="48">
+      <c r="W26" s="48">
         <v>31</v>
       </c>
-      <c r="W26" s="26">
+      <c r="X26" s="26">
         <v>1.9</v>
       </c>
-      <c r="X26" s="26">
+      <c r="Y26" s="26">
         <v>100</v>
       </c>
-      <c r="Y26" s="26">
+      <c r="Z26" s="26">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z26" s="26">
+      <c r="AA26" s="26">
         <v>19</v>
       </c>
-      <c r="AA26" s="26">
+      <c r="AB26" s="26">
         <v>12</v>
       </c>
-      <c r="AB26" s="48">
+      <c r="AC26" s="48">
         <v>475</v>
       </c>
-      <c r="AC26" s="47">
+      <c r="AD26" s="47">
         <v>12</v>
       </c>
-      <c r="AD26" s="26">
+      <c r="AE26" s="26">
         <v>6</v>
       </c>
-      <c r="AE26" s="47">
+      <c r="AF26" s="47">
         <v>10</v>
       </c>
-      <c r="AF26" s="26">
+      <c r="AG26" s="26">
         <v>30000</v>
       </c>
-      <c r="AG26" s="25">
+      <c r="AH26" s="25">
         <v>5</v>
       </c>
-      <c r="AH26" s="50">
+      <c r="AI26" s="50">
         <v>0.05</v>
       </c>
-      <c r="AI26" s="64">
+      <c r="AJ26" s="64">
         <v>0.04</v>
       </c>
-      <c r="AJ26" s="71">
+      <c r="AK26" s="71">
         <v>0</v>
       </c>
-      <c r="AK26" s="45">
+      <c r="AL26" s="45">
         <v>12</v>
       </c>
-      <c r="AL26" s="44" t="s">
+      <c r="AM26" s="44" t="s">
         <v>78</v>
-      </c>
-      <c r="AM26" s="24" t="s">
-        <v>77</v>
       </c>
       <c r="AN26" s="24" t="s">
         <v>77</v>
       </c>
       <c r="AO26" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP26" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AP26" s="24" t="s">
+      <c r="AQ26" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AQ26" s="24">
+      <c r="AR26" s="24">
         <v>1.1000000000000001</v>
-      </c>
-      <c r="AR26" s="24">
-        <v>2</v>
       </c>
       <c r="AS26" s="24">
         <v>2</v>
       </c>
-      <c r="AT26" s="24" t="b">
-        <v>1</v>
+      <c r="AT26" s="24">
+        <v>2</v>
       </c>
       <c r="AU26" s="24" t="b">
         <v>1</v>
@@ -6530,59 +6594,62 @@
       <c r="AV26" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW26" s="24">
+      <c r="AW26" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX26" s="24">
         <v>23</v>
       </c>
-      <c r="AX26" s="24">
+      <c r="AY26" s="24">
         <v>0.75</v>
       </c>
-      <c r="AY26" s="24">
+      <c r="AZ26" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ26" s="43" t="s">
+      <c r="BA26" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="BA26" s="42" t="s">
+      <c r="BB26" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="BB26" s="41">
+      <c r="BC26" s="41">
         <v>1.5E-3</v>
       </c>
-      <c r="BC26" s="40">
+      <c r="BD26" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD26" s="39">
+      <c r="BE26" s="39">
         <v>680</v>
       </c>
-      <c r="BE26" s="111">
+      <c r="BF26" s="111">
         <v>730</v>
       </c>
-      <c r="BF26" s="38">
+      <c r="BG26" s="38">
         <v>4.7</v>
       </c>
-      <c r="BG26" s="38">
+      <c r="BH26" s="38">
         <v>9.5</v>
       </c>
-      <c r="BH26" s="38">
+      <c r="BI26" s="38">
         <v>1.7</v>
       </c>
-      <c r="BI26" s="38">
+      <c r="BJ26" s="38">
         <v>0.7</v>
       </c>
-      <c r="BJ26" s="38">
+      <c r="BK26" s="38">
         <v>1.03</v>
       </c>
-      <c r="BK26" s="38">
+      <c r="BL26" s="38">
         <v>59</v>
       </c>
-      <c r="BL26" s="38">
+      <c r="BM26" s="38">
         <v>15</v>
       </c>
-      <c r="BM26" s="37" t="s">
+      <c r="BN26" s="37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="31" t="s">
         <v>3</v>
       </c>
@@ -6592,132 +6659,132 @@
       <c r="D27" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E27" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="54">
         <v>11</v>
       </c>
-      <c r="F27" s="53" t="s">
+      <c r="G27" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="30">
+      <c r="H27" s="30">
         <v>4800000</v>
       </c>
-      <c r="H27" s="52">
+      <c r="I27" s="52">
         <v>1100</v>
       </c>
-      <c r="I27" s="51">
+      <c r="J27" s="51">
         <v>35</v>
       </c>
-      <c r="J27" s="130">
+      <c r="K27" s="118">
         <v>45</v>
       </c>
-      <c r="K27" s="25">
+      <c r="L27" s="25">
         <v>25</v>
       </c>
-      <c r="L27" s="50">
+      <c r="M27" s="50">
         <v>0</v>
       </c>
-      <c r="M27" s="131">
+      <c r="N27" s="119">
         <v>1000</v>
       </c>
-      <c r="N27" s="26">
+      <c r="O27" s="26">
         <v>1500</v>
       </c>
-      <c r="O27" s="26">
+      <c r="P27" s="26">
         <v>2.6</v>
       </c>
-      <c r="P27" s="26">
+      <c r="Q27" s="26">
         <v>0</v>
       </c>
-      <c r="Q27" s="29">
+      <c r="R27" s="29">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="R27" s="49">
+      <c r="S27" s="49">
         <v>20</v>
       </c>
-      <c r="S27" s="49">
+      <c r="T27" s="49">
         <v>0.8</v>
       </c>
-      <c r="T27" s="46">
+      <c r="U27" s="46">
         <v>2</v>
       </c>
-      <c r="U27" s="26">
+      <c r="V27" s="26">
         <v>2.1</v>
       </c>
-      <c r="V27" s="48">
+      <c r="W27" s="48">
         <v>31</v>
       </c>
-      <c r="W27" s="26">
+      <c r="X27" s="26">
         <v>1.9</v>
       </c>
-      <c r="X27" s="26">
+      <c r="Y27" s="26">
         <v>100</v>
       </c>
-      <c r="Y27" s="26">
+      <c r="Z27" s="26">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="Z27" s="26">
-        <v>19</v>
-      </c>
       <c r="AA27" s="26">
         <v>19</v>
       </c>
-      <c r="AB27" s="48">
+      <c r="AB27" s="26">
+        <v>19</v>
+      </c>
+      <c r="AC27" s="48">
         <v>475</v>
       </c>
-      <c r="AC27" s="47">
+      <c r="AD27" s="47">
         <v>12</v>
       </c>
-      <c r="AD27" s="26">
+      <c r="AE27" s="26">
         <v>6</v>
       </c>
-      <c r="AE27" s="47">
+      <c r="AF27" s="47">
         <v>10</v>
       </c>
-      <c r="AF27" s="26">
+      <c r="AG27" s="26">
         <v>20000</v>
       </c>
-      <c r="AG27" s="132">
+      <c r="AH27" s="120">
         <v>5</v>
       </c>
-      <c r="AH27" s="115">
+      <c r="AI27" s="115">
         <v>0.05</v>
       </c>
-      <c r="AI27" s="64">
+      <c r="AJ27" s="64">
         <v>0.04</v>
       </c>
-      <c r="AJ27" s="71">
+      <c r="AK27" s="71">
         <v>0</v>
       </c>
-      <c r="AK27" s="45">
+      <c r="AL27" s="45">
         <v>12</v>
       </c>
-      <c r="AL27" s="44" t="s">
+      <c r="AM27" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="AM27" s="24" t="s">
+      <c r="AN27" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="AN27" s="24" t="s">
+      <c r="AO27" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="AO27" s="24" t="s">
+      <c r="AP27" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AP27" s="24" t="s">
+      <c r="AQ27" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="AQ27" s="24">
+      <c r="AR27" s="24">
         <v>1.1000000000000001</v>
-      </c>
-      <c r="AR27" s="24">
-        <v>2</v>
       </c>
       <c r="AS27" s="24">
         <v>2</v>
       </c>
-      <c r="AT27" s="24" t="b">
-        <v>1</v>
+      <c r="AT27" s="24">
+        <v>2</v>
       </c>
       <c r="AU27" s="24" t="b">
         <v>1</v>
@@ -6725,59 +6792,62 @@
       <c r="AV27" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AW27" s="24">
+      <c r="AW27" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX27" s="24">
         <v>23</v>
       </c>
-      <c r="AX27" s="24">
+      <c r="AY27" s="24">
         <v>0.75</v>
       </c>
-      <c r="AY27" s="24">
+      <c r="AZ27" s="24">
         <v>0.6</v>
       </c>
-      <c r="AZ27" s="43" t="s">
+      <c r="BA27" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="BA27" s="42" t="s">
+      <c r="BB27" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="BB27" s="41">
+      <c r="BC27" s="41">
         <v>8.7000000000000001E-4</v>
       </c>
-      <c r="BC27" s="40">
+      <c r="BD27" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BD27" s="39">
+      <c r="BE27" s="39">
         <v>680</v>
       </c>
-      <c r="BE27" s="111">
+      <c r="BF27" s="111">
         <v>730</v>
       </c>
-      <c r="BF27" s="38">
+      <c r="BG27" s="38">
         <v>4.7</v>
       </c>
-      <c r="BG27" s="38">
+      <c r="BH27" s="38">
         <v>9.5</v>
       </c>
-      <c r="BH27" s="38">
+      <c r="BI27" s="38">
         <v>1.7</v>
       </c>
-      <c r="BI27" s="38">
+      <c r="BJ27" s="38">
         <v>0.7</v>
       </c>
-      <c r="BJ27" s="38">
+      <c r="BK27" s="38">
         <v>1.03</v>
       </c>
-      <c r="BK27" s="38">
+      <c r="BL27" s="38">
         <v>59</v>
       </c>
-      <c r="BL27" s="38">
+      <c r="BM27" s="38">
         <v>15</v>
       </c>
-      <c r="BM27" s="37" t="s">
+      <c r="BN27" s="37" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="2:65" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:66" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
@@ -6785,58 +6855,58 @@
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
-      <c r="I28" s="120" t="s">
+      <c r="I28" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="121"/>
-      <c r="K28" s="121"/>
-      <c r="L28" s="122"/>
+      <c r="J28" s="124"/>
+      <c r="K28" s="124"/>
+      <c r="L28" s="125"/>
       <c r="M28" s="36"/>
-      <c r="N28" s="124" t="s">
+      <c r="N28" s="127" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="124"/>
-      <c r="P28" s="124"/>
-      <c r="Q28" s="124"/>
-      <c r="R28" s="124"/>
-      <c r="S28" s="125"/>
-      <c r="T28" s="123" t="s">
+      <c r="O28" s="127"/>
+      <c r="P28" s="127"/>
+      <c r="Q28" s="127"/>
+      <c r="R28" s="127"/>
+      <c r="S28" s="128"/>
+      <c r="T28" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="U28" s="123"/>
+      <c r="U28" s="126"/>
       <c r="V28" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W28" s="126" t="s">
+      <c r="W28" s="129" t="s">
         <v>70</v>
       </c>
-      <c r="X28" s="126"/>
-      <c r="Y28" s="126"/>
-      <c r="Z28" s="126"/>
-      <c r="AA28" s="126"/>
-      <c r="AB28" s="127" t="s">
+      <c r="X28" s="129"/>
+      <c r="Y28" s="129"/>
+      <c r="Z28" s="129"/>
+      <c r="AA28" s="129"/>
+      <c r="AB28" s="130" t="s">
         <v>69</v>
       </c>
-      <c r="AC28" s="127"/>
-      <c r="AD28" s="127"/>
-      <c r="AE28" s="127"/>
-      <c r="AF28" s="128"/>
-      <c r="AH28" s="129" t="s">
+      <c r="AC28" s="130"/>
+      <c r="AD28" s="130"/>
+      <c r="AE28" s="130"/>
+      <c r="AF28" s="131"/>
+      <c r="AH28" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="AI28" s="129"/>
-      <c r="BD28" s="118" t="s">
+      <c r="AI28" s="132"/>
+      <c r="BD28" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="BE28" s="118"/>
-      <c r="BF28" s="118"/>
-      <c r="BG28" s="118"/>
-      <c r="BH28" s="118"/>
-      <c r="BI28" s="118"/>
-      <c r="BJ28" s="118"/>
+      <c r="BE28" s="121"/>
+      <c r="BF28" s="121"/>
+      <c r="BG28" s="121"/>
+      <c r="BH28" s="121"/>
+      <c r="BI28" s="121"/>
+      <c r="BJ28" s="121"/>
     </row>
-    <row r="30" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:65" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:66" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
@@ -6850,7 +6920,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:65" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:66" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
@@ -7922,25 +7992,25 @@
     <mergeCell ref="AH28:AI28"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="101" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="100" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM16:BM23 BM25:BM26">
-    <cfRule type="duplicateValues" dxfId="99" priority="5"/>
+  <conditionalFormatting sqref="BN16:BN23 BN25:BN26">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="98" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM24">
-    <cfRule type="duplicateValues" dxfId="97" priority="3"/>
+  <conditionalFormatting sqref="BN24">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM27">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="BN27">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">

</xml_diff>

<commit_message>
[CONTENT] Added columns related to the "mummy" pet
Former-commit-id: 8f3e91615c76127ef5c2e20d2f652df8143d99ce
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="207">
   <si>
     <t>[sku]</t>
   </si>
@@ -639,6 +639,12 @@
   </si>
   <si>
     <t>normal</t>
+  </si>
+  <si>
+    <t>[mummyHealthFactor]</t>
+  </si>
+  <si>
+    <t>[mummyDuration]</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1548,13 +1554,15 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="103">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+  <dxfs count="105">
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1646,6 +1654,29 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3515,6 +3546,30 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3617,99 +3672,101 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BN27" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101" tableBorderDxfId="99" totalsRowBorderDxfId="98">
-  <autoFilter ref="B15:BN27"/>
-  <tableColumns count="65">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="97"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="96"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="95"/>
-    <tableColumn id="65" name="[type]" dataDxfId="0"/>
-    <tableColumn id="3" name="[order]" dataDxfId="94"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="93"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="92"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="91"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="90"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="89"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="88"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="87"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="86"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="85"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="84"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="83"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="82"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="81"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="80"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="79"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="78"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="77"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="76"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="75"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BP27" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101" totalsRowBorderDxfId="100">
+  <autoFilter ref="B15:BP27"/>
+  <tableColumns count="67">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="99"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="98"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="97"/>
+    <tableColumn id="65" name="[type]" dataDxfId="96"/>
+    <tableColumn id="3" name="[order]" dataDxfId="95"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="94"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="93"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="92"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="91"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="90"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="89"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="88"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="87"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="86"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="85"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="84"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="83"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="82"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="81"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="80"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="79"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="78"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="77"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="76"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="75">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="73"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="72"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="71"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="70"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="69"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="68"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="67"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="66"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="65"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="64">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="74"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="73"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="72"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="71"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="70"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="69"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="68"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="67"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="66"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="65">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="63"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="62"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="61"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="60"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="59"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="58"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="57"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="56"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="55"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="54"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="53"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="52"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="51"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="50"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="49"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="48"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="47">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="64"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="63"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="62"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="61"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="60"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="59"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="58"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="57"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="56"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="55"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="54"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="53"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="52"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="51"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="50"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="49"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="48">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="46">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="47">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="45"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="44"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="43"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="42">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="46"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="45"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="44"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="43">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="41"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="40"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="39"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="38"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="37"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="36"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="35"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="34"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="42"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="41"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="40"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="39"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="38"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="37"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="36"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="0"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="8"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="29"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="30"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="28"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="27"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="26">
+    <tableColumn id="10" name="[icon]" dataDxfId="29"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="28"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="27">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3718,11 +3775,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="B33:I34"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="21"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="20"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="22"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="21"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3735,7 +3792,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B45:W57"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3766,14 +3823,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B38:F41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="11"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="9"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="8"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="10"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4045,10 +4102,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BN57"/>
+  <dimension ref="B1:BP57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="BK28" sqref="BK28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4075,10 +4132,11 @@
     <col min="48" max="48" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="16.5703125" customWidth="1"/>
     <col min="65" max="65" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:66" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:68" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>183</v>
       </c>
@@ -4107,7 +4165,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4115,7 +4173,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:66" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:68" ht="117" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>182</v>
       </c>
@@ -4135,7 +4193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -4156,7 +4214,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -4177,7 +4235,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4198,7 +4256,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4219,7 +4277,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4240,8 +4298,8 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:66" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:68" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4270,7 +4328,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:66" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:68" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
         <v>174</v>
       </c>
@@ -4295,7 +4353,7 @@
       <c r="AQ14" s="122"/>
       <c r="AR14" s="122"/>
     </row>
-    <row r="15" spans="2:66" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:68" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
         <v>170</v>
       </c>
@@ -4488,11 +4546,17 @@
       <c r="BM15" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="BN15" s="72" t="s">
+      <c r="BN15" s="133" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO15" s="133" t="s">
+        <v>206</v>
+      </c>
+      <c r="BP15" s="72" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4681,11 +4745,17 @@
       <c r="BM16" s="70">
         <v>8</v>
       </c>
-      <c r="BN16" s="55" t="s">
+      <c r="BN16" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO16" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP16" s="55" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -4876,11 +4946,17 @@
       <c r="BM17" s="55">
         <v>8</v>
       </c>
-      <c r="BN17" s="55" t="s">
+      <c r="BN17" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO17" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP17" s="55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -5071,11 +5147,17 @@
       <c r="BM18" s="55">
         <v>8</v>
       </c>
-      <c r="BN18" s="37" t="s">
+      <c r="BN18" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO18" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP18" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -5266,11 +5348,17 @@
       <c r="BM19" s="55">
         <v>8</v>
       </c>
-      <c r="BN19" s="37" t="s">
+      <c r="BN19" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO19" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP19" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5461,11 +5549,17 @@
       <c r="BM20" s="55">
         <v>8</v>
       </c>
-      <c r="BN20" s="37" t="s">
+      <c r="BN20" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO20" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP20" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5656,11 +5750,17 @@
       <c r="BM21" s="55">
         <v>8</v>
       </c>
-      <c r="BN21" s="37" t="s">
+      <c r="BN21" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO21" s="70">
         <v>10</v>
       </c>
+      <c r="BP21" s="37" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="22" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -5851,11 +5951,17 @@
       <c r="BM22" s="55">
         <v>8</v>
       </c>
-      <c r="BN22" s="37" t="s">
+      <c r="BN22" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO22" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP22" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -6050,11 +6156,17 @@
       <c r="BM23" s="55">
         <v>15</v>
       </c>
-      <c r="BN23" s="37" t="s">
+      <c r="BN23" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO23" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP23" s="37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
@@ -6248,11 +6360,17 @@
       <c r="BM24" s="100">
         <v>15</v>
       </c>
-      <c r="BN24" s="97" t="s">
+      <c r="BN24" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO24" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP24" s="97" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -6447,11 +6565,17 @@
       <c r="BM25" s="55">
         <v>15</v>
       </c>
-      <c r="BN25" s="37" t="s">
+      <c r="BN25" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO25" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP25" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:66" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:68" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6645,11 +6769,17 @@
       <c r="BM26" s="38">
         <v>15</v>
       </c>
-      <c r="BN26" s="37" t="s">
+      <c r="BN26" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO26" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP26" s="37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="31" t="s">
         <v>3</v>
       </c>
@@ -6843,11 +6973,17 @@
       <c r="BM27" s="38">
         <v>15</v>
       </c>
-      <c r="BN27" s="37" t="s">
+      <c r="BN27" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="BO27" s="70">
+        <v>10</v>
+      </c>
+      <c r="BP27" s="37" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="2:66" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:68" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
@@ -6905,8 +7041,8 @@
       <c r="BI28" s="121"/>
       <c r="BJ28" s="121"/>
     </row>
-    <row r="30" spans="2:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:66" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:68" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
@@ -6920,7 +7056,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:66" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:68" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
@@ -7997,19 +8133,19 @@
   <conditionalFormatting sqref="C5:C9">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN16:BN23 BN25:BN26">
+  <conditionalFormatting sqref="BP16:BP23 BP25:BP26">
     <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
     <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN24">
+  <conditionalFormatting sqref="BP24">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN27">
+  <conditionalFormatting sqref="BP27">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">

</xml_diff>

<commit_message>
[CONTENT] Added animoji column to dragons def.
Former-commit-id: 1dc97bc998b6a9afb6d1b295d96e11ed46b69a20
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="212">
   <si>
     <t>[sku]</t>
   </si>
@@ -645,6 +645,21 @@
   </si>
   <si>
     <t>[mummyDuration]</t>
+  </si>
+  <si>
+    <t>[animojiPrefab]</t>
+  </si>
+  <si>
+    <t>PF_DragonBabyAnimoji</t>
+  </si>
+  <si>
+    <t>PF_DragonBugAnimoji</t>
+  </si>
+  <si>
+    <t>PF_DragonClassicAnimoji</t>
+  </si>
+  <si>
+    <t>PF_DragonGoldheistAnimoji</t>
   </si>
 </sst>
 </file>
@@ -797,7 +812,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1188,11 +1203,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1518,6 +1544,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1554,14 +1583,54 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="105">
+  <dxfs count="110">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1577,9 +1646,7 @@
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
+        <top/>
         <bottom/>
         <vertical/>
         <horizontal/>
@@ -1654,29 +1721,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2210,6 +2254,52 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -3672,101 +3762,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BP27" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101" totalsRowBorderDxfId="100">
-  <autoFilter ref="B15:BP27"/>
-  <tableColumns count="67">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="99"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="98"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="97"/>
-    <tableColumn id="65" name="[type]" dataDxfId="96"/>
-    <tableColumn id="3" name="[order]" dataDxfId="95"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="94"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="93"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="92"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="91"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="90"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="89"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="88"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="87"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="86"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="85"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="84"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="83"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="82"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="81"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="80"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="79"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="78"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="77"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="76"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BQ27" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106" totalsRowBorderDxfId="105">
+  <autoFilter ref="B15:BQ27"/>
+  <tableColumns count="68">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="104"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="103"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="102"/>
+    <tableColumn id="65" name="[type]" dataDxfId="101"/>
+    <tableColumn id="3" name="[order]" dataDxfId="100"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="99"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="98"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="97"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="96"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="95"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="94"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="93"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="92"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="91"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="90"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="89"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="88"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="87"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="86"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="85"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="84"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="83"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="82"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="81"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="80">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="74"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="73"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="72"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="71"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="70"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="69"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="68"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="67"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="66"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="65">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="79"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="78"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="77"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="76"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="75"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="74"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="73"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="72"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="71"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="70">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="64"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="63"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="62"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="61"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="60"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="59"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="58"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="57"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="56"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="55"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="54"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="53"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="52"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="51"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="50"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="49"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="48">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="69"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="68"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="67"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="66"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="65"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="64"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="63"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="62"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="61"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="60"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="59"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="58"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="57"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="56"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="55"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="54"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="53">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="47">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="52">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="46"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="45"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="44"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="43">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="51"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="50"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="49"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="48">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="42"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="41"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="40"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="39"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="38"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="37"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="36"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="0"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="8"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="35"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="47"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="46"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="45"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="44"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="43"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="42"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="41"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="40"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="39"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="4"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="30"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="33"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="29"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="28"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="27">
+    <tableColumn id="10" name="[icon]" dataDxfId="32"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="31"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="30">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3775,11 +3866,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B33:I34"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="22"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="21"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3792,7 +3883,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B45:W57"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3823,14 +3914,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B38:F41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="10"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="9"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="13"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4102,10 +4193,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BP57"/>
+  <dimension ref="B1:BQ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="BK28" sqref="BK28"/>
+    <sheetView tabSelected="1" topLeftCell="AW5" workbookViewId="0">
+      <selection activeCell="BP27" sqref="BP27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4132,11 +4223,11 @@
     <col min="48" max="48" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="16.5703125" customWidth="1"/>
     <col min="65" max="65" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="16.5703125" customWidth="1"/>
+    <col min="66" max="68" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:68" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:69" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>183</v>
       </c>
@@ -4165,7 +4256,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4173,7 +4264,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:68" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:69" ht="117" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>182</v>
       </c>
@@ -4193,7 +4284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -4214,7 +4305,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -4235,7 +4326,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4256,7 +4347,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4277,7 +4368,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4298,8 +4389,8 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:68" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:69" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4328,7 +4419,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:68" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:69" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
         <v>174</v>
       </c>
@@ -4348,12 +4439,12 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="122"/>
-      <c r="AP14" s="122"/>
-      <c r="AQ14" s="122"/>
-      <c r="AR14" s="122"/>
+      <c r="AO14" s="123"/>
+      <c r="AP14" s="123"/>
+      <c r="AQ14" s="123"/>
+      <c r="AR14" s="123"/>
     </row>
-    <row r="15" spans="2:68" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:69" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
         <v>170</v>
       </c>
@@ -4546,17 +4637,20 @@
       <c r="BM15" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="BN15" s="133" t="s">
+      <c r="BN15" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="BO15" s="133" t="s">
+      <c r="BO15" s="121" t="s">
         <v>206</v>
       </c>
-      <c r="BP15" s="72" t="s">
+      <c r="BP15" s="121" t="s">
+        <v>207</v>
+      </c>
+      <c r="BQ15" s="72" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4752,10 +4846,13 @@
         <v>10</v>
       </c>
       <c r="BP16" s="55" t="s">
+        <v>208</v>
+      </c>
+      <c r="BQ16" s="55" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -4952,11 +5049,12 @@
       <c r="BO17" s="70">
         <v>10</v>
       </c>
-      <c r="BP17" s="55" t="s">
+      <c r="BP17" s="70"/>
+      <c r="BQ17" s="55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -5153,11 +5251,12 @@
       <c r="BO18" s="70">
         <v>10</v>
       </c>
-      <c r="BP18" s="37" t="s">
+      <c r="BP18" s="134"/>
+      <c r="BQ18" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -5354,11 +5453,12 @@
       <c r="BO19" s="70">
         <v>10</v>
       </c>
-      <c r="BP19" s="37" t="s">
+      <c r="BP19" s="134"/>
+      <c r="BQ19" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5556,10 +5656,13 @@
         <v>10</v>
       </c>
       <c r="BP20" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="BQ20" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5756,11 +5859,12 @@
       <c r="BO21" s="70">
         <v>10</v>
       </c>
-      <c r="BP21" s="37" t="s">
+      <c r="BP21" s="134"/>
+      <c r="BQ21" s="37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -5958,10 +6062,13 @@
         <v>10</v>
       </c>
       <c r="BP22" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BQ22" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -6162,11 +6269,12 @@
       <c r="BO23" s="70">
         <v>10</v>
       </c>
-      <c r="BP23" s="37" t="s">
+      <c r="BP23" s="134"/>
+      <c r="BQ23" s="37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
@@ -6366,11 +6474,12 @@
       <c r="BO24" s="70">
         <v>10</v>
       </c>
-      <c r="BP24" s="97" t="s">
+      <c r="BP24" s="134"/>
+      <c r="BQ24" s="97" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -6571,11 +6680,12 @@
       <c r="BO25" s="70">
         <v>10</v>
       </c>
-      <c r="BP25" s="37" t="s">
+      <c r="BP25" s="134"/>
+      <c r="BQ25" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:68" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6775,11 +6885,12 @@
       <c r="BO26" s="70">
         <v>10</v>
       </c>
-      <c r="BP26" s="37" t="s">
+      <c r="BP26" s="134"/>
+      <c r="BQ26" s="37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="31" t="s">
         <v>3</v>
       </c>
@@ -6980,10 +7091,13 @@
         <v>10</v>
       </c>
       <c r="BP27" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="BQ27" s="37" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="2:68" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:69" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
@@ -6991,58 +7105,58 @@
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
-      <c r="I28" s="123" t="s">
+      <c r="I28" s="124" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="124"/>
-      <c r="K28" s="124"/>
-      <c r="L28" s="125"/>
+      <c r="J28" s="125"/>
+      <c r="K28" s="125"/>
+      <c r="L28" s="126"/>
       <c r="M28" s="36"/>
-      <c r="N28" s="127" t="s">
+      <c r="N28" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="127"/>
-      <c r="P28" s="127"/>
-      <c r="Q28" s="127"/>
-      <c r="R28" s="127"/>
-      <c r="S28" s="128"/>
-      <c r="T28" s="126" t="s">
+      <c r="O28" s="128"/>
+      <c r="P28" s="128"/>
+      <c r="Q28" s="128"/>
+      <c r="R28" s="128"/>
+      <c r="S28" s="129"/>
+      <c r="T28" s="127" t="s">
         <v>72</v>
       </c>
-      <c r="U28" s="126"/>
+      <c r="U28" s="127"/>
       <c r="V28" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W28" s="129" t="s">
+      <c r="W28" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="X28" s="129"/>
-      <c r="Y28" s="129"/>
-      <c r="Z28" s="129"/>
-      <c r="AA28" s="129"/>
-      <c r="AB28" s="130" t="s">
+      <c r="X28" s="130"/>
+      <c r="Y28" s="130"/>
+      <c r="Z28" s="130"/>
+      <c r="AA28" s="130"/>
+      <c r="AB28" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="AC28" s="130"/>
-      <c r="AD28" s="130"/>
-      <c r="AE28" s="130"/>
-      <c r="AF28" s="131"/>
-      <c r="AH28" s="132" t="s">
+      <c r="AC28" s="131"/>
+      <c r="AD28" s="131"/>
+      <c r="AE28" s="131"/>
+      <c r="AF28" s="132"/>
+      <c r="AH28" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="AI28" s="132"/>
-      <c r="BD28" s="121" t="s">
+      <c r="AI28" s="133"/>
+      <c r="BD28" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="BE28" s="121"/>
-      <c r="BF28" s="121"/>
-      <c r="BG28" s="121"/>
-      <c r="BH28" s="121"/>
-      <c r="BI28" s="121"/>
-      <c r="BJ28" s="121"/>
+      <c r="BE28" s="122"/>
+      <c r="BF28" s="122"/>
+      <c r="BG28" s="122"/>
+      <c r="BH28" s="122"/>
+      <c r="BI28" s="122"/>
+      <c r="BJ28" s="122"/>
     </row>
-    <row r="30" spans="2:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:68" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:69" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
@@ -7056,7 +7170,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:68" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:69" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
@@ -8128,25 +8242,37 @@
     <mergeCell ref="AH28:AI28"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP16:BP23 BP25:BP26">
+  <conditionalFormatting sqref="BQ16:BQ23 BQ25:BQ26">
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ24">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ27">
     <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="BP16">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP24">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  <conditionalFormatting sqref="BP20">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="BP22">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP27">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">

</xml_diff>

<commit_message>
Goldhesit stats bar size reduced
Former-commit-id: c4df2a99c052a87ecb3ed3ec02640c285905b65f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1547,6 +1547,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1582,146 +1585,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="110">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2251,6 +2120,27 @@
         <right style="thin">
           <color auto="1"/>
         </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -3748,6 +3638,116 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3762,102 +3762,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BQ27" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106" totalsRowBorderDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BQ27" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
   <autoFilter ref="B15:BQ27"/>
   <tableColumns count="68">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="104"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="103"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="102"/>
-    <tableColumn id="65" name="[type]" dataDxfId="101"/>
-    <tableColumn id="3" name="[order]" dataDxfId="100"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="99"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="98"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="97"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="96"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="95"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="94"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="93"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="92"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="91"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="90"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="89"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="88"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="87"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="86"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="85"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="84"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="83"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="82"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="81"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="80">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="93"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="92"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="91"/>
+    <tableColumn id="65" name="[type]" dataDxfId="90"/>
+    <tableColumn id="3" name="[order]" dataDxfId="89"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="88"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="87"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="86"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="85"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="84"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="83"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="82"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="81"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="80"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="79"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="78"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="77"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="76"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="75"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="74"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="73"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="72"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="71"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="70"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="69">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="79"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="78"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="77"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="76"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="75"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="74"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="73"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="72"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="71"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="70">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="68"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="67"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="66"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="65"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="64"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="63"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="62"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="61"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="60"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="59">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="69"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="68"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="67"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="66"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="65"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="64"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="63"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="62"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="61"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="60"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="59"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="58"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="57"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="56"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="55"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="54"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="53">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="58"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="57"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="56"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="55"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="54"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="53"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="52"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="51"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="50"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="49"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="48"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="47"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="46"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="45"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="44"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="43"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="42">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="52">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="41">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="51"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="50"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="49"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="48">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="40"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="39"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="38"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="37">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="47"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="46"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="45"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="44"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="43"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="42"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="41"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="40"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="39"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="4"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="38"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="36"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="35"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="34"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="33"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="32"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="31"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="30"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="29"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="28"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="27"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="33"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="32"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="31"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="30">
+    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="18">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3866,11 +3866,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B33:I34"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3883,7 +3883,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B45:W57"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3914,14 +3914,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B38:F41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="13"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="12"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4196,7 +4196,7 @@
   <dimension ref="B1:BQ57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AW5" workbookViewId="0">
-      <selection activeCell="BP27" sqref="BP27"/>
+      <selection activeCell="BC28" sqref="BC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4439,10 +4439,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="123"/>
-      <c r="AP14" s="123"/>
-      <c r="AQ14" s="123"/>
-      <c r="AR14" s="123"/>
+      <c r="AO14" s="124"/>
+      <c r="AP14" s="124"/>
+      <c r="AQ14" s="124"/>
+      <c r="AR14" s="124"/>
     </row>
     <row r="15" spans="2:69" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
@@ -5251,7 +5251,7 @@
       <c r="BO18" s="70">
         <v>10</v>
       </c>
-      <c r="BP18" s="134"/>
+      <c r="BP18" s="122"/>
       <c r="BQ18" s="37" t="s">
         <v>7</v>
       </c>
@@ -5453,7 +5453,7 @@
       <c r="BO19" s="70">
         <v>10</v>
       </c>
-      <c r="BP19" s="134"/>
+      <c r="BP19" s="122"/>
       <c r="BQ19" s="37" t="s">
         <v>8</v>
       </c>
@@ -5859,7 +5859,7 @@
       <c r="BO21" s="70">
         <v>10</v>
       </c>
-      <c r="BP21" s="134"/>
+      <c r="BP21" s="122"/>
       <c r="BQ21" s="37" t="s">
         <v>10</v>
       </c>
@@ -6269,7 +6269,7 @@
       <c r="BO23" s="70">
         <v>10</v>
       </c>
-      <c r="BP23" s="134"/>
+      <c r="BP23" s="122"/>
       <c r="BQ23" s="37" t="s">
         <v>12</v>
       </c>
@@ -6474,7 +6474,7 @@
       <c r="BO24" s="70">
         <v>10</v>
       </c>
-      <c r="BP24" s="134"/>
+      <c r="BP24" s="122"/>
       <c r="BQ24" s="97" t="s">
         <v>184</v>
       </c>
@@ -6680,7 +6680,7 @@
       <c r="BO25" s="70">
         <v>10</v>
       </c>
-      <c r="BP25" s="134"/>
+      <c r="BP25" s="122"/>
       <c r="BQ25" s="37" t="s">
         <v>13</v>
       </c>
@@ -6885,7 +6885,7 @@
       <c r="BO26" s="70">
         <v>10</v>
       </c>
-      <c r="BP26" s="134"/>
+      <c r="BP26" s="122"/>
       <c r="BQ26" s="37" t="s">
         <v>14</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>199</v>
       </c>
       <c r="BC27" s="41">
-        <v>8.7000000000000001E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="BD27" s="40">
         <v>5.0000000000000001E-3</v>
@@ -7105,55 +7105,55 @@
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
-      <c r="I28" s="124" t="s">
+      <c r="I28" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="125"/>
-      <c r="K28" s="125"/>
-      <c r="L28" s="126"/>
+      <c r="J28" s="126"/>
+      <c r="K28" s="126"/>
+      <c r="L28" s="127"/>
       <c r="M28" s="36"/>
-      <c r="N28" s="128" t="s">
+      <c r="N28" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="128"/>
-      <c r="P28" s="128"/>
-      <c r="Q28" s="128"/>
-      <c r="R28" s="128"/>
-      <c r="S28" s="129"/>
-      <c r="T28" s="127" t="s">
+      <c r="O28" s="129"/>
+      <c r="P28" s="129"/>
+      <c r="Q28" s="129"/>
+      <c r="R28" s="129"/>
+      <c r="S28" s="130"/>
+      <c r="T28" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="U28" s="127"/>
+      <c r="U28" s="128"/>
       <c r="V28" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W28" s="130" t="s">
+      <c r="W28" s="131" t="s">
         <v>70</v>
       </c>
-      <c r="X28" s="130"/>
-      <c r="Y28" s="130"/>
-      <c r="Z28" s="130"/>
-      <c r="AA28" s="130"/>
-      <c r="AB28" s="131" t="s">
+      <c r="X28" s="131"/>
+      <c r="Y28" s="131"/>
+      <c r="Z28" s="131"/>
+      <c r="AA28" s="131"/>
+      <c r="AB28" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="AC28" s="131"/>
-      <c r="AD28" s="131"/>
-      <c r="AE28" s="131"/>
-      <c r="AF28" s="132"/>
-      <c r="AH28" s="133" t="s">
+      <c r="AC28" s="132"/>
+      <c r="AD28" s="132"/>
+      <c r="AE28" s="132"/>
+      <c r="AF28" s="133"/>
+      <c r="AH28" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="AI28" s="133"/>
-      <c r="BD28" s="122" t="s">
+      <c r="AI28" s="134"/>
+      <c r="BD28" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="BE28" s="122"/>
-      <c r="BF28" s="122"/>
-      <c r="BG28" s="122"/>
-      <c r="BH28" s="122"/>
-      <c r="BI28" s="122"/>
-      <c r="BJ28" s="122"/>
+      <c r="BE28" s="123"/>
+      <c r="BF28" s="123"/>
+      <c r="BG28" s="123"/>
+      <c r="BH28" s="123"/>
+      <c r="BI28" s="123"/>
+      <c r="BJ28" s="123"/>
     </row>
     <row r="30" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:69" ht="23.25" x14ac:dyDescent="0.35">
@@ -8242,37 +8242,37 @@
     <mergeCell ref="AH28:AI28"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BQ23 BQ25:BQ26">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ24">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP16">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP20">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP22">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP27">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">

</xml_diff>

<commit_message>
Adding reptile prefab for animojis
Former-commit-id: 06de7cd4df2f3443ee8f9121f5df1cd0e647179f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="213">
   <si>
     <t>[sku]</t>
   </si>
@@ -660,6 +660,9 @@
   </si>
   <si>
     <t>PF_DragonGoldheistAnimoji</t>
+  </si>
+  <si>
+    <t>PF_DragonReptileAnimoji</t>
   </si>
 </sst>
 </file>
@@ -4196,7 +4199,7 @@
   <dimension ref="B1:BQ57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AW5" workbookViewId="0">
-      <selection activeCell="BC28" sqref="BC28"/>
+      <selection activeCell="AZ8" sqref="AZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4223,7 +4226,8 @@
     <col min="48" max="48" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="16.5703125" customWidth="1"/>
     <col min="65" max="65" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="66" max="68" width="16.5703125" customWidth="1"/>
+    <col min="66" max="67" width="16.5703125" customWidth="1"/>
+    <col min="68" max="68" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5251,7 +5255,9 @@
       <c r="BO18" s="70">
         <v>10</v>
       </c>
-      <c r="BP18" s="122"/>
+      <c r="BP18" s="122" t="s">
+        <v>212</v>
+      </c>
       <c r="BQ18" s="37" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
[ CHANGE ] [CONTENT] Changed values for Mummy Power (refilled health and time duration)
Former-commit-id: bb8588f8e009024b7e5e07de551811154df9b857
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4199,7 +4199,7 @@
   <dimension ref="B1:BQ57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AW5" workbookViewId="0">
-      <selection activeCell="AZ8" sqref="AZ8"/>
+      <selection activeCell="BN16" sqref="BN16:BN27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4844,10 +4844,10 @@
         <v>8</v>
       </c>
       <c r="BN16" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO16" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP16" s="55" t="s">
         <v>208</v>
@@ -5048,10 +5048,10 @@
         <v>8</v>
       </c>
       <c r="BN17" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO17" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP17" s="70"/>
       <c r="BQ17" s="55" t="s">
@@ -5250,10 +5250,10 @@
         <v>8</v>
       </c>
       <c r="BN18" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO18" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP18" s="122" t="s">
         <v>212</v>
@@ -5454,10 +5454,10 @@
         <v>8</v>
       </c>
       <c r="BN19" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO19" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP19" s="122"/>
       <c r="BQ19" s="37" t="s">
@@ -5656,10 +5656,10 @@
         <v>8</v>
       </c>
       <c r="BN20" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO20" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP20" s="37" t="s">
         <v>209</v>
@@ -5860,10 +5860,10 @@
         <v>8</v>
       </c>
       <c r="BN21" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO21" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP21" s="122"/>
       <c r="BQ21" s="37" t="s">
@@ -6062,10 +6062,10 @@
         <v>8</v>
       </c>
       <c r="BN22" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO22" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP22" s="37" t="s">
         <v>210</v>
@@ -6270,10 +6270,10 @@
         <v>15</v>
       </c>
       <c r="BN23" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO23" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP23" s="122"/>
       <c r="BQ23" s="37" t="s">
@@ -6475,10 +6475,10 @@
         <v>15</v>
       </c>
       <c r="BN24" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO24" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP24" s="122"/>
       <c r="BQ24" s="97" t="s">
@@ -6681,10 +6681,10 @@
         <v>15</v>
       </c>
       <c r="BN25" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO25" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP25" s="122"/>
       <c r="BQ25" s="37" t="s">
@@ -6886,10 +6886,10 @@
         <v>15</v>
       </c>
       <c r="BN26" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO26" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP26" s="122"/>
       <c r="BQ26" s="37" t="s">
@@ -7091,10 +7091,10 @@
         <v>15</v>
       </c>
       <c r="BN27" s="70">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="BO27" s="70">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BP27" s="37" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
Added Titan prefab animoji
Former-commit-id: 8744fca35199830c194c53bc2b77be585722c344
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="214">
   <si>
     <t>[sku]</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>PF_DragonReptileAnimoji</t>
+  </si>
+  <si>
+    <t>PF_DragonTitanAnimoji</t>
   </si>
 </sst>
 </file>
@@ -4199,7 +4202,7 @@
   <dimension ref="B1:BQ57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AW5" workbookViewId="0">
-      <selection activeCell="BN16" sqref="BN16:BN27"/>
+      <selection activeCell="BP26" sqref="BP26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6891,7 +6894,9 @@
       <c r="BO26" s="70">
         <v>25</v>
       </c>
-      <c r="BP26" s="122"/>
+      <c r="BP26" s="122" t="s">
+        <v>213</v>
+      </c>
       <c r="BQ26" s="37" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Adding 2 parameters to control boost restarts
Former-commit-id: 387c8be42c5eca551af98446b3fe0444dbc3f44a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="217">
   <si>
     <t>[sku]</t>
   </si>
@@ -666,6 +666,15 @@
   </si>
   <si>
     <t>PF_DragonTitanAnimoji</t>
+  </si>
+  <si>
+    <t>[energyRestartThreshold]</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0,2</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1605,159 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
+  <dxfs count="112">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3644,116 +3805,6 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3768,102 +3819,104 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BQ27" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
-  <autoFilter ref="B15:BQ27"/>
-  <tableColumns count="68">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="93"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="92"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="91"/>
-    <tableColumn id="65" name="[type]" dataDxfId="90"/>
-    <tableColumn id="3" name="[order]" dataDxfId="89"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="88"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="87"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="86"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="85"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="84"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="83"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="82"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="81"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="80"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="79"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="78"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="77"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="76"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="75"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="74"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="73"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="72"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="71"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="70"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BS27" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
+  <autoFilter ref="B15:BS27"/>
+  <tableColumns count="70">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="106"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="105"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="104"/>
+    <tableColumn id="65" name="[type]" dataDxfId="103"/>
+    <tableColumn id="3" name="[order]" dataDxfId="102"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="101"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="100"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="99"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="98"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="97"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="96"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="95"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="94"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="93"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="92"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="91"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="90"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="89"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="88"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="87"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="86"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="85"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="84"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="83"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="82">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="68"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="67"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="66"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="65"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="64"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="63"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="62"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="61"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="60"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="59">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="81"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="80"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="79"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="78"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="77"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="76"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="75"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="74"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="73"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="72">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="58"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="57"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="56"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="55"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="54"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="53"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="52"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="51"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="50"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="49"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="48"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="47"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="46"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="45"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="44"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="43"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="42">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="71"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="70"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="69"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="68"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="67"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="66"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="65"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="64"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="63"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="62"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="61"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="60"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="59"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="58"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="57"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="56"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="55">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="41">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="54">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="40"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="39"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="38"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="37">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="53"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="52"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="51"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="50">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="36"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="35"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="34"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="33"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="32"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="31"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="30"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="29"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="28"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="27"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="49"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="48"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="47"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="46"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="45"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="44"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="43"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="42"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="41"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="40"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="0"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="12"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="34"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="18">
+    <tableColumn id="10" name="[icon]" dataDxfId="33"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="32"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="31">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3872,11 +3925,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="B33:I34"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="26"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3889,7 +3942,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="B45:W57"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3920,14 +3973,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B38:F41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="16"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="14"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4199,10 +4252,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BQ57"/>
+  <dimension ref="B1:BS57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW5" workbookViewId="0">
-      <selection activeCell="BP26" sqref="BP26"/>
+    <sheetView tabSelected="1" topLeftCell="BE7" workbookViewId="0">
+      <selection activeCell="BR28" sqref="BR28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4233,8 +4286,8 @@
     <col min="68" max="68" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:69" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:71" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>183</v>
       </c>
@@ -4263,7 +4316,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4271,7 +4324,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:69" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:71" ht="117" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>182</v>
       </c>
@@ -4291,7 +4344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -4312,7 +4365,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
@@ -4333,7 +4386,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4354,7 +4407,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4375,7 +4428,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -4396,8 +4449,8 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:69" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:71" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4426,7 +4479,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:69" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:71" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
         <v>174</v>
       </c>
@@ -4451,7 +4504,7 @@
       <c r="AQ14" s="124"/>
       <c r="AR14" s="124"/>
     </row>
-    <row r="15" spans="2:69" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:71" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
         <v>170</v>
       </c>
@@ -4653,11 +4706,17 @@
       <c r="BP15" s="121" t="s">
         <v>207</v>
       </c>
-      <c r="BQ15" s="72" t="s">
+      <c r="BQ15" s="121" t="s">
+        <v>63</v>
+      </c>
+      <c r="BR15" s="121" t="s">
+        <v>214</v>
+      </c>
+      <c r="BS15" s="72" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -4855,11 +4914,17 @@
       <c r="BP16" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="BQ16" s="55" t="s">
+      <c r="BQ16" s="55">
+        <v>1</v>
+      </c>
+      <c r="BR16" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="BS16" s="55" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>3</v>
       </c>
@@ -5057,11 +5122,17 @@
         <v>25</v>
       </c>
       <c r="BP17" s="70"/>
-      <c r="BQ17" s="55" t="s">
+      <c r="BQ17" s="70">
+        <v>1</v>
+      </c>
+      <c r="BR17" s="70">
+        <v>0.2</v>
+      </c>
+      <c r="BS17" s="55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>3</v>
       </c>
@@ -5261,11 +5332,17 @@
       <c r="BP18" s="122" t="s">
         <v>212</v>
       </c>
-      <c r="BQ18" s="37" t="s">
+      <c r="BQ18" s="122">
+        <v>1</v>
+      </c>
+      <c r="BR18" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BS18" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -5463,11 +5540,17 @@
         <v>25</v>
       </c>
       <c r="BP19" s="122"/>
-      <c r="BQ19" s="37" t="s">
+      <c r="BQ19" s="122">
+        <v>1</v>
+      </c>
+      <c r="BR19" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BS19" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>3</v>
       </c>
@@ -5668,10 +5751,16 @@
         <v>209</v>
       </c>
       <c r="BQ20" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="BR20" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="BS20" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -5869,11 +5958,17 @@
         <v>25</v>
       </c>
       <c r="BP21" s="122"/>
-      <c r="BQ21" s="37" t="s">
+      <c r="BQ21" s="122">
+        <v>1</v>
+      </c>
+      <c r="BR21" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BS21" s="37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>3</v>
       </c>
@@ -6074,10 +6169,16 @@
         <v>210</v>
       </c>
       <c r="BQ22" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="BR22" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="BS22" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>3</v>
       </c>
@@ -6279,11 +6380,17 @@
         <v>25</v>
       </c>
       <c r="BP23" s="122"/>
-      <c r="BQ23" s="37" t="s">
+      <c r="BQ23" s="122">
+        <v>1</v>
+      </c>
+      <c r="BR23" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BS23" s="37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>3</v>
       </c>
@@ -6484,11 +6591,17 @@
         <v>25</v>
       </c>
       <c r="BP24" s="122"/>
-      <c r="BQ24" s="97" t="s">
+      <c r="BQ24" s="122">
+        <v>1</v>
+      </c>
+      <c r="BR24" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BS24" s="97" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>3</v>
       </c>
@@ -6690,11 +6803,17 @@
         <v>25</v>
       </c>
       <c r="BP25" s="122"/>
-      <c r="BQ25" s="37" t="s">
+      <c r="BQ25" s="122">
+        <v>1</v>
+      </c>
+      <c r="BR25" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BS25" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
         <v>3</v>
       </c>
@@ -6897,11 +7016,17 @@
       <c r="BP26" s="122" t="s">
         <v>213</v>
       </c>
-      <c r="BQ26" s="37" t="s">
+      <c r="BQ26" s="122">
+        <v>1</v>
+      </c>
+      <c r="BR26" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BS26" s="37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="31" t="s">
         <v>3</v>
       </c>
@@ -7105,10 +7230,16 @@
         <v>211</v>
       </c>
       <c r="BQ27" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="BR27" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="BS27" s="37" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="2:69" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:71" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
@@ -7166,8 +7297,8 @@
       <c r="BI28" s="123"/>
       <c r="BJ28" s="123"/>
     </row>
-    <row r="30" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:69" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:71" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
@@ -7181,7 +7312,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:69" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:71" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
@@ -8253,37 +8384,37 @@
     <mergeCell ref="AH28:AI28"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="109" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="108" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ16:BQ23 BQ25:BQ26">
-    <cfRule type="duplicateValues" dxfId="107" priority="9"/>
+  <conditionalFormatting sqref="BS16:BS23 BS25:BS26">
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="106" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ24">
-    <cfRule type="duplicateValues" dxfId="105" priority="7"/>
+  <conditionalFormatting sqref="BS24">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="104" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ27">
-    <cfRule type="duplicateValues" dxfId="103" priority="5"/>
+  <conditionalFormatting sqref="BS27">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP16">
-    <cfRule type="duplicateValues" dxfId="102" priority="4"/>
+  <conditionalFormatting sqref="BP16:BR16">
+    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP20">
-    <cfRule type="duplicateValues" dxfId="101" priority="3"/>
+  <conditionalFormatting sqref="BP20:BR20">
+    <cfRule type="duplicateValues" dxfId="3" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP22">
-    <cfRule type="duplicateValues" dxfId="100" priority="2"/>
+  <conditionalFormatting sqref="BP22:BR22">
+    <cfRule type="duplicateValues" dxfId="2" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP27">
-    <cfRule type="duplicateValues" dxfId="99" priority="1"/>
+  <conditionalFormatting sqref="BP27:BR27">
+    <cfRule type="duplicateValues" dxfId="1" priority="19"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">

</xml_diff>

<commit_message>
Switching values for those 2 parameters
Former-commit-id: 234ebec9cc260aa09398c5ae038d0a114322778f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -4255,7 +4255,7 @@
   <dimension ref="B1:BS57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BE7" workbookViewId="0">
-      <selection activeCell="BR28" sqref="BR28"/>
+      <selection activeCell="BQ28" sqref="BQ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4915,10 +4915,10 @@
         <v>208</v>
       </c>
       <c r="BQ16" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="BR16" s="55">
         <v>1</v>
-      </c>
-      <c r="BR16" s="55">
-        <v>0.2</v>
       </c>
       <c r="BS16" s="55" t="s">
         <v>5</v>
@@ -5123,10 +5123,10 @@
       </c>
       <c r="BP17" s="70"/>
       <c r="BQ17" s="70">
+        <v>0.2</v>
+      </c>
+      <c r="BR17" s="70">
         <v>1</v>
-      </c>
-      <c r="BR17" s="70">
-        <v>0.2</v>
       </c>
       <c r="BS17" s="55" t="s">
         <v>6</v>
@@ -5333,10 +5333,10 @@
         <v>212</v>
       </c>
       <c r="BQ18" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BR18" s="122">
         <v>1</v>
-      </c>
-      <c r="BR18" s="122">
-        <v>0.2</v>
       </c>
       <c r="BS18" s="37" t="s">
         <v>7</v>
@@ -5541,10 +5541,10 @@
       </c>
       <c r="BP19" s="122"/>
       <c r="BQ19" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BR19" s="122">
         <v>1</v>
-      </c>
-      <c r="BR19" s="122">
-        <v>0.2</v>
       </c>
       <c r="BS19" s="37" t="s">
         <v>8</v>
@@ -5751,10 +5751,10 @@
         <v>209</v>
       </c>
       <c r="BQ20" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="BR20" s="37" t="s">
         <v>215</v>
-      </c>
-      <c r="BR20" s="37" t="s">
-        <v>216</v>
       </c>
       <c r="BS20" s="37" t="s">
         <v>9</v>
@@ -5959,10 +5959,10 @@
       </c>
       <c r="BP21" s="122"/>
       <c r="BQ21" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BR21" s="122">
         <v>1</v>
-      </c>
-      <c r="BR21" s="122">
-        <v>0.2</v>
       </c>
       <c r="BS21" s="37" t="s">
         <v>10</v>
@@ -6169,10 +6169,10 @@
         <v>210</v>
       </c>
       <c r="BQ22" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="BR22" s="37" t="s">
         <v>215</v>
-      </c>
-      <c r="BR22" s="37" t="s">
-        <v>216</v>
       </c>
       <c r="BS22" s="37" t="s">
         <v>11</v>
@@ -6381,10 +6381,10 @@
       </c>
       <c r="BP23" s="122"/>
       <c r="BQ23" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BR23" s="122">
         <v>1</v>
-      </c>
-      <c r="BR23" s="122">
-        <v>0.2</v>
       </c>
       <c r="BS23" s="37" t="s">
         <v>12</v>
@@ -6592,10 +6592,10 @@
       </c>
       <c r="BP24" s="122"/>
       <c r="BQ24" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BR24" s="122">
         <v>1</v>
-      </c>
-      <c r="BR24" s="122">
-        <v>0.2</v>
       </c>
       <c r="BS24" s="97" t="s">
         <v>184</v>
@@ -6804,10 +6804,10 @@
       </c>
       <c r="BP25" s="122"/>
       <c r="BQ25" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BR25" s="122">
         <v>1</v>
-      </c>
-      <c r="BR25" s="122">
-        <v>0.2</v>
       </c>
       <c r="BS25" s="37" t="s">
         <v>13</v>
@@ -7017,10 +7017,10 @@
         <v>213</v>
       </c>
       <c r="BQ26" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="BR26" s="122">
         <v>1</v>
-      </c>
-      <c r="BR26" s="122">
-        <v>0.2</v>
       </c>
       <c r="BS26" s="37" t="s">
         <v>14</v>
@@ -7230,10 +7230,10 @@
         <v>211</v>
       </c>
       <c r="BQ27" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="BR27" s="37" t="s">
         <v>215</v>
-      </c>
-      <c r="BR27" s="37" t="s">
-        <v>216</v>
       </c>
       <c r="BS27" s="37" t="s">
         <v>197</v>

</xml_diff>

<commit_message>
Fixing excel cells, that some of them were TEXT instead of NUMBER
Former-commit-id: 81e581d54c1bef2417999630b637bc9d89bd93ac
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="215">
   <si>
     <t>[sku]</t>
   </si>
@@ -669,12 +669,6 @@
   </si>
   <si>
     <t>[energyRestartThreshold]</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0,2</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1601,163 +1595,17 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="112">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2308,6 +2156,48 @@
         <right style="thin">
           <color auto="1"/>
         </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -3805,6 +3695,116 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3819,104 +3819,104 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BS27" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BS27" totalsRowShown="0" headerRowDxfId="100" dataDxfId="98" headerRowBorderDxfId="99" tableBorderDxfId="97" totalsRowBorderDxfId="96">
   <autoFilter ref="B15:BS27"/>
   <tableColumns count="70">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="106"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="105"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="104"/>
-    <tableColumn id="65" name="[type]" dataDxfId="103"/>
-    <tableColumn id="3" name="[order]" dataDxfId="102"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="101"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="100"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="99"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="98"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="97"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="96"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="95"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="94"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="93"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="92"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="91"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="90"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="89"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="88"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="87"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="86"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="85"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="84"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="83"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="82">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="95"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="94"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="93"/>
+    <tableColumn id="65" name="[type]" dataDxfId="92"/>
+    <tableColumn id="3" name="[order]" dataDxfId="91"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="90"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="89"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="88"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="87"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="86"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="85"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="84"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="83"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="82"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="81"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="80"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="79"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="78"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="77"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="76"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="75"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="74"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="73"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="72"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="71">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="81"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="80"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="79"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="78"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="77"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="76"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="75"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="74"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="73"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="72">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="70"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="69"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="68"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="67"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="66"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="65"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="64"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="63"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="62"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="61">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="71"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="70"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="69"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="68"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="67"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="66"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="65"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="64"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="63"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="62"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="61"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="60"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="59"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="58"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="57"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="56"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="55">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="60"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="59"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="58"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="57"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="56"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="55"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="54"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="53"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="52"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="51"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="50"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="49"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="48"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="47"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="46"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="45"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="44">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="54">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="43">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="53"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="52"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="51"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="50">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="42"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="41"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="40"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="39">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="49"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="48"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="47"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="46"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="45"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="44"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="43"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="42"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="41"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="40"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="0"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="12"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="39"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="38"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="37"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="36"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="35"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="34"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="33"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="32"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="31"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="30"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="29"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="28"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="27"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="34"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="21"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="33"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="32"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="31">
+    <tableColumn id="10" name="[icon]" dataDxfId="20"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="19"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="18">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3925,11 +3925,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B33:I34"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="26"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" name="[superfuryMax]"/>
     <tableColumn id="9" name="[superFuryLengthModifier]"/>
@@ -3942,7 +3942,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B45:W57"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -3973,14 +3973,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B38:F41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="16"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="14"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="13"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4255,7 +4255,7 @@
   <dimension ref="B1:BS57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BE7" workbookViewId="0">
-      <selection activeCell="BQ28" sqref="BQ28"/>
+      <selection activeCell="BQ30" sqref="BQ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5750,11 +5750,11 @@
       <c r="BP20" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="BQ20" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="BR20" s="37" t="s">
-        <v>215</v>
+      <c r="BQ20" s="135">
+        <v>0.2</v>
+      </c>
+      <c r="BR20" s="136">
+        <v>1</v>
       </c>
       <c r="BS20" s="37" t="s">
         <v>9</v>
@@ -6168,11 +6168,11 @@
       <c r="BP22" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="BQ22" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="BR22" s="37" t="s">
-        <v>215</v>
+      <c r="BQ22" s="136">
+        <v>0.2</v>
+      </c>
+      <c r="BR22" s="136">
+        <v>1</v>
       </c>
       <c r="BS22" s="37" t="s">
         <v>11</v>
@@ -7229,11 +7229,11 @@
       <c r="BP27" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="BQ27" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="BR27" s="37" t="s">
-        <v>215</v>
+      <c r="BQ27" s="136">
+        <v>0.2</v>
+      </c>
+      <c r="BR27" s="136">
+        <v>1</v>
       </c>
       <c r="BS27" s="37" t="s">
         <v>197</v>
@@ -8384,37 +8384,37 @@
     <mergeCell ref="AH28:AI28"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS16:BS23 BS25:BS26">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS24">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS27">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP16:BR16">
-    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP20:BR20">
-    <cfRule type="duplicateValues" dxfId="3" priority="15"/>
+  <conditionalFormatting sqref="BP20 BR20">
+    <cfRule type="duplicateValues" dxfId="103" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP22:BR22">
-    <cfRule type="duplicateValues" dxfId="2" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP27:BR27">
-    <cfRule type="duplicateValues" dxfId="1" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="19"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">

</xml_diff>

<commit_message>
XL dragons, furyMax (score needed to start FR, increased from 20k to 60k)
Former-commit-id: b357b601c125839e0a0ae61b33b6742cab71c00c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1559,6 +1559,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1594,12 +1600,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4254,8 +4254,8 @@
   </sheetPr>
   <dimension ref="B1:BS57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE7" workbookViewId="0">
-      <selection activeCell="BQ30" sqref="BQ30"/>
+    <sheetView tabSelected="1" topLeftCell="X7" workbookViewId="0">
+      <selection activeCell="AG28" sqref="AG28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4499,10 +4499,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="124"/>
-      <c r="AP14" s="124"/>
-      <c r="AQ14" s="124"/>
-      <c r="AR14" s="124"/>
+      <c r="AO14" s="126"/>
+      <c r="AP14" s="126"/>
+      <c r="AQ14" s="126"/>
+      <c r="AR14" s="126"/>
     </row>
     <row r="15" spans="2:71" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
@@ -5750,10 +5750,10 @@
       <c r="BP20" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="BQ20" s="135">
+      <c r="BQ20" s="123">
         <v>0.2</v>
       </c>
-      <c r="BR20" s="136">
+      <c r="BR20" s="124">
         <v>1</v>
       </c>
       <c r="BS20" s="37" t="s">
@@ -6168,10 +6168,10 @@
       <c r="BP22" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="BQ22" s="136">
+      <c r="BQ22" s="124">
         <v>0.2</v>
       </c>
-      <c r="BR22" s="136">
+      <c r="BR22" s="124">
         <v>1</v>
       </c>
       <c r="BS22" s="37" t="s">
@@ -6697,7 +6697,7 @@
         <v>10</v>
       </c>
       <c r="AG25" s="29">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="AH25" s="59">
         <v>4</v>
@@ -6909,7 +6909,7 @@
         <v>10</v>
       </c>
       <c r="AG26" s="26">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="AH26" s="25">
         <v>5</v>
@@ -7122,7 +7122,7 @@
         <v>10</v>
       </c>
       <c r="AG27" s="26">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="AH27" s="120">
         <v>5</v>
@@ -7229,10 +7229,10 @@
       <c r="BP27" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="BQ27" s="136">
+      <c r="BQ27" s="124">
         <v>0.2</v>
       </c>
-      <c r="BR27" s="136">
+      <c r="BR27" s="124">
         <v>1</v>
       </c>
       <c r="BS27" s="37" t="s">
@@ -7247,55 +7247,55 @@
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
-      <c r="I28" s="125" t="s">
+      <c r="I28" s="127" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="126"/>
-      <c r="K28" s="126"/>
-      <c r="L28" s="127"/>
+      <c r="J28" s="128"/>
+      <c r="K28" s="128"/>
+      <c r="L28" s="129"/>
       <c r="M28" s="36"/>
-      <c r="N28" s="129" t="s">
+      <c r="N28" s="131" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="129"/>
-      <c r="P28" s="129"/>
-      <c r="Q28" s="129"/>
-      <c r="R28" s="129"/>
-      <c r="S28" s="130"/>
-      <c r="T28" s="128" t="s">
+      <c r="O28" s="131"/>
+      <c r="P28" s="131"/>
+      <c r="Q28" s="131"/>
+      <c r="R28" s="131"/>
+      <c r="S28" s="132"/>
+      <c r="T28" s="130" t="s">
         <v>72</v>
       </c>
-      <c r="U28" s="128"/>
+      <c r="U28" s="130"/>
       <c r="V28" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W28" s="131" t="s">
+      <c r="W28" s="133" t="s">
         <v>70</v>
       </c>
-      <c r="X28" s="131"/>
-      <c r="Y28" s="131"/>
-      <c r="Z28" s="131"/>
-      <c r="AA28" s="131"/>
-      <c r="AB28" s="132" t="s">
+      <c r="X28" s="133"/>
+      <c r="Y28" s="133"/>
+      <c r="Z28" s="133"/>
+      <c r="AA28" s="133"/>
+      <c r="AB28" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="AC28" s="132"/>
-      <c r="AD28" s="132"/>
-      <c r="AE28" s="132"/>
-      <c r="AF28" s="133"/>
-      <c r="AH28" s="134" t="s">
+      <c r="AC28" s="134"/>
+      <c r="AD28" s="134"/>
+      <c r="AE28" s="134"/>
+      <c r="AF28" s="135"/>
+      <c r="AH28" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="AI28" s="134"/>
-      <c r="BD28" s="123" t="s">
+      <c r="AI28" s="136"/>
+      <c r="BD28" s="125" t="s">
         <v>67</v>
       </c>
-      <c r="BE28" s="123"/>
-      <c r="BF28" s="123"/>
-      <c r="BG28" s="123"/>
-      <c r="BH28" s="123"/>
-      <c r="BI28" s="123"/>
-      <c r="BJ28" s="123"/>
+      <c r="BE28" s="125"/>
+      <c r="BF28" s="125"/>
+      <c r="BG28" s="125"/>
+      <c r="BH28" s="125"/>
+      <c r="BI28" s="125"/>
+      <c r="BJ28" s="125"/>
     </row>
     <row r="30" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:71" ht="23.25" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Titan and Goldheist, reduced size (1,1 to 1,05) when all letters collected)
Former-commit-id: e05c16e22a52877c442f2341221bbc01b4dbe321
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -4254,8 +4254,8 @@
   </sheetPr>
   <dimension ref="B1:BS57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X7" workbookViewId="0">
-      <selection activeCell="AG28" sqref="AG28"/>
+    <sheetView tabSelected="1" topLeftCell="AL7" workbookViewId="0">
+      <selection activeCell="AX28" sqref="AX28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4858,7 +4858,7 @@
         <v>1</v>
       </c>
       <c r="AX16" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY16" s="24">
         <v>0.55999999999999994</v>
@@ -5068,7 +5068,7 @@
         <v>1</v>
       </c>
       <c r="AX17" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY17" s="24">
         <v>0.7</v>
@@ -5276,7 +5276,7 @@
         <v>1</v>
       </c>
       <c r="AX18" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY18" s="24">
         <v>0.7</v>
@@ -5486,7 +5486,7 @@
         <v>1</v>
       </c>
       <c r="AX19" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY19" s="24">
         <v>0.7</v>
@@ -5694,7 +5694,7 @@
         <v>1</v>
       </c>
       <c r="AX20" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY20" s="24">
         <v>0.7</v>
@@ -5904,7 +5904,7 @@
         <v>1</v>
       </c>
       <c r="AX21" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY21" s="24">
         <v>0.7</v>
@@ -6112,7 +6112,7 @@
         <v>1</v>
       </c>
       <c r="AX22" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY22" s="24">
         <v>0.7</v>
@@ -6326,7 +6326,7 @@
         <v>1</v>
       </c>
       <c r="AX23" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY23" s="24">
         <v>0.7</v>
@@ -6537,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="AX24" s="95">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY24" s="95">
         <v>0.7</v>
@@ -6749,7 +6749,7 @@
         <v>1</v>
       </c>
       <c r="AX25" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY25" s="24">
         <v>0.7</v>
@@ -6942,7 +6942,7 @@
         <v>13</v>
       </c>
       <c r="AR26" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="AS26" s="24">
         <v>2</v>
@@ -6960,7 +6960,7 @@
         <v>1</v>
       </c>
       <c r="AX26" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY26" s="24">
         <v>0.75</v>
@@ -7155,7 +7155,7 @@
         <v>14</v>
       </c>
       <c r="AR27" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="AS27" s="24">
         <v>2</v>
@@ -7173,7 +7173,7 @@
         <v>1</v>
       </c>
       <c r="AX27" s="24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AY27" s="24">
         <v>0.75</v>

</xml_diff>

<commit_message>
Modified petScale (menu screen)
Former-commit-id: b237107544a090d872129f584a61bc6cf7cb58d6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -4255,7 +4255,7 @@
   <dimension ref="B1:BS57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AL7" workbookViewId="0">
-      <selection activeCell="AX28" sqref="AX28"/>
+      <selection activeCell="AX25" sqref="AX25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6329,7 +6329,7 @@
         <v>25</v>
       </c>
       <c r="AY23" s="24">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AZ23" s="24">
         <v>0.6</v>
@@ -6540,7 +6540,7 @@
         <v>25</v>
       </c>
       <c r="AY24" s="95">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AZ24" s="95">
         <v>0.6</v>
@@ -6752,7 +6752,7 @@
         <v>25</v>
       </c>
       <c r="AY25" s="24">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="AZ25" s="24">
         <v>0.6</v>
@@ -6963,7 +6963,7 @@
         <v>25</v>
       </c>
       <c r="AY26" s="24">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="AZ26" s="24">
         <v>0.6</v>
@@ -7176,7 +7176,7 @@
         <v>25</v>
       </c>
       <c r="AY27" s="24">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="AZ27" s="24">
         <v>0.6</v>

</xml_diff>

<commit_message>
Fix previous petScale commit
Former-commit-id: e87fee217a2ebe066b76a72041c80c3d43ad564b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -4255,7 +4255,7 @@
   <dimension ref="B1:BS57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AL7" workbookViewId="0">
-      <selection activeCell="AX25" sqref="AX25"/>
+      <selection activeCell="AZ28" sqref="AZ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6329,10 +6329,10 @@
         <v>25</v>
       </c>
       <c r="AY23" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ23" s="24">
         <v>0.5</v>
-      </c>
-      <c r="AZ23" s="24">
-        <v>0.6</v>
       </c>
       <c r="BA23" s="57" t="s">
         <v>86</v>
@@ -6540,10 +6540,10 @@
         <v>25</v>
       </c>
       <c r="AY24" s="95">
+        <v>0.7</v>
+      </c>
+      <c r="AZ24" s="95">
         <v>0.5</v>
-      </c>
-      <c r="AZ24" s="95">
-        <v>0.6</v>
       </c>
       <c r="BA24" s="99" t="s">
         <v>187</v>
@@ -6752,10 +6752,10 @@
         <v>25</v>
       </c>
       <c r="AY25" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="AZ25" s="24">
         <v>0.4</v>
-      </c>
-      <c r="AZ25" s="24">
-        <v>0.6</v>
       </c>
       <c r="BA25" s="57" t="s">
         <v>81</v>
@@ -6963,10 +6963,10 @@
         <v>25</v>
       </c>
       <c r="AY26" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="AZ26" s="24">
         <v>0.4</v>
-      </c>
-      <c r="AZ26" s="24">
-        <v>0.6</v>
       </c>
       <c r="BA26" s="43" t="s">
         <v>76</v>
@@ -7176,10 +7176,10 @@
         <v>25</v>
       </c>
       <c r="AY27" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="AZ27" s="24">
         <v>0.4</v>
-      </c>
-      <c r="AZ27" s="24">
-        <v>0.6</v>
       </c>
       <c r="BA27" s="43" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
Chinese dragon head animoji
Former-commit-id: 1f4735863d07ff274148dca09514c7e25c48293f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcampos/projects/HungryDragon/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B11280-D188-C644-8528-4097E7B5B0B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF5738A-F7AD-D846-A5E6-5C52D7861ADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37480" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37480" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="217">
   <si>
     <t>[sku]</t>
   </si>
@@ -673,6 +673,9 @@
   </si>
   <si>
     <t>[unlockFromDragon]</t>
+  </si>
+  <si>
+    <t>PF_DragonChineseAnimoji</t>
   </si>
 </sst>
 </file>
@@ -1590,6 +1593,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1625,245 +1637,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="113">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2993,6 +2772,120 @@
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -3878,6 +3771,116 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3892,105 +3895,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT27" totalsRowShown="0" headerRowDxfId="112" dataDxfId="110" headerRowBorderDxfId="111" tableBorderDxfId="109" totalsRowBorderDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT27" totalsRowShown="0" headerRowDxfId="101" dataDxfId="99" headerRowBorderDxfId="100" tableBorderDxfId="98" totalsRowBorderDxfId="97">
   <autoFilter ref="B15:BT27" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="71">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{dragonDefinitions}" dataDxfId="107"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="106"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[tier]" dataDxfId="105"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="[type]" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[order]" dataDxfId="103"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[previousDragonSku]" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[unlockPriceCoins]" dataDxfId="101"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[unlockPricePC]" dataDxfId="100"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[cameraDefaultZoom]" dataDxfId="99"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[cameraFarZoom]" dataDxfId="98"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[defaultSize]" dataDxfId="97"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[cameraFrameWidthModifier]" dataDxfId="96"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[healthMin]" dataDxfId="95"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[healthMax]" dataDxfId="94"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[healthDrain]" dataDxfId="93"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="[healthDrainSpacePlus]" dataDxfId="92"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[healthDrainAmpPerSecond]" dataDxfId="91"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[sessionStartHealthDrainTime]" dataDxfId="90"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[sessionStartHealthDrainModifier]" dataDxfId="89"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[scaleMin]" dataDxfId="88"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[scaleMax]" dataDxfId="87"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[speedBase]" dataDxfId="86"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[boostMultiplier]" dataDxfId="85"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[energyBaseMin]" dataDxfId="84"/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="[energyBaseMax]" dataDxfId="83">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{dragonDefinitions}" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="95"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[tier]" dataDxfId="94"/>
+    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="[type]" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[order]" dataDxfId="92"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[previousDragonSku]" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[unlockPriceCoins]" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[unlockPricePC]" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[cameraDefaultZoom]" dataDxfId="88"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[cameraFarZoom]" dataDxfId="87"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[defaultSize]" dataDxfId="86"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[cameraFrameWidthModifier]" dataDxfId="85"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[healthMin]" dataDxfId="84"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[healthMax]" dataDxfId="83"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[healthDrain]" dataDxfId="82"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="[healthDrainSpacePlus]" dataDxfId="81"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[healthDrainAmpPerSecond]" dataDxfId="80"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[sessionStartHealthDrainTime]" dataDxfId="79"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[sessionStartHealthDrainModifier]" dataDxfId="78"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[scaleMin]" dataDxfId="77"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[scaleMax]" dataDxfId="76"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[speedBase]" dataDxfId="75"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[boostMultiplier]" dataDxfId="74"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[energyBaseMin]" dataDxfId="73"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="[energyBaseMax]" dataDxfId="72">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[energyDrain]" dataDxfId="82"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[energyRefillRate]" dataDxfId="81"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[furyBaseDamage]" dataDxfId="80"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[furyBaseLength]" dataDxfId="79"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[furyScoreMultiplier]" dataDxfId="78"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[furyBaseDuration]" dataDxfId="77"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[furyMax]" dataDxfId="76"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="[scoreTextThresholdMultiplier]" dataDxfId="75"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[eatSpeedFactorMin]" dataDxfId="74"/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="[eatSpeedFactorMax]" dataDxfId="73">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[energyDrain]" dataDxfId="71"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[energyRefillRate]" dataDxfId="70"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[furyBaseDamage]" dataDxfId="69"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[furyBaseLength]" dataDxfId="68"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[furyScoreMultiplier]" dataDxfId="67"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[furyBaseDuration]" dataDxfId="66"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[furyMax]" dataDxfId="65"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="[scoreTextThresholdMultiplier]" dataDxfId="64"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[eatSpeedFactorMin]" dataDxfId="63"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="[eatSpeedFactorMax]" dataDxfId="62">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAlcohol]" dataDxfId="72"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[alcoholDrain]" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[gamePrefab]" dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[menuPrefab]" dataDxfId="69"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="[resultsPrefab]" dataDxfId="3"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="[shadowFromDragon]" dataDxfId="2"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="[revealFromDragon]" dataDxfId="0"/>
-    <tableColumn id="71" xr3:uid="{C1B678A3-BE4D-7A40-A6A9-6FBC1632467F}" name="[unlockFromDragon]" dataDxfId="1"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="[sizeUpMultiplier]" dataDxfId="68"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="[speedUpMultiplier]" dataDxfId="67"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="[biteUpMultiplier]" dataDxfId="66"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="[invincible]" dataDxfId="65"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="[infiniteBoost]" dataDxfId="64"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[eatEverything]" dataDxfId="63"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[modeDuration]" dataDxfId="62"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="[petScale]" dataDxfId="61"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="[petScaleMenu]" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="59">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAlcohol]" dataDxfId="61"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[alcoholDrain]" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[gamePrefab]" dataDxfId="59"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[menuPrefab]" dataDxfId="58"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="[resultsPrefab]" dataDxfId="57"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="[shadowFromDragon]" dataDxfId="56"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="[revealFromDragon]" dataDxfId="55"/>
+    <tableColumn id="71" xr3:uid="{C1B678A3-BE4D-7A40-A6A9-6FBC1632467F}" name="[unlockFromDragon]" dataDxfId="54"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="[sizeUpMultiplier]" dataDxfId="53"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="[speedUpMultiplier]" dataDxfId="52"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="[biteUpMultiplier]" dataDxfId="51"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="[invincible]" dataDxfId="50"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="[infiniteBoost]" dataDxfId="49"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[eatEverything]" dataDxfId="48"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[modeDuration]" dataDxfId="47"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="[petScale]" dataDxfId="46"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="[petScaleMenu]" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="44">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[tidDesc]" dataDxfId="58">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[tidDesc]" dataDxfId="43">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[statsBarRatio]" dataDxfId="57"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[furyBarRatio]" dataDxfId="56"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[forceMin]" dataDxfId="55"/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="[forceMax]" dataDxfId="54">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[statsBarRatio]" dataDxfId="42"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[furyBarRatio]" dataDxfId="41"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[forceMin]" dataDxfId="40"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="[forceMax]" dataDxfId="39">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[mass]" dataDxfId="53"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[friction]" dataDxfId="52"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[gravityModifier]" dataDxfId="51"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[airGravityModifier]" dataDxfId="50"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[waterGravityModifier]" dataDxfId="49"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="[damageAnimationThreshold]" dataDxfId="48"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="[dotAnimationThreshold]" dataDxfId="47"/>
-    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="[mummyHealthFactor]" dataDxfId="46"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="[mummyDuration]" dataDxfId="45"/>
-    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="[animojiPrefab]" dataDxfId="44"/>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="[energyRequiredToBoost]" dataDxfId="43"/>
-    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="[energyRestartThreshold]" dataDxfId="42"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="[trackingSku]" dataDxfId="41"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[mass]" dataDxfId="38"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[friction]" dataDxfId="37"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[gravityModifier]" dataDxfId="36"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[airGravityModifier]" dataDxfId="35"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[waterGravityModifier]" dataDxfId="34"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="[damageAnimationThreshold]" dataDxfId="33"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="[dotAnimationThreshold]" dataDxfId="32"/>
+    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="[mummyHealthFactor]" dataDxfId="31"/>
+    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="[mummyDuration]" dataDxfId="30"/>
+    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="[animojiPrefab]" dataDxfId="29"/>
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="[energyRequiredToBoost]" dataDxfId="28"/>
+    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="[energyRestartThreshold]" dataDxfId="27"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="[trackingSku]" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B4:G9" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{dragonTierDefinitions}" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{dragonTierDefinitions}" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="[order]"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[icon]" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[maxPetEquipped]" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="33">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[icon]" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[maxPetEquipped]" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="18">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3999,11 +4002,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B33:I34" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{dragonSettings}" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{dragonSettings}" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="12"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="[energyRequiredToBoost]"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="[superfuryMax]"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="[superFuryLengthModifier]"/>
@@ -4016,7 +4019,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B45:W57" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{dragonProgressionDefinitions}"/>
@@ -4047,14 +4050,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B38:F41" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{dragonHealthModifiersDefinitions}" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="[threshold]"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[modifier]" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="[tid]" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4328,8 +4331,8 @@
   </sheetPr>
   <dimension ref="B1:BT57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL7" workbookViewId="0">
-      <selection activeCell="AQ32" sqref="AQ32"/>
+    <sheetView tabSelected="1" topLeftCell="AW9" workbookViewId="0">
+      <selection activeCell="BQ21" sqref="BQ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4573,10 +4576,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="126"/>
-      <c r="AP14" s="126"/>
-      <c r="AQ14" s="126"/>
-      <c r="AR14" s="126"/>
+      <c r="AO14" s="129"/>
+      <c r="AP14" s="129"/>
+      <c r="AQ14" s="129"/>
+      <c r="AR14" s="129"/>
     </row>
     <row r="15" spans="2:72" ht="161" x14ac:dyDescent="0.2">
       <c r="B15" s="72" t="s">
@@ -4699,10 +4702,10 @@
       <c r="AO15" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="AP15" s="137" t="s">
+      <c r="AP15" s="125" t="s">
         <v>140</v>
       </c>
-      <c r="AQ15" s="137" t="s">
+      <c r="AQ15" s="125" t="s">
         <v>139</v>
       </c>
       <c r="AR15" s="79" t="s">
@@ -4914,8 +4917,8 @@
       <c r="AO16" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="AP16" s="138"/>
-      <c r="AQ16" s="138"/>
+      <c r="AP16" s="126"/>
+      <c r="AQ16" s="126"/>
       <c r="AR16" s="24"/>
       <c r="AS16" s="24">
         <v>4.0999999999999996</v>
@@ -5125,8 +5128,8 @@
       <c r="AO17" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="AP17" s="138"/>
-      <c r="AQ17" s="138"/>
+      <c r="AP17" s="126"/>
+      <c r="AQ17" s="126"/>
       <c r="AR17" s="24"/>
       <c r="AS17" s="24">
         <v>2.2999999999999998</v>
@@ -5334,8 +5337,8 @@
       <c r="AO18" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AP18" s="138"/>
-      <c r="AQ18" s="138"/>
+      <c r="AP18" s="126"/>
+      <c r="AQ18" s="126"/>
       <c r="AR18" s="24"/>
       <c r="AS18" s="24">
         <v>2.1</v>
@@ -5545,8 +5548,8 @@
       <c r="AO19" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="AP19" s="138"/>
-      <c r="AQ19" s="138"/>
+      <c r="AP19" s="126"/>
+      <c r="AQ19" s="126"/>
       <c r="AR19" s="24"/>
       <c r="AS19" s="24">
         <v>2.1</v>
@@ -5754,8 +5757,8 @@
       <c r="AO20" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="AP20" s="138"/>
-      <c r="AQ20" s="138"/>
+      <c r="AP20" s="126"/>
+      <c r="AQ20" s="126"/>
       <c r="AR20" s="24"/>
       <c r="AS20" s="24">
         <v>2.1</v>
@@ -5965,8 +5968,8 @@
       <c r="AO21" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AP21" s="138"/>
-      <c r="AQ21" s="138"/>
+      <c r="AP21" s="126"/>
+      <c r="AQ21" s="126"/>
       <c r="AR21" s="24"/>
       <c r="AS21" s="24">
         <v>2</v>
@@ -6040,7 +6043,9 @@
       <c r="BP21" s="70">
         <v>25</v>
       </c>
-      <c r="BQ21" s="122"/>
+      <c r="BQ21" s="122" t="s">
+        <v>216</v>
+      </c>
       <c r="BR21" s="122">
         <v>0.2</v>
       </c>
@@ -6174,8 +6179,8 @@
       <c r="AO22" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="AP22" s="138"/>
-      <c r="AQ22" s="138"/>
+      <c r="AP22" s="126"/>
+      <c r="AQ22" s="126"/>
       <c r="AR22" s="24"/>
       <c r="AS22" s="24">
         <v>1.6</v>
@@ -6385,9 +6390,9 @@
       <c r="AO23" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="AP23" s="138"/>
-      <c r="AQ23" s="138"/>
-      <c r="AR23" s="139" t="s">
+      <c r="AP23" s="126"/>
+      <c r="AQ23" s="126"/>
+      <c r="AR23" s="127" t="s">
         <v>11</v>
       </c>
       <c r="AS23" s="24">
@@ -6595,9 +6600,9 @@
       <c r="AO24" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="AP24" s="138"/>
-      <c r="AQ24" s="138"/>
-      <c r="AR24" s="139" t="s">
+      <c r="AP24" s="126"/>
+      <c r="AQ24" s="126"/>
+      <c r="AR24" s="127" t="s">
         <v>12</v>
       </c>
       <c r="AS24" s="95">
@@ -6806,9 +6811,9 @@
       <c r="AO25" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="AP25" s="138"/>
-      <c r="AQ25" s="138"/>
-      <c r="AR25" s="139" t="s">
+      <c r="AP25" s="126"/>
+      <c r="AQ25" s="126"/>
+      <c r="AR25" s="127" t="s">
         <v>184</v>
       </c>
       <c r="AS25" s="24">
@@ -7016,9 +7021,9 @@
       <c r="AO26" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AP26" s="138"/>
-      <c r="AQ26" s="138"/>
-      <c r="AR26" s="139" t="s">
+      <c r="AP26" s="126"/>
+      <c r="AQ26" s="126"/>
+      <c r="AR26" s="127" t="s">
         <v>13</v>
       </c>
       <c r="AS26" s="24">
@@ -7228,9 +7233,9 @@
       <c r="AO27" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="AP27" s="138"/>
-      <c r="AQ27" s="138"/>
-      <c r="AR27" s="139" t="s">
+      <c r="AP27" s="126"/>
+      <c r="AQ27" s="126"/>
+      <c r="AR27" s="127" t="s">
         <v>14</v>
       </c>
       <c r="AS27" s="24">
@@ -7326,55 +7331,55 @@
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
-      <c r="I28" s="127" t="s">
+      <c r="I28" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="128"/>
-      <c r="K28" s="128"/>
-      <c r="L28" s="129"/>
+      <c r="J28" s="131"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="132"/>
       <c r="M28" s="36"/>
-      <c r="N28" s="131" t="s">
+      <c r="N28" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="131"/>
-      <c r="P28" s="131"/>
-      <c r="Q28" s="131"/>
-      <c r="R28" s="131"/>
-      <c r="S28" s="132"/>
-      <c r="T28" s="130" t="s">
+      <c r="O28" s="134"/>
+      <c r="P28" s="134"/>
+      <c r="Q28" s="134"/>
+      <c r="R28" s="134"/>
+      <c r="S28" s="135"/>
+      <c r="T28" s="133" t="s">
         <v>72</v>
       </c>
-      <c r="U28" s="130"/>
+      <c r="U28" s="133"/>
       <c r="V28" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="W28" s="133" t="s">
+      <c r="W28" s="136" t="s">
         <v>70</v>
       </c>
-      <c r="X28" s="133"/>
-      <c r="Y28" s="133"/>
-      <c r="Z28" s="133"/>
-      <c r="AA28" s="133"/>
-      <c r="AB28" s="134" t="s">
+      <c r="X28" s="136"/>
+      <c r="Y28" s="136"/>
+      <c r="Z28" s="136"/>
+      <c r="AA28" s="136"/>
+      <c r="AB28" s="137" t="s">
         <v>69</v>
       </c>
-      <c r="AC28" s="134"/>
-      <c r="AD28" s="134"/>
-      <c r="AE28" s="134"/>
-      <c r="AF28" s="135"/>
-      <c r="AH28" s="136" t="s">
+      <c r="AC28" s="137"/>
+      <c r="AD28" s="137"/>
+      <c r="AE28" s="137"/>
+      <c r="AF28" s="138"/>
+      <c r="AH28" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="AI28" s="136"/>
-      <c r="BD28" s="125" t="s">
+      <c r="AI28" s="139"/>
+      <c r="BD28" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="BE28" s="125"/>
-      <c r="BF28" s="125"/>
-      <c r="BG28" s="125"/>
-      <c r="BH28" s="125"/>
-      <c r="BI28" s="125"/>
-      <c r="BJ28" s="125"/>
+      <c r="BE28" s="128"/>
+      <c r="BF28" s="128"/>
+      <c r="BG28" s="128"/>
+      <c r="BH28" s="128"/>
+      <c r="BI28" s="128"/>
+      <c r="BJ28" s="128"/>
     </row>
     <row r="30" spans="2:72" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:72" ht="24" x14ac:dyDescent="0.3">
@@ -8463,37 +8468,37 @@
     <mergeCell ref="AH28:AI28"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="14" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="7" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="6" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="5" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="4" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="19"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Results prefab for all dragons
Former-commit-id: 3025a8f2f62ca29bf47cf746b73a444f42bfd150
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="226">
   <si>
     <t>[sku]</t>
   </si>
@@ -675,6 +675,33 @@
   </si>
   <si>
     <t>PF_DragonChineseAnimoji</t>
+  </si>
+  <si>
+    <t>PF_DragonBabyResults</t>
+  </si>
+  <si>
+    <t>PF_DragonCrocodileResults</t>
+  </si>
+  <si>
+    <t>PF_DragonFatResults</t>
+  </si>
+  <si>
+    <t>PF_DragonBugResults</t>
+  </si>
+  <si>
+    <t>PF_DragonClassicResults</t>
+  </si>
+  <si>
+    <t>PF_DragonDevilResults</t>
+  </si>
+  <si>
+    <t>PF_DragonJawfreyResults</t>
+  </si>
+  <si>
+    <t>PF_DragonBalrogResults</t>
+  </si>
+  <si>
+    <t>PF_DragonTitanResults</t>
   </si>
 </sst>
 </file>
@@ -4328,8 +4355,8 @@
   </sheetPr>
   <dimension ref="B1:BT57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO10" workbookViewId="0">
-      <selection activeCell="AS17" sqref="AS17"/>
+    <sheetView tabSelected="1" topLeftCell="AF10" workbookViewId="0">
+      <selection activeCell="AO28" sqref="AO28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4912,7 +4939,7 @@
         <v>119</v>
       </c>
       <c r="AO16" s="24" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
       <c r="AP16" s="126"/>
       <c r="AQ16" s="126"/>
@@ -5123,7 +5150,7 @@
         <v>115</v>
       </c>
       <c r="AO17" s="24" t="s">
-        <v>115</v>
+        <v>218</v>
       </c>
       <c r="AP17" s="126"/>
       <c r="AQ17" s="126"/>
@@ -5543,7 +5570,7 @@
         <v>105</v>
       </c>
       <c r="AO19" s="24" t="s">
-        <v>105</v>
+        <v>219</v>
       </c>
       <c r="AP19" s="126"/>
       <c r="AQ19" s="126"/>
@@ -5752,7 +5779,7 @@
         <v>101</v>
       </c>
       <c r="AO20" s="24" t="s">
-        <v>101</v>
+        <v>220</v>
       </c>
       <c r="AP20" s="126"/>
       <c r="AQ20" s="126"/>
@@ -6174,7 +6201,7 @@
         <v>91</v>
       </c>
       <c r="AO22" s="24" t="s">
-        <v>91</v>
+        <v>221</v>
       </c>
       <c r="AP22" s="126"/>
       <c r="AQ22" s="126"/>
@@ -6385,7 +6412,7 @@
         <v>87</v>
       </c>
       <c r="AO23" s="24" t="s">
-        <v>87</v>
+        <v>222</v>
       </c>
       <c r="AP23" s="126"/>
       <c r="AQ23" s="126"/>
@@ -6595,7 +6622,7 @@
         <v>186</v>
       </c>
       <c r="AO24" s="95" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="AP24" s="126"/>
       <c r="AQ24" s="126"/>
@@ -6806,7 +6833,7 @@
         <v>82</v>
       </c>
       <c r="AO25" s="24" t="s">
-        <v>82</v>
+        <v>224</v>
       </c>
       <c r="AP25" s="126"/>
       <c r="AQ25" s="126"/>
@@ -7016,7 +7043,7 @@
         <v>77</v>
       </c>
       <c r="AO26" s="24" t="s">
-        <v>77</v>
+        <v>225</v>
       </c>
       <c r="AP26" s="126"/>
       <c r="AQ26" s="126"/>

</xml_diff>

<commit_message>
Fire Rush score needed reduced for: Devil, from 20k to 16k Balrog from 60k to 52k
Former-commit-id: 200eed7fa291dd1663c5effab0149d44afce1567
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4355,8 +4355,8 @@
   </sheetPr>
   <dimension ref="B1:BT57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF10" workbookViewId="0">
-      <selection activeCell="AO28" sqref="AO28"/>
+    <sheetView tabSelected="1" topLeftCell="W10" workbookViewId="0">
+      <selection activeCell="AG25" sqref="AG25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6387,7 +6387,7 @@
         <v>10</v>
       </c>
       <c r="AG23" s="29">
-        <v>20000</v>
+        <v>16000</v>
       </c>
       <c r="AH23" s="59">
         <v>4</v>
@@ -6808,7 +6808,7 @@
         <v>10</v>
       </c>
       <c r="AG25" s="29">
-        <v>60000</v>
+        <v>52000</v>
       </c>
       <c r="AH25" s="59">
         <v>4</v>

</xml_diff>

<commit_message>
Adding disguises to Dark dragon
Former-commit-id: c1b5542ff2c099a7c71e4a47f64c04efb7bda689
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="243">
   <si>
     <t>[sku]</t>
   </si>
@@ -759,7 +759,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,14 +836,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1349,7 +1341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1733,9 +1725,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1862,28 +1851,28 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1895,6 +1884,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1920,36 +1939,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4821,8 +4810,8 @@
   </sheetPr>
   <dimension ref="B1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="BV25" sqref="BV25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5085,10 +5074,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="208"/>
-      <c r="AP14" s="208"/>
-      <c r="AQ14" s="208"/>
-      <c r="AR14" s="208"/>
+      <c r="AO14" s="198"/>
+      <c r="AP14" s="198"/>
+      <c r="AQ14" s="198"/>
+      <c r="AR14" s="198"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -5196,10 +5185,10 @@
       <c r="AJ15" s="116" t="s">
         <v>194</v>
       </c>
-      <c r="AK15" s="184" t="s">
+      <c r="AK15" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="AL15" s="185" t="s">
+      <c r="AL15" s="184" t="s">
         <v>142</v>
       </c>
       <c r="AM15" s="74" t="s">
@@ -5410,19 +5399,19 @@
       <c r="AJ16" s="59">
         <v>0.19</v>
       </c>
-      <c r="AK16" s="186">
+      <c r="AK16" s="185">
         <v>0</v>
       </c>
-      <c r="AL16" s="187">
+      <c r="AL16" s="186">
         <v>12</v>
       </c>
-      <c r="AM16" s="179" t="s">
+      <c r="AM16" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="AN16" s="179" t="s">
+      <c r="AN16" s="178" t="s">
         <v>119</v>
       </c>
-      <c r="AO16" s="179" t="s">
+      <c r="AO16" s="178" t="s">
         <v>217</v>
       </c>
       <c r="AP16" s="109"/>
@@ -5500,7 +5489,7 @@
       <c r="BP16" s="64">
         <v>25</v>
       </c>
-      <c r="BQ16" s="171" t="s">
+      <c r="BQ16" s="170" t="s">
         <v>208</v>
       </c>
       <c r="BR16" s="52">
@@ -5509,7 +5498,7 @@
       <c r="BS16" s="52">
         <v>1</v>
       </c>
-      <c r="BT16" s="173" t="s">
+      <c r="BT16" s="172" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5620,19 +5609,19 @@
       <c r="AJ17" s="59">
         <v>0.15</v>
       </c>
-      <c r="AK17" s="186">
+      <c r="AK17" s="185">
         <v>0</v>
       </c>
-      <c r="AL17" s="187">
+      <c r="AL17" s="186">
         <v>12</v>
       </c>
-      <c r="AM17" s="181" t="s">
+      <c r="AM17" s="180" t="s">
         <v>116</v>
       </c>
-      <c r="AN17" s="179" t="s">
+      <c r="AN17" s="178" t="s">
         <v>115</v>
       </c>
-      <c r="AO17" s="179" t="s">
+      <c r="AO17" s="178" t="s">
         <v>218</v>
       </c>
       <c r="AP17" s="109"/>
@@ -5710,14 +5699,14 @@
       <c r="BP17" s="64">
         <v>25</v>
       </c>
-      <c r="BQ17" s="171"/>
+      <c r="BQ17" s="170"/>
       <c r="BR17" s="52">
         <v>0.2</v>
       </c>
       <c r="BS17" s="52">
         <v>1</v>
       </c>
-      <c r="BT17" s="173" t="s">
+      <c r="BT17" s="172" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5828,19 +5817,19 @@
       <c r="AJ18" s="59">
         <v>0.13</v>
       </c>
-      <c r="AK18" s="188">
+      <c r="AK18" s="187">
         <v>0</v>
       </c>
-      <c r="AL18" s="189">
+      <c r="AL18" s="188">
         <v>12</v>
       </c>
-      <c r="AM18" s="181" t="s">
+      <c r="AM18" s="180" t="s">
         <v>112</v>
       </c>
-      <c r="AN18" s="179" t="s">
+      <c r="AN18" s="178" t="s">
         <v>111</v>
       </c>
-      <c r="AO18" s="179" t="s">
+      <c r="AO18" s="178" t="s">
         <v>110</v>
       </c>
       <c r="AP18" s="109"/>
@@ -5918,7 +5907,7 @@
       <c r="BP18" s="64">
         <v>25</v>
       </c>
-      <c r="BQ18" s="171" t="s">
+      <c r="BQ18" s="170" t="s">
         <v>212</v>
       </c>
       <c r="BR18" s="52">
@@ -5927,7 +5916,7 @@
       <c r="BS18" s="52">
         <v>1</v>
       </c>
-      <c r="BT18" s="174" t="s">
+      <c r="BT18" s="173" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6038,19 +6027,19 @@
       <c r="AJ19" s="59">
         <v>0.11</v>
       </c>
-      <c r="AK19" s="186">
+      <c r="AK19" s="185">
         <v>0</v>
       </c>
-      <c r="AL19" s="187">
+      <c r="AL19" s="186">
         <v>12</v>
       </c>
-      <c r="AM19" s="181" t="s">
+      <c r="AM19" s="180" t="s">
         <v>106</v>
       </c>
-      <c r="AN19" s="179" t="s">
+      <c r="AN19" s="178" t="s">
         <v>105</v>
       </c>
-      <c r="AO19" s="179" t="s">
+      <c r="AO19" s="178" t="s">
         <v>219</v>
       </c>
       <c r="AP19" s="109"/>
@@ -6128,14 +6117,14 @@
       <c r="BP19" s="64">
         <v>25</v>
       </c>
-      <c r="BQ19" s="171"/>
+      <c r="BQ19" s="170"/>
       <c r="BR19" s="52">
         <v>0.2</v>
       </c>
       <c r="BS19" s="52">
         <v>1</v>
       </c>
-      <c r="BT19" s="174" t="s">
+      <c r="BT19" s="173" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6246,19 +6235,19 @@
       <c r="AJ20" s="59">
         <v>0.09</v>
       </c>
-      <c r="AK20" s="186">
+      <c r="AK20" s="185">
         <v>0</v>
       </c>
-      <c r="AL20" s="187">
+      <c r="AL20" s="186">
         <v>12</v>
       </c>
-      <c r="AM20" s="181" t="s">
+      <c r="AM20" s="180" t="s">
         <v>102</v>
       </c>
-      <c r="AN20" s="179" t="s">
+      <c r="AN20" s="178" t="s">
         <v>101</v>
       </c>
-      <c r="AO20" s="179" t="s">
+      <c r="AO20" s="178" t="s">
         <v>220</v>
       </c>
       <c r="AP20" s="109"/>
@@ -6336,16 +6325,16 @@
       <c r="BP20" s="64">
         <v>25</v>
       </c>
-      <c r="BQ20" s="172" t="s">
+      <c r="BQ20" s="171" t="s">
         <v>209</v>
       </c>
-      <c r="BR20" s="169">
+      <c r="BR20" s="168">
         <v>0.2</v>
       </c>
-      <c r="BS20" s="169">
+      <c r="BS20" s="168">
         <v>1</v>
       </c>
-      <c r="BT20" s="174" t="s">
+      <c r="BT20" s="173" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6456,19 +6445,19 @@
       <c r="AJ21" s="59">
         <v>0.08</v>
       </c>
-      <c r="AK21" s="186">
+      <c r="AK21" s="185">
         <v>0</v>
       </c>
-      <c r="AL21" s="187">
+      <c r="AL21" s="186">
         <v>12</v>
       </c>
-      <c r="AM21" s="181" t="s">
+      <c r="AM21" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="AN21" s="179" t="s">
+      <c r="AN21" s="178" t="s">
         <v>97</v>
       </c>
-      <c r="AO21" s="179" t="s">
+      <c r="AO21" s="178" t="s">
         <v>96</v>
       </c>
       <c r="AP21" s="109"/>
@@ -6546,7 +6535,7 @@
       <c r="BP21" s="64">
         <v>25</v>
       </c>
-      <c r="BQ21" s="171" t="s">
+      <c r="BQ21" s="170" t="s">
         <v>216</v>
       </c>
       <c r="BR21" s="52">
@@ -6555,7 +6544,7 @@
       <c r="BS21" s="52">
         <v>1</v>
       </c>
-      <c r="BT21" s="174" t="s">
+      <c r="BT21" s="173" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6666,19 +6655,19 @@
       <c r="AJ22" s="59">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK22" s="186">
+      <c r="AK22" s="185">
         <v>0</v>
       </c>
-      <c r="AL22" s="187">
+      <c r="AL22" s="186">
         <v>12</v>
       </c>
-      <c r="AM22" s="181" t="s">
+      <c r="AM22" s="180" t="s">
         <v>92</v>
       </c>
-      <c r="AN22" s="179" t="s">
+      <c r="AN22" s="178" t="s">
         <v>91</v>
       </c>
-      <c r="AO22" s="179" t="s">
+      <c r="AO22" s="178" t="s">
         <v>221</v>
       </c>
       <c r="AP22" s="109"/>
@@ -6756,16 +6745,16 @@
       <c r="BP22" s="64">
         <v>25</v>
       </c>
-      <c r="BQ22" s="172" t="s">
+      <c r="BQ22" s="171" t="s">
         <v>210</v>
       </c>
-      <c r="BR22" s="169">
+      <c r="BR22" s="168">
         <v>0.2</v>
       </c>
-      <c r="BS22" s="169">
+      <c r="BS22" s="168">
         <v>1</v>
       </c>
-      <c r="BT22" s="174" t="s">
+      <c r="BT22" s="173" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6876,24 +6865,24 @@
       <c r="AJ23" s="59">
         <v>0.06</v>
       </c>
-      <c r="AK23" s="188">
+      <c r="AK23" s="187">
         <v>0</v>
       </c>
-      <c r="AL23" s="189">
+      <c r="AL23" s="188">
         <v>12</v>
       </c>
-      <c r="AM23" s="181" t="s">
+      <c r="AM23" s="180" t="s">
         <v>88</v>
       </c>
-      <c r="AN23" s="179" t="s">
+      <c r="AN23" s="178" t="s">
         <v>87</v>
       </c>
-      <c r="AO23" s="179" t="s">
+      <c r="AO23" s="178" t="s">
         <v>222</v>
       </c>
       <c r="AP23" s="109"/>
       <c r="AQ23" s="109"/>
-      <c r="AR23" s="177" t="s">
+      <c r="AR23" s="176" t="s">
         <v>11</v>
       </c>
       <c r="AS23" s="41">
@@ -6968,14 +6957,14 @@
       <c r="BP23" s="64">
         <v>25</v>
       </c>
-      <c r="BQ23" s="171"/>
+      <c r="BQ23" s="170"/>
       <c r="BR23" s="52">
         <v>0.2</v>
       </c>
       <c r="BS23" s="52">
         <v>1</v>
       </c>
-      <c r="BT23" s="174" t="s">
+      <c r="BT23" s="173" t="s">
         <v>12</v>
       </c>
     </row>
@@ -7086,24 +7075,24 @@
       <c r="AJ24" s="103">
         <v>0.05</v>
       </c>
-      <c r="AK24" s="188">
+      <c r="AK24" s="187">
         <v>0</v>
       </c>
-      <c r="AL24" s="189">
+      <c r="AL24" s="188">
         <v>12</v>
       </c>
-      <c r="AM24" s="182" t="s">
+      <c r="AM24" s="181" t="s">
         <v>185</v>
       </c>
-      <c r="AN24" s="180" t="s">
+      <c r="AN24" s="179" t="s">
         <v>186</v>
       </c>
-      <c r="AO24" s="180" t="s">
+      <c r="AO24" s="179" t="s">
         <v>223</v>
       </c>
       <c r="AP24" s="109"/>
       <c r="AQ24" s="109"/>
-      <c r="AR24" s="177" t="s">
+      <c r="AR24" s="176" t="s">
         <v>12</v>
       </c>
       <c r="AS24" s="89">
@@ -7178,14 +7167,14 @@
       <c r="BP24" s="64">
         <v>25</v>
       </c>
-      <c r="BQ24" s="171"/>
+      <c r="BQ24" s="170"/>
       <c r="BR24" s="52">
         <v>0.2</v>
       </c>
       <c r="BS24" s="52">
         <v>1</v>
       </c>
-      <c r="BT24" s="175" t="s">
+      <c r="BT24" s="174" t="s">
         <v>184</v>
       </c>
     </row>
@@ -7296,24 +7285,24 @@
       <c r="AJ25" s="59">
         <v>0.05</v>
       </c>
-      <c r="AK25" s="188">
+      <c r="AK25" s="187">
         <v>0</v>
       </c>
-      <c r="AL25" s="189">
+      <c r="AL25" s="188">
         <v>12</v>
       </c>
-      <c r="AM25" s="181" t="s">
+      <c r="AM25" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="AN25" s="179" t="s">
+      <c r="AN25" s="178" t="s">
         <v>82</v>
       </c>
-      <c r="AO25" s="179" t="s">
+      <c r="AO25" s="178" t="s">
         <v>224</v>
       </c>
       <c r="AP25" s="109"/>
       <c r="AQ25" s="109"/>
-      <c r="AR25" s="177" t="s">
+      <c r="AR25" s="176" t="s">
         <v>184</v>
       </c>
       <c r="AS25" s="41">
@@ -7388,14 +7377,14 @@
       <c r="BP25" s="64">
         <v>25</v>
       </c>
-      <c r="BQ25" s="171"/>
+      <c r="BQ25" s="170"/>
       <c r="BR25" s="52">
         <v>0.2</v>
       </c>
       <c r="BS25" s="52">
         <v>1</v>
       </c>
-      <c r="BT25" s="174" t="s">
+      <c r="BT25" s="173" t="s">
         <v>13</v>
       </c>
     </row>
@@ -7506,24 +7495,24 @@
       <c r="AJ26" s="59">
         <v>0.04</v>
       </c>
-      <c r="AK26" s="186">
+      <c r="AK26" s="185">
         <v>0</v>
       </c>
-      <c r="AL26" s="187">
+      <c r="AL26" s="186">
         <v>12</v>
       </c>
-      <c r="AM26" s="181" t="s">
+      <c r="AM26" s="180" t="s">
         <v>78</v>
       </c>
-      <c r="AN26" s="179" t="s">
+      <c r="AN26" s="178" t="s">
         <v>77</v>
       </c>
-      <c r="AO26" s="179" t="s">
+      <c r="AO26" s="178" t="s">
         <v>225</v>
       </c>
       <c r="AP26" s="109"/>
       <c r="AQ26" s="109"/>
-      <c r="AR26" s="177" t="s">
+      <c r="AR26" s="176" t="s">
         <v>13</v>
       </c>
       <c r="AS26" s="41">
@@ -7598,7 +7587,7 @@
       <c r="BP26" s="64">
         <v>25</v>
       </c>
-      <c r="BQ26" s="171" t="s">
+      <c r="BQ26" s="170" t="s">
         <v>213</v>
       </c>
       <c r="BR26" s="52">
@@ -7607,7 +7596,7 @@
       <c r="BS26" s="52">
         <v>1</v>
       </c>
-      <c r="BT26" s="174" t="s">
+      <c r="BT26" s="173" t="s">
         <v>14</v>
       </c>
     </row>
@@ -7615,10 +7604,10 @@
       <c r="B27" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="168" t="s">
+      <c r="C27" s="167" t="s">
         <v>197</v>
       </c>
-      <c r="D27" s="168" t="s">
+      <c r="D27" s="167" t="s">
         <v>79</v>
       </c>
       <c r="E27" s="52" t="s">
@@ -7718,24 +7707,24 @@
       <c r="AJ27" s="54">
         <v>0.04</v>
       </c>
-      <c r="AK27" s="190">
+      <c r="AK27" s="189">
         <v>0</v>
       </c>
-      <c r="AL27" s="191">
+      <c r="AL27" s="190">
         <v>12</v>
       </c>
-      <c r="AM27" s="181" t="s">
+      <c r="AM27" s="180" t="s">
         <v>200</v>
       </c>
-      <c r="AN27" s="179" t="s">
+      <c r="AN27" s="178" t="s">
         <v>201</v>
       </c>
-      <c r="AO27" s="179" t="s">
+      <c r="AO27" s="178" t="s">
         <v>202</v>
       </c>
       <c r="AP27" s="109"/>
       <c r="AQ27" s="109"/>
-      <c r="AR27" s="177" t="s">
+      <c r="AR27" s="176" t="s">
         <v>14</v>
       </c>
       <c r="AS27" s="41">
@@ -7810,7 +7799,7 @@
       <c r="BP27" s="64">
         <v>25</v>
       </c>
-      <c r="BQ27" s="172" t="s">
+      <c r="BQ27" s="171" t="s">
         <v>211</v>
       </c>
       <c r="BR27" s="52">
@@ -7819,216 +7808,218 @@
       <c r="BS27" s="52">
         <v>1</v>
       </c>
-      <c r="BT27" s="174" t="s">
+      <c r="BT27" s="173" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="28" spans="2:72" x14ac:dyDescent="0.25">
-      <c r="B28" s="141"/>
-      <c r="C28" s="142" t="s">
+      <c r="B28" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="141" t="s">
         <v>236</v>
       </c>
-      <c r="D28" s="170" t="s">
+      <c r="D28" s="169" t="s">
         <v>235</v>
       </c>
-      <c r="E28" s="143" t="s">
+      <c r="E28" s="142" t="s">
         <v>204</v>
       </c>
-      <c r="F28" s="144">
+      <c r="F28" s="143">
         <v>12</v>
       </c>
-      <c r="G28" s="144" t="s">
+      <c r="G28" s="143" t="s">
         <v>197</v>
       </c>
-      <c r="H28" s="145">
+      <c r="H28" s="144">
         <v>5000000</v>
       </c>
-      <c r="I28" s="146">
+      <c r="I28" s="145">
         <v>1200</v>
       </c>
-      <c r="J28" s="147">
+      <c r="J28" s="146">
         <v>35</v>
       </c>
-      <c r="K28" s="148">
+      <c r="K28" s="147">
         <v>45</v>
       </c>
-      <c r="L28" s="148">
+      <c r="L28" s="147">
         <v>25</v>
       </c>
-      <c r="M28" s="149">
+      <c r="M28" s="148">
         <v>0</v>
       </c>
-      <c r="N28" s="150">
+      <c r="N28" s="149">
         <v>500</v>
       </c>
-      <c r="O28" s="151">
+      <c r="O28" s="150">
         <v>600</v>
       </c>
-      <c r="P28" s="148">
+      <c r="P28" s="147">
         <v>2.5</v>
       </c>
-      <c r="Q28" s="152">
+      <c r="Q28" s="151">
         <v>0</v>
       </c>
-      <c r="R28" s="192">
+      <c r="R28" s="191">
         <v>0.02</v>
       </c>
-      <c r="S28" s="152">
+      <c r="S28" s="151">
         <v>20</v>
       </c>
-      <c r="T28" s="152">
+      <c r="T28" s="151">
         <v>0.8</v>
       </c>
-      <c r="U28" s="150">
+      <c r="U28" s="149">
         <v>2</v>
       </c>
-      <c r="V28" s="153">
+      <c r="V28" s="152">
         <v>2.1</v>
       </c>
-      <c r="W28" s="150">
+      <c r="W28" s="149">
         <v>31</v>
       </c>
-      <c r="X28" s="150">
+      <c r="X28" s="149">
         <v>2.0099999999999998</v>
       </c>
-      <c r="Y28" s="152">
+      <c r="Y28" s="151">
         <v>100</v>
       </c>
-      <c r="Z28" s="151">
+      <c r="Z28" s="150">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA28" s="152">
+      <c r="AA28" s="151">
         <v>20</v>
       </c>
-      <c r="AB28" s="152">
+      <c r="AB28" s="151">
         <v>14</v>
       </c>
-      <c r="AC28" s="150">
+      <c r="AC28" s="149">
         <v>475</v>
       </c>
-      <c r="AD28" s="152">
+      <c r="AD28" s="151">
         <v>12</v>
       </c>
-      <c r="AE28" s="152">
+      <c r="AE28" s="151">
         <v>7</v>
       </c>
-      <c r="AF28" s="152">
+      <c r="AF28" s="151">
         <v>10</v>
       </c>
-      <c r="AG28" s="152">
+      <c r="AG28" s="151">
         <v>65000</v>
       </c>
-      <c r="AH28" s="165">
+      <c r="AH28" s="164">
         <v>6</v>
       </c>
-      <c r="AI28" s="150">
+      <c r="AI28" s="149">
         <v>0.04</v>
       </c>
-      <c r="AJ28" s="154">
+      <c r="AJ28" s="153">
         <v>0.03</v>
       </c>
-      <c r="AK28" s="150">
+      <c r="AK28" s="149">
         <v>0</v>
       </c>
-      <c r="AL28" s="152">
+      <c r="AL28" s="151">
         <v>12</v>
       </c>
-      <c r="AM28" s="183" t="s">
+      <c r="AM28" s="182" t="s">
         <v>237</v>
       </c>
-      <c r="AN28" s="178" t="s">
+      <c r="AN28" s="177" t="s">
         <v>238</v>
       </c>
-      <c r="AO28" s="178" t="s">
+      <c r="AO28" s="177" t="s">
         <v>239</v>
       </c>
-      <c r="AP28" s="156"/>
-      <c r="AQ28" s="156"/>
-      <c r="AR28" s="178" t="s">
+      <c r="AP28" s="155"/>
+      <c r="AQ28" s="155"/>
+      <c r="AR28" s="177" t="s">
         <v>197</v>
       </c>
-      <c r="AS28" s="155">
+      <c r="AS28" s="154">
         <v>1.05</v>
       </c>
-      <c r="AT28" s="156">
+      <c r="AT28" s="155">
         <v>2</v>
       </c>
-      <c r="AU28" s="156">
+      <c r="AU28" s="155">
         <v>2</v>
       </c>
-      <c r="AV28" s="156" t="b">
+      <c r="AV28" s="155" t="b">
         <v>1</v>
       </c>
-      <c r="AW28" s="156" t="b">
+      <c r="AW28" s="155" t="b">
         <v>1</v>
       </c>
-      <c r="AX28" s="156" t="b">
+      <c r="AX28" s="155" t="b">
         <v>1</v>
       </c>
-      <c r="AY28" s="157">
+      <c r="AY28" s="156">
         <v>25</v>
       </c>
-      <c r="AZ28" s="156">
+      <c r="AZ28" s="155">
         <v>0.75</v>
       </c>
-      <c r="BA28" s="156">
+      <c r="BA28" s="155">
         <v>0.4</v>
       </c>
-      <c r="BB28" s="158" t="s">
+      <c r="BB28" s="157" t="s">
         <v>240</v>
       </c>
-      <c r="BC28" s="159" t="s">
+      <c r="BC28" s="158" t="s">
         <v>241</v>
       </c>
-      <c r="BD28" s="160">
+      <c r="BD28" s="159">
         <v>1.5E-3</v>
       </c>
-      <c r="BE28" s="144">
+      <c r="BE28" s="143">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF28" s="161">
+      <c r="BF28" s="160">
         <v>700</v>
       </c>
-      <c r="BG28" s="162">
+      <c r="BG28" s="161">
         <f>dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
         <v>750</v>
       </c>
-      <c r="BH28" s="163">
+      <c r="BH28" s="162">
         <v>4.9000000000000004</v>
       </c>
-      <c r="BI28" s="163">
+      <c r="BI28" s="162">
         <v>9.5</v>
       </c>
-      <c r="BJ28" s="163">
+      <c r="BJ28" s="162">
         <v>1.7</v>
       </c>
-      <c r="BK28" s="163">
+      <c r="BK28" s="162">
         <v>0.7</v>
       </c>
-      <c r="BL28" s="163">
+      <c r="BL28" s="162">
         <v>1.03</v>
       </c>
-      <c r="BM28" s="161">
+      <c r="BM28" s="160">
         <v>59</v>
       </c>
-      <c r="BN28" s="163">
+      <c r="BN28" s="162">
         <v>15</v>
       </c>
-      <c r="BO28" s="163">
+      <c r="BO28" s="162">
         <v>0.4</v>
       </c>
-      <c r="BP28" s="163">
+      <c r="BP28" s="162">
         <v>25</v>
       </c>
-      <c r="BQ28" s="164"/>
-      <c r="BR28" s="166">
+      <c r="BQ28" s="163"/>
+      <c r="BR28" s="165">
         <v>0.2</v>
       </c>
-      <c r="BS28" s="167">
+      <c r="BS28" s="166">
         <v>1</v>
       </c>
-      <c r="BT28" s="176" t="s">
+      <c r="BT28" s="175" t="s">
         <v>236</v>
       </c>
     </row>
@@ -8040,76 +8031,76 @@
       <c r="F29" s="33"/>
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
-      <c r="J29" s="203" t="s">
+      <c r="J29" s="212" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="203"/>
-      <c r="L29" s="203"/>
-      <c r="M29" s="203"/>
-      <c r="N29" s="201" t="s">
+      <c r="K29" s="212"/>
+      <c r="L29" s="212"/>
+      <c r="M29" s="212"/>
+      <c r="N29" s="210" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="202"/>
-      <c r="P29" s="202"/>
-      <c r="Q29" s="202"/>
-      <c r="R29" s="202"/>
-      <c r="S29" s="202"/>
-      <c r="T29" s="202"/>
-      <c r="U29" s="199" t="s">
+      <c r="O29" s="211"/>
+      <c r="P29" s="211"/>
+      <c r="Q29" s="211"/>
+      <c r="R29" s="211"/>
+      <c r="S29" s="211"/>
+      <c r="T29" s="211"/>
+      <c r="U29" s="208" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="200"/>
+      <c r="V29" s="209"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="196" t="s">
+      <c r="X29" s="205" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="197"/>
-      <c r="Z29" s="197"/>
-      <c r="AA29" s="197"/>
-      <c r="AB29" s="198"/>
-      <c r="AC29" s="195" t="s">
+      <c r="Y29" s="206"/>
+      <c r="Z29" s="206"/>
+      <c r="AA29" s="206"/>
+      <c r="AB29" s="207"/>
+      <c r="AC29" s="204" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="195"/>
-      <c r="AE29" s="195"/>
-      <c r="AF29" s="195"/>
-      <c r="AG29" s="195"/>
-      <c r="AI29" s="210" t="s">
+      <c r="AD29" s="204"/>
+      <c r="AE29" s="204"/>
+      <c r="AF29" s="204"/>
+      <c r="AG29" s="204"/>
+      <c r="AI29" s="200" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="210"/>
-      <c r="AK29" s="204" t="s">
+      <c r="AJ29" s="200"/>
+      <c r="AK29" s="194" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="204"/>
-      <c r="AM29" s="211" t="s">
+      <c r="AL29" s="194"/>
+      <c r="AM29" s="201" t="s">
         <v>242</v>
       </c>
-      <c r="AN29" s="212"/>
-      <c r="AO29" s="212"/>
-      <c r="AP29" s="212"/>
-      <c r="AQ29" s="212"/>
-      <c r="AR29" s="213"/>
-      <c r="AS29" s="205" t="s">
+      <c r="AN29" s="202"/>
+      <c r="AO29" s="202"/>
+      <c r="AP29" s="202"/>
+      <c r="AQ29" s="202"/>
+      <c r="AR29" s="203"/>
+      <c r="AS29" s="195" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="206"/>
-      <c r="AU29" s="206"/>
-      <c r="AV29" s="206"/>
-      <c r="AW29" s="206"/>
-      <c r="AX29" s="206"/>
-      <c r="AY29" s="207"/>
-      <c r="BF29" s="209" t="s">
+      <c r="AT29" s="196"/>
+      <c r="AU29" s="196"/>
+      <c r="AV29" s="196"/>
+      <c r="AW29" s="196"/>
+      <c r="AX29" s="196"/>
+      <c r="AY29" s="197"/>
+      <c r="BF29" s="199" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="209"/>
-      <c r="BH29" s="209"/>
-      <c r="BI29" s="209"/>
-      <c r="BJ29" s="209"/>
-      <c r="BK29" s="209"/>
-      <c r="BL29" s="209"/>
+      <c r="BG29" s="199"/>
+      <c r="BH29" s="199"/>
+      <c r="BI29" s="199"/>
+      <c r="BJ29" s="199"/>
+      <c r="BK29" s="199"/>
+      <c r="BL29" s="199"/>
     </row>
     <row r="31" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:72" ht="23.25" x14ac:dyDescent="0.35">
@@ -9193,77 +9184,77 @@
       <c r="D59">
         <v>20</v>
       </c>
-      <c r="E59" s="193">
+      <c r="E59" s="192">
         <v>4571</v>
       </c>
-      <c r="F59" s="194">
+      <c r="F59" s="193">
         <v>13714</v>
       </c>
-      <c r="G59" s="194">
+      <c r="G59" s="193">
         <v>27428</v>
       </c>
-      <c r="H59" s="194">
+      <c r="H59" s="193">
         <v>45713</v>
       </c>
-      <c r="I59" s="194">
+      <c r="I59" s="193">
         <v>68569</v>
       </c>
-      <c r="J59" s="194">
+      <c r="J59" s="193">
         <v>95997</v>
       </c>
-      <c r="K59" s="194">
+      <c r="K59" s="193">
         <v>127995</v>
       </c>
-      <c r="L59" s="194">
+      <c r="L59" s="193">
         <v>164565</v>
       </c>
-      <c r="M59" s="194">
+      <c r="M59" s="193">
         <v>205707</v>
       </c>
-      <c r="N59" s="194">
+      <c r="N59" s="193">
         <v>251419</v>
       </c>
-      <c r="O59" s="194">
+      <c r="O59" s="193">
         <v>301703</v>
       </c>
-      <c r="P59" s="194">
+      <c r="P59" s="193">
         <v>356559</v>
       </c>
-      <c r="Q59" s="194">
+      <c r="Q59" s="193">
         <v>415985</v>
       </c>
-      <c r="R59" s="194">
+      <c r="R59" s="193">
         <v>479983</v>
       </c>
-      <c r="S59" s="194">
+      <c r="S59" s="193">
         <v>548552</v>
       </c>
-      <c r="T59" s="194">
+      <c r="T59" s="193">
         <v>621692</v>
       </c>
-      <c r="U59" s="194">
+      <c r="U59" s="193">
         <v>699403</v>
       </c>
-      <c r="V59" s="194">
+      <c r="V59" s="193">
         <v>781686</v>
       </c>
-      <c r="W59" s="194">
+      <c r="W59" s="193">
         <v>868540</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="117" priority="10"/>

</xml_diff>

<commit_message>
Dragon Baby progression shorter from lv. 5
Former-commit-id: 9a25995750aa07d904f194f30bb4a18d8fff662e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1884,6 +1884,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1912,33 +1939,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4810,8 +4810,8 @@
   </sheetPr>
   <dimension ref="B1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5074,10 +5074,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="198"/>
-      <c r="AP14" s="198"/>
-      <c r="AQ14" s="198"/>
-      <c r="AR14" s="198"/>
+      <c r="AO14" s="207"/>
+      <c r="AP14" s="207"/>
+      <c r="AQ14" s="207"/>
+      <c r="AR14" s="207"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -5388,7 +5388,7 @@
         <v>8</v>
       </c>
       <c r="AG16" s="28">
-        <v>3000</v>
+        <v>2700</v>
       </c>
       <c r="AH16" s="112">
         <v>1</v>
@@ -8031,76 +8031,76 @@
       <c r="F29" s="33"/>
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
-      <c r="J29" s="212" t="s">
+      <c r="J29" s="202" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="212"/>
-      <c r="L29" s="212"/>
-      <c r="M29" s="212"/>
-      <c r="N29" s="210" t="s">
+      <c r="K29" s="202"/>
+      <c r="L29" s="202"/>
+      <c r="M29" s="202"/>
+      <c r="N29" s="200" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="211"/>
-      <c r="P29" s="211"/>
-      <c r="Q29" s="211"/>
-      <c r="R29" s="211"/>
-      <c r="S29" s="211"/>
-      <c r="T29" s="211"/>
-      <c r="U29" s="208" t="s">
+      <c r="O29" s="201"/>
+      <c r="P29" s="201"/>
+      <c r="Q29" s="201"/>
+      <c r="R29" s="201"/>
+      <c r="S29" s="201"/>
+      <c r="T29" s="201"/>
+      <c r="U29" s="198" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="209"/>
+      <c r="V29" s="199"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="205" t="s">
+      <c r="X29" s="195" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="206"/>
-      <c r="Z29" s="206"/>
-      <c r="AA29" s="206"/>
-      <c r="AB29" s="207"/>
-      <c r="AC29" s="204" t="s">
+      <c r="Y29" s="196"/>
+      <c r="Z29" s="196"/>
+      <c r="AA29" s="196"/>
+      <c r="AB29" s="197"/>
+      <c r="AC29" s="194" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="204"/>
-      <c r="AE29" s="204"/>
-      <c r="AF29" s="204"/>
-      <c r="AG29" s="204"/>
-      <c r="AI29" s="200" t="s">
+      <c r="AD29" s="194"/>
+      <c r="AE29" s="194"/>
+      <c r="AF29" s="194"/>
+      <c r="AG29" s="194"/>
+      <c r="AI29" s="209" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="200"/>
-      <c r="AK29" s="194" t="s">
+      <c r="AJ29" s="209"/>
+      <c r="AK29" s="203" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="194"/>
-      <c r="AM29" s="201" t="s">
+      <c r="AL29" s="203"/>
+      <c r="AM29" s="210" t="s">
         <v>242</v>
       </c>
-      <c r="AN29" s="202"/>
-      <c r="AO29" s="202"/>
-      <c r="AP29" s="202"/>
-      <c r="AQ29" s="202"/>
-      <c r="AR29" s="203"/>
-      <c r="AS29" s="195" t="s">
+      <c r="AN29" s="211"/>
+      <c r="AO29" s="211"/>
+      <c r="AP29" s="211"/>
+      <c r="AQ29" s="211"/>
+      <c r="AR29" s="212"/>
+      <c r="AS29" s="204" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="196"/>
-      <c r="AU29" s="196"/>
-      <c r="AV29" s="196"/>
-      <c r="AW29" s="196"/>
-      <c r="AX29" s="196"/>
-      <c r="AY29" s="197"/>
-      <c r="BF29" s="199" t="s">
+      <c r="AT29" s="205"/>
+      <c r="AU29" s="205"/>
+      <c r="AV29" s="205"/>
+      <c r="AW29" s="205"/>
+      <c r="AX29" s="205"/>
+      <c r="AY29" s="206"/>
+      <c r="BF29" s="208" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="199"/>
-      <c r="BH29" s="199"/>
-      <c r="BI29" s="199"/>
-      <c r="BJ29" s="199"/>
-      <c r="BK29" s="199"/>
-      <c r="BL29" s="199"/>
+      <c r="BG29" s="208"/>
+      <c r="BH29" s="208"/>
+      <c r="BI29" s="208"/>
+      <c r="BJ29" s="208"/>
+      <c r="BK29" s="208"/>
+      <c r="BL29" s="208"/>
     </row>
     <row r="31" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:72" ht="23.25" x14ac:dyDescent="0.35">
@@ -8384,13 +8384,13 @@
         <v>5714</v>
       </c>
       <c r="I47">
-        <v>8571</v>
+        <v>8069</v>
       </c>
       <c r="J47">
-        <v>12000</v>
+        <v>10895</v>
       </c>
       <c r="K47">
-        <v>16000</v>
+        <v>14192</v>
       </c>
       <c r="L47" t="s">
         <v>20</v>
@@ -9247,17 +9247,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="117" priority="10"/>

</xml_diff>

<commit_message>
added new column in Dragon Settings: anniversaryCakeSlices
Former-commit-id: 73504ed55f4e59e2e65f125175836c57d7057e4b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msana/Workspace/Unity/HungryDragon/ios/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB197146-F222-684B-A1DE-0DEFDF1D1398}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="37485" windowHeight="19845"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37480" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="181029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="229">
   <si>
     <t>[sku]</t>
   </si>
@@ -708,12 +709,15 @@
   </si>
   <si>
     <t>LETTERS</t>
+  </si>
+  <si>
+    <t>[anniversaryCakeSlices]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1270,7 +1274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1695,6 +1699,30 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1713,256 +1741,12 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="118">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="119">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1986,6 +1770,227 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2076,6 +2081,28 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
@@ -4174,105 +4201,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT27" totalsRowShown="0" headerRowDxfId="106" dataDxfId="104" headerRowBorderDxfId="105" tableBorderDxfId="103" totalsRowBorderDxfId="102">
-  <autoFilter ref="B15:BT27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT27" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104" totalsRowBorderDxfId="103">
+  <autoFilter ref="B15:BT27" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="101"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="100"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="99"/>
-    <tableColumn id="65" name="[type]" dataDxfId="98"/>
-    <tableColumn id="3" name="[order]" dataDxfId="97"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="96"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="95"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="94"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="93"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="92"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="91"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="90"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="89"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="88"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="87"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="86"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="85"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="84"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="83"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="82"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="81"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="80"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="79"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="78"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="77">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{dragonDefinitions}" dataDxfId="102"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="101"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[tier]" dataDxfId="100"/>
+    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="[type]" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[order]" dataDxfId="98"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="[previousDragonSku]" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[unlockPriceCoins]" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[unlockPricePC]" dataDxfId="95"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[cameraDefaultZoom]" dataDxfId="94"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[cameraFarZoom]" dataDxfId="93"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="[defaultSize]" dataDxfId="92"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="[cameraFrameWidthModifier]" dataDxfId="91"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[healthMin]" dataDxfId="90"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[healthMax]" dataDxfId="89"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[healthDrain]" dataDxfId="88"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="[healthDrainSpacePlus]" dataDxfId="87"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="[healthDrainAmpPerSecond]" dataDxfId="86"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[sessionStartHealthDrainTime]" dataDxfId="85"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[sessionStartHealthDrainModifier]" dataDxfId="84"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[scaleMin]" dataDxfId="83"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[scaleMax]" dataDxfId="82"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="[speedBase]" dataDxfId="81"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[boostMultiplier]" dataDxfId="80"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="[energyBaseMin]" dataDxfId="79"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="[energyBaseMax]" dataDxfId="78">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="76"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="75"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="74"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="73"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="72"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="71"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="70"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="69"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="68"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="67">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[energyDrain]" dataDxfId="77"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[energyRefillRate]" dataDxfId="76"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[furyBaseDamage]" dataDxfId="75"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="[furyBaseLength]" dataDxfId="74"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[furyScoreMultiplier]" dataDxfId="73"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[furyBaseDuration]" dataDxfId="72"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[furyMax]" dataDxfId="71"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="[scoreTextThresholdMultiplier]" dataDxfId="70"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[eatSpeedFactorMin]" dataDxfId="69"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="[eatSpeedFactorMax]" dataDxfId="68">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="66"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="65"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="64"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="63"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="62"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="61"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="60"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="59"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="58"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="57"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="56"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="55"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="54"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="53"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="52"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="51"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="50"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="49">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAlcohol]" dataDxfId="67"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[alcoholDrain]" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[gamePrefab]" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[menuPrefab]" dataDxfId="64"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="[resultsPrefab]" dataDxfId="63"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="[shadowFromDragon]" dataDxfId="62"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="[revealFromDragon]" dataDxfId="61"/>
+    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="[unlockFromDragon]" dataDxfId="60"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="[sizeUpMultiplier]" dataDxfId="59"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="[speedUpMultiplier]" dataDxfId="58"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="[biteUpMultiplier]" dataDxfId="57"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="[invincible]" dataDxfId="56"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="[infiniteBoost]" dataDxfId="55"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="[eatEverything]" dataDxfId="54"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="[modeDuration]" dataDxfId="53"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="[petScale]" dataDxfId="52"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="[petScaleMenu]" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="50">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="48">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[tidDesc]" dataDxfId="49">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="47"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="46"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="45"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="44">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="[statsBarRatio]" dataDxfId="48"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[furyBarRatio]" dataDxfId="47"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[forceMin]" dataDxfId="46"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="[forceMax]" dataDxfId="45">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="43"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="42"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="41"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="40"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="39"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="38"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="37"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="36"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="35"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="34"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="33"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="32"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="31"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[mass]" dataDxfId="44"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="[friction]" dataDxfId="43"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="[gravityModifier]" dataDxfId="42"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="[airGravityModifier]" dataDxfId="41"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="[waterGravityModifier]" dataDxfId="40"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="[damageAnimationThreshold]" dataDxfId="39"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="[dotAnimationThreshold]" dataDxfId="38"/>
+    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="[mummyHealthFactor]" dataDxfId="37"/>
+    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="[mummyDuration]" dataDxfId="36"/>
+    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="[animojiPrefab]" dataDxfId="35"/>
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="[energyRequiredToBoost]" dataDxfId="34"/>
+    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="[energyRestartThreshold]" dataDxfId="33"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="[trackingSku]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="B4:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="B4:G9" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="26"/>
-    <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="25"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="24"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{dragonTierDefinitions}" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="[order]"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[icon]" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[maxPetEquipped]" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[tidName]" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4281,62 +4308,63 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
-  <autoFilter ref="B33:I34"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="18"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
-    <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="16"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="15"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="14"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="13"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="dragonSettings" displayName="dragonSettings" ref="B33:J34" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="B33:J34" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{dragonSettings}" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="[energyRequiredToBoost]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="[superfuryMax]" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="[superFuryLengthModifier]" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="[superFuryCoinsMultiplier]" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="[superFuryDurationModifier]" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="[superFuryDamageModifier]" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{7898D356-2C02-CB41-9B92-5857FBBDE5CD}" name="[anniversaryCakeSlices]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B45:W57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="B45:W57" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <tableColumns count="22">
-    <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
-    <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[maxLevel]"/>
-    <tableColumn id="4" name="[xpLevel1]"/>
-    <tableColumn id="5" name="[xpLevel2]"/>
-    <tableColumn id="6" name="[xpLevel3]"/>
-    <tableColumn id="7" name="[xpLevel4]"/>
-    <tableColumn id="8" name="[xpLevel5]"/>
-    <tableColumn id="9" name="[xpLevel6]"/>
-    <tableColumn id="10" name="[xpLevel7]"/>
-    <tableColumn id="11" name="[xpLevel8]"/>
-    <tableColumn id="12" name="[xpLevel9]"/>
-    <tableColumn id="13" name="[xpLevel10]"/>
-    <tableColumn id="14" name="[xpLevel11]"/>
-    <tableColumn id="15" name="[xpLevel12]"/>
-    <tableColumn id="16" name="[xpLevel13]"/>
-    <tableColumn id="17" name="[xpLevel14]"/>
-    <tableColumn id="18" name="[xpLevel15]"/>
-    <tableColumn id="19" name="[xpLevel16]"/>
-    <tableColumn id="20" name="[xpLevel17]"/>
-    <tableColumn id="21" name="[xpLevel18]"/>
-    <tableColumn id="22" name="[xpLevel19]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{dragonProgressionDefinitions}"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[sku]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[maxLevel]"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[xpLevel1]"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[xpLevel2]"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[xpLevel3]"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="[xpLevel4]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="[xpLevel5]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="[xpLevel6]"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="[xpLevel7]"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="[xpLevel8]"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="[xpLevel9]"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="[xpLevel10]"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="[xpLevel11]"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="[xpLevel12]"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="[xpLevel13]"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="[xpLevel14]"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="[xpLevel15]"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="[xpLevel16]"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0300-000014000000}" name="[xpLevel17]"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0300-000015000000}" name="[xpLevel18]"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0300-000016000000}" name="[xpLevel19]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B38:F41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="B38:F41" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{dragonHealthModifiersDefinitions}" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[sku]" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="[threshold]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[modifier]" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="[tid]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4604,46 +4632,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="B1:BT57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.42578125" customWidth="1"/>
-    <col min="39" max="39" width="18.85546875" customWidth="1"/>
-    <col min="40" max="40" width="23.7109375" customWidth="1"/>
-    <col min="41" max="44" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="16.42578125" customWidth="1"/>
-    <col min="65" max="65" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="16.42578125" customWidth="1"/>
-    <col min="68" max="68" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="32" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.5" customWidth="1"/>
+    <col min="39" max="39" width="18.83203125" customWidth="1"/>
+    <col min="40" max="40" width="23.6640625" customWidth="1"/>
+    <col min="41" max="44" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16.5" customWidth="1"/>
+    <col min="65" max="65" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="16.5" customWidth="1"/>
+    <col min="68" max="68" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:72" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:72" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:72" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>183</v>
       </c>
@@ -4672,7 +4700,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B3" s="18"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4680,7 +4708,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:72" ht="117" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:72" ht="115" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>182</v>
       </c>
@@ -4700,7 +4728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
@@ -4721,7 +4749,7 @@
         <v>TID_DRAGON_TIER_0_NAME</v>
       </c>
     </row>
-    <row r="6" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
@@ -4742,7 +4770,7 @@
         <v>TID_DRAGON_TIER_1_NAME</v>
       </c>
     </row>
-    <row r="7" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
@@ -4763,7 +4791,7 @@
         <v>TID_DRAGON_TIER_2_NAME</v>
       </c>
     </row>
-    <row r="8" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
@@ -4784,7 +4812,7 @@
         <v>TID_DRAGON_TIER_3_NAME</v>
       </c>
     </row>
-    <row r="9" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B9" s="14" t="s">
         <v>3</v>
       </c>
@@ -4805,8 +4833,8 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
-    <row r="12" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:72" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:72" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:72" ht="24" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4835,7 +4863,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="2:72" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:72" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="J14" s="2" t="s">
         <v>174</v>
       </c>
@@ -4855,12 +4883,12 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="157"/>
-      <c r="AP14" s="157"/>
-      <c r="AQ14" s="157"/>
-      <c r="AR14" s="157"/>
+      <c r="AO14" s="165"/>
+      <c r="AP14" s="165"/>
+      <c r="AQ14" s="165"/>
+      <c r="AR14" s="165"/>
     </row>
-    <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:72" ht="161" x14ac:dyDescent="0.2">
       <c r="B15" s="65" t="s">
         <v>170</v>
       </c>
@@ -5075,7 +5103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B16" s="22" t="s">
         <v>3</v>
       </c>
@@ -5284,7 +5312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B17" s="22" t="s">
         <v>3</v>
       </c>
@@ -5493,7 +5521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B18" s="30" t="s">
         <v>3</v>
       </c>
@@ -5704,7 +5732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B19" s="30" t="s">
         <v>3</v>
       </c>
@@ -5913,7 +5941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B20" s="30" t="s">
         <v>3</v>
       </c>
@@ -6124,7 +6152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B21" s="30" t="s">
         <v>3</v>
       </c>
@@ -6335,7 +6363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B22" s="30" t="s">
         <v>3</v>
       </c>
@@ -6546,7 +6574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B23" s="30" t="s">
         <v>3</v>
       </c>
@@ -6757,7 +6785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B24" s="30" t="s">
         <v>3</v>
       </c>
@@ -6967,7 +6995,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B25" s="30" t="s">
         <v>3</v>
       </c>
@@ -7178,7 +7206,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:72" x14ac:dyDescent="0.2">
       <c r="B26" s="30" t="s">
         <v>3</v>
       </c>
@@ -7390,7 +7418,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:72" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
         <v>3</v>
       </c>
@@ -7602,7 +7630,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="2:72" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:72" s="32" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
@@ -7610,35 +7638,35 @@
       <c r="F28" s="33"/>
       <c r="G28" s="33"/>
       <c r="H28" s="33"/>
-      <c r="J28" s="167" t="s">
+      <c r="J28" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="K28" s="167"/>
-      <c r="L28" s="167"/>
-      <c r="M28" s="167"/>
-      <c r="N28" s="165" t="s">
+      <c r="K28" s="161"/>
+      <c r="L28" s="161"/>
+      <c r="M28" s="161"/>
+      <c r="N28" s="159" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="166"/>
-      <c r="P28" s="166"/>
-      <c r="Q28" s="166"/>
-      <c r="R28" s="166"/>
-      <c r="S28" s="166"/>
-      <c r="T28" s="166"/>
-      <c r="U28" s="163" t="s">
+      <c r="O28" s="160"/>
+      <c r="P28" s="160"/>
+      <c r="Q28" s="160"/>
+      <c r="R28" s="160"/>
+      <c r="S28" s="160"/>
+      <c r="T28" s="160"/>
+      <c r="U28" s="157" t="s">
         <v>72</v>
       </c>
-      <c r="V28" s="164"/>
+      <c r="V28" s="158"/>
       <c r="W28" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X28" s="160" t="s">
+      <c r="X28" s="154" t="s">
         <v>70</v>
       </c>
-      <c r="Y28" s="161"/>
-      <c r="Z28" s="161"/>
-      <c r="AA28" s="161"/>
-      <c r="AB28" s="162"/>
+      <c r="Y28" s="155"/>
+      <c r="Z28" s="155"/>
+      <c r="AA28" s="155"/>
+      <c r="AB28" s="156"/>
       <c r="AC28" s="153" t="s">
         <v>69</v>
       </c>
@@ -7646,10 +7674,10 @@
       <c r="AE28" s="153"/>
       <c r="AF28" s="153"/>
       <c r="AG28" s="153"/>
-      <c r="AI28" s="159" t="s">
+      <c r="AI28" s="167" t="s">
         <v>68</v>
       </c>
-      <c r="AJ28" s="159"/>
+      <c r="AJ28" s="167"/>
       <c r="AK28" s="153" t="s">
         <v>226</v>
       </c>
@@ -7657,27 +7685,27 @@
       <c r="AM28"/>
       <c r="AN28"/>
       <c r="AO28"/>
-      <c r="AS28" s="154" t="s">
+      <c r="AS28" s="162" t="s">
         <v>227</v>
       </c>
-      <c r="AT28" s="155"/>
-      <c r="AU28" s="155"/>
-      <c r="AV28" s="155"/>
-      <c r="AW28" s="155"/>
-      <c r="AX28" s="155"/>
-      <c r="AY28" s="156"/>
-      <c r="BF28" s="158" t="s">
+      <c r="AT28" s="163"/>
+      <c r="AU28" s="163"/>
+      <c r="AV28" s="163"/>
+      <c r="AW28" s="163"/>
+      <c r="AX28" s="163"/>
+      <c r="AY28" s="164"/>
+      <c r="BF28" s="166" t="s">
         <v>67</v>
       </c>
-      <c r="BG28" s="158"/>
-      <c r="BH28" s="158"/>
-      <c r="BI28" s="158"/>
-      <c r="BJ28" s="158"/>
-      <c r="BK28" s="158"/>
-      <c r="BL28" s="158"/>
+      <c r="BG28" s="166"/>
+      <c r="BH28" s="166"/>
+      <c r="BI28" s="166"/>
+      <c r="BJ28" s="166"/>
+      <c r="BK28" s="166"/>
+      <c r="BL28" s="166"/>
     </row>
-    <row r="30" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:72" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:72" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:72" ht="24" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
@@ -7691,7 +7719,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:72" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:72" s="19" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="B32" s="18"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
@@ -7700,7 +7728,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:23" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:23" ht="139" x14ac:dyDescent="0.2">
       <c r="B33" s="9" t="s">
         <v>64</v>
       </c>
@@ -7725,8 +7753,11 @@
       <c r="I33" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="J33" s="3" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>3</v>
       </c>
@@ -7751,9 +7782,12 @@
       <c r="I34" s="146">
         <v>10</v>
       </c>
+      <c r="J34" s="168">
+        <v>6</v>
+      </c>
     </row>
-    <row r="35" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:23" ht="24" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>56</v>
       </c>
@@ -7767,7 +7801,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="2:23" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:23" s="19" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="B37" s="18"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
@@ -7779,7 +7813,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="2:23" ht="169.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:23" ht="166" x14ac:dyDescent="0.2">
       <c r="B38" s="9" t="s">
         <v>53</v>
       </c>
@@ -7796,7 +7830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B39" s="7" t="s">
         <v>3</v>
       </c>
@@ -7813,7 +7847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B40" s="7" t="s">
         <v>3</v>
       </c>
@@ -7830,7 +7864,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B41" s="7" t="s">
         <v>3</v>
       </c>
@@ -7847,8 +7881,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:23" ht="24" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
@@ -7862,12 +7896,12 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
       <c r="E44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:23" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:23" ht="149" x14ac:dyDescent="0.2">
       <c r="B45" s="9" t="s">
         <v>41</v>
       </c>
@@ -7935,7 +7969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>3</v>
       </c>
@@ -8003,7 +8037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>3</v>
       </c>
@@ -8071,7 +8105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>3</v>
       </c>
@@ -8139,7 +8173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>3</v>
       </c>
@@ -8207,7 +8241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>3</v>
       </c>
@@ -8275,7 +8309,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -8343,7 +8377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -8411,7 +8445,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -8479,7 +8513,7 @@
         <v>485030</v>
       </c>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -8547,7 +8581,7 @@
         <v>558660</v>
       </c>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>3</v>
       </c>
@@ -8615,7 +8649,7 @@
         <v>633960</v>
       </c>
     </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>3</v>
       </c>
@@ -8683,7 +8717,7 @@
         <v>710770</v>
       </c>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>3</v>
       </c>
@@ -8753,56 +8787,56 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AK28:AL28"/>
+    <mergeCell ref="AS28:AY28"/>
+    <mergeCell ref="AO14:AR14"/>
+    <mergeCell ref="BF28:BL28"/>
+    <mergeCell ref="AI28:AJ28"/>
     <mergeCell ref="AC28:AG28"/>
     <mergeCell ref="X28:AB28"/>
     <mergeCell ref="U28:V28"/>
     <mergeCell ref="N28:T28"/>
     <mergeCell ref="J28:M28"/>
-    <mergeCell ref="AK28:AL28"/>
-    <mergeCell ref="AS28:AY28"/>
-    <mergeCell ref="AO14:AR14"/>
-    <mergeCell ref="BF28:BL28"/>
-    <mergeCell ref="AI28:AJ28"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="117" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="116" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="115" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="114" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="113" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="112" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="110" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="109" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="108" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="107" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="19"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT("dragonTierDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D46:D57 F46:W57 E47:E57"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D34:D35 D39:D41">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D46:D57 F46:W57 E47:E57" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D34:D35 D39:D41" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
fixing merge with 1.32
Former-commit-id: 7a673c807fe3951e964efe08b47211f09275c964
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="238">
   <si>
     <t>[sku]</t>
   </si>
@@ -708,13 +711,43 @@
   </si>
   <si>
     <t>LETTERS</t>
+  </si>
+  <si>
+    <t>tier_5</t>
+  </si>
+  <si>
+    <t>icon_xxl</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_TIER_5_NAME</t>
+  </si>
+  <si>
+    <t>dragon_dark</t>
+  </si>
+  <si>
+    <t>PF_DragonDark</t>
+  </si>
+  <si>
+    <t>PF_DragonDarkMenu</t>
+  </si>
+  <si>
+    <t>PF_DragonDarkResults</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_DARK_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_DARK_DESC</t>
+  </si>
+  <si>
+    <t>PREFABS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -784,6 +817,40 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -881,7 +948,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1233,19 +1300,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1266,11 +1320,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1574,9 +1646,6 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
@@ -1595,20 +1664,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1683,7 +1740,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1695,6 +1752,30 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1713,35 +1794,492 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="118">
+  <dxfs count="122">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3095,156 +3633,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -3462,30 +3850,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -4050,116 +4414,6 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4173,106 +4427,119 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="dragons"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT27" totalsRowShown="0" headerRowDxfId="106" dataDxfId="104" headerRowBorderDxfId="105" tableBorderDxfId="103" totalsRowBorderDxfId="102">
-  <autoFilter ref="B15:BT27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="121" dataDxfId="119" headerRowBorderDxfId="120" tableBorderDxfId="118" totalsRowBorderDxfId="117">
+  <autoFilter ref="B15:BT28"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="101"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="100"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="99"/>
-    <tableColumn id="65" name="[type]" dataDxfId="98"/>
-    <tableColumn id="3" name="[order]" dataDxfId="97"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="96"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="95"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="94"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="93"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="92"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="91"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="90"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="89"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="88"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="87"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="86"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="85"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="84"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="83"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="82"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="81"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="80"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="79"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="78"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="77">
-      <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="116"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="115"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="114"/>
+    <tableColumn id="65" name="[type]" dataDxfId="113"/>
+    <tableColumn id="3" name="[order]" dataDxfId="112"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="111"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="110"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="109"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="108"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="107"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="106"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="105"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="104"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="103"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="102"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="101"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="100"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="99"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="98"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="97"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="96"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="95"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="94"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="93"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="6">
+      <calculatedColumnFormula>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="76"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="75"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="74"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="73"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="72"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="71"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="70"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="69"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="68"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="67">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="92"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="91"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="90"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="89"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="88"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="87"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="86"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="85"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="84"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="83">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="66"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="65"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="64"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="63"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="62"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="61"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="60"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="59"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="58"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="57"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="56"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="55"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="54"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="53"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="52"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="51"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="50"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="49">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="5"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="4"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="3"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="2"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="0"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="1"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="82"/>
+    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="81"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="80"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="79"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="78"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="77"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="76"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="75"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="74"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="73"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="72"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="71">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="48">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="70">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="47"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="46"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="45"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="44">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="69"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="68"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="67"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="66">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="43"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="42"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="41"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="40"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="39"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="38"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="37"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="36"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="35"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="34"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="33"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="32"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="31"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="65"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="64"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="63"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="62"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="61"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="60"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="59"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="58"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="57"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="56"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="55"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="54"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G9" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="B4:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G10" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+  <autoFilter ref="B4:G10"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="26"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="48"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="25"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="24"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="23">
+    <tableColumn id="10" name="[icon]" dataDxfId="47"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="46"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="45">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4281,25 +4548,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B33:I34" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
-  <autoFilter ref="B33:I34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:I35" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+  <autoFilter ref="B34:I35"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="18"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="40"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="16"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="15"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="14"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="13"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="12"/>
+    <tableColumn id="8" name="[superfuryMax]" dataDxfId="38"/>
+    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="37"/>
+    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="36"/>
+    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="35"/>
+    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B45:W57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B45:W57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+  <autoFilter ref="B46:W59"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
     <tableColumn id="2" name="[sku]"/>
@@ -4329,14 +4596,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B38:F41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B38:F41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B39:F42"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="23"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4608,10 +4875,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:BT57"/>
+  <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4633,7 +4900,9 @@
     <col min="38" max="38" width="24.42578125" customWidth="1"/>
     <col min="39" max="39" width="18.85546875" customWidth="1"/>
     <col min="40" max="40" width="23.7109375" customWidth="1"/>
-    <col min="41" max="44" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="24.7109375" customWidth="1"/>
+    <col min="42" max="43" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.140625" customWidth="1"/>
     <col min="47" max="47" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="16.42578125" customWidth="1"/>
@@ -4805,6 +5074,26 @@
         <v>TID_DRAGON_TIER_4_NAME</v>
       </c>
     </row>
+    <row r="10" spans="2:72" x14ac:dyDescent="0.25">
+      <c r="B10" s="165" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="166">
+        <v>5</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="F10" s="15">
+        <v>4</v>
+      </c>
+      <c r="G10" s="164" t="s">
+        <v>230</v>
+      </c>
+    </row>
     <row r="12" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:72" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
@@ -4855,10 +5144,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="157"/>
-      <c r="AP14" s="157"/>
-      <c r="AQ14" s="157"/>
-      <c r="AR14" s="157"/>
+      <c r="AO14" s="160"/>
+      <c r="AP14" s="160"/>
+      <c r="AQ14" s="160"/>
+      <c r="AR14" s="160"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -4954,22 +5243,22 @@
       <c r="AF15" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="AG15" s="114" t="s">
+      <c r="AG15" s="113" t="s">
         <v>145</v>
       </c>
-      <c r="AH15" s="115" t="s">
+      <c r="AH15" s="114" t="s">
         <v>144</v>
       </c>
-      <c r="AI15" s="115" t="s">
+      <c r="AI15" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="AJ15" s="121" t="s">
+      <c r="AJ15" s="119" t="s">
         <v>194</v>
       </c>
-      <c r="AK15" s="115" t="s">
+      <c r="AK15" s="81" t="s">
         <v>143</v>
       </c>
-      <c r="AL15" s="79" t="s">
+      <c r="AL15" s="80" t="s">
         <v>142</v>
       </c>
       <c r="AM15" s="74" t="s">
@@ -4987,7 +5276,7 @@
       <c r="AQ15" s="111" t="s">
         <v>139</v>
       </c>
-      <c r="AR15" s="127" t="s">
+      <c r="AR15" s="122" t="s">
         <v>215</v>
       </c>
       <c r="AS15" s="74" t="s">
@@ -5008,16 +5297,16 @@
       <c r="AX15" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="AY15" s="150" t="s">
+      <c r="AY15" s="145" t="s">
         <v>132</v>
       </c>
       <c r="AZ15" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="BA15" s="127" t="s">
+      <c r="BA15" s="122" t="s">
         <v>196</v>
       </c>
-      <c r="BB15" s="130" t="s">
+      <c r="BB15" s="125" t="s">
         <v>4</v>
       </c>
       <c r="BC15" s="71" t="s">
@@ -5047,7 +5336,7 @@
       <c r="BK15" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="BL15" s="136" t="s">
+      <c r="BL15" s="131" t="s">
         <v>124</v>
       </c>
       <c r="BM15" s="70" t="s">
@@ -5147,7 +5436,7 @@
         <v>100</v>
       </c>
       <c r="Z16" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA16" s="28">
@@ -5171,7 +5460,7 @@
       <c r="AG16" s="28">
         <v>3000</v>
       </c>
-      <c r="AH16" s="116">
+      <c r="AH16" s="115">
         <v>1</v>
       </c>
       <c r="AI16" s="104">
@@ -5181,24 +5470,24 @@
         <f t="shared" ref="AJ16:AJ23" si="0">AI17</f>
         <v>0.19</v>
       </c>
-      <c r="AK16" s="94">
+      <c r="AK16" s="197">
         <v>0</v>
       </c>
-      <c r="AL16" s="93">
+      <c r="AL16" s="61">
         <v>12</v>
       </c>
-      <c r="AM16" s="23" t="s">
+      <c r="AM16" s="201" t="s">
         <v>120</v>
       </c>
-      <c r="AN16" s="23" t="s">
+      <c r="AN16" s="201" t="s">
         <v>119</v>
       </c>
-      <c r="AO16" s="23" t="s">
+      <c r="AO16" s="201" t="s">
         <v>217</v>
       </c>
       <c r="AP16" s="112"/>
       <c r="AQ16" s="112"/>
-      <c r="AR16" s="128"/>
+      <c r="AR16" s="123"/>
       <c r="AS16" s="41">
         <v>3</v>
       </c>
@@ -5217,16 +5506,16 @@
       <c r="AX16" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY16" s="151">
+      <c r="AY16" s="146">
         <v>25</v>
       </c>
-      <c r="AZ16" s="148">
+      <c r="AZ16" s="143">
         <v>0.55999999999999994</v>
       </c>
-      <c r="BA16" s="128">
+      <c r="BA16" s="123">
         <v>0.6</v>
       </c>
-      <c r="BB16" s="131" t="s">
+      <c r="BB16" s="126" t="s">
         <v>118</v>
       </c>
       <c r="BC16" s="63" t="s">
@@ -5256,10 +5545,10 @@
       <c r="BK16" s="64">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BL16" s="137">
+      <c r="BL16" s="132">
         <v>1.75</v>
       </c>
-      <c r="BM16" s="141">
+      <c r="BM16" s="136">
         <v>0</v>
       </c>
       <c r="BN16" s="64">
@@ -5277,14 +5566,14 @@
       <c r="BR16" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS16" s="138">
+      <c r="BS16" s="133">
         <v>1</v>
       </c>
       <c r="BT16" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
         <v>3</v>
       </c>
@@ -5358,7 +5647,7 @@
         <v>100</v>
       </c>
       <c r="Z17" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA17" s="28">
@@ -5382,7 +5671,7 @@
       <c r="AG17" s="28">
         <v>7000</v>
       </c>
-      <c r="AH17" s="116">
+      <c r="AH17" s="115">
         <v>2</v>
       </c>
       <c r="AI17" s="104">
@@ -5392,24 +5681,24 @@
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="AK17" s="94">
+      <c r="AK17" s="197">
         <v>0</v>
       </c>
-      <c r="AL17" s="93">
+      <c r="AL17" s="61">
         <v>12</v>
       </c>
-      <c r="AM17" s="41" t="s">
+      <c r="AM17" s="202" t="s">
         <v>116</v>
       </c>
-      <c r="AN17" s="23" t="s">
+      <c r="AN17" s="201" t="s">
         <v>115</v>
       </c>
-      <c r="AO17" s="23" t="s">
+      <c r="AO17" s="201" t="s">
         <v>218</v>
       </c>
       <c r="AP17" s="112"/>
       <c r="AQ17" s="112"/>
-      <c r="AR17" s="128"/>
+      <c r="AR17" s="123"/>
       <c r="AS17" s="41">
         <v>2.2999999999999998</v>
       </c>
@@ -5428,16 +5717,16 @@
       <c r="AX17" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY17" s="151">
+      <c r="AY17" s="146">
         <v>25</v>
       </c>
-      <c r="AZ17" s="148">
+      <c r="AZ17" s="143">
         <v>0.7</v>
       </c>
-      <c r="BA17" s="128">
+      <c r="BA17" s="123">
         <v>0.8</v>
       </c>
-      <c r="BB17" s="131" t="s">
+      <c r="BB17" s="126" t="s">
         <v>114</v>
       </c>
       <c r="BC17" s="63" t="s">
@@ -5467,7 +5756,7 @@
       <c r="BK17" s="52">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BL17" s="138">
+      <c r="BL17" s="133">
         <v>2.1</v>
       </c>
       <c r="BM17" s="37">
@@ -5486,14 +5775,14 @@
       <c r="BR17" s="64">
         <v>0.2</v>
       </c>
-      <c r="BS17" s="137">
+      <c r="BS17" s="132">
         <v>1</v>
       </c>
       <c r="BT17" s="37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B18" s="30" t="s">
         <v>3</v>
       </c>
@@ -5567,7 +5856,7 @@
         <v>100</v>
       </c>
       <c r="Z18" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA18" s="28">
@@ -5591,7 +5880,7 @@
       <c r="AG18" s="28">
         <v>8000</v>
       </c>
-      <c r="AH18" s="117">
+      <c r="AH18" s="116">
         <v>2</v>
       </c>
       <c r="AI18" s="105">
@@ -5601,24 +5890,24 @@
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="AK18" s="113">
+      <c r="AK18" s="198">
         <v>0</v>
       </c>
-      <c r="AL18" s="122">
+      <c r="AL18" s="163">
         <v>12</v>
       </c>
-      <c r="AM18" s="41" t="s">
+      <c r="AM18" s="202" t="s">
         <v>112</v>
       </c>
-      <c r="AN18" s="23" t="s">
+      <c r="AN18" s="201" t="s">
         <v>111</v>
       </c>
-      <c r="AO18" s="23" t="s">
+      <c r="AO18" s="201" t="s">
         <v>110</v>
       </c>
       <c r="AP18" s="112"/>
       <c r="AQ18" s="112"/>
-      <c r="AR18" s="128"/>
+      <c r="AR18" s="123"/>
       <c r="AS18" s="41">
         <v>2.1</v>
       </c>
@@ -5637,16 +5926,16 @@
       <c r="AX18" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY18" s="151">
+      <c r="AY18" s="146">
         <v>25</v>
       </c>
-      <c r="AZ18" s="148">
+      <c r="AZ18" s="143">
         <v>0.7</v>
       </c>
-      <c r="BA18" s="128">
+      <c r="BA18" s="123">
         <v>0.7</v>
       </c>
-      <c r="BB18" s="132" t="s">
+      <c r="BB18" s="127" t="s">
         <v>109</v>
       </c>
       <c r="BC18" s="53" t="s">
@@ -5676,7 +5965,7 @@
       <c r="BK18" s="52">
         <v>0.9</v>
       </c>
-      <c r="BL18" s="138">
+      <c r="BL18" s="133">
         <v>2.25</v>
       </c>
       <c r="BM18" s="37">
@@ -5697,14 +5986,14 @@
       <c r="BR18" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS18" s="142">
+      <c r="BS18" s="137">
         <v>1</v>
       </c>
-      <c r="BT18" s="144" t="s">
+      <c r="BT18" s="139" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B19" s="30" t="s">
         <v>3</v>
       </c>
@@ -5778,7 +6067,7 @@
         <v>100</v>
       </c>
       <c r="Z19" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA19" s="28">
@@ -5802,7 +6091,7 @@
       <c r="AG19" s="28">
         <v>9000</v>
       </c>
-      <c r="AH19" s="116">
+      <c r="AH19" s="115">
         <v>2</v>
       </c>
       <c r="AI19" s="104">
@@ -5812,24 +6101,24 @@
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="AK19" s="94">
+      <c r="AK19" s="197">
         <v>0</v>
       </c>
-      <c r="AL19" s="93">
+      <c r="AL19" s="61">
         <v>12</v>
       </c>
-      <c r="AM19" s="41" t="s">
+      <c r="AM19" s="202" t="s">
         <v>106</v>
       </c>
-      <c r="AN19" s="23" t="s">
+      <c r="AN19" s="201" t="s">
         <v>105</v>
       </c>
-      <c r="AO19" s="23" t="s">
+      <c r="AO19" s="201" t="s">
         <v>219</v>
       </c>
       <c r="AP19" s="112"/>
       <c r="AQ19" s="112"/>
-      <c r="AR19" s="128"/>
+      <c r="AR19" s="123"/>
       <c r="AS19" s="41">
         <v>2.1</v>
       </c>
@@ -5848,16 +6137,16 @@
       <c r="AX19" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY19" s="151">
+      <c r="AY19" s="146">
         <v>25</v>
       </c>
-      <c r="AZ19" s="148">
+      <c r="AZ19" s="143">
         <v>0.7</v>
       </c>
-      <c r="BA19" s="128">
+      <c r="BA19" s="123">
         <v>0.7</v>
       </c>
-      <c r="BB19" s="132" t="s">
+      <c r="BB19" s="127" t="s">
         <v>104</v>
       </c>
       <c r="BC19" s="53" t="s">
@@ -5887,7 +6176,7 @@
       <c r="BK19" s="52">
         <v>1.2</v>
       </c>
-      <c r="BL19" s="138">
+      <c r="BL19" s="133">
         <v>0.77</v>
       </c>
       <c r="BM19" s="37">
@@ -5906,14 +6195,14 @@
       <c r="BR19" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS19" s="142">
+      <c r="BS19" s="137">
         <v>1</v>
       </c>
-      <c r="BT19" s="144" t="s">
+      <c r="BT19" s="139" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B20" s="30" t="s">
         <v>3</v>
       </c>
@@ -5987,7 +6276,7 @@
         <v>100</v>
       </c>
       <c r="Z20" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA20" s="28">
@@ -6011,7 +6300,7 @@
       <c r="AG20" s="28">
         <v>10000</v>
       </c>
-      <c r="AH20" s="116">
+      <c r="AH20" s="115">
         <v>3</v>
       </c>
       <c r="AI20" s="104">
@@ -6021,24 +6310,24 @@
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="AK20" s="94">
+      <c r="AK20" s="197">
         <v>0</v>
       </c>
-      <c r="AL20" s="93">
+      <c r="AL20" s="61">
         <v>12</v>
       </c>
-      <c r="AM20" s="41" t="s">
+      <c r="AM20" s="202" t="s">
         <v>102</v>
       </c>
-      <c r="AN20" s="23" t="s">
+      <c r="AN20" s="201" t="s">
         <v>101</v>
       </c>
-      <c r="AO20" s="23" t="s">
+      <c r="AO20" s="201" t="s">
         <v>220</v>
       </c>
       <c r="AP20" s="112"/>
       <c r="AQ20" s="112"/>
-      <c r="AR20" s="128"/>
+      <c r="AR20" s="123"/>
       <c r="AS20" s="41">
         <v>2.1</v>
       </c>
@@ -6057,16 +6346,16 @@
       <c r="AX20" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY20" s="151">
+      <c r="AY20" s="146">
         <v>25</v>
       </c>
-      <c r="AZ20" s="148">
+      <c r="AZ20" s="143">
         <v>0.7</v>
       </c>
-      <c r="BA20" s="128">
+      <c r="BA20" s="123">
         <v>0.6</v>
       </c>
-      <c r="BB20" s="132" t="s">
+      <c r="BB20" s="127" t="s">
         <v>100</v>
       </c>
       <c r="BC20" s="53" t="s">
@@ -6096,7 +6385,7 @@
       <c r="BK20" s="52">
         <v>1</v>
       </c>
-      <c r="BL20" s="138">
+      <c r="BL20" s="133">
         <v>1.6</v>
       </c>
       <c r="BM20" s="37">
@@ -6117,14 +6406,14 @@
       <c r="BR20" s="109">
         <v>0.2</v>
       </c>
-      <c r="BS20" s="143">
+      <c r="BS20" s="138">
         <v>1</v>
       </c>
-      <c r="BT20" s="144" t="s">
+      <c r="BT20" s="139" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B21" s="30" t="s">
         <v>3</v>
       </c>
@@ -6198,7 +6487,7 @@
         <v>100</v>
       </c>
       <c r="Z21" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA21" s="28">
@@ -6222,7 +6511,7 @@
       <c r="AG21" s="28">
         <v>10000</v>
       </c>
-      <c r="AH21" s="116">
+      <c r="AH21" s="115">
         <v>3</v>
       </c>
       <c r="AI21" s="104">
@@ -6232,24 +6521,24 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="AK21" s="94">
+      <c r="AK21" s="197">
         <v>0</v>
       </c>
-      <c r="AL21" s="93">
+      <c r="AL21" s="61">
         <v>12</v>
       </c>
-      <c r="AM21" s="41" t="s">
+      <c r="AM21" s="202" t="s">
         <v>98</v>
       </c>
-      <c r="AN21" s="23" t="s">
+      <c r="AN21" s="201" t="s">
         <v>97</v>
       </c>
-      <c r="AO21" s="23" t="s">
+      <c r="AO21" s="201" t="s">
         <v>96</v>
       </c>
       <c r="AP21" s="112"/>
       <c r="AQ21" s="112"/>
-      <c r="AR21" s="128"/>
+      <c r="AR21" s="123"/>
       <c r="AS21" s="41">
         <v>2</v>
       </c>
@@ -6268,16 +6557,16 @@
       <c r="AX21" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY21" s="151">
+      <c r="AY21" s="146">
         <v>25</v>
       </c>
-      <c r="AZ21" s="148">
+      <c r="AZ21" s="143">
         <v>0.7</v>
       </c>
-      <c r="BA21" s="128">
+      <c r="BA21" s="123">
         <v>0.5</v>
       </c>
-      <c r="BB21" s="132" t="s">
+      <c r="BB21" s="127" t="s">
         <v>95</v>
       </c>
       <c r="BC21" s="53" t="s">
@@ -6307,7 +6596,7 @@
       <c r="BK21" s="52">
         <v>0.5</v>
       </c>
-      <c r="BL21" s="138">
+      <c r="BL21" s="133">
         <v>1.7</v>
       </c>
       <c r="BM21" s="37">
@@ -6328,14 +6617,14 @@
       <c r="BR21" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS21" s="142">
+      <c r="BS21" s="137">
         <v>1</v>
       </c>
-      <c r="BT21" s="144" t="s">
+      <c r="BT21" s="139" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B22" s="30" t="s">
         <v>3</v>
       </c>
@@ -6409,7 +6698,7 @@
         <v>100</v>
       </c>
       <c r="Z22" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA22" s="28">
@@ -6433,7 +6722,7 @@
       <c r="AG22" s="28">
         <v>10000</v>
       </c>
-      <c r="AH22" s="116">
+      <c r="AH22" s="115">
         <v>3</v>
       </c>
       <c r="AI22" s="104">
@@ -6443,24 +6732,24 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK22" s="94">
+      <c r="AK22" s="197">
         <v>0</v>
       </c>
-      <c r="AL22" s="93">
+      <c r="AL22" s="61">
         <v>12</v>
       </c>
-      <c r="AM22" s="41" t="s">
+      <c r="AM22" s="202" t="s">
         <v>92</v>
       </c>
-      <c r="AN22" s="23" t="s">
+      <c r="AN22" s="201" t="s">
         <v>91</v>
       </c>
-      <c r="AO22" s="23" t="s">
+      <c r="AO22" s="201" t="s">
         <v>221</v>
       </c>
       <c r="AP22" s="112"/>
       <c r="AQ22" s="112"/>
-      <c r="AR22" s="128"/>
+      <c r="AR22" s="123"/>
       <c r="AS22" s="41">
         <v>1.6</v>
       </c>
@@ -6479,16 +6768,16 @@
       <c r="AX22" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY22" s="151">
+      <c r="AY22" s="146">
         <v>25</v>
       </c>
-      <c r="AZ22" s="148">
+      <c r="AZ22" s="143">
         <v>0.7</v>
       </c>
-      <c r="BA22" s="128">
+      <c r="BA22" s="123">
         <v>0.5</v>
       </c>
-      <c r="BB22" s="132" t="s">
+      <c r="BB22" s="127" t="s">
         <v>90</v>
       </c>
       <c r="BC22" s="53" t="s">
@@ -6518,7 +6807,7 @@
       <c r="BK22" s="52">
         <v>0.5</v>
       </c>
-      <c r="BL22" s="138">
+      <c r="BL22" s="133">
         <v>0.9</v>
       </c>
       <c r="BM22" s="37">
@@ -6539,14 +6828,14 @@
       <c r="BR22" s="110">
         <v>0.2</v>
       </c>
-      <c r="BS22" s="143">
+      <c r="BS22" s="138">
         <v>1</v>
       </c>
-      <c r="BT22" s="144" t="s">
+      <c r="BT22" s="139" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B23" s="30" t="s">
         <v>3</v>
       </c>
@@ -6620,7 +6909,7 @@
         <v>100</v>
       </c>
       <c r="Z23" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA23" s="28">
@@ -6644,7 +6933,7 @@
       <c r="AG23" s="28">
         <v>16000</v>
       </c>
-      <c r="AH23" s="117">
+      <c r="AH23" s="116">
         <v>4</v>
       </c>
       <c r="AI23" s="105">
@@ -6654,24 +6943,24 @@
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="AK23" s="113">
+      <c r="AK23" s="198">
         <v>0</v>
       </c>
-      <c r="AL23" s="122">
+      <c r="AL23" s="163">
         <v>12</v>
       </c>
-      <c r="AM23" s="41" t="s">
+      <c r="AM23" s="202" t="s">
         <v>88</v>
       </c>
-      <c r="AN23" s="23" t="s">
+      <c r="AN23" s="201" t="s">
         <v>87</v>
       </c>
-      <c r="AO23" s="23" t="s">
+      <c r="AO23" s="201" t="s">
         <v>222</v>
       </c>
       <c r="AP23" s="112"/>
       <c r="AQ23" s="112"/>
-      <c r="AR23" s="147" t="s">
+      <c r="AR23" s="142" t="s">
         <v>11</v>
       </c>
       <c r="AS23" s="41">
@@ -6692,16 +6981,16 @@
       <c r="AX23" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY23" s="151">
+      <c r="AY23" s="146">
         <v>25</v>
       </c>
-      <c r="AZ23" s="148">
+      <c r="AZ23" s="143">
         <v>0.7</v>
       </c>
-      <c r="BA23" s="128">
+      <c r="BA23" s="123">
         <v>0.5</v>
       </c>
-      <c r="BB23" s="132" t="s">
+      <c r="BB23" s="127" t="s">
         <v>86</v>
       </c>
       <c r="BC23" s="53" t="s">
@@ -6731,7 +7020,7 @@
       <c r="BK23" s="52">
         <v>0.5</v>
       </c>
-      <c r="BL23" s="138">
+      <c r="BL23" s="133">
         <v>1.2</v>
       </c>
       <c r="BM23" s="37">
@@ -6750,14 +7039,14 @@
       <c r="BR23" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS23" s="142">
+      <c r="BS23" s="137">
         <v>1</v>
       </c>
-      <c r="BT23" s="144" t="s">
+      <c r="BT23" s="139" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B24" s="30" t="s">
         <v>3</v>
       </c>
@@ -6831,7 +7120,7 @@
         <v>100</v>
       </c>
       <c r="Z24" s="46">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA24" s="46">
@@ -6855,7 +7144,7 @@
       <c r="AG24" s="46">
         <v>20000</v>
       </c>
-      <c r="AH24" s="118">
+      <c r="AH24" s="117">
         <v>4</v>
       </c>
       <c r="AI24" s="106">
@@ -6864,24 +7153,24 @@
       <c r="AJ24" s="103">
         <v>0.05</v>
       </c>
-      <c r="AK24" s="113">
+      <c r="AK24" s="198">
         <v>0</v>
       </c>
-      <c r="AL24" s="122">
+      <c r="AL24" s="163">
         <v>12</v>
       </c>
-      <c r="AM24" s="89" t="s">
+      <c r="AM24" s="203" t="s">
         <v>185</v>
       </c>
-      <c r="AN24" s="88" t="s">
+      <c r="AN24" s="204" t="s">
         <v>186</v>
       </c>
-      <c r="AO24" s="88" t="s">
+      <c r="AO24" s="204" t="s">
         <v>223</v>
       </c>
       <c r="AP24" s="112"/>
       <c r="AQ24" s="112"/>
-      <c r="AR24" s="147" t="s">
+      <c r="AR24" s="142" t="s">
         <v>12</v>
       </c>
       <c r="AS24" s="89">
@@ -6902,16 +7191,16 @@
       <c r="AX24" s="88" t="b">
         <v>1</v>
       </c>
-      <c r="AY24" s="152">
+      <c r="AY24" s="147">
         <v>25</v>
       </c>
-      <c r="AZ24" s="149">
+      <c r="AZ24" s="144">
         <v>0.7</v>
       </c>
-      <c r="BA24" s="129">
+      <c r="BA24" s="124">
         <v>0.5</v>
       </c>
-      <c r="BB24" s="133" t="s">
+      <c r="BB24" s="128" t="s">
         <v>187</v>
       </c>
       <c r="BC24" s="20" t="s">
@@ -6941,7 +7230,7 @@
       <c r="BK24" s="92">
         <v>0.6</v>
       </c>
-      <c r="BL24" s="139">
+      <c r="BL24" s="134">
         <v>1</v>
       </c>
       <c r="BM24" s="97">
@@ -6960,14 +7249,14 @@
       <c r="BR24" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS24" s="142">
+      <c r="BS24" s="137">
         <v>1</v>
       </c>
-      <c r="BT24" s="145" t="s">
+      <c r="BT24" s="140" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B25" s="30" t="s">
         <v>3</v>
       </c>
@@ -7041,7 +7330,7 @@
         <v>100</v>
       </c>
       <c r="Z25" s="28">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA25" s="28">
@@ -7065,7 +7354,7 @@
       <c r="AG25" s="28">
         <v>52000</v>
       </c>
-      <c r="AH25" s="117">
+      <c r="AH25" s="116">
         <v>4</v>
       </c>
       <c r="AI25" s="105">
@@ -7075,24 +7364,24 @@
         <f>AI26</f>
         <v>0.05</v>
       </c>
-      <c r="AK25" s="113">
+      <c r="AK25" s="198">
         <v>0</v>
       </c>
-      <c r="AL25" s="122">
+      <c r="AL25" s="163">
         <v>12</v>
       </c>
-      <c r="AM25" s="41" t="s">
+      <c r="AM25" s="202" t="s">
         <v>83</v>
       </c>
-      <c r="AN25" s="23" t="s">
+      <c r="AN25" s="201" t="s">
         <v>82</v>
       </c>
-      <c r="AO25" s="23" t="s">
+      <c r="AO25" s="201" t="s">
         <v>224</v>
       </c>
       <c r="AP25" s="112"/>
       <c r="AQ25" s="112"/>
-      <c r="AR25" s="147" t="s">
+      <c r="AR25" s="142" t="s">
         <v>184</v>
       </c>
       <c r="AS25" s="41">
@@ -7113,16 +7402,16 @@
       <c r="AX25" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY25" s="151">
+      <c r="AY25" s="146">
         <v>25</v>
       </c>
-      <c r="AZ25" s="148">
+      <c r="AZ25" s="143">
         <v>0.7</v>
       </c>
-      <c r="BA25" s="128">
+      <c r="BA25" s="123">
         <v>0.4</v>
       </c>
-      <c r="BB25" s="132" t="s">
+      <c r="BB25" s="127" t="s">
         <v>81</v>
       </c>
       <c r="BC25" s="53" t="s">
@@ -7152,7 +7441,7 @@
       <c r="BK25" s="52">
         <v>0.3</v>
       </c>
-      <c r="BL25" s="138">
+      <c r="BL25" s="133">
         <v>0.4</v>
       </c>
       <c r="BM25" s="37">
@@ -7171,14 +7460,14 @@
       <c r="BR25" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS25" s="142">
+      <c r="BS25" s="137">
         <v>1</v>
       </c>
-      <c r="BT25" s="144" t="s">
+      <c r="BT25" s="139" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:72" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B26" s="30" t="s">
         <v>3</v>
       </c>
@@ -7252,7 +7541,7 @@
         <v>100</v>
       </c>
       <c r="Z26" s="25">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA26" s="25">
@@ -7285,24 +7574,24 @@
       <c r="AJ26" s="59">
         <v>0.04</v>
       </c>
-      <c r="AK26" s="94">
+      <c r="AK26" s="197">
         <v>0</v>
       </c>
-      <c r="AL26" s="93">
+      <c r="AL26" s="61">
         <v>12</v>
       </c>
-      <c r="AM26" s="41" t="s">
+      <c r="AM26" s="202" t="s">
         <v>78</v>
       </c>
-      <c r="AN26" s="23" t="s">
+      <c r="AN26" s="201" t="s">
         <v>77</v>
       </c>
-      <c r="AO26" s="23" t="s">
+      <c r="AO26" s="201" t="s">
         <v>225</v>
       </c>
       <c r="AP26" s="112"/>
       <c r="AQ26" s="112"/>
-      <c r="AR26" s="147" t="s">
+      <c r="AR26" s="142" t="s">
         <v>13</v>
       </c>
       <c r="AS26" s="41">
@@ -7323,16 +7612,16 @@
       <c r="AX26" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY26" s="151">
+      <c r="AY26" s="146">
         <v>25</v>
       </c>
-      <c r="AZ26" s="148">
+      <c r="AZ26" s="143">
         <v>0.75</v>
       </c>
-      <c r="BA26" s="128">
+      <c r="BA26" s="123">
         <v>0.4</v>
       </c>
-      <c r="BB26" s="134" t="s">
+      <c r="BB26" s="129" t="s">
         <v>76</v>
       </c>
       <c r="BC26" s="40" t="s">
@@ -7362,10 +7651,10 @@
       <c r="BK26" s="36">
         <v>0.7</v>
       </c>
-      <c r="BL26" s="140">
+      <c r="BL26" s="135">
         <v>1.03</v>
       </c>
-      <c r="BM26" s="135">
+      <c r="BM26" s="130">
         <v>59</v>
       </c>
       <c r="BN26" s="36">
@@ -7383,14 +7672,14 @@
       <c r="BR26" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS26" s="142">
+      <c r="BS26" s="137">
         <v>1</v>
       </c>
-      <c r="BT26" s="144" t="s">
+      <c r="BT26" s="139" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
         <v>3</v>
       </c>
@@ -7418,16 +7707,16 @@
       <c r="J27" s="48">
         <v>35</v>
       </c>
-      <c r="K27" s="125">
+      <c r="K27" s="120">
         <v>45</v>
       </c>
-      <c r="L27" s="126">
+      <c r="L27" s="121">
         <v>25</v>
       </c>
       <c r="M27" s="47">
         <v>0</v>
       </c>
-      <c r="N27" s="120">
+      <c r="N27" s="118">
         <v>1000</v>
       </c>
       <c r="O27" s="25">
@@ -7464,7 +7753,7 @@
         <v>100</v>
       </c>
       <c r="Z27" s="25">
-        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA27" s="25">
@@ -7488,7 +7777,7 @@
       <c r="AG27" s="25">
         <v>60000</v>
       </c>
-      <c r="AH27" s="119">
+      <c r="AH27" s="115">
         <v>5</v>
       </c>
       <c r="AI27" s="105">
@@ -7497,24 +7786,24 @@
       <c r="AJ27" s="54">
         <v>0.04</v>
       </c>
-      <c r="AK27" s="123">
+      <c r="AK27" s="167">
         <v>0</v>
       </c>
-      <c r="AL27" s="124">
+      <c r="AL27" s="58">
         <v>12</v>
       </c>
-      <c r="AM27" s="41" t="s">
+      <c r="AM27" s="202" t="s">
         <v>200</v>
       </c>
-      <c r="AN27" s="23" t="s">
+      <c r="AN27" s="201" t="s">
         <v>201</v>
       </c>
-      <c r="AO27" s="23" t="s">
+      <c r="AO27" s="201" t="s">
         <v>202</v>
       </c>
       <c r="AP27" s="112"/>
       <c r="AQ27" s="112"/>
-      <c r="AR27" s="147" t="s">
+      <c r="AR27" s="142" t="s">
         <v>14</v>
       </c>
       <c r="AS27" s="41">
@@ -7535,16 +7824,16 @@
       <c r="AX27" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY27" s="151">
+      <c r="AY27" s="146">
         <v>25</v>
       </c>
-      <c r="AZ27" s="148">
+      <c r="AZ27" s="143">
         <v>0.75</v>
       </c>
-      <c r="BA27" s="128">
+      <c r="BA27" s="123">
         <v>0.4</v>
       </c>
-      <c r="BB27" s="134" t="s">
+      <c r="BB27" s="129" t="s">
         <v>198</v>
       </c>
       <c r="BC27" s="40" t="s">
@@ -7556,7 +7845,7 @@
       <c r="BE27" s="38">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF27" s="135">
+      <c r="BF27" s="130">
         <v>680</v>
       </c>
       <c r="BG27" s="102">
@@ -7574,10 +7863,10 @@
       <c r="BK27" s="36">
         <v>0.7</v>
       </c>
-      <c r="BL27" s="140">
+      <c r="BL27" s="135">
         <v>1.03</v>
       </c>
-      <c r="BM27" s="135">
+      <c r="BM27" s="130">
         <v>59</v>
       </c>
       <c r="BN27" s="36">
@@ -7595,450 +7884,867 @@
       <c r="BR27" s="110">
         <v>0.2</v>
       </c>
-      <c r="BS27" s="143">
+      <c r="BS27" s="138">
         <v>1</v>
       </c>
-      <c r="BT27" s="144" t="s">
+      <c r="BT27" s="139" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="2:72" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="J28" s="167" t="s">
+    <row r="28" spans="1:72" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="182" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="183" t="s">
+        <v>231</v>
+      </c>
+      <c r="D28" s="168" t="s">
+        <v>228</v>
+      </c>
+      <c r="E28" s="168" t="s">
+        <v>204</v>
+      </c>
+      <c r="F28" s="169">
+        <v>12</v>
+      </c>
+      <c r="G28" s="169" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" s="184">
+        <v>700000</v>
+      </c>
+      <c r="I28" s="185">
+        <v>550</v>
+      </c>
+      <c r="J28" s="170">
+        <v>35</v>
+      </c>
+      <c r="K28" s="58">
+        <v>45</v>
+      </c>
+      <c r="L28" s="172">
+        <v>25</v>
+      </c>
+      <c r="M28" s="174">
+        <v>0</v>
+      </c>
+      <c r="N28" s="177">
+        <v>500</v>
+      </c>
+      <c r="O28" s="171">
+        <v>600</v>
+      </c>
+      <c r="P28" s="172">
+        <v>2.5</v>
+      </c>
+      <c r="Q28" s="173">
+        <v>0</v>
+      </c>
+      <c r="R28" s="174">
+        <v>0.02</v>
+      </c>
+      <c r="S28" s="173">
+        <v>20</v>
+      </c>
+      <c r="T28" s="173">
+        <v>0.8</v>
+      </c>
+      <c r="U28" s="177">
+        <v>2</v>
+      </c>
+      <c r="V28" s="175">
+        <v>2.1</v>
+      </c>
+      <c r="W28" s="176">
+        <v>31</v>
+      </c>
+      <c r="X28" s="177">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="Y28" s="173">
+        <v>100</v>
+      </c>
+      <c r="Z28" s="171">
+        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="AA28" s="173">
+        <v>20</v>
+      </c>
+      <c r="AB28" s="173">
+        <v>14</v>
+      </c>
+      <c r="AC28" s="45">
+        <v>475</v>
+      </c>
+      <c r="AD28" s="173">
+        <v>12</v>
+      </c>
+      <c r="AE28" s="173">
+        <v>7</v>
+      </c>
+      <c r="AF28" s="173">
+        <v>10</v>
+      </c>
+      <c r="AG28" s="173">
+        <v>65000</v>
+      </c>
+      <c r="AH28" s="196">
+        <v>6</v>
+      </c>
+      <c r="AI28" s="177">
+        <v>0.04</v>
+      </c>
+      <c r="AJ28" s="186">
+        <v>0.03</v>
+      </c>
+      <c r="AK28" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="199">
+        <v>12</v>
+      </c>
+      <c r="AM28" s="205" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN28" s="206" t="s">
+        <v>233</v>
+      </c>
+      <c r="AO28" s="206" t="s">
+        <v>234</v>
+      </c>
+      <c r="AP28" s="188"/>
+      <c r="AQ28" s="188"/>
+      <c r="AR28" s="178" t="s">
+        <v>197</v>
+      </c>
+      <c r="AS28" s="187">
+        <v>1.05</v>
+      </c>
+      <c r="AT28" s="178">
+        <v>2</v>
+      </c>
+      <c r="AU28" s="178">
+        <v>2</v>
+      </c>
+      <c r="AV28" s="178" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW28" s="178" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX28" s="178" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY28" s="189">
+        <v>25</v>
+      </c>
+      <c r="AZ28" s="178">
+        <v>0.75</v>
+      </c>
+      <c r="BA28" s="178">
+        <v>0.4</v>
+      </c>
+      <c r="BB28" s="190" t="s">
+        <v>235</v>
+      </c>
+      <c r="BC28" s="191" t="s">
+        <v>236</v>
+      </c>
+      <c r="BD28" s="192">
+        <v>1.5E-3</v>
+      </c>
+      <c r="BE28" s="169">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="BF28" s="193">
+        <v>700</v>
+      </c>
+      <c r="BG28" s="194">
+        <f>[1]!dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+        <v>750</v>
+      </c>
+      <c r="BH28" s="179">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="BI28" s="179">
+        <v>9.5</v>
+      </c>
+      <c r="BJ28" s="179">
+        <v>1.7</v>
+      </c>
+      <c r="BK28" s="179">
+        <v>0.7</v>
+      </c>
+      <c r="BL28" s="179">
+        <v>1.03</v>
+      </c>
+      <c r="BM28" s="193">
+        <v>59</v>
+      </c>
+      <c r="BN28" s="179">
+        <v>15</v>
+      </c>
+      <c r="BO28" s="179">
+        <v>0.4</v>
+      </c>
+      <c r="BP28" s="179">
+        <v>25</v>
+      </c>
+      <c r="BQ28" s="180"/>
+      <c r="BR28" s="181">
+        <v>0.2</v>
+      </c>
+      <c r="BS28" s="181">
+        <v>1</v>
+      </c>
+      <c r="BT28" s="195" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:72" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="156" t="s">
         <v>74</v>
       </c>
-      <c r="K28" s="167"/>
-      <c r="L28" s="167"/>
-      <c r="M28" s="167"/>
-      <c r="N28" s="165" t="s">
+      <c r="K29" s="156"/>
+      <c r="L29" s="156"/>
+      <c r="M29" s="156"/>
+      <c r="N29" s="154" t="s">
         <v>73</v>
       </c>
-      <c r="O28" s="166"/>
-      <c r="P28" s="166"/>
-      <c r="Q28" s="166"/>
-      <c r="R28" s="166"/>
-      <c r="S28" s="166"/>
-      <c r="T28" s="166"/>
-      <c r="U28" s="163" t="s">
+      <c r="O29" s="155"/>
+      <c r="P29" s="155"/>
+      <c r="Q29" s="155"/>
+      <c r="R29" s="155"/>
+      <c r="S29" s="155"/>
+      <c r="T29" s="155"/>
+      <c r="U29" s="152" t="s">
         <v>72</v>
       </c>
-      <c r="V28" s="164"/>
-      <c r="W28" s="34" t="s">
+      <c r="V29" s="153"/>
+      <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X28" s="160" t="s">
+      <c r="X29" s="149" t="s">
         <v>70</v>
       </c>
-      <c r="Y28" s="161"/>
-      <c r="Z28" s="161"/>
-      <c r="AA28" s="161"/>
-      <c r="AB28" s="162"/>
-      <c r="AC28" s="153" t="s">
+      <c r="Y29" s="150"/>
+      <c r="Z29" s="150"/>
+      <c r="AA29" s="150"/>
+      <c r="AB29" s="151"/>
+      <c r="AC29" s="148" t="s">
         <v>69</v>
       </c>
-      <c r="AD28" s="153"/>
-      <c r="AE28" s="153"/>
-      <c r="AF28" s="153"/>
-      <c r="AG28" s="153"/>
-      <c r="AI28" s="159" t="s">
+      <c r="AD29" s="148"/>
+      <c r="AE29" s="148"/>
+      <c r="AF29" s="148"/>
+      <c r="AG29" s="148"/>
+      <c r="AH29" s="32"/>
+      <c r="AI29" s="162" t="s">
         <v>68</v>
       </c>
-      <c r="AJ28" s="159"/>
-      <c r="AK28" s="153" t="s">
+      <c r="AJ29" s="162"/>
+      <c r="AK29" s="200" t="s">
         <v>226</v>
       </c>
-      <c r="AL28" s="153"/>
-      <c r="AM28"/>
-      <c r="AN28"/>
-      <c r="AO28"/>
-      <c r="AS28" s="154" t="s">
+      <c r="AL29" s="200"/>
+      <c r="AM29" s="207" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN29" s="208"/>
+      <c r="AO29" s="208"/>
+      <c r="AP29" s="208"/>
+      <c r="AQ29" s="208"/>
+      <c r="AR29" s="209"/>
+      <c r="AS29" s="157" t="s">
         <v>227</v>
       </c>
-      <c r="AT28" s="155"/>
-      <c r="AU28" s="155"/>
-      <c r="AV28" s="155"/>
-      <c r="AW28" s="155"/>
-      <c r="AX28" s="155"/>
-      <c r="AY28" s="156"/>
-      <c r="BF28" s="158" t="s">
+      <c r="AT29" s="158"/>
+      <c r="AU29" s="158"/>
+      <c r="AV29" s="158"/>
+      <c r="AW29" s="158"/>
+      <c r="AX29" s="158"/>
+      <c r="AY29" s="159"/>
+      <c r="AZ29" s="32"/>
+      <c r="BA29" s="32"/>
+      <c r="BB29" s="32"/>
+      <c r="BC29" s="32"/>
+      <c r="BD29" s="32"/>
+      <c r="BE29" s="32"/>
+      <c r="BF29" s="161" t="s">
         <v>67</v>
       </c>
-      <c r="BG28" s="158"/>
-      <c r="BH28" s="158"/>
-      <c r="BI28" s="158"/>
-      <c r="BJ28" s="158"/>
-      <c r="BK28" s="158"/>
-      <c r="BL28" s="158"/>
+      <c r="BG29" s="161"/>
+      <c r="BH29" s="161"/>
+      <c r="BI29" s="161"/>
+      <c r="BJ29" s="161"/>
+      <c r="BK29" s="161"/>
+      <c r="BL29" s="161"/>
+      <c r="BM29" s="32"/>
+      <c r="BN29" s="32"/>
+      <c r="BO29" s="32"/>
+      <c r="BP29" s="32"/>
+      <c r="BQ29" s="32"/>
+      <c r="BR29" s="32"/>
+      <c r="BS29" s="32"/>
     </row>
-    <row r="30" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:72" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B31" s="1" t="s">
+    <row r="31" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:72" s="19" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A32"/>
+      <c r="B32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
+      <c r="AB32"/>
+      <c r="AC32"/>
+      <c r="AD32"/>
+      <c r="AE32"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
+      <c r="AJ32"/>
+      <c r="AK32"/>
+      <c r="AL32"/>
+      <c r="AM32"/>
+      <c r="AN32"/>
+      <c r="AO32"/>
+      <c r="AP32"/>
+      <c r="AQ32"/>
+      <c r="AR32"/>
+      <c r="AS32"/>
+      <c r="AT32"/>
+      <c r="AU32"/>
+      <c r="AV32"/>
+      <c r="AW32"/>
+      <c r="AX32"/>
+      <c r="AY32"/>
+      <c r="AZ32"/>
+      <c r="BA32"/>
+      <c r="BB32"/>
+      <c r="BC32"/>
+      <c r="BD32"/>
+      <c r="BE32"/>
+      <c r="BF32"/>
+      <c r="BG32"/>
+      <c r="BH32"/>
+      <c r="BI32"/>
+      <c r="BJ32"/>
+      <c r="BK32"/>
+      <c r="BL32"/>
+      <c r="BM32"/>
+      <c r="BN32"/>
+      <c r="BO32"/>
+      <c r="BP32"/>
+      <c r="BQ32"/>
+      <c r="BR32"/>
+      <c r="BS32"/>
     </row>
-    <row r="32" spans="2:72" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B32" s="18"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
+    <row r="33" spans="1:71" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="19"/>
+      <c r="Z33" s="19"/>
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="19"/>
+      <c r="AC33" s="19"/>
+      <c r="AD33" s="19"/>
+      <c r="AE33" s="19"/>
+      <c r="AF33" s="19"/>
+      <c r="AG33" s="19"/>
+      <c r="AH33" s="19"/>
+      <c r="AI33" s="19"/>
+      <c r="AJ33" s="19"/>
+      <c r="AK33" s="19"/>
+      <c r="AL33" s="19"/>
+      <c r="AM33" s="19"/>
+      <c r="AN33" s="19"/>
+      <c r="AO33" s="19"/>
+      <c r="AP33" s="19"/>
+      <c r="AQ33" s="19"/>
+      <c r="AR33" s="19"/>
+      <c r="AS33" s="19"/>
+      <c r="AT33" s="19"/>
+      <c r="AU33" s="19"/>
+      <c r="AV33" s="19"/>
+      <c r="AW33" s="19"/>
+      <c r="AX33" s="19"/>
+      <c r="AY33" s="19"/>
+      <c r="AZ33" s="19"/>
+      <c r="BA33" s="19"/>
+      <c r="BB33" s="19"/>
+      <c r="BC33" s="19"/>
+      <c r="BD33" s="19"/>
+      <c r="BE33" s="19"/>
+      <c r="BF33" s="19"/>
+      <c r="BG33" s="19"/>
+      <c r="BH33" s="19"/>
+      <c r="BI33" s="19"/>
+      <c r="BJ33" s="19"/>
+      <c r="BK33" s="19"/>
+      <c r="BL33" s="19"/>
+      <c r="BM33" s="19"/>
+      <c r="BN33" s="19"/>
+      <c r="BO33" s="19"/>
+      <c r="BP33" s="19"/>
+      <c r="BQ33" s="19"/>
+      <c r="BR33" s="19"/>
+      <c r="BS33" s="19"/>
     </row>
-    <row r="33" spans="2:23" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
+    <row r="34" spans="1:71" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D34" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H34" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
+    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C35" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="31">
+      <c r="D35" s="31">
         <v>0.2</v>
       </c>
-      <c r="E34" s="146">
+      <c r="E35" s="141">
         <v>8</v>
       </c>
-      <c r="F34" s="146">
+      <c r="F35" s="141">
         <v>1.5</v>
       </c>
-      <c r="G34" s="146">
+      <c r="G35" s="141">
         <v>1.2</v>
       </c>
-      <c r="H34" s="146">
+      <c r="H35" s="141">
         <v>1.2</v>
       </c>
-      <c r="I34" s="146">
+      <c r="I35" s="141">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B36" s="1" t="s">
+    <row r="36" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:71" s="19" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A37"/>
+      <c r="B37" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37"/>
+      <c r="AC37"/>
+      <c r="AD37"/>
+      <c r="AE37"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
+      <c r="AH37"/>
+      <c r="AI37"/>
+      <c r="AJ37"/>
+      <c r="AK37"/>
+      <c r="AL37"/>
+      <c r="AM37"/>
+      <c r="AN37"/>
+      <c r="AO37"/>
+      <c r="AP37"/>
+      <c r="AQ37"/>
+      <c r="AR37"/>
+      <c r="AS37"/>
+      <c r="AT37"/>
+      <c r="AU37"/>
+      <c r="AV37"/>
+      <c r="AW37"/>
+      <c r="AX37"/>
+      <c r="AY37"/>
+      <c r="AZ37"/>
+      <c r="BA37"/>
+      <c r="BB37"/>
+      <c r="BC37"/>
+      <c r="BD37"/>
+      <c r="BE37"/>
+      <c r="BF37"/>
+      <c r="BG37"/>
+      <c r="BH37"/>
+      <c r="BI37"/>
+      <c r="BJ37"/>
+      <c r="BK37"/>
+      <c r="BL37"/>
+      <c r="BM37"/>
+      <c r="BN37"/>
+      <c r="BO37"/>
+      <c r="BP37"/>
+      <c r="BQ37"/>
+      <c r="BR37"/>
+      <c r="BS37"/>
     </row>
-    <row r="37" spans="2:23" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B37" s="18"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
+    <row r="38" spans="1:71" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19"/>
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="19"/>
+      <c r="AC38" s="19"/>
+      <c r="AD38" s="19"/>
+      <c r="AE38" s="19"/>
+      <c r="AF38" s="19"/>
+      <c r="AG38" s="19"/>
+      <c r="AH38" s="19"/>
+      <c r="AI38" s="19"/>
+      <c r="AJ38" s="19"/>
+      <c r="AK38" s="19"/>
+      <c r="AL38" s="19"/>
+      <c r="AM38" s="19"/>
+      <c r="AN38" s="19"/>
+      <c r="AO38" s="19"/>
+      <c r="AP38" s="19"/>
+      <c r="AQ38" s="19"/>
+      <c r="AR38" s="19"/>
+      <c r="AS38" s="19"/>
+      <c r="AT38" s="19"/>
+      <c r="AU38" s="19"/>
+      <c r="AV38" s="19"/>
+      <c r="AW38" s="19"/>
+      <c r="AX38" s="19"/>
+      <c r="AY38" s="19"/>
+      <c r="AZ38" s="19"/>
+      <c r="BA38" s="19"/>
+      <c r="BB38" s="19"/>
+      <c r="BC38" s="19"/>
+      <c r="BD38" s="19"/>
+      <c r="BE38" s="19"/>
+      <c r="BF38" s="19"/>
+      <c r="BG38" s="19"/>
+      <c r="BH38" s="19"/>
+      <c r="BI38" s="19"/>
+      <c r="BJ38" s="19"/>
+      <c r="BK38" s="19"/>
+      <c r="BL38" s="19"/>
+      <c r="BM38" s="19"/>
+      <c r="BN38" s="19"/>
+      <c r="BO38" s="19"/>
+      <c r="BP38" s="19"/>
+      <c r="BQ38" s="19"/>
+      <c r="BR38" s="19"/>
+      <c r="BS38" s="19"/>
     </row>
-    <row r="38" spans="2:23" ht="169.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
+    <row r="39" spans="1:71" ht="169.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D39" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E39" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F39" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="31">
-        <v>0.25</v>
-      </c>
-      <c r="E39" s="31">
-        <v>1</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D40" s="31">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="E40" s="31">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C41" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E41" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="31">
+      <c r="D42" s="31">
         <v>0.05</v>
       </c>
-      <c r="E41" s="31">
+      <c r="E42" s="31">
         <v>0.4</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F42" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B43" s="1" t="s">
+    <row r="43" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:71" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E44" t="s">
+    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:23" ht="150" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
+    <row r="46" spans="1:71" ht="150" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="J46" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="L46" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M45" s="4" t="s">
+      <c r="M46" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N45" s="4" t="s">
+      <c r="N46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="O45" s="4" t="s">
+      <c r="O46" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P45" s="4" t="s">
+      <c r="P46" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q45" s="4" t="s">
+      <c r="Q46" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R45" s="4" t="s">
+      <c r="R46" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S45" s="4" t="s">
+      <c r="S46" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T45" s="4" t="s">
+      <c r="T46" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U45" s="4" t="s">
+      <c r="U46" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="V45" s="4" t="s">
+      <c r="V46" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="W45" s="4" t="s">
+      <c r="W46" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46">
-        <v>8</v>
-      </c>
-      <c r="E46">
-        <v>571</v>
-      </c>
-      <c r="F46">
-        <v>1714</v>
-      </c>
-      <c r="G46">
-        <v>3429</v>
-      </c>
-      <c r="H46">
-        <v>5714</v>
-      </c>
-      <c r="I46">
-        <v>8571</v>
-      </c>
-      <c r="J46">
-        <v>12000</v>
-      </c>
-      <c r="K46">
-        <v>16000</v>
-      </c>
-      <c r="L46" t="s">
-        <v>20</v>
-      </c>
-      <c r="M46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N46" t="s">
-        <v>20</v>
-      </c>
-      <c r="O46" t="s">
-        <v>20</v>
-      </c>
-      <c r="P46" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>20</v>
-      </c>
-      <c r="R46" t="s">
-        <v>20</v>
-      </c>
-      <c r="S46" t="s">
-        <v>20</v>
-      </c>
-      <c r="T46" t="s">
-        <v>20</v>
-      </c>
-      <c r="U46" t="s">
-        <v>20</v>
-      </c>
-      <c r="V46" t="s">
-        <v>20</v>
-      </c>
-      <c r="W46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D47">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E47">
-        <v>1021</v>
+        <v>571</v>
       </c>
       <c r="F47">
-        <v>3063</v>
+        <v>1714</v>
       </c>
       <c r="G47">
-        <v>6127</v>
+        <v>3429</v>
       </c>
       <c r="H47">
-        <v>10211</v>
+        <v>5714</v>
       </c>
       <c r="I47">
-        <v>15317</v>
+        <v>8069</v>
       </c>
       <c r="J47">
-        <v>21443</v>
+        <v>10895</v>
       </c>
       <c r="K47">
-        <v>28591</v>
-      </c>
-      <c r="L47">
-        <v>36760</v>
-      </c>
-      <c r="M47">
-        <v>45950</v>
+        <v>14192</v>
+      </c>
+      <c r="L47" t="s">
+        <v>20</v>
+      </c>
+      <c r="M47" t="s">
+        <v>20</v>
       </c>
       <c r="N47" t="s">
         <v>20</v>
@@ -8071,42 +8777,42 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D48">
         <v>10</v>
       </c>
       <c r="E48">
-        <v>1661</v>
+        <v>1021</v>
       </c>
       <c r="F48">
-        <v>4983</v>
+        <v>3063</v>
       </c>
       <c r="G48">
-        <v>9966</v>
+        <v>6127</v>
       </c>
       <c r="H48">
-        <v>16610</v>
+        <v>10211</v>
       </c>
       <c r="I48">
-        <v>24915</v>
+        <v>15317</v>
       </c>
       <c r="J48">
-        <v>34881</v>
+        <v>21443</v>
       </c>
       <c r="K48">
-        <v>46508</v>
+        <v>28591</v>
       </c>
       <c r="L48">
-        <v>59796</v>
+        <v>36760</v>
       </c>
       <c r="M48">
-        <v>74745</v>
+        <v>45950</v>
       </c>
       <c r="N48" t="s">
         <v>20</v>
@@ -8144,37 +8850,37 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D49">
         <v>10</v>
       </c>
       <c r="E49">
-        <v>2346</v>
+        <v>1661</v>
       </c>
       <c r="F49">
-        <v>7037</v>
+        <v>4983</v>
       </c>
       <c r="G49">
-        <v>14075</v>
+        <v>9966</v>
       </c>
       <c r="H49">
-        <v>23458</v>
+        <v>16610</v>
       </c>
       <c r="I49">
-        <v>35187</v>
+        <v>24915</v>
       </c>
       <c r="J49">
-        <v>49261</v>
+        <v>34881</v>
       </c>
       <c r="K49">
-        <v>65682</v>
+        <v>46508</v>
       </c>
       <c r="L49">
-        <v>84448</v>
+        <v>59796</v>
       </c>
       <c r="M49">
-        <v>105560</v>
+        <v>74745</v>
       </c>
       <c r="N49" t="s">
         <v>20</v>
@@ -8212,52 +8918,52 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E50">
-        <v>1971</v>
+        <v>2346</v>
       </c>
       <c r="F50">
-        <v>5913</v>
+        <v>7037</v>
       </c>
       <c r="G50">
-        <v>11826</v>
+        <v>14075</v>
       </c>
       <c r="H50">
-        <v>19711</v>
+        <v>23458</v>
       </c>
       <c r="I50">
-        <v>29566</v>
+        <v>35187</v>
       </c>
       <c r="J50">
-        <v>41393</v>
+        <v>49261</v>
       </c>
       <c r="K50">
-        <v>55190</v>
+        <v>65682</v>
       </c>
       <c r="L50">
-        <v>70959</v>
+        <v>84448</v>
       </c>
       <c r="M50">
-        <v>88698</v>
-      </c>
-      <c r="N50">
-        <v>108409</v>
-      </c>
-      <c r="O50">
-        <v>130091</v>
-      </c>
-      <c r="P50">
-        <v>153744</v>
-      </c>
-      <c r="Q50">
-        <v>179368</v>
-      </c>
-      <c r="R50">
-        <v>206963</v>
+        <v>105560</v>
+      </c>
+      <c r="N50" t="s">
+        <v>20</v>
+      </c>
+      <c r="O50" t="s">
+        <v>20</v>
+      </c>
+      <c r="P50" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>20</v>
+      </c>
+      <c r="R50" t="s">
+        <v>20</v>
       </c>
       <c r="S50" t="s">
         <v>20</v>
@@ -8280,52 +8986,52 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D51">
         <v>15</v>
       </c>
       <c r="E51">
-        <v>2453</v>
+        <v>1971</v>
       </c>
       <c r="F51">
-        <v>7359</v>
+        <v>5913</v>
       </c>
       <c r="G51">
-        <v>14718</v>
+        <v>11826</v>
       </c>
       <c r="H51">
-        <v>24531</v>
+        <v>19711</v>
       </c>
       <c r="I51">
-        <v>36796</v>
+        <v>29566</v>
       </c>
       <c r="J51">
-        <v>51515</v>
+        <v>41393</v>
       </c>
       <c r="K51">
-        <v>68686</v>
+        <v>55190</v>
       </c>
       <c r="L51">
-        <v>88311</v>
+        <v>70959</v>
       </c>
       <c r="M51">
-        <v>110388</v>
+        <v>88698</v>
       </c>
       <c r="N51">
-        <v>134919</v>
+        <v>108409</v>
       </c>
       <c r="O51">
-        <v>161903</v>
+        <v>130091</v>
       </c>
       <c r="P51">
-        <v>191340</v>
+        <v>153744</v>
       </c>
       <c r="Q51">
-        <v>223230</v>
+        <v>179368</v>
       </c>
       <c r="R51">
-        <v>257573</v>
+        <v>206963</v>
       </c>
       <c r="S51" t="s">
         <v>20</v>
@@ -8348,52 +9054,52 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52">
         <v>15</v>
       </c>
       <c r="E52">
-        <v>2952</v>
+        <v>2453</v>
       </c>
       <c r="F52">
-        <v>8855</v>
+        <v>7359</v>
       </c>
       <c r="G52">
-        <v>17709</v>
+        <v>14718</v>
       </c>
       <c r="H52">
-        <v>29516</v>
+        <v>24531</v>
       </c>
       <c r="I52">
-        <v>44274</v>
+        <v>36796</v>
       </c>
       <c r="J52">
-        <v>61983</v>
+        <v>51515</v>
       </c>
       <c r="K52">
-        <v>82644</v>
+        <v>68686</v>
       </c>
       <c r="L52">
-        <v>106257</v>
+        <v>88311</v>
       </c>
       <c r="M52">
-        <v>132821</v>
+        <v>110388</v>
       </c>
       <c r="N52">
-        <v>162336</v>
+        <v>134919</v>
       </c>
       <c r="O52">
-        <v>194804</v>
+        <v>161903</v>
       </c>
       <c r="P52">
-        <v>230223</v>
+        <v>191340</v>
       </c>
       <c r="Q52">
-        <v>268593</v>
+        <v>223230</v>
       </c>
       <c r="R52">
-        <v>309915</v>
+        <v>257573</v>
       </c>
       <c r="S52" t="s">
         <v>20</v>
@@ -8416,67 +9122,67 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D53">
+        <v>15</v>
+      </c>
+      <c r="E53">
+        <v>2952</v>
+      </c>
+      <c r="F53">
+        <v>8855</v>
+      </c>
+      <c r="G53">
+        <v>17709</v>
+      </c>
+      <c r="H53">
+        <v>29516</v>
+      </c>
+      <c r="I53">
+        <v>44274</v>
+      </c>
+      <c r="J53">
+        <v>61983</v>
+      </c>
+      <c r="K53">
+        <v>82644</v>
+      </c>
+      <c r="L53">
+        <v>106257</v>
+      </c>
+      <c r="M53">
+        <v>132821</v>
+      </c>
+      <c r="N53">
+        <v>162336</v>
+      </c>
+      <c r="O53">
+        <v>194804</v>
+      </c>
+      <c r="P53">
+        <v>230223</v>
+      </c>
+      <c r="Q53">
+        <v>268593</v>
+      </c>
+      <c r="R53">
+        <v>309915</v>
+      </c>
+      <c r="S53" t="s">
         <v>20</v>
       </c>
-      <c r="E53">
-        <v>2553</v>
-      </c>
-      <c r="F53">
-        <v>7658</v>
-      </c>
-      <c r="G53">
-        <v>15317</v>
-      </c>
-      <c r="H53">
-        <v>25528</v>
-      </c>
-      <c r="I53">
-        <v>38292</v>
-      </c>
-      <c r="J53">
-        <v>53609</v>
-      </c>
-      <c r="K53">
-        <v>71478</v>
-      </c>
-      <c r="L53">
-        <v>91900</v>
-      </c>
-      <c r="M53">
-        <v>114876</v>
-      </c>
-      <c r="N53">
-        <v>140403</v>
-      </c>
-      <c r="O53">
-        <v>168484</v>
-      </c>
-      <c r="P53">
-        <v>199118</v>
-      </c>
-      <c r="Q53">
-        <v>232304</v>
-      </c>
-      <c r="R53">
-        <v>268043</v>
-      </c>
-      <c r="S53">
-        <v>306335</v>
-      </c>
-      <c r="T53">
-        <v>347179</v>
-      </c>
-      <c r="U53">
-        <v>390577</v>
-      </c>
-      <c r="V53">
-        <v>436527</v>
-      </c>
-      <c r="W53">
-        <v>485030</v>
+      <c r="T53" t="s">
+        <v>20</v>
+      </c>
+      <c r="U53" t="s">
+        <v>20</v>
+      </c>
+      <c r="V53" t="s">
+        <v>20</v>
+      </c>
+      <c r="W53" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
@@ -8484,67 +9190,67 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="D54">
         <v>20</v>
       </c>
-      <c r="E54" s="99">
-        <v>2940</v>
-      </c>
-      <c r="F54" s="99">
-        <v>8821</v>
-      </c>
-      <c r="G54" s="99">
-        <v>17642</v>
-      </c>
-      <c r="H54" s="99">
-        <v>29403</v>
-      </c>
-      <c r="I54" s="99">
-        <v>44105</v>
-      </c>
-      <c r="J54" s="99">
-        <v>61747</v>
-      </c>
-      <c r="K54" s="99">
-        <v>82329</v>
-      </c>
-      <c r="L54" s="99">
-        <v>105851</v>
-      </c>
-      <c r="M54" s="99">
-        <v>132314</v>
-      </c>
-      <c r="N54" s="99">
-        <v>161717</v>
-      </c>
-      <c r="O54" s="99">
-        <v>194061</v>
-      </c>
-      <c r="P54" s="99">
-        <v>229345</v>
-      </c>
-      <c r="Q54" s="99">
-        <v>267569</v>
-      </c>
-      <c r="R54" s="99">
-        <v>308733</v>
-      </c>
-      <c r="S54" s="99">
-        <v>352838</v>
-      </c>
-      <c r="T54" s="99">
-        <v>399883</v>
-      </c>
-      <c r="U54" s="99">
-        <v>449868</v>
-      </c>
-      <c r="V54" s="99">
-        <v>502794</v>
-      </c>
-      <c r="W54" s="99">
-        <v>558660</v>
+      <c r="E54">
+        <v>2553</v>
+      </c>
+      <c r="F54">
+        <v>7658</v>
+      </c>
+      <c r="G54">
+        <v>15317</v>
+      </c>
+      <c r="H54">
+        <v>25528</v>
+      </c>
+      <c r="I54">
+        <v>38292</v>
+      </c>
+      <c r="J54">
+        <v>53609</v>
+      </c>
+      <c r="K54">
+        <v>71478</v>
+      </c>
+      <c r="L54">
+        <v>91900</v>
+      </c>
+      <c r="M54">
+        <v>114876</v>
+      </c>
+      <c r="N54">
+        <v>140403</v>
+      </c>
+      <c r="O54">
+        <v>168484</v>
+      </c>
+      <c r="P54">
+        <v>199118</v>
+      </c>
+      <c r="Q54">
+        <v>232304</v>
+      </c>
+      <c r="R54">
+        <v>268043</v>
+      </c>
+      <c r="S54">
+        <v>306335</v>
+      </c>
+      <c r="T54">
+        <v>347179</v>
+      </c>
+      <c r="U54">
+        <v>390577</v>
+      </c>
+      <c r="V54">
+        <v>436527</v>
+      </c>
+      <c r="W54">
+        <v>485030</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
@@ -8552,67 +9258,67 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D55">
         <v>20</v>
       </c>
-      <c r="E55">
-        <v>3337</v>
-      </c>
-      <c r="F55">
-        <v>10010</v>
-      </c>
-      <c r="G55">
-        <v>20020</v>
-      </c>
-      <c r="H55">
-        <v>33366</v>
-      </c>
-      <c r="I55">
-        <v>50049</v>
-      </c>
-      <c r="J55">
-        <v>70069</v>
-      </c>
-      <c r="K55">
-        <v>93426</v>
-      </c>
-      <c r="L55">
-        <v>120119</v>
-      </c>
-      <c r="M55">
-        <v>150148</v>
-      </c>
-      <c r="N55">
-        <v>183515</v>
-      </c>
-      <c r="O55">
-        <v>220218</v>
-      </c>
-      <c r="P55">
-        <v>260257</v>
-      </c>
-      <c r="Q55">
-        <v>303633</v>
-      </c>
-      <c r="R55">
-        <v>350346</v>
-      </c>
-      <c r="S55">
-        <v>400396</v>
-      </c>
-      <c r="T55">
-        <v>453782</v>
-      </c>
-      <c r="U55">
-        <v>510505</v>
-      </c>
-      <c r="V55">
-        <v>570564</v>
-      </c>
-      <c r="W55">
-        <v>633960</v>
+      <c r="E55" s="99">
+        <v>2940</v>
+      </c>
+      <c r="F55" s="99">
+        <v>8821</v>
+      </c>
+      <c r="G55" s="99">
+        <v>17642</v>
+      </c>
+      <c r="H55" s="99">
+        <v>29403</v>
+      </c>
+      <c r="I55" s="99">
+        <v>44105</v>
+      </c>
+      <c r="J55" s="99">
+        <v>61747</v>
+      </c>
+      <c r="K55" s="99">
+        <v>82329</v>
+      </c>
+      <c r="L55" s="99">
+        <v>105851</v>
+      </c>
+      <c r="M55" s="99">
+        <v>132314</v>
+      </c>
+      <c r="N55" s="99">
+        <v>161717</v>
+      </c>
+      <c r="O55" s="99">
+        <v>194061</v>
+      </c>
+      <c r="P55" s="99">
+        <v>229345</v>
+      </c>
+      <c r="Q55" s="99">
+        <v>267569</v>
+      </c>
+      <c r="R55" s="99">
+        <v>308733</v>
+      </c>
+      <c r="S55" s="99">
+        <v>352838</v>
+      </c>
+      <c r="T55" s="99">
+        <v>399883</v>
+      </c>
+      <c r="U55" s="99">
+        <v>449868</v>
+      </c>
+      <c r="V55" s="99">
+        <v>502794</v>
+      </c>
+      <c r="W55" s="99">
+        <v>558660</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
@@ -8620,67 +9326,67 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D56">
         <v>20</v>
       </c>
       <c r="E56">
-        <v>3741</v>
+        <v>3337</v>
       </c>
       <c r="F56">
-        <v>11223</v>
+        <v>10010</v>
       </c>
       <c r="G56">
-        <v>22445</v>
+        <v>20020</v>
       </c>
       <c r="H56">
-        <v>37409</v>
+        <v>33366</v>
       </c>
       <c r="I56">
-        <v>56113</v>
+        <v>50049</v>
       </c>
       <c r="J56">
-        <v>78559</v>
+        <v>70069</v>
       </c>
       <c r="K56">
-        <v>104745</v>
+        <v>93426</v>
       </c>
       <c r="L56">
-        <v>134672</v>
+        <v>120119</v>
       </c>
       <c r="M56">
-        <v>168340</v>
+        <v>150148</v>
       </c>
       <c r="N56">
-        <v>205749</v>
+        <v>183515</v>
       </c>
       <c r="O56">
-        <v>246899</v>
+        <v>220218</v>
       </c>
       <c r="P56">
-        <v>291790</v>
+        <v>260257</v>
       </c>
       <c r="Q56">
-        <v>340421</v>
+        <v>303633</v>
       </c>
       <c r="R56">
-        <v>392794</v>
+        <v>350346</v>
       </c>
       <c r="S56">
-        <v>448907</v>
+        <v>400396</v>
       </c>
       <c r="T56">
-        <v>508762</v>
+        <v>453782</v>
       </c>
       <c r="U56">
-        <v>572357</v>
+        <v>510505</v>
       </c>
       <c r="V56">
-        <v>639693</v>
+        <v>570564</v>
       </c>
       <c r="W56">
-        <v>710770</v>
+        <v>633960</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
@@ -8688,121 +9394,270 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>197</v>
+        <v>14</v>
       </c>
       <c r="D57">
         <v>20</v>
       </c>
       <c r="E57">
+        <v>3741</v>
+      </c>
+      <c r="F57">
+        <v>11223</v>
+      </c>
+      <c r="G57">
+        <v>22445</v>
+      </c>
+      <c r="H57">
+        <v>37409</v>
+      </c>
+      <c r="I57">
+        <v>56113</v>
+      </c>
+      <c r="J57">
+        <v>78559</v>
+      </c>
+      <c r="K57">
+        <v>104745</v>
+      </c>
+      <c r="L57">
+        <v>134672</v>
+      </c>
+      <c r="M57">
+        <v>168340</v>
+      </c>
+      <c r="N57">
+        <v>205749</v>
+      </c>
+      <c r="O57">
+        <v>246899</v>
+      </c>
+      <c r="P57">
+        <v>291790</v>
+      </c>
+      <c r="Q57">
+        <v>340421</v>
+      </c>
+      <c r="R57">
+        <v>392794</v>
+      </c>
+      <c r="S57">
+        <v>448907</v>
+      </c>
+      <c r="T57">
+        <v>508762</v>
+      </c>
+      <c r="U57">
+        <v>572357</v>
+      </c>
+      <c r="V57">
+        <v>639693</v>
+      </c>
+      <c r="W57">
+        <v>710770</v>
+      </c>
+    </row>
+    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58">
+        <v>20</v>
+      </c>
+      <c r="E58">
         <v>4153</v>
       </c>
-      <c r="F57">
+      <c r="F58">
         <v>12458</v>
       </c>
-      <c r="G57">
+      <c r="G58">
         <v>24916</v>
       </c>
-      <c r="H57">
+      <c r="H58">
         <v>41526</v>
       </c>
-      <c r="I57">
+      <c r="I58">
         <v>62289</v>
       </c>
-      <c r="J57">
+      <c r="J58">
         <v>87205</v>
       </c>
-      <c r="K57">
+      <c r="K58">
         <v>116274</v>
       </c>
-      <c r="L57">
+      <c r="L58">
         <v>149495</v>
       </c>
-      <c r="M57">
+      <c r="M58">
         <v>186868</v>
       </c>
-      <c r="N57">
+      <c r="N58">
         <v>228395</v>
       </c>
-      <c r="O57">
+      <c r="O58">
         <v>274074</v>
       </c>
-      <c r="P57">
+      <c r="P58">
         <v>323905</v>
       </c>
-      <c r="Q57">
+      <c r="Q58">
         <v>377889</v>
       </c>
-      <c r="R57">
+      <c r="R58">
         <v>436026</v>
       </c>
-      <c r="S57">
+      <c r="S58">
         <v>498316</v>
       </c>
-      <c r="T57">
+      <c r="T58">
         <v>564758</v>
       </c>
-      <c r="U57">
+      <c r="U58">
         <v>635353</v>
       </c>
-      <c r="V57">
+      <c r="V58">
         <v>710100</v>
       </c>
-      <c r="W57">
+      <c r="W58">
         <v>789000</v>
+      </c>
+    </row>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>231</v>
+      </c>
+      <c r="D59">
+        <v>20</v>
+      </c>
+      <c r="E59" s="210">
+        <v>4571</v>
+      </c>
+      <c r="F59" s="211">
+        <v>13714</v>
+      </c>
+      <c r="G59" s="211">
+        <v>27428</v>
+      </c>
+      <c r="H59" s="211">
+        <v>45713</v>
+      </c>
+      <c r="I59" s="211">
+        <v>68569</v>
+      </c>
+      <c r="J59" s="211">
+        <v>95997</v>
+      </c>
+      <c r="K59" s="211">
+        <v>127995</v>
+      </c>
+      <c r="L59" s="211">
+        <v>164565</v>
+      </c>
+      <c r="M59" s="211">
+        <v>205707</v>
+      </c>
+      <c r="N59" s="211">
+        <v>251419</v>
+      </c>
+      <c r="O59" s="211">
+        <v>301703</v>
+      </c>
+      <c r="P59" s="211">
+        <v>356559</v>
+      </c>
+      <c r="Q59" s="211">
+        <v>415985</v>
+      </c>
+      <c r="R59" s="211">
+        <v>479983</v>
+      </c>
+      <c r="S59" s="211">
+        <v>548552</v>
+      </c>
+      <c r="T59" s="211">
+        <v>621692</v>
+      </c>
+      <c r="U59" s="211">
+        <v>699403</v>
+      </c>
+      <c r="V59" s="211">
+        <v>781686</v>
+      </c>
+      <c r="W59" s="211">
+        <v>868540</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="AC28:AG28"/>
-    <mergeCell ref="X28:AB28"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="N28:T28"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="AK28:AL28"/>
-    <mergeCell ref="AS28:AY28"/>
+  <mergeCells count="11">
+    <mergeCell ref="AK29:AL29"/>
+    <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
-    <mergeCell ref="BF28:BL28"/>
-    <mergeCell ref="AI28:AJ28"/>
+    <mergeCell ref="BF29:BL29"/>
+    <mergeCell ref="AI29:AJ29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="117" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="116" priority="11"/>
+  <conditionalFormatting sqref="C5:C10">
+    <cfRule type="duplicateValues" dxfId="20" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="115" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="114" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="113" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="112" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="110" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="109" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="108" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="107" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BT28">
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ28">
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D27">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D28">
       <formula1>INDIRECT("dragonTierDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D46:D57 F46:W57 E47:E57"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D34:D35 D39:D41">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D47:D59 E48:E58 F47:W59"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D35:D36 D40:D42">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Fixing merges. Now we have in 1.32: new economy + new disguises + dark dragon
Former-commit-id: c574580732fe1bd147a130324a30a30185c8a30d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1749,51 +1746,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1899,26 +1851,77 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1928,358 +1931,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="122">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3633,6 +3290,172 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -3850,6 +3673,30 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -4414,6 +4261,156 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4427,119 +4424,106 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="dragons"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="121" dataDxfId="119" headerRowBorderDxfId="120" tableBorderDxfId="118" totalsRowBorderDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="106" dataDxfId="104" headerRowBorderDxfId="105" tableBorderDxfId="103" totalsRowBorderDxfId="102">
   <autoFilter ref="B15:BT28"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="116"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="115"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="114"/>
-    <tableColumn id="65" name="[type]" dataDxfId="113"/>
-    <tableColumn id="3" name="[order]" dataDxfId="112"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="111"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="110"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="109"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="108"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="107"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="106"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="105"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="104"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="103"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="102"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="101"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="100"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="99"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="98"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="97"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="96"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="95"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="94"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="93"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="6">
-      <calculatedColumnFormula>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="101"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="100"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="99"/>
+    <tableColumn id="65" name="[type]" dataDxfId="98"/>
+    <tableColumn id="3" name="[order]" dataDxfId="97"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="96"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="95"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="94"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="93"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="92"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="91"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="90"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="89"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="88"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="87"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="86"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="85"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="84"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="83"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="82"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="81"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="80"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="79"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="78"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="77">
+      <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="92"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="91"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="90"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="89"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="88"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="87"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="86"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="85"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="84"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="83">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="76"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="75"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="74"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="73"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="72"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="71"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="70"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="69"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="68"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="67">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="5"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="4"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="3"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="2"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="0"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="1"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="82"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="81"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="80"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="79"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="78"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="77"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="76"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="75"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="74"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="73"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="72"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="71">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="66"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="65"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="64"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="63"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="62"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="61"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="60"/>
+    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="59"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="58"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="57"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="56"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="55"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="54"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="53"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="52"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="51"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="50"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="49">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="70">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="48">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="69"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="68"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="67"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="66">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="47"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="46"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="45"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="44">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="65"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="64"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="63"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="62"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="61"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="60"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="59"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="58"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="57"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="56"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="55"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="54"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="53"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="43"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="42"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="41"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="40"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="39"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="38"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="37"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="36"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="35"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="34"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="33"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="32"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G10" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G10" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="B4:G10"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="48"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="26"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="47"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="46"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="45">
+    <tableColumn id="10" name="[icon]" dataDxfId="25"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="24"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="23">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4548,24 +4532,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:I35" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:I35" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="B34:I35"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="18"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="38"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="37"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="36"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="35"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="34"/>
+    <tableColumn id="8" name="[superfuryMax]" dataDxfId="16"/>
+    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="15"/>
+    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="14"/>
+    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="13"/>
+    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B46:W59"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -4596,14 +4580,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B39:F42"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="23"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="22"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4877,8 +4861,8 @@
   </sheetPr>
   <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BG28" sqref="BG28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5075,13 +5059,13 @@
       </c>
     </row>
     <row r="10" spans="2:72" x14ac:dyDescent="0.25">
-      <c r="B10" s="165" t="s">
+      <c r="B10" s="150" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="85" t="s">
         <v>228</v>
       </c>
-      <c r="D10" s="166">
+      <c r="D10" s="151">
         <v>5</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -5090,7 +5074,7 @@
       <c r="F10" s="15">
         <v>4</v>
       </c>
-      <c r="G10" s="164" t="s">
+      <c r="G10" s="149" t="s">
         <v>230</v>
       </c>
     </row>
@@ -5144,10 +5128,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="160"/>
-      <c r="AP14" s="160"/>
-      <c r="AQ14" s="160"/>
-      <c r="AR14" s="160"/>
+      <c r="AO14" s="206"/>
+      <c r="AP14" s="206"/>
+      <c r="AQ14" s="206"/>
+      <c r="AR14" s="206"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -5436,7 +5420,7 @@
         <v>100</v>
       </c>
       <c r="Z16" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA16" s="28">
@@ -5470,19 +5454,19 @@
         <f t="shared" ref="AJ16:AJ23" si="0">AI17</f>
         <v>0.19</v>
       </c>
-      <c r="AK16" s="197">
+      <c r="AK16" s="182">
         <v>0</v>
       </c>
       <c r="AL16" s="61">
         <v>12</v>
       </c>
-      <c r="AM16" s="201" t="s">
+      <c r="AM16" s="185" t="s">
         <v>120</v>
       </c>
-      <c r="AN16" s="201" t="s">
+      <c r="AN16" s="185" t="s">
         <v>119</v>
       </c>
-      <c r="AO16" s="201" t="s">
+      <c r="AO16" s="185" t="s">
         <v>217</v>
       </c>
       <c r="AP16" s="112"/>
@@ -5647,7 +5631,7 @@
         <v>100</v>
       </c>
       <c r="Z17" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA17" s="28">
@@ -5681,19 +5665,19 @@
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="AK17" s="197">
+      <c r="AK17" s="182">
         <v>0</v>
       </c>
       <c r="AL17" s="61">
         <v>12</v>
       </c>
-      <c r="AM17" s="202" t="s">
+      <c r="AM17" s="186" t="s">
         <v>116</v>
       </c>
-      <c r="AN17" s="201" t="s">
+      <c r="AN17" s="185" t="s">
         <v>115</v>
       </c>
-      <c r="AO17" s="201" t="s">
+      <c r="AO17" s="185" t="s">
         <v>218</v>
       </c>
       <c r="AP17" s="112"/>
@@ -5856,7 +5840,7 @@
         <v>100</v>
       </c>
       <c r="Z18" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA18" s="28">
@@ -5890,19 +5874,19 @@
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="AK18" s="198">
+      <c r="AK18" s="183">
         <v>0</v>
       </c>
-      <c r="AL18" s="163">
+      <c r="AL18" s="148">
         <v>12</v>
       </c>
-      <c r="AM18" s="202" t="s">
+      <c r="AM18" s="186" t="s">
         <v>112</v>
       </c>
-      <c r="AN18" s="201" t="s">
+      <c r="AN18" s="185" t="s">
         <v>111</v>
       </c>
-      <c r="AO18" s="201" t="s">
+      <c r="AO18" s="185" t="s">
         <v>110</v>
       </c>
       <c r="AP18" s="112"/>
@@ -6067,7 +6051,7 @@
         <v>100</v>
       </c>
       <c r="Z19" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA19" s="28">
@@ -6101,19 +6085,19 @@
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="AK19" s="197">
+      <c r="AK19" s="182">
         <v>0</v>
       </c>
       <c r="AL19" s="61">
         <v>12</v>
       </c>
-      <c r="AM19" s="202" t="s">
+      <c r="AM19" s="186" t="s">
         <v>106</v>
       </c>
-      <c r="AN19" s="201" t="s">
+      <c r="AN19" s="185" t="s">
         <v>105</v>
       </c>
-      <c r="AO19" s="201" t="s">
+      <c r="AO19" s="185" t="s">
         <v>219</v>
       </c>
       <c r="AP19" s="112"/>
@@ -6276,7 +6260,7 @@
         <v>100</v>
       </c>
       <c r="Z20" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA20" s="28">
@@ -6310,19 +6294,19 @@
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="AK20" s="197">
+      <c r="AK20" s="182">
         <v>0</v>
       </c>
       <c r="AL20" s="61">
         <v>12</v>
       </c>
-      <c r="AM20" s="202" t="s">
+      <c r="AM20" s="186" t="s">
         <v>102</v>
       </c>
-      <c r="AN20" s="201" t="s">
+      <c r="AN20" s="185" t="s">
         <v>101</v>
       </c>
-      <c r="AO20" s="201" t="s">
+      <c r="AO20" s="185" t="s">
         <v>220</v>
       </c>
       <c r="AP20" s="112"/>
@@ -6487,7 +6471,7 @@
         <v>100</v>
       </c>
       <c r="Z21" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA21" s="28">
@@ -6521,19 +6505,19 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="AK21" s="197">
+      <c r="AK21" s="182">
         <v>0</v>
       </c>
       <c r="AL21" s="61">
         <v>12</v>
       </c>
-      <c r="AM21" s="202" t="s">
+      <c r="AM21" s="186" t="s">
         <v>98</v>
       </c>
-      <c r="AN21" s="201" t="s">
+      <c r="AN21" s="185" t="s">
         <v>97</v>
       </c>
-      <c r="AO21" s="201" t="s">
+      <c r="AO21" s="185" t="s">
         <v>96</v>
       </c>
       <c r="AP21" s="112"/>
@@ -6698,7 +6682,7 @@
         <v>100</v>
       </c>
       <c r="Z22" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA22" s="28">
@@ -6732,19 +6716,19 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK22" s="197">
+      <c r="AK22" s="182">
         <v>0</v>
       </c>
       <c r="AL22" s="61">
         <v>12</v>
       </c>
-      <c r="AM22" s="202" t="s">
+      <c r="AM22" s="186" t="s">
         <v>92</v>
       </c>
-      <c r="AN22" s="201" t="s">
+      <c r="AN22" s="185" t="s">
         <v>91</v>
       </c>
-      <c r="AO22" s="201" t="s">
+      <c r="AO22" s="185" t="s">
         <v>221</v>
       </c>
       <c r="AP22" s="112"/>
@@ -6909,7 +6893,7 @@
         <v>100</v>
       </c>
       <c r="Z23" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA23" s="28">
@@ -6943,19 +6927,19 @@
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="AK23" s="198">
+      <c r="AK23" s="183">
         <v>0</v>
       </c>
-      <c r="AL23" s="163">
+      <c r="AL23" s="148">
         <v>12</v>
       </c>
-      <c r="AM23" s="202" t="s">
+      <c r="AM23" s="186" t="s">
         <v>88</v>
       </c>
-      <c r="AN23" s="201" t="s">
+      <c r="AN23" s="185" t="s">
         <v>87</v>
       </c>
-      <c r="AO23" s="201" t="s">
+      <c r="AO23" s="185" t="s">
         <v>222</v>
       </c>
       <c r="AP23" s="112"/>
@@ -7120,7 +7104,7 @@
         <v>100</v>
       </c>
       <c r="Z24" s="46">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA24" s="46">
@@ -7153,19 +7137,19 @@
       <c r="AJ24" s="103">
         <v>0.05</v>
       </c>
-      <c r="AK24" s="198">
+      <c r="AK24" s="183">
         <v>0</v>
       </c>
-      <c r="AL24" s="163">
+      <c r="AL24" s="148">
         <v>12</v>
       </c>
-      <c r="AM24" s="203" t="s">
+      <c r="AM24" s="187" t="s">
         <v>185</v>
       </c>
-      <c r="AN24" s="204" t="s">
+      <c r="AN24" s="188" t="s">
         <v>186</v>
       </c>
-      <c r="AO24" s="204" t="s">
+      <c r="AO24" s="188" t="s">
         <v>223</v>
       </c>
       <c r="AP24" s="112"/>
@@ -7330,7 +7314,7 @@
         <v>100</v>
       </c>
       <c r="Z25" s="28">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA25" s="28">
@@ -7364,19 +7348,19 @@
         <f>AI26</f>
         <v>0.05</v>
       </c>
-      <c r="AK25" s="198">
+      <c r="AK25" s="183">
         <v>0</v>
       </c>
-      <c r="AL25" s="163">
+      <c r="AL25" s="148">
         <v>12</v>
       </c>
-      <c r="AM25" s="202" t="s">
+      <c r="AM25" s="186" t="s">
         <v>83</v>
       </c>
-      <c r="AN25" s="201" t="s">
+      <c r="AN25" s="185" t="s">
         <v>82</v>
       </c>
-      <c r="AO25" s="201" t="s">
+      <c r="AO25" s="185" t="s">
         <v>224</v>
       </c>
       <c r="AP25" s="112"/>
@@ -7541,7 +7525,7 @@
         <v>100</v>
       </c>
       <c r="Z26" s="25">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA26" s="25">
@@ -7574,19 +7558,19 @@
       <c r="AJ26" s="59">
         <v>0.04</v>
       </c>
-      <c r="AK26" s="197">
+      <c r="AK26" s="182">
         <v>0</v>
       </c>
       <c r="AL26" s="61">
         <v>12</v>
       </c>
-      <c r="AM26" s="202" t="s">
+      <c r="AM26" s="186" t="s">
         <v>78</v>
       </c>
-      <c r="AN26" s="201" t="s">
+      <c r="AN26" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="AO26" s="201" t="s">
+      <c r="AO26" s="185" t="s">
         <v>225</v>
       </c>
       <c r="AP26" s="112"/>
@@ -7753,7 +7737,7 @@
         <v>100</v>
       </c>
       <c r="Z27" s="25">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
       <c r="AA27" s="25">
@@ -7786,19 +7770,19 @@
       <c r="AJ27" s="54">
         <v>0.04</v>
       </c>
-      <c r="AK27" s="167">
+      <c r="AK27" s="152">
         <v>0</v>
       </c>
       <c r="AL27" s="58">
         <v>12</v>
       </c>
-      <c r="AM27" s="202" t="s">
+      <c r="AM27" s="186" t="s">
         <v>200</v>
       </c>
-      <c r="AN27" s="201" t="s">
+      <c r="AN27" s="185" t="s">
         <v>201</v>
       </c>
-      <c r="AO27" s="201" t="s">
+      <c r="AO27" s="185" t="s">
         <v>202</v>
       </c>
       <c r="AP27" s="112"/>
@@ -7892,213 +7876,212 @@
       </c>
     </row>
     <row r="28" spans="1:72" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="182" t="s">
+      <c r="B28" s="167" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="183" t="s">
+      <c r="C28" s="168" t="s">
         <v>231</v>
       </c>
-      <c r="D28" s="168" t="s">
+      <c r="D28" s="153" t="s">
         <v>228</v>
       </c>
-      <c r="E28" s="168" t="s">
+      <c r="E28" s="153" t="s">
         <v>204</v>
       </c>
-      <c r="F28" s="169">
+      <c r="F28" s="154">
         <v>12</v>
       </c>
-      <c r="G28" s="169" t="s">
+      <c r="G28" s="154" t="s">
         <v>197</v>
       </c>
-      <c r="H28" s="184">
+      <c r="H28" s="169">
         <v>700000</v>
       </c>
-      <c r="I28" s="185">
+      <c r="I28" s="170">
         <v>550</v>
       </c>
-      <c r="J28" s="170">
+      <c r="J28" s="155">
         <v>35</v>
       </c>
       <c r="K28" s="58">
         <v>45</v>
       </c>
-      <c r="L28" s="172">
+      <c r="L28" s="157">
         <v>25</v>
       </c>
-      <c r="M28" s="174">
+      <c r="M28" s="159">
         <v>0</v>
       </c>
-      <c r="N28" s="177">
+      <c r="N28" s="162">
         <v>500</v>
       </c>
-      <c r="O28" s="171">
+      <c r="O28" s="156">
         <v>600</v>
       </c>
-      <c r="P28" s="172">
+      <c r="P28" s="157">
         <v>2.5</v>
       </c>
-      <c r="Q28" s="173">
+      <c r="Q28" s="158">
         <v>0</v>
       </c>
-      <c r="R28" s="174">
+      <c r="R28" s="159">
         <v>0.02</v>
       </c>
-      <c r="S28" s="173">
+      <c r="S28" s="158">
         <v>20</v>
       </c>
-      <c r="T28" s="173">
+      <c r="T28" s="158">
         <v>0.8</v>
       </c>
-      <c r="U28" s="177">
+      <c r="U28" s="162">
         <v>2</v>
       </c>
-      <c r="V28" s="175">
+      <c r="V28" s="160">
         <v>2.1</v>
       </c>
-      <c r="W28" s="176">
+      <c r="W28" s="161">
         <v>31</v>
       </c>
-      <c r="X28" s="177">
+      <c r="X28" s="162">
         <v>2.0099999999999998</v>
       </c>
-      <c r="Y28" s="173">
+      <c r="Y28" s="158">
         <v>100</v>
       </c>
-      <c r="Z28" s="171">
-        <f>[1]!dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+      <c r="Z28" s="156">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA28" s="173">
+      <c r="AA28" s="158">
         <v>20</v>
       </c>
-      <c r="AB28" s="173">
+      <c r="AB28" s="158">
         <v>14</v>
       </c>
       <c r="AC28" s="45">
         <v>475</v>
       </c>
-      <c r="AD28" s="173">
+      <c r="AD28" s="158">
         <v>12</v>
       </c>
-      <c r="AE28" s="173">
+      <c r="AE28" s="158">
         <v>7</v>
       </c>
-      <c r="AF28" s="173">
+      <c r="AF28" s="158">
         <v>10</v>
       </c>
-      <c r="AG28" s="173">
+      <c r="AG28" s="158">
         <v>65000</v>
       </c>
-      <c r="AH28" s="196">
+      <c r="AH28" s="181">
         <v>6</v>
       </c>
-      <c r="AI28" s="177">
+      <c r="AI28" s="162">
         <v>0.04</v>
       </c>
-      <c r="AJ28" s="186">
+      <c r="AJ28" s="171">
         <v>0.03</v>
       </c>
       <c r="AK28" s="45">
         <v>0</v>
       </c>
-      <c r="AL28" s="199">
+      <c r="AL28" s="184">
         <v>12</v>
       </c>
-      <c r="AM28" s="205" t="s">
+      <c r="AM28" s="189" t="s">
         <v>232</v>
       </c>
-      <c r="AN28" s="206" t="s">
+      <c r="AN28" s="190" t="s">
         <v>233</v>
       </c>
-      <c r="AO28" s="206" t="s">
+      <c r="AO28" s="190" t="s">
         <v>234</v>
       </c>
-      <c r="AP28" s="188"/>
-      <c r="AQ28" s="188"/>
-      <c r="AR28" s="178" t="s">
+      <c r="AP28" s="173"/>
+      <c r="AQ28" s="173"/>
+      <c r="AR28" s="163" t="s">
         <v>197</v>
       </c>
-      <c r="AS28" s="187">
+      <c r="AS28" s="172">
         <v>1.05</v>
       </c>
-      <c r="AT28" s="178">
+      <c r="AT28" s="163">
         <v>2</v>
       </c>
-      <c r="AU28" s="178">
+      <c r="AU28" s="163">
         <v>2</v>
       </c>
-      <c r="AV28" s="178" t="b">
+      <c r="AV28" s="163" t="b">
         <v>1</v>
       </c>
-      <c r="AW28" s="178" t="b">
+      <c r="AW28" s="163" t="b">
         <v>1</v>
       </c>
-      <c r="AX28" s="178" t="b">
+      <c r="AX28" s="163" t="b">
         <v>1</v>
       </c>
-      <c r="AY28" s="189">
+      <c r="AY28" s="174">
         <v>25</v>
       </c>
-      <c r="AZ28" s="178">
+      <c r="AZ28" s="163">
         <v>0.75</v>
       </c>
-      <c r="BA28" s="178">
+      <c r="BA28" s="163">
         <v>0.4</v>
       </c>
-      <c r="BB28" s="190" t="s">
+      <c r="BB28" s="175" t="s">
         <v>235</v>
       </c>
-      <c r="BC28" s="191" t="s">
+      <c r="BC28" s="176" t="s">
         <v>236</v>
       </c>
-      <c r="BD28" s="192">
+      <c r="BD28" s="177">
         <v>1.5E-3</v>
       </c>
-      <c r="BE28" s="169">
+      <c r="BE28" s="154">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF28" s="193">
+      <c r="BF28" s="178">
         <v>700</v>
       </c>
-      <c r="BG28" s="194">
-        <f>[1]!dragonDefinitions[[#This Row],['[forceMin']]]+50</f>
+      <c r="BG28" s="179">
         <v>750</v>
       </c>
-      <c r="BH28" s="179">
+      <c r="BH28" s="164">
         <v>4.9000000000000004</v>
       </c>
-      <c r="BI28" s="179">
+      <c r="BI28" s="164">
         <v>9.5</v>
       </c>
-      <c r="BJ28" s="179">
+      <c r="BJ28" s="164">
         <v>1.7</v>
       </c>
-      <c r="BK28" s="179">
+      <c r="BK28" s="164">
         <v>0.7</v>
       </c>
-      <c r="BL28" s="179">
+      <c r="BL28" s="164">
         <v>1.03</v>
       </c>
-      <c r="BM28" s="193">
+      <c r="BM28" s="178">
         <v>59</v>
       </c>
-      <c r="BN28" s="179">
+      <c r="BN28" s="164">
         <v>15</v>
       </c>
-      <c r="BO28" s="179">
+      <c r="BO28" s="164">
         <v>0.4</v>
       </c>
-      <c r="BP28" s="179">
+      <c r="BP28" s="164">
         <v>25</v>
       </c>
-      <c r="BQ28" s="180"/>
-      <c r="BR28" s="181">
+      <c r="BQ28" s="165"/>
+      <c r="BR28" s="166">
         <v>0.2</v>
       </c>
-      <c r="BS28" s="181">
+      <c r="BS28" s="166">
         <v>1</v>
       </c>
-      <c r="BT28" s="195" t="s">
+      <c r="BT28" s="180" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8112,83 +8095,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="156" t="s">
+      <c r="J29" s="201" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="156"/>
-      <c r="L29" s="156"/>
-      <c r="M29" s="156"/>
-      <c r="N29" s="154" t="s">
+      <c r="K29" s="201"/>
+      <c r="L29" s="201"/>
+      <c r="M29" s="201"/>
+      <c r="N29" s="199" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="155"/>
-      <c r="P29" s="155"/>
-      <c r="Q29" s="155"/>
-      <c r="R29" s="155"/>
-      <c r="S29" s="155"/>
-      <c r="T29" s="155"/>
-      <c r="U29" s="152" t="s">
+      <c r="O29" s="200"/>
+      <c r="P29" s="200"/>
+      <c r="Q29" s="200"/>
+      <c r="R29" s="200"/>
+      <c r="S29" s="200"/>
+      <c r="T29" s="200"/>
+      <c r="U29" s="197" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="153"/>
+      <c r="V29" s="198"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="149" t="s">
+      <c r="X29" s="194" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="150"/>
-      <c r="Z29" s="150"/>
-      <c r="AA29" s="150"/>
-      <c r="AB29" s="151"/>
-      <c r="AC29" s="148" t="s">
+      <c r="Y29" s="195"/>
+      <c r="Z29" s="195"/>
+      <c r="AA29" s="195"/>
+      <c r="AB29" s="196"/>
+      <c r="AC29" s="193" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="148"/>
-      <c r="AE29" s="148"/>
-      <c r="AF29" s="148"/>
-      <c r="AG29" s="148"/>
+      <c r="AD29" s="193"/>
+      <c r="AE29" s="193"/>
+      <c r="AF29" s="193"/>
+      <c r="AG29" s="193"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="162" t="s">
+      <c r="AI29" s="208" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="162"/>
-      <c r="AK29" s="200" t="s">
+      <c r="AJ29" s="208"/>
+      <c r="AK29" s="202" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="200"/>
-      <c r="AM29" s="207" t="s">
+      <c r="AL29" s="202"/>
+      <c r="AM29" s="209" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="208"/>
-      <c r="AO29" s="208"/>
-      <c r="AP29" s="208"/>
-      <c r="AQ29" s="208"/>
-      <c r="AR29" s="209"/>
-      <c r="AS29" s="157" t="s">
+      <c r="AN29" s="210"/>
+      <c r="AO29" s="210"/>
+      <c r="AP29" s="210"/>
+      <c r="AQ29" s="210"/>
+      <c r="AR29" s="211"/>
+      <c r="AS29" s="203" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="158"/>
-      <c r="AU29" s="158"/>
-      <c r="AV29" s="158"/>
-      <c r="AW29" s="158"/>
-      <c r="AX29" s="158"/>
-      <c r="AY29" s="159"/>
+      <c r="AT29" s="204"/>
+      <c r="AU29" s="204"/>
+      <c r="AV29" s="204"/>
+      <c r="AW29" s="204"/>
+      <c r="AX29" s="204"/>
+      <c r="AY29" s="205"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="161" t="s">
+      <c r="BF29" s="207" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="161"/>
-      <c r="BH29" s="161"/>
-      <c r="BI29" s="161"/>
-      <c r="BJ29" s="161"/>
-      <c r="BK29" s="161"/>
-      <c r="BL29" s="161"/>
+      <c r="BG29" s="207"/>
+      <c r="BH29" s="207"/>
+      <c r="BI29" s="207"/>
+      <c r="BJ29" s="207"/>
+      <c r="BK29" s="207"/>
+      <c r="BL29" s="207"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -9535,61 +9518,61 @@
       <c r="D59">
         <v>20</v>
       </c>
-      <c r="E59" s="210">
+      <c r="E59" s="191">
         <v>4571</v>
       </c>
-      <c r="F59" s="211">
+      <c r="F59" s="192">
         <v>13714</v>
       </c>
-      <c r="G59" s="211">
+      <c r="G59" s="192">
         <v>27428</v>
       </c>
-      <c r="H59" s="211">
+      <c r="H59" s="192">
         <v>45713</v>
       </c>
-      <c r="I59" s="211">
+      <c r="I59" s="192">
         <v>68569</v>
       </c>
-      <c r="J59" s="211">
+      <c r="J59" s="192">
         <v>95997</v>
       </c>
-      <c r="K59" s="211">
+      <c r="K59" s="192">
         <v>127995</v>
       </c>
-      <c r="L59" s="211">
+      <c r="L59" s="192">
         <v>164565</v>
       </c>
-      <c r="M59" s="211">
+      <c r="M59" s="192">
         <v>205707</v>
       </c>
-      <c r="N59" s="211">
+      <c r="N59" s="192">
         <v>251419</v>
       </c>
-      <c r="O59" s="211">
+      <c r="O59" s="192">
         <v>301703</v>
       </c>
-      <c r="P59" s="211">
+      <c r="P59" s="192">
         <v>356559</v>
       </c>
-      <c r="Q59" s="211">
+      <c r="Q59" s="192">
         <v>415985</v>
       </c>
-      <c r="R59" s="211">
+      <c r="R59" s="192">
         <v>479983</v>
       </c>
-      <c r="S59" s="211">
+      <c r="S59" s="192">
         <v>548552</v>
       </c>
-      <c r="T59" s="211">
+      <c r="T59" s="192">
         <v>621692</v>
       </c>
-      <c r="U59" s="211">
+      <c r="U59" s="192">
         <v>699403</v>
       </c>
-      <c r="V59" s="211">
+      <c r="V59" s="192">
         <v>781686</v>
       </c>
-      <c r="W59" s="211">
+      <c r="W59" s="192">
         <v>868540</v>
       </c>
     </row>
@@ -9608,49 +9591,49 @@
     <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="21" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C10">
-    <cfRule type="duplicateValues" dxfId="20" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="19" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="18" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="17" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="15" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="13" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="12" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT28">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ28">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D28">

</xml_diff>

<commit_message>
Increased Nibble boost multiplier, from 1.95 to 2.1
Former-commit-id: 0d7c7691fba91e62e1df2ee84729b027568cb867
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1875,6 +1875,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1900,36 +1930,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4861,8 +4861,8 @@
   </sheetPr>
   <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BG28" sqref="BG28"/>
+    <sheetView tabSelected="1" topLeftCell="K7" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5128,10 +5128,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="206"/>
-      <c r="AP14" s="206"/>
-      <c r="AQ14" s="206"/>
-      <c r="AR14" s="206"/>
+      <c r="AO14" s="197"/>
+      <c r="AP14" s="197"/>
+      <c r="AQ14" s="197"/>
+      <c r="AR14" s="197"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -5414,7 +5414,7 @@
         <v>14</v>
       </c>
       <c r="X16" s="56">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="Y16" s="28">
         <v>100</v>
@@ -8095,83 +8095,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="201" t="s">
+      <c r="J29" s="211" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="201"/>
-      <c r="L29" s="201"/>
-      <c r="M29" s="201"/>
-      <c r="N29" s="199" t="s">
+      <c r="K29" s="211"/>
+      <c r="L29" s="211"/>
+      <c r="M29" s="211"/>
+      <c r="N29" s="209" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="200"/>
-      <c r="P29" s="200"/>
-      <c r="Q29" s="200"/>
-      <c r="R29" s="200"/>
-      <c r="S29" s="200"/>
-      <c r="T29" s="200"/>
-      <c r="U29" s="197" t="s">
+      <c r="O29" s="210"/>
+      <c r="P29" s="210"/>
+      <c r="Q29" s="210"/>
+      <c r="R29" s="210"/>
+      <c r="S29" s="210"/>
+      <c r="T29" s="210"/>
+      <c r="U29" s="207" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="198"/>
+      <c r="V29" s="208"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="194" t="s">
+      <c r="X29" s="204" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="195"/>
-      <c r="Z29" s="195"/>
-      <c r="AA29" s="195"/>
-      <c r="AB29" s="196"/>
-      <c r="AC29" s="193" t="s">
+      <c r="Y29" s="205"/>
+      <c r="Z29" s="205"/>
+      <c r="AA29" s="205"/>
+      <c r="AB29" s="206"/>
+      <c r="AC29" s="203" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="193"/>
-      <c r="AE29" s="193"/>
-      <c r="AF29" s="193"/>
-      <c r="AG29" s="193"/>
+      <c r="AD29" s="203"/>
+      <c r="AE29" s="203"/>
+      <c r="AF29" s="203"/>
+      <c r="AG29" s="203"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="208" t="s">
+      <c r="AI29" s="199" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="208"/>
-      <c r="AK29" s="202" t="s">
+      <c r="AJ29" s="199"/>
+      <c r="AK29" s="193" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="202"/>
-      <c r="AM29" s="209" t="s">
+      <c r="AL29" s="193"/>
+      <c r="AM29" s="200" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="210"/>
-      <c r="AO29" s="210"/>
-      <c r="AP29" s="210"/>
-      <c r="AQ29" s="210"/>
-      <c r="AR29" s="211"/>
-      <c r="AS29" s="203" t="s">
+      <c r="AN29" s="201"/>
+      <c r="AO29" s="201"/>
+      <c r="AP29" s="201"/>
+      <c r="AQ29" s="201"/>
+      <c r="AR29" s="202"/>
+      <c r="AS29" s="194" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="204"/>
-      <c r="AU29" s="204"/>
-      <c r="AV29" s="204"/>
-      <c r="AW29" s="204"/>
-      <c r="AX29" s="204"/>
-      <c r="AY29" s="205"/>
+      <c r="AT29" s="195"/>
+      <c r="AU29" s="195"/>
+      <c r="AV29" s="195"/>
+      <c r="AW29" s="195"/>
+      <c r="AX29" s="195"/>
+      <c r="AY29" s="196"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="207" t="s">
+      <c r="BF29" s="198" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="207"/>
-      <c r="BH29" s="207"/>
-      <c r="BI29" s="207"/>
-      <c r="BJ29" s="207"/>
-      <c r="BK29" s="207"/>
-      <c r="BL29" s="207"/>
+      <c r="BG29" s="198"/>
+      <c r="BH29" s="198"/>
+      <c r="BI29" s="198"/>
+      <c r="BJ29" s="198"/>
+      <c r="BK29" s="198"/>
+      <c r="BL29" s="198"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -9578,17 +9578,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="121" priority="14"/>

</xml_diff>

<commit_message>
Increased boost duration for Baby
Former-commit-id: 74d138ee3fa23cfbb87df3765b581c9a9495493a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -830,18 +830,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1875,6 +1878,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1903,33 +1933,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4862,7 +4865,7 @@
   <dimension ref="A1:BT59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K7" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5128,10 +5131,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="197"/>
-      <c r="AP14" s="197"/>
-      <c r="AQ14" s="197"/>
-      <c r="AR14" s="197"/>
+      <c r="AO14" s="206"/>
+      <c r="AP14" s="206"/>
+      <c r="AQ14" s="206"/>
+      <c r="AR14" s="206"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -5424,7 +5427,7 @@
         <v>125</v>
       </c>
       <c r="AA16" s="28">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="AB16" s="28">
         <v>28</v>
@@ -8095,83 +8098,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="211" t="s">
+      <c r="J29" s="201" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="211"/>
-      <c r="L29" s="211"/>
-      <c r="M29" s="211"/>
-      <c r="N29" s="209" t="s">
+      <c r="K29" s="201"/>
+      <c r="L29" s="201"/>
+      <c r="M29" s="201"/>
+      <c r="N29" s="199" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="210"/>
-      <c r="P29" s="210"/>
-      <c r="Q29" s="210"/>
-      <c r="R29" s="210"/>
-      <c r="S29" s="210"/>
-      <c r="T29" s="210"/>
-      <c r="U29" s="207" t="s">
+      <c r="O29" s="200"/>
+      <c r="P29" s="200"/>
+      <c r="Q29" s="200"/>
+      <c r="R29" s="200"/>
+      <c r="S29" s="200"/>
+      <c r="T29" s="200"/>
+      <c r="U29" s="197" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="208"/>
+      <c r="V29" s="198"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="204" t="s">
+      <c r="X29" s="194" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="205"/>
-      <c r="Z29" s="205"/>
-      <c r="AA29" s="205"/>
-      <c r="AB29" s="206"/>
-      <c r="AC29" s="203" t="s">
+      <c r="Y29" s="195"/>
+      <c r="Z29" s="195"/>
+      <c r="AA29" s="195"/>
+      <c r="AB29" s="196"/>
+      <c r="AC29" s="193" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="203"/>
-      <c r="AE29" s="203"/>
-      <c r="AF29" s="203"/>
-      <c r="AG29" s="203"/>
+      <c r="AD29" s="193"/>
+      <c r="AE29" s="193"/>
+      <c r="AF29" s="193"/>
+      <c r="AG29" s="193"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="199" t="s">
+      <c r="AI29" s="208" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="199"/>
-      <c r="AK29" s="193" t="s">
+      <c r="AJ29" s="208"/>
+      <c r="AK29" s="202" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="193"/>
-      <c r="AM29" s="200" t="s">
+      <c r="AL29" s="202"/>
+      <c r="AM29" s="209" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="201"/>
-      <c r="AO29" s="201"/>
-      <c r="AP29" s="201"/>
-      <c r="AQ29" s="201"/>
-      <c r="AR29" s="202"/>
-      <c r="AS29" s="194" t="s">
+      <c r="AN29" s="210"/>
+      <c r="AO29" s="210"/>
+      <c r="AP29" s="210"/>
+      <c r="AQ29" s="210"/>
+      <c r="AR29" s="211"/>
+      <c r="AS29" s="203" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="195"/>
-      <c r="AU29" s="195"/>
-      <c r="AV29" s="195"/>
-      <c r="AW29" s="195"/>
-      <c r="AX29" s="195"/>
-      <c r="AY29" s="196"/>
+      <c r="AT29" s="204"/>
+      <c r="AU29" s="204"/>
+      <c r="AV29" s="204"/>
+      <c r="AW29" s="204"/>
+      <c r="AX29" s="204"/>
+      <c r="AY29" s="205"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="198" t="s">
+      <c r="BF29" s="207" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="198"/>
-      <c r="BH29" s="198"/>
-      <c r="BI29" s="198"/>
-      <c r="BJ29" s="198"/>
-      <c r="BK29" s="198"/>
-      <c r="BL29" s="198"/>
+      <c r="BG29" s="207"/>
+      <c r="BH29" s="207"/>
+      <c r="BI29" s="207"/>
+      <c r="BJ29" s="207"/>
+      <c r="BK29" s="207"/>
+      <c r="BL29" s="207"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -9578,17 +9581,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="121" priority="14"/>

</xml_diff>

<commit_message>
Setting dark dragon scale. tiers L and XL reduced a bit their size
Former-commit-id: c263641f5ed3d3a16b61006a4b0aeabaa9666342
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -744,7 +744,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -819,30 +819,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -948,7 +927,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1234,15 +1213,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1320,29 +1290,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1631,12 +1583,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1652,19 +1598,19 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1718,16 +1664,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1740,7 +1680,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1749,109 +1689,19 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1866,18 +1716,42 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1905,41 +1779,59 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="122">
+  <dxfs count="125">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -4428,105 +4320,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="106" dataDxfId="104" headerRowBorderDxfId="105" tableBorderDxfId="103" totalsRowBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106" totalsRowBorderDxfId="105">
   <autoFilter ref="B15:BT28"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="101"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="100"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="99"/>
-    <tableColumn id="65" name="[type]" dataDxfId="98"/>
-    <tableColumn id="3" name="[order]" dataDxfId="97"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="96"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="95"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="94"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="93"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="92"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="91"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="90"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="89"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="88"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="87"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="86"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="85"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="84"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="83"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="82"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="81"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="80"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="79"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="78"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="77">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="104"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="103"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="102"/>
+    <tableColumn id="65" name="[type]" dataDxfId="101"/>
+    <tableColumn id="3" name="[order]" dataDxfId="100"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="99"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="98"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="97"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="96"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="95"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="94"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="93"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="92"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="91"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="90"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="89"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="88"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="87"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="86"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="85"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="84"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="83"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="82"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="81"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="80">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="76"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="75"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="74"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="73"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="72"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="71"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="70"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="69"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="68"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="67">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="79"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="78"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="77"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="76"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="75"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="74"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="73"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="72"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="71"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="70">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="66"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="65"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="64"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="63"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="62"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="61"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="60"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="59"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="58"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="57"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="56"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="55"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="54"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="53"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="52"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="51"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="50"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="49">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="69"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="68"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="67"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="66"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="65"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="64"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="63"/>
+    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="62"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="61"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="60"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="59"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="58"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="57"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="56"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="55"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="54"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="53"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="52">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="48">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="51">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="47"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="46"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="45"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="44">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="50"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="49"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="48"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="47">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="43"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="42"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="41"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="40"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="39"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="38"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="37"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="36"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="35"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="34"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="33"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="32"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="31"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="46"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="45"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="44"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="43"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="42"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="41"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="40"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="39"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="38"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="37"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="36"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="35"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G10" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G10" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="B4:G10"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="26"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="29"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="25"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="24"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="23">
+    <tableColumn id="10" name="[icon]" dataDxfId="28"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="27"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="26">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4535,24 +4427,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:I35" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:I35" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B34:I35"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="18"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="21"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="20"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="16"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="15"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="14"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="13"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="12"/>
+    <tableColumn id="8" name="[superfuryMax]" dataDxfId="19"/>
+    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="18"/>
+    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="17"/>
+    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="16"/>
+    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="B46:W59"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -4583,14 +4475,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B39:F42"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="6"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="4"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4864,8 +4756,8 @@
   </sheetPr>
   <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K7" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="BP21" sqref="BP21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4880,7 +4772,7 @@
     <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" customWidth="1"/>
     <col min="34" max="35" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="24.42578125" bestFit="1" customWidth="1"/>
@@ -5062,13 +4954,13 @@
       </c>
     </row>
     <row r="10" spans="2:72" x14ac:dyDescent="0.25">
-      <c r="B10" s="150" t="s">
+      <c r="B10" s="146" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="85" t="s">
         <v>228</v>
       </c>
-      <c r="D10" s="151">
+      <c r="D10" s="147">
         <v>5</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -5077,7 +4969,7 @@
       <c r="F10" s="15">
         <v>4</v>
       </c>
-      <c r="G10" s="149" t="s">
+      <c r="G10" s="145" t="s">
         <v>230</v>
       </c>
     </row>
@@ -5131,10 +5023,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="206"/>
-      <c r="AP14" s="206"/>
-      <c r="AQ14" s="206"/>
-      <c r="AR14" s="206"/>
+      <c r="AO14" s="161"/>
+      <c r="AP14" s="161"/>
+      <c r="AQ14" s="161"/>
+      <c r="AR14" s="161"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -5230,16 +5122,16 @@
       <c r="AF15" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="AG15" s="113" t="s">
+      <c r="AG15" s="111" t="s">
         <v>145</v>
       </c>
-      <c r="AH15" s="114" t="s">
+      <c r="AH15" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="AI15" s="114" t="s">
+      <c r="AI15" s="112" t="s">
         <v>193</v>
       </c>
-      <c r="AJ15" s="119" t="s">
+      <c r="AJ15" s="117" t="s">
         <v>194</v>
       </c>
       <c r="AK15" s="81" t="s">
@@ -5257,13 +5149,13 @@
       <c r="AO15" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="AP15" s="111" t="s">
+      <c r="AP15" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="AQ15" s="111" t="s">
+      <c r="AQ15" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="AR15" s="122" t="s">
+      <c r="AR15" s="120" t="s">
         <v>215</v>
       </c>
       <c r="AS15" s="74" t="s">
@@ -5284,16 +5176,16 @@
       <c r="AX15" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="AY15" s="145" t="s">
+      <c r="AY15" s="141" t="s">
         <v>132</v>
       </c>
       <c r="AZ15" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="BA15" s="122" t="s">
+      <c r="BA15" s="120" t="s">
         <v>196</v>
       </c>
-      <c r="BB15" s="125" t="s">
+      <c r="BB15" s="123" t="s">
         <v>4</v>
       </c>
       <c r="BC15" s="71" t="s">
@@ -5323,7 +5215,7 @@
       <c r="BK15" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="BL15" s="131" t="s">
+      <c r="BL15" s="129" t="s">
         <v>124</v>
       </c>
       <c r="BM15" s="70" t="s">
@@ -5447,7 +5339,7 @@
       <c r="AG16" s="28">
         <v>3000</v>
       </c>
-      <c r="AH16" s="115">
+      <c r="AH16" s="113">
         <v>1</v>
       </c>
       <c r="AI16" s="104">
@@ -5457,24 +5349,24 @@
         <f t="shared" ref="AJ16:AJ23" si="0">AI17</f>
         <v>0.19</v>
       </c>
-      <c r="AK16" s="182">
+      <c r="AK16" s="149">
         <v>0</v>
       </c>
       <c r="AL16" s="61">
         <v>12</v>
       </c>
-      <c r="AM16" s="185" t="s">
+      <c r="AM16" s="151" t="s">
         <v>120</v>
       </c>
-      <c r="AN16" s="185" t="s">
+      <c r="AN16" s="151" t="s">
         <v>119</v>
       </c>
-      <c r="AO16" s="185" t="s">
+      <c r="AO16" s="151" t="s">
         <v>217</v>
       </c>
-      <c r="AP16" s="112"/>
-      <c r="AQ16" s="112"/>
-      <c r="AR16" s="123"/>
+      <c r="AP16" s="110"/>
+      <c r="AQ16" s="110"/>
+      <c r="AR16" s="121"/>
       <c r="AS16" s="41">
         <v>3</v>
       </c>
@@ -5493,16 +5385,16 @@
       <c r="AX16" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY16" s="146">
+      <c r="AY16" s="142">
         <v>25</v>
       </c>
-      <c r="AZ16" s="143">
+      <c r="AZ16" s="139">
         <v>0.55999999999999994</v>
       </c>
-      <c r="BA16" s="123">
+      <c r="BA16" s="121">
         <v>0.6</v>
       </c>
-      <c r="BB16" s="126" t="s">
+      <c r="BB16" s="124" t="s">
         <v>118</v>
       </c>
       <c r="BC16" s="63" t="s">
@@ -5532,10 +5424,10 @@
       <c r="BK16" s="64">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BL16" s="132">
+      <c r="BL16" s="130">
         <v>1.75</v>
       </c>
-      <c r="BM16" s="136">
+      <c r="BM16" s="134">
         <v>0</v>
       </c>
       <c r="BN16" s="64">
@@ -5553,7 +5445,7 @@
       <c r="BR16" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS16" s="133">
+      <c r="BS16" s="131">
         <v>1</v>
       </c>
       <c r="BT16" s="37" t="s">
@@ -5658,7 +5550,7 @@
       <c r="AG17" s="28">
         <v>7000</v>
       </c>
-      <c r="AH17" s="115">
+      <c r="AH17" s="113">
         <v>2</v>
       </c>
       <c r="AI17" s="104">
@@ -5668,24 +5560,24 @@
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="AK17" s="182">
+      <c r="AK17" s="149">
         <v>0</v>
       </c>
       <c r="AL17" s="61">
         <v>12</v>
       </c>
-      <c r="AM17" s="186" t="s">
+      <c r="AM17" s="152" t="s">
         <v>116</v>
       </c>
-      <c r="AN17" s="185" t="s">
+      <c r="AN17" s="151" t="s">
         <v>115</v>
       </c>
-      <c r="AO17" s="185" t="s">
+      <c r="AO17" s="151" t="s">
         <v>218</v>
       </c>
-      <c r="AP17" s="112"/>
-      <c r="AQ17" s="112"/>
-      <c r="AR17" s="123"/>
+      <c r="AP17" s="110"/>
+      <c r="AQ17" s="110"/>
+      <c r="AR17" s="121"/>
       <c r="AS17" s="41">
         <v>2.2999999999999998</v>
       </c>
@@ -5704,16 +5596,16 @@
       <c r="AX17" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY17" s="146">
+      <c r="AY17" s="142">
         <v>25</v>
       </c>
-      <c r="AZ17" s="143">
+      <c r="AZ17" s="139">
         <v>0.7</v>
       </c>
-      <c r="BA17" s="123">
+      <c r="BA17" s="121">
         <v>0.8</v>
       </c>
-      <c r="BB17" s="126" t="s">
+      <c r="BB17" s="124" t="s">
         <v>114</v>
       </c>
       <c r="BC17" s="63" t="s">
@@ -5743,7 +5635,7 @@
       <c r="BK17" s="52">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BL17" s="133">
+      <c r="BL17" s="131">
         <v>2.1</v>
       </c>
       <c r="BM17" s="37">
@@ -5758,11 +5650,11 @@
       <c r="BP17" s="64">
         <v>25</v>
       </c>
-      <c r="BQ17" s="64"/>
-      <c r="BR17" s="64">
+      <c r="BQ17" s="52"/>
+      <c r="BR17" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS17" s="132">
+      <c r="BS17" s="130">
         <v>1</v>
       </c>
       <c r="BT17" s="37" t="s">
@@ -5867,7 +5759,7 @@
       <c r="AG18" s="28">
         <v>8000</v>
       </c>
-      <c r="AH18" s="116">
+      <c r="AH18" s="114">
         <v>2</v>
       </c>
       <c r="AI18" s="105">
@@ -5877,24 +5769,24 @@
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="AK18" s="183">
+      <c r="AK18" s="150">
         <v>0</v>
       </c>
-      <c r="AL18" s="148">
+      <c r="AL18" s="144">
         <v>12</v>
       </c>
-      <c r="AM18" s="186" t="s">
+      <c r="AM18" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="AN18" s="185" t="s">
+      <c r="AN18" s="151" t="s">
         <v>111</v>
       </c>
-      <c r="AO18" s="185" t="s">
+      <c r="AO18" s="151" t="s">
         <v>110</v>
       </c>
-      <c r="AP18" s="112"/>
-      <c r="AQ18" s="112"/>
-      <c r="AR18" s="123"/>
+      <c r="AP18" s="110"/>
+      <c r="AQ18" s="110"/>
+      <c r="AR18" s="121"/>
       <c r="AS18" s="41">
         <v>2.1</v>
       </c>
@@ -5913,16 +5805,16 @@
       <c r="AX18" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY18" s="146">
+      <c r="AY18" s="142">
         <v>25</v>
       </c>
-      <c r="AZ18" s="143">
+      <c r="AZ18" s="139">
         <v>0.7</v>
       </c>
-      <c r="BA18" s="123">
+      <c r="BA18" s="121">
         <v>0.7</v>
       </c>
-      <c r="BB18" s="127" t="s">
+      <c r="BB18" s="125" t="s">
         <v>109</v>
       </c>
       <c r="BC18" s="53" t="s">
@@ -5952,7 +5844,7 @@
       <c r="BK18" s="52">
         <v>0.9</v>
       </c>
-      <c r="BL18" s="133">
+      <c r="BL18" s="131">
         <v>2.25</v>
       </c>
       <c r="BM18" s="37">
@@ -5967,16 +5859,16 @@
       <c r="BP18" s="64">
         <v>25</v>
       </c>
-      <c r="BQ18" s="108" t="s">
+      <c r="BQ18" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="BR18" s="108">
+      <c r="BR18" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS18" s="137">
+      <c r="BS18" s="180">
         <v>1</v>
       </c>
-      <c r="BT18" s="139" t="s">
+      <c r="BT18" s="178" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6078,7 +5970,7 @@
       <c r="AG19" s="28">
         <v>9000</v>
       </c>
-      <c r="AH19" s="115">
+      <c r="AH19" s="113">
         <v>2</v>
       </c>
       <c r="AI19" s="104">
@@ -6088,24 +5980,24 @@
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="AK19" s="182">
+      <c r="AK19" s="149">
         <v>0</v>
       </c>
       <c r="AL19" s="61">
         <v>12</v>
       </c>
-      <c r="AM19" s="186" t="s">
+      <c r="AM19" s="152" t="s">
         <v>106</v>
       </c>
-      <c r="AN19" s="185" t="s">
+      <c r="AN19" s="151" t="s">
         <v>105</v>
       </c>
-      <c r="AO19" s="185" t="s">
+      <c r="AO19" s="151" t="s">
         <v>219</v>
       </c>
-      <c r="AP19" s="112"/>
-      <c r="AQ19" s="112"/>
-      <c r="AR19" s="123"/>
+      <c r="AP19" s="110"/>
+      <c r="AQ19" s="110"/>
+      <c r="AR19" s="121"/>
       <c r="AS19" s="41">
         <v>2.1</v>
       </c>
@@ -6124,16 +6016,16 @@
       <c r="AX19" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY19" s="146">
+      <c r="AY19" s="142">
         <v>25</v>
       </c>
-      <c r="AZ19" s="143">
+      <c r="AZ19" s="139">
         <v>0.7</v>
       </c>
-      <c r="BA19" s="123">
+      <c r="BA19" s="121">
         <v>0.7</v>
       </c>
-      <c r="BB19" s="127" t="s">
+      <c r="BB19" s="125" t="s">
         <v>104</v>
       </c>
       <c r="BC19" s="53" t="s">
@@ -6163,7 +6055,7 @@
       <c r="BK19" s="52">
         <v>1.2</v>
       </c>
-      <c r="BL19" s="133">
+      <c r="BL19" s="131">
         <v>0.77</v>
       </c>
       <c r="BM19" s="37">
@@ -6178,14 +6070,14 @@
       <c r="BP19" s="64">
         <v>25</v>
       </c>
-      <c r="BQ19" s="108"/>
-      <c r="BR19" s="108">
+      <c r="BQ19" s="52"/>
+      <c r="BR19" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS19" s="137">
+      <c r="BS19" s="180">
         <v>1</v>
       </c>
-      <c r="BT19" s="139" t="s">
+      <c r="BT19" s="178" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6287,7 +6179,7 @@
       <c r="AG20" s="28">
         <v>10000</v>
       </c>
-      <c r="AH20" s="115">
+      <c r="AH20" s="113">
         <v>3</v>
       </c>
       <c r="AI20" s="104">
@@ -6297,24 +6189,24 @@
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="AK20" s="182">
+      <c r="AK20" s="149">
         <v>0</v>
       </c>
       <c r="AL20" s="61">
         <v>12</v>
       </c>
-      <c r="AM20" s="186" t="s">
+      <c r="AM20" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="AN20" s="185" t="s">
+      <c r="AN20" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="AO20" s="185" t="s">
+      <c r="AO20" s="151" t="s">
         <v>220</v>
       </c>
-      <c r="AP20" s="112"/>
-      <c r="AQ20" s="112"/>
-      <c r="AR20" s="123"/>
+      <c r="AP20" s="110"/>
+      <c r="AQ20" s="110"/>
+      <c r="AR20" s="121"/>
       <c r="AS20" s="41">
         <v>2.1</v>
       </c>
@@ -6333,16 +6225,16 @@
       <c r="AX20" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY20" s="146">
+      <c r="AY20" s="142">
         <v>25</v>
       </c>
-      <c r="AZ20" s="143">
+      <c r="AZ20" s="139">
         <v>0.7</v>
       </c>
-      <c r="BA20" s="123">
+      <c r="BA20" s="121">
         <v>0.6</v>
       </c>
-      <c r="BB20" s="127" t="s">
+      <c r="BB20" s="125" t="s">
         <v>100</v>
       </c>
       <c r="BC20" s="53" t="s">
@@ -6372,7 +6264,7 @@
       <c r="BK20" s="52">
         <v>1</v>
       </c>
-      <c r="BL20" s="133">
+      <c r="BL20" s="131">
         <v>1.6</v>
       </c>
       <c r="BM20" s="37">
@@ -6387,16 +6279,16 @@
       <c r="BP20" s="64">
         <v>25</v>
       </c>
-      <c r="BQ20" s="35" t="s">
+      <c r="BQ20" s="176" t="s">
         <v>209</v>
       </c>
-      <c r="BR20" s="109">
+      <c r="BR20" s="177">
         <v>0.2</v>
       </c>
-      <c r="BS20" s="138">
+      <c r="BS20" s="181">
         <v>1</v>
       </c>
-      <c r="BT20" s="139" t="s">
+      <c r="BT20" s="178" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6498,7 +6390,7 @@
       <c r="AG21" s="28">
         <v>10000</v>
       </c>
-      <c r="AH21" s="115">
+      <c r="AH21" s="113">
         <v>3</v>
       </c>
       <c r="AI21" s="104">
@@ -6508,24 +6400,24 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="AK21" s="182">
+      <c r="AK21" s="149">
         <v>0</v>
       </c>
       <c r="AL21" s="61">
         <v>12</v>
       </c>
-      <c r="AM21" s="186" t="s">
+      <c r="AM21" s="152" t="s">
         <v>98</v>
       </c>
-      <c r="AN21" s="185" t="s">
+      <c r="AN21" s="151" t="s">
         <v>97</v>
       </c>
-      <c r="AO21" s="185" t="s">
+      <c r="AO21" s="151" t="s">
         <v>96</v>
       </c>
-      <c r="AP21" s="112"/>
-      <c r="AQ21" s="112"/>
-      <c r="AR21" s="123"/>
+      <c r="AP21" s="110"/>
+      <c r="AQ21" s="110"/>
+      <c r="AR21" s="121"/>
       <c r="AS21" s="41">
         <v>2</v>
       </c>
@@ -6544,16 +6436,16 @@
       <c r="AX21" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY21" s="146">
+      <c r="AY21" s="142">
         <v>25</v>
       </c>
-      <c r="AZ21" s="143">
+      <c r="AZ21" s="139">
         <v>0.7</v>
       </c>
-      <c r="BA21" s="123">
+      <c r="BA21" s="121">
         <v>0.5</v>
       </c>
-      <c r="BB21" s="127" t="s">
+      <c r="BB21" s="125" t="s">
         <v>95</v>
       </c>
       <c r="BC21" s="53" t="s">
@@ -6583,7 +6475,7 @@
       <c r="BK21" s="52">
         <v>0.5</v>
       </c>
-      <c r="BL21" s="133">
+      <c r="BL21" s="131">
         <v>1.7</v>
       </c>
       <c r="BM21" s="37">
@@ -6598,16 +6490,16 @@
       <c r="BP21" s="64">
         <v>25</v>
       </c>
-      <c r="BQ21" s="108" t="s">
+      <c r="BQ21" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="BR21" s="108">
+      <c r="BR21" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS21" s="137">
+      <c r="BS21" s="180">
         <v>1</v>
       </c>
-      <c r="BT21" s="139" t="s">
+      <c r="BT21" s="178" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6709,7 +6601,7 @@
       <c r="AG22" s="28">
         <v>10000</v>
       </c>
-      <c r="AH22" s="115">
+      <c r="AH22" s="113">
         <v>3</v>
       </c>
       <c r="AI22" s="104">
@@ -6719,24 +6611,24 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK22" s="182">
+      <c r="AK22" s="149">
         <v>0</v>
       </c>
       <c r="AL22" s="61">
         <v>12</v>
       </c>
-      <c r="AM22" s="186" t="s">
+      <c r="AM22" s="152" t="s">
         <v>92</v>
       </c>
-      <c r="AN22" s="185" t="s">
+      <c r="AN22" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="AO22" s="185" t="s">
+      <c r="AO22" s="151" t="s">
         <v>221</v>
       </c>
-      <c r="AP22" s="112"/>
-      <c r="AQ22" s="112"/>
-      <c r="AR22" s="123"/>
+      <c r="AP22" s="110"/>
+      <c r="AQ22" s="110"/>
+      <c r="AR22" s="121"/>
       <c r="AS22" s="41">
         <v>1.6</v>
       </c>
@@ -6755,16 +6647,16 @@
       <c r="AX22" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY22" s="146">
+      <c r="AY22" s="142">
         <v>25</v>
       </c>
-      <c r="AZ22" s="143">
+      <c r="AZ22" s="139">
         <v>0.7</v>
       </c>
-      <c r="BA22" s="123">
+      <c r="BA22" s="121">
         <v>0.5</v>
       </c>
-      <c r="BB22" s="127" t="s">
+      <c r="BB22" s="125" t="s">
         <v>90</v>
       </c>
       <c r="BC22" s="53" t="s">
@@ -6794,7 +6686,7 @@
       <c r="BK22" s="52">
         <v>0.5</v>
       </c>
-      <c r="BL22" s="133">
+      <c r="BL22" s="131">
         <v>0.9</v>
       </c>
       <c r="BM22" s="37">
@@ -6809,16 +6701,16 @@
       <c r="BP22" s="64">
         <v>25</v>
       </c>
-      <c r="BQ22" s="35" t="s">
+      <c r="BQ22" s="176" t="s">
         <v>210</v>
       </c>
-      <c r="BR22" s="110">
+      <c r="BR22" s="177">
         <v>0.2</v>
       </c>
-      <c r="BS22" s="138">
+      <c r="BS22" s="181">
         <v>1</v>
       </c>
-      <c r="BT22" s="139" t="s">
+      <c r="BT22" s="178" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6881,10 +6773,10 @@
         <v>0.7</v>
       </c>
       <c r="U23" s="56">
-        <v>1.54</v>
+        <v>1.44</v>
       </c>
       <c r="V23" s="28">
-        <v>1.74</v>
+        <v>1.64</v>
       </c>
       <c r="W23" s="48">
         <v>25</v>
@@ -6920,7 +6812,7 @@
       <c r="AG23" s="28">
         <v>16000</v>
       </c>
-      <c r="AH23" s="116">
+      <c r="AH23" s="114">
         <v>4</v>
       </c>
       <c r="AI23" s="105">
@@ -6930,24 +6822,24 @@
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="AK23" s="183">
+      <c r="AK23" s="150">
         <v>0</v>
       </c>
-      <c r="AL23" s="148">
+      <c r="AL23" s="144">
         <v>12</v>
       </c>
-      <c r="AM23" s="186" t="s">
+      <c r="AM23" s="152" t="s">
         <v>88</v>
       </c>
-      <c r="AN23" s="185" t="s">
+      <c r="AN23" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="AO23" s="185" t="s">
+      <c r="AO23" s="151" t="s">
         <v>222</v>
       </c>
-      <c r="AP23" s="112"/>
-      <c r="AQ23" s="112"/>
-      <c r="AR23" s="142" t="s">
+      <c r="AP23" s="110"/>
+      <c r="AQ23" s="110"/>
+      <c r="AR23" s="138" t="s">
         <v>11</v>
       </c>
       <c r="AS23" s="41">
@@ -6968,16 +6860,16 @@
       <c r="AX23" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY23" s="146">
+      <c r="AY23" s="142">
         <v>25</v>
       </c>
-      <c r="AZ23" s="143">
+      <c r="AZ23" s="139">
         <v>0.7</v>
       </c>
-      <c r="BA23" s="123">
+      <c r="BA23" s="121">
         <v>0.5</v>
       </c>
-      <c r="BB23" s="127" t="s">
+      <c r="BB23" s="125" t="s">
         <v>86</v>
       </c>
       <c r="BC23" s="53" t="s">
@@ -7007,7 +6899,7 @@
       <c r="BK23" s="52">
         <v>0.5</v>
       </c>
-      <c r="BL23" s="133">
+      <c r="BL23" s="131">
         <v>1.2</v>
       </c>
       <c r="BM23" s="37">
@@ -7022,14 +6914,14 @@
       <c r="BP23" s="64">
         <v>25</v>
       </c>
-      <c r="BQ23" s="108"/>
-      <c r="BR23" s="108">
+      <c r="BQ23" s="52"/>
+      <c r="BR23" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS23" s="137">
+      <c r="BS23" s="180">
         <v>1</v>
       </c>
-      <c r="BT23" s="139" t="s">
+      <c r="BT23" s="178" t="s">
         <v>12</v>
       </c>
     </row>
@@ -7092,10 +6984,10 @@
         <v>0.7</v>
       </c>
       <c r="U24" s="42">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="V24" s="46">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="W24" s="48">
         <v>25</v>
@@ -7131,7 +7023,7 @@
       <c r="AG24" s="46">
         <v>20000</v>
       </c>
-      <c r="AH24" s="117">
+      <c r="AH24" s="115">
         <v>4</v>
       </c>
       <c r="AI24" s="106">
@@ -7140,24 +7032,24 @@
       <c r="AJ24" s="103">
         <v>0.05</v>
       </c>
-      <c r="AK24" s="183">
+      <c r="AK24" s="150">
         <v>0</v>
       </c>
-      <c r="AL24" s="148">
+      <c r="AL24" s="144">
         <v>12</v>
       </c>
-      <c r="AM24" s="187" t="s">
+      <c r="AM24" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="AN24" s="188" t="s">
+      <c r="AN24" s="154" t="s">
         <v>186</v>
       </c>
-      <c r="AO24" s="188" t="s">
+      <c r="AO24" s="154" t="s">
         <v>223</v>
       </c>
-      <c r="AP24" s="112"/>
-      <c r="AQ24" s="112"/>
-      <c r="AR24" s="142" t="s">
+      <c r="AP24" s="110"/>
+      <c r="AQ24" s="110"/>
+      <c r="AR24" s="138" t="s">
         <v>12</v>
       </c>
       <c r="AS24" s="89">
@@ -7178,16 +7070,16 @@
       <c r="AX24" s="88" t="b">
         <v>1</v>
       </c>
-      <c r="AY24" s="147">
+      <c r="AY24" s="143">
         <v>25</v>
       </c>
-      <c r="AZ24" s="144">
+      <c r="AZ24" s="140">
         <v>0.7</v>
       </c>
-      <c r="BA24" s="124">
+      <c r="BA24" s="122">
         <v>0.5</v>
       </c>
-      <c r="BB24" s="128" t="s">
+      <c r="BB24" s="126" t="s">
         <v>187</v>
       </c>
       <c r="BC24" s="20" t="s">
@@ -7217,7 +7109,7 @@
       <c r="BK24" s="92">
         <v>0.6</v>
       </c>
-      <c r="BL24" s="134">
+      <c r="BL24" s="132">
         <v>1</v>
       </c>
       <c r="BM24" s="97">
@@ -7232,14 +7124,14 @@
       <c r="BP24" s="64">
         <v>25</v>
       </c>
-      <c r="BQ24" s="108"/>
-      <c r="BR24" s="108">
+      <c r="BQ24" s="52"/>
+      <c r="BR24" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS24" s="137">
+      <c r="BS24" s="180">
         <v>1</v>
       </c>
-      <c r="BT24" s="140" t="s">
+      <c r="BT24" s="179" t="s">
         <v>184</v>
       </c>
     </row>
@@ -7302,10 +7194,10 @@
         <v>0.7</v>
       </c>
       <c r="U25" s="43">
-        <v>1.37</v>
+        <v>1.27</v>
       </c>
       <c r="V25" s="25">
-        <v>1.57</v>
+        <v>1.47</v>
       </c>
       <c r="W25" s="48">
         <v>28</v>
@@ -7341,7 +7233,7 @@
       <c r="AG25" s="28">
         <v>52000</v>
       </c>
-      <c r="AH25" s="116">
+      <c r="AH25" s="114">
         <v>4</v>
       </c>
       <c r="AI25" s="105">
@@ -7351,24 +7243,24 @@
         <f>AI26</f>
         <v>0.05</v>
       </c>
-      <c r="AK25" s="183">
+      <c r="AK25" s="150">
         <v>0</v>
       </c>
-      <c r="AL25" s="148">
+      <c r="AL25" s="144">
         <v>12</v>
       </c>
-      <c r="AM25" s="186" t="s">
+      <c r="AM25" s="152" t="s">
         <v>83</v>
       </c>
-      <c r="AN25" s="185" t="s">
+      <c r="AN25" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="AO25" s="185" t="s">
+      <c r="AO25" s="151" t="s">
         <v>224</v>
       </c>
-      <c r="AP25" s="112"/>
-      <c r="AQ25" s="112"/>
-      <c r="AR25" s="142" t="s">
+      <c r="AP25" s="110"/>
+      <c r="AQ25" s="110"/>
+      <c r="AR25" s="138" t="s">
         <v>184</v>
       </c>
       <c r="AS25" s="41">
@@ -7389,16 +7281,16 @@
       <c r="AX25" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY25" s="146">
+      <c r="AY25" s="142">
         <v>25</v>
       </c>
-      <c r="AZ25" s="143">
+      <c r="AZ25" s="139">
         <v>0.7</v>
       </c>
-      <c r="BA25" s="123">
+      <c r="BA25" s="121">
         <v>0.4</v>
       </c>
-      <c r="BB25" s="127" t="s">
+      <c r="BB25" s="125" t="s">
         <v>81</v>
       </c>
       <c r="BC25" s="53" t="s">
@@ -7428,7 +7320,7 @@
       <c r="BK25" s="52">
         <v>0.3</v>
       </c>
-      <c r="BL25" s="133">
+      <c r="BL25" s="131">
         <v>0.4</v>
       </c>
       <c r="BM25" s="37">
@@ -7443,14 +7335,14 @@
       <c r="BP25" s="64">
         <v>25</v>
       </c>
-      <c r="BQ25" s="108"/>
-      <c r="BR25" s="108">
+      <c r="BQ25" s="52"/>
+      <c r="BR25" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS25" s="137">
+      <c r="BS25" s="180">
         <v>1</v>
       </c>
-      <c r="BT25" s="139" t="s">
+      <c r="BT25" s="178" t="s">
         <v>13</v>
       </c>
     </row>
@@ -7513,10 +7405,10 @@
         <v>0.8</v>
       </c>
       <c r="U26" s="43">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="V26" s="25">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="W26" s="48">
         <v>31</v>
@@ -7561,24 +7453,24 @@
       <c r="AJ26" s="59">
         <v>0.04</v>
       </c>
-      <c r="AK26" s="182">
+      <c r="AK26" s="149">
         <v>0</v>
       </c>
       <c r="AL26" s="61">
         <v>12</v>
       </c>
-      <c r="AM26" s="186" t="s">
+      <c r="AM26" s="152" t="s">
         <v>78</v>
       </c>
-      <c r="AN26" s="185" t="s">
+      <c r="AN26" s="151" t="s">
         <v>77</v>
       </c>
-      <c r="AO26" s="185" t="s">
+      <c r="AO26" s="151" t="s">
         <v>225</v>
       </c>
-      <c r="AP26" s="112"/>
-      <c r="AQ26" s="112"/>
-      <c r="AR26" s="142" t="s">
+      <c r="AP26" s="110"/>
+      <c r="AQ26" s="110"/>
+      <c r="AR26" s="138" t="s">
         <v>13</v>
       </c>
       <c r="AS26" s="41">
@@ -7599,16 +7491,16 @@
       <c r="AX26" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY26" s="146">
+      <c r="AY26" s="142">
         <v>25</v>
       </c>
-      <c r="AZ26" s="143">
+      <c r="AZ26" s="139">
         <v>0.75</v>
       </c>
-      <c r="BA26" s="123">
+      <c r="BA26" s="121">
         <v>0.4</v>
       </c>
-      <c r="BB26" s="129" t="s">
+      <c r="BB26" s="127" t="s">
         <v>76</v>
       </c>
       <c r="BC26" s="40" t="s">
@@ -7638,10 +7530,10 @@
       <c r="BK26" s="36">
         <v>0.7</v>
       </c>
-      <c r="BL26" s="135">
+      <c r="BL26" s="133">
         <v>1.03</v>
       </c>
-      <c r="BM26" s="130">
+      <c r="BM26" s="128">
         <v>59</v>
       </c>
       <c r="BN26" s="36">
@@ -7653,16 +7545,16 @@
       <c r="BP26" s="64">
         <v>25</v>
       </c>
-      <c r="BQ26" s="108" t="s">
+      <c r="BQ26" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="BR26" s="108">
+      <c r="BR26" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS26" s="137">
+      <c r="BS26" s="180">
         <v>1</v>
       </c>
-      <c r="BT26" s="139" t="s">
+      <c r="BT26" s="178" t="s">
         <v>14</v>
       </c>
     </row>
@@ -7694,16 +7586,16 @@
       <c r="J27" s="48">
         <v>35</v>
       </c>
-      <c r="K27" s="120">
+      <c r="K27" s="61">
         <v>45</v>
       </c>
-      <c r="L27" s="121">
+      <c r="L27" s="119">
         <v>25</v>
       </c>
       <c r="M27" s="47">
         <v>0</v>
       </c>
-      <c r="N27" s="118">
+      <c r="N27" s="116">
         <v>1000</v>
       </c>
       <c r="O27" s="25">
@@ -7725,10 +7617,10 @@
         <v>0.8</v>
       </c>
       <c r="U27" s="43">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="V27" s="25">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="W27" s="48">
         <v>31</v>
@@ -7764,7 +7656,7 @@
       <c r="AG27" s="25">
         <v>60000</v>
       </c>
-      <c r="AH27" s="115">
+      <c r="AH27" s="113">
         <v>5</v>
       </c>
       <c r="AI27" s="105">
@@ -7773,24 +7665,24 @@
       <c r="AJ27" s="54">
         <v>0.04</v>
       </c>
-      <c r="AK27" s="152">
+      <c r="AK27" s="148">
         <v>0</v>
       </c>
       <c r="AL27" s="58">
         <v>12</v>
       </c>
-      <c r="AM27" s="186" t="s">
+      <c r="AM27" s="152" t="s">
         <v>200</v>
       </c>
-      <c r="AN27" s="185" t="s">
+      <c r="AN27" s="151" t="s">
         <v>201</v>
       </c>
-      <c r="AO27" s="185" t="s">
+      <c r="AO27" s="151" t="s">
         <v>202</v>
       </c>
-      <c r="AP27" s="112"/>
-      <c r="AQ27" s="112"/>
-      <c r="AR27" s="142" t="s">
+      <c r="AP27" s="110"/>
+      <c r="AQ27" s="110"/>
+      <c r="AR27" s="138" t="s">
         <v>14</v>
       </c>
       <c r="AS27" s="41">
@@ -7811,16 +7703,16 @@
       <c r="AX27" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY27" s="146">
+      <c r="AY27" s="142">
         <v>25</v>
       </c>
-      <c r="AZ27" s="143">
+      <c r="AZ27" s="139">
         <v>0.75</v>
       </c>
-      <c r="BA27" s="123">
+      <c r="BA27" s="121">
         <v>0.4</v>
       </c>
-      <c r="BB27" s="129" t="s">
+      <c r="BB27" s="127" t="s">
         <v>198</v>
       </c>
       <c r="BC27" s="40" t="s">
@@ -7832,7 +7724,7 @@
       <c r="BE27" s="38">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF27" s="130">
+      <c r="BF27" s="128">
         <v>680</v>
       </c>
       <c r="BG27" s="102">
@@ -7850,10 +7742,10 @@
       <c r="BK27" s="36">
         <v>0.7</v>
       </c>
-      <c r="BL27" s="135">
+      <c r="BL27" s="133">
         <v>1.03</v>
       </c>
-      <c r="BM27" s="130">
+      <c r="BM27" s="128">
         <v>59</v>
       </c>
       <c r="BN27" s="36">
@@ -7868,223 +7760,223 @@
       <c r="BQ27" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="BR27" s="110">
+      <c r="BR27" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS27" s="138">
+      <c r="BS27" s="135">
         <v>1</v>
       </c>
-      <c r="BT27" s="139" t="s">
+      <c r="BT27" s="136" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:72" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="167" t="s">
+    <row r="28" spans="1:72" x14ac:dyDescent="0.25">
+      <c r="B28" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="168" t="s">
+      <c r="C28" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="D28" s="153" t="s">
+      <c r="D28" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="E28" s="153" t="s">
+      <c r="E28" s="52" t="s">
         <v>204</v>
       </c>
-      <c r="F28" s="154">
+      <c r="F28" s="51">
         <v>12</v>
       </c>
-      <c r="G28" s="154" t="s">
+      <c r="G28" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="H28" s="169">
+      <c r="H28" s="29">
         <v>700000</v>
       </c>
-      <c r="I28" s="170">
+      <c r="I28" s="49">
         <v>550</v>
       </c>
-      <c r="J28" s="155">
+      <c r="J28" s="48">
         <v>35</v>
       </c>
-      <c r="K28" s="58">
+      <c r="K28" s="118">
         <v>45</v>
       </c>
-      <c r="L28" s="157">
+      <c r="L28" s="119">
         <v>25</v>
       </c>
-      <c r="M28" s="159">
+      <c r="M28" s="47">
         <v>0</v>
       </c>
-      <c r="N28" s="162">
+      <c r="N28" s="116">
         <v>500</v>
       </c>
-      <c r="O28" s="156">
+      <c r="O28" s="25">
         <v>600</v>
       </c>
-      <c r="P28" s="157">
+      <c r="P28" s="25">
         <v>2.5</v>
       </c>
-      <c r="Q28" s="158">
+      <c r="Q28" s="25">
         <v>0</v>
       </c>
-      <c r="R28" s="159">
+      <c r="R28" s="25">
         <v>0.02</v>
       </c>
-      <c r="S28" s="158">
+      <c r="S28" s="44">
         <v>20</v>
       </c>
-      <c r="T28" s="158">
+      <c r="T28" s="44">
         <v>0.8</v>
       </c>
-      <c r="U28" s="162">
-        <v>2</v>
-      </c>
-      <c r="V28" s="160">
-        <v>2.1</v>
-      </c>
-      <c r="W28" s="161">
+      <c r="U28" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V28" s="25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W28" s="48">
         <v>31</v>
       </c>
-      <c r="X28" s="162">
+      <c r="X28" s="56">
         <v>2.0099999999999998</v>
       </c>
-      <c r="Y28" s="158">
+      <c r="Y28" s="25">
         <v>100</v>
       </c>
-      <c r="Z28" s="156">
+      <c r="Z28" s="25">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA28" s="158">
+      <c r="AA28" s="25">
         <v>20</v>
       </c>
-      <c r="AB28" s="158">
+      <c r="AB28" s="25">
         <v>14</v>
       </c>
       <c r="AC28" s="45">
         <v>475</v>
       </c>
-      <c r="AD28" s="158">
+      <c r="AD28" s="44">
         <v>12</v>
       </c>
-      <c r="AE28" s="158">
+      <c r="AE28" s="25">
         <v>7</v>
       </c>
-      <c r="AF28" s="158">
+      <c r="AF28" s="44">
         <v>10</v>
       </c>
-      <c r="AG28" s="158">
+      <c r="AG28" s="25">
         <v>65000</v>
       </c>
-      <c r="AH28" s="181">
+      <c r="AH28" s="113">
         <v>6</v>
       </c>
-      <c r="AI28" s="162">
+      <c r="AI28" s="105">
         <v>0.04</v>
       </c>
-      <c r="AJ28" s="171">
+      <c r="AJ28" s="54">
         <v>0.03</v>
       </c>
-      <c r="AK28" s="45">
+      <c r="AK28" s="148">
         <v>0</v>
       </c>
-      <c r="AL28" s="184">
+      <c r="AL28" s="58">
         <v>12</v>
       </c>
-      <c r="AM28" s="189" t="s">
+      <c r="AM28" s="152" t="s">
         <v>232</v>
       </c>
-      <c r="AN28" s="190" t="s">
+      <c r="AN28" s="151" t="s">
         <v>233</v>
       </c>
-      <c r="AO28" s="190" t="s">
+      <c r="AO28" s="151" t="s">
         <v>234</v>
       </c>
-      <c r="AP28" s="173"/>
-      <c r="AQ28" s="173"/>
-      <c r="AR28" s="163" t="s">
+      <c r="AP28" s="110"/>
+      <c r="AQ28" s="110"/>
+      <c r="AR28" s="138" t="s">
         <v>197</v>
       </c>
-      <c r="AS28" s="172">
+      <c r="AS28" s="41">
         <v>1.05</v>
       </c>
-      <c r="AT28" s="163">
+      <c r="AT28" s="23">
         <v>2</v>
       </c>
-      <c r="AU28" s="163">
+      <c r="AU28" s="23">
         <v>2</v>
       </c>
-      <c r="AV28" s="163" t="b">
+      <c r="AV28" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AW28" s="163" t="b">
+      <c r="AW28" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AX28" s="163" t="b">
+      <c r="AX28" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="AY28" s="174">
+      <c r="AY28" s="142">
         <v>25</v>
       </c>
-      <c r="AZ28" s="163">
+      <c r="AZ28" s="139">
         <v>0.75</v>
       </c>
-      <c r="BA28" s="163">
+      <c r="BA28" s="121">
         <v>0.4</v>
       </c>
-      <c r="BB28" s="175" t="s">
+      <c r="BB28" s="127" t="s">
         <v>235</v>
       </c>
-      <c r="BC28" s="176" t="s">
+      <c r="BC28" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="BD28" s="177">
+      <c r="BD28" s="39">
         <v>1.5E-3</v>
       </c>
-      <c r="BE28" s="154">
+      <c r="BE28" s="38">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF28" s="178">
+      <c r="BF28" s="128">
         <v>700</v>
       </c>
-      <c r="BG28" s="179">
+      <c r="BG28" s="102">
         <v>750</v>
       </c>
-      <c r="BH28" s="164">
+      <c r="BH28" s="36">
         <v>4.9000000000000004</v>
       </c>
-      <c r="BI28" s="164">
+      <c r="BI28" s="36">
         <v>9.5</v>
       </c>
-      <c r="BJ28" s="164">
+      <c r="BJ28" s="36">
         <v>1.7</v>
       </c>
-      <c r="BK28" s="164">
+      <c r="BK28" s="36">
         <v>0.7</v>
       </c>
-      <c r="BL28" s="164">
+      <c r="BL28" s="133">
         <v>1.03</v>
       </c>
-      <c r="BM28" s="178">
+      <c r="BM28" s="128">
         <v>59</v>
       </c>
-      <c r="BN28" s="164">
+      <c r="BN28" s="36">
         <v>15</v>
       </c>
-      <c r="BO28" s="164">
+      <c r="BO28" s="64">
         <v>0.4</v>
       </c>
-      <c r="BP28" s="164">
+      <c r="BP28" s="64">
         <v>25</v>
       </c>
-      <c r="BQ28" s="165"/>
-      <c r="BR28" s="166">
+      <c r="BQ28" s="35"/>
+      <c r="BR28" s="108">
         <v>0.2</v>
       </c>
-      <c r="BS28" s="166">
+      <c r="BS28" s="135">
         <v>1</v>
       </c>
-      <c r="BT28" s="180" t="s">
+      <c r="BT28" s="136" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8098,83 +7990,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="201" t="s">
+      <c r="J29" s="175" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="201"/>
-      <c r="L29" s="201"/>
-      <c r="M29" s="201"/>
-      <c r="N29" s="199" t="s">
+      <c r="K29" s="175"/>
+      <c r="L29" s="175"/>
+      <c r="M29" s="175"/>
+      <c r="N29" s="173" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="200"/>
-      <c r="P29" s="200"/>
-      <c r="Q29" s="200"/>
-      <c r="R29" s="200"/>
-      <c r="S29" s="200"/>
-      <c r="T29" s="200"/>
-      <c r="U29" s="197" t="s">
+      <c r="O29" s="174"/>
+      <c r="P29" s="174"/>
+      <c r="Q29" s="174"/>
+      <c r="R29" s="174"/>
+      <c r="S29" s="174"/>
+      <c r="T29" s="174"/>
+      <c r="U29" s="171" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="198"/>
+      <c r="V29" s="172"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="194" t="s">
+      <c r="X29" s="168" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="195"/>
-      <c r="Z29" s="195"/>
-      <c r="AA29" s="195"/>
-      <c r="AB29" s="196"/>
-      <c r="AC29" s="193" t="s">
+      <c r="Y29" s="169"/>
+      <c r="Z29" s="169"/>
+      <c r="AA29" s="169"/>
+      <c r="AB29" s="170"/>
+      <c r="AC29" s="167" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="193"/>
-      <c r="AE29" s="193"/>
-      <c r="AF29" s="193"/>
-      <c r="AG29" s="193"/>
+      <c r="AD29" s="167"/>
+      <c r="AE29" s="167"/>
+      <c r="AF29" s="167"/>
+      <c r="AG29" s="167"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="208" t="s">
+      <c r="AI29" s="163" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="208"/>
-      <c r="AK29" s="202" t="s">
+      <c r="AJ29" s="163"/>
+      <c r="AK29" s="157" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="202"/>
-      <c r="AM29" s="209" t="s">
+      <c r="AL29" s="157"/>
+      <c r="AM29" s="164" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="210"/>
-      <c r="AO29" s="210"/>
-      <c r="AP29" s="210"/>
-      <c r="AQ29" s="210"/>
-      <c r="AR29" s="211"/>
-      <c r="AS29" s="203" t="s">
+      <c r="AN29" s="165"/>
+      <c r="AO29" s="165"/>
+      <c r="AP29" s="165"/>
+      <c r="AQ29" s="165"/>
+      <c r="AR29" s="166"/>
+      <c r="AS29" s="158" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="204"/>
-      <c r="AU29" s="204"/>
-      <c r="AV29" s="204"/>
-      <c r="AW29" s="204"/>
-      <c r="AX29" s="204"/>
-      <c r="AY29" s="205"/>
+      <c r="AT29" s="159"/>
+      <c r="AU29" s="159"/>
+      <c r="AV29" s="159"/>
+      <c r="AW29" s="159"/>
+      <c r="AX29" s="159"/>
+      <c r="AY29" s="160"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="207" t="s">
+      <c r="BF29" s="162" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="207"/>
-      <c r="BH29" s="207"/>
-      <c r="BI29" s="207"/>
-      <c r="BJ29" s="207"/>
-      <c r="BK29" s="207"/>
-      <c r="BL29" s="207"/>
+      <c r="BG29" s="162"/>
+      <c r="BH29" s="162"/>
+      <c r="BI29" s="162"/>
+      <c r="BJ29" s="162"/>
+      <c r="BK29" s="162"/>
+      <c r="BL29" s="162"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -8370,19 +8262,19 @@
       <c r="D35" s="31">
         <v>0.2</v>
       </c>
-      <c r="E35" s="141">
+      <c r="E35" s="137">
         <v>8</v>
       </c>
-      <c r="F35" s="141">
+      <c r="F35" s="137">
         <v>1.5</v>
       </c>
-      <c r="G35" s="141">
+      <c r="G35" s="137">
         <v>1.2</v>
       </c>
-      <c r="H35" s="141">
+      <c r="H35" s="137">
         <v>1.2</v>
       </c>
-      <c r="I35" s="141">
+      <c r="I35" s="137">
         <v>10</v>
       </c>
     </row>
@@ -9521,122 +9413,122 @@
       <c r="D59">
         <v>20</v>
       </c>
-      <c r="E59" s="191">
+      <c r="E59" s="155">
         <v>4571</v>
       </c>
-      <c r="F59" s="192">
+      <c r="F59" s="156">
         <v>13714</v>
       </c>
-      <c r="G59" s="192">
+      <c r="G59" s="156">
         <v>27428</v>
       </c>
-      <c r="H59" s="192">
+      <c r="H59" s="156">
         <v>45713</v>
       </c>
-      <c r="I59" s="192">
+      <c r="I59" s="156">
         <v>68569</v>
       </c>
-      <c r="J59" s="192">
+      <c r="J59" s="156">
         <v>95997</v>
       </c>
-      <c r="K59" s="192">
+      <c r="K59" s="156">
         <v>127995</v>
       </c>
-      <c r="L59" s="192">
+      <c r="L59" s="156">
         <v>164565</v>
       </c>
-      <c r="M59" s="192">
+      <c r="M59" s="156">
         <v>205707</v>
       </c>
-      <c r="N59" s="192">
+      <c r="N59" s="156">
         <v>251419</v>
       </c>
-      <c r="O59" s="192">
+      <c r="O59" s="156">
         <v>301703</v>
       </c>
-      <c r="P59" s="192">
+      <c r="P59" s="156">
         <v>356559</v>
       </c>
-      <c r="Q59" s="192">
+      <c r="Q59" s="156">
         <v>415985</v>
       </c>
-      <c r="R59" s="192">
+      <c r="R59" s="156">
         <v>479983</v>
       </c>
-      <c r="S59" s="192">
+      <c r="S59" s="156">
         <v>548552</v>
       </c>
-      <c r="T59" s="192">
+      <c r="T59" s="156">
         <v>621692</v>
       </c>
-      <c r="U59" s="192">
+      <c r="U59" s="156">
         <v>699403</v>
       </c>
-      <c r="V59" s="192">
+      <c r="V59" s="156">
         <v>781686</v>
       </c>
-      <c r="W59" s="192">
+      <c r="W59" s="156">
         <v>868540</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="121" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C10">
-    <cfRule type="duplicateValues" dxfId="120" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
+    <cfRule type="duplicateValues" dxfId="122" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="duplicateValues" dxfId="121" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BT24">
+    <cfRule type="duplicateValues" dxfId="120" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
     <cfRule type="duplicateValues" dxfId="119" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
+  <conditionalFormatting sqref="BT27">
     <cfRule type="duplicateValues" dxfId="118" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="117" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="116" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="115" priority="9"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="114" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="113" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="112" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="111" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="110" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT28">
-    <cfRule type="duplicateValues" dxfId="108" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ28">
-    <cfRule type="duplicateValues" dxfId="107" priority="3"/>
+  <conditionalFormatting sqref="BQ28:BS28">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D28">

</xml_diff>

<commit_message>
added content for Anniversary and Pet gelato
Former-commit-id: 147ddfd3aa0f3d5df65ae27681d7ce7a688f4a09
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="239">
   <si>
     <t>[sku]</t>
   </si>
@@ -738,13 +738,16 @@
   </si>
   <si>
     <t>PREFABS</t>
+  </si>
+  <si>
+    <t>[anniversaryCakeSlices]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -832,6 +835,12 @@
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1294,7 +1303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1722,6 +1731,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1752,85 +1806,36 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="125">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+  <dxfs count="123">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -4320,105 +4325,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106" totalsRowBorderDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104" totalsRowBorderDxfId="103">
   <autoFilter ref="B15:BT28"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="104"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="103"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="102"/>
-    <tableColumn id="65" name="[type]" dataDxfId="101"/>
-    <tableColumn id="3" name="[order]" dataDxfId="100"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="99"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="98"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="97"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="96"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="95"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="94"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="93"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="92"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="91"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="90"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="89"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="88"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="87"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="86"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="85"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="84"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="83"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="82"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="81"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="80">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="102"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="101"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="100"/>
+    <tableColumn id="65" name="[type]" dataDxfId="99"/>
+    <tableColumn id="3" name="[order]" dataDxfId="98"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="97"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="96"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="95"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="94"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="93"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="92"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="91"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="90"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="89"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="88"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="87"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="86"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="85"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="84"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="83"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="82"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="81"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="80"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="79"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="78">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="79"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="78"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="77"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="76"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="75"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="74"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="73"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="72"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="71"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="70">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="77"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="76"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="75"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="74"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="73"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="72"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="71"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="70"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="69"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="68">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="69"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="68"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="67"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="66"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="65"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="64"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="63"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="62"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="61"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="60"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="59"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="58"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="57"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="56"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="55"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="54"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="53"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="52">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="67"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="66"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="65"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="64"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="63"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="62"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="61"/>
+    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="60"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="59"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="58"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="57"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="56"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="55"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="54"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="53"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="52"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="51"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="50">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="51">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="49">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="50"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="49"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="48"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="47">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="48"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="47"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="46"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="45">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="46"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="45"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="44"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="43"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="42"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="41"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="40"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="39"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="38"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="37"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="36"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="35"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="34"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="44"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="43"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="42"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="41"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="40"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="39"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="38"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="37"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="36"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="35"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="34"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="33"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G10" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G10" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B4:G10"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="29"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="28"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="27"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="26">
+    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4427,24 +4432,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:I35" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
-  <autoFilter ref="B34:I35"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="21"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:J35" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="B34:J35"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="19"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="18"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="17"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="16"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="15"/>
+    <tableColumn id="8" name="[superfuryMax]" dataDxfId="17"/>
+    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="16"/>
+    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="15"/>
+    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="14"/>
+    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="13"/>
+    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="B46:W59"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -4475,14 +4481,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="B39:F42"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="6"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="4"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="3"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="4"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="3"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="2"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4756,8 +4762,8 @@
   </sheetPr>
   <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="BP21" sqref="BP21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5023,10 +5029,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="161"/>
-      <c r="AP14" s="161"/>
-      <c r="AQ14" s="161"/>
-      <c r="AR14" s="161"/>
+      <c r="AO14" s="176"/>
+      <c r="AP14" s="176"/>
+      <c r="AQ14" s="176"/>
+      <c r="AR14" s="176"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -5865,10 +5871,10 @@
       <c r="BR18" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS18" s="180">
+      <c r="BS18" s="161">
         <v>1</v>
       </c>
-      <c r="BT18" s="178" t="s">
+      <c r="BT18" s="159" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6074,10 +6080,10 @@
       <c r="BR19" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS19" s="180">
+      <c r="BS19" s="161">
         <v>1</v>
       </c>
-      <c r="BT19" s="178" t="s">
+      <c r="BT19" s="159" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6279,16 +6285,16 @@
       <c r="BP20" s="64">
         <v>25</v>
       </c>
-      <c r="BQ20" s="176" t="s">
+      <c r="BQ20" s="157" t="s">
         <v>209</v>
       </c>
-      <c r="BR20" s="177">
+      <c r="BR20" s="158">
         <v>0.2</v>
       </c>
-      <c r="BS20" s="181">
+      <c r="BS20" s="162">
         <v>1</v>
       </c>
-      <c r="BT20" s="178" t="s">
+      <c r="BT20" s="159" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6496,10 +6502,10 @@
       <c r="BR21" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS21" s="180">
+      <c r="BS21" s="161">
         <v>1</v>
       </c>
-      <c r="BT21" s="178" t="s">
+      <c r="BT21" s="159" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6701,16 +6707,16 @@
       <c r="BP22" s="64">
         <v>25</v>
       </c>
-      <c r="BQ22" s="176" t="s">
+      <c r="BQ22" s="157" t="s">
         <v>210</v>
       </c>
-      <c r="BR22" s="177">
+      <c r="BR22" s="158">
         <v>0.2</v>
       </c>
-      <c r="BS22" s="181">
+      <c r="BS22" s="162">
         <v>1</v>
       </c>
-      <c r="BT22" s="178" t="s">
+      <c r="BT22" s="159" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6918,10 +6924,10 @@
       <c r="BR23" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS23" s="180">
+      <c r="BS23" s="161">
         <v>1</v>
       </c>
-      <c r="BT23" s="178" t="s">
+      <c r="BT23" s="159" t="s">
         <v>12</v>
       </c>
     </row>
@@ -7128,10 +7134,10 @@
       <c r="BR24" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS24" s="180">
+      <c r="BS24" s="161">
         <v>1</v>
       </c>
-      <c r="BT24" s="179" t="s">
+      <c r="BT24" s="160" t="s">
         <v>184</v>
       </c>
     </row>
@@ -7339,10 +7345,10 @@
       <c r="BR25" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS25" s="180">
+      <c r="BS25" s="161">
         <v>1</v>
       </c>
-      <c r="BT25" s="178" t="s">
+      <c r="BT25" s="159" t="s">
         <v>13</v>
       </c>
     </row>
@@ -7551,10 +7557,10 @@
       <c r="BR26" s="52">
         <v>0.2</v>
       </c>
-      <c r="BS26" s="180">
+      <c r="BS26" s="161">
         <v>1</v>
       </c>
-      <c r="BT26" s="178" t="s">
+      <c r="BT26" s="159" t="s">
         <v>14</v>
       </c>
     </row>
@@ -7990,83 +7996,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="175" t="s">
+      <c r="J29" s="171" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="175"/>
-      <c r="L29" s="175"/>
-      <c r="M29" s="175"/>
-      <c r="N29" s="173" t="s">
+      <c r="K29" s="171"/>
+      <c r="L29" s="171"/>
+      <c r="M29" s="171"/>
+      <c r="N29" s="169" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="174"/>
-      <c r="P29" s="174"/>
-      <c r="Q29" s="174"/>
-      <c r="R29" s="174"/>
-      <c r="S29" s="174"/>
-      <c r="T29" s="174"/>
-      <c r="U29" s="171" t="s">
+      <c r="O29" s="170"/>
+      <c r="P29" s="170"/>
+      <c r="Q29" s="170"/>
+      <c r="R29" s="170"/>
+      <c r="S29" s="170"/>
+      <c r="T29" s="170"/>
+      <c r="U29" s="167" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="172"/>
+      <c r="V29" s="168"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="168" t="s">
+      <c r="X29" s="164" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="169"/>
-      <c r="Z29" s="169"/>
-      <c r="AA29" s="169"/>
-      <c r="AB29" s="170"/>
-      <c r="AC29" s="167" t="s">
+      <c r="Y29" s="165"/>
+      <c r="Z29" s="165"/>
+      <c r="AA29" s="165"/>
+      <c r="AB29" s="166"/>
+      <c r="AC29" s="163" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="167"/>
-      <c r="AE29" s="167"/>
-      <c r="AF29" s="167"/>
-      <c r="AG29" s="167"/>
+      <c r="AD29" s="163"/>
+      <c r="AE29" s="163"/>
+      <c r="AF29" s="163"/>
+      <c r="AG29" s="163"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="163" t="s">
+      <c r="AI29" s="178" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="163"/>
-      <c r="AK29" s="157" t="s">
+      <c r="AJ29" s="178"/>
+      <c r="AK29" s="172" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="157"/>
-      <c r="AM29" s="164" t="s">
+      <c r="AL29" s="172"/>
+      <c r="AM29" s="179" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="165"/>
-      <c r="AO29" s="165"/>
-      <c r="AP29" s="165"/>
-      <c r="AQ29" s="165"/>
-      <c r="AR29" s="166"/>
-      <c r="AS29" s="158" t="s">
+      <c r="AN29" s="180"/>
+      <c r="AO29" s="180"/>
+      <c r="AP29" s="180"/>
+      <c r="AQ29" s="180"/>
+      <c r="AR29" s="181"/>
+      <c r="AS29" s="173" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="159"/>
-      <c r="AU29" s="159"/>
-      <c r="AV29" s="159"/>
-      <c r="AW29" s="159"/>
-      <c r="AX29" s="159"/>
-      <c r="AY29" s="160"/>
+      <c r="AT29" s="174"/>
+      <c r="AU29" s="174"/>
+      <c r="AV29" s="174"/>
+      <c r="AW29" s="174"/>
+      <c r="AX29" s="174"/>
+      <c r="AY29" s="175"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="162" t="s">
+      <c r="BF29" s="177" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="162"/>
-      <c r="BH29" s="162"/>
-      <c r="BI29" s="162"/>
-      <c r="BJ29" s="162"/>
-      <c r="BK29" s="162"/>
-      <c r="BL29" s="162"/>
+      <c r="BG29" s="177"/>
+      <c r="BH29" s="177"/>
+      <c r="BI29" s="177"/>
+      <c r="BJ29" s="177"/>
+      <c r="BK29" s="177"/>
+      <c r="BL29" s="177"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -8251,6 +8257,9 @@
       <c r="I34" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="J34" s="183" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="35" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
@@ -8276,6 +8285,9 @@
       </c>
       <c r="I35" s="137">
         <v>10</v>
+      </c>
+      <c r="J35" s="182">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -9473,62 +9485,62 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="124" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C10">
-    <cfRule type="duplicateValues" dxfId="123" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="122" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="121" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="120" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="119" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="118" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="117" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="116" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="115" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="114" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="113" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT28">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ28:BS28">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D28">

</xml_diff>

<commit_message>
Dragons from Devil will be unlocked (available to buy with PC) as soon as player gets Blaze
Former-commit-id: baed704e133e2d312ae6c8c54c2977b38191e1a0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -841,6 +841,7 @@
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1749,94 +1750,72 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="123">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2056,6 +2035,28 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -4443,14 +4444,14 @@
     <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="15"/>
     <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="14"/>
     <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="13"/>
-    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="0"/>
+    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B46:W59"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -4481,14 +4482,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B39:F42"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="4"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="3"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="2"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="1"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4762,8 +4763,8 @@
   </sheetPr>
   <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="AF7" workbookViewId="0">
+      <selection activeCell="AR27" sqref="AR27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5029,10 +5030,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="176"/>
-      <c r="AP14" s="176"/>
-      <c r="AQ14" s="176"/>
-      <c r="AR14" s="176"/>
+      <c r="AO14" s="169"/>
+      <c r="AP14" s="169"/>
+      <c r="AQ14" s="169"/>
+      <c r="AR14" s="169"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -7056,7 +7057,7 @@
       <c r="AP24" s="110"/>
       <c r="AQ24" s="110"/>
       <c r="AR24" s="138" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AS24" s="89">
         <v>1.3</v>
@@ -7267,7 +7268,7 @@
       <c r="AP25" s="110"/>
       <c r="AQ25" s="110"/>
       <c r="AR25" s="138" t="s">
-        <v>184</v>
+        <v>11</v>
       </c>
       <c r="AS25" s="41">
         <v>1.2</v>
@@ -7477,7 +7478,7 @@
       <c r="AP26" s="110"/>
       <c r="AQ26" s="110"/>
       <c r="AR26" s="138" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AS26" s="41">
         <v>1.05</v>
@@ -7689,7 +7690,7 @@
       <c r="AP27" s="110"/>
       <c r="AQ27" s="110"/>
       <c r="AR27" s="138" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AS27" s="41">
         <v>1.05</v>
@@ -7901,7 +7902,7 @@
       <c r="AP28" s="110"/>
       <c r="AQ28" s="110"/>
       <c r="AR28" s="138" t="s">
-        <v>197</v>
+        <v>11</v>
       </c>
       <c r="AS28" s="41">
         <v>1.05</v>
@@ -7996,83 +7997,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="171" t="s">
+      <c r="J29" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="171"/>
-      <c r="L29" s="171"/>
-      <c r="M29" s="171"/>
-      <c r="N29" s="169" t="s">
+      <c r="K29" s="183"/>
+      <c r="L29" s="183"/>
+      <c r="M29" s="183"/>
+      <c r="N29" s="181" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="170"/>
-      <c r="P29" s="170"/>
-      <c r="Q29" s="170"/>
-      <c r="R29" s="170"/>
-      <c r="S29" s="170"/>
-      <c r="T29" s="170"/>
-      <c r="U29" s="167" t="s">
+      <c r="O29" s="182"/>
+      <c r="P29" s="182"/>
+      <c r="Q29" s="182"/>
+      <c r="R29" s="182"/>
+      <c r="S29" s="182"/>
+      <c r="T29" s="182"/>
+      <c r="U29" s="179" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="168"/>
+      <c r="V29" s="180"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="164" t="s">
+      <c r="X29" s="176" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="165"/>
-      <c r="Z29" s="165"/>
-      <c r="AA29" s="165"/>
-      <c r="AB29" s="166"/>
-      <c r="AC29" s="163" t="s">
+      <c r="Y29" s="177"/>
+      <c r="Z29" s="177"/>
+      <c r="AA29" s="177"/>
+      <c r="AB29" s="178"/>
+      <c r="AC29" s="175" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="163"/>
-      <c r="AE29" s="163"/>
-      <c r="AF29" s="163"/>
-      <c r="AG29" s="163"/>
+      <c r="AD29" s="175"/>
+      <c r="AE29" s="175"/>
+      <c r="AF29" s="175"/>
+      <c r="AG29" s="175"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="178" t="s">
+      <c r="AI29" s="171" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="178"/>
-      <c r="AK29" s="172" t="s">
+      <c r="AJ29" s="171"/>
+      <c r="AK29" s="165" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="172"/>
-      <c r="AM29" s="179" t="s">
+      <c r="AL29" s="165"/>
+      <c r="AM29" s="172" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="180"/>
-      <c r="AO29" s="180"/>
-      <c r="AP29" s="180"/>
-      <c r="AQ29" s="180"/>
-      <c r="AR29" s="181"/>
-      <c r="AS29" s="173" t="s">
+      <c r="AN29" s="173"/>
+      <c r="AO29" s="173"/>
+      <c r="AP29" s="173"/>
+      <c r="AQ29" s="173"/>
+      <c r="AR29" s="174"/>
+      <c r="AS29" s="166" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="174"/>
-      <c r="AU29" s="174"/>
-      <c r="AV29" s="174"/>
-      <c r="AW29" s="174"/>
-      <c r="AX29" s="174"/>
-      <c r="AY29" s="175"/>
+      <c r="AT29" s="167"/>
+      <c r="AU29" s="167"/>
+      <c r="AV29" s="167"/>
+      <c r="AW29" s="167"/>
+      <c r="AX29" s="167"/>
+      <c r="AY29" s="168"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="177" t="s">
+      <c r="BF29" s="170" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="177"/>
-      <c r="BH29" s="177"/>
-      <c r="BI29" s="177"/>
-      <c r="BJ29" s="177"/>
-      <c r="BK29" s="177"/>
-      <c r="BL29" s="177"/>
+      <c r="BG29" s="170"/>
+      <c r="BH29" s="170"/>
+      <c r="BI29" s="170"/>
+      <c r="BJ29" s="170"/>
+      <c r="BK29" s="170"/>
+      <c r="BL29" s="170"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -8257,7 +8258,7 @@
       <c r="I34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J34" s="183" t="s">
+      <c r="J34" s="164" t="s">
         <v>238</v>
       </c>
     </row>
@@ -8286,7 +8287,7 @@
       <c r="I35" s="137">
         <v>10</v>
       </c>
-      <c r="J35" s="182">
+      <c r="J35" s="163">
         <v>6</v>
       </c>
     </row>
@@ -9485,17 +9486,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="122" priority="17"/>

</xml_diff>

<commit_message>
As we can't do the AB to test unlock dragons options right now, we keep current flow
Former-commit-id: 113d38f374aedf79f51d531923dbe95a997f9c24
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1754,6 +1754,33 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1782,33 +1809,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4763,8 +4763,8 @@
   </sheetPr>
   <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF7" workbookViewId="0">
-      <selection activeCell="AR27" sqref="AR27"/>
+    <sheetView tabSelected="1" topLeftCell="AG7" workbookViewId="0">
+      <selection activeCell="AR23" sqref="AR23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5030,10 +5030,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="169"/>
-      <c r="AP14" s="169"/>
-      <c r="AQ14" s="169"/>
-      <c r="AR14" s="169"/>
+      <c r="AO14" s="178"/>
+      <c r="AP14" s="178"/>
+      <c r="AQ14" s="178"/>
+      <c r="AR14" s="178"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -7057,7 +7057,7 @@
       <c r="AP24" s="110"/>
       <c r="AQ24" s="110"/>
       <c r="AR24" s="138" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AS24" s="89">
         <v>1.3</v>
@@ -7268,7 +7268,7 @@
       <c r="AP25" s="110"/>
       <c r="AQ25" s="110"/>
       <c r="AR25" s="138" t="s">
-        <v>11</v>
+        <v>184</v>
       </c>
       <c r="AS25" s="41">
         <v>1.2</v>
@@ -7478,7 +7478,7 @@
       <c r="AP26" s="110"/>
       <c r="AQ26" s="110"/>
       <c r="AR26" s="138" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AS26" s="41">
         <v>1.05</v>
@@ -7690,7 +7690,7 @@
       <c r="AP27" s="110"/>
       <c r="AQ27" s="110"/>
       <c r="AR27" s="138" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AS27" s="41">
         <v>1.05</v>
@@ -7902,7 +7902,7 @@
       <c r="AP28" s="110"/>
       <c r="AQ28" s="110"/>
       <c r="AR28" s="138" t="s">
-        <v>11</v>
+        <v>197</v>
       </c>
       <c r="AS28" s="41">
         <v>1.05</v>
@@ -7997,83 +7997,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="183" t="s">
+      <c r="J29" s="173" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="183"/>
-      <c r="L29" s="183"/>
-      <c r="M29" s="183"/>
-      <c r="N29" s="181" t="s">
+      <c r="K29" s="173"/>
+      <c r="L29" s="173"/>
+      <c r="M29" s="173"/>
+      <c r="N29" s="171" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="182"/>
-      <c r="P29" s="182"/>
-      <c r="Q29" s="182"/>
-      <c r="R29" s="182"/>
-      <c r="S29" s="182"/>
-      <c r="T29" s="182"/>
-      <c r="U29" s="179" t="s">
+      <c r="O29" s="172"/>
+      <c r="P29" s="172"/>
+      <c r="Q29" s="172"/>
+      <c r="R29" s="172"/>
+      <c r="S29" s="172"/>
+      <c r="T29" s="172"/>
+      <c r="U29" s="169" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="180"/>
+      <c r="V29" s="170"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="176" t="s">
+      <c r="X29" s="166" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="177"/>
-      <c r="Z29" s="177"/>
-      <c r="AA29" s="177"/>
-      <c r="AB29" s="178"/>
-      <c r="AC29" s="175" t="s">
+      <c r="Y29" s="167"/>
+      <c r="Z29" s="167"/>
+      <c r="AA29" s="167"/>
+      <c r="AB29" s="168"/>
+      <c r="AC29" s="165" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="175"/>
-      <c r="AE29" s="175"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="175"/>
+      <c r="AD29" s="165"/>
+      <c r="AE29" s="165"/>
+      <c r="AF29" s="165"/>
+      <c r="AG29" s="165"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="171" t="s">
+      <c r="AI29" s="180" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="171"/>
-      <c r="AK29" s="165" t="s">
+      <c r="AJ29" s="180"/>
+      <c r="AK29" s="174" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="165"/>
-      <c r="AM29" s="172" t="s">
+      <c r="AL29" s="174"/>
+      <c r="AM29" s="181" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="173"/>
-      <c r="AO29" s="173"/>
-      <c r="AP29" s="173"/>
-      <c r="AQ29" s="173"/>
-      <c r="AR29" s="174"/>
-      <c r="AS29" s="166" t="s">
+      <c r="AN29" s="182"/>
+      <c r="AO29" s="182"/>
+      <c r="AP29" s="182"/>
+      <c r="AQ29" s="182"/>
+      <c r="AR29" s="183"/>
+      <c r="AS29" s="175" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="167"/>
-      <c r="AU29" s="167"/>
-      <c r="AV29" s="167"/>
-      <c r="AW29" s="167"/>
-      <c r="AX29" s="167"/>
-      <c r="AY29" s="168"/>
+      <c r="AT29" s="176"/>
+      <c r="AU29" s="176"/>
+      <c r="AV29" s="176"/>
+      <c r="AW29" s="176"/>
+      <c r="AX29" s="176"/>
+      <c r="AY29" s="177"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="170" t="s">
+      <c r="BF29" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="170"/>
-      <c r="BH29" s="170"/>
-      <c r="BI29" s="170"/>
-      <c r="BJ29" s="170"/>
-      <c r="BK29" s="170"/>
-      <c r="BL29" s="170"/>
+      <c r="BG29" s="179"/>
+      <c r="BH29" s="179"/>
+      <c r="BI29" s="179"/>
+      <c r="BJ29" s="179"/>
+      <c r="BK29" s="179"/>
+      <c r="BL29" s="179"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -9486,17 +9486,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="122" priority="17"/>

</xml_diff>

<commit_message>
Adding new tier for Legendary dragons
Former-commit-id: 8d45f9c70ac3913c26ef56b2ac682ef9bd62fcb7
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="242">
   <si>
     <t>[sku]</t>
   </si>
@@ -741,13 +741,22 @@
   </si>
   <si>
     <t>[anniversaryCakeSlices]</t>
+  </si>
+  <si>
+    <t>tier_6</t>
+  </si>
+  <si>
+    <t>icon_special</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_TIER_6_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,6 +851,13 @@
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1304,7 +1320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1754,6 +1770,36 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1781,41 +1827,42 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="123">
+  <dxfs count="126">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -4326,105 +4373,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104" totalsRowBorderDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="110" dataDxfId="108" headerRowBorderDxfId="109" tableBorderDxfId="107" totalsRowBorderDxfId="106">
   <autoFilter ref="B15:BT28"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="102"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="101"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="100"/>
-    <tableColumn id="65" name="[type]" dataDxfId="99"/>
-    <tableColumn id="3" name="[order]" dataDxfId="98"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="97"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="96"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="95"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="94"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="93"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="92"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="91"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="90"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="89"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="88"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="87"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="86"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="85"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="84"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="83"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="82"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="81"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="80"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="79"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="78">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="105"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="104"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="103"/>
+    <tableColumn id="65" name="[type]" dataDxfId="102"/>
+    <tableColumn id="3" name="[order]" dataDxfId="101"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="100"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="99"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="98"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="97"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="96"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="95"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="94"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="93"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="92"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="91"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="90"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="89"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="88"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="87"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="86"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="85"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="84"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="83"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="82"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="81">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="77"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="76"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="75"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="74"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="73"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="72"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="71"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="70"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="69"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="68">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="80"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="79"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="78"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="77"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="76"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="75"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="74"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="73"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="72"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="71">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="67"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="66"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="65"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="64"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="63"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="62"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="61"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="60"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="59"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="58"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="57"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="56"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="55"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="54"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="53"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="52"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="51"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="50">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="70"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="69"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="68"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="67"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="66"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="65"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="64"/>
+    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="63"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="62"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="61"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="60"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="59"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="58"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="57"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="56"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="55"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="54"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="53">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="49">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="52">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="48"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="47"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="46"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="45">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="51"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="50"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="49"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="48">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="44"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="43"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="42"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="41"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="40"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="39"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="38"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="37"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="36"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="35"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="34"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="33"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="47"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="46"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="45"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="44"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="43"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="42"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="41"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="40"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="39"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="38"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="37"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="36"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G10" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="B4:G10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G11" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+  <autoFilter ref="B4:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="30"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="24">
+    <tableColumn id="10" name="[icon]" dataDxfId="29"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="28"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="27">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4433,25 +4480,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:J35" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:J35" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="B34:J35"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="22"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="21"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="17"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="16"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="15"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="14"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="13"/>
-    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="12"/>
+    <tableColumn id="8" name="[superfuryMax]" dataDxfId="20"/>
+    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="19"/>
+    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="18"/>
+    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="17"/>
+    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="16"/>
+    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="B46:W59"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -4482,14 +4529,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B39:F42"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="6"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="4"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4763,8 +4810,8 @@
   </sheetPr>
   <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG7" workbookViewId="0">
-      <selection activeCell="AR23" sqref="AR23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4980,6 +5027,26 @@
         <v>230</v>
       </c>
     </row>
+    <row r="11" spans="2:72" x14ac:dyDescent="0.25">
+      <c r="B11" s="184" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="85" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="147">
+        <v>5</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="F11" s="15">
+        <v>4</v>
+      </c>
+      <c r="G11" s="145" t="s">
+        <v>241</v>
+      </c>
+    </row>
     <row r="12" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:72" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
@@ -5030,10 +5097,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="178"/>
-      <c r="AP14" s="178"/>
-      <c r="AQ14" s="178"/>
-      <c r="AR14" s="178"/>
+      <c r="AO14" s="169"/>
+      <c r="AP14" s="169"/>
+      <c r="AQ14" s="169"/>
+      <c r="AR14" s="169"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -7997,83 +8064,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="173" t="s">
+      <c r="J29" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="173"/>
-      <c r="L29" s="173"/>
-      <c r="M29" s="173"/>
-      <c r="N29" s="171" t="s">
+      <c r="K29" s="183"/>
+      <c r="L29" s="183"/>
+      <c r="M29" s="183"/>
+      <c r="N29" s="181" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="172"/>
-      <c r="P29" s="172"/>
-      <c r="Q29" s="172"/>
-      <c r="R29" s="172"/>
-      <c r="S29" s="172"/>
-      <c r="T29" s="172"/>
-      <c r="U29" s="169" t="s">
+      <c r="O29" s="182"/>
+      <c r="P29" s="182"/>
+      <c r="Q29" s="182"/>
+      <c r="R29" s="182"/>
+      <c r="S29" s="182"/>
+      <c r="T29" s="182"/>
+      <c r="U29" s="179" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="170"/>
+      <c r="V29" s="180"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="166" t="s">
+      <c r="X29" s="176" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="167"/>
-      <c r="Z29" s="167"/>
-      <c r="AA29" s="167"/>
-      <c r="AB29" s="168"/>
-      <c r="AC29" s="165" t="s">
+      <c r="Y29" s="177"/>
+      <c r="Z29" s="177"/>
+      <c r="AA29" s="177"/>
+      <c r="AB29" s="178"/>
+      <c r="AC29" s="175" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="165"/>
-      <c r="AE29" s="165"/>
-      <c r="AF29" s="165"/>
-      <c r="AG29" s="165"/>
+      <c r="AD29" s="175"/>
+      <c r="AE29" s="175"/>
+      <c r="AF29" s="175"/>
+      <c r="AG29" s="175"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="180" t="s">
+      <c r="AI29" s="171" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="180"/>
-      <c r="AK29" s="174" t="s">
+      <c r="AJ29" s="171"/>
+      <c r="AK29" s="165" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="174"/>
-      <c r="AM29" s="181" t="s">
+      <c r="AL29" s="165"/>
+      <c r="AM29" s="172" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="182"/>
-      <c r="AO29" s="182"/>
-      <c r="AP29" s="182"/>
-      <c r="AQ29" s="182"/>
-      <c r="AR29" s="183"/>
-      <c r="AS29" s="175" t="s">
+      <c r="AN29" s="173"/>
+      <c r="AO29" s="173"/>
+      <c r="AP29" s="173"/>
+      <c r="AQ29" s="173"/>
+      <c r="AR29" s="174"/>
+      <c r="AS29" s="166" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="176"/>
-      <c r="AU29" s="176"/>
-      <c r="AV29" s="176"/>
-      <c r="AW29" s="176"/>
-      <c r="AX29" s="176"/>
-      <c r="AY29" s="177"/>
+      <c r="AT29" s="167"/>
+      <c r="AU29" s="167"/>
+      <c r="AV29" s="167"/>
+      <c r="AW29" s="167"/>
+      <c r="AX29" s="167"/>
+      <c r="AY29" s="168"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="179" t="s">
+      <c r="BF29" s="170" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="179"/>
-      <c r="BH29" s="179"/>
-      <c r="BI29" s="179"/>
-      <c r="BJ29" s="179"/>
-      <c r="BK29" s="179"/>
-      <c r="BL29" s="179"/>
+      <c r="BG29" s="170"/>
+      <c r="BH29" s="170"/>
+      <c r="BI29" s="170"/>
+      <c r="BJ29" s="170"/>
+      <c r="BK29" s="170"/>
+      <c r="BL29" s="170"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -9486,62 +9553,68 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
+    <cfRule type="duplicateValues" dxfId="125" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C11">
+    <cfRule type="duplicateValues" dxfId="124" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
+    <cfRule type="duplicateValues" dxfId="123" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
     <cfRule type="duplicateValues" dxfId="122" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C10">
-    <cfRule type="duplicateValues" dxfId="121" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="120" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="119" priority="15"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="118" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="117" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="116" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="115" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="114" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="113" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="112" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="111" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="duplicateValues" dxfId="110" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT28">
-    <cfRule type="duplicateValues" dxfId="109" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ28:BS28">
-    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D28">

</xml_diff>

<commit_message>
Fixing Dino dragon walk, some texts changes and setting special dragon max pets to 0, as it depends on something different
Former-commit-id: a9737dfc5fb690f6aa6259def5ce3d5b6f4348e7
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -1770,6 +1770,34 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1800,69 +1828,11 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="126">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="125">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -4359,6 +4329,26 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4373,105 +4363,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="110" dataDxfId="108" headerRowBorderDxfId="109" tableBorderDxfId="107" totalsRowBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104" totalsRowBorderDxfId="103">
   <autoFilter ref="B15:BT28"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="105"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="104"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="103"/>
-    <tableColumn id="65" name="[type]" dataDxfId="102"/>
-    <tableColumn id="3" name="[order]" dataDxfId="101"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="100"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="99"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="98"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="97"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="96"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="95"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="94"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="93"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="92"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="91"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="90"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="89"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="88"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="87"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="86"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="85"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="84"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="83"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="82"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="81">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="102"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="101"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="100"/>
+    <tableColumn id="65" name="[type]" dataDxfId="99"/>
+    <tableColumn id="3" name="[order]" dataDxfId="98"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="97"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="96"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="95"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="94"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="93"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="92"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="91"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="90"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="89"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="88"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="87"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="86"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="85"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="84"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="83"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="82"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="81"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="80"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="79"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="78">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="80"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="79"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="78"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="77"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="76"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="75"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="74"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="73"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="72"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="71">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="77"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="76"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="75"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="74"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="73"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="72"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="71"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="70"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="69"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="68">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="70"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="69"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="68"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="67"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="66"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="65"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="64"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="63"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="62"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="61"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="60"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="59"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="58"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="57"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="56"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="55"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="54"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="53">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="67"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="66"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="65"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="64"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="63"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="62"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="61"/>
+    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="60"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="59"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="58"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="57"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="56"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="55"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="54"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="53"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="52"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="51"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="50">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="52">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="49">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="51"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="50"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="49"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="48">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="48"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="47"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="46"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="45">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="47"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="46"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="45"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="44"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="43"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="42"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="41"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="40"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="39"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="38"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="37"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="36"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="35"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="44"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="43"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="42"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="41"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="40"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="39"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="38"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="37"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="36"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="35"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="34"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="33"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G11" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G11" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B4:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="30"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="29"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="28"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="27">
+    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4480,25 +4470,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:J35" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:J35" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B34:J35"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="22"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="21"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="20"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="19"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="18"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="17"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="16"/>
-    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="15"/>
+    <tableColumn id="8" name="[superfuryMax]" dataDxfId="17"/>
+    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="16"/>
+    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="15"/>
+    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="14"/>
+    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="13"/>
+    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B46:W59"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -4529,14 +4519,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B39:F42"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="6"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="4"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="3"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4811,7 +4801,7 @@
   <dimension ref="A1:BT59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5028,7 +5018,7 @@
       </c>
     </row>
     <row r="11" spans="2:72" x14ac:dyDescent="0.25">
-      <c r="B11" s="184" t="s">
+      <c r="B11" s="165" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="85" t="s">
@@ -5041,7 +5031,7 @@
         <v>240</v>
       </c>
       <c r="F11" s="15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G11" s="145" t="s">
         <v>241</v>
@@ -5097,10 +5087,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="169"/>
-      <c r="AP14" s="169"/>
-      <c r="AQ14" s="169"/>
-      <c r="AR14" s="169"/>
+      <c r="AO14" s="179"/>
+      <c r="AP14" s="179"/>
+      <c r="AQ14" s="179"/>
+      <c r="AR14" s="179"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -8064,83 +8054,83 @@
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32"/>
-      <c r="J29" s="183" t="s">
+      <c r="J29" s="174" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="183"/>
-      <c r="L29" s="183"/>
-      <c r="M29" s="183"/>
-      <c r="N29" s="181" t="s">
+      <c r="K29" s="174"/>
+      <c r="L29" s="174"/>
+      <c r="M29" s="174"/>
+      <c r="N29" s="172" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="182"/>
-      <c r="P29" s="182"/>
-      <c r="Q29" s="182"/>
-      <c r="R29" s="182"/>
-      <c r="S29" s="182"/>
-      <c r="T29" s="182"/>
-      <c r="U29" s="179" t="s">
+      <c r="O29" s="173"/>
+      <c r="P29" s="173"/>
+      <c r="Q29" s="173"/>
+      <c r="R29" s="173"/>
+      <c r="S29" s="173"/>
+      <c r="T29" s="173"/>
+      <c r="U29" s="170" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="180"/>
+      <c r="V29" s="171"/>
       <c r="W29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="176" t="s">
+      <c r="X29" s="167" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="177"/>
-      <c r="Z29" s="177"/>
-      <c r="AA29" s="177"/>
-      <c r="AB29" s="178"/>
-      <c r="AC29" s="175" t="s">
+      <c r="Y29" s="168"/>
+      <c r="Z29" s="168"/>
+      <c r="AA29" s="168"/>
+      <c r="AB29" s="169"/>
+      <c r="AC29" s="166" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="175"/>
-      <c r="AE29" s="175"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="175"/>
+      <c r="AD29" s="166"/>
+      <c r="AE29" s="166"/>
+      <c r="AF29" s="166"/>
+      <c r="AG29" s="166"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="171" t="s">
+      <c r="AI29" s="181" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="171"/>
-      <c r="AK29" s="165" t="s">
+      <c r="AJ29" s="181"/>
+      <c r="AK29" s="175" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="165"/>
-      <c r="AM29" s="172" t="s">
+      <c r="AL29" s="175"/>
+      <c r="AM29" s="182" t="s">
         <v>237</v>
       </c>
-      <c r="AN29" s="173"/>
-      <c r="AO29" s="173"/>
-      <c r="AP29" s="173"/>
-      <c r="AQ29" s="173"/>
-      <c r="AR29" s="174"/>
-      <c r="AS29" s="166" t="s">
+      <c r="AN29" s="183"/>
+      <c r="AO29" s="183"/>
+      <c r="AP29" s="183"/>
+      <c r="AQ29" s="183"/>
+      <c r="AR29" s="184"/>
+      <c r="AS29" s="176" t="s">
         <v>227</v>
       </c>
-      <c r="AT29" s="167"/>
-      <c r="AU29" s="167"/>
-      <c r="AV29" s="167"/>
-      <c r="AW29" s="167"/>
-      <c r="AX29" s="167"/>
-      <c r="AY29" s="168"/>
+      <c r="AT29" s="177"/>
+      <c r="AU29" s="177"/>
+      <c r="AV29" s="177"/>
+      <c r="AW29" s="177"/>
+      <c r="AX29" s="177"/>
+      <c r="AY29" s="178"/>
       <c r="AZ29" s="32"/>
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
-      <c r="BF29" s="170" t="s">
+      <c r="BF29" s="180" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="170"/>
-      <c r="BH29" s="170"/>
-      <c r="BI29" s="170"/>
-      <c r="BJ29" s="170"/>
-      <c r="BK29" s="170"/>
-      <c r="BL29" s="170"/>
+      <c r="BG29" s="180"/>
+      <c r="BH29" s="180"/>
+      <c r="BI29" s="180"/>
+      <c r="BJ29" s="180"/>
+      <c r="BK29" s="180"/>
+      <c r="BL29" s="180"/>
       <c r="BM29" s="32"/>
       <c r="BN29" s="32"/>
       <c r="BO29" s="32"/>
@@ -9553,68 +9543,68 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="125" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C11">
-    <cfRule type="duplicateValues" dxfId="124" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="123" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="122" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="121" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="120" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="119" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="118" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="117" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="116" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="115" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="114" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="duplicateValues" dxfId="113" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT28">
-    <cfRule type="duplicateValues" dxfId="112" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ28:BS28">
-    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D28">

</xml_diff>

<commit_message>
Content excels split into more excels
Former-commit-id: 41fd5cd75f2cd93cce7e7389bead853f81f0b337
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -704,9 +704,6 @@
     <t>PF_DragonTitanResults</t>
   </si>
   <si>
-    <t>ALCOHOL</t>
-  </si>
-  <si>
     <t>LETTERS</t>
   </si>
   <si>
@@ -765,6 +762,9 @@
   </si>
   <si>
     <t>TID_DRAGON_TIER_0_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2034,6 +2034,36 @@
     <xf numFmtId="49" fontId="0" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2059,36 +2089,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5056,7 +5056,7 @@
   <dimension ref="A1:BT59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="AT12" sqref="AT12"/>
+      <selection activeCell="AK29" sqref="AK29:AL29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5165,7 +5165,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="2:72" x14ac:dyDescent="0.25">
@@ -5185,7 +5185,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="2:72" x14ac:dyDescent="0.25">
@@ -5205,7 +5205,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="83" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="2:72" x14ac:dyDescent="0.25">
@@ -5225,7 +5225,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="81" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="2:72" x14ac:dyDescent="0.25">
@@ -5245,7 +5245,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="2:72" x14ac:dyDescent="0.25">
@@ -5253,19 +5253,19 @@
         <v>3</v>
       </c>
       <c r="C10" s="82" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D10" s="122">
         <v>5</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F10" s="15">
         <v>4</v>
       </c>
       <c r="G10" s="120" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="2:72" x14ac:dyDescent="0.25">
@@ -5273,19 +5273,19 @@
         <v>3</v>
       </c>
       <c r="C11" s="82" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D11" s="122">
         <v>6</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F11" s="15">
         <v>0</v>
       </c>
       <c r="G11" s="120" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="2:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5338,10 +5338,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="249"/>
-      <c r="AP14" s="249"/>
-      <c r="AQ14" s="249"/>
-      <c r="AR14" s="249"/>
+      <c r="AO14" s="240"/>
+      <c r="AP14" s="240"/>
+      <c r="AQ14" s="240"/>
+      <c r="AR14" s="240"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -8081,10 +8081,10 @@
         <v>3</v>
       </c>
       <c r="C28" s="140" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D28" s="140" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E28" s="138" t="s">
         <v>204</v>
@@ -8190,13 +8190,13 @@
         <v>12</v>
       </c>
       <c r="AM28" s="191" t="s">
+        <v>231</v>
+      </c>
+      <c r="AN28" s="192" t="s">
         <v>232</v>
       </c>
-      <c r="AN28" s="192" t="s">
+      <c r="AO28" s="192" t="s">
         <v>233</v>
-      </c>
-      <c r="AO28" s="192" t="s">
-        <v>234</v>
       </c>
       <c r="AP28" s="193"/>
       <c r="AQ28" s="193"/>
@@ -8231,10 +8231,10 @@
         <v>0.4</v>
       </c>
       <c r="BB28" s="209" t="s">
+        <v>234</v>
+      </c>
+      <c r="BC28" s="210" t="s">
         <v>235</v>
-      </c>
-      <c r="BC28" s="210" t="s">
-        <v>236</v>
       </c>
       <c r="BD28" s="211">
         <v>1.5E-3</v>
@@ -8283,7 +8283,7 @@
         <v>1</v>
       </c>
       <c r="BT28" s="235" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:72" ht="23.25" x14ac:dyDescent="0.35">
@@ -8296,83 +8296,83 @@
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
       <c r="I29" s="30"/>
-      <c r="J29" s="244" t="s">
+      <c r="J29" s="254" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="244"/>
-      <c r="L29" s="244"/>
-      <c r="M29" s="244"/>
-      <c r="N29" s="242" t="s">
+      <c r="K29" s="254"/>
+      <c r="L29" s="254"/>
+      <c r="M29" s="254"/>
+      <c r="N29" s="252" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="243"/>
-      <c r="P29" s="243"/>
-      <c r="Q29" s="243"/>
-      <c r="R29" s="243"/>
-      <c r="S29" s="243"/>
-      <c r="T29" s="243"/>
-      <c r="U29" s="240" t="s">
+      <c r="O29" s="253"/>
+      <c r="P29" s="253"/>
+      <c r="Q29" s="253"/>
+      <c r="R29" s="253"/>
+      <c r="S29" s="253"/>
+      <c r="T29" s="253"/>
+      <c r="U29" s="250" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="241"/>
+      <c r="V29" s="251"/>
       <c r="W29" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="237" t="s">
+      <c r="X29" s="247" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="238"/>
-      <c r="Z29" s="238"/>
-      <c r="AA29" s="238"/>
-      <c r="AB29" s="239"/>
-      <c r="AC29" s="236" t="s">
+      <c r="Y29" s="248"/>
+      <c r="Z29" s="248"/>
+      <c r="AA29" s="248"/>
+      <c r="AB29" s="249"/>
+      <c r="AC29" s="246" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="236"/>
-      <c r="AE29" s="236"/>
-      <c r="AF29" s="236"/>
-      <c r="AG29" s="236"/>
+      <c r="AD29" s="246"/>
+      <c r="AE29" s="246"/>
+      <c r="AF29" s="246"/>
+      <c r="AG29" s="246"/>
       <c r="AH29" s="30"/>
-      <c r="AI29" s="251" t="s">
+      <c r="AI29" s="242" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="251"/>
-      <c r="AK29" s="245" t="s">
+      <c r="AJ29" s="242"/>
+      <c r="AK29" s="236" t="s">
+        <v>246</v>
+      </c>
+      <c r="AL29" s="236"/>
+      <c r="AM29" s="243" t="s">
+        <v>236</v>
+      </c>
+      <c r="AN29" s="244"/>
+      <c r="AO29" s="244"/>
+      <c r="AP29" s="244"/>
+      <c r="AQ29" s="244"/>
+      <c r="AR29" s="245"/>
+      <c r="AS29" s="237" t="s">
         <v>226</v>
       </c>
-      <c r="AL29" s="245"/>
-      <c r="AM29" s="252" t="s">
-        <v>237</v>
-      </c>
-      <c r="AN29" s="253"/>
-      <c r="AO29" s="253"/>
-      <c r="AP29" s="253"/>
-      <c r="AQ29" s="253"/>
-      <c r="AR29" s="254"/>
-      <c r="AS29" s="246" t="s">
-        <v>227</v>
-      </c>
-      <c r="AT29" s="247"/>
-      <c r="AU29" s="247"/>
-      <c r="AV29" s="247"/>
-      <c r="AW29" s="247"/>
-      <c r="AX29" s="247"/>
-      <c r="AY29" s="248"/>
+      <c r="AT29" s="238"/>
+      <c r="AU29" s="238"/>
+      <c r="AV29" s="238"/>
+      <c r="AW29" s="238"/>
+      <c r="AX29" s="238"/>
+      <c r="AY29" s="239"/>
       <c r="AZ29" s="30"/>
       <c r="BA29" s="30"/>
       <c r="BB29" s="30"/>
       <c r="BC29" s="30"/>
       <c r="BD29" s="30"/>
       <c r="BE29" s="30"/>
-      <c r="BF29" s="250" t="s">
+      <c r="BF29" s="241" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="250"/>
-      <c r="BH29" s="250"/>
-      <c r="BI29" s="250"/>
-      <c r="BJ29" s="250"/>
-      <c r="BK29" s="250"/>
-      <c r="BL29" s="250"/>
+      <c r="BG29" s="241"/>
+      <c r="BH29" s="241"/>
+      <c r="BI29" s="241"/>
+      <c r="BJ29" s="241"/>
+      <c r="BK29" s="241"/>
+      <c r="BL29" s="241"/>
       <c r="BM29" s="30"/>
       <c r="BN29" s="30"/>
       <c r="BO29" s="30"/>
@@ -8558,7 +8558,7 @@
         <v>58</v>
       </c>
       <c r="J34" s="135" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:71" x14ac:dyDescent="0.25">
@@ -9720,7 +9720,7 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D59">
         <v>20</v>
@@ -9785,17 +9785,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="124" priority="19"/>

</xml_diff>

<commit_message>
Adding Alien dragon balancing and progression to tables
Former-commit-id: 5000bf1837d846146895ecb4ab4be20cf2e9c67c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="253">
   <si>
     <t>[sku]</t>
   </si>
@@ -765,6 +765,24 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>dragon_alien</t>
+  </si>
+  <si>
+    <t>PF_DragonAlien</t>
+  </si>
+  <si>
+    <t>PF_DragonAlienMenu</t>
+  </si>
+  <si>
+    <t>PF_DragonAlienResults</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_ALIEN_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_ALIEN_DESC</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1022,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1367,11 +1385,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2034,6 +2080,33 @@
     <xf numFmtId="49" fontId="0" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2064,38 +2137,268 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="125">
+  <dxfs count="128">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -4434,176 +4737,6 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4618,105 +4751,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT28" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104" totalsRowBorderDxfId="103">
-  <autoFilter ref="B15:BT28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT29" totalsRowShown="0" headerRowDxfId="127" dataDxfId="125" headerRowBorderDxfId="126" tableBorderDxfId="124" totalsRowBorderDxfId="123">
+  <autoFilter ref="B15:BT29"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="102"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="101"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="100"/>
-    <tableColumn id="65" name="[type]" dataDxfId="99"/>
-    <tableColumn id="3" name="[order]" dataDxfId="98"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="97"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="96"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="95"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="94"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="93"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="92"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="91"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="90"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="89"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="88"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="87"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="86"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="85"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="84"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="83"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="82"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="81"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="80"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="79"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="78">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="122"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="121"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="120"/>
+    <tableColumn id="65" name="[type]" dataDxfId="119"/>
+    <tableColumn id="3" name="[order]" dataDxfId="118"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="117"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="116"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="115"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="114"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="113"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="112"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="111"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="110"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="109"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="108"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="107"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="106"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="105"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="104"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="103"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="102"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="101"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="100"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="99"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="98">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="77"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="76"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="75"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="74"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="73"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="72"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="71"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="70"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="69"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="68">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="97"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="96"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="95"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="94"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="93"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="92"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="91"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="90"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="89"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="88">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="67"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="66"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="65"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="64"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="63"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="62"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="61"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="60"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="59"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="58"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="57"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="56"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="55"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="54"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="53"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="52"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="51"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="50">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="87"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="86"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="85"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="84"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="83"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="82"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="81"/>
+    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="80"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="79"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="78"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="77"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="76"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="75"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="74"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="73"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="72"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="71"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="70">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="49">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="69">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="48"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="47"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="46"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="45">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="68"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="67"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="66"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="65">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="44"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="43"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="42"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="41"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="40"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="39"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="38"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="37"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="36"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="35"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="34"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="33"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="64"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="63"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="62"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="61"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="60"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="59"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="58"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="57"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="56"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="55"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="54"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="53"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G11" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G11" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
   <autoFilter ref="B4:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="47"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="24">
+    <tableColumn id="10" name="[icon]" dataDxfId="46"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="45"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="44">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4725,26 +4858,26 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B34:J35" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="B34:J35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B35:J36" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+  <autoFilter ref="B35:J36"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="39"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="38"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="17"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="16"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="15"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="14"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="13"/>
-    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="12"/>
+    <tableColumn id="8" name="[superfuryMax]" dataDxfId="37"/>
+    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="36"/>
+    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="35"/>
+    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="34"/>
+    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="33"/>
+    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B46:W59" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B46:W59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B47:W61" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="B47:W61"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
     <tableColumn id="2" name="[sku]"/>
@@ -4774,14 +4907,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B39:F42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B39:F42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B40:F43" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="B40:F43"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="23"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="22"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5050,13 +5183,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:BT59"/>
+  <dimension ref="A1:BT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="AK29" sqref="AK29:AL29"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="M69" sqref="M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5338,10 +5471,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="240"/>
-      <c r="AP14" s="240"/>
-      <c r="AQ14" s="240"/>
-      <c r="AR14" s="240"/>
+      <c r="AO14" s="249"/>
+      <c r="AP14" s="249"/>
+      <c r="AQ14" s="249"/>
+      <c r="AR14" s="249"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -8286,495 +8419,688 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:72" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A29" s="30"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="254" t="s">
+    <row r="29" spans="1:72" x14ac:dyDescent="0.25">
+      <c r="B29" s="139" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="140" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29" s="140" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="138" t="s">
+        <v>204</v>
+      </c>
+      <c r="F29" s="143">
+        <v>13</v>
+      </c>
+      <c r="G29" s="144" t="s">
+        <v>230</v>
+      </c>
+      <c r="H29" s="149">
+        <v>1000000</v>
+      </c>
+      <c r="I29" s="150">
+        <v>650</v>
+      </c>
+      <c r="J29" s="255">
+        <v>35</v>
+      </c>
+      <c r="K29" s="55">
+        <v>45</v>
+      </c>
+      <c r="L29" s="99">
+        <v>25</v>
+      </c>
+      <c r="M29" s="44">
+        <v>0</v>
+      </c>
+      <c r="N29" s="40">
+        <v>500</v>
+      </c>
+      <c r="O29" s="256">
+        <v>600</v>
+      </c>
+      <c r="P29" s="99">
+        <v>2.5</v>
+      </c>
+      <c r="Q29" s="23">
+        <v>0</v>
+      </c>
+      <c r="R29" s="270">
+        <v>0.02</v>
+      </c>
+      <c r="S29" s="268">
+        <v>20</v>
+      </c>
+      <c r="T29" s="41">
+        <v>0.8</v>
+      </c>
+      <c r="U29" s="40">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V29" s="51">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W29" s="42">
+        <v>31</v>
+      </c>
+      <c r="X29" s="40">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="Y29" s="23">
+        <v>100</v>
+      </c>
+      <c r="Z29" s="256">
+        <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
+        <v>125</v>
+      </c>
+      <c r="AA29" s="23">
+        <v>20</v>
+      </c>
+      <c r="AB29" s="23">
+        <v>14</v>
+      </c>
+      <c r="AC29" s="42">
+        <v>475</v>
+      </c>
+      <c r="AD29" s="41">
+        <v>12</v>
+      </c>
+      <c r="AE29" s="23">
+        <v>7</v>
+      </c>
+      <c r="AF29" s="41">
+        <v>10</v>
+      </c>
+      <c r="AG29" s="23">
+        <v>65000</v>
+      </c>
+      <c r="AH29" s="88">
+        <v>6</v>
+      </c>
+      <c r="AI29" s="40">
+        <v>0.04</v>
+      </c>
+      <c r="AJ29" s="258">
+        <v>0.03</v>
+      </c>
+      <c r="AK29" s="42">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="259">
+        <v>12</v>
+      </c>
+      <c r="AM29" s="260" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN29" s="261" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO29" s="261" t="s">
+        <v>250</v>
+      </c>
+      <c r="AP29" s="262"/>
+      <c r="AQ29" s="262"/>
+      <c r="AR29" s="263" t="s">
+        <v>230</v>
+      </c>
+      <c r="AS29" s="264">
+        <v>1.05</v>
+      </c>
+      <c r="AT29" s="257">
+        <v>2</v>
+      </c>
+      <c r="AU29" s="257">
+        <v>2</v>
+      </c>
+      <c r="AV29" s="257" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW29" s="257" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX29" s="257" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY29" s="265">
+        <v>25</v>
+      </c>
+      <c r="AZ29" s="257">
+        <v>0.75</v>
+      </c>
+      <c r="BA29" s="257">
+        <v>0.4</v>
+      </c>
+      <c r="BB29" s="105" t="s">
+        <v>251</v>
+      </c>
+      <c r="BC29" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="BD29" s="266">
+        <v>1.5E-3</v>
+      </c>
+      <c r="BE29" s="47">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="BF29" s="106">
+        <v>700</v>
+      </c>
+      <c r="BG29" s="267">
+        <v>750</v>
+      </c>
+      <c r="BH29" s="34">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="BI29" s="34">
+        <v>9.5</v>
+      </c>
+      <c r="BJ29" s="34">
+        <v>1.7</v>
+      </c>
+      <c r="BK29" s="34">
+        <v>0.7</v>
+      </c>
+      <c r="BL29" s="34">
+        <v>1.03</v>
+      </c>
+      <c r="BM29" s="106">
+        <v>59</v>
+      </c>
+      <c r="BN29" s="34">
+        <v>15</v>
+      </c>
+      <c r="BO29" s="34">
+        <v>0.4</v>
+      </c>
+      <c r="BP29" s="110">
+        <v>25</v>
+      </c>
+      <c r="BQ29" s="271"/>
+      <c r="BR29" s="272">
+        <v>0.2</v>
+      </c>
+      <c r="BS29" s="273">
+        <v>1</v>
+      </c>
+      <c r="BT29" s="113" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:72" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="244" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="254"/>
-      <c r="L29" s="254"/>
-      <c r="M29" s="254"/>
-      <c r="N29" s="252" t="s">
+      <c r="K30" s="244"/>
+      <c r="L30" s="244"/>
+      <c r="M30" s="244"/>
+      <c r="N30" s="242" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="253"/>
-      <c r="P29" s="253"/>
-      <c r="Q29" s="253"/>
-      <c r="R29" s="253"/>
-      <c r="S29" s="253"/>
-      <c r="T29" s="253"/>
-      <c r="U29" s="250" t="s">
+      <c r="O30" s="243"/>
+      <c r="P30" s="243"/>
+      <c r="Q30" s="243"/>
+      <c r="R30" s="269"/>
+      <c r="S30" s="243"/>
+      <c r="T30" s="243"/>
+      <c r="U30" s="240" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="251"/>
-      <c r="W29" s="32" t="s">
+      <c r="V30" s="241"/>
+      <c r="W30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="247" t="s">
+      <c r="X30" s="237" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="248"/>
-      <c r="Z29" s="248"/>
-      <c r="AA29" s="248"/>
-      <c r="AB29" s="249"/>
-      <c r="AC29" s="246" t="s">
+      <c r="Y30" s="238"/>
+      <c r="Z30" s="238"/>
+      <c r="AA30" s="238"/>
+      <c r="AB30" s="239"/>
+      <c r="AC30" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="246"/>
-      <c r="AE29" s="246"/>
-      <c r="AF29" s="246"/>
-      <c r="AG29" s="246"/>
-      <c r="AH29" s="30"/>
-      <c r="AI29" s="242" t="s">
+      <c r="AD30" s="236"/>
+      <c r="AE30" s="236"/>
+      <c r="AF30" s="236"/>
+      <c r="AG30" s="236"/>
+      <c r="AH30" s="30"/>
+      <c r="AI30" s="251" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="242"/>
-      <c r="AK29" s="236" t="s">
+      <c r="AJ30" s="251"/>
+      <c r="AK30" s="245" t="s">
         <v>246</v>
       </c>
-      <c r="AL29" s="236"/>
-      <c r="AM29" s="243" t="s">
+      <c r="AL30" s="245"/>
+      <c r="AM30" s="252" t="s">
         <v>236</v>
       </c>
-      <c r="AN29" s="244"/>
-      <c r="AO29" s="244"/>
-      <c r="AP29" s="244"/>
-      <c r="AQ29" s="244"/>
-      <c r="AR29" s="245"/>
-      <c r="AS29" s="237" t="s">
+      <c r="AN30" s="253"/>
+      <c r="AO30" s="253"/>
+      <c r="AP30" s="253"/>
+      <c r="AQ30" s="253"/>
+      <c r="AR30" s="254"/>
+      <c r="AS30" s="246" t="s">
         <v>226</v>
       </c>
-      <c r="AT29" s="238"/>
-      <c r="AU29" s="238"/>
-      <c r="AV29" s="238"/>
-      <c r="AW29" s="238"/>
-      <c r="AX29" s="238"/>
-      <c r="AY29" s="239"/>
-      <c r="AZ29" s="30"/>
-      <c r="BA29" s="30"/>
-      <c r="BB29" s="30"/>
-      <c r="BC29" s="30"/>
-      <c r="BD29" s="30"/>
-      <c r="BE29" s="30"/>
-      <c r="BF29" s="241" t="s">
+      <c r="AT30" s="247"/>
+      <c r="AU30" s="247"/>
+      <c r="AV30" s="247"/>
+      <c r="AW30" s="247"/>
+      <c r="AX30" s="247"/>
+      <c r="AY30" s="248"/>
+      <c r="AZ30" s="30"/>
+      <c r="BA30" s="30"/>
+      <c r="BB30" s="30"/>
+      <c r="BC30" s="30"/>
+      <c r="BD30" s="30"/>
+      <c r="BE30" s="30"/>
+      <c r="BF30" s="250" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="241"/>
-      <c r="BH29" s="241"/>
-      <c r="BI29" s="241"/>
-      <c r="BJ29" s="241"/>
-      <c r="BK29" s="241"/>
-      <c r="BL29" s="241"/>
-      <c r="BM29" s="30"/>
-      <c r="BN29" s="30"/>
-      <c r="BO29" s="30"/>
-      <c r="BP29" s="30"/>
-      <c r="BQ29" s="30"/>
-      <c r="BR29" s="30"/>
-      <c r="BS29" s="30"/>
+      <c r="BG30" s="250"/>
+      <c r="BH30" s="250"/>
+      <c r="BI30" s="250"/>
+      <c r="BJ30" s="250"/>
+      <c r="BK30" s="250"/>
+      <c r="BL30" s="250"/>
+      <c r="BM30" s="30"/>
+      <c r="BN30" s="30"/>
+      <c r="BO30" s="30"/>
+      <c r="BP30" s="30"/>
+      <c r="BQ30" s="30"/>
+      <c r="BR30" s="30"/>
+      <c r="BS30" s="30"/>
     </row>
-    <row r="31" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:72" s="19" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A32"/>
-      <c r="B32" s="1" t="s">
+    <row r="32" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:71" s="19" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A33"/>
+      <c r="B33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32"/>
-      <c r="AD32"/>
-      <c r="AE32"/>
-      <c r="AF32"/>
-      <c r="AG32"/>
-      <c r="AH32"/>
-      <c r="AI32"/>
-      <c r="AJ32"/>
-      <c r="AK32"/>
-      <c r="AL32"/>
-      <c r="AM32"/>
-      <c r="AN32"/>
-      <c r="AO32"/>
-      <c r="AP32"/>
-      <c r="AQ32"/>
-      <c r="AR32"/>
-      <c r="AS32"/>
-      <c r="AT32"/>
-      <c r="AU32"/>
-      <c r="AV32"/>
-      <c r="AW32"/>
-      <c r="AX32"/>
-      <c r="AY32"/>
-      <c r="AZ32"/>
-      <c r="BA32"/>
-      <c r="BB32"/>
-      <c r="BC32"/>
-      <c r="BD32"/>
-      <c r="BE32"/>
-      <c r="BF32"/>
-      <c r="BG32"/>
-      <c r="BH32"/>
-      <c r="BI32"/>
-      <c r="BJ32"/>
-      <c r="BK32"/>
-      <c r="BL32"/>
-      <c r="BM32"/>
-      <c r="BN32"/>
-      <c r="BO32"/>
-      <c r="BP32"/>
-      <c r="BQ32"/>
-      <c r="BR32"/>
-      <c r="BS32"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+      <c r="Z33"/>
+      <c r="AA33"/>
+      <c r="AB33"/>
+      <c r="AC33"/>
+      <c r="AD33"/>
+      <c r="AE33"/>
+      <c r="AF33"/>
+      <c r="AG33"/>
+      <c r="AH33"/>
+      <c r="AI33"/>
+      <c r="AJ33"/>
+      <c r="AK33"/>
+      <c r="AL33"/>
+      <c r="AM33"/>
+      <c r="AN33"/>
+      <c r="AO33"/>
+      <c r="AP33"/>
+      <c r="AQ33"/>
+      <c r="AR33"/>
+      <c r="AS33"/>
+      <c r="AT33"/>
+      <c r="AU33"/>
+      <c r="AV33"/>
+      <c r="AW33"/>
+      <c r="AX33"/>
+      <c r="AY33"/>
+      <c r="AZ33"/>
+      <c r="BA33"/>
+      <c r="BB33"/>
+      <c r="BC33"/>
+      <c r="BD33"/>
+      <c r="BE33"/>
+      <c r="BF33"/>
+      <c r="BG33"/>
+      <c r="BH33"/>
+      <c r="BI33"/>
+      <c r="BJ33"/>
+      <c r="BK33"/>
+      <c r="BL33"/>
+      <c r="BM33"/>
+      <c r="BN33"/>
+      <c r="BO33"/>
+      <c r="BP33"/>
+      <c r="BQ33"/>
+      <c r="BR33"/>
+      <c r="BS33"/>
     </row>
-    <row r="33" spans="1:71" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
+    <row r="34" spans="1:71" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="19"/>
-      <c r="X33" s="19"/>
-      <c r="Y33" s="19"/>
-      <c r="Z33" s="19"/>
-      <c r="AA33" s="19"/>
-      <c r="AB33" s="19"/>
-      <c r="AC33" s="19"/>
-      <c r="AD33" s="19"/>
-      <c r="AE33" s="19"/>
-      <c r="AF33" s="19"/>
-      <c r="AG33" s="19"/>
-      <c r="AH33" s="19"/>
-      <c r="AI33" s="19"/>
-      <c r="AJ33" s="19"/>
-      <c r="AK33" s="19"/>
-      <c r="AL33" s="19"/>
-      <c r="AM33" s="19"/>
-      <c r="AN33" s="19"/>
-      <c r="AO33" s="19"/>
-      <c r="AP33" s="19"/>
-      <c r="AQ33" s="19"/>
-      <c r="AR33" s="19"/>
-      <c r="AS33" s="19"/>
-      <c r="AT33" s="19"/>
-      <c r="AU33" s="19"/>
-      <c r="AV33" s="19"/>
-      <c r="AW33" s="19"/>
-      <c r="AX33" s="19"/>
-      <c r="AY33" s="19"/>
-      <c r="AZ33" s="19"/>
-      <c r="BA33" s="19"/>
-      <c r="BB33" s="19"/>
-      <c r="BC33" s="19"/>
-      <c r="BD33" s="19"/>
-      <c r="BE33" s="19"/>
-      <c r="BF33" s="19"/>
-      <c r="BG33" s="19"/>
-      <c r="BH33" s="19"/>
-      <c r="BI33" s="19"/>
-      <c r="BJ33" s="19"/>
-      <c r="BK33" s="19"/>
-      <c r="BL33" s="19"/>
-      <c r="BM33" s="19"/>
-      <c r="BN33" s="19"/>
-      <c r="BO33" s="19"/>
-      <c r="BP33" s="19"/>
-      <c r="BQ33" s="19"/>
-      <c r="BR33" s="19"/>
-      <c r="BS33" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="19"/>
+      <c r="Z34" s="19"/>
+      <c r="AA34" s="19"/>
+      <c r="AB34" s="19"/>
+      <c r="AC34" s="19"/>
+      <c r="AD34" s="19"/>
+      <c r="AE34" s="19"/>
+      <c r="AF34" s="19"/>
+      <c r="AG34" s="19"/>
+      <c r="AH34" s="19"/>
+      <c r="AI34" s="19"/>
+      <c r="AJ34" s="19"/>
+      <c r="AK34" s="19"/>
+      <c r="AL34" s="19"/>
+      <c r="AM34" s="19"/>
+      <c r="AN34" s="19"/>
+      <c r="AO34" s="19"/>
+      <c r="AP34" s="19"/>
+      <c r="AQ34" s="19"/>
+      <c r="AR34" s="19"/>
+      <c r="AS34" s="19"/>
+      <c r="AT34" s="19"/>
+      <c r="AU34" s="19"/>
+      <c r="AV34" s="19"/>
+      <c r="AW34" s="19"/>
+      <c r="AX34" s="19"/>
+      <c r="AY34" s="19"/>
+      <c r="AZ34" s="19"/>
+      <c r="BA34" s="19"/>
+      <c r="BB34" s="19"/>
+      <c r="BC34" s="19"/>
+      <c r="BD34" s="19"/>
+      <c r="BE34" s="19"/>
+      <c r="BF34" s="19"/>
+      <c r="BG34" s="19"/>
+      <c r="BH34" s="19"/>
+      <c r="BI34" s="19"/>
+      <c r="BJ34" s="19"/>
+      <c r="BK34" s="19"/>
+      <c r="BL34" s="19"/>
+      <c r="BM34" s="19"/>
+      <c r="BN34" s="19"/>
+      <c r="BO34" s="19"/>
+      <c r="BP34" s="19"/>
+      <c r="BQ34" s="19"/>
+      <c r="BR34" s="19"/>
+      <c r="BS34" s="19"/>
     </row>
-    <row r="34" spans="1:71" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="9" t="s">
+    <row r="35" spans="1:71" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D35" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I35" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J34" s="135" t="s">
+      <c r="J35" s="135" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
+    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C36" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D36" s="29">
         <v>0.2</v>
       </c>
-      <c r="E35" s="114">
+      <c r="E36" s="114">
         <v>8</v>
       </c>
-      <c r="F35" s="114">
+      <c r="F36" s="114">
         <v>1.5</v>
       </c>
-      <c r="G35" s="114">
+      <c r="G36" s="114">
         <v>1.2</v>
       </c>
-      <c r="H35" s="114">
+      <c r="H36" s="114">
         <v>1.2</v>
       </c>
-      <c r="I35" s="114">
+      <c r="I36" s="114">
         <v>10</v>
       </c>
-      <c r="J35" s="114">
+      <c r="J36" s="114">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:71" s="19" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A37"/>
-      <c r="B37" s="1" t="s">
+    <row r="37" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:71" s="19" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A38"/>
+      <c r="B38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37"/>
-      <c r="AC37"/>
-      <c r="AD37"/>
-      <c r="AE37"/>
-      <c r="AF37"/>
-      <c r="AG37"/>
-      <c r="AH37"/>
-      <c r="AI37"/>
-      <c r="AJ37"/>
-      <c r="AK37"/>
-      <c r="AL37"/>
-      <c r="AM37"/>
-      <c r="AN37"/>
-      <c r="AO37"/>
-      <c r="AP37"/>
-      <c r="AQ37"/>
-      <c r="AR37"/>
-      <c r="AS37"/>
-      <c r="AT37"/>
-      <c r="AU37"/>
-      <c r="AV37"/>
-      <c r="AW37"/>
-      <c r="AX37"/>
-      <c r="AY37"/>
-      <c r="AZ37"/>
-      <c r="BA37"/>
-      <c r="BB37"/>
-      <c r="BC37"/>
-      <c r="BD37"/>
-      <c r="BE37"/>
-      <c r="BF37"/>
-      <c r="BG37"/>
-      <c r="BH37"/>
-      <c r="BI37"/>
-      <c r="BJ37"/>
-      <c r="BK37"/>
-      <c r="BL37"/>
-      <c r="BM37"/>
-      <c r="BN37"/>
-      <c r="BO37"/>
-      <c r="BP37"/>
-      <c r="BQ37"/>
-      <c r="BR37"/>
-      <c r="BS37"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+      <c r="Z38"/>
+      <c r="AA38"/>
+      <c r="AB38"/>
+      <c r="AC38"/>
+      <c r="AD38"/>
+      <c r="AE38"/>
+      <c r="AF38"/>
+      <c r="AG38"/>
+      <c r="AH38"/>
+      <c r="AI38"/>
+      <c r="AJ38"/>
+      <c r="AK38"/>
+      <c r="AL38"/>
+      <c r="AM38"/>
+      <c r="AN38"/>
+      <c r="AO38"/>
+      <c r="AP38"/>
+      <c r="AQ38"/>
+      <c r="AR38"/>
+      <c r="AS38"/>
+      <c r="AT38"/>
+      <c r="AU38"/>
+      <c r="AV38"/>
+      <c r="AW38"/>
+      <c r="AX38"/>
+      <c r="AY38"/>
+      <c r="AZ38"/>
+      <c r="BA38"/>
+      <c r="BB38"/>
+      <c r="BC38"/>
+      <c r="BD38"/>
+      <c r="BE38"/>
+      <c r="BF38"/>
+      <c r="BG38"/>
+      <c r="BH38"/>
+      <c r="BI38"/>
+      <c r="BJ38"/>
+      <c r="BK38"/>
+      <c r="BL38"/>
+      <c r="BM38"/>
+      <c r="BN38"/>
+      <c r="BO38"/>
+      <c r="BP38"/>
+      <c r="BQ38"/>
+      <c r="BR38"/>
+      <c r="BS38"/>
     </row>
-    <row r="38" spans="1:71" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2" t="s">
+    <row r="39" spans="1:71" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
-      <c r="Z38" s="19"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
-      <c r="AD38" s="19"/>
-      <c r="AE38" s="19"/>
-      <c r="AF38" s="19"/>
-      <c r="AG38" s="19"/>
-      <c r="AH38" s="19"/>
-      <c r="AI38" s="19"/>
-      <c r="AJ38" s="19"/>
-      <c r="AK38" s="19"/>
-      <c r="AL38" s="19"/>
-      <c r="AM38" s="19"/>
-      <c r="AN38" s="19"/>
-      <c r="AO38" s="19"/>
-      <c r="AP38" s="19"/>
-      <c r="AQ38" s="19"/>
-      <c r="AR38" s="19"/>
-      <c r="AS38" s="19"/>
-      <c r="AT38" s="19"/>
-      <c r="AU38" s="19"/>
-      <c r="AV38" s="19"/>
-      <c r="AW38" s="19"/>
-      <c r="AX38" s="19"/>
-      <c r="AY38" s="19"/>
-      <c r="AZ38" s="19"/>
-      <c r="BA38" s="19"/>
-      <c r="BB38" s="19"/>
-      <c r="BC38" s="19"/>
-      <c r="BD38" s="19"/>
-      <c r="BE38" s="19"/>
-      <c r="BF38" s="19"/>
-      <c r="BG38" s="19"/>
-      <c r="BH38" s="19"/>
-      <c r="BI38" s="19"/>
-      <c r="BJ38" s="19"/>
-      <c r="BK38" s="19"/>
-      <c r="BL38" s="19"/>
-      <c r="BM38" s="19"/>
-      <c r="BN38" s="19"/>
-      <c r="BO38" s="19"/>
-      <c r="BP38" s="19"/>
-      <c r="BQ38" s="19"/>
-      <c r="BR38" s="19"/>
-      <c r="BS38" s="19"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+      <c r="Y39" s="19"/>
+      <c r="Z39" s="19"/>
+      <c r="AA39" s="19"/>
+      <c r="AB39" s="19"/>
+      <c r="AC39" s="19"/>
+      <c r="AD39" s="19"/>
+      <c r="AE39" s="19"/>
+      <c r="AF39" s="19"/>
+      <c r="AG39" s="19"/>
+      <c r="AH39" s="19"/>
+      <c r="AI39" s="19"/>
+      <c r="AJ39" s="19"/>
+      <c r="AK39" s="19"/>
+      <c r="AL39" s="19"/>
+      <c r="AM39" s="19"/>
+      <c r="AN39" s="19"/>
+      <c r="AO39" s="19"/>
+      <c r="AP39" s="19"/>
+      <c r="AQ39" s="19"/>
+      <c r="AR39" s="19"/>
+      <c r="AS39" s="19"/>
+      <c r="AT39" s="19"/>
+      <c r="AU39" s="19"/>
+      <c r="AV39" s="19"/>
+      <c r="AW39" s="19"/>
+      <c r="AX39" s="19"/>
+      <c r="AY39" s="19"/>
+      <c r="AZ39" s="19"/>
+      <c r="BA39" s="19"/>
+      <c r="BB39" s="19"/>
+      <c r="BC39" s="19"/>
+      <c r="BD39" s="19"/>
+      <c r="BE39" s="19"/>
+      <c r="BF39" s="19"/>
+      <c r="BG39" s="19"/>
+      <c r="BH39" s="19"/>
+      <c r="BI39" s="19"/>
+      <c r="BJ39" s="19"/>
+      <c r="BK39" s="19"/>
+      <c r="BL39" s="19"/>
+      <c r="BM39" s="19"/>
+      <c r="BN39" s="19"/>
+      <c r="BO39" s="19"/>
+      <c r="BP39" s="19"/>
+      <c r="BQ39" s="19"/>
+      <c r="BR39" s="19"/>
+      <c r="BS39" s="19"/>
     </row>
-    <row r="39" spans="1:71" ht="169.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
+    <row r="40" spans="1:71" ht="169.5" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D40" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E40" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="29">
-        <v>0.25</v>
-      </c>
-      <c r="E40" s="29">
-        <v>1</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:71" x14ac:dyDescent="0.25">
@@ -8782,16 +9108,16 @@
         <v>3</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D41" s="29">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="E41" s="29">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:71" x14ac:dyDescent="0.25">
@@ -8799,172 +9125,121 @@
         <v>3</v>
       </c>
       <c r="C42" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="E42" s="29">
+        <v>0.7</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D43" s="29">
         <v>0.05</v>
       </c>
-      <c r="E42" s="29">
+      <c r="E43" s="29">
         <v>0.4</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F43" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:71" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B44" s="1" t="s">
+    <row r="44" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:71" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
     </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="E45" t="s">
+    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:71" ht="150" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
+    <row r="47" spans="1:71" ht="150" x14ac:dyDescent="0.25">
+      <c r="B47" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="J47" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="K47" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L46" s="4" t="s">
+      <c r="L47" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M46" s="4" t="s">
+      <c r="M47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N46" s="4" t="s">
+      <c r="N47" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="O46" s="4" t="s">
+      <c r="O47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P46" s="4" t="s">
+      <c r="P47" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q46" s="4" t="s">
+      <c r="Q47" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R46" s="4" t="s">
+      <c r="R47" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S46" s="4" t="s">
+      <c r="S47" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T46" s="4" t="s">
+      <c r="T47" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U46" s="4" t="s">
+      <c r="U47" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="V46" s="4" t="s">
+      <c r="V47" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="W46" s="4" t="s">
+      <c r="W47" s="4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47">
-        <v>8</v>
-      </c>
-      <c r="E47">
-        <v>571</v>
-      </c>
-      <c r="F47">
-        <v>1714</v>
-      </c>
-      <c r="G47">
-        <v>3429</v>
-      </c>
-      <c r="H47">
-        <v>5714</v>
-      </c>
-      <c r="I47">
-        <v>8069</v>
-      </c>
-      <c r="J47">
-        <v>10895</v>
-      </c>
-      <c r="K47">
-        <v>14192</v>
-      </c>
-      <c r="L47" t="s">
-        <v>20</v>
-      </c>
-      <c r="M47" t="s">
-        <v>20</v>
-      </c>
-      <c r="N47" t="s">
-        <v>20</v>
-      </c>
-      <c r="O47" t="s">
-        <v>20</v>
-      </c>
-      <c r="P47" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>20</v>
-      </c>
-      <c r="R47" t="s">
-        <v>20</v>
-      </c>
-      <c r="S47" t="s">
-        <v>20</v>
-      </c>
-      <c r="T47" t="s">
-        <v>20</v>
-      </c>
-      <c r="U47" t="s">
-        <v>20</v>
-      </c>
-      <c r="V47" t="s">
-        <v>20</v>
-      </c>
-      <c r="W47" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:71" x14ac:dyDescent="0.25">
@@ -8972,37 +9247,37 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E48">
-        <v>1021</v>
+        <v>571</v>
       </c>
       <c r="F48">
-        <v>3063</v>
+        <v>1714</v>
       </c>
       <c r="G48">
-        <v>6127</v>
+        <v>3429</v>
       </c>
       <c r="H48">
-        <v>10211</v>
+        <v>5714</v>
       </c>
       <c r="I48">
-        <v>15317</v>
+        <v>8069</v>
       </c>
       <c r="J48">
-        <v>21443</v>
+        <v>10895</v>
       </c>
       <c r="K48">
-        <v>28591</v>
-      </c>
-      <c r="L48">
-        <v>36760</v>
-      </c>
-      <c r="M48">
-        <v>45950</v>
+        <v>14192</v>
+      </c>
+      <c r="L48" t="s">
+        <v>20</v>
+      </c>
+      <c r="M48" t="s">
+        <v>20</v>
       </c>
       <c r="N48" t="s">
         <v>20</v>
@@ -9040,37 +9315,37 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D49">
         <v>10</v>
       </c>
       <c r="E49">
-        <v>1661</v>
+        <v>1021</v>
       </c>
       <c r="F49">
-        <v>4983</v>
+        <v>3063</v>
       </c>
       <c r="G49">
-        <v>9966</v>
+        <v>6127</v>
       </c>
       <c r="H49">
-        <v>16610</v>
+        <v>10211</v>
       </c>
       <c r="I49">
-        <v>24915</v>
+        <v>15317</v>
       </c>
       <c r="J49">
-        <v>34881</v>
+        <v>21443</v>
       </c>
       <c r="K49">
-        <v>46508</v>
+        <v>28591</v>
       </c>
       <c r="L49">
-        <v>59796</v>
+        <v>36760</v>
       </c>
       <c r="M49">
-        <v>74745</v>
+        <v>45950</v>
       </c>
       <c r="N49" t="s">
         <v>20</v>
@@ -9108,37 +9383,37 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D50">
         <v>10</v>
       </c>
       <c r="E50">
-        <v>2346</v>
+        <v>1661</v>
       </c>
       <c r="F50">
-        <v>7037</v>
+        <v>4983</v>
       </c>
       <c r="G50">
-        <v>14075</v>
+        <v>9966</v>
       </c>
       <c r="H50">
-        <v>23458</v>
+        <v>16610</v>
       </c>
       <c r="I50">
-        <v>35187</v>
+        <v>24915</v>
       </c>
       <c r="J50">
-        <v>49261</v>
+        <v>34881</v>
       </c>
       <c r="K50">
-        <v>65682</v>
+        <v>46508</v>
       </c>
       <c r="L50">
-        <v>84448</v>
+        <v>59796</v>
       </c>
       <c r="M50">
-        <v>105560</v>
+        <v>74745</v>
       </c>
       <c r="N50" t="s">
         <v>20</v>
@@ -9176,52 +9451,52 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D51">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E51">
-        <v>1971</v>
+        <v>2346</v>
       </c>
       <c r="F51">
-        <v>5913</v>
+        <v>7037</v>
       </c>
       <c r="G51">
-        <v>11826</v>
+        <v>14075</v>
       </c>
       <c r="H51">
-        <v>19711</v>
+        <v>23458</v>
       </c>
       <c r="I51">
-        <v>29566</v>
+        <v>35187</v>
       </c>
       <c r="J51">
-        <v>41393</v>
+        <v>49261</v>
       </c>
       <c r="K51">
-        <v>55190</v>
+        <v>65682</v>
       </c>
       <c r="L51">
-        <v>70959</v>
+        <v>84448</v>
       </c>
       <c r="M51">
-        <v>88698</v>
-      </c>
-      <c r="N51">
-        <v>108409</v>
-      </c>
-      <c r="O51">
-        <v>130091</v>
-      </c>
-      <c r="P51">
-        <v>153744</v>
-      </c>
-      <c r="Q51">
-        <v>179368</v>
-      </c>
-      <c r="R51">
-        <v>206963</v>
+        <v>105560</v>
+      </c>
+      <c r="N51" t="s">
+        <v>20</v>
+      </c>
+      <c r="O51" t="s">
+        <v>20</v>
+      </c>
+      <c r="P51" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>20</v>
+      </c>
+      <c r="R51" t="s">
+        <v>20</v>
       </c>
       <c r="S51" t="s">
         <v>20</v>
@@ -9244,52 +9519,52 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D52">
         <v>15</v>
       </c>
       <c r="E52">
-        <v>2453</v>
+        <v>1971</v>
       </c>
       <c r="F52">
-        <v>7359</v>
+        <v>5913</v>
       </c>
       <c r="G52">
-        <v>14718</v>
+        <v>11826</v>
       </c>
       <c r="H52">
-        <v>24531</v>
+        <v>19711</v>
       </c>
       <c r="I52">
-        <v>36796</v>
+        <v>29566</v>
       </c>
       <c r="J52">
-        <v>51515</v>
+        <v>41393</v>
       </c>
       <c r="K52">
-        <v>68686</v>
+        <v>55190</v>
       </c>
       <c r="L52">
-        <v>88311</v>
+        <v>70959</v>
       </c>
       <c r="M52">
-        <v>110388</v>
+        <v>88698</v>
       </c>
       <c r="N52">
-        <v>134919</v>
+        <v>108409</v>
       </c>
       <c r="O52">
-        <v>161903</v>
+        <v>130091</v>
       </c>
       <c r="P52">
-        <v>191340</v>
+        <v>153744</v>
       </c>
       <c r="Q52">
-        <v>223230</v>
+        <v>179368</v>
       </c>
       <c r="R52">
-        <v>257573</v>
+        <v>206963</v>
       </c>
       <c r="S52" t="s">
         <v>20</v>
@@ -9312,52 +9587,52 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D53">
         <v>15</v>
       </c>
       <c r="E53">
-        <v>2952</v>
+        <v>2453</v>
       </c>
       <c r="F53">
-        <v>8855</v>
+        <v>7359</v>
       </c>
       <c r="G53">
-        <v>17709</v>
+        <v>14718</v>
       </c>
       <c r="H53">
-        <v>29516</v>
+        <v>24531</v>
       </c>
       <c r="I53">
-        <v>44274</v>
+        <v>36796</v>
       </c>
       <c r="J53">
-        <v>61983</v>
+        <v>51515</v>
       </c>
       <c r="K53">
-        <v>82644</v>
+        <v>68686</v>
       </c>
       <c r="L53">
-        <v>106257</v>
+        <v>88311</v>
       </c>
       <c r="M53">
-        <v>132821</v>
+        <v>110388</v>
       </c>
       <c r="N53">
-        <v>162336</v>
+        <v>134919</v>
       </c>
       <c r="O53">
-        <v>194804</v>
+        <v>161903</v>
       </c>
       <c r="P53">
-        <v>230223</v>
+        <v>191340</v>
       </c>
       <c r="Q53">
-        <v>268593</v>
+        <v>223230</v>
       </c>
       <c r="R53">
-        <v>309915</v>
+        <v>257573</v>
       </c>
       <c r="S53" t="s">
         <v>20</v>
@@ -9380,67 +9655,67 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D54">
+        <v>15</v>
+      </c>
+      <c r="E54">
+        <v>2952</v>
+      </c>
+      <c r="F54">
+        <v>8855</v>
+      </c>
+      <c r="G54">
+        <v>17709</v>
+      </c>
+      <c r="H54">
+        <v>29516</v>
+      </c>
+      <c r="I54">
+        <v>44274</v>
+      </c>
+      <c r="J54">
+        <v>61983</v>
+      </c>
+      <c r="K54">
+        <v>82644</v>
+      </c>
+      <c r="L54">
+        <v>106257</v>
+      </c>
+      <c r="M54">
+        <v>132821</v>
+      </c>
+      <c r="N54">
+        <v>162336</v>
+      </c>
+      <c r="O54">
+        <v>194804</v>
+      </c>
+      <c r="P54">
+        <v>230223</v>
+      </c>
+      <c r="Q54">
+        <v>268593</v>
+      </c>
+      <c r="R54">
+        <v>309915</v>
+      </c>
+      <c r="S54" t="s">
         <v>20</v>
       </c>
-      <c r="E54">
-        <v>2553</v>
-      </c>
-      <c r="F54">
-        <v>7658</v>
-      </c>
-      <c r="G54">
-        <v>15317</v>
-      </c>
-      <c r="H54">
-        <v>25528</v>
-      </c>
-      <c r="I54">
-        <v>38292</v>
-      </c>
-      <c r="J54">
-        <v>53609</v>
-      </c>
-      <c r="K54">
-        <v>71478</v>
-      </c>
-      <c r="L54">
-        <v>91900</v>
-      </c>
-      <c r="M54">
-        <v>114876</v>
-      </c>
-      <c r="N54">
-        <v>140403</v>
-      </c>
-      <c r="O54">
-        <v>168484</v>
-      </c>
-      <c r="P54">
-        <v>199118</v>
-      </c>
-      <c r="Q54">
-        <v>232304</v>
-      </c>
-      <c r="R54">
-        <v>268043</v>
-      </c>
-      <c r="S54">
-        <v>306335</v>
-      </c>
-      <c r="T54">
-        <v>347179</v>
-      </c>
-      <c r="U54">
-        <v>390577</v>
-      </c>
-      <c r="V54">
-        <v>436527</v>
-      </c>
-      <c r="W54">
-        <v>485030</v>
+      <c r="T54" t="s">
+        <v>20</v>
+      </c>
+      <c r="U54" t="s">
+        <v>20</v>
+      </c>
+      <c r="V54" t="s">
+        <v>20</v>
+      </c>
+      <c r="W54" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
@@ -9448,67 +9723,67 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="D55">
         <v>20</v>
       </c>
-      <c r="E55" s="84">
-        <v>2940</v>
-      </c>
-      <c r="F55" s="84">
-        <v>8821</v>
-      </c>
-      <c r="G55" s="84">
-        <v>17642</v>
-      </c>
-      <c r="H55" s="84">
-        <v>29403</v>
-      </c>
-      <c r="I55" s="84">
-        <v>44105</v>
-      </c>
-      <c r="J55" s="84">
-        <v>61747</v>
-      </c>
-      <c r="K55" s="84">
-        <v>82329</v>
-      </c>
-      <c r="L55" s="84">
-        <v>105851</v>
-      </c>
-      <c r="M55" s="84">
-        <v>132314</v>
-      </c>
-      <c r="N55" s="84">
-        <v>161717</v>
-      </c>
-      <c r="O55" s="84">
-        <v>194061</v>
-      </c>
-      <c r="P55" s="84">
-        <v>229345</v>
-      </c>
-      <c r="Q55" s="84">
-        <v>267569</v>
-      </c>
-      <c r="R55" s="84">
-        <v>308733</v>
-      </c>
-      <c r="S55" s="84">
-        <v>352838</v>
-      </c>
-      <c r="T55" s="84">
-        <v>399883</v>
-      </c>
-      <c r="U55" s="84">
-        <v>449868</v>
-      </c>
-      <c r="V55" s="84">
-        <v>502794</v>
-      </c>
-      <c r="W55" s="84">
-        <v>558660</v>
+      <c r="E55">
+        <v>2553</v>
+      </c>
+      <c r="F55">
+        <v>7658</v>
+      </c>
+      <c r="G55">
+        <v>15317</v>
+      </c>
+      <c r="H55">
+        <v>25528</v>
+      </c>
+      <c r="I55">
+        <v>38292</v>
+      </c>
+      <c r="J55">
+        <v>53609</v>
+      </c>
+      <c r="K55">
+        <v>71478</v>
+      </c>
+      <c r="L55">
+        <v>91900</v>
+      </c>
+      <c r="M55">
+        <v>114876</v>
+      </c>
+      <c r="N55">
+        <v>140403</v>
+      </c>
+      <c r="O55">
+        <v>168484</v>
+      </c>
+      <c r="P55">
+        <v>199118</v>
+      </c>
+      <c r="Q55">
+        <v>232304</v>
+      </c>
+      <c r="R55">
+        <v>268043</v>
+      </c>
+      <c r="S55">
+        <v>306335</v>
+      </c>
+      <c r="T55">
+        <v>347179</v>
+      </c>
+      <c r="U55">
+        <v>390577</v>
+      </c>
+      <c r="V55">
+        <v>436527</v>
+      </c>
+      <c r="W55">
+        <v>485030</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
@@ -9516,67 +9791,67 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D56">
         <v>20</v>
       </c>
-      <c r="E56">
-        <v>3337</v>
-      </c>
-      <c r="F56">
-        <v>10010</v>
-      </c>
-      <c r="G56">
-        <v>20020</v>
-      </c>
-      <c r="H56">
-        <v>33366</v>
-      </c>
-      <c r="I56">
-        <v>50049</v>
-      </c>
-      <c r="J56">
-        <v>70069</v>
-      </c>
-      <c r="K56">
-        <v>93426</v>
-      </c>
-      <c r="L56">
-        <v>120119</v>
-      </c>
-      <c r="M56">
-        <v>150148</v>
-      </c>
-      <c r="N56">
-        <v>183515</v>
-      </c>
-      <c r="O56">
-        <v>220218</v>
-      </c>
-      <c r="P56">
-        <v>260257</v>
-      </c>
-      <c r="Q56">
-        <v>303633</v>
-      </c>
-      <c r="R56">
-        <v>350346</v>
-      </c>
-      <c r="S56">
-        <v>400396</v>
-      </c>
-      <c r="T56">
-        <v>453782</v>
-      </c>
-      <c r="U56">
-        <v>510505</v>
-      </c>
-      <c r="V56">
-        <v>570564</v>
-      </c>
-      <c r="W56">
-        <v>633960</v>
+      <c r="E56" s="84">
+        <v>2940</v>
+      </c>
+      <c r="F56" s="84">
+        <v>8821</v>
+      </c>
+      <c r="G56" s="84">
+        <v>17642</v>
+      </c>
+      <c r="H56" s="84">
+        <v>29403</v>
+      </c>
+      <c r="I56" s="84">
+        <v>44105</v>
+      </c>
+      <c r="J56" s="84">
+        <v>61747</v>
+      </c>
+      <c r="K56" s="84">
+        <v>82329</v>
+      </c>
+      <c r="L56" s="84">
+        <v>105851</v>
+      </c>
+      <c r="M56" s="84">
+        <v>132314</v>
+      </c>
+      <c r="N56" s="84">
+        <v>161717</v>
+      </c>
+      <c r="O56" s="84">
+        <v>194061</v>
+      </c>
+      <c r="P56" s="84">
+        <v>229345</v>
+      </c>
+      <c r="Q56" s="84">
+        <v>267569</v>
+      </c>
+      <c r="R56" s="84">
+        <v>308733</v>
+      </c>
+      <c r="S56" s="84">
+        <v>352838</v>
+      </c>
+      <c r="T56" s="84">
+        <v>399883</v>
+      </c>
+      <c r="U56" s="84">
+        <v>449868</v>
+      </c>
+      <c r="V56" s="84">
+        <v>502794</v>
+      </c>
+      <c r="W56" s="84">
+        <v>558660</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
@@ -9584,67 +9859,67 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D57">
         <v>20</v>
       </c>
       <c r="E57">
-        <v>3741</v>
+        <v>3337</v>
       </c>
       <c r="F57">
-        <v>11223</v>
+        <v>10010</v>
       </c>
       <c r="G57">
-        <v>22445</v>
+        <v>20020</v>
       </c>
       <c r="H57">
-        <v>37409</v>
+        <v>33366</v>
       </c>
       <c r="I57">
-        <v>56113</v>
+        <v>50049</v>
       </c>
       <c r="J57">
-        <v>78559</v>
+        <v>70069</v>
       </c>
       <c r="K57">
-        <v>104745</v>
+        <v>93426</v>
       </c>
       <c r="L57">
-        <v>134672</v>
+        <v>120119</v>
       </c>
       <c r="M57">
-        <v>168340</v>
+        <v>150148</v>
       </c>
       <c r="N57">
-        <v>205749</v>
+        <v>183515</v>
       </c>
       <c r="O57">
-        <v>246899</v>
+        <v>220218</v>
       </c>
       <c r="P57">
-        <v>291790</v>
+        <v>260257</v>
       </c>
       <c r="Q57">
-        <v>340421</v>
+        <v>303633</v>
       </c>
       <c r="R57">
-        <v>392794</v>
+        <v>350346</v>
       </c>
       <c r="S57">
-        <v>448907</v>
+        <v>400396</v>
       </c>
       <c r="T57">
-        <v>508762</v>
+        <v>453782</v>
       </c>
       <c r="U57">
-        <v>572357</v>
+        <v>510505</v>
       </c>
       <c r="V57">
-        <v>639693</v>
+        <v>570564</v>
       </c>
       <c r="W57">
-        <v>710770</v>
+        <v>633960</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
@@ -9652,67 +9927,67 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>197</v>
+        <v>14</v>
       </c>
       <c r="D58">
         <v>20</v>
       </c>
       <c r="E58">
-        <v>4153</v>
+        <v>3741</v>
       </c>
       <c r="F58">
-        <v>12458</v>
+        <v>11223</v>
       </c>
       <c r="G58">
-        <v>24916</v>
+        <v>22445</v>
       </c>
       <c r="H58">
-        <v>41526</v>
+        <v>37409</v>
       </c>
       <c r="I58">
-        <v>62289</v>
+        <v>56113</v>
       </c>
       <c r="J58">
-        <v>87205</v>
+        <v>78559</v>
       </c>
       <c r="K58">
-        <v>116274</v>
+        <v>104745</v>
       </c>
       <c r="L58">
-        <v>149495</v>
+        <v>134672</v>
       </c>
       <c r="M58">
-        <v>186868</v>
+        <v>168340</v>
       </c>
       <c r="N58">
-        <v>228395</v>
+        <v>205749</v>
       </c>
       <c r="O58">
-        <v>274074</v>
+        <v>246899</v>
       </c>
       <c r="P58">
-        <v>323905</v>
+        <v>291790</v>
       </c>
       <c r="Q58">
-        <v>377889</v>
+        <v>340421</v>
       </c>
       <c r="R58">
-        <v>436026</v>
+        <v>392794</v>
       </c>
       <c r="S58">
-        <v>498316</v>
+        <v>448907</v>
       </c>
       <c r="T58">
-        <v>564758</v>
+        <v>508762</v>
       </c>
       <c r="U58">
-        <v>635353</v>
+        <v>572357</v>
       </c>
       <c r="V58">
-        <v>710100</v>
+        <v>639693</v>
       </c>
       <c r="W58">
-        <v>789000</v>
+        <v>710770</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
@@ -9720,140 +9995,285 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>230</v>
+        <v>197</v>
       </c>
       <c r="D59">
         <v>20</v>
       </c>
-      <c r="E59" s="128">
+      <c r="E59">
+        <v>4153</v>
+      </c>
+      <c r="F59">
+        <v>12458</v>
+      </c>
+      <c r="G59">
+        <v>24916</v>
+      </c>
+      <c r="H59">
+        <v>41526</v>
+      </c>
+      <c r="I59">
+        <v>62289</v>
+      </c>
+      <c r="J59">
+        <v>87205</v>
+      </c>
+      <c r="K59">
+        <v>116274</v>
+      </c>
+      <c r="L59">
+        <v>149495</v>
+      </c>
+      <c r="M59">
+        <v>186868</v>
+      </c>
+      <c r="N59">
+        <v>228395</v>
+      </c>
+      <c r="O59">
+        <v>274074</v>
+      </c>
+      <c r="P59">
+        <v>323905</v>
+      </c>
+      <c r="Q59">
+        <v>377889</v>
+      </c>
+      <c r="R59">
+        <v>436026</v>
+      </c>
+      <c r="S59">
+        <v>498316</v>
+      </c>
+      <c r="T59">
+        <v>564758</v>
+      </c>
+      <c r="U59">
+        <v>635353</v>
+      </c>
+      <c r="V59">
+        <v>710100</v>
+      </c>
+      <c r="W59">
+        <v>789000</v>
+      </c>
+    </row>
+    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>230</v>
+      </c>
+      <c r="D60">
+        <v>20</v>
+      </c>
+      <c r="E60" s="128">
         <v>4571</v>
       </c>
-      <c r="F59" s="129">
+      <c r="F60" s="129">
         <v>13714</v>
       </c>
-      <c r="G59" s="129">
+      <c r="G60" s="129">
         <v>27428</v>
       </c>
-      <c r="H59" s="129">
+      <c r="H60" s="129">
         <v>45713</v>
       </c>
-      <c r="I59" s="129">
+      <c r="I60" s="129">
         <v>68569</v>
       </c>
-      <c r="J59" s="129">
+      <c r="J60" s="129">
         <v>95997</v>
       </c>
-      <c r="K59" s="129">
+      <c r="K60" s="129">
         <v>127995</v>
       </c>
-      <c r="L59" s="129">
+      <c r="L60" s="129">
         <v>164565</v>
       </c>
-      <c r="M59" s="129">
+      <c r="M60" s="129">
         <v>205707</v>
       </c>
-      <c r="N59" s="129">
+      <c r="N60" s="129">
         <v>251419</v>
       </c>
-      <c r="O59" s="129">
+      <c r="O60" s="129">
         <v>301703</v>
       </c>
-      <c r="P59" s="129">
+      <c r="P60" s="129">
         <v>356559</v>
       </c>
-      <c r="Q59" s="129">
+      <c r="Q60" s="129">
         <v>415985</v>
       </c>
-      <c r="R59" s="129">
+      <c r="R60" s="129">
         <v>479983</v>
       </c>
-      <c r="S59" s="129">
+      <c r="S60" s="129">
         <v>548552</v>
       </c>
-      <c r="T59" s="129">
+      <c r="T60" s="129">
         <v>621692</v>
       </c>
-      <c r="U59" s="129">
+      <c r="U60" s="129">
         <v>699403</v>
       </c>
-      <c r="V59" s="129">
+      <c r="V60" s="129">
         <v>781686</v>
       </c>
-      <c r="W59" s="129">
+      <c r="W60" s="129">
         <v>868540</v>
+      </c>
+    </row>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>247</v>
+      </c>
+      <c r="D61">
+        <v>20</v>
+      </c>
+      <c r="E61" s="128">
+        <v>4996</v>
+      </c>
+      <c r="F61" s="129">
+        <v>14989</v>
+      </c>
+      <c r="G61" s="129">
+        <v>29979</v>
+      </c>
+      <c r="H61" s="129">
+        <v>49964</v>
+      </c>
+      <c r="I61" s="129">
+        <v>74946</v>
+      </c>
+      <c r="J61" s="129">
+        <v>104925</v>
+      </c>
+      <c r="K61" s="129">
+        <v>139900</v>
+      </c>
+      <c r="L61" s="129">
+        <v>179871</v>
+      </c>
+      <c r="M61" s="129">
+        <v>224839</v>
+      </c>
+      <c r="N61" s="129">
+        <v>274803</v>
+      </c>
+      <c r="O61" s="129">
+        <v>329764</v>
+      </c>
+      <c r="P61" s="129">
+        <v>389721</v>
+      </c>
+      <c r="Q61" s="129">
+        <v>454674</v>
+      </c>
+      <c r="R61" s="129">
+        <v>524624</v>
+      </c>
+      <c r="S61" s="129">
+        <v>599571</v>
+      </c>
+      <c r="T61" s="129">
+        <v>679513</v>
+      </c>
+      <c r="U61" s="129">
+        <v>764452</v>
+      </c>
+      <c r="V61" s="129">
+        <v>854388</v>
+      </c>
+      <c r="W61" s="129">
+        <v>949320</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="AK29:AL29"/>
-    <mergeCell ref="AS29:AY29"/>
+    <mergeCell ref="AK30:AL30"/>
+    <mergeCell ref="AS30:AY30"/>
     <mergeCell ref="AO14:AR14"/>
-    <mergeCell ref="BF29:BL29"/>
-    <mergeCell ref="AI29:AJ29"/>
-    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="BF30:BL30"/>
+    <mergeCell ref="AI30:AJ30"/>
+    <mergeCell ref="AM30:AR30"/>
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="N30:T30"/>
+    <mergeCell ref="J30:M30"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="124" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C11">
-    <cfRule type="duplicateValues" dxfId="123" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="122" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="121" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="120" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="119" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="118" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="117" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="116" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="115" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="114" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="113" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="duplicateValues" dxfId="112" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT28">
-    <cfRule type="duplicateValues" dxfId="111" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ28:BS28">
-    <cfRule type="duplicateValues" dxfId="110" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="108" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BT29">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ29:BS29">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D28">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D29">
       <formula1>INDIRECT("dragonTierDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D47:D59 E48:E58 F47:W59"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D35:D36 D40:D42">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D48:D61 E49:E59 F48:W61"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D36:D37 D41:D43">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
bug fix 6156 . Reduced speed multiplier when in Hungry mode
Former-commit-id: b9a0e769987d89f01908619ad401aa3e9beb9e87
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -2034,6 +2034,33 @@
     <xf numFmtId="49" fontId="0" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2062,33 +2089,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5055,8 +5055,8 @@
   </sheetPr>
   <dimension ref="A1:BT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="AK29" sqref="AK29:AL29"/>
+    <sheetView tabSelected="1" topLeftCell="AM13" workbookViewId="0">
+      <selection activeCell="AT28" sqref="AT28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5338,10 +5338,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="240"/>
-      <c r="AP14" s="240"/>
-      <c r="AQ14" s="240"/>
-      <c r="AR14" s="240"/>
+      <c r="AO14" s="249"/>
+      <c r="AP14" s="249"/>
+      <c r="AQ14" s="249"/>
+      <c r="AR14" s="249"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -8207,7 +8207,7 @@
         <v>1.05</v>
       </c>
       <c r="AT28" s="196">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AU28" s="196">
         <v>2</v>
@@ -8296,83 +8296,83 @@
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
       <c r="I29" s="30"/>
-      <c r="J29" s="254" t="s">
+      <c r="J29" s="244" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="254"/>
-      <c r="L29" s="254"/>
-      <c r="M29" s="254"/>
-      <c r="N29" s="252" t="s">
+      <c r="K29" s="244"/>
+      <c r="L29" s="244"/>
+      <c r="M29" s="244"/>
+      <c r="N29" s="242" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="253"/>
-      <c r="P29" s="253"/>
-      <c r="Q29" s="253"/>
-      <c r="R29" s="253"/>
-      <c r="S29" s="253"/>
-      <c r="T29" s="253"/>
-      <c r="U29" s="250" t="s">
+      <c r="O29" s="243"/>
+      <c r="P29" s="243"/>
+      <c r="Q29" s="243"/>
+      <c r="R29" s="243"/>
+      <c r="S29" s="243"/>
+      <c r="T29" s="243"/>
+      <c r="U29" s="240" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="251"/>
+      <c r="V29" s="241"/>
       <c r="W29" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X29" s="247" t="s">
+      <c r="X29" s="237" t="s">
         <v>70</v>
       </c>
-      <c r="Y29" s="248"/>
-      <c r="Z29" s="248"/>
-      <c r="AA29" s="248"/>
-      <c r="AB29" s="249"/>
-      <c r="AC29" s="246" t="s">
+      <c r="Y29" s="238"/>
+      <c r="Z29" s="238"/>
+      <c r="AA29" s="238"/>
+      <c r="AB29" s="239"/>
+      <c r="AC29" s="236" t="s">
         <v>69</v>
       </c>
-      <c r="AD29" s="246"/>
-      <c r="AE29" s="246"/>
-      <c r="AF29" s="246"/>
-      <c r="AG29" s="246"/>
+      <c r="AD29" s="236"/>
+      <c r="AE29" s="236"/>
+      <c r="AF29" s="236"/>
+      <c r="AG29" s="236"/>
       <c r="AH29" s="30"/>
-      <c r="AI29" s="242" t="s">
+      <c r="AI29" s="251" t="s">
         <v>68</v>
       </c>
-      <c r="AJ29" s="242"/>
-      <c r="AK29" s="236" t="s">
+      <c r="AJ29" s="251"/>
+      <c r="AK29" s="245" t="s">
         <v>246</v>
       </c>
-      <c r="AL29" s="236"/>
-      <c r="AM29" s="243" t="s">
+      <c r="AL29" s="245"/>
+      <c r="AM29" s="252" t="s">
         <v>236</v>
       </c>
-      <c r="AN29" s="244"/>
-      <c r="AO29" s="244"/>
-      <c r="AP29" s="244"/>
-      <c r="AQ29" s="244"/>
-      <c r="AR29" s="245"/>
-      <c r="AS29" s="237" t="s">
+      <c r="AN29" s="253"/>
+      <c r="AO29" s="253"/>
+      <c r="AP29" s="253"/>
+      <c r="AQ29" s="253"/>
+      <c r="AR29" s="254"/>
+      <c r="AS29" s="246" t="s">
         <v>226</v>
       </c>
-      <c r="AT29" s="238"/>
-      <c r="AU29" s="238"/>
-      <c r="AV29" s="238"/>
-      <c r="AW29" s="238"/>
-      <c r="AX29" s="238"/>
-      <c r="AY29" s="239"/>
+      <c r="AT29" s="247"/>
+      <c r="AU29" s="247"/>
+      <c r="AV29" s="247"/>
+      <c r="AW29" s="247"/>
+      <c r="AX29" s="247"/>
+      <c r="AY29" s="248"/>
       <c r="AZ29" s="30"/>
       <c r="BA29" s="30"/>
       <c r="BB29" s="30"/>
       <c r="BC29" s="30"/>
       <c r="BD29" s="30"/>
       <c r="BE29" s="30"/>
-      <c r="BF29" s="241" t="s">
+      <c r="BF29" s="250" t="s">
         <v>67</v>
       </c>
-      <c r="BG29" s="241"/>
-      <c r="BH29" s="241"/>
-      <c r="BI29" s="241"/>
-      <c r="BJ29" s="241"/>
-      <c r="BK29" s="241"/>
-      <c r="BL29" s="241"/>
+      <c r="BG29" s="250"/>
+      <c r="BH29" s="250"/>
+      <c r="BI29" s="250"/>
+      <c r="BJ29" s="250"/>
+      <c r="BK29" s="250"/>
+      <c r="BL29" s="250"/>
       <c r="BM29" s="30"/>
       <c r="BN29" s="30"/>
       <c r="BO29" s="30"/>
@@ -9785,17 +9785,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="X29:AB29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="N29:T29"/>
-    <mergeCell ref="J29:M29"/>
     <mergeCell ref="AK29:AL29"/>
     <mergeCell ref="AS29:AY29"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF29:BL29"/>
     <mergeCell ref="AI29:AJ29"/>
     <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="N29:T29"/>
+    <mergeCell ref="J29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="124" priority="19"/>

</xml_diff>

<commit_message>
Speed mod. for Hungry mode, reduced to Umbra and Alien
Former-commit-id: 88eacdf6e44988817aae9f3e9c8dc2c36b33f35c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -2080,6 +2080,90 @@
     <xf numFmtId="49" fontId="0" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2104,301 +2188,17 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="128">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -4737,6 +4537,206 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4751,105 +4751,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT29" totalsRowShown="0" headerRowDxfId="127" dataDxfId="125" headerRowBorderDxfId="126" tableBorderDxfId="124" totalsRowBorderDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT29" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104" totalsRowBorderDxfId="103">
   <autoFilter ref="B15:BT29"/>
   <tableColumns count="71">
-    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="122"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="121"/>
-    <tableColumn id="9" name="[tier]" dataDxfId="120"/>
-    <tableColumn id="65" name="[type]" dataDxfId="119"/>
-    <tableColumn id="3" name="[order]" dataDxfId="118"/>
-    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="117"/>
-    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="116"/>
-    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="115"/>
-    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="114"/>
-    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="113"/>
-    <tableColumn id="39" name="[defaultSize]" dataDxfId="112"/>
-    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="111"/>
-    <tableColumn id="17" name="[healthMin]" dataDxfId="110"/>
-    <tableColumn id="18" name="[healthMax]" dataDxfId="109"/>
-    <tableColumn id="21" name="[healthDrain]" dataDxfId="108"/>
-    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="107"/>
-    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="106"/>
-    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="105"/>
-    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="104"/>
-    <tableColumn id="19" name="[scaleMin]" dataDxfId="103"/>
-    <tableColumn id="20" name="[scaleMax]" dataDxfId="102"/>
-    <tableColumn id="42" name="[speedBase]" dataDxfId="101"/>
-    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="100"/>
-    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="99"/>
-    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="98">
+    <tableColumn id="1" name="{dragonDefinitions}" dataDxfId="102"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="101"/>
+    <tableColumn id="9" name="[tier]" dataDxfId="100"/>
+    <tableColumn id="65" name="[type]" dataDxfId="99"/>
+    <tableColumn id="3" name="[order]" dataDxfId="98"/>
+    <tableColumn id="40" name="[previousDragonSku]" dataDxfId="97"/>
+    <tableColumn id="4" name="[unlockPriceCoins]" dataDxfId="96"/>
+    <tableColumn id="5" name="[unlockPricePC]" dataDxfId="95"/>
+    <tableColumn id="11" name="[cameraDefaultZoom]" dataDxfId="94"/>
+    <tableColumn id="16" name="[cameraFarZoom]" dataDxfId="93"/>
+    <tableColumn id="39" name="[defaultSize]" dataDxfId="92"/>
+    <tableColumn id="38" name="[cameraFrameWidthModifier]" dataDxfId="91"/>
+    <tableColumn id="17" name="[healthMin]" dataDxfId="90"/>
+    <tableColumn id="18" name="[healthMax]" dataDxfId="89"/>
+    <tableColumn id="21" name="[healthDrain]" dataDxfId="88"/>
+    <tableColumn id="52" name="[healthDrainSpacePlus]" dataDxfId="87"/>
+    <tableColumn id="32" name="[healthDrainAmpPerSecond]" dataDxfId="86"/>
+    <tableColumn id="31" name="[sessionStartHealthDrainTime]" dataDxfId="85"/>
+    <tableColumn id="30" name="[sessionStartHealthDrainModifier]" dataDxfId="84"/>
+    <tableColumn id="19" name="[scaleMin]" dataDxfId="83"/>
+    <tableColumn id="20" name="[scaleMax]" dataDxfId="82"/>
+    <tableColumn id="42" name="[speedBase]" dataDxfId="81"/>
+    <tableColumn id="22" name="[boostMultiplier]" dataDxfId="80"/>
+    <tableColumn id="41" name="[energyBaseMin]" dataDxfId="79"/>
+    <tableColumn id="62" name="[energyBaseMax]" dataDxfId="78">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="[energyDrain]" dataDxfId="97"/>
-    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="96"/>
-    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="95"/>
-    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="94"/>
-    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="93"/>
-    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="92"/>
-    <tableColumn id="25" name="[furyMax]" dataDxfId="91"/>
-    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="90"/>
-    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="89"/>
-    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="88">
+    <tableColumn id="23" name="[energyDrain]" dataDxfId="77"/>
+    <tableColumn id="24" name="[energyRefillRate]" dataDxfId="76"/>
+    <tableColumn id="29" name="[furyBaseDamage]" dataDxfId="75"/>
+    <tableColumn id="33" name="[furyBaseLength]" dataDxfId="74"/>
+    <tableColumn id="12" name="[furyScoreMultiplier]" dataDxfId="73"/>
+    <tableColumn id="26" name="[furyBaseDuration]" dataDxfId="72"/>
+    <tableColumn id="25" name="[furyMax]" dataDxfId="71"/>
+    <tableColumn id="54" name="[scoreTextThresholdMultiplier]" dataDxfId="70"/>
+    <tableColumn id="14" name="[eatSpeedFactorMin]" dataDxfId="69"/>
+    <tableColumn id="64" name="[eatSpeedFactorMax]" dataDxfId="68">
       <calculatedColumnFormula>AI17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="87"/>
-    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="86"/>
-    <tableColumn id="6" name="[gamePrefab]" dataDxfId="85"/>
-    <tableColumn id="10" name="[menuPrefab]" dataDxfId="84"/>
-    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="83"/>
-    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="82"/>
-    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="81"/>
-    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="80"/>
-    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="79"/>
-    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="78"/>
-    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="77"/>
-    <tableColumn id="47" name="[invincible]" dataDxfId="76"/>
-    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="75"/>
-    <tableColumn id="45" name="[eatEverything]" dataDxfId="74"/>
-    <tableColumn id="46" name="[modeDuration]" dataDxfId="73"/>
-    <tableColumn id="53" name="[petScale]" dataDxfId="72"/>
-    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="71"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="70">
+    <tableColumn id="15" name="[maxAlcohol]" dataDxfId="67"/>
+    <tableColumn id="13" name="[alcoholDrain]" dataDxfId="66"/>
+    <tableColumn id="6" name="[gamePrefab]" dataDxfId="65"/>
+    <tableColumn id="10" name="[menuPrefab]" dataDxfId="64"/>
+    <tableColumn id="60" name="[resultsPrefab]" dataDxfId="63"/>
+    <tableColumn id="57" name="[shadowFromDragon]" dataDxfId="62"/>
+    <tableColumn id="56" name="[revealFromDragon]" dataDxfId="61"/>
+    <tableColumn id="71" name="[unlockFromDragon]" dataDxfId="60"/>
+    <tableColumn id="49" name="[sizeUpMultiplier]" dataDxfId="59"/>
+    <tableColumn id="50" name="[speedUpMultiplier]" dataDxfId="58"/>
+    <tableColumn id="51" name="[biteUpMultiplier]" dataDxfId="57"/>
+    <tableColumn id="47" name="[invincible]" dataDxfId="56"/>
+    <tableColumn id="48" name="[infiniteBoost]" dataDxfId="55"/>
+    <tableColumn id="45" name="[eatEverything]" dataDxfId="54"/>
+    <tableColumn id="46" name="[modeDuration]" dataDxfId="53"/>
+    <tableColumn id="53" name="[petScale]" dataDxfId="52"/>
+    <tableColumn id="63" name="[petScaleMenu]" dataDxfId="51"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="50">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="69">
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="49">
       <calculatedColumnFormula>CONCATENATE("TID_",UPPER(dragonDefinitions[[#This Row],['[sku']]]),"_DESC")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="68"/>
-    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="67"/>
-    <tableColumn id="34" name="[forceMin]" dataDxfId="66"/>
-    <tableColumn id="61" name="[forceMax]" dataDxfId="65">
+    <tableColumn id="27" name="[statsBarRatio]" dataDxfId="48"/>
+    <tableColumn id="28" name="[furyBarRatio]" dataDxfId="47"/>
+    <tableColumn id="34" name="[forceMin]" dataDxfId="46"/>
+    <tableColumn id="61" name="[forceMax]" dataDxfId="45">
       <calculatedColumnFormula>dragonDefinitions[[#This Row],['[forceMin']]]+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="[mass]" dataDxfId="64"/>
-    <tableColumn id="36" name="[friction]" dataDxfId="63"/>
-    <tableColumn id="37" name="[gravityModifier]" dataDxfId="62"/>
-    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="61"/>
-    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="60"/>
-    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="59"/>
-    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="58"/>
-    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="57"/>
-    <tableColumn id="66" name="[mummyDuration]" dataDxfId="56"/>
-    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="55"/>
-    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="54"/>
-    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="53"/>
-    <tableColumn id="59" name="[trackingSku]" dataDxfId="52"/>
+    <tableColumn id="35" name="[mass]" dataDxfId="44"/>
+    <tableColumn id="36" name="[friction]" dataDxfId="43"/>
+    <tableColumn id="37" name="[gravityModifier]" dataDxfId="42"/>
+    <tableColumn id="43" name="[airGravityModifier]" dataDxfId="41"/>
+    <tableColumn id="44" name="[waterGravityModifier]" dataDxfId="40"/>
+    <tableColumn id="55" name="[damageAnimationThreshold]" dataDxfId="39"/>
+    <tableColumn id="58" name="[dotAnimationThreshold]" dataDxfId="38"/>
+    <tableColumn id="67" name="[mummyHealthFactor]" dataDxfId="37"/>
+    <tableColumn id="66" name="[mummyDuration]" dataDxfId="36"/>
+    <tableColumn id="68" name="[animojiPrefab]" dataDxfId="35"/>
+    <tableColumn id="70" name="[energyRequiredToBoost]" dataDxfId="34"/>
+    <tableColumn id="69" name="[energyRestartThreshold]" dataDxfId="33"/>
+    <tableColumn id="59" name="[trackingSku]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G11" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="dragonTierDefinitions" displayName="dragonTierDefinitions" ref="B4:G11" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B4:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="47"/>
+    <tableColumn id="1" name="{dragonTierDefinitions}" dataDxfId="27"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="9" name="[order]"/>
-    <tableColumn id="10" name="[icon]" dataDxfId="46"/>
-    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="45"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="44">
+    <tableColumn id="10" name="[icon]" dataDxfId="26"/>
+    <tableColumn id="3" name="[maxPetEquipped]" dataDxfId="25"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE("TID_","DRAGON_",UPPER(dragonTierDefinitions[[#This Row],['[sku']]]),"_NAME")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4858,25 +4858,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B35:J36" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="dragonSettings" displayName="dragonSettings" ref="B35:J36" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B35:J36"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="{dragonSettings}" dataDxfId="39"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="38"/>
+    <tableColumn id="1" name="{dragonSettings}" dataDxfId="19"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
     <tableColumn id="7" name="[energyRequiredToBoost]"/>
-    <tableColumn id="8" name="[superfuryMax]" dataDxfId="37"/>
-    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="36"/>
-    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="35"/>
-    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="34"/>
-    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="33"/>
-    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="32"/>
+    <tableColumn id="8" name="[superfuryMax]" dataDxfId="17"/>
+    <tableColumn id="9" name="[superFuryLengthModifier]" dataDxfId="16"/>
+    <tableColumn id="10" name="[superFuryCoinsMultiplier]" dataDxfId="15"/>
+    <tableColumn id="11" name="[superFuryDurationModifier]" dataDxfId="14"/>
+    <tableColumn id="12" name="[superFuryDamageModifier]" dataDxfId="13"/>
+    <tableColumn id="3" name="[anniversaryCakeSlices]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B47:W61" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B47:W61" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B47:W61"/>
   <tableColumns count="22">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
@@ -4907,14 +4907,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B40:F43" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="dragonHealthModifiersDefinitions" displayName="dragonHealthModifiersDefinitions" ref="B40:F43" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B40:F43"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="23"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="22"/>
+    <tableColumn id="1" name="{dragonHealthModifiersDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
     <tableColumn id="7" name="[threshold]"/>
-    <tableColumn id="8" name="[modifier]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tid]" dataDxfId="20"/>
+    <tableColumn id="8" name="[modifier]" dataDxfId="1"/>
+    <tableColumn id="9" name="[tid]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5188,8 +5188,8 @@
   </sheetPr>
   <dimension ref="A1:BT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="M69" sqref="M69"/>
+    <sheetView tabSelected="1" topLeftCell="AK13" workbookViewId="0">
+      <selection activeCell="AS30" sqref="AS30:AY30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5471,10 +5471,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="249"/>
-      <c r="AP14" s="249"/>
-      <c r="AQ14" s="249"/>
-      <c r="AR14" s="249"/>
+      <c r="AO14" s="258"/>
+      <c r="AP14" s="258"/>
+      <c r="AQ14" s="258"/>
+      <c r="AR14" s="258"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -8340,7 +8340,7 @@
         <v>1.05</v>
       </c>
       <c r="AT28" s="196">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AU28" s="196">
         <v>2</v>
@@ -8444,7 +8444,7 @@
       <c r="I29" s="150">
         <v>650</v>
       </c>
-      <c r="J29" s="255">
+      <c r="J29" s="236">
         <v>35</v>
       </c>
       <c r="K29" s="55">
@@ -8459,7 +8459,7 @@
       <c r="N29" s="40">
         <v>500</v>
       </c>
-      <c r="O29" s="256">
+      <c r="O29" s="237">
         <v>600</v>
       </c>
       <c r="P29" s="99">
@@ -8468,10 +8468,10 @@
       <c r="Q29" s="23">
         <v>0</v>
       </c>
-      <c r="R29" s="270">
+      <c r="R29" s="250">
         <v>0.02</v>
       </c>
-      <c r="S29" s="268">
+      <c r="S29" s="249">
         <v>20</v>
       </c>
       <c r="T29" s="41">
@@ -8492,7 +8492,7 @@
       <c r="Y29" s="23">
         <v>100</v>
       </c>
-      <c r="Z29" s="256">
+      <c r="Z29" s="237">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
@@ -8523,54 +8523,54 @@
       <c r="AI29" s="40">
         <v>0.04</v>
       </c>
-      <c r="AJ29" s="258">
+      <c r="AJ29" s="239">
         <v>0.03</v>
       </c>
       <c r="AK29" s="42">
         <v>0</v>
       </c>
-      <c r="AL29" s="259">
+      <c r="AL29" s="240">
         <v>12</v>
       </c>
-      <c r="AM29" s="260" t="s">
+      <c r="AM29" s="241" t="s">
         <v>248</v>
       </c>
-      <c r="AN29" s="261" t="s">
+      <c r="AN29" s="242" t="s">
         <v>249</v>
       </c>
-      <c r="AO29" s="261" t="s">
+      <c r="AO29" s="242" t="s">
         <v>250</v>
       </c>
-      <c r="AP29" s="262"/>
-      <c r="AQ29" s="262"/>
-      <c r="AR29" s="263" t="s">
+      <c r="AP29" s="243"/>
+      <c r="AQ29" s="243"/>
+      <c r="AR29" s="244" t="s">
         <v>230</v>
       </c>
-      <c r="AS29" s="264">
+      <c r="AS29" s="245">
         <v>1.05</v>
       </c>
-      <c r="AT29" s="257">
+      <c r="AT29" s="238">
+        <v>1.5</v>
+      </c>
+      <c r="AU29" s="238">
         <v>2</v>
       </c>
-      <c r="AU29" s="257">
-        <v>2</v>
-      </c>
-      <c r="AV29" s="257" t="b">
+      <c r="AV29" s="238" t="b">
         <v>1</v>
       </c>
-      <c r="AW29" s="257" t="b">
+      <c r="AW29" s="238" t="b">
         <v>1</v>
       </c>
-      <c r="AX29" s="257" t="b">
+      <c r="AX29" s="238" t="b">
         <v>1</v>
       </c>
-      <c r="AY29" s="265">
+      <c r="AY29" s="246">
         <v>25</v>
       </c>
-      <c r="AZ29" s="257">
+      <c r="AZ29" s="238">
         <v>0.75</v>
       </c>
-      <c r="BA29" s="257">
+      <c r="BA29" s="238">
         <v>0.4</v>
       </c>
       <c r="BB29" s="105" t="s">
@@ -8579,7 +8579,7 @@
       <c r="BC29" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="BD29" s="266">
+      <c r="BD29" s="247">
         <v>1.5E-3</v>
       </c>
       <c r="BE29" s="47">
@@ -8588,7 +8588,7 @@
       <c r="BF29" s="106">
         <v>700</v>
       </c>
-      <c r="BG29" s="267">
+      <c r="BG29" s="248">
         <v>750</v>
       </c>
       <c r="BH29" s="34">
@@ -8618,11 +8618,11 @@
       <c r="BP29" s="110">
         <v>25</v>
       </c>
-      <c r="BQ29" s="271"/>
-      <c r="BR29" s="272">
+      <c r="BQ29" s="251"/>
+      <c r="BR29" s="252">
         <v>0.2</v>
       </c>
-      <c r="BS29" s="273">
+      <c r="BS29" s="253">
         <v>1</v>
       </c>
       <c r="BT29" s="113" t="s">
@@ -8639,83 +8639,83 @@
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="30"/>
-      <c r="J30" s="244" t="s">
+      <c r="J30" s="273" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="244"/>
-      <c r="L30" s="244"/>
-      <c r="M30" s="244"/>
-      <c r="N30" s="242" t="s">
+      <c r="K30" s="273"/>
+      <c r="L30" s="273"/>
+      <c r="M30" s="273"/>
+      <c r="N30" s="270" t="s">
         <v>73</v>
       </c>
-      <c r="O30" s="243"/>
-      <c r="P30" s="243"/>
-      <c r="Q30" s="243"/>
-      <c r="R30" s="269"/>
-      <c r="S30" s="243"/>
-      <c r="T30" s="243"/>
-      <c r="U30" s="240" t="s">
+      <c r="O30" s="271"/>
+      <c r="P30" s="271"/>
+      <c r="Q30" s="271"/>
+      <c r="R30" s="272"/>
+      <c r="S30" s="271"/>
+      <c r="T30" s="271"/>
+      <c r="U30" s="268" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="241"/>
+      <c r="V30" s="269"/>
       <c r="W30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X30" s="237" t="s">
+      <c r="X30" s="265" t="s">
         <v>70</v>
       </c>
-      <c r="Y30" s="238"/>
-      <c r="Z30" s="238"/>
-      <c r="AA30" s="238"/>
-      <c r="AB30" s="239"/>
-      <c r="AC30" s="236" t="s">
+      <c r="Y30" s="266"/>
+      <c r="Z30" s="266"/>
+      <c r="AA30" s="266"/>
+      <c r="AB30" s="267"/>
+      <c r="AC30" s="264" t="s">
         <v>69</v>
       </c>
-      <c r="AD30" s="236"/>
-      <c r="AE30" s="236"/>
-      <c r="AF30" s="236"/>
-      <c r="AG30" s="236"/>
+      <c r="AD30" s="264"/>
+      <c r="AE30" s="264"/>
+      <c r="AF30" s="264"/>
+      <c r="AG30" s="264"/>
       <c r="AH30" s="30"/>
-      <c r="AI30" s="251" t="s">
+      <c r="AI30" s="260" t="s">
         <v>68</v>
       </c>
-      <c r="AJ30" s="251"/>
-      <c r="AK30" s="245" t="s">
+      <c r="AJ30" s="260"/>
+      <c r="AK30" s="254" t="s">
         <v>246</v>
       </c>
-      <c r="AL30" s="245"/>
-      <c r="AM30" s="252" t="s">
+      <c r="AL30" s="254"/>
+      <c r="AM30" s="261" t="s">
         <v>236</v>
       </c>
-      <c r="AN30" s="253"/>
-      <c r="AO30" s="253"/>
-      <c r="AP30" s="253"/>
-      <c r="AQ30" s="253"/>
-      <c r="AR30" s="254"/>
-      <c r="AS30" s="246" t="s">
+      <c r="AN30" s="262"/>
+      <c r="AO30" s="262"/>
+      <c r="AP30" s="262"/>
+      <c r="AQ30" s="262"/>
+      <c r="AR30" s="263"/>
+      <c r="AS30" s="255" t="s">
         <v>226</v>
       </c>
-      <c r="AT30" s="247"/>
-      <c r="AU30" s="247"/>
-      <c r="AV30" s="247"/>
-      <c r="AW30" s="247"/>
-      <c r="AX30" s="247"/>
-      <c r="AY30" s="248"/>
+      <c r="AT30" s="256"/>
+      <c r="AU30" s="256"/>
+      <c r="AV30" s="256"/>
+      <c r="AW30" s="256"/>
+      <c r="AX30" s="256"/>
+      <c r="AY30" s="257"/>
       <c r="AZ30" s="30"/>
       <c r="BA30" s="30"/>
       <c r="BB30" s="30"/>
       <c r="BC30" s="30"/>
       <c r="BD30" s="30"/>
       <c r="BE30" s="30"/>
-      <c r="BF30" s="250" t="s">
+      <c r="BF30" s="259" t="s">
         <v>67</v>
       </c>
-      <c r="BG30" s="250"/>
-      <c r="BH30" s="250"/>
-      <c r="BI30" s="250"/>
-      <c r="BJ30" s="250"/>
-      <c r="BK30" s="250"/>
-      <c r="BL30" s="250"/>
+      <c r="BG30" s="259"/>
+      <c r="BH30" s="259"/>
+      <c r="BI30" s="259"/>
+      <c r="BJ30" s="259"/>
+      <c r="BK30" s="259"/>
+      <c r="BL30" s="259"/>
       <c r="BM30" s="30"/>
       <c r="BN30" s="30"/>
       <c r="BO30" s="30"/>
@@ -10196,77 +10196,77 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="N30:T30"/>
+    <mergeCell ref="J30:M30"/>
     <mergeCell ref="AK30:AL30"/>
     <mergeCell ref="AS30:AY30"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF30:BL30"/>
     <mergeCell ref="AI30:AJ30"/>
     <mergeCell ref="AM30:AR30"/>
-    <mergeCell ref="AC30:AG30"/>
-    <mergeCell ref="X30:AB30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="N30:T30"/>
-    <mergeCell ref="J30:M30"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
-    <cfRule type="duplicateValues" dxfId="19" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C11">
-    <cfRule type="duplicateValues" dxfId="18" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT16:BT23 BT25:BT26">
-    <cfRule type="duplicateValues" dxfId="17" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="16" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT24">
-    <cfRule type="duplicateValues" dxfId="15" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="duplicateValues" dxfId="14" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT27">
-    <cfRule type="duplicateValues" dxfId="13" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BS16">
-    <cfRule type="duplicateValues" dxfId="12" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ20 BS20">
-    <cfRule type="duplicateValues" dxfId="11" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BS22">
-    <cfRule type="duplicateValues" dxfId="10" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ27:BS27">
-    <cfRule type="duplicateValues" dxfId="9" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT28">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ28:BS28">
-    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT29">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ29:BS29">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D16:D29">

</xml_diff>

<commit_message>
Increasing score needed to start a FR (Alien dragon)
Former-commit-id: 34c115ae9829b7208806a8867df9e5a9ec47248d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -2080,6 +2080,90 @@
     <xf numFmtId="49" fontId="0" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2109,90 +2193,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5188,8 +5188,8 @@
   </sheetPr>
   <dimension ref="A1:BT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="Q13" workbookViewId="0">
+      <selection activeCell="AG32" sqref="AG32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5471,10 +5471,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="250"/>
-      <c r="AP14" s="250"/>
-      <c r="AQ14" s="250"/>
-      <c r="AR14" s="250"/>
+      <c r="AO14" s="258"/>
+      <c r="AP14" s="258"/>
+      <c r="AQ14" s="258"/>
+      <c r="AR14" s="258"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -8444,7 +8444,7 @@
       <c r="I29" s="150">
         <v>650</v>
       </c>
-      <c r="J29" s="256">
+      <c r="J29" s="236">
         <v>35</v>
       </c>
       <c r="K29" s="172">
@@ -8459,7 +8459,7 @@
       <c r="N29" s="164">
         <v>550</v>
       </c>
-      <c r="O29" s="257">
+      <c r="O29" s="237">
         <v>650</v>
       </c>
       <c r="P29" s="187">
@@ -8468,10 +8468,10 @@
       <c r="Q29" s="165">
         <v>0</v>
       </c>
-      <c r="R29" s="258">
+      <c r="R29" s="238">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="S29" s="259">
+      <c r="S29" s="239">
         <v>20</v>
       </c>
       <c r="T29" s="183">
@@ -8492,7 +8492,7 @@
       <c r="Y29" s="165">
         <v>100</v>
       </c>
-      <c r="Z29" s="257">
+      <c r="Z29" s="237">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>10</v>
       </c>
       <c r="AG29" s="165">
-        <v>65000</v>
+        <v>75000</v>
       </c>
       <c r="AH29" s="176">
         <v>6</v>
@@ -8523,54 +8523,54 @@
       <c r="AI29" s="164">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AJ29" s="260">
+      <c r="AJ29" s="240">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AK29" s="173">
         <v>0</v>
       </c>
-      <c r="AL29" s="261">
+      <c r="AL29" s="241">
         <v>12</v>
       </c>
-      <c r="AM29" s="262" t="s">
+      <c r="AM29" s="242" t="s">
         <v>248</v>
       </c>
-      <c r="AN29" s="263" t="s">
+      <c r="AN29" s="243" t="s">
         <v>249</v>
       </c>
-      <c r="AO29" s="263" t="s">
+      <c r="AO29" s="243" t="s">
         <v>250</v>
       </c>
-      <c r="AP29" s="264"/>
-      <c r="AQ29" s="264"/>
-      <c r="AR29" s="265" t="s">
+      <c r="AP29" s="244"/>
+      <c r="AQ29" s="244"/>
+      <c r="AR29" s="245" t="s">
         <v>230</v>
       </c>
-      <c r="AS29" s="266">
+      <c r="AS29" s="246">
         <v>1.05</v>
       </c>
-      <c r="AT29" s="267">
+      <c r="AT29" s="247">
         <v>1.5</v>
       </c>
-      <c r="AU29" s="267">
+      <c r="AU29" s="247">
         <v>2</v>
       </c>
-      <c r="AV29" s="267" t="b">
+      <c r="AV29" s="247" t="b">
         <v>1</v>
       </c>
-      <c r="AW29" s="267" t="b">
+      <c r="AW29" s="247" t="b">
         <v>1</v>
       </c>
-      <c r="AX29" s="267" t="b">
+      <c r="AX29" s="247" t="b">
         <v>1</v>
       </c>
-      <c r="AY29" s="268">
+      <c r="AY29" s="248">
         <v>25</v>
       </c>
-      <c r="AZ29" s="267">
+      <c r="AZ29" s="247">
         <v>0.75</v>
       </c>
-      <c r="BA29" s="267">
+      <c r="BA29" s="247">
         <v>0.4</v>
       </c>
       <c r="BB29" s="209" t="s">
@@ -8579,7 +8579,7 @@
       <c r="BC29" s="210" t="s">
         <v>252</v>
       </c>
-      <c r="BD29" s="269">
+      <c r="BD29" s="249">
         <v>1.5E-3</v>
       </c>
       <c r="BE29" s="144">
@@ -8588,7 +8588,7 @@
       <c r="BF29" s="229">
         <v>700</v>
       </c>
-      <c r="BG29" s="270">
+      <c r="BG29" s="250">
         <v>750</v>
       </c>
       <c r="BH29" s="231">
@@ -8618,11 +8618,11 @@
       <c r="BP29" s="232">
         <v>25</v>
       </c>
-      <c r="BQ29" s="271"/>
-      <c r="BR29" s="272">
+      <c r="BQ29" s="251"/>
+      <c r="BR29" s="252">
         <v>0.2</v>
       </c>
-      <c r="BS29" s="273">
+      <c r="BS29" s="253">
         <v>1</v>
       </c>
       <c r="BT29" s="235" t="s">
@@ -8639,83 +8639,83 @@
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="30"/>
-      <c r="J30" s="245" t="s">
+      <c r="J30" s="273" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="245"/>
-      <c r="L30" s="245"/>
-      <c r="M30" s="245"/>
-      <c r="N30" s="242" t="s">
+      <c r="K30" s="273"/>
+      <c r="L30" s="273"/>
+      <c r="M30" s="273"/>
+      <c r="N30" s="270" t="s">
         <v>73</v>
       </c>
-      <c r="O30" s="243"/>
-      <c r="P30" s="243"/>
-      <c r="Q30" s="243"/>
-      <c r="R30" s="244"/>
-      <c r="S30" s="243"/>
-      <c r="T30" s="243"/>
-      <c r="U30" s="240" t="s">
+      <c r="O30" s="271"/>
+      <c r="P30" s="271"/>
+      <c r="Q30" s="271"/>
+      <c r="R30" s="272"/>
+      <c r="S30" s="271"/>
+      <c r="T30" s="271"/>
+      <c r="U30" s="268" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="241"/>
+      <c r="V30" s="269"/>
       <c r="W30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X30" s="237" t="s">
+      <c r="X30" s="265" t="s">
         <v>70</v>
       </c>
-      <c r="Y30" s="238"/>
-      <c r="Z30" s="238"/>
-      <c r="AA30" s="238"/>
-      <c r="AB30" s="239"/>
-      <c r="AC30" s="236" t="s">
+      <c r="Y30" s="266"/>
+      <c r="Z30" s="266"/>
+      <c r="AA30" s="266"/>
+      <c r="AB30" s="267"/>
+      <c r="AC30" s="264" t="s">
         <v>69</v>
       </c>
-      <c r="AD30" s="236"/>
-      <c r="AE30" s="236"/>
-      <c r="AF30" s="236"/>
-      <c r="AG30" s="236"/>
+      <c r="AD30" s="264"/>
+      <c r="AE30" s="264"/>
+      <c r="AF30" s="264"/>
+      <c r="AG30" s="264"/>
       <c r="AH30" s="30"/>
-      <c r="AI30" s="252" t="s">
+      <c r="AI30" s="260" t="s">
         <v>68</v>
       </c>
-      <c r="AJ30" s="252"/>
-      <c r="AK30" s="246" t="s">
+      <c r="AJ30" s="260"/>
+      <c r="AK30" s="254" t="s">
         <v>246</v>
       </c>
-      <c r="AL30" s="246"/>
-      <c r="AM30" s="253" t="s">
+      <c r="AL30" s="254"/>
+      <c r="AM30" s="261" t="s">
         <v>236</v>
       </c>
-      <c r="AN30" s="254"/>
-      <c r="AO30" s="254"/>
-      <c r="AP30" s="254"/>
-      <c r="AQ30" s="254"/>
-      <c r="AR30" s="255"/>
-      <c r="AS30" s="247" t="s">
+      <c r="AN30" s="262"/>
+      <c r="AO30" s="262"/>
+      <c r="AP30" s="262"/>
+      <c r="AQ30" s="262"/>
+      <c r="AR30" s="263"/>
+      <c r="AS30" s="255" t="s">
         <v>226</v>
       </c>
-      <c r="AT30" s="248"/>
-      <c r="AU30" s="248"/>
-      <c r="AV30" s="248"/>
-      <c r="AW30" s="248"/>
-      <c r="AX30" s="248"/>
-      <c r="AY30" s="249"/>
+      <c r="AT30" s="256"/>
+      <c r="AU30" s="256"/>
+      <c r="AV30" s="256"/>
+      <c r="AW30" s="256"/>
+      <c r="AX30" s="256"/>
+      <c r="AY30" s="257"/>
       <c r="AZ30" s="30"/>
       <c r="BA30" s="30"/>
       <c r="BB30" s="30"/>
       <c r="BC30" s="30"/>
       <c r="BD30" s="30"/>
       <c r="BE30" s="30"/>
-      <c r="BF30" s="251" t="s">
+      <c r="BF30" s="259" t="s">
         <v>67</v>
       </c>
-      <c r="BG30" s="251"/>
-      <c r="BH30" s="251"/>
-      <c r="BI30" s="251"/>
-      <c r="BJ30" s="251"/>
-      <c r="BK30" s="251"/>
-      <c r="BL30" s="251"/>
+      <c r="BG30" s="259"/>
+      <c r="BH30" s="259"/>
+      <c r="BI30" s="259"/>
+      <c r="BJ30" s="259"/>
+      <c r="BK30" s="259"/>
+      <c r="BL30" s="259"/>
       <c r="BM30" s="30"/>
       <c r="BN30" s="30"/>
       <c r="BO30" s="30"/>
@@ -10196,17 +10196,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="N30:T30"/>
+    <mergeCell ref="J30:M30"/>
     <mergeCell ref="AK30:AL30"/>
     <mergeCell ref="AS30:AY30"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF30:BL30"/>
     <mergeCell ref="AI30:AJ30"/>
     <mergeCell ref="AM30:AR30"/>
-    <mergeCell ref="AC30:AG30"/>
-    <mergeCell ref="X30:AB30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="N30:T30"/>
-    <mergeCell ref="J30:M30"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="127" priority="22"/>

</xml_diff>

<commit_message>
Reduced from 20Gems to 10Gems cost for Crocodile
Former-commit-id: c7ba484147a314c09d6bb3a3d2e8159dfbea7086
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2134,6 +2134,36 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2162,36 +2192,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5188,8 +5188,8 @@
   </sheetPr>
   <dimension ref="A1:BT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q13" workbookViewId="0">
-      <selection activeCell="AG32" sqref="AG32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5471,10 +5471,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="258"/>
-      <c r="AP14" s="258"/>
-      <c r="AQ14" s="258"/>
-      <c r="AR14" s="258"/>
+      <c r="AO14" s="268"/>
+      <c r="AP14" s="268"/>
+      <c r="AQ14" s="268"/>
+      <c r="AR14" s="268"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -5922,7 +5922,7 @@
         <v>2000</v>
       </c>
       <c r="I17" s="148">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J17" s="157">
         <v>35</v>
@@ -8639,83 +8639,83 @@
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="30"/>
-      <c r="J30" s="273" t="s">
+      <c r="J30" s="263" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="273"/>
-      <c r="L30" s="273"/>
-      <c r="M30" s="273"/>
-      <c r="N30" s="270" t="s">
+      <c r="K30" s="263"/>
+      <c r="L30" s="263"/>
+      <c r="M30" s="263"/>
+      <c r="N30" s="260" t="s">
         <v>73</v>
       </c>
-      <c r="O30" s="271"/>
-      <c r="P30" s="271"/>
-      <c r="Q30" s="271"/>
-      <c r="R30" s="272"/>
-      <c r="S30" s="271"/>
-      <c r="T30" s="271"/>
-      <c r="U30" s="268" t="s">
+      <c r="O30" s="261"/>
+      <c r="P30" s="261"/>
+      <c r="Q30" s="261"/>
+      <c r="R30" s="262"/>
+      <c r="S30" s="261"/>
+      <c r="T30" s="261"/>
+      <c r="U30" s="258" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="269"/>
+      <c r="V30" s="259"/>
       <c r="W30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X30" s="265" t="s">
+      <c r="X30" s="255" t="s">
         <v>70</v>
       </c>
-      <c r="Y30" s="266"/>
-      <c r="Z30" s="266"/>
-      <c r="AA30" s="266"/>
-      <c r="AB30" s="267"/>
-      <c r="AC30" s="264" t="s">
+      <c r="Y30" s="256"/>
+      <c r="Z30" s="256"/>
+      <c r="AA30" s="256"/>
+      <c r="AB30" s="257"/>
+      <c r="AC30" s="254" t="s">
         <v>69</v>
       </c>
-      <c r="AD30" s="264"/>
-      <c r="AE30" s="264"/>
-      <c r="AF30" s="264"/>
-      <c r="AG30" s="264"/>
+      <c r="AD30" s="254"/>
+      <c r="AE30" s="254"/>
+      <c r="AF30" s="254"/>
+      <c r="AG30" s="254"/>
       <c r="AH30" s="30"/>
-      <c r="AI30" s="260" t="s">
+      <c r="AI30" s="270" t="s">
         <v>68</v>
       </c>
-      <c r="AJ30" s="260"/>
-      <c r="AK30" s="254" t="s">
+      <c r="AJ30" s="270"/>
+      <c r="AK30" s="264" t="s">
         <v>246</v>
       </c>
-      <c r="AL30" s="254"/>
-      <c r="AM30" s="261" t="s">
+      <c r="AL30" s="264"/>
+      <c r="AM30" s="271" t="s">
         <v>236</v>
       </c>
-      <c r="AN30" s="262"/>
-      <c r="AO30" s="262"/>
-      <c r="AP30" s="262"/>
-      <c r="AQ30" s="262"/>
-      <c r="AR30" s="263"/>
-      <c r="AS30" s="255" t="s">
+      <c r="AN30" s="272"/>
+      <c r="AO30" s="272"/>
+      <c r="AP30" s="272"/>
+      <c r="AQ30" s="272"/>
+      <c r="AR30" s="273"/>
+      <c r="AS30" s="265" t="s">
         <v>226</v>
       </c>
-      <c r="AT30" s="256"/>
-      <c r="AU30" s="256"/>
-      <c r="AV30" s="256"/>
-      <c r="AW30" s="256"/>
-      <c r="AX30" s="256"/>
-      <c r="AY30" s="257"/>
+      <c r="AT30" s="266"/>
+      <c r="AU30" s="266"/>
+      <c r="AV30" s="266"/>
+      <c r="AW30" s="266"/>
+      <c r="AX30" s="266"/>
+      <c r="AY30" s="267"/>
       <c r="AZ30" s="30"/>
       <c r="BA30" s="30"/>
       <c r="BB30" s="30"/>
       <c r="BC30" s="30"/>
       <c r="BD30" s="30"/>
       <c r="BE30" s="30"/>
-      <c r="BF30" s="259" t="s">
+      <c r="BF30" s="269" t="s">
         <v>67</v>
       </c>
-      <c r="BG30" s="259"/>
-      <c r="BH30" s="259"/>
-      <c r="BI30" s="259"/>
-      <c r="BJ30" s="259"/>
-      <c r="BK30" s="259"/>
-      <c r="BL30" s="259"/>
+      <c r="BG30" s="269"/>
+      <c r="BH30" s="269"/>
+      <c r="BI30" s="269"/>
+      <c r="BJ30" s="269"/>
+      <c r="BK30" s="269"/>
+      <c r="BL30" s="269"/>
       <c r="BM30" s="30"/>
       <c r="BN30" s="30"/>
       <c r="BO30" s="30"/>
@@ -10196,17 +10196,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC30:AG30"/>
-    <mergeCell ref="X30:AB30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="N30:T30"/>
-    <mergeCell ref="J30:M30"/>
     <mergeCell ref="AK30:AL30"/>
     <mergeCell ref="AS30:AY30"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF30:BL30"/>
     <mergeCell ref="AI30:AJ30"/>
     <mergeCell ref="AM30:AR30"/>
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="N30:T30"/>
+    <mergeCell ref="J30:M30"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="127" priority="22"/>

</xml_diff>

<commit_message>
All dragons get unlocked when getting Blaze!
Former-commit-id: 435644aaafb0dbead997ccd17a6282280d0244d6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1417,7 +1417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="274">
+  <cellXfs count="272">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1725,9 +1725,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2107,9 +2104,6 @@
     <xf numFmtId="0" fontId="8" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2133,6 +2127,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2162,36 +2186,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5188,8 +5182,8 @@
   </sheetPr>
   <dimension ref="A1:BT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q13" workbookViewId="0">
-      <selection activeCell="AG32" sqref="AG32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5382,13 +5376,13 @@
       </c>
     </row>
     <row r="10" spans="2:72" x14ac:dyDescent="0.25">
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="120" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="82" t="s">
         <v>227</v>
       </c>
-      <c r="D10" s="122">
+      <c r="D10" s="121">
         <v>5</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -5397,18 +5391,18 @@
       <c r="F10" s="15">
         <v>4</v>
       </c>
-      <c r="G10" s="120" t="s">
+      <c r="G10" s="119" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="11" spans="2:72" x14ac:dyDescent="0.25">
-      <c r="B11" s="136" t="s">
+      <c r="B11" s="135" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="82" t="s">
         <v>238</v>
       </c>
-      <c r="D11" s="122">
+      <c r="D11" s="121">
         <v>6</v>
       </c>
       <c r="E11" s="15" t="s">
@@ -5417,7 +5411,7 @@
       <c r="F11" s="15">
         <v>0</v>
       </c>
-      <c r="G11" s="120" t="s">
+      <c r="G11" s="119" t="s">
         <v>240</v>
       </c>
     </row>
@@ -5471,10 +5465,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="258"/>
-      <c r="AP14" s="258"/>
-      <c r="AQ14" s="258"/>
-      <c r="AR14" s="258"/>
+      <c r="AO14" s="266"/>
+      <c r="AP14" s="266"/>
+      <c r="AQ14" s="266"/>
+      <c r="AR14" s="266"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -5624,7 +5618,7 @@
       <c r="AX15" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="AY15" s="117" t="s">
+      <c r="AY15" s="116" t="s">
         <v>132</v>
       </c>
       <c r="AZ15" s="70" t="s">
@@ -5796,19 +5790,19 @@
       <c r="AJ16" s="56">
         <v>0.19</v>
       </c>
-      <c r="AK16" s="124">
+      <c r="AK16" s="123">
         <v>0</v>
       </c>
       <c r="AL16" s="58">
         <v>12</v>
       </c>
-      <c r="AM16" s="126" t="s">
+      <c r="AM16" s="125" t="s">
         <v>120</v>
       </c>
-      <c r="AN16" s="126" t="s">
+      <c r="AN16" s="125" t="s">
         <v>119</v>
       </c>
-      <c r="AO16" s="126" t="s">
+      <c r="AO16" s="125" t="s">
         <v>217</v>
       </c>
       <c r="AP16" s="92"/>
@@ -5832,10 +5826,10 @@
       <c r="AX16" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AY16" s="118">
+      <c r="AY16" s="117">
         <v>25</v>
       </c>
-      <c r="AZ16" s="116">
+      <c r="AZ16" s="115">
         <v>0.55999999999999994</v>
       </c>
       <c r="BA16" s="101">
@@ -5900,420 +5894,420 @@
       </c>
     </row>
     <row r="17" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="B17" s="137" t="s">
+      <c r="B17" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="138" t="s">
+      <c r="C17" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="138" t="s">
+      <c r="D17" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="138" t="s">
+      <c r="E17" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="F17" s="143">
+      <c r="F17" s="142">
         <v>1</v>
       </c>
-      <c r="G17" s="144" t="s">
+      <c r="G17" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="147">
+      <c r="H17" s="146">
         <v>2000</v>
       </c>
-      <c r="I17" s="148">
+      <c r="I17" s="147">
         <v>20</v>
       </c>
-      <c r="J17" s="157">
+      <c r="J17" s="156">
         <v>35</v>
       </c>
-      <c r="K17" s="158">
+      <c r="K17" s="157">
         <v>45</v>
       </c>
-      <c r="L17" s="159">
+      <c r="L17" s="158">
         <v>3</v>
       </c>
-      <c r="M17" s="160">
+      <c r="M17" s="159">
         <v>-2</v>
       </c>
-      <c r="N17" s="161">
+      <c r="N17" s="160">
         <v>95</v>
       </c>
-      <c r="O17" s="162">
+      <c r="O17" s="161">
         <v>145</v>
       </c>
-      <c r="P17" s="162">
+      <c r="P17" s="161">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q17" s="162">
+      <c r="Q17" s="161">
         <v>0</v>
       </c>
-      <c r="R17" s="162">
+      <c r="R17" s="161">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="S17" s="163">
+      <c r="S17" s="162">
         <v>30</v>
       </c>
-      <c r="T17" s="163">
+      <c r="T17" s="162">
         <v>0.5</v>
       </c>
-      <c r="U17" s="164">
+      <c r="U17" s="163">
         <v>0.8</v>
       </c>
-      <c r="V17" s="165">
+      <c r="V17" s="164">
         <v>0.95</v>
       </c>
-      <c r="W17" s="157">
+      <c r="W17" s="156">
         <v>16</v>
       </c>
-      <c r="X17" s="161">
+      <c r="X17" s="160">
         <v>1.75</v>
       </c>
-      <c r="Y17" s="162">
+      <c r="Y17" s="161">
         <v>100</v>
       </c>
-      <c r="Z17" s="162">
+      <c r="Z17" s="161">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA17" s="162">
+      <c r="AA17" s="161">
         <v>20</v>
       </c>
-      <c r="AB17" s="162">
+      <c r="AB17" s="161">
         <v>10</v>
       </c>
-      <c r="AC17" s="166">
+      <c r="AC17" s="165">
         <v>275</v>
       </c>
-      <c r="AD17" s="163">
+      <c r="AD17" s="162">
         <v>8</v>
       </c>
-      <c r="AE17" s="162">
+      <c r="AE17" s="161">
         <v>3</v>
       </c>
-      <c r="AF17" s="163">
+      <c r="AF17" s="162">
         <v>9</v>
       </c>
-      <c r="AG17" s="162">
+      <c r="AG17" s="161">
         <v>7000</v>
       </c>
-      <c r="AH17" s="167">
+      <c r="AH17" s="166">
         <v>2</v>
       </c>
-      <c r="AI17" s="168">
+      <c r="AI17" s="167">
         <v>0.19</v>
       </c>
-      <c r="AJ17" s="169">
+      <c r="AJ17" s="168">
         <v>0.15</v>
       </c>
-      <c r="AK17" s="170">
+      <c r="AK17" s="169">
         <v>0</v>
       </c>
-      <c r="AL17" s="158">
+      <c r="AL17" s="157">
         <v>12</v>
       </c>
-      <c r="AM17" s="191" t="s">
+      <c r="AM17" s="190" t="s">
         <v>116</v>
       </c>
-      <c r="AN17" s="192" t="s">
+      <c r="AN17" s="191" t="s">
         <v>115</v>
       </c>
-      <c r="AO17" s="192" t="s">
+      <c r="AO17" s="191" t="s">
         <v>218</v>
       </c>
-      <c r="AP17" s="193"/>
-      <c r="AQ17" s="193"/>
-      <c r="AR17" s="194"/>
-      <c r="AS17" s="195">
+      <c r="AP17" s="192"/>
+      <c r="AQ17" s="192"/>
+      <c r="AR17" s="193"/>
+      <c r="AS17" s="194">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AT17" s="196">
+      <c r="AT17" s="195">
         <v>2</v>
       </c>
-      <c r="AU17" s="196">
+      <c r="AU17" s="195">
         <v>2</v>
       </c>
-      <c r="AV17" s="196" t="b">
+      <c r="AV17" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AW17" s="196" t="b">
+      <c r="AW17" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AX17" s="196" t="b">
+      <c r="AX17" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AY17" s="197">
+      <c r="AY17" s="196">
         <v>25</v>
       </c>
-      <c r="AZ17" s="198">
+      <c r="AZ17" s="197">
         <v>0.7</v>
       </c>
-      <c r="BA17" s="194">
+      <c r="BA17" s="193">
         <v>0.8</v>
       </c>
-      <c r="BB17" s="153" t="s">
+      <c r="BB17" s="152" t="s">
         <v>114</v>
       </c>
-      <c r="BC17" s="154" t="s">
+      <c r="BC17" s="153" t="s">
         <v>113</v>
       </c>
-      <c r="BD17" s="211">
+      <c r="BD17" s="210">
         <v>2.3E-3</v>
       </c>
-      <c r="BE17" s="212">
+      <c r="BE17" s="211">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF17" s="215">
+      <c r="BF17" s="214">
         <v>210</v>
       </c>
-      <c r="BG17" s="216">
+      <c r="BG17" s="215">
         <v>235</v>
       </c>
-      <c r="BH17" s="138">
+      <c r="BH17" s="137">
         <v>2.1</v>
       </c>
-      <c r="BI17" s="138">
+      <c r="BI17" s="137">
         <v>9.5</v>
       </c>
-      <c r="BJ17" s="138">
+      <c r="BJ17" s="137">
         <v>1.7</v>
       </c>
-      <c r="BK17" s="138">
+      <c r="BK17" s="137">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BL17" s="217">
+      <c r="BL17" s="216">
         <v>2.1</v>
       </c>
-      <c r="BM17" s="215">
+      <c r="BM17" s="214">
         <v>0</v>
       </c>
-      <c r="BN17" s="138">
+      <c r="BN17" s="137">
         <v>8</v>
       </c>
-      <c r="BO17" s="218">
+      <c r="BO17" s="217">
         <v>0.4</v>
       </c>
-      <c r="BP17" s="218">
+      <c r="BP17" s="217">
         <v>25</v>
       </c>
-      <c r="BQ17" s="138"/>
-      <c r="BR17" s="138">
+      <c r="BQ17" s="137"/>
+      <c r="BR17" s="137">
         <v>0.2</v>
       </c>
-      <c r="BS17" s="219">
+      <c r="BS17" s="218">
         <v>1</v>
       </c>
-      <c r="BT17" s="215" t="s">
+      <c r="BT17" s="214" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="B18" s="139" t="s">
+      <c r="B18" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="140" t="s">
+      <c r="C18" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="140" t="s">
+      <c r="D18" s="139" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="138" t="s">
+      <c r="E18" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="F18" s="143">
+      <c r="F18" s="142">
         <v>2</v>
       </c>
-      <c r="G18" s="143" t="s">
+      <c r="G18" s="142" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="149">
+      <c r="H18" s="148">
         <v>11000</v>
       </c>
-      <c r="I18" s="150">
+      <c r="I18" s="149">
         <v>35</v>
       </c>
-      <c r="J18" s="171">
+      <c r="J18" s="170">
         <v>35</v>
       </c>
-      <c r="K18" s="172">
+      <c r="K18" s="171">
         <v>45</v>
       </c>
-      <c r="L18" s="159">
+      <c r="L18" s="158">
         <v>5</v>
       </c>
-      <c r="M18" s="160">
+      <c r="M18" s="159">
         <v>-2</v>
       </c>
-      <c r="N18" s="161">
+      <c r="N18" s="160">
         <v>140</v>
       </c>
-      <c r="O18" s="165">
+      <c r="O18" s="164">
         <v>200</v>
       </c>
-      <c r="P18" s="165">
+      <c r="P18" s="164">
         <v>1.5</v>
       </c>
-      <c r="Q18" s="165">
+      <c r="Q18" s="164">
         <v>0</v>
       </c>
-      <c r="R18" s="162">
+      <c r="R18" s="161">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="S18" s="163">
+      <c r="S18" s="162">
         <v>30</v>
       </c>
-      <c r="T18" s="163">
+      <c r="T18" s="162">
         <v>0.5</v>
       </c>
-      <c r="U18" s="161">
+      <c r="U18" s="160">
         <v>0.85</v>
       </c>
-      <c r="V18" s="162">
+      <c r="V18" s="161">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W18" s="171">
+      <c r="W18" s="170">
         <v>23.5</v>
       </c>
-      <c r="X18" s="161">
+      <c r="X18" s="160">
         <v>2.0099999999999998</v>
       </c>
-      <c r="Y18" s="162">
+      <c r="Y18" s="161">
         <v>100</v>
       </c>
-      <c r="Z18" s="162">
+      <c r="Z18" s="161">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA18" s="162">
+      <c r="AA18" s="161">
         <v>40</v>
       </c>
-      <c r="AB18" s="162">
+      <c r="AB18" s="161">
         <v>14</v>
       </c>
-      <c r="AC18" s="173">
+      <c r="AC18" s="172">
         <v>300</v>
       </c>
-      <c r="AD18" s="163">
+      <c r="AD18" s="162">
         <v>9</v>
       </c>
-      <c r="AE18" s="165">
+      <c r="AE18" s="164">
         <v>3</v>
       </c>
-      <c r="AF18" s="174">
+      <c r="AF18" s="173">
         <v>9</v>
       </c>
-      <c r="AG18" s="162">
+      <c r="AG18" s="161">
         <v>8000</v>
       </c>
-      <c r="AH18" s="175">
+      <c r="AH18" s="174">
         <v>2</v>
       </c>
-      <c r="AI18" s="176">
+      <c r="AI18" s="175">
         <v>0.15</v>
       </c>
-      <c r="AJ18" s="169">
+      <c r="AJ18" s="168">
         <v>0.13</v>
       </c>
-      <c r="AK18" s="177">
+      <c r="AK18" s="176">
         <v>0</v>
       </c>
-      <c r="AL18" s="178">
+      <c r="AL18" s="177">
         <v>12</v>
       </c>
-      <c r="AM18" s="191" t="s">
+      <c r="AM18" s="190" t="s">
         <v>112</v>
       </c>
-      <c r="AN18" s="192" t="s">
+      <c r="AN18" s="191" t="s">
         <v>111</v>
       </c>
-      <c r="AO18" s="192" t="s">
+      <c r="AO18" s="191" t="s">
         <v>110</v>
       </c>
-      <c r="AP18" s="193"/>
-      <c r="AQ18" s="193"/>
-      <c r="AR18" s="194"/>
-      <c r="AS18" s="195">
+      <c r="AP18" s="192"/>
+      <c r="AQ18" s="192"/>
+      <c r="AR18" s="193"/>
+      <c r="AS18" s="194">
         <v>2.1</v>
       </c>
-      <c r="AT18" s="196">
+      <c r="AT18" s="195">
         <v>2</v>
       </c>
-      <c r="AU18" s="196">
+      <c r="AU18" s="195">
         <v>2</v>
       </c>
-      <c r="AV18" s="196" t="b">
+      <c r="AV18" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AW18" s="196" t="b">
+      <c r="AW18" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AX18" s="196" t="b">
+      <c r="AX18" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AY18" s="197">
+      <c r="AY18" s="196">
         <v>25</v>
       </c>
-      <c r="AZ18" s="198">
+      <c r="AZ18" s="197">
         <v>0.7</v>
       </c>
-      <c r="BA18" s="194">
+      <c r="BA18" s="193">
         <v>0.7</v>
       </c>
-      <c r="BB18" s="155" t="s">
+      <c r="BB18" s="154" t="s">
         <v>109</v>
       </c>
-      <c r="BC18" s="156" t="s">
+      <c r="BC18" s="155" t="s">
         <v>108</v>
       </c>
-      <c r="BD18" s="211">
+      <c r="BD18" s="210">
         <v>2E-3</v>
       </c>
-      <c r="BE18" s="212">
+      <c r="BE18" s="211">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF18" s="215">
+      <c r="BF18" s="214">
         <v>240</v>
       </c>
-      <c r="BG18" s="216">
+      <c r="BG18" s="215">
         <v>280</v>
       </c>
-      <c r="BH18" s="138">
+      <c r="BH18" s="137">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BI18" s="138">
+      <c r="BI18" s="137">
         <v>9.5</v>
       </c>
-      <c r="BJ18" s="138">
+      <c r="BJ18" s="137">
         <v>1.7</v>
       </c>
-      <c r="BK18" s="138">
+      <c r="BK18" s="137">
         <v>0.9</v>
       </c>
-      <c r="BL18" s="217">
+      <c r="BL18" s="216">
         <v>2.25</v>
       </c>
-      <c r="BM18" s="215">
+      <c r="BM18" s="214">
         <v>0</v>
       </c>
-      <c r="BN18" s="138">
+      <c r="BN18" s="137">
         <v>8</v>
       </c>
-      <c r="BO18" s="218">
+      <c r="BO18" s="217">
         <v>0.4</v>
       </c>
-      <c r="BP18" s="218">
+      <c r="BP18" s="217">
         <v>25</v>
       </c>
-      <c r="BQ18" s="138" t="s">
+      <c r="BQ18" s="137" t="s">
         <v>212</v>
       </c>
-      <c r="BR18" s="138">
+      <c r="BR18" s="137">
         <v>0.2</v>
       </c>
-      <c r="BS18" s="220">
+      <c r="BS18" s="219">
         <v>1</v>
       </c>
-      <c r="BT18" s="221" t="s">
+      <c r="BT18" s="220" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6424,19 +6418,19 @@
       <c r="AJ19" s="56">
         <v>0.11</v>
       </c>
-      <c r="AK19" s="124">
+      <c r="AK19" s="123">
         <v>0</v>
       </c>
       <c r="AL19" s="58">
         <v>12</v>
       </c>
-      <c r="AM19" s="127" t="s">
+      <c r="AM19" s="126" t="s">
         <v>106</v>
       </c>
-      <c r="AN19" s="126" t="s">
+      <c r="AN19" s="125" t="s">
         <v>105</v>
       </c>
-      <c r="AO19" s="126" t="s">
+      <c r="AO19" s="125" t="s">
         <v>219</v>
       </c>
       <c r="AP19" s="92"/>
@@ -6460,10 +6454,10 @@
       <c r="AX19" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AY19" s="118">
+      <c r="AY19" s="117">
         <v>25</v>
       </c>
-      <c r="AZ19" s="116">
+      <c r="AZ19" s="115">
         <v>0.7</v>
       </c>
       <c r="BA19" s="101">
@@ -6518,10 +6512,10 @@
       <c r="BR19" s="49">
         <v>0.2</v>
       </c>
-      <c r="BS19" s="133">
+      <c r="BS19" s="132">
         <v>1</v>
       </c>
-      <c r="BT19" s="132" t="s">
+      <c r="BT19" s="131" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6632,19 +6626,19 @@
       <c r="AJ20" s="56">
         <v>0.09</v>
       </c>
-      <c r="AK20" s="124">
+      <c r="AK20" s="123">
         <v>0</v>
       </c>
       <c r="AL20" s="58">
         <v>12</v>
       </c>
-      <c r="AM20" s="127" t="s">
+      <c r="AM20" s="126" t="s">
         <v>102</v>
       </c>
-      <c r="AN20" s="126" t="s">
+      <c r="AN20" s="125" t="s">
         <v>101</v>
       </c>
-      <c r="AO20" s="126" t="s">
+      <c r="AO20" s="125" t="s">
         <v>220</v>
       </c>
       <c r="AP20" s="92"/>
@@ -6668,10 +6662,10 @@
       <c r="AX20" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AY20" s="118">
+      <c r="AY20" s="117">
         <v>25</v>
       </c>
-      <c r="AZ20" s="116">
+      <c r="AZ20" s="115">
         <v>0.7</v>
       </c>
       <c r="BA20" s="101">
@@ -6722,16 +6716,16 @@
       <c r="BP20" s="61">
         <v>25</v>
       </c>
-      <c r="BQ20" s="130" t="s">
+      <c r="BQ20" s="129" t="s">
         <v>209</v>
       </c>
-      <c r="BR20" s="131">
+      <c r="BR20" s="130">
         <v>0.2</v>
       </c>
-      <c r="BS20" s="134">
+      <c r="BS20" s="133">
         <v>1</v>
       </c>
-      <c r="BT20" s="132" t="s">
+      <c r="BT20" s="131" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6842,19 +6836,19 @@
       <c r="AJ21" s="56">
         <v>0.08</v>
       </c>
-      <c r="AK21" s="124">
+      <c r="AK21" s="123">
         <v>0</v>
       </c>
       <c r="AL21" s="58">
         <v>12</v>
       </c>
-      <c r="AM21" s="127" t="s">
+      <c r="AM21" s="126" t="s">
         <v>98</v>
       </c>
-      <c r="AN21" s="126" t="s">
+      <c r="AN21" s="125" t="s">
         <v>97</v>
       </c>
-      <c r="AO21" s="126" t="s">
+      <c r="AO21" s="125" t="s">
         <v>96</v>
       </c>
       <c r="AP21" s="92"/>
@@ -6878,10 +6872,10 @@
       <c r="AX21" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AY21" s="118">
+      <c r="AY21" s="117">
         <v>25</v>
       </c>
-      <c r="AZ21" s="116">
+      <c r="AZ21" s="115">
         <v>0.7</v>
       </c>
       <c r="BA21" s="101">
@@ -6938,640 +6932,640 @@
       <c r="BR21" s="49">
         <v>0.2</v>
       </c>
-      <c r="BS21" s="133">
+      <c r="BS21" s="132">
         <v>1</v>
       </c>
-      <c r="BT21" s="132" t="s">
+      <c r="BT21" s="131" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="B22" s="139" t="s">
+      <c r="B22" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="140" t="s">
+      <c r="C22" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="138" t="s">
+      <c r="D22" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="138" t="s">
+      <c r="E22" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="F22" s="143">
+      <c r="F22" s="142">
         <v>6</v>
       </c>
-      <c r="G22" s="144" t="s">
+      <c r="G22" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="147">
+      <c r="H22" s="146">
         <v>480000</v>
       </c>
-      <c r="I22" s="148">
+      <c r="I22" s="147">
         <v>100</v>
       </c>
-      <c r="J22" s="157">
+      <c r="J22" s="156">
         <v>35</v>
       </c>
-      <c r="K22" s="158">
+      <c r="K22" s="157">
         <v>45</v>
       </c>
-      <c r="L22" s="159">
+      <c r="L22" s="158">
         <v>12.5</v>
       </c>
-      <c r="M22" s="160">
+      <c r="M22" s="159">
         <v>0</v>
       </c>
-      <c r="N22" s="161">
+      <c r="N22" s="160">
         <v>290</v>
       </c>
-      <c r="O22" s="162">
+      <c r="O22" s="161">
         <v>350</v>
       </c>
-      <c r="P22" s="162">
+      <c r="P22" s="161">
         <v>2.1</v>
       </c>
-      <c r="Q22" s="162">
+      <c r="Q22" s="161">
         <v>0</v>
       </c>
-      <c r="R22" s="162">
+      <c r="R22" s="161">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="S22" s="163">
+      <c r="S22" s="162">
         <v>25</v>
       </c>
-      <c r="T22" s="163">
+      <c r="T22" s="162">
         <v>0.6</v>
       </c>
-      <c r="U22" s="161">
+      <c r="U22" s="160">
         <v>1.35</v>
       </c>
-      <c r="V22" s="162">
+      <c r="V22" s="161">
         <v>1.55</v>
       </c>
-      <c r="W22" s="157">
+      <c r="W22" s="156">
         <v>23.5</v>
       </c>
-      <c r="X22" s="161">
+      <c r="X22" s="160">
         <v>1.5</v>
       </c>
-      <c r="Y22" s="162">
+      <c r="Y22" s="161">
         <v>100</v>
       </c>
-      <c r="Z22" s="162">
+      <c r="Z22" s="161">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA22" s="162">
+      <c r="AA22" s="161">
         <v>29</v>
       </c>
-      <c r="AB22" s="162">
+      <c r="AB22" s="161">
         <v>17</v>
       </c>
-      <c r="AC22" s="166">
+      <c r="AC22" s="165">
         <v>400</v>
       </c>
-      <c r="AD22" s="163">
+      <c r="AD22" s="162">
         <v>11</v>
       </c>
-      <c r="AE22" s="162">
+      <c r="AE22" s="161">
         <v>5</v>
       </c>
-      <c r="AF22" s="163">
+      <c r="AF22" s="162">
         <v>10</v>
       </c>
-      <c r="AG22" s="162">
+      <c r="AG22" s="161">
         <v>10000</v>
       </c>
-      <c r="AH22" s="167">
+      <c r="AH22" s="166">
         <v>3</v>
       </c>
-      <c r="AI22" s="168">
+      <c r="AI22" s="167">
         <v>0.08</v>
       </c>
-      <c r="AJ22" s="169">
+      <c r="AJ22" s="168">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK22" s="170">
+      <c r="AK22" s="169">
         <v>0</v>
       </c>
-      <c r="AL22" s="158">
+      <c r="AL22" s="157">
         <v>12</v>
       </c>
-      <c r="AM22" s="191" t="s">
+      <c r="AM22" s="190" t="s">
         <v>92</v>
       </c>
-      <c r="AN22" s="192" t="s">
+      <c r="AN22" s="191" t="s">
         <v>91</v>
       </c>
-      <c r="AO22" s="192" t="s">
+      <c r="AO22" s="191" t="s">
         <v>221</v>
       </c>
-      <c r="AP22" s="193"/>
-      <c r="AQ22" s="193"/>
-      <c r="AR22" s="194"/>
-      <c r="AS22" s="195">
+      <c r="AP22" s="192"/>
+      <c r="AQ22" s="192"/>
+      <c r="AR22" s="193"/>
+      <c r="AS22" s="194">
         <v>1.6</v>
       </c>
-      <c r="AT22" s="196">
+      <c r="AT22" s="195">
         <v>2</v>
       </c>
-      <c r="AU22" s="196">
+      <c r="AU22" s="195">
         <v>2</v>
       </c>
-      <c r="AV22" s="196" t="b">
+      <c r="AV22" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AW22" s="196" t="b">
+      <c r="AW22" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AX22" s="196" t="b">
+      <c r="AX22" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AY22" s="197">
+      <c r="AY22" s="196">
         <v>25</v>
       </c>
-      <c r="AZ22" s="198">
+      <c r="AZ22" s="197">
         <v>0.7</v>
       </c>
-      <c r="BA22" s="194">
+      <c r="BA22" s="193">
         <v>0.5</v>
       </c>
-      <c r="BB22" s="155" t="s">
+      <c r="BB22" s="154" t="s">
         <v>90</v>
       </c>
-      <c r="BC22" s="156" t="s">
+      <c r="BC22" s="155" t="s">
         <v>89</v>
       </c>
-      <c r="BD22" s="211">
+      <c r="BD22" s="210">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="BE22" s="212">
+      <c r="BE22" s="211">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF22" s="215">
+      <c r="BF22" s="214">
         <v>343</v>
       </c>
-      <c r="BG22" s="216">
+      <c r="BG22" s="215">
         <v>372</v>
       </c>
-      <c r="BH22" s="138">
+      <c r="BH22" s="137">
         <v>2.6</v>
       </c>
-      <c r="BI22" s="138">
+      <c r="BI22" s="137">
         <v>9.5</v>
       </c>
-      <c r="BJ22" s="138">
+      <c r="BJ22" s="137">
         <v>1.7</v>
       </c>
-      <c r="BK22" s="138">
+      <c r="BK22" s="137">
         <v>0.5</v>
       </c>
-      <c r="BL22" s="217">
+      <c r="BL22" s="216">
         <v>0.9</v>
       </c>
-      <c r="BM22" s="215">
+      <c r="BM22" s="214">
         <v>9</v>
       </c>
-      <c r="BN22" s="138">
+      <c r="BN22" s="137">
         <v>8</v>
       </c>
-      <c r="BO22" s="218">
+      <c r="BO22" s="217">
         <v>0.4</v>
       </c>
-      <c r="BP22" s="218">
+      <c r="BP22" s="217">
         <v>25</v>
       </c>
-      <c r="BQ22" s="225" t="s">
+      <c r="BQ22" s="224" t="s">
         <v>210</v>
       </c>
-      <c r="BR22" s="226">
+      <c r="BR22" s="225">
         <v>0.2</v>
       </c>
-      <c r="BS22" s="227">
+      <c r="BS22" s="226">
         <v>1</v>
       </c>
-      <c r="BT22" s="221" t="s">
+      <c r="BT22" s="220" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="B23" s="139" t="s">
+      <c r="B23" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="140" t="s">
+      <c r="C23" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="140" t="s">
+      <c r="D23" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="138" t="s">
+      <c r="E23" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="F23" s="143">
+      <c r="F23" s="142">
         <v>7</v>
       </c>
-      <c r="G23" s="144" t="s">
+      <c r="G23" s="143" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="149">
+      <c r="H23" s="148">
         <v>530000</v>
       </c>
-      <c r="I23" s="150">
+      <c r="I23" s="149">
         <v>140</v>
       </c>
-      <c r="J23" s="171">
+      <c r="J23" s="170">
         <v>35</v>
       </c>
-      <c r="K23" s="172">
+      <c r="K23" s="171">
         <v>45</v>
       </c>
-      <c r="L23" s="159">
+      <c r="L23" s="158">
         <v>17</v>
       </c>
-      <c r="M23" s="160">
+      <c r="M23" s="159">
         <v>0</v>
       </c>
-      <c r="N23" s="161">
+      <c r="N23" s="160">
         <v>330</v>
       </c>
-      <c r="O23" s="162">
+      <c r="O23" s="161">
         <v>400</v>
       </c>
-      <c r="P23" s="162">
+      <c r="P23" s="161">
         <v>2.2999999999999998</v>
       </c>
-      <c r="Q23" s="162">
+      <c r="Q23" s="161">
         <v>0</v>
       </c>
-      <c r="R23" s="162">
+      <c r="R23" s="161">
         <v>1.4E-2</v>
       </c>
-      <c r="S23" s="163">
+      <c r="S23" s="162">
         <v>25</v>
       </c>
-      <c r="T23" s="163">
+      <c r="T23" s="162">
         <v>0.7</v>
       </c>
-      <c r="U23" s="161">
+      <c r="U23" s="160">
         <v>1.44</v>
       </c>
-      <c r="V23" s="162">
+      <c r="V23" s="161">
         <v>1.64</v>
       </c>
-      <c r="W23" s="171">
+      <c r="W23" s="170">
         <v>25</v>
       </c>
-      <c r="X23" s="161">
+      <c r="X23" s="160">
         <v>1.4</v>
       </c>
-      <c r="Y23" s="162">
+      <c r="Y23" s="161">
         <v>100</v>
       </c>
-      <c r="Z23" s="162">
+      <c r="Z23" s="161">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA23" s="162">
+      <c r="AA23" s="161">
         <v>20</v>
       </c>
-      <c r="AB23" s="162">
+      <c r="AB23" s="161">
         <v>18</v>
       </c>
-      <c r="AC23" s="173">
+      <c r="AC23" s="172">
         <v>425</v>
       </c>
-      <c r="AD23" s="163">
+      <c r="AD23" s="162">
         <v>11.5</v>
       </c>
-      <c r="AE23" s="165">
+      <c r="AE23" s="164">
         <v>5</v>
       </c>
-      <c r="AF23" s="174">
+      <c r="AF23" s="173">
         <v>10</v>
       </c>
-      <c r="AG23" s="162">
+      <c r="AG23" s="161">
         <v>16000</v>
       </c>
-      <c r="AH23" s="175">
+      <c r="AH23" s="174">
         <v>4</v>
       </c>
-      <c r="AI23" s="176">
+      <c r="AI23" s="175">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AJ23" s="169">
+      <c r="AJ23" s="168">
         <v>0.06</v>
       </c>
-      <c r="AK23" s="177">
+      <c r="AK23" s="176">
         <v>0</v>
       </c>
-      <c r="AL23" s="178">
+      <c r="AL23" s="177">
         <v>12</v>
       </c>
-      <c r="AM23" s="191" t="s">
+      <c r="AM23" s="190" t="s">
         <v>88</v>
       </c>
-      <c r="AN23" s="192" t="s">
+      <c r="AN23" s="191" t="s">
         <v>87</v>
       </c>
-      <c r="AO23" s="192" t="s">
+      <c r="AO23" s="191" t="s">
         <v>222</v>
       </c>
-      <c r="AP23" s="193"/>
-      <c r="AQ23" s="193"/>
-      <c r="AR23" s="206" t="s">
+      <c r="AP23" s="192"/>
+      <c r="AQ23" s="192"/>
+      <c r="AR23" s="205" t="s">
         <v>11</v>
       </c>
-      <c r="AS23" s="195">
+      <c r="AS23" s="194">
         <v>1.4</v>
       </c>
-      <c r="AT23" s="196">
+      <c r="AT23" s="195">
         <v>2</v>
       </c>
-      <c r="AU23" s="196">
+      <c r="AU23" s="195">
         <v>2</v>
       </c>
-      <c r="AV23" s="196" t="b">
+      <c r="AV23" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AW23" s="196" t="b">
+      <c r="AW23" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AX23" s="196" t="b">
+      <c r="AX23" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AY23" s="197">
+      <c r="AY23" s="196">
         <v>25</v>
       </c>
-      <c r="AZ23" s="198">
+      <c r="AZ23" s="197">
         <v>0.7</v>
       </c>
-      <c r="BA23" s="194">
+      <c r="BA23" s="193">
         <v>0.5</v>
       </c>
-      <c r="BB23" s="155" t="s">
+      <c r="BB23" s="154" t="s">
         <v>86</v>
       </c>
-      <c r="BC23" s="156" t="s">
+      <c r="BC23" s="155" t="s">
         <v>85</v>
       </c>
-      <c r="BD23" s="211">
+      <c r="BD23" s="210">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BE23" s="212">
+      <c r="BE23" s="211">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF23" s="215">
+      <c r="BF23" s="214">
         <v>435</v>
       </c>
-      <c r="BG23" s="216">
+      <c r="BG23" s="215">
         <v>465</v>
       </c>
-      <c r="BH23" s="138">
+      <c r="BH23" s="137">
         <v>3.2</v>
       </c>
-      <c r="BI23" s="138">
+      <c r="BI23" s="137">
         <v>9.5</v>
       </c>
-      <c r="BJ23" s="138">
+      <c r="BJ23" s="137">
         <v>1.7</v>
       </c>
-      <c r="BK23" s="138">
+      <c r="BK23" s="137">
         <v>0.5</v>
       </c>
-      <c r="BL23" s="217">
+      <c r="BL23" s="216">
         <v>1.2</v>
       </c>
-      <c r="BM23" s="215">
+      <c r="BM23" s="214">
         <v>45</v>
       </c>
-      <c r="BN23" s="138">
+      <c r="BN23" s="137">
         <v>15</v>
       </c>
-      <c r="BO23" s="218">
+      <c r="BO23" s="217">
         <v>0.4</v>
       </c>
-      <c r="BP23" s="218">
+      <c r="BP23" s="217">
         <v>25</v>
       </c>
-      <c r="BQ23" s="138"/>
-      <c r="BR23" s="138">
+      <c r="BQ23" s="137"/>
+      <c r="BR23" s="137">
         <v>0.2</v>
       </c>
-      <c r="BS23" s="220">
+      <c r="BS23" s="219">
         <v>1</v>
       </c>
-      <c r="BT23" s="221" t="s">
+      <c r="BT23" s="220" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="B24" s="139" t="s">
+      <c r="B24" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="142" t="s">
+      <c r="C24" s="141" t="s">
         <v>184</v>
       </c>
-      <c r="D24" s="142" t="s">
+      <c r="D24" s="141" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="138" t="s">
+      <c r="E24" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="F24" s="145">
+      <c r="F24" s="144">
         <v>8</v>
       </c>
-      <c r="G24" s="146" t="s">
+      <c r="G24" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="151">
+      <c r="H24" s="150">
         <v>550000</v>
       </c>
-      <c r="I24" s="152">
+      <c r="I24" s="151">
         <v>175</v>
       </c>
-      <c r="J24" s="171">
+      <c r="J24" s="170">
         <v>35</v>
       </c>
-      <c r="K24" s="172">
+      <c r="K24" s="171">
         <v>45</v>
       </c>
-      <c r="L24" s="179">
+      <c r="L24" s="178">
         <v>25</v>
       </c>
-      <c r="M24" s="180">
+      <c r="M24" s="179">
         <v>0</v>
       </c>
-      <c r="N24" s="181">
+      <c r="N24" s="180">
         <v>360</v>
       </c>
-      <c r="O24" s="163">
+      <c r="O24" s="162">
         <v>430</v>
       </c>
-      <c r="P24" s="163">
+      <c r="P24" s="162">
         <v>2.2999999999999998</v>
       </c>
-      <c r="Q24" s="163">
+      <c r="Q24" s="162">
         <v>0</v>
       </c>
-      <c r="R24" s="163">
+      <c r="R24" s="162">
         <v>1.4E-2</v>
       </c>
-      <c r="S24" s="163">
+      <c r="S24" s="162">
         <v>25</v>
       </c>
-      <c r="T24" s="163">
+      <c r="T24" s="162">
         <v>0.7</v>
       </c>
-      <c r="U24" s="181">
+      <c r="U24" s="180">
         <v>1.6</v>
       </c>
-      <c r="V24" s="163">
+      <c r="V24" s="162">
         <v>1.85</v>
       </c>
-      <c r="W24" s="171">
+      <c r="W24" s="170">
         <v>25</v>
       </c>
-      <c r="X24" s="181">
+      <c r="X24" s="180">
         <v>1.8</v>
       </c>
-      <c r="Y24" s="163">
+      <c r="Y24" s="162">
         <v>100</v>
       </c>
-      <c r="Z24" s="163">
+      <c r="Z24" s="162">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA24" s="163">
+      <c r="AA24" s="162">
         <v>40</v>
       </c>
-      <c r="AB24" s="163">
+      <c r="AB24" s="162">
         <v>14</v>
       </c>
-      <c r="AC24" s="173">
+      <c r="AC24" s="172">
         <v>425</v>
       </c>
-      <c r="AD24" s="163">
+      <c r="AD24" s="162">
         <v>11.5</v>
       </c>
-      <c r="AE24" s="183">
+      <c r="AE24" s="182">
         <v>5</v>
       </c>
-      <c r="AF24" s="174">
+      <c r="AF24" s="173">
         <v>10</v>
       </c>
-      <c r="AG24" s="163">
+      <c r="AG24" s="162">
         <v>20000</v>
       </c>
-      <c r="AH24" s="184">
+      <c r="AH24" s="183">
         <v>4</v>
       </c>
-      <c r="AI24" s="185">
+      <c r="AI24" s="184">
         <v>0.06</v>
       </c>
-      <c r="AJ24" s="182">
+      <c r="AJ24" s="181">
         <v>0.05</v>
       </c>
-      <c r="AK24" s="177">
+      <c r="AK24" s="176">
         <v>0</v>
       </c>
-      <c r="AL24" s="178">
+      <c r="AL24" s="177">
         <v>12</v>
       </c>
-      <c r="AM24" s="199" t="s">
+      <c r="AM24" s="198" t="s">
         <v>185</v>
       </c>
-      <c r="AN24" s="200" t="s">
+      <c r="AN24" s="199" t="s">
         <v>186</v>
       </c>
-      <c r="AO24" s="200" t="s">
+      <c r="AO24" s="199" t="s">
         <v>223</v>
       </c>
-      <c r="AP24" s="193"/>
-      <c r="AQ24" s="193"/>
-      <c r="AR24" s="206" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS24" s="202">
+      <c r="AP24" s="192"/>
+      <c r="AQ24" s="192"/>
+      <c r="AR24" s="205" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS24" s="201">
         <v>1.3</v>
       </c>
-      <c r="AT24" s="203">
+      <c r="AT24" s="202">
         <v>2</v>
       </c>
-      <c r="AU24" s="203">
+      <c r="AU24" s="202">
         <v>2</v>
       </c>
-      <c r="AV24" s="203" t="b">
+      <c r="AV24" s="202" t="b">
         <v>1</v>
       </c>
-      <c r="AW24" s="203" t="b">
+      <c r="AW24" s="202" t="b">
         <v>1</v>
       </c>
-      <c r="AX24" s="203" t="b">
+      <c r="AX24" s="202" t="b">
         <v>1</v>
       </c>
-      <c r="AY24" s="204">
+      <c r="AY24" s="203">
         <v>25</v>
       </c>
-      <c r="AZ24" s="205">
+      <c r="AZ24" s="204">
         <v>0.7</v>
       </c>
-      <c r="BA24" s="201">
+      <c r="BA24" s="200">
         <v>0.5</v>
       </c>
-      <c r="BB24" s="207" t="s">
+      <c r="BB24" s="206" t="s">
         <v>187</v>
       </c>
-      <c r="BC24" s="208" t="s">
+      <c r="BC24" s="207" t="s">
         <v>188</v>
       </c>
-      <c r="BD24" s="213">
+      <c r="BD24" s="212">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="BE24" s="214">
+      <c r="BE24" s="213">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF24" s="222">
+      <c r="BF24" s="221">
         <v>450</v>
       </c>
-      <c r="BG24" s="223">
+      <c r="BG24" s="222">
         <v>505</v>
       </c>
-      <c r="BH24" s="141">
+      <c r="BH24" s="140">
         <v>3.4</v>
       </c>
-      <c r="BI24" s="141">
+      <c r="BI24" s="140">
         <v>9.5</v>
       </c>
-      <c r="BJ24" s="141">
+      <c r="BJ24" s="140">
         <v>1.7</v>
       </c>
-      <c r="BK24" s="141">
+      <c r="BK24" s="140">
         <v>0.6</v>
       </c>
-      <c r="BL24" s="224">
+      <c r="BL24" s="223">
         <v>1</v>
       </c>
-      <c r="BM24" s="222">
+      <c r="BM24" s="221">
         <v>45</v>
       </c>
-      <c r="BN24" s="141">
+      <c r="BN24" s="140">
         <v>15</v>
       </c>
-      <c r="BO24" s="218">
+      <c r="BO24" s="217">
         <v>0.4</v>
       </c>
-      <c r="BP24" s="218">
+      <c r="BP24" s="217">
         <v>25</v>
       </c>
-      <c r="BQ24" s="138"/>
-      <c r="BR24" s="138">
+      <c r="BQ24" s="137"/>
+      <c r="BR24" s="137">
         <v>0.2</v>
       </c>
-      <c r="BS24" s="220">
+      <c r="BS24" s="219">
         <v>1</v>
       </c>
-      <c r="BT24" s="228" t="s">
+      <c r="BT24" s="227" t="s">
         <v>184</v>
       </c>
     </row>
@@ -7682,25 +7676,25 @@
       <c r="AJ25" s="56">
         <v>0.05</v>
       </c>
-      <c r="AK25" s="125">
+      <c r="AK25" s="124">
         <v>0</v>
       </c>
-      <c r="AL25" s="119">
+      <c r="AL25" s="118">
         <v>12</v>
       </c>
-      <c r="AM25" s="127" t="s">
+      <c r="AM25" s="126" t="s">
         <v>83</v>
       </c>
-      <c r="AN25" s="126" t="s">
+      <c r="AN25" s="125" t="s">
         <v>82</v>
       </c>
-      <c r="AO25" s="126" t="s">
+      <c r="AO25" s="125" t="s">
         <v>224</v>
       </c>
       <c r="AP25" s="92"/>
       <c r="AQ25" s="92"/>
-      <c r="AR25" s="115" t="s">
-        <v>184</v>
+      <c r="AR25" s="205" t="s">
+        <v>11</v>
       </c>
       <c r="AS25" s="39">
         <v>1.2</v>
@@ -7720,10 +7714,10 @@
       <c r="AX25" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AY25" s="118">
+      <c r="AY25" s="117">
         <v>25</v>
       </c>
-      <c r="AZ25" s="116">
+      <c r="AZ25" s="115">
         <v>0.7</v>
       </c>
       <c r="BA25" s="101">
@@ -7778,10 +7772,10 @@
       <c r="BR25" s="49">
         <v>0.2</v>
       </c>
-      <c r="BS25" s="133">
+      <c r="BS25" s="132">
         <v>1</v>
       </c>
-      <c r="BT25" s="132" t="s">
+      <c r="BT25" s="131" t="s">
         <v>13</v>
       </c>
     </row>
@@ -7892,25 +7886,25 @@
       <c r="AJ26" s="56">
         <v>0.04</v>
       </c>
-      <c r="AK26" s="124">
+      <c r="AK26" s="123">
         <v>0</v>
       </c>
       <c r="AL26" s="58">
         <v>12</v>
       </c>
-      <c r="AM26" s="127" t="s">
+      <c r="AM26" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="AN26" s="126" t="s">
+      <c r="AN26" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="AO26" s="126" t="s">
+      <c r="AO26" s="125" t="s">
         <v>225</v>
       </c>
       <c r="AP26" s="92"/>
       <c r="AQ26" s="92"/>
-      <c r="AR26" s="115" t="s">
-        <v>13</v>
+      <c r="AR26" s="205" t="s">
+        <v>11</v>
       </c>
       <c r="AS26" s="39">
         <v>1.05</v>
@@ -7930,10 +7924,10 @@
       <c r="AX26" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AY26" s="118">
+      <c r="AY26" s="117">
         <v>25</v>
       </c>
-      <c r="AZ26" s="116">
+      <c r="AZ26" s="115">
         <v>0.75</v>
       </c>
       <c r="BA26" s="101">
@@ -7990,10 +7984,10 @@
       <c r="BR26" s="49">
         <v>0.2</v>
       </c>
-      <c r="BS26" s="133">
+      <c r="BS26" s="132">
         <v>1</v>
       </c>
-      <c r="BT26" s="132" t="s">
+      <c r="BT26" s="131" t="s">
         <v>14</v>
       </c>
     </row>
@@ -8104,25 +8098,25 @@
       <c r="AJ27" s="51">
         <v>0.04</v>
       </c>
-      <c r="AK27" s="123">
+      <c r="AK27" s="122">
         <v>0</v>
       </c>
       <c r="AL27" s="55">
         <v>12</v>
       </c>
-      <c r="AM27" s="127" t="s">
+      <c r="AM27" s="126" t="s">
         <v>200</v>
       </c>
-      <c r="AN27" s="126" t="s">
+      <c r="AN27" s="125" t="s">
         <v>201</v>
       </c>
-      <c r="AO27" s="126" t="s">
+      <c r="AO27" s="125" t="s">
         <v>202</v>
       </c>
       <c r="AP27" s="92"/>
       <c r="AQ27" s="92"/>
-      <c r="AR27" s="115" t="s">
-        <v>14</v>
+      <c r="AR27" s="205" t="s">
+        <v>11</v>
       </c>
       <c r="AS27" s="39">
         <v>1.05</v>
@@ -8142,10 +8136,10 @@
       <c r="AX27" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AY27" s="118">
+      <c r="AY27" s="117">
         <v>25</v>
       </c>
-      <c r="AZ27" s="116">
+      <c r="AZ27" s="115">
         <v>0.75</v>
       </c>
       <c r="BA27" s="101">
@@ -8210,422 +8204,422 @@
       </c>
     </row>
     <row r="28" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="B28" s="139" t="s">
+      <c r="B28" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="140" t="s">
+      <c r="C28" s="139" t="s">
         <v>230</v>
       </c>
-      <c r="D28" s="140" t="s">
+      <c r="D28" s="139" t="s">
         <v>227</v>
       </c>
-      <c r="E28" s="138" t="s">
+      <c r="E28" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="F28" s="143">
+      <c r="F28" s="142">
         <v>12</v>
       </c>
-      <c r="G28" s="144" t="s">
+      <c r="G28" s="143" t="s">
         <v>197</v>
       </c>
-      <c r="H28" s="149">
+      <c r="H28" s="148">
         <v>700000</v>
       </c>
-      <c r="I28" s="150">
+      <c r="I28" s="149">
         <v>550</v>
       </c>
-      <c r="J28" s="171">
+      <c r="J28" s="170">
         <v>35</v>
       </c>
-      <c r="K28" s="186">
+      <c r="K28" s="185">
         <v>45</v>
       </c>
-      <c r="L28" s="187">
+      <c r="L28" s="186">
         <v>25</v>
       </c>
-      <c r="M28" s="188">
+      <c r="M28" s="187">
         <v>0</v>
       </c>
-      <c r="N28" s="161">
+      <c r="N28" s="160">
         <v>500</v>
       </c>
-      <c r="O28" s="165">
+      <c r="O28" s="164">
         <v>600</v>
       </c>
-      <c r="P28" s="165">
+      <c r="P28" s="164">
         <v>2.5</v>
       </c>
-      <c r="Q28" s="165">
+      <c r="Q28" s="164">
         <v>0</v>
       </c>
-      <c r="R28" s="165">
+      <c r="R28" s="164">
         <v>0.02</v>
       </c>
-      <c r="S28" s="183">
+      <c r="S28" s="182">
         <v>20</v>
       </c>
-      <c r="T28" s="183">
+      <c r="T28" s="182">
         <v>0.8</v>
       </c>
-      <c r="U28" s="164">
+      <c r="U28" s="163">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V28" s="165">
+      <c r="V28" s="164">
         <v>2.2000000000000002</v>
       </c>
-      <c r="W28" s="171">
+      <c r="W28" s="170">
         <v>31</v>
       </c>
-      <c r="X28" s="161">
+      <c r="X28" s="160">
         <v>2.0099999999999998</v>
       </c>
-      <c r="Y28" s="165">
+      <c r="Y28" s="164">
         <v>100</v>
       </c>
-      <c r="Z28" s="165">
+      <c r="Z28" s="164">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA28" s="165">
+      <c r="AA28" s="164">
         <v>20</v>
       </c>
-      <c r="AB28" s="165">
+      <c r="AB28" s="164">
         <v>14</v>
       </c>
-      <c r="AC28" s="173">
+      <c r="AC28" s="172">
         <v>475</v>
       </c>
-      <c r="AD28" s="183">
+      <c r="AD28" s="182">
         <v>12</v>
       </c>
-      <c r="AE28" s="165">
+      <c r="AE28" s="164">
         <v>7</v>
       </c>
-      <c r="AF28" s="183">
+      <c r="AF28" s="182">
         <v>10</v>
       </c>
-      <c r="AG28" s="165">
+      <c r="AG28" s="164">
         <v>65000</v>
       </c>
-      <c r="AH28" s="167">
+      <c r="AH28" s="166">
         <v>6</v>
       </c>
-      <c r="AI28" s="176">
+      <c r="AI28" s="175">
         <v>0.04</v>
       </c>
-      <c r="AJ28" s="189">
+      <c r="AJ28" s="188">
         <v>0.03</v>
       </c>
-      <c r="AK28" s="190">
+      <c r="AK28" s="189">
         <v>0</v>
       </c>
-      <c r="AL28" s="172">
+      <c r="AL28" s="171">
         <v>12</v>
       </c>
-      <c r="AM28" s="191" t="s">
+      <c r="AM28" s="190" t="s">
         <v>231</v>
       </c>
-      <c r="AN28" s="192" t="s">
+      <c r="AN28" s="191" t="s">
         <v>232</v>
       </c>
-      <c r="AO28" s="192" t="s">
+      <c r="AO28" s="191" t="s">
         <v>233</v>
       </c>
-      <c r="AP28" s="193"/>
-      <c r="AQ28" s="193"/>
-      <c r="AR28" s="206" t="s">
-        <v>197</v>
-      </c>
-      <c r="AS28" s="195">
+      <c r="AP28" s="192"/>
+      <c r="AQ28" s="192"/>
+      <c r="AR28" s="205" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS28" s="194">
         <v>1.05</v>
       </c>
-      <c r="AT28" s="196">
+      <c r="AT28" s="195">
         <v>1.5</v>
       </c>
-      <c r="AU28" s="196">
+      <c r="AU28" s="195">
         <v>2</v>
       </c>
-      <c r="AV28" s="196" t="b">
+      <c r="AV28" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AW28" s="196" t="b">
+      <c r="AW28" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AX28" s="196" t="b">
+      <c r="AX28" s="195" t="b">
         <v>1</v>
       </c>
-      <c r="AY28" s="197">
+      <c r="AY28" s="196">
         <v>25</v>
       </c>
-      <c r="AZ28" s="198">
+      <c r="AZ28" s="197">
         <v>0.75</v>
       </c>
-      <c r="BA28" s="194">
+      <c r="BA28" s="193">
         <v>0.4</v>
       </c>
-      <c r="BB28" s="209" t="s">
+      <c r="BB28" s="208" t="s">
         <v>234</v>
       </c>
-      <c r="BC28" s="210" t="s">
+      <c r="BC28" s="209" t="s">
         <v>235</v>
       </c>
-      <c r="BD28" s="211">
+      <c r="BD28" s="210">
         <v>1.5E-3</v>
       </c>
-      <c r="BE28" s="212">
+      <c r="BE28" s="211">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF28" s="229">
+      <c r="BF28" s="228">
         <v>700</v>
       </c>
-      <c r="BG28" s="230">
+      <c r="BG28" s="229">
         <v>750</v>
       </c>
-      <c r="BH28" s="231">
+      <c r="BH28" s="230">
         <v>4.9000000000000004</v>
       </c>
-      <c r="BI28" s="231">
+      <c r="BI28" s="230">
         <v>9.5</v>
       </c>
-      <c r="BJ28" s="231">
+      <c r="BJ28" s="230">
         <v>1.7</v>
       </c>
-      <c r="BK28" s="231">
+      <c r="BK28" s="230">
         <v>0.7</v>
       </c>
-      <c r="BL28" s="232">
+      <c r="BL28" s="231">
         <v>1.03</v>
       </c>
-      <c r="BM28" s="229">
+      <c r="BM28" s="228">
         <v>59</v>
       </c>
-      <c r="BN28" s="231">
+      <c r="BN28" s="230">
         <v>15</v>
       </c>
-      <c r="BO28" s="218">
+      <c r="BO28" s="217">
         <v>0.4</v>
       </c>
-      <c r="BP28" s="218">
+      <c r="BP28" s="217">
         <v>25</v>
       </c>
-      <c r="BQ28" s="140"/>
-      <c r="BR28" s="233">
+      <c r="BQ28" s="139"/>
+      <c r="BR28" s="232">
         <v>0.2</v>
       </c>
-      <c r="BS28" s="234">
+      <c r="BS28" s="233">
         <v>1</v>
       </c>
-      <c r="BT28" s="235" t="s">
+      <c r="BT28" s="234" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="B29" s="139" t="s">
+      <c r="B29" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="140" t="s">
+      <c r="C29" s="139" t="s">
         <v>247</v>
       </c>
-      <c r="D29" s="140" t="s">
+      <c r="D29" s="139" t="s">
         <v>227</v>
       </c>
-      <c r="E29" s="138" t="s">
+      <c r="E29" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="F29" s="143">
+      <c r="F29" s="142">
         <v>13</v>
       </c>
-      <c r="G29" s="144" t="s">
+      <c r="G29" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="H29" s="149">
+      <c r="H29" s="148">
         <v>1000000</v>
       </c>
-      <c r="I29" s="150">
+      <c r="I29" s="149">
         <v>650</v>
       </c>
-      <c r="J29" s="236">
+      <c r="J29" s="235">
         <v>35</v>
       </c>
-      <c r="K29" s="172">
+      <c r="K29" s="171">
         <v>45</v>
       </c>
-      <c r="L29" s="187">
+      <c r="L29" s="186">
         <v>25</v>
       </c>
-      <c r="M29" s="188">
+      <c r="M29" s="187">
         <v>0</v>
       </c>
-      <c r="N29" s="164">
+      <c r="N29" s="163">
         <v>550</v>
       </c>
-      <c r="O29" s="237">
+      <c r="O29" s="236">
         <v>650</v>
       </c>
-      <c r="P29" s="187">
+      <c r="P29" s="186">
         <v>2.6</v>
       </c>
-      <c r="Q29" s="165">
+      <c r="Q29" s="164">
         <v>0</v>
       </c>
-      <c r="R29" s="238">
+      <c r="R29" s="237">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="S29" s="239">
+      <c r="S29" s="238">
         <v>20</v>
       </c>
-      <c r="T29" s="183">
+      <c r="T29" s="182">
         <v>0.8</v>
       </c>
-      <c r="U29" s="164">
+      <c r="U29" s="163">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V29" s="189">
+      <c r="V29" s="188">
         <v>2.2000000000000002</v>
       </c>
-      <c r="W29" s="173">
+      <c r="W29" s="172">
         <v>31</v>
       </c>
-      <c r="X29" s="164">
+      <c r="X29" s="163">
         <v>2</v>
       </c>
-      <c r="Y29" s="165">
+      <c r="Y29" s="164">
         <v>100</v>
       </c>
-      <c r="Z29" s="237">
+      <c r="Z29" s="236">
         <f>dragonDefinitions[[#This Row],['[energyBaseMin']]]+25</f>
         <v>125</v>
       </c>
-      <c r="AA29" s="165">
+      <c r="AA29" s="164">
         <v>20</v>
       </c>
-      <c r="AB29" s="165">
+      <c r="AB29" s="164">
         <v>14</v>
       </c>
-      <c r="AC29" s="173">
+      <c r="AC29" s="172">
         <v>475</v>
       </c>
-      <c r="AD29" s="183">
+      <c r="AD29" s="182">
         <v>12</v>
       </c>
-      <c r="AE29" s="165">
+      <c r="AE29" s="164">
         <v>7</v>
       </c>
-      <c r="AF29" s="183">
+      <c r="AF29" s="182">
         <v>10</v>
       </c>
-      <c r="AG29" s="165">
+      <c r="AG29" s="164">
         <v>75000</v>
       </c>
-      <c r="AH29" s="176">
+      <c r="AH29" s="175">
         <v>6</v>
       </c>
-      <c r="AI29" s="164">
+      <c r="AI29" s="163">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AJ29" s="240">
+      <c r="AJ29" s="239">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AK29" s="173">
+      <c r="AK29" s="172">
         <v>0</v>
       </c>
-      <c r="AL29" s="241">
+      <c r="AL29" s="240">
         <v>12</v>
       </c>
-      <c r="AM29" s="242" t="s">
+      <c r="AM29" s="241" t="s">
         <v>248</v>
       </c>
-      <c r="AN29" s="243" t="s">
+      <c r="AN29" s="242" t="s">
         <v>249</v>
       </c>
-      <c r="AO29" s="243" t="s">
+      <c r="AO29" s="242" t="s">
         <v>250</v>
       </c>
-      <c r="AP29" s="244"/>
-      <c r="AQ29" s="244"/>
-      <c r="AR29" s="245" t="s">
-        <v>230</v>
-      </c>
-      <c r="AS29" s="246">
+      <c r="AP29" s="243"/>
+      <c r="AQ29" s="243"/>
+      <c r="AR29" s="205" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS29" s="244">
         <v>1.05</v>
       </c>
-      <c r="AT29" s="247">
+      <c r="AT29" s="245">
         <v>1.5</v>
       </c>
-      <c r="AU29" s="247">
+      <c r="AU29" s="245">
         <v>2</v>
       </c>
-      <c r="AV29" s="247" t="b">
+      <c r="AV29" s="245" t="b">
         <v>1</v>
       </c>
-      <c r="AW29" s="247" t="b">
+      <c r="AW29" s="245" t="b">
         <v>1</v>
       </c>
-      <c r="AX29" s="247" t="b">
+      <c r="AX29" s="245" t="b">
         <v>1</v>
       </c>
-      <c r="AY29" s="248">
+      <c r="AY29" s="246">
         <v>25</v>
       </c>
-      <c r="AZ29" s="247">
+      <c r="AZ29" s="245">
         <v>0.75</v>
       </c>
-      <c r="BA29" s="247">
+      <c r="BA29" s="245">
         <v>0.4</v>
       </c>
-      <c r="BB29" s="209" t="s">
+      <c r="BB29" s="208" t="s">
         <v>251</v>
       </c>
-      <c r="BC29" s="210" t="s">
+      <c r="BC29" s="209" t="s">
         <v>252</v>
       </c>
-      <c r="BD29" s="249">
+      <c r="BD29" s="247">
         <v>1.5E-3</v>
       </c>
-      <c r="BE29" s="144">
+      <c r="BE29" s="143">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BF29" s="229">
+      <c r="BF29" s="228">
         <v>700</v>
       </c>
-      <c r="BG29" s="250">
+      <c r="BG29" s="248">
         <v>750</v>
       </c>
-      <c r="BH29" s="231">
+      <c r="BH29" s="230">
         <v>4.9000000000000004</v>
       </c>
-      <c r="BI29" s="231">
+      <c r="BI29" s="230">
         <v>9.5</v>
       </c>
-      <c r="BJ29" s="231">
+      <c r="BJ29" s="230">
         <v>1.7</v>
       </c>
-      <c r="BK29" s="231">
+      <c r="BK29" s="230">
         <v>0.7</v>
       </c>
-      <c r="BL29" s="231">
+      <c r="BL29" s="230">
         <v>1.03</v>
       </c>
-      <c r="BM29" s="229">
+      <c r="BM29" s="228">
         <v>59</v>
       </c>
-      <c r="BN29" s="231">
+      <c r="BN29" s="230">
         <v>15</v>
       </c>
-      <c r="BO29" s="231">
+      <c r="BO29" s="230">
         <v>0.4</v>
       </c>
-      <c r="BP29" s="232">
+      <c r="BP29" s="231">
         <v>25</v>
       </c>
-      <c r="BQ29" s="251"/>
-      <c r="BR29" s="252">
+      <c r="BQ29" s="249"/>
+      <c r="BR29" s="250">
         <v>0.2</v>
       </c>
-      <c r="BS29" s="253">
+      <c r="BS29" s="251">
         <v>1</v>
       </c>
-      <c r="BT29" s="235" t="s">
+      <c r="BT29" s="234" t="s">
         <v>247</v>
       </c>
     </row>
@@ -8639,83 +8633,83 @@
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="30"/>
-      <c r="J30" s="273" t="s">
+      <c r="J30" s="261" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="273"/>
-      <c r="L30" s="273"/>
-      <c r="M30" s="273"/>
-      <c r="N30" s="270" t="s">
+      <c r="K30" s="261"/>
+      <c r="L30" s="261"/>
+      <c r="M30" s="261"/>
+      <c r="N30" s="258" t="s">
         <v>73</v>
       </c>
-      <c r="O30" s="271"/>
-      <c r="P30" s="271"/>
-      <c r="Q30" s="271"/>
-      <c r="R30" s="272"/>
-      <c r="S30" s="271"/>
-      <c r="T30" s="271"/>
-      <c r="U30" s="268" t="s">
+      <c r="O30" s="259"/>
+      <c r="P30" s="259"/>
+      <c r="Q30" s="259"/>
+      <c r="R30" s="260"/>
+      <c r="S30" s="259"/>
+      <c r="T30" s="259"/>
+      <c r="U30" s="256" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="269"/>
+      <c r="V30" s="257"/>
       <c r="W30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X30" s="265" t="s">
+      <c r="X30" s="253" t="s">
         <v>70</v>
       </c>
-      <c r="Y30" s="266"/>
-      <c r="Z30" s="266"/>
-      <c r="AA30" s="266"/>
-      <c r="AB30" s="267"/>
-      <c r="AC30" s="264" t="s">
+      <c r="Y30" s="254"/>
+      <c r="Z30" s="254"/>
+      <c r="AA30" s="254"/>
+      <c r="AB30" s="255"/>
+      <c r="AC30" s="252" t="s">
         <v>69</v>
       </c>
-      <c r="AD30" s="264"/>
-      <c r="AE30" s="264"/>
-      <c r="AF30" s="264"/>
-      <c r="AG30" s="264"/>
+      <c r="AD30" s="252"/>
+      <c r="AE30" s="252"/>
+      <c r="AF30" s="252"/>
+      <c r="AG30" s="252"/>
       <c r="AH30" s="30"/>
-      <c r="AI30" s="260" t="s">
+      <c r="AI30" s="268" t="s">
         <v>68</v>
       </c>
-      <c r="AJ30" s="260"/>
-      <c r="AK30" s="254" t="s">
+      <c r="AJ30" s="268"/>
+      <c r="AK30" s="262" t="s">
         <v>246</v>
       </c>
-      <c r="AL30" s="254"/>
-      <c r="AM30" s="261" t="s">
+      <c r="AL30" s="262"/>
+      <c r="AM30" s="269" t="s">
         <v>236</v>
       </c>
-      <c r="AN30" s="262"/>
-      <c r="AO30" s="262"/>
-      <c r="AP30" s="262"/>
-      <c r="AQ30" s="262"/>
-      <c r="AR30" s="263"/>
-      <c r="AS30" s="255" t="s">
+      <c r="AN30" s="270"/>
+      <c r="AO30" s="270"/>
+      <c r="AP30" s="270"/>
+      <c r="AQ30" s="270"/>
+      <c r="AR30" s="271"/>
+      <c r="AS30" s="263" t="s">
         <v>226</v>
       </c>
-      <c r="AT30" s="256"/>
-      <c r="AU30" s="256"/>
-      <c r="AV30" s="256"/>
-      <c r="AW30" s="256"/>
-      <c r="AX30" s="256"/>
-      <c r="AY30" s="257"/>
+      <c r="AT30" s="264"/>
+      <c r="AU30" s="264"/>
+      <c r="AV30" s="264"/>
+      <c r="AW30" s="264"/>
+      <c r="AX30" s="264"/>
+      <c r="AY30" s="265"/>
       <c r="AZ30" s="30"/>
       <c r="BA30" s="30"/>
       <c r="BB30" s="30"/>
       <c r="BC30" s="30"/>
       <c r="BD30" s="30"/>
       <c r="BE30" s="30"/>
-      <c r="BF30" s="259" t="s">
+      <c r="BF30" s="267" t="s">
         <v>67</v>
       </c>
-      <c r="BG30" s="259"/>
-      <c r="BH30" s="259"/>
-      <c r="BI30" s="259"/>
-      <c r="BJ30" s="259"/>
-      <c r="BK30" s="259"/>
-      <c r="BL30" s="259"/>
+      <c r="BG30" s="267"/>
+      <c r="BH30" s="267"/>
+      <c r="BI30" s="267"/>
+      <c r="BJ30" s="267"/>
+      <c r="BK30" s="267"/>
+      <c r="BL30" s="267"/>
       <c r="BM30" s="30"/>
       <c r="BN30" s="30"/>
       <c r="BO30" s="30"/>
@@ -8900,7 +8894,7 @@
       <c r="I35" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J35" s="135" t="s">
+      <c r="J35" s="134" t="s">
         <v>237</v>
       </c>
     </row>
@@ -10068,61 +10062,61 @@
       <c r="D60">
         <v>20</v>
       </c>
-      <c r="E60" s="128">
+      <c r="E60" s="127">
         <v>4571</v>
       </c>
-      <c r="F60" s="129">
+      <c r="F60" s="128">
         <v>13714</v>
       </c>
-      <c r="G60" s="129">
+      <c r="G60" s="128">
         <v>27428</v>
       </c>
-      <c r="H60" s="129">
+      <c r="H60" s="128">
         <v>45713</v>
       </c>
-      <c r="I60" s="129">
+      <c r="I60" s="128">
         <v>68569</v>
       </c>
-      <c r="J60" s="129">
+      <c r="J60" s="128">
         <v>95997</v>
       </c>
-      <c r="K60" s="129">
+      <c r="K60" s="128">
         <v>127995</v>
       </c>
-      <c r="L60" s="129">
+      <c r="L60" s="128">
         <v>164565</v>
       </c>
-      <c r="M60" s="129">
+      <c r="M60" s="128">
         <v>205707</v>
       </c>
-      <c r="N60" s="129">
+      <c r="N60" s="128">
         <v>251419</v>
       </c>
-      <c r="O60" s="129">
+      <c r="O60" s="128">
         <v>301703</v>
       </c>
-      <c r="P60" s="129">
+      <c r="P60" s="128">
         <v>356559</v>
       </c>
-      <c r="Q60" s="129">
+      <c r="Q60" s="128">
         <v>415985</v>
       </c>
-      <c r="R60" s="129">
+      <c r="R60" s="128">
         <v>479983</v>
       </c>
-      <c r="S60" s="129">
+      <c r="S60" s="128">
         <v>548552</v>
       </c>
-      <c r="T60" s="129">
+      <c r="T60" s="128">
         <v>621692</v>
       </c>
-      <c r="U60" s="129">
+      <c r="U60" s="128">
         <v>699403</v>
       </c>
-      <c r="V60" s="129">
+      <c r="V60" s="128">
         <v>781686</v>
       </c>
-      <c r="W60" s="129">
+      <c r="W60" s="128">
         <v>868540</v>
       </c>
     </row>
@@ -10136,77 +10130,77 @@
       <c r="D61">
         <v>20</v>
       </c>
-      <c r="E61" s="128">
+      <c r="E61" s="127">
         <v>4996</v>
       </c>
-      <c r="F61" s="129">
+      <c r="F61" s="128">
         <v>14989</v>
       </c>
-      <c r="G61" s="129">
+      <c r="G61" s="128">
         <v>29979</v>
       </c>
-      <c r="H61" s="129">
+      <c r="H61" s="128">
         <v>49964</v>
       </c>
-      <c r="I61" s="129">
+      <c r="I61" s="128">
         <v>74946</v>
       </c>
-      <c r="J61" s="129">
+      <c r="J61" s="128">
         <v>104925</v>
       </c>
-      <c r="K61" s="129">
+      <c r="K61" s="128">
         <v>139900</v>
       </c>
-      <c r="L61" s="129">
+      <c r="L61" s="128">
         <v>179871</v>
       </c>
-      <c r="M61" s="129">
+      <c r="M61" s="128">
         <v>224839</v>
       </c>
-      <c r="N61" s="129">
+      <c r="N61" s="128">
         <v>274803</v>
       </c>
-      <c r="O61" s="129">
+      <c r="O61" s="128">
         <v>329764</v>
       </c>
-      <c r="P61" s="129">
+      <c r="P61" s="128">
         <v>389721</v>
       </c>
-      <c r="Q61" s="129">
+      <c r="Q61" s="128">
         <v>454674</v>
       </c>
-      <c r="R61" s="129">
+      <c r="R61" s="128">
         <v>524624</v>
       </c>
-      <c r="S61" s="129">
+      <c r="S61" s="128">
         <v>599571</v>
       </c>
-      <c r="T61" s="129">
+      <c r="T61" s="128">
         <v>679513</v>
       </c>
-      <c r="U61" s="129">
+      <c r="U61" s="128">
         <v>764452</v>
       </c>
-      <c r="V61" s="129">
+      <c r="V61" s="128">
         <v>854388</v>
       </c>
-      <c r="W61" s="129">
+      <c r="W61" s="128">
         <v>949320</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC30:AG30"/>
-    <mergeCell ref="X30:AB30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="N30:T30"/>
-    <mergeCell ref="J30:M30"/>
     <mergeCell ref="AK30:AL30"/>
     <mergeCell ref="AS30:AY30"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF30:BL30"/>
     <mergeCell ref="AI30:AJ30"/>
     <mergeCell ref="AM30:AR30"/>
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="N30:T30"/>
+    <mergeCell ref="J30:M30"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="127" priority="22"/>

</xml_diff>

<commit_message>
Merge conflict fix (related to unlocking missing dragons from Classic)
Former-commit-id: e65d4344c039846d89e10c31992c1b143f382b14
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -2134,6 +2134,36 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2162,36 +2192,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5188,8 +5188,8 @@
   </sheetPr>
   <dimension ref="A1:BT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="AI13" workbookViewId="0">
+      <selection activeCell="AR28" sqref="AR28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5471,10 +5471,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="268"/>
-      <c r="AP14" s="268"/>
-      <c r="AQ14" s="268"/>
-      <c r="AR14" s="268"/>
+      <c r="AO14" s="258"/>
+      <c r="AP14" s="258"/>
+      <c r="AQ14" s="258"/>
+      <c r="AR14" s="258"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -7490,7 +7490,7 @@
       <c r="AP24" s="193"/>
       <c r="AQ24" s="193"/>
       <c r="AR24" s="206" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AS24" s="202">
         <v>1.3</v>
@@ -7700,7 +7700,7 @@
       <c r="AP25" s="92"/>
       <c r="AQ25" s="92"/>
       <c r="AR25" s="115" t="s">
-        <v>184</v>
+        <v>11</v>
       </c>
       <c r="AS25" s="39">
         <v>1.2</v>
@@ -7910,7 +7910,7 @@
       <c r="AP26" s="92"/>
       <c r="AQ26" s="92"/>
       <c r="AR26" s="115" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AS26" s="39">
         <v>1.05</v>
@@ -8122,7 +8122,7 @@
       <c r="AP27" s="92"/>
       <c r="AQ27" s="92"/>
       <c r="AR27" s="115" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AS27" s="39">
         <v>1.05</v>
@@ -8334,7 +8334,7 @@
       <c r="AP28" s="193"/>
       <c r="AQ28" s="193"/>
       <c r="AR28" s="206" t="s">
-        <v>197</v>
+        <v>11</v>
       </c>
       <c r="AS28" s="195">
         <v>1.05</v>
@@ -8544,7 +8544,7 @@
       <c r="AP29" s="244"/>
       <c r="AQ29" s="244"/>
       <c r="AR29" s="245" t="s">
-        <v>230</v>
+        <v>11</v>
       </c>
       <c r="AS29" s="246">
         <v>1.05</v>
@@ -8639,83 +8639,83 @@
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="30"/>
-      <c r="J30" s="263" t="s">
+      <c r="J30" s="273" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="263"/>
-      <c r="L30" s="263"/>
-      <c r="M30" s="263"/>
-      <c r="N30" s="260" t="s">
+      <c r="K30" s="273"/>
+      <c r="L30" s="273"/>
+      <c r="M30" s="273"/>
+      <c r="N30" s="270" t="s">
         <v>73</v>
       </c>
-      <c r="O30" s="261"/>
-      <c r="P30" s="261"/>
-      <c r="Q30" s="261"/>
-      <c r="R30" s="262"/>
-      <c r="S30" s="261"/>
-      <c r="T30" s="261"/>
-      <c r="U30" s="258" t="s">
+      <c r="O30" s="271"/>
+      <c r="P30" s="271"/>
+      <c r="Q30" s="271"/>
+      <c r="R30" s="272"/>
+      <c r="S30" s="271"/>
+      <c r="T30" s="271"/>
+      <c r="U30" s="268" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="259"/>
+      <c r="V30" s="269"/>
       <c r="W30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X30" s="255" t="s">
+      <c r="X30" s="265" t="s">
         <v>70</v>
       </c>
-      <c r="Y30" s="256"/>
-      <c r="Z30" s="256"/>
-      <c r="AA30" s="256"/>
-      <c r="AB30" s="257"/>
-      <c r="AC30" s="254" t="s">
+      <c r="Y30" s="266"/>
+      <c r="Z30" s="266"/>
+      <c r="AA30" s="266"/>
+      <c r="AB30" s="267"/>
+      <c r="AC30" s="264" t="s">
         <v>69</v>
       </c>
-      <c r="AD30" s="254"/>
-      <c r="AE30" s="254"/>
-      <c r="AF30" s="254"/>
-      <c r="AG30" s="254"/>
+      <c r="AD30" s="264"/>
+      <c r="AE30" s="264"/>
+      <c r="AF30" s="264"/>
+      <c r="AG30" s="264"/>
       <c r="AH30" s="30"/>
-      <c r="AI30" s="270" t="s">
+      <c r="AI30" s="260" t="s">
         <v>68</v>
       </c>
-      <c r="AJ30" s="270"/>
-      <c r="AK30" s="264" t="s">
+      <c r="AJ30" s="260"/>
+      <c r="AK30" s="254" t="s">
         <v>246</v>
       </c>
-      <c r="AL30" s="264"/>
-      <c r="AM30" s="271" t="s">
+      <c r="AL30" s="254"/>
+      <c r="AM30" s="261" t="s">
         <v>236</v>
       </c>
-      <c r="AN30" s="272"/>
-      <c r="AO30" s="272"/>
-      <c r="AP30" s="272"/>
-      <c r="AQ30" s="272"/>
-      <c r="AR30" s="273"/>
-      <c r="AS30" s="265" t="s">
+      <c r="AN30" s="262"/>
+      <c r="AO30" s="262"/>
+      <c r="AP30" s="262"/>
+      <c r="AQ30" s="262"/>
+      <c r="AR30" s="263"/>
+      <c r="AS30" s="255" t="s">
         <v>226</v>
       </c>
-      <c r="AT30" s="266"/>
-      <c r="AU30" s="266"/>
-      <c r="AV30" s="266"/>
-      <c r="AW30" s="266"/>
-      <c r="AX30" s="266"/>
-      <c r="AY30" s="267"/>
+      <c r="AT30" s="256"/>
+      <c r="AU30" s="256"/>
+      <c r="AV30" s="256"/>
+      <c r="AW30" s="256"/>
+      <c r="AX30" s="256"/>
+      <c r="AY30" s="257"/>
       <c r="AZ30" s="30"/>
       <c r="BA30" s="30"/>
       <c r="BB30" s="30"/>
       <c r="BC30" s="30"/>
       <c r="BD30" s="30"/>
       <c r="BE30" s="30"/>
-      <c r="BF30" s="269" t="s">
+      <c r="BF30" s="259" t="s">
         <v>67</v>
       </c>
-      <c r="BG30" s="269"/>
-      <c r="BH30" s="269"/>
-      <c r="BI30" s="269"/>
-      <c r="BJ30" s="269"/>
-      <c r="BK30" s="269"/>
-      <c r="BL30" s="269"/>
+      <c r="BG30" s="259"/>
+      <c r="BH30" s="259"/>
+      <c r="BI30" s="259"/>
+      <c r="BJ30" s="259"/>
+      <c r="BK30" s="259"/>
+      <c r="BL30" s="259"/>
       <c r="BM30" s="30"/>
       <c r="BN30" s="30"/>
       <c r="BO30" s="30"/>
@@ -10196,17 +10196,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="N30:T30"/>
+    <mergeCell ref="J30:M30"/>
     <mergeCell ref="AK30:AL30"/>
     <mergeCell ref="AS30:AY30"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF30:BL30"/>
     <mergeCell ref="AI30:AJ30"/>
     <mergeCell ref="AM30:AR30"/>
-    <mergeCell ref="AC30:AG30"/>
-    <mergeCell ref="X30:AB30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="N30:T30"/>
-    <mergeCell ref="J30:M30"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="127" priority="22"/>

</xml_diff>

<commit_message>
Added and changed dragon skus!
Former-commit-id: 0c348b41ae023e1c86df66cd6ce45eeca884ea43
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="254">
   <si>
     <t>[sku]</t>
   </si>
@@ -783,13 +783,16 @@
   </si>
   <si>
     <t>TID_DRAGON_ALIEN_DESC</t>
+  </si>
+  <si>
+    <t>[dragonSku]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -890,6 +893,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -1417,7 +1426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="274">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2133,6 +2142,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4876,9 +4888,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B47:W61" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B47:W61"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="dragonSettings22" displayName="dragonSettings22" ref="B47:X61" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="B47:X61"/>
+  <tableColumns count="23">
     <tableColumn id="1" name="{dragonProgressionDefinitions}"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[maxLevel]"/>
@@ -4901,6 +4913,7 @@
     <tableColumn id="20" name="[xpLevel17]"/>
     <tableColumn id="21" name="[xpLevel18]"/>
     <tableColumn id="22" name="[xpLevel19]"/>
+    <tableColumn id="23" name="[dragonSku]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5188,8 +5201,8 @@
   </sheetPr>
   <dimension ref="A1:BT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI13" workbookViewId="0">
-      <selection activeCell="AR28" sqref="AR28"/>
+    <sheetView tabSelected="1" topLeftCell="N43" workbookViewId="0">
+      <selection activeCell="AB63" sqref="AB63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5203,7 +5216,9 @@
     <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.7109375" customWidth="1"/>
+    <col min="25" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14.28515625" customWidth="1"/>
     <col min="34" max="35" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="19.140625" bestFit="1" customWidth="1"/>
@@ -5471,10 +5486,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="258"/>
-      <c r="AP14" s="258"/>
-      <c r="AQ14" s="258"/>
-      <c r="AR14" s="258"/>
+      <c r="AO14" s="259"/>
+      <c r="AP14" s="259"/>
+      <c r="AQ14" s="259"/>
+      <c r="AR14" s="259"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -8639,83 +8654,83 @@
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="30"/>
-      <c r="J30" s="273" t="s">
+      <c r="J30" s="274" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="273"/>
-      <c r="L30" s="273"/>
-      <c r="M30" s="273"/>
-      <c r="N30" s="270" t="s">
+      <c r="K30" s="274"/>
+      <c r="L30" s="274"/>
+      <c r="M30" s="274"/>
+      <c r="N30" s="271" t="s">
         <v>73</v>
       </c>
-      <c r="O30" s="271"/>
-      <c r="P30" s="271"/>
-      <c r="Q30" s="271"/>
-      <c r="R30" s="272"/>
-      <c r="S30" s="271"/>
-      <c r="T30" s="271"/>
-      <c r="U30" s="268" t="s">
+      <c r="O30" s="272"/>
+      <c r="P30" s="272"/>
+      <c r="Q30" s="272"/>
+      <c r="R30" s="273"/>
+      <c r="S30" s="272"/>
+      <c r="T30" s="272"/>
+      <c r="U30" s="269" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="269"/>
+      <c r="V30" s="270"/>
       <c r="W30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X30" s="265" t="s">
+      <c r="X30" s="266" t="s">
         <v>70</v>
       </c>
-      <c r="Y30" s="266"/>
-      <c r="Z30" s="266"/>
-      <c r="AA30" s="266"/>
-      <c r="AB30" s="267"/>
-      <c r="AC30" s="264" t="s">
+      <c r="Y30" s="267"/>
+      <c r="Z30" s="267"/>
+      <c r="AA30" s="267"/>
+      <c r="AB30" s="268"/>
+      <c r="AC30" s="265" t="s">
         <v>69</v>
       </c>
-      <c r="AD30" s="264"/>
-      <c r="AE30" s="264"/>
-      <c r="AF30" s="264"/>
-      <c r="AG30" s="264"/>
+      <c r="AD30" s="265"/>
+      <c r="AE30" s="265"/>
+      <c r="AF30" s="265"/>
+      <c r="AG30" s="265"/>
       <c r="AH30" s="30"/>
-      <c r="AI30" s="260" t="s">
+      <c r="AI30" s="261" t="s">
         <v>68</v>
       </c>
-      <c r="AJ30" s="260"/>
-      <c r="AK30" s="254" t="s">
+      <c r="AJ30" s="261"/>
+      <c r="AK30" s="255" t="s">
         <v>246</v>
       </c>
-      <c r="AL30" s="254"/>
-      <c r="AM30" s="261" t="s">
+      <c r="AL30" s="255"/>
+      <c r="AM30" s="262" t="s">
         <v>236</v>
       </c>
-      <c r="AN30" s="262"/>
-      <c r="AO30" s="262"/>
-      <c r="AP30" s="262"/>
-      <c r="AQ30" s="262"/>
-      <c r="AR30" s="263"/>
-      <c r="AS30" s="255" t="s">
+      <c r="AN30" s="263"/>
+      <c r="AO30" s="263"/>
+      <c r="AP30" s="263"/>
+      <c r="AQ30" s="263"/>
+      <c r="AR30" s="264"/>
+      <c r="AS30" s="256" t="s">
         <v>226</v>
       </c>
-      <c r="AT30" s="256"/>
-      <c r="AU30" s="256"/>
-      <c r="AV30" s="256"/>
-      <c r="AW30" s="256"/>
-      <c r="AX30" s="256"/>
-      <c r="AY30" s="257"/>
+      <c r="AT30" s="257"/>
+      <c r="AU30" s="257"/>
+      <c r="AV30" s="257"/>
+      <c r="AW30" s="257"/>
+      <c r="AX30" s="257"/>
+      <c r="AY30" s="258"/>
       <c r="AZ30" s="30"/>
       <c r="BA30" s="30"/>
       <c r="BB30" s="30"/>
       <c r="BC30" s="30"/>
       <c r="BD30" s="30"/>
       <c r="BE30" s="30"/>
-      <c r="BF30" s="259" t="s">
+      <c r="BF30" s="260" t="s">
         <v>67</v>
       </c>
-      <c r="BG30" s="259"/>
-      <c r="BH30" s="259"/>
-      <c r="BI30" s="259"/>
-      <c r="BJ30" s="259"/>
-      <c r="BK30" s="259"/>
-      <c r="BL30" s="259"/>
+      <c r="BG30" s="260"/>
+      <c r="BH30" s="260"/>
+      <c r="BI30" s="260"/>
+      <c r="BJ30" s="260"/>
+      <c r="BK30" s="260"/>
+      <c r="BL30" s="260"/>
       <c r="BM30" s="30"/>
       <c r="BN30" s="30"/>
       <c r="BO30" s="30"/>
@@ -9241,6 +9256,9 @@
       <c r="W47" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="X47" s="254" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="48" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
@@ -9309,8 +9327,11 @@
       <c r="W48" t="s">
         <v>20</v>
       </c>
+      <c r="X48" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>3</v>
       </c>
@@ -9377,8 +9398,11 @@
       <c r="W49" t="s">
         <v>20</v>
       </c>
+      <c r="X49" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>3</v>
       </c>
@@ -9445,8 +9469,11 @@
       <c r="W50" t="s">
         <v>20</v>
       </c>
+      <c r="X50" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -9513,8 +9540,11 @@
       <c r="W51" t="s">
         <v>20</v>
       </c>
+      <c r="X51" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -9581,8 +9611,11 @@
       <c r="W52" t="s">
         <v>20</v>
       </c>
+      <c r="X52" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>3</v>
       </c>
@@ -9649,8 +9682,11 @@
       <c r="W53" t="s">
         <v>20</v>
       </c>
+      <c r="X53" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -9717,8 +9753,11 @@
       <c r="W54" t="s">
         <v>20</v>
       </c>
+      <c r="X54" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>3</v>
       </c>
@@ -9785,8 +9824,11 @@
       <c r="W55">
         <v>485030</v>
       </c>
+      <c r="X55" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>3</v>
       </c>
@@ -9853,8 +9895,11 @@
       <c r="W56" s="84">
         <v>558660</v>
       </c>
+      <c r="X56" t="s">
+        <v>184</v>
+      </c>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>3</v>
       </c>
@@ -9921,8 +9966,11 @@
       <c r="W57">
         <v>633960</v>
       </c>
+      <c r="X57" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>3</v>
       </c>
@@ -9989,8 +10037,11 @@
       <c r="W58">
         <v>710770</v>
       </c>
+      <c r="X58" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>3</v>
       </c>
@@ -10057,8 +10108,11 @@
       <c r="W59">
         <v>789000</v>
       </c>
+      <c r="X59" t="s">
+        <v>197</v>
+      </c>
     </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>3</v>
       </c>
@@ -10125,8 +10179,11 @@
       <c r="W60" s="129">
         <v>868540</v>
       </c>
+      <c r="X60" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>3</v>
       </c>
@@ -10192,6 +10249,9 @@
       </c>
       <c r="W61" s="129">
         <v>949320</v>
+      </c>
+      <c r="X61" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sku in missionDragonModifiersDefinitions and in dragonProgressionDefinitions changed.
Former-commit-id: bf999275867295e0bdf1fafb888924955a838e6e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="268">
   <si>
     <t>[sku]</t>
   </si>
@@ -786,6 +786,48 @@
   </si>
   <si>
     <t>[dragonSku]</t>
+  </si>
+  <si>
+    <t>dragon_baby_progression</t>
+  </si>
+  <si>
+    <t>dragon_crocodile_progression</t>
+  </si>
+  <si>
+    <t>dragon_reptile_progression</t>
+  </si>
+  <si>
+    <t>dragon_fat_progression</t>
+  </si>
+  <si>
+    <t>dragon_bug_progression</t>
+  </si>
+  <si>
+    <t>dragon_chinese_progression</t>
+  </si>
+  <si>
+    <t>dragon_classic_progression</t>
+  </si>
+  <si>
+    <t>dragon_devil_progression</t>
+  </si>
+  <si>
+    <t>dragon_jawfrey_progression</t>
+  </si>
+  <si>
+    <t>dragon_balrog_progression</t>
+  </si>
+  <si>
+    <t>dragon_titan_progression</t>
+  </si>
+  <si>
+    <t>dragon_goldheist_progression</t>
+  </si>
+  <si>
+    <t>dragon_dark_progression</t>
+  </si>
+  <si>
+    <t>dragon_alien_progression</t>
   </si>
 </sst>
 </file>
@@ -2146,6 +2188,36 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2174,36 +2246,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5201,8 +5243,8 @@
   </sheetPr>
   <dimension ref="A1:BT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N43" workbookViewId="0">
-      <selection activeCell="AB63" sqref="AB63"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5486,10 +5528,10 @@
       <c r="AG14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AO14" s="259"/>
-      <c r="AP14" s="259"/>
-      <c r="AQ14" s="259"/>
-      <c r="AR14" s="259"/>
+      <c r="AO14" s="269"/>
+      <c r="AP14" s="269"/>
+      <c r="AQ14" s="269"/>
+      <c r="AR14" s="269"/>
     </row>
     <row r="15" spans="2:72" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
@@ -8654,83 +8696,83 @@
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="30"/>
-      <c r="J30" s="274" t="s">
+      <c r="J30" s="264" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="274"/>
-      <c r="L30" s="274"/>
-      <c r="M30" s="274"/>
-      <c r="N30" s="271" t="s">
+      <c r="K30" s="264"/>
+      <c r="L30" s="264"/>
+      <c r="M30" s="264"/>
+      <c r="N30" s="261" t="s">
         <v>73</v>
       </c>
-      <c r="O30" s="272"/>
-      <c r="P30" s="272"/>
-      <c r="Q30" s="272"/>
-      <c r="R30" s="273"/>
-      <c r="S30" s="272"/>
-      <c r="T30" s="272"/>
-      <c r="U30" s="269" t="s">
+      <c r="O30" s="262"/>
+      <c r="P30" s="262"/>
+      <c r="Q30" s="262"/>
+      <c r="R30" s="263"/>
+      <c r="S30" s="262"/>
+      <c r="T30" s="262"/>
+      <c r="U30" s="259" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="270"/>
+      <c r="V30" s="260"/>
       <c r="W30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="X30" s="266" t="s">
+      <c r="X30" s="256" t="s">
         <v>70</v>
       </c>
-      <c r="Y30" s="267"/>
-      <c r="Z30" s="267"/>
-      <c r="AA30" s="267"/>
-      <c r="AB30" s="268"/>
-      <c r="AC30" s="265" t="s">
+      <c r="Y30" s="257"/>
+      <c r="Z30" s="257"/>
+      <c r="AA30" s="257"/>
+      <c r="AB30" s="258"/>
+      <c r="AC30" s="255" t="s">
         <v>69</v>
       </c>
-      <c r="AD30" s="265"/>
-      <c r="AE30" s="265"/>
-      <c r="AF30" s="265"/>
-      <c r="AG30" s="265"/>
+      <c r="AD30" s="255"/>
+      <c r="AE30" s="255"/>
+      <c r="AF30" s="255"/>
+      <c r="AG30" s="255"/>
       <c r="AH30" s="30"/>
-      <c r="AI30" s="261" t="s">
+      <c r="AI30" s="271" t="s">
         <v>68</v>
       </c>
-      <c r="AJ30" s="261"/>
-      <c r="AK30" s="255" t="s">
+      <c r="AJ30" s="271"/>
+      <c r="AK30" s="265" t="s">
         <v>246</v>
       </c>
-      <c r="AL30" s="255"/>
-      <c r="AM30" s="262" t="s">
+      <c r="AL30" s="265"/>
+      <c r="AM30" s="272" t="s">
         <v>236</v>
       </c>
-      <c r="AN30" s="263"/>
-      <c r="AO30" s="263"/>
-      <c r="AP30" s="263"/>
-      <c r="AQ30" s="263"/>
-      <c r="AR30" s="264"/>
-      <c r="AS30" s="256" t="s">
+      <c r="AN30" s="273"/>
+      <c r="AO30" s="273"/>
+      <c r="AP30" s="273"/>
+      <c r="AQ30" s="273"/>
+      <c r="AR30" s="274"/>
+      <c r="AS30" s="266" t="s">
         <v>226</v>
       </c>
-      <c r="AT30" s="257"/>
-      <c r="AU30" s="257"/>
-      <c r="AV30" s="257"/>
-      <c r="AW30" s="257"/>
-      <c r="AX30" s="257"/>
-      <c r="AY30" s="258"/>
+      <c r="AT30" s="267"/>
+      <c r="AU30" s="267"/>
+      <c r="AV30" s="267"/>
+      <c r="AW30" s="267"/>
+      <c r="AX30" s="267"/>
+      <c r="AY30" s="268"/>
       <c r="AZ30" s="30"/>
       <c r="BA30" s="30"/>
       <c r="BB30" s="30"/>
       <c r="BC30" s="30"/>
       <c r="BD30" s="30"/>
       <c r="BE30" s="30"/>
-      <c r="BF30" s="260" t="s">
+      <c r="BF30" s="270" t="s">
         <v>67</v>
       </c>
-      <c r="BG30" s="260"/>
-      <c r="BH30" s="260"/>
-      <c r="BI30" s="260"/>
-      <c r="BJ30" s="260"/>
-      <c r="BK30" s="260"/>
-      <c r="BL30" s="260"/>
+      <c r="BG30" s="270"/>
+      <c r="BH30" s="270"/>
+      <c r="BI30" s="270"/>
+      <c r="BJ30" s="270"/>
+      <c r="BK30" s="270"/>
+      <c r="BL30" s="270"/>
       <c r="BM30" s="30"/>
       <c r="BN30" s="30"/>
       <c r="BO30" s="30"/>
@@ -9265,7 +9307,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>254</v>
       </c>
       <c r="D48">
         <v>8</v>
@@ -9336,7 +9378,7 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>255</v>
       </c>
       <c r="D49">
         <v>10</v>
@@ -9407,7 +9449,7 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>256</v>
       </c>
       <c r="D50">
         <v>10</v>
@@ -9478,7 +9520,7 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>257</v>
       </c>
       <c r="D51">
         <v>10</v>
@@ -9549,7 +9591,7 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>258</v>
       </c>
       <c r="D52">
         <v>15</v>
@@ -9620,7 +9662,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>259</v>
       </c>
       <c r="D53">
         <v>15</v>
@@ -9691,7 +9733,7 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>260</v>
       </c>
       <c r="D54">
         <v>15</v>
@@ -9762,7 +9804,7 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>261</v>
       </c>
       <c r="D55">
         <v>20</v>
@@ -9833,7 +9875,7 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>184</v>
+        <v>262</v>
       </c>
       <c r="D56">
         <v>20</v>
@@ -9904,7 +9946,7 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="D57">
         <v>20</v>
@@ -9975,7 +10017,7 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>264</v>
       </c>
       <c r="D58">
         <v>20</v>
@@ -10046,7 +10088,7 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>197</v>
+        <v>265</v>
       </c>
       <c r="D59">
         <v>20</v>
@@ -10117,7 +10159,7 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="D60">
         <v>20</v>
@@ -10188,7 +10230,7 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="D61">
         <v>20</v>
@@ -10256,17 +10298,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AC30:AG30"/>
-    <mergeCell ref="X30:AB30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="N30:T30"/>
-    <mergeCell ref="J30:M30"/>
     <mergeCell ref="AK30:AL30"/>
     <mergeCell ref="AS30:AY30"/>
     <mergeCell ref="AO14:AR14"/>
     <mergeCell ref="BF30:BL30"/>
     <mergeCell ref="AI30:AJ30"/>
     <mergeCell ref="AM30:AR30"/>
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="N30:T30"/>
+    <mergeCell ref="J30:M30"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:C23 C25:C26">
     <cfRule type="duplicateValues" dxfId="127" priority="22"/>

</xml_diff>

<commit_message>
Umbra, Alien and Skeleton same price: 550 gems
Former-commit-id: 57310b6900afd2e7015725106f78d7b9314eeaaf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Dragons.xlsx
+++ b/Docs/Content/HungryDragonContent_Dragons.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="dragons" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2153,6 +2153,36 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2181,303 +2211,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="134">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="131">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -4816,6 +4556,236 @@
       </font>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4830,105 +4800,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT30" totalsRowShown="0" headerRowDxfId="133" dataDxfId="131" headerRowBorderDxfId="132" tableBorderDxfId="130" totalsRowBorderDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="dragonDefinitions" displayName="dragonDefinitions" ref="B15:BT30" totalsRowShown="0" headerRowDxfId="107" da